<commit_message>
Created Models for Issues #16 Sink and #15 Bathtub Updated Timetable
</commit_message>
<xml_diff>
--- a/Documents/Zeitplan.xlsx
+++ b/Documents/Zeitplan.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin.wuestner\Documents\SiemensVR\Dokumente\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VirtualReality\Documents\SiemensVR\Software\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22140" windowHeight="9465"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22140" windowHeight="9468"/>
   </bookViews>
   <sheets>
     <sheet name="Mai 2017" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Mai 2017'!$A$4:$G$90</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="161">
   <si>
     <t>Projekttitel</t>
   </si>
@@ -503,6 +503,9 @@
   </si>
   <si>
     <t>Ist-Zeit (Beide)</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -1161,6 +1164,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1173,32 +1194,31 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1206,42 +1226,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1250,6 +1234,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1297,24 +1284,40 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1415,8 +1418,8 @@
       <xdr:rowOff>51955</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1797380</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>212420</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>34638</xdr:rowOff>
     </xdr:to>
@@ -1784,60 +1787,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GI90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AN53" sqref="AN53"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA51" sqref="AA51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="1" customWidth="1"/>
-    <col min="8" max="91" width="3.42578125" style="1" customWidth="1"/>
-    <col min="92" max="256" width="3.28515625" style="1" customWidth="1"/>
-    <col min="257" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="191" width="5.77734375" style="1" customWidth="1"/>
+    <col min="192" max="256" width="3.33203125" style="1" customWidth="1"/>
+    <col min="257" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:191" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="112" t="s">
+    <row r="1" spans="1:191" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="112"/>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="112"/>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
     </row>
-    <row r="2" spans="1:191" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:191" x14ac:dyDescent="0.25">
       <c r="T2" s="9"/>
       <c r="U2" s="9"/>
       <c r="V2" s="9"/>
       <c r="AD2" s="48"/>
     </row>
-    <row r="3" spans="1:191" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:191" x14ac:dyDescent="0.25">
       <c r="T3" s="9"/>
       <c r="U3" s="9"/>
       <c r="V3" s="9"/>
     </row>
-    <row r="4" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1853,20 +1849,23 @@
       <c r="G4" s="11">
         <v>42856</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="N4" s="57"/>
-      <c r="P4" s="67" t="s">
+      <c r="P4" s="81" t="s">
         <v>157</v>
       </c>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="67"/>
-      <c r="W4" s="67"/>
-      <c r="X4" s="67"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="81"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
     </row>
-    <row r="5" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1881,24 +1880,24 @@
       <c r="F5" s="5"/>
       <c r="G5" s="7"/>
       <c r="N5" s="24"/>
-      <c r="P5" s="67" t="s">
+      <c r="P5" s="81" t="s">
         <v>158</v>
       </c>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="67"/>
-      <c r="S5" s="67"/>
-      <c r="T5" s="67"/>
-      <c r="U5" s="67"/>
-      <c r="V5" s="67"/>
-      <c r="W5" s="67"/>
-      <c r="X5" s="67"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="81"/>
+      <c r="S5" s="81"/>
+      <c r="T5" s="81"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
+      <c r="W5" s="81"/>
+      <c r="X5" s="81"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
       <c r="AC5" s="5"/>
     </row>
-    <row r="6" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -1915,24 +1914,24 @@
         <v>15</v>
       </c>
       <c r="N6" s="16"/>
-      <c r="P6" s="67" t="s">
+      <c r="P6" s="81" t="s">
         <v>159</v>
       </c>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="67"/>
-      <c r="V6" s="67"/>
-      <c r="W6" s="67"/>
-      <c r="X6" s="67"/>
+      <c r="Q6" s="81"/>
+      <c r="R6" s="81"/>
+      <c r="S6" s="81"/>
+      <c r="T6" s="81"/>
+      <c r="U6" s="81"/>
+      <c r="V6" s="81"/>
+      <c r="W6" s="81"/>
+      <c r="X6" s="81"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
       <c r="AC6" s="5"/>
     </row>
-    <row r="7" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1943,19 +1942,19 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="N7" s="21"/>
-      <c r="P7" s="67" t="s">
+      <c r="P7" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="67"/>
-      <c r="R7" s="67"/>
-      <c r="S7" s="67"/>
-      <c r="T7" s="67"/>
-      <c r="U7" s="67"/>
-      <c r="V7" s="67"/>
-      <c r="W7" s="67"/>
-      <c r="X7" s="67"/>
+      <c r="Q7" s="81"/>
+      <c r="R7" s="81"/>
+      <c r="S7" s="81"/>
+      <c r="T7" s="81"/>
+      <c r="U7" s="81"/>
+      <c r="V7" s="81"/>
+      <c r="W7" s="81"/>
+      <c r="X7" s="81"/>
     </row>
-    <row r="8" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1968,41 +1967,41 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="N8" s="20"/>
-      <c r="P8" s="70" t="s">
+      <c r="P8" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="70"/>
-      <c r="R8" s="70"/>
-      <c r="S8" s="70"/>
-      <c r="T8" s="70"/>
-      <c r="U8" s="70"/>
-      <c r="V8" s="70"/>
-      <c r="W8" s="70"/>
-      <c r="X8" s="70"/>
+      <c r="Q8" s="113"/>
+      <c r="R8" s="113"/>
+      <c r="S8" s="113"/>
+      <c r="T8" s="113"/>
+      <c r="U8" s="113"/>
+      <c r="V8" s="113"/>
+      <c r="W8" s="113"/>
+      <c r="X8" s="113"/>
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
       <c r="AC8" s="5"/>
     </row>
-    <row r="9" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="68"/>
+    <row r="9" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="118"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="12"/>
       <c r="N9" s="49"/>
-      <c r="P9" s="70" t="s">
+      <c r="P9" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="Q9" s="70"/>
-      <c r="R9" s="70"/>
-      <c r="S9" s="70"/>
-      <c r="T9" s="70"/>
-      <c r="U9" s="70"/>
-      <c r="V9" s="70"/>
-      <c r="W9" s="70"/>
-      <c r="X9" s="70"/>
+      <c r="Q9" s="113"/>
+      <c r="R9" s="113"/>
+      <c r="S9" s="113"/>
+      <c r="T9" s="113"/>
+      <c r="U9" s="113"/>
+      <c r="V9" s="113"/>
+      <c r="W9" s="113"/>
+      <c r="X9" s="113"/>
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
@@ -2011,8 +2010,8 @@
       <c r="AE9" s="12"/>
       <c r="AJ9" s="13"/>
     </row>
-    <row r="10" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="68"/>
+    <row r="10" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="118"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -2028,19 +2027,19 @@
       <c r="AB10" s="5"/>
       <c r="AC10" s="5"/>
     </row>
-    <row r="11" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="68"/>
-      <c r="C11" s="78" t="s">
+    <row r="11" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="118"/>
+      <c r="C11" s="116" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="76" t="s">
+      <c r="D11" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76" t="s">
+      <c r="E11" s="114"/>
+      <c r="F11" s="114" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="76"/>
+      <c r="G11" s="114"/>
       <c r="T11" s="9"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
@@ -2052,597 +2051,597 @@
       <c r="AB11" s="5"/>
       <c r="AC11" s="5"/>
     </row>
-    <row r="12" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="68"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="62" t="s">
+    <row r="12" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="118"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="114"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="114"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="63"/>
-      <c r="J12" s="63"/>
-      <c r="K12" s="63"/>
-      <c r="L12" s="63"/>
-      <c r="M12" s="63"/>
-      <c r="N12" s="63"/>
-      <c r="O12" s="63"/>
-      <c r="P12" s="63"/>
-      <c r="Q12" s="63"/>
-      <c r="R12" s="63"/>
-      <c r="S12" s="63"/>
-      <c r="T12" s="63"/>
-      <c r="U12" s="63"/>
-      <c r="V12" s="63"/>
-      <c r="W12" s="63"/>
-      <c r="X12" s="63"/>
-      <c r="Y12" s="63"/>
-      <c r="Z12" s="63"/>
-      <c r="AA12" s="63"/>
-      <c r="AB12" s="63"/>
-      <c r="AC12" s="63"/>
-      <c r="AD12" s="63"/>
-      <c r="AE12" s="63"/>
-      <c r="AF12" s="63"/>
-      <c r="AG12" s="63"/>
-      <c r="AH12" s="63"/>
-      <c r="AI12" s="63"/>
-      <c r="AJ12" s="63"/>
-      <c r="AK12" s="63"/>
-      <c r="AL12" s="63"/>
-      <c r="AM12" s="63"/>
-      <c r="AN12" s="63"/>
-      <c r="AO12" s="63"/>
-      <c r="AP12" s="63"/>
-      <c r="AQ12" s="63"/>
-      <c r="AR12" s="63"/>
-      <c r="AS12" s="63"/>
-      <c r="AT12" s="63"/>
-      <c r="AU12" s="63"/>
-      <c r="AV12" s="63"/>
-      <c r="AW12" s="63"/>
-      <c r="AX12" s="63"/>
-      <c r="AY12" s="63"/>
-      <c r="AZ12" s="63"/>
-      <c r="BA12" s="63"/>
-      <c r="BB12" s="63"/>
-      <c r="BC12" s="63"/>
-      <c r="BD12" s="63"/>
-      <c r="BE12" s="63"/>
-      <c r="BF12" s="63"/>
-      <c r="BG12" s="63"/>
-      <c r="BH12" s="63"/>
-      <c r="BI12" s="63"/>
-      <c r="BJ12" s="63"/>
-      <c r="BK12" s="63"/>
-      <c r="BL12" s="63"/>
-      <c r="BM12" s="63"/>
-      <c r="BN12" s="63"/>
-      <c r="BO12" s="63"/>
-      <c r="BP12" s="63"/>
-      <c r="BQ12" s="64"/>
-      <c r="BR12" s="62" t="s">
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="71"/>
+      <c r="O12" s="71"/>
+      <c r="P12" s="71"/>
+      <c r="Q12" s="71"/>
+      <c r="R12" s="71"/>
+      <c r="S12" s="71"/>
+      <c r="T12" s="71"/>
+      <c r="U12" s="71"/>
+      <c r="V12" s="71"/>
+      <c r="W12" s="71"/>
+      <c r="X12" s="71"/>
+      <c r="Y12" s="71"/>
+      <c r="Z12" s="71"/>
+      <c r="AA12" s="71"/>
+      <c r="AB12" s="71"/>
+      <c r="AC12" s="71"/>
+      <c r="AD12" s="71"/>
+      <c r="AE12" s="71"/>
+      <c r="AF12" s="71"/>
+      <c r="AG12" s="71"/>
+      <c r="AH12" s="71"/>
+      <c r="AI12" s="71"/>
+      <c r="AJ12" s="71"/>
+      <c r="AK12" s="71"/>
+      <c r="AL12" s="71"/>
+      <c r="AM12" s="71"/>
+      <c r="AN12" s="71"/>
+      <c r="AO12" s="71"/>
+      <c r="AP12" s="71"/>
+      <c r="AQ12" s="71"/>
+      <c r="AR12" s="71"/>
+      <c r="AS12" s="71"/>
+      <c r="AT12" s="71"/>
+      <c r="AU12" s="71"/>
+      <c r="AV12" s="71"/>
+      <c r="AW12" s="71"/>
+      <c r="AX12" s="71"/>
+      <c r="AY12" s="71"/>
+      <c r="AZ12" s="71"/>
+      <c r="BA12" s="71"/>
+      <c r="BB12" s="71"/>
+      <c r="BC12" s="71"/>
+      <c r="BD12" s="71"/>
+      <c r="BE12" s="71"/>
+      <c r="BF12" s="71"/>
+      <c r="BG12" s="71"/>
+      <c r="BH12" s="71"/>
+      <c r="BI12" s="71"/>
+      <c r="BJ12" s="71"/>
+      <c r="BK12" s="71"/>
+      <c r="BL12" s="71"/>
+      <c r="BM12" s="71"/>
+      <c r="BN12" s="71"/>
+      <c r="BO12" s="71"/>
+      <c r="BP12" s="71"/>
+      <c r="BQ12" s="119"/>
+      <c r="BR12" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="BS12" s="63"/>
-      <c r="BT12" s="63"/>
-      <c r="BU12" s="63"/>
-      <c r="BV12" s="63"/>
-      <c r="BW12" s="63"/>
-      <c r="BX12" s="63"/>
-      <c r="BY12" s="63"/>
-      <c r="BZ12" s="63"/>
-      <c r="CA12" s="63"/>
-      <c r="CB12" s="63"/>
-      <c r="CC12" s="63"/>
-      <c r="CD12" s="63"/>
-      <c r="CE12" s="63"/>
-      <c r="CF12" s="63"/>
-      <c r="CG12" s="63"/>
-      <c r="CH12" s="63"/>
-      <c r="CI12" s="63"/>
-      <c r="CJ12" s="63"/>
-      <c r="CK12" s="63"/>
-      <c r="CL12" s="63"/>
-      <c r="CM12" s="63"/>
-      <c r="CN12" s="63"/>
-      <c r="CO12" s="63"/>
-      <c r="CP12" s="63"/>
-      <c r="CQ12" s="63"/>
-      <c r="CR12" s="63"/>
-      <c r="CS12" s="63"/>
-      <c r="CT12" s="63"/>
-      <c r="CU12" s="63"/>
-      <c r="CV12" s="63"/>
-      <c r="CW12" s="63"/>
-      <c r="CX12" s="63"/>
-      <c r="CY12" s="63"/>
-      <c r="CZ12" s="63"/>
-      <c r="DA12" s="63"/>
-      <c r="DB12" s="63"/>
-      <c r="DC12" s="63"/>
-      <c r="DD12" s="63"/>
-      <c r="DE12" s="63"/>
-      <c r="DF12" s="63"/>
-      <c r="DG12" s="63"/>
-      <c r="DH12" s="63"/>
-      <c r="DI12" s="63"/>
-      <c r="DJ12" s="63"/>
-      <c r="DK12" s="63"/>
-      <c r="DL12" s="63"/>
-      <c r="DM12" s="63"/>
-      <c r="DN12" s="63"/>
-      <c r="DO12" s="63"/>
-      <c r="DP12" s="63"/>
-      <c r="DQ12" s="63"/>
-      <c r="DR12" s="63"/>
-      <c r="DS12" s="63"/>
-      <c r="DT12" s="63"/>
-      <c r="DU12" s="63"/>
-      <c r="DV12" s="63"/>
-      <c r="DW12" s="63"/>
-      <c r="DX12" s="63"/>
-      <c r="DY12" s="64"/>
-      <c r="DZ12" s="62" t="s">
+      <c r="BS12" s="71"/>
+      <c r="BT12" s="71"/>
+      <c r="BU12" s="71"/>
+      <c r="BV12" s="71"/>
+      <c r="BW12" s="71"/>
+      <c r="BX12" s="71"/>
+      <c r="BY12" s="71"/>
+      <c r="BZ12" s="71"/>
+      <c r="CA12" s="71"/>
+      <c r="CB12" s="71"/>
+      <c r="CC12" s="71"/>
+      <c r="CD12" s="71"/>
+      <c r="CE12" s="71"/>
+      <c r="CF12" s="71"/>
+      <c r="CG12" s="71"/>
+      <c r="CH12" s="71"/>
+      <c r="CI12" s="71"/>
+      <c r="CJ12" s="71"/>
+      <c r="CK12" s="71"/>
+      <c r="CL12" s="71"/>
+      <c r="CM12" s="71"/>
+      <c r="CN12" s="71"/>
+      <c r="CO12" s="71"/>
+      <c r="CP12" s="71"/>
+      <c r="CQ12" s="71"/>
+      <c r="CR12" s="71"/>
+      <c r="CS12" s="71"/>
+      <c r="CT12" s="71"/>
+      <c r="CU12" s="71"/>
+      <c r="CV12" s="71"/>
+      <c r="CW12" s="71"/>
+      <c r="CX12" s="71"/>
+      <c r="CY12" s="71"/>
+      <c r="CZ12" s="71"/>
+      <c r="DA12" s="71"/>
+      <c r="DB12" s="71"/>
+      <c r="DC12" s="71"/>
+      <c r="DD12" s="71"/>
+      <c r="DE12" s="71"/>
+      <c r="DF12" s="71"/>
+      <c r="DG12" s="71"/>
+      <c r="DH12" s="71"/>
+      <c r="DI12" s="71"/>
+      <c r="DJ12" s="71"/>
+      <c r="DK12" s="71"/>
+      <c r="DL12" s="71"/>
+      <c r="DM12" s="71"/>
+      <c r="DN12" s="71"/>
+      <c r="DO12" s="71"/>
+      <c r="DP12" s="71"/>
+      <c r="DQ12" s="71"/>
+      <c r="DR12" s="71"/>
+      <c r="DS12" s="71"/>
+      <c r="DT12" s="71"/>
+      <c r="DU12" s="71"/>
+      <c r="DV12" s="71"/>
+      <c r="DW12" s="71"/>
+      <c r="DX12" s="71"/>
+      <c r="DY12" s="119"/>
+      <c r="DZ12" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="EA12" s="63"/>
-      <c r="EB12" s="63"/>
-      <c r="EC12" s="63"/>
-      <c r="ED12" s="63"/>
-      <c r="EE12" s="63"/>
-      <c r="EF12" s="63"/>
-      <c r="EG12" s="63"/>
-      <c r="EH12" s="63"/>
-      <c r="EI12" s="63"/>
-      <c r="EJ12" s="63"/>
-      <c r="EK12" s="63"/>
-      <c r="EL12" s="63"/>
-      <c r="EM12" s="63"/>
-      <c r="EN12" s="63"/>
-      <c r="EO12" s="63"/>
-      <c r="EP12" s="63"/>
-      <c r="EQ12" s="63"/>
-      <c r="ER12" s="63"/>
-      <c r="ES12" s="63"/>
-      <c r="ET12" s="63"/>
-      <c r="EU12" s="63"/>
-      <c r="EV12" s="63"/>
-      <c r="EW12" s="63"/>
-      <c r="EX12" s="63"/>
-      <c r="EY12" s="63"/>
-      <c r="EZ12" s="63"/>
-      <c r="FA12" s="63"/>
-      <c r="FB12" s="63"/>
-      <c r="FC12" s="63"/>
-      <c r="FD12" s="63"/>
-      <c r="FE12" s="63"/>
-      <c r="FF12" s="63"/>
-      <c r="FG12" s="63"/>
-      <c r="FH12" s="63"/>
-      <c r="FI12" s="63"/>
-      <c r="FJ12" s="63"/>
-      <c r="FK12" s="63"/>
-      <c r="FL12" s="63"/>
-      <c r="FM12" s="63"/>
-      <c r="FN12" s="63"/>
-      <c r="FO12" s="63"/>
-      <c r="FP12" s="63"/>
-      <c r="FQ12" s="63"/>
-      <c r="FR12" s="63"/>
-      <c r="FS12" s="63"/>
-      <c r="FT12" s="63"/>
-      <c r="FU12" s="63"/>
-      <c r="FV12" s="63"/>
-      <c r="FW12" s="63"/>
-      <c r="FX12" s="63"/>
-      <c r="FY12" s="63"/>
-      <c r="FZ12" s="63"/>
-      <c r="GA12" s="63"/>
-      <c r="GB12" s="63"/>
-      <c r="GC12" s="63"/>
-      <c r="GD12" s="63"/>
-      <c r="GE12" s="63"/>
-      <c r="GF12" s="63"/>
-      <c r="GG12" s="63"/>
-      <c r="GH12" s="63"/>
-      <c r="GI12" s="120"/>
+      <c r="EA12" s="71"/>
+      <c r="EB12" s="71"/>
+      <c r="EC12" s="71"/>
+      <c r="ED12" s="71"/>
+      <c r="EE12" s="71"/>
+      <c r="EF12" s="71"/>
+      <c r="EG12" s="71"/>
+      <c r="EH12" s="71"/>
+      <c r="EI12" s="71"/>
+      <c r="EJ12" s="71"/>
+      <c r="EK12" s="71"/>
+      <c r="EL12" s="71"/>
+      <c r="EM12" s="71"/>
+      <c r="EN12" s="71"/>
+      <c r="EO12" s="71"/>
+      <c r="EP12" s="71"/>
+      <c r="EQ12" s="71"/>
+      <c r="ER12" s="71"/>
+      <c r="ES12" s="71"/>
+      <c r="ET12" s="71"/>
+      <c r="EU12" s="71"/>
+      <c r="EV12" s="71"/>
+      <c r="EW12" s="71"/>
+      <c r="EX12" s="71"/>
+      <c r="EY12" s="71"/>
+      <c r="EZ12" s="71"/>
+      <c r="FA12" s="71"/>
+      <c r="FB12" s="71"/>
+      <c r="FC12" s="71"/>
+      <c r="FD12" s="71"/>
+      <c r="FE12" s="71"/>
+      <c r="FF12" s="71"/>
+      <c r="FG12" s="71"/>
+      <c r="FH12" s="71"/>
+      <c r="FI12" s="71"/>
+      <c r="FJ12" s="71"/>
+      <c r="FK12" s="71"/>
+      <c r="FL12" s="71"/>
+      <c r="FM12" s="71"/>
+      <c r="FN12" s="71"/>
+      <c r="FO12" s="71"/>
+      <c r="FP12" s="71"/>
+      <c r="FQ12" s="71"/>
+      <c r="FR12" s="71"/>
+      <c r="FS12" s="71"/>
+      <c r="FT12" s="71"/>
+      <c r="FU12" s="71"/>
+      <c r="FV12" s="71"/>
+      <c r="FW12" s="71"/>
+      <c r="FX12" s="71"/>
+      <c r="FY12" s="71"/>
+      <c r="FZ12" s="71"/>
+      <c r="GA12" s="71"/>
+      <c r="GB12" s="71"/>
+      <c r="GC12" s="71"/>
+      <c r="GD12" s="71"/>
+      <c r="GE12" s="71"/>
+      <c r="GF12" s="71"/>
+      <c r="GG12" s="71"/>
+      <c r="GH12" s="71"/>
+      <c r="GI12" s="72"/>
     </row>
-    <row r="13" spans="1:191" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:191" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="60">
+      <c r="C13" s="117"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="68">
         <v>1</v>
       </c>
-      <c r="I13" s="61"/>
-      <c r="J13" s="60">
+      <c r="I13" s="69"/>
+      <c r="J13" s="68">
         <v>2</v>
       </c>
-      <c r="K13" s="61"/>
-      <c r="L13" s="60">
+      <c r="K13" s="69"/>
+      <c r="L13" s="68">
         <v>3</v>
       </c>
-      <c r="M13" s="61"/>
-      <c r="N13" s="60">
+      <c r="M13" s="69"/>
+      <c r="N13" s="68">
         <v>4</v>
       </c>
-      <c r="O13" s="61"/>
-      <c r="P13" s="60">
+      <c r="O13" s="69"/>
+      <c r="P13" s="68">
         <v>5</v>
       </c>
-      <c r="Q13" s="61"/>
-      <c r="R13" s="60">
+      <c r="Q13" s="69"/>
+      <c r="R13" s="68">
         <v>6</v>
       </c>
-      <c r="S13" s="61"/>
-      <c r="T13" s="60">
+      <c r="S13" s="69"/>
+      <c r="T13" s="68">
         <v>7</v>
       </c>
-      <c r="U13" s="61"/>
-      <c r="V13" s="60">
+      <c r="U13" s="69"/>
+      <c r="V13" s="68">
         <v>8</v>
       </c>
-      <c r="W13" s="61"/>
-      <c r="X13" s="60">
+      <c r="W13" s="69"/>
+      <c r="X13" s="68">
         <v>9</v>
       </c>
-      <c r="Y13" s="61"/>
-      <c r="Z13" s="60">
+      <c r="Y13" s="69"/>
+      <c r="Z13" s="68">
         <v>10</v>
       </c>
-      <c r="AA13" s="61"/>
-      <c r="AB13" s="60">
+      <c r="AA13" s="69"/>
+      <c r="AB13" s="68">
         <v>11</v>
       </c>
-      <c r="AC13" s="61"/>
-      <c r="AD13" s="60">
+      <c r="AC13" s="69"/>
+      <c r="AD13" s="68">
         <v>12</v>
       </c>
-      <c r="AE13" s="61"/>
-      <c r="AF13" s="60">
+      <c r="AE13" s="69"/>
+      <c r="AF13" s="68">
         <v>13</v>
       </c>
-      <c r="AG13" s="61"/>
-      <c r="AH13" s="60">
+      <c r="AG13" s="69"/>
+      <c r="AH13" s="68">
         <v>14</v>
       </c>
-      <c r="AI13" s="61"/>
-      <c r="AJ13" s="60">
+      <c r="AI13" s="69"/>
+      <c r="AJ13" s="68">
         <v>15</v>
       </c>
-      <c r="AK13" s="61"/>
-      <c r="AL13" s="60">
+      <c r="AK13" s="69"/>
+      <c r="AL13" s="68">
         <v>16</v>
       </c>
-      <c r="AM13" s="61"/>
-      <c r="AN13" s="60">
+      <c r="AM13" s="69"/>
+      <c r="AN13" s="68">
         <v>17</v>
       </c>
-      <c r="AO13" s="61"/>
-      <c r="AP13" s="60">
+      <c r="AO13" s="69"/>
+      <c r="AP13" s="68">
         <v>18</v>
       </c>
-      <c r="AQ13" s="61"/>
-      <c r="AR13" s="60">
+      <c r="AQ13" s="69"/>
+      <c r="AR13" s="68">
         <v>19</v>
       </c>
-      <c r="AS13" s="61"/>
-      <c r="AT13" s="60">
+      <c r="AS13" s="69"/>
+      <c r="AT13" s="68">
         <v>20</v>
       </c>
-      <c r="AU13" s="61"/>
-      <c r="AV13" s="60">
+      <c r="AU13" s="69"/>
+      <c r="AV13" s="68">
         <v>21</v>
       </c>
-      <c r="AW13" s="61"/>
-      <c r="AX13" s="60">
+      <c r="AW13" s="69"/>
+      <c r="AX13" s="68">
         <v>22</v>
       </c>
-      <c r="AY13" s="61"/>
-      <c r="AZ13" s="60">
+      <c r="AY13" s="69"/>
+      <c r="AZ13" s="68">
         <v>23</v>
       </c>
-      <c r="BA13" s="61"/>
-      <c r="BB13" s="60">
+      <c r="BA13" s="69"/>
+      <c r="BB13" s="68">
         <v>24</v>
       </c>
-      <c r="BC13" s="61"/>
-      <c r="BD13" s="60">
+      <c r="BC13" s="69"/>
+      <c r="BD13" s="68">
         <v>25</v>
       </c>
-      <c r="BE13" s="61"/>
-      <c r="BF13" s="60">
+      <c r="BE13" s="69"/>
+      <c r="BF13" s="68">
         <v>26</v>
       </c>
-      <c r="BG13" s="61"/>
-      <c r="BH13" s="60">
+      <c r="BG13" s="69"/>
+      <c r="BH13" s="68">
         <v>27</v>
       </c>
-      <c r="BI13" s="61"/>
-      <c r="BJ13" s="60">
+      <c r="BI13" s="69"/>
+      <c r="BJ13" s="68">
         <v>28</v>
       </c>
-      <c r="BK13" s="61"/>
-      <c r="BL13" s="60">
+      <c r="BK13" s="69"/>
+      <c r="BL13" s="68">
         <v>29</v>
       </c>
-      <c r="BM13" s="61"/>
-      <c r="BN13" s="60">
+      <c r="BM13" s="69"/>
+      <c r="BN13" s="68">
         <v>30</v>
       </c>
-      <c r="BO13" s="61"/>
-      <c r="BP13" s="60">
+      <c r="BO13" s="69"/>
+      <c r="BP13" s="68">
         <v>31</v>
       </c>
-      <c r="BQ13" s="69"/>
-      <c r="BR13" s="60">
+      <c r="BQ13" s="120"/>
+      <c r="BR13" s="68">
         <v>1</v>
       </c>
-      <c r="BS13" s="61"/>
-      <c r="BT13" s="60">
+      <c r="BS13" s="69"/>
+      <c r="BT13" s="68">
         <v>2</v>
       </c>
-      <c r="BU13" s="61"/>
-      <c r="BV13" s="60">
+      <c r="BU13" s="69"/>
+      <c r="BV13" s="68">
         <v>3</v>
       </c>
-      <c r="BW13" s="61"/>
-      <c r="BX13" s="60">
+      <c r="BW13" s="69"/>
+      <c r="BX13" s="68">
         <v>4</v>
       </c>
-      <c r="BY13" s="61"/>
-      <c r="BZ13" s="60">
+      <c r="BY13" s="69"/>
+      <c r="BZ13" s="68">
         <v>5</v>
       </c>
-      <c r="CA13" s="61"/>
-      <c r="CB13" s="60">
+      <c r="CA13" s="69"/>
+      <c r="CB13" s="68">
         <v>6</v>
       </c>
-      <c r="CC13" s="61"/>
-      <c r="CD13" s="60">
+      <c r="CC13" s="69"/>
+      <c r="CD13" s="68">
         <v>7</v>
       </c>
-      <c r="CE13" s="61"/>
-      <c r="CF13" s="60">
+      <c r="CE13" s="69"/>
+      <c r="CF13" s="68">
         <v>8</v>
       </c>
-      <c r="CG13" s="61"/>
-      <c r="CH13" s="60">
+      <c r="CG13" s="69"/>
+      <c r="CH13" s="68">
         <v>9</v>
       </c>
-      <c r="CI13" s="61"/>
-      <c r="CJ13" s="60">
+      <c r="CI13" s="69"/>
+      <c r="CJ13" s="68">
         <v>10</v>
       </c>
-      <c r="CK13" s="61"/>
-      <c r="CL13" s="60">
+      <c r="CK13" s="69"/>
+      <c r="CL13" s="68">
         <v>11</v>
       </c>
-      <c r="CM13" s="61"/>
-      <c r="CN13" s="60">
+      <c r="CM13" s="69"/>
+      <c r="CN13" s="68">
         <v>12</v>
       </c>
-      <c r="CO13" s="61"/>
-      <c r="CP13" s="60">
+      <c r="CO13" s="69"/>
+      <c r="CP13" s="68">
         <v>13</v>
       </c>
-      <c r="CQ13" s="61"/>
-      <c r="CR13" s="60">
+      <c r="CQ13" s="69"/>
+      <c r="CR13" s="68">
         <v>14</v>
       </c>
-      <c r="CS13" s="61"/>
-      <c r="CT13" s="60">
+      <c r="CS13" s="69"/>
+      <c r="CT13" s="68">
         <v>15</v>
       </c>
-      <c r="CU13" s="61"/>
-      <c r="CV13" s="60">
+      <c r="CU13" s="69"/>
+      <c r="CV13" s="68">
         <v>16</v>
       </c>
-      <c r="CW13" s="61"/>
-      <c r="CX13" s="60">
+      <c r="CW13" s="69"/>
+      <c r="CX13" s="68">
         <v>17</v>
       </c>
-      <c r="CY13" s="61"/>
-      <c r="CZ13" s="60">
+      <c r="CY13" s="69"/>
+      <c r="CZ13" s="68">
         <v>18</v>
       </c>
-      <c r="DA13" s="61"/>
-      <c r="DB13" s="60">
+      <c r="DA13" s="69"/>
+      <c r="DB13" s="68">
         <v>19</v>
       </c>
-      <c r="DC13" s="61"/>
-      <c r="DD13" s="60">
+      <c r="DC13" s="69"/>
+      <c r="DD13" s="68">
         <v>20</v>
       </c>
-      <c r="DE13" s="61"/>
-      <c r="DF13" s="60">
+      <c r="DE13" s="69"/>
+      <c r="DF13" s="68">
         <v>21</v>
       </c>
-      <c r="DG13" s="61"/>
-      <c r="DH13" s="60">
+      <c r="DG13" s="69"/>
+      <c r="DH13" s="68">
         <v>22</v>
       </c>
-      <c r="DI13" s="61"/>
-      <c r="DJ13" s="60">
+      <c r="DI13" s="69"/>
+      <c r="DJ13" s="68">
         <v>23</v>
       </c>
-      <c r="DK13" s="61"/>
-      <c r="DL13" s="60">
+      <c r="DK13" s="69"/>
+      <c r="DL13" s="68">
         <v>24</v>
       </c>
-      <c r="DM13" s="61"/>
-      <c r="DN13" s="60">
+      <c r="DM13" s="69"/>
+      <c r="DN13" s="68">
         <v>25</v>
       </c>
-      <c r="DO13" s="61"/>
-      <c r="DP13" s="60">
+      <c r="DO13" s="69"/>
+      <c r="DP13" s="68">
         <v>26</v>
       </c>
-      <c r="DQ13" s="61"/>
-      <c r="DR13" s="60">
+      <c r="DQ13" s="69"/>
+      <c r="DR13" s="68">
         <v>27</v>
       </c>
-      <c r="DS13" s="61"/>
-      <c r="DT13" s="60">
+      <c r="DS13" s="69"/>
+      <c r="DT13" s="68">
         <v>28</v>
       </c>
-      <c r="DU13" s="61"/>
-      <c r="DV13" s="60">
+      <c r="DU13" s="69"/>
+      <c r="DV13" s="68">
         <v>29</v>
       </c>
-      <c r="DW13" s="61"/>
-      <c r="DX13" s="60">
+      <c r="DW13" s="69"/>
+      <c r="DX13" s="68">
         <v>30</v>
       </c>
-      <c r="DY13" s="61"/>
-      <c r="DZ13" s="60">
+      <c r="DY13" s="69"/>
+      <c r="DZ13" s="68">
         <v>1</v>
       </c>
-      <c r="EA13" s="61"/>
-      <c r="EB13" s="60">
+      <c r="EA13" s="69"/>
+      <c r="EB13" s="68">
         <v>2</v>
       </c>
-      <c r="EC13" s="61"/>
-      <c r="ED13" s="60">
+      <c r="EC13" s="69"/>
+      <c r="ED13" s="68">
         <v>3</v>
       </c>
-      <c r="EE13" s="61"/>
-      <c r="EF13" s="60">
+      <c r="EE13" s="69"/>
+      <c r="EF13" s="68">
         <v>4</v>
       </c>
-      <c r="EG13" s="61"/>
-      <c r="EH13" s="60">
+      <c r="EG13" s="69"/>
+      <c r="EH13" s="68">
         <v>5</v>
       </c>
-      <c r="EI13" s="61"/>
-      <c r="EJ13" s="60">
+      <c r="EI13" s="69"/>
+      <c r="EJ13" s="68">
         <v>6</v>
       </c>
-      <c r="EK13" s="61"/>
-      <c r="EL13" s="60">
+      <c r="EK13" s="69"/>
+      <c r="EL13" s="68">
         <v>7</v>
       </c>
-      <c r="EM13" s="61"/>
-      <c r="EN13" s="60">
+      <c r="EM13" s="69"/>
+      <c r="EN13" s="68">
         <v>8</v>
       </c>
-      <c r="EO13" s="61"/>
-      <c r="EP13" s="60">
+      <c r="EO13" s="69"/>
+      <c r="EP13" s="68">
         <v>9</v>
       </c>
-      <c r="EQ13" s="61"/>
-      <c r="ER13" s="60">
+      <c r="EQ13" s="69"/>
+      <c r="ER13" s="68">
         <v>10</v>
       </c>
-      <c r="ES13" s="61"/>
-      <c r="ET13" s="60">
+      <c r="ES13" s="69"/>
+      <c r="ET13" s="68">
         <v>11</v>
       </c>
-      <c r="EU13" s="61"/>
-      <c r="EV13" s="60">
+      <c r="EU13" s="69"/>
+      <c r="EV13" s="68">
         <v>12</v>
       </c>
-      <c r="EW13" s="61"/>
-      <c r="EX13" s="60">
+      <c r="EW13" s="69"/>
+      <c r="EX13" s="68">
         <v>13</v>
       </c>
-      <c r="EY13" s="61"/>
-      <c r="EZ13" s="60">
+      <c r="EY13" s="69"/>
+      <c r="EZ13" s="68">
         <v>14</v>
       </c>
-      <c r="FA13" s="61"/>
-      <c r="FB13" s="60">
+      <c r="FA13" s="69"/>
+      <c r="FB13" s="68">
         <v>15</v>
       </c>
-      <c r="FC13" s="61"/>
-      <c r="FD13" s="60">
+      <c r="FC13" s="69"/>
+      <c r="FD13" s="68">
         <v>16</v>
       </c>
-      <c r="FE13" s="61"/>
-      <c r="FF13" s="60">
+      <c r="FE13" s="69"/>
+      <c r="FF13" s="68">
         <v>17</v>
       </c>
-      <c r="FG13" s="61"/>
-      <c r="FH13" s="60">
+      <c r="FG13" s="69"/>
+      <c r="FH13" s="68">
         <v>18</v>
       </c>
-      <c r="FI13" s="61"/>
-      <c r="FJ13" s="60">
+      <c r="FI13" s="69"/>
+      <c r="FJ13" s="68">
         <v>19</v>
       </c>
-      <c r="FK13" s="61"/>
-      <c r="FL13" s="60">
+      <c r="FK13" s="69"/>
+      <c r="FL13" s="68">
         <v>20</v>
       </c>
-      <c r="FM13" s="61"/>
-      <c r="FN13" s="60">
+      <c r="FM13" s="69"/>
+      <c r="FN13" s="68">
         <v>21</v>
       </c>
-      <c r="FO13" s="61"/>
-      <c r="FP13" s="60">
+      <c r="FO13" s="69"/>
+      <c r="FP13" s="68">
         <v>22</v>
       </c>
-      <c r="FQ13" s="61"/>
-      <c r="FR13" s="60">
+      <c r="FQ13" s="69"/>
+      <c r="FR13" s="68">
         <v>23</v>
       </c>
-      <c r="FS13" s="61"/>
-      <c r="FT13" s="60">
+      <c r="FS13" s="69"/>
+      <c r="FT13" s="68">
         <v>24</v>
       </c>
-      <c r="FU13" s="61"/>
-      <c r="FV13" s="60">
+      <c r="FU13" s="69"/>
+      <c r="FV13" s="68">
         <v>25</v>
       </c>
-      <c r="FW13" s="61"/>
-      <c r="FX13" s="60">
+      <c r="FW13" s="69"/>
+      <c r="FX13" s="68">
         <v>26</v>
       </c>
-      <c r="FY13" s="61"/>
-      <c r="FZ13" s="60">
+      <c r="FY13" s="69"/>
+      <c r="FZ13" s="68">
         <v>27</v>
       </c>
-      <c r="GA13" s="61"/>
-      <c r="GB13" s="60">
+      <c r="GA13" s="69"/>
+      <c r="GB13" s="68">
         <v>28</v>
       </c>
-      <c r="GC13" s="61"/>
-      <c r="GD13" s="60">
+      <c r="GC13" s="69"/>
+      <c r="GD13" s="68">
         <v>29</v>
       </c>
-      <c r="GE13" s="61"/>
-      <c r="GF13" s="60">
+      <c r="GE13" s="69"/>
+      <c r="GF13" s="68">
         <v>30</v>
       </c>
-      <c r="GG13" s="61"/>
-      <c r="GH13" s="60">
+      <c r="GG13" s="69"/>
+      <c r="GH13" s="68">
         <v>31</v>
       </c>
-      <c r="GI13" s="61"/>
+      <c r="GI13" s="69"/>
     </row>
-    <row r="14" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="113" t="s">
+    <row r="14" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A14" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="114"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="37"/>
-      <c r="D14" s="97">
+      <c r="D14" s="91">
         <f>SUM(D15:E61)</f>
         <v>51.050000000000011</v>
       </c>
-      <c r="E14" s="99"/>
-      <c r="F14" s="97">
+      <c r="E14" s="93"/>
+      <c r="F14" s="91">
         <f>SUM(F15:G61)</f>
-        <v>22.900000000000002</v>
-      </c>
-      <c r="G14" s="98"/>
+        <v>30.650000000000002</v>
+      </c>
+      <c r="G14" s="92"/>
       <c r="H14" s="18"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -2828,23 +2827,23 @@
       <c r="GH14" s="14"/>
       <c r="GI14" s="14"/>
     </row>
-    <row r="15" spans="1:191" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="73" t="s">
+    <row r="15" spans="1:191" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="74"/>
+      <c r="B15" s="83"/>
       <c r="C15" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="65">
+      <c r="D15" s="62">
         <v>1.5</v>
       </c>
-      <c r="E15" s="66"/>
-      <c r="F15" s="65">
+      <c r="E15" s="63"/>
+      <c r="F15" s="62">
         <f>SUM(H15:GI15)</f>
         <v>0.5</v>
       </c>
-      <c r="G15" s="80"/>
+      <c r="G15" s="64"/>
       <c r="H15" s="47"/>
       <c r="I15" s="12"/>
       <c r="J15" s="24">
@@ -3032,23 +3031,23 @@
       <c r="GH15" s="34"/>
       <c r="GI15" s="34"/>
     </row>
-    <row r="16" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="81" t="s">
+    <row r="16" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A16" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="82"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="62">
         <v>0.6</v>
       </c>
-      <c r="E16" s="66"/>
-      <c r="F16" s="65">
+      <c r="E16" s="63"/>
+      <c r="F16" s="62">
         <f>SUM(H16:GI16)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="80"/>
+      <c r="G16" s="64"/>
       <c r="H16" s="47"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
@@ -3234,23 +3233,23 @@
       <c r="GH16" s="32"/>
       <c r="GI16" s="32"/>
     </row>
-    <row r="17" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="81" t="s">
+    <row r="17" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A17" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="82"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="65">
+      <c r="D17" s="62">
         <v>1</v>
       </c>
-      <c r="E17" s="66"/>
-      <c r="F17" s="65">
+      <c r="E17" s="63"/>
+      <c r="F17" s="62">
         <f>SUM(H17:GI17)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="80"/>
+      <c r="G17" s="64"/>
       <c r="H17" s="47"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
@@ -3440,23 +3439,23 @@
       <c r="GH17" s="32"/>
       <c r="GI17" s="32"/>
     </row>
-    <row r="18" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="81" t="s">
+    <row r="18" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A18" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="82"/>
+      <c r="B18" s="67"/>
       <c r="C18" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="65">
+      <c r="D18" s="62">
         <v>0.8</v>
       </c>
-      <c r="E18" s="66"/>
-      <c r="F18" s="65">
+      <c r="E18" s="63"/>
+      <c r="F18" s="62">
         <f t="shared" ref="F18:F60" si="0">SUM(H18:GI18)</f>
         <v>0.75</v>
       </c>
-      <c r="G18" s="80"/>
+      <c r="G18" s="64"/>
       <c r="H18" s="26"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
@@ -3644,23 +3643,23 @@
       <c r="GH18" s="32"/>
       <c r="GI18" s="32"/>
     </row>
-    <row r="19" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="81" t="s">
+    <row r="19" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A19" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="82"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="65">
+      <c r="D19" s="62">
         <v>0.5</v>
       </c>
-      <c r="E19" s="66"/>
-      <c r="F19" s="65">
+      <c r="E19" s="63"/>
+      <c r="F19" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="80"/>
+      <c r="G19" s="64"/>
       <c r="H19" s="26"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
@@ -3846,23 +3845,23 @@
       <c r="GH19" s="32"/>
       <c r="GI19" s="36"/>
     </row>
-    <row r="20" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="81" t="s">
+    <row r="20" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A20" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="82"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="65">
+      <c r="D20" s="62">
         <v>0.3</v>
       </c>
-      <c r="E20" s="66"/>
-      <c r="F20" s="65">
+      <c r="E20" s="63"/>
+      <c r="F20" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="80"/>
+      <c r="G20" s="64"/>
       <c r="H20" s="26"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -4048,23 +4047,23 @@
       <c r="GH20" s="32"/>
       <c r="GI20" s="36"/>
     </row>
-    <row r="21" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="81" t="s">
+    <row r="21" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A21" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="82"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="65">
+      <c r="D21" s="62">
         <v>1</v>
       </c>
-      <c r="E21" s="66"/>
-      <c r="F21" s="65">
+      <c r="E21" s="63"/>
+      <c r="F21" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="80"/>
+      <c r="G21" s="64"/>
       <c r="H21" s="26"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
@@ -4250,23 +4249,23 @@
       <c r="GH21" s="32"/>
       <c r="GI21" s="36"/>
     </row>
-    <row r="22" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="81" t="s">
+    <row r="22" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A22" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="82"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="65">
+      <c r="D22" s="62">
         <v>0.6</v>
       </c>
-      <c r="E22" s="66"/>
-      <c r="F22" s="65">
+      <c r="E22" s="63"/>
+      <c r="F22" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="80"/>
+      <c r="G22" s="64"/>
       <c r="H22" s="26"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
@@ -4452,23 +4451,23 @@
       <c r="GH22" s="32"/>
       <c r="GI22" s="36"/>
     </row>
-    <row r="23" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="81" t="s">
+    <row r="23" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A23" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="82"/>
+      <c r="B23" s="67"/>
       <c r="C23" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="65">
+      <c r="D23" s="62">
         <v>0.6</v>
       </c>
-      <c r="E23" s="66"/>
-      <c r="F23" s="65">
+      <c r="E23" s="63"/>
+      <c r="F23" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="80"/>
+      <c r="G23" s="64"/>
       <c r="H23" s="26"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
@@ -4654,23 +4653,23 @@
       <c r="GH23" s="32"/>
       <c r="GI23" s="36"/>
     </row>
-    <row r="24" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="81" t="s">
+    <row r="24" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A24" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="82"/>
+      <c r="B24" s="67"/>
       <c r="C24" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="65">
+      <c r="D24" s="62">
         <v>3</v>
       </c>
-      <c r="E24" s="66"/>
-      <c r="F24" s="65">
+      <c r="E24" s="63"/>
+      <c r="F24" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="80"/>
+      <c r="G24" s="64"/>
       <c r="H24" s="26"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
@@ -4856,23 +4855,23 @@
       <c r="GH24" s="32"/>
       <c r="GI24" s="36"/>
     </row>
-    <row r="25" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="81" t="s">
+    <row r="25" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A25" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="82"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="65">
+      <c r="D25" s="62">
         <v>1.5</v>
       </c>
-      <c r="E25" s="66"/>
-      <c r="F25" s="65">
+      <c r="E25" s="63"/>
+      <c r="F25" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="80"/>
+      <c r="G25" s="64"/>
       <c r="H25" s="26"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
@@ -5058,23 +5057,23 @@
       <c r="GH25" s="32"/>
       <c r="GI25" s="36"/>
     </row>
-    <row r="26" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="81" t="s">
+    <row r="26" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A26" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="82"/>
+      <c r="B26" s="67"/>
       <c r="C26" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="65">
+      <c r="D26" s="62">
         <v>1</v>
       </c>
-      <c r="E26" s="66"/>
-      <c r="F26" s="65">
+      <c r="E26" s="63"/>
+      <c r="F26" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="80"/>
+      <c r="G26" s="64"/>
       <c r="H26" s="26"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
@@ -5260,23 +5259,23 @@
       <c r="GH26" s="32"/>
       <c r="GI26" s="36"/>
     </row>
-    <row r="27" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="81" t="s">
+    <row r="27" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A27" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="82"/>
+      <c r="B27" s="67"/>
       <c r="C27" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="65">
+      <c r="D27" s="62">
         <v>1</v>
       </c>
-      <c r="E27" s="66"/>
-      <c r="F27" s="65">
+      <c r="E27" s="63"/>
+      <c r="F27" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G27" s="80"/>
+      <c r="G27" s="64"/>
       <c r="H27" s="26"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
@@ -5462,23 +5461,23 @@
       <c r="GH27" s="32"/>
       <c r="GI27" s="36"/>
     </row>
-    <row r="28" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="81" t="s">
+    <row r="28" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A28" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="82"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="65">
+      <c r="D28" s="62">
         <v>1</v>
       </c>
-      <c r="E28" s="66"/>
-      <c r="F28" s="65">
+      <c r="E28" s="63"/>
+      <c r="F28" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G28" s="80"/>
+      <c r="G28" s="64"/>
       <c r="H28" s="26"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
@@ -5664,23 +5663,23 @@
       <c r="GH28" s="32"/>
       <c r="GI28" s="36"/>
     </row>
-    <row r="29" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" s="81" t="s">
+    <row r="29" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A29" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="82"/>
+      <c r="B29" s="67"/>
       <c r="C29" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="65">
+      <c r="D29" s="62">
         <v>1</v>
       </c>
-      <c r="E29" s="66"/>
-      <c r="F29" s="65">
+      <c r="E29" s="63"/>
+      <c r="F29" s="62">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G29" s="80"/>
+      <c r="G29" s="64"/>
       <c r="H29" s="26"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
@@ -5868,23 +5867,23 @@
       <c r="GH29" s="32"/>
       <c r="GI29" s="36"/>
     </row>
-    <row r="30" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="81" t="s">
+    <row r="30" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A30" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="82"/>
+      <c r="B30" s="67"/>
       <c r="C30" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="65">
+      <c r="D30" s="62">
         <v>1</v>
       </c>
-      <c r="E30" s="66"/>
-      <c r="F30" s="65">
+      <c r="E30" s="63"/>
+      <c r="F30" s="62">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G30" s="80"/>
+      <c r="G30" s="64"/>
       <c r="H30" s="26"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
@@ -6072,23 +6071,23 @@
       <c r="GH30" s="32"/>
       <c r="GI30" s="36"/>
     </row>
-    <row r="31" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="81" t="s">
+    <row r="31" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A31" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="82"/>
+      <c r="B31" s="67"/>
       <c r="C31" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="65">
+      <c r="D31" s="62">
         <v>4</v>
       </c>
-      <c r="E31" s="66"/>
-      <c r="F31" s="65">
+      <c r="E31" s="63"/>
+      <c r="F31" s="62">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G31" s="80"/>
+      <c r="G31" s="64"/>
       <c r="H31" s="26"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
@@ -6278,23 +6277,23 @@
       <c r="GH31" s="32"/>
       <c r="GI31" s="36"/>
     </row>
-    <row r="32" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A32" s="81" t="s">
+    <row r="32" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A32" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="82"/>
+      <c r="B32" s="67"/>
       <c r="C32" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="65">
+      <c r="D32" s="62">
         <v>0.6</v>
       </c>
-      <c r="E32" s="66"/>
-      <c r="F32" s="65">
+      <c r="E32" s="63"/>
+      <c r="F32" s="62">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G32" s="80"/>
+      <c r="G32" s="64"/>
       <c r="H32" s="26"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
@@ -6482,23 +6481,23 @@
       <c r="GH32" s="32"/>
       <c r="GI32" s="36"/>
     </row>
-    <row r="33" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A33" s="81" t="s">
+    <row r="33" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A33" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="82"/>
+      <c r="B33" s="67"/>
       <c r="C33" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="65">
+      <c r="D33" s="62">
         <v>0.5</v>
       </c>
-      <c r="E33" s="66"/>
-      <c r="F33" s="65">
+      <c r="E33" s="63"/>
+      <c r="F33" s="62">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G33" s="80"/>
+      <c r="G33" s="64"/>
       <c r="H33" s="26"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
@@ -6686,23 +6685,23 @@
       <c r="GH33" s="32"/>
       <c r="GI33" s="36"/>
     </row>
-    <row r="34" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A34" s="81" t="s">
+    <row r="34" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A34" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="82"/>
+      <c r="B34" s="67"/>
       <c r="C34" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="65">
+      <c r="D34" s="62">
         <v>0.3</v>
       </c>
-      <c r="E34" s="66"/>
-      <c r="F34" s="65">
+      <c r="E34" s="63"/>
+      <c r="F34" s="62">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G34" s="80"/>
+      <c r="G34" s="64"/>
       <c r="H34" s="26"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
@@ -6890,23 +6889,23 @@
       <c r="GH34" s="32"/>
       <c r="GI34" s="36"/>
     </row>
-    <row r="35" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="81" t="s">
+    <row r="35" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A35" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="82"/>
+      <c r="B35" s="67"/>
       <c r="C35" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="65">
+      <c r="D35" s="62">
         <v>0.3</v>
       </c>
-      <c r="E35" s="66"/>
-      <c r="F35" s="65">
+      <c r="E35" s="63"/>
+      <c r="F35" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G35" s="80"/>
+      <c r="G35" s="64"/>
       <c r="H35" s="26"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
@@ -7092,23 +7091,23 @@
       <c r="GH35" s="32"/>
       <c r="GI35" s="36"/>
     </row>
-    <row r="36" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A36" s="81" t="s">
+    <row r="36" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A36" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="82"/>
+      <c r="B36" s="67"/>
       <c r="C36" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="65">
+      <c r="D36" s="62">
         <v>1.5</v>
       </c>
-      <c r="E36" s="66"/>
-      <c r="F36" s="65">
+      <c r="E36" s="63"/>
+      <c r="F36" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G36" s="80"/>
+      <c r="G36" s="64"/>
       <c r="H36" s="26"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
@@ -7294,23 +7293,23 @@
       <c r="GH36" s="32"/>
       <c r="GI36" s="36"/>
     </row>
-    <row r="37" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A37" s="81" t="s">
+    <row r="37" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A37" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="82"/>
+      <c r="B37" s="67"/>
       <c r="C37" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="65">
+      <c r="D37" s="62">
         <v>0.5</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="65">
+      <c r="E37" s="63"/>
+      <c r="F37" s="62">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G37" s="80"/>
+      <c r="G37" s="64"/>
       <c r="H37" s="26"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
@@ -7498,23 +7497,23 @@
       <c r="GH37" s="32"/>
       <c r="GI37" s="36"/>
     </row>
-    <row r="38" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="81" t="s">
+    <row r="38" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A38" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="82"/>
+      <c r="B38" s="67"/>
       <c r="C38" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="65">
+      <c r="D38" s="62">
         <v>0.25</v>
       </c>
-      <c r="E38" s="66"/>
-      <c r="F38" s="65">
+      <c r="E38" s="63"/>
+      <c r="F38" s="62">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G38" s="80"/>
+      <c r="G38" s="64"/>
       <c r="H38" s="26"/>
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
@@ -7702,23 +7701,23 @@
       <c r="GH38" s="32"/>
       <c r="GI38" s="36"/>
     </row>
-    <row r="39" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A39" s="81" t="s">
+    <row r="39" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A39" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="82"/>
+      <c r="B39" s="67"/>
       <c r="C39" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="65">
+      <c r="D39" s="62">
         <v>0.5</v>
       </c>
-      <c r="E39" s="66"/>
-      <c r="F39" s="65">
+      <c r="E39" s="63"/>
+      <c r="F39" s="62">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="G39" s="80"/>
+      <c r="G39" s="64"/>
       <c r="H39" s="26"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
@@ -7906,23 +7905,23 @@
       <c r="GH39" s="32"/>
       <c r="GI39" s="36"/>
     </row>
-    <row r="40" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A40" s="81" t="s">
+    <row r="40" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A40" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="82"/>
+      <c r="B40" s="67"/>
       <c r="C40" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="65">
+      <c r="D40" s="62">
         <v>0.5</v>
       </c>
-      <c r="E40" s="66"/>
-      <c r="F40" s="65">
+      <c r="E40" s="63"/>
+      <c r="F40" s="62">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G40" s="80"/>
+      <c r="G40" s="64"/>
       <c r="H40" s="26"/>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
@@ -8110,23 +8109,23 @@
       <c r="GH40" s="32"/>
       <c r="GI40" s="36"/>
     </row>
-    <row r="41" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="81" t="s">
+    <row r="41" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A41" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="82"/>
+      <c r="B41" s="67"/>
       <c r="C41" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="65">
+      <c r="D41" s="62">
         <v>0.3</v>
       </c>
-      <c r="E41" s="66"/>
-      <c r="F41" s="65">
+      <c r="E41" s="63"/>
+      <c r="F41" s="62">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G41" s="80"/>
+      <c r="G41" s="64"/>
       <c r="H41" s="26"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
@@ -8314,23 +8313,23 @@
       <c r="GH41" s="32"/>
       <c r="GI41" s="36"/>
     </row>
-    <row r="42" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A42" s="81" t="s">
+    <row r="42" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A42" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="82"/>
+      <c r="B42" s="67"/>
       <c r="C42" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="65">
+      <c r="D42" s="62">
         <v>0.5</v>
       </c>
-      <c r="E42" s="66"/>
-      <c r="F42" s="65">
+      <c r="E42" s="63"/>
+      <c r="F42" s="62">
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-      <c r="G42" s="80"/>
+      <c r="G42" s="64"/>
       <c r="H42" s="26"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
@@ -8518,23 +8517,23 @@
       <c r="GH42" s="32"/>
       <c r="GI42" s="36"/>
     </row>
-    <row r="43" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A43" s="81" t="s">
+    <row r="43" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A43" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="82"/>
+      <c r="B43" s="67"/>
       <c r="C43" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D43" s="65">
+      <c r="D43" s="62">
         <v>1.3</v>
       </c>
-      <c r="E43" s="66"/>
-      <c r="F43" s="65">
+      <c r="E43" s="63"/>
+      <c r="F43" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G43" s="80"/>
+      <c r="G43" s="64"/>
       <c r="H43" s="26"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
@@ -8720,23 +8719,23 @@
       <c r="GH43" s="32"/>
       <c r="GI43" s="36"/>
     </row>
-    <row r="44" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="81" t="s">
+    <row r="44" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A44" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="82"/>
+      <c r="B44" s="67"/>
       <c r="C44" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="65">
+      <c r="D44" s="62">
         <v>1.3</v>
       </c>
-      <c r="E44" s="66"/>
-      <c r="F44" s="65">
+      <c r="E44" s="63"/>
+      <c r="F44" s="62">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G44" s="80"/>
+        <v>2</v>
+      </c>
+      <c r="G44" s="64"/>
       <c r="H44" s="26"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
@@ -8765,7 +8764,9 @@
       <c r="AG44" s="51"/>
       <c r="AH44" s="51"/>
       <c r="AI44" s="51"/>
-      <c r="AJ44" s="32"/>
+      <c r="AJ44" s="24">
+        <v>2</v>
+      </c>
       <c r="AK44" s="32"/>
       <c r="AL44" s="32"/>
       <c r="AM44" s="32"/>
@@ -8922,23 +8923,23 @@
       <c r="GH44" s="32"/>
       <c r="GI44" s="36"/>
     </row>
-    <row r="45" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="81" t="s">
+    <row r="45" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A45" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="82"/>
+      <c r="B45" s="67"/>
       <c r="C45" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="65">
+      <c r="D45" s="62">
         <v>1</v>
       </c>
-      <c r="E45" s="66"/>
-      <c r="F45" s="65">
+      <c r="E45" s="63"/>
+      <c r="F45" s="62">
         <f t="shared" si="0"/>
         <v>1.05</v>
       </c>
-      <c r="G45" s="80"/>
+      <c r="G45" s="64"/>
       <c r="H45" s="26"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
@@ -9128,23 +9129,23 @@
       <c r="GH45" s="32"/>
       <c r="GI45" s="36"/>
     </row>
-    <row r="46" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A46" s="81" t="s">
+    <row r="46" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A46" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="82"/>
+      <c r="B46" s="67"/>
       <c r="C46" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="D46" s="65">
+      <c r="D46" s="62">
         <v>1</v>
       </c>
-      <c r="E46" s="66"/>
-      <c r="F46" s="65">
+      <c r="E46" s="63"/>
+      <c r="F46" s="62">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="G46" s="80"/>
+      <c r="G46" s="64"/>
       <c r="H46" s="26"/>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
@@ -9332,23 +9333,23 @@
       <c r="GH46" s="32"/>
       <c r="GI46" s="36"/>
     </row>
-    <row r="47" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A47" s="81" t="s">
+    <row r="47" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A47" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="82"/>
+      <c r="B47" s="67"/>
       <c r="C47" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="D47" s="65">
+      <c r="D47" s="62">
         <v>1</v>
       </c>
-      <c r="E47" s="66"/>
-      <c r="F47" s="65">
+      <c r="E47" s="63"/>
+      <c r="F47" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G47" s="80"/>
+      <c r="G47" s="64"/>
       <c r="H47" s="26"/>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
@@ -9534,23 +9535,23 @@
       <c r="GH47" s="32"/>
       <c r="GI47" s="36"/>
     </row>
-    <row r="48" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A48" s="81" t="s">
+    <row r="48" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A48" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="B48" s="82"/>
+      <c r="B48" s="67"/>
       <c r="C48" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D48" s="65">
+      <c r="D48" s="62">
         <v>0.3</v>
       </c>
-      <c r="E48" s="66"/>
-      <c r="F48" s="65">
+      <c r="E48" s="63"/>
+      <c r="F48" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G48" s="80"/>
+      <c r="G48" s="64"/>
       <c r="H48" s="26"/>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
@@ -9736,23 +9737,23 @@
       <c r="GH48" s="32"/>
       <c r="GI48" s="36"/>
     </row>
-    <row r="49" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="81" t="s">
+    <row r="49" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A49" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="82"/>
+      <c r="B49" s="67"/>
       <c r="C49" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="65">
+      <c r="D49" s="62">
         <v>2</v>
       </c>
-      <c r="E49" s="66"/>
-      <c r="F49" s="65">
+      <c r="E49" s="63"/>
+      <c r="F49" s="62">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G49" s="80"/>
+        <v>3.25</v>
+      </c>
+      <c r="G49" s="64"/>
       <c r="H49" s="26"/>
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
@@ -9782,8 +9783,12 @@
       <c r="AH49" s="51"/>
       <c r="AI49" s="51"/>
       <c r="AJ49" s="32"/>
-      <c r="AK49" s="32"/>
-      <c r="AL49" s="32"/>
+      <c r="AK49" s="58">
+        <v>2</v>
+      </c>
+      <c r="AL49" s="58">
+        <v>1.25</v>
+      </c>
       <c r="AM49" s="32"/>
       <c r="AN49" s="49"/>
       <c r="AO49" s="52"/>
@@ -9938,23 +9943,23 @@
       <c r="GH49" s="32"/>
       <c r="GI49" s="36"/>
     </row>
-    <row r="50" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A50" s="81" t="s">
+    <row r="50" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A50" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="82"/>
+      <c r="B50" s="67"/>
       <c r="C50" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="D50" s="65">
+      <c r="D50" s="62">
         <v>2</v>
       </c>
-      <c r="E50" s="66"/>
-      <c r="F50" s="65">
+      <c r="E50" s="63"/>
+      <c r="F50" s="62">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G50" s="80"/>
+        <v>2.5</v>
+      </c>
+      <c r="G50" s="64"/>
       <c r="H50" s="26"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
@@ -9984,8 +9989,12 @@
       <c r="AH50" s="51"/>
       <c r="AI50" s="51"/>
       <c r="AJ50" s="32"/>
-      <c r="AK50" s="32"/>
-      <c r="AL50" s="32"/>
+      <c r="AK50" s="58">
+        <v>2</v>
+      </c>
+      <c r="AL50" s="58">
+        <v>0.5</v>
+      </c>
       <c r="AM50" s="32"/>
       <c r="AN50" s="49"/>
       <c r="AO50" s="52"/>
@@ -10140,23 +10149,23 @@
       <c r="GH50" s="32"/>
       <c r="GI50" s="36"/>
     </row>
-    <row r="51" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="81" t="s">
+    <row r="51" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A51" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="82"/>
+      <c r="B51" s="67"/>
       <c r="C51" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D51" s="65">
+      <c r="D51" s="62">
         <v>2</v>
       </c>
-      <c r="E51" s="66"/>
-      <c r="F51" s="65">
+      <c r="E51" s="63"/>
+      <c r="F51" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G51" s="80"/>
+      <c r="G51" s="64"/>
       <c r="H51" s="26"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
@@ -10342,23 +10351,23 @@
       <c r="GH51" s="32"/>
       <c r="GI51" s="36"/>
     </row>
-    <row r="52" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A52" s="81" t="s">
+    <row r="52" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A52" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="82"/>
+      <c r="B52" s="67"/>
       <c r="C52" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="65">
+      <c r="D52" s="62">
         <v>2</v>
       </c>
-      <c r="E52" s="66"/>
-      <c r="F52" s="65">
+      <c r="E52" s="63"/>
+      <c r="F52" s="62">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G52" s="80"/>
+      <c r="G52" s="64"/>
       <c r="H52" s="26"/>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
@@ -10548,23 +10557,23 @@
       <c r="GH52" s="32"/>
       <c r="GI52" s="36"/>
     </row>
-    <row r="53" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="81" t="s">
+    <row r="53" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A53" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="82"/>
+      <c r="B53" s="67"/>
       <c r="C53" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D53" s="65">
+      <c r="D53" s="62">
         <v>2</v>
       </c>
-      <c r="E53" s="66"/>
-      <c r="F53" s="65">
+      <c r="E53" s="63"/>
+      <c r="F53" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G53" s="80"/>
+      <c r="G53" s="64"/>
       <c r="H53" s="26"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
@@ -10750,23 +10759,23 @@
       <c r="GH53" s="32"/>
       <c r="GI53" s="36"/>
     </row>
-    <row r="54" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A54" s="81" t="s">
+    <row r="54" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A54" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="82"/>
+      <c r="B54" s="67"/>
       <c r="C54" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="D54" s="65">
+      <c r="D54" s="62">
         <v>0.25</v>
       </c>
-      <c r="E54" s="66"/>
-      <c r="F54" s="65">
+      <c r="E54" s="63"/>
+      <c r="F54" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G54" s="80"/>
+      <c r="G54" s="64"/>
       <c r="H54" s="26"/>
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
@@ -10952,23 +10961,23 @@
       <c r="GH54" s="32"/>
       <c r="GI54" s="36"/>
     </row>
-    <row r="55" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A55" s="81" t="s">
+    <row r="55" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A55" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="82"/>
+      <c r="B55" s="67"/>
       <c r="C55" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="D55" s="65">
+      <c r="D55" s="62">
         <v>1</v>
       </c>
-      <c r="E55" s="66"/>
-      <c r="F55" s="65">
+      <c r="E55" s="63"/>
+      <c r="F55" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G55" s="80"/>
+      <c r="G55" s="64"/>
       <c r="H55" s="26"/>
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
@@ -11154,23 +11163,23 @@
       <c r="GH55" s="32"/>
       <c r="GI55" s="36"/>
     </row>
-    <row r="56" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="81" t="s">
+    <row r="56" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A56" s="66" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="82"/>
+      <c r="B56" s="67"/>
       <c r="C56" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="D56" s="65">
+      <c r="D56" s="62">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E56" s="66"/>
-      <c r="F56" s="65">
+      <c r="E56" s="63"/>
+      <c r="F56" s="62">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G56" s="80"/>
+      <c r="G56" s="64"/>
       <c r="H56" s="26"/>
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
@@ -11360,23 +11369,23 @@
       <c r="GH56" s="32"/>
       <c r="GI56" s="36"/>
     </row>
-    <row r="57" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A57" s="81" t="s">
+    <row r="57" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A57" s="66" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="82"/>
+      <c r="B57" s="67"/>
       <c r="C57" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="D57" s="65">
+      <c r="D57" s="62">
         <v>1.75</v>
       </c>
-      <c r="E57" s="66"/>
-      <c r="F57" s="65">
+      <c r="E57" s="63"/>
+      <c r="F57" s="62">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G57" s="80"/>
+      <c r="G57" s="64"/>
       <c r="H57" s="26"/>
       <c r="I57" s="12"/>
       <c r="J57" s="12"/>
@@ -11564,23 +11573,23 @@
       <c r="GH57" s="32"/>
       <c r="GI57" s="36"/>
     </row>
-    <row r="58" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A58" s="81" t="s">
+    <row r="58" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A58" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="B58" s="82"/>
+      <c r="B58" s="67"/>
       <c r="C58" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="D58" s="65">
+      <c r="D58" s="62">
         <v>0.6</v>
       </c>
-      <c r="E58" s="66"/>
-      <c r="F58" s="65">
+      <c r="E58" s="63"/>
+      <c r="F58" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G58" s="80"/>
+      <c r="G58" s="64"/>
       <c r="H58" s="26"/>
       <c r="I58" s="12"/>
       <c r="J58" s="12"/>
@@ -11766,23 +11775,23 @@
       <c r="GH58" s="32"/>
       <c r="GI58" s="36"/>
     </row>
-    <row r="59" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A59" s="81" t="s">
+    <row r="59" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A59" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="B59" s="82"/>
+      <c r="B59" s="67"/>
       <c r="C59" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="65">
+      <c r="D59" s="62">
         <v>1</v>
       </c>
-      <c r="E59" s="66"/>
-      <c r="F59" s="65">
+      <c r="E59" s="63"/>
+      <c r="F59" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G59" s="80"/>
+      <c r="G59" s="64"/>
       <c r="H59" s="26"/>
       <c r="I59" s="12"/>
       <c r="J59" s="12"/>
@@ -11968,23 +11977,23 @@
       <c r="GH59" s="32"/>
       <c r="GI59" s="36"/>
     </row>
-    <row r="60" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A60" s="81" t="s">
+    <row r="60" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A60" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="B60" s="82"/>
+      <c r="B60" s="67"/>
       <c r="C60" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="D60" s="65">
+      <c r="D60" s="62">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E60" s="66"/>
-      <c r="F60" s="65">
+      <c r="E60" s="63"/>
+      <c r="F60" s="62">
         <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
-      <c r="G60" s="80"/>
+      <c r="G60" s="64"/>
       <c r="H60" s="26"/>
       <c r="I60" s="12"/>
       <c r="J60" s="12"/>
@@ -12172,23 +12181,23 @@
       <c r="GH60" s="32"/>
       <c r="GI60" s="36"/>
     </row>
-    <row r="61" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A61" s="81" t="s">
+    <row r="61" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A61" s="66" t="s">
         <v>115</v>
       </c>
-      <c r="B61" s="82"/>
+      <c r="B61" s="67"/>
       <c r="C61" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="D61" s="65">
+      <c r="D61" s="62">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E61" s="66"/>
-      <c r="F61" s="65">
+      <c r="E61" s="63"/>
+      <c r="F61" s="62">
         <f>SUM(H61:GI61)</f>
         <v>1</v>
       </c>
-      <c r="G61" s="80"/>
+      <c r="G61" s="64"/>
       <c r="H61" s="26"/>
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
@@ -12376,22 +12385,22 @@
       <c r="GH61" s="32"/>
       <c r="GI61" s="36"/>
     </row>
-    <row r="62" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A62" s="115" t="s">
+    <row r="62" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A62" s="76" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="116"/>
+      <c r="B62" s="77"/>
       <c r="C62" s="39"/>
-      <c r="D62" s="71">
+      <c r="D62" s="78">
         <f>SUM(D63:E80)</f>
         <v>88.6</v>
       </c>
-      <c r="E62" s="117"/>
-      <c r="F62" s="71">
+      <c r="E62" s="79"/>
+      <c r="F62" s="78">
         <f>SUM(F63:G80)</f>
         <v>0</v>
       </c>
-      <c r="G62" s="75"/>
+      <c r="G62" s="80"/>
       <c r="H62" s="29"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
@@ -12577,23 +12586,23 @@
       <c r="GH62" s="8"/>
       <c r="GI62" s="29"/>
     </row>
-    <row r="63" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A63" s="118" t="s">
+    <row r="63" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A63" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="119"/>
+      <c r="B63" s="61"/>
       <c r="C63" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D63" s="65">
+      <c r="D63" s="62">
         <v>0.6</v>
       </c>
-      <c r="E63" s="66"/>
-      <c r="F63" s="65">
+      <c r="E63" s="63"/>
+      <c r="F63" s="62">
         <f>SUM(H63:GI63)</f>
         <v>0</v>
       </c>
-      <c r="G63" s="80"/>
+      <c r="G63" s="64"/>
       <c r="H63" s="47"/>
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
@@ -12779,23 +12788,23 @@
       <c r="GH63" s="32"/>
       <c r="GI63" s="32"/>
     </row>
-    <row r="64" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A64" s="118" t="s">
+    <row r="64" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A64" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="B64" s="119"/>
+      <c r="B64" s="61"/>
       <c r="C64" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D64" s="65">
+      <c r="D64" s="62">
         <v>1.5</v>
       </c>
-      <c r="E64" s="66"/>
-      <c r="F64" s="65">
+      <c r="E64" s="63"/>
+      <c r="F64" s="62">
         <f>SUM(H64:GI64)</f>
         <v>0</v>
       </c>
-      <c r="G64" s="80"/>
+      <c r="G64" s="64"/>
       <c r="H64" s="47"/>
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
@@ -12981,23 +12990,23 @@
       <c r="GH64" s="32"/>
       <c r="GI64" s="32"/>
     </row>
-    <row r="65" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A65" s="118" t="s">
+    <row r="65" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A65" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="B65" s="119"/>
+      <c r="B65" s="61"/>
       <c r="C65" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D65" s="65">
+      <c r="D65" s="62">
         <v>1</v>
       </c>
-      <c r="E65" s="66"/>
-      <c r="F65" s="65">
+      <c r="E65" s="63"/>
+      <c r="F65" s="62">
         <f t="shared" ref="F65:F80" si="1">SUM(H65:GI65)</f>
         <v>0</v>
       </c>
-      <c r="G65" s="80"/>
+      <c r="G65" s="64"/>
       <c r="H65" s="47"/>
       <c r="I65" s="12"/>
       <c r="J65" s="12"/>
@@ -13183,23 +13192,23 @@
       <c r="GH65" s="32"/>
       <c r="GI65" s="32"/>
     </row>
-    <row r="66" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A66" s="118" t="s">
+    <row r="66" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A66" s="60" t="s">
         <v>125</v>
       </c>
-      <c r="B66" s="119"/>
+      <c r="B66" s="61"/>
       <c r="C66" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D66" s="65">
+      <c r="D66" s="62">
         <v>0.5</v>
       </c>
-      <c r="E66" s="66"/>
-      <c r="F66" s="65">
+      <c r="E66" s="63"/>
+      <c r="F66" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G66" s="80"/>
+      <c r="G66" s="64"/>
       <c r="H66" s="47"/>
       <c r="I66" s="12"/>
       <c r="J66" s="12"/>
@@ -13385,23 +13394,23 @@
       <c r="GH66" s="32"/>
       <c r="GI66" s="32"/>
     </row>
-    <row r="67" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A67" s="118" t="s">
+    <row r="67" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A67" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="119"/>
+      <c r="B67" s="61"/>
       <c r="C67" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D67" s="65">
+      <c r="D67" s="62">
         <v>1</v>
       </c>
-      <c r="E67" s="66"/>
-      <c r="F67" s="65">
+      <c r="E67" s="63"/>
+      <c r="F67" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G67" s="80"/>
+      <c r="G67" s="64"/>
       <c r="H67" s="47"/>
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
@@ -13587,23 +13596,23 @@
       <c r="GH67" s="32"/>
       <c r="GI67" s="32"/>
     </row>
-    <row r="68" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A68" s="118" t="s">
+    <row r="68" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A68" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="B68" s="119"/>
+      <c r="B68" s="61"/>
       <c r="C68" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D68" s="65">
+      <c r="D68" s="62">
         <v>1</v>
       </c>
-      <c r="E68" s="66"/>
-      <c r="F68" s="65">
+      <c r="E68" s="63"/>
+      <c r="F68" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G68" s="80"/>
+      <c r="G68" s="64"/>
       <c r="H68" s="47"/>
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
@@ -13789,23 +13798,23 @@
       <c r="GH68" s="32"/>
       <c r="GI68" s="32"/>
     </row>
-    <row r="69" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A69" s="118" t="s">
+    <row r="69" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A69" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="B69" s="119"/>
+      <c r="B69" s="61"/>
       <c r="C69" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="D69" s="65">
+      <c r="D69" s="62">
         <v>4</v>
       </c>
-      <c r="E69" s="66"/>
-      <c r="F69" s="65">
+      <c r="E69" s="63"/>
+      <c r="F69" s="62">
         <f>SUM(H69:GI69)</f>
         <v>0</v>
       </c>
-      <c r="G69" s="80"/>
+      <c r="G69" s="64"/>
       <c r="H69" s="47"/>
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
@@ -13991,23 +14000,23 @@
       <c r="GH69" s="32"/>
       <c r="GI69" s="32"/>
     </row>
-    <row r="70" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A70" s="118" t="s">
+    <row r="70" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A70" s="60" t="s">
         <v>133</v>
       </c>
-      <c r="B70" s="119"/>
+      <c r="B70" s="61"/>
       <c r="C70" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="D70" s="65">
+      <c r="D70" s="62">
         <v>8</v>
       </c>
-      <c r="E70" s="66"/>
-      <c r="F70" s="65">
+      <c r="E70" s="63"/>
+      <c r="F70" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G70" s="80"/>
+      <c r="G70" s="64"/>
       <c r="H70" s="47"/>
       <c r="I70" s="12"/>
       <c r="J70" s="12"/>
@@ -14193,23 +14202,23 @@
       <c r="GH70" s="32"/>
       <c r="GI70" s="32"/>
     </row>
-    <row r="71" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A71" s="118" t="s">
+    <row r="71" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A71" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="B71" s="119"/>
+      <c r="B71" s="61"/>
       <c r="C71" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="D71" s="65">
+      <c r="D71" s="62">
         <v>1</v>
       </c>
-      <c r="E71" s="66"/>
-      <c r="F71" s="65">
+      <c r="E71" s="63"/>
+      <c r="F71" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G71" s="80"/>
+      <c r="G71" s="64"/>
       <c r="H71" s="47"/>
       <c r="I71" s="12"/>
       <c r="J71" s="12"/>
@@ -14395,23 +14404,23 @@
       <c r="GH71" s="32"/>
       <c r="GI71" s="32"/>
     </row>
-    <row r="72" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A72" s="118" t="s">
+    <row r="72" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A72" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="B72" s="119"/>
+      <c r="B72" s="61"/>
       <c r="C72" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="D72" s="65">
+      <c r="D72" s="62">
         <v>1</v>
       </c>
-      <c r="E72" s="66"/>
-      <c r="F72" s="65">
+      <c r="E72" s="63"/>
+      <c r="F72" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G72" s="80"/>
+      <c r="G72" s="64"/>
       <c r="H72" s="47"/>
       <c r="I72" s="12"/>
       <c r="J72" s="12"/>
@@ -14597,23 +14606,23 @@
       <c r="GH72" s="32"/>
       <c r="GI72" s="32"/>
     </row>
-    <row r="73" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A73" s="118" t="s">
+    <row r="73" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A73" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="B73" s="119"/>
+      <c r="B73" s="61"/>
       <c r="C73" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="D73" s="65">
+      <c r="D73" s="62">
         <v>4</v>
       </c>
-      <c r="E73" s="66"/>
-      <c r="F73" s="65">
+      <c r="E73" s="63"/>
+      <c r="F73" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G73" s="80"/>
+      <c r="G73" s="64"/>
       <c r="H73" s="47"/>
       <c r="I73" s="12"/>
       <c r="J73" s="12"/>
@@ -14799,23 +14808,23 @@
       <c r="GH73" s="32"/>
       <c r="GI73" s="32"/>
     </row>
-    <row r="74" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A74" s="118" t="s">
+    <row r="74" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A74" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="B74" s="119"/>
+      <c r="B74" s="61"/>
       <c r="C74" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="D74" s="65">
+      <c r="D74" s="62">
         <v>12</v>
       </c>
-      <c r="E74" s="66"/>
-      <c r="F74" s="65">
+      <c r="E74" s="63"/>
+      <c r="F74" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G74" s="80"/>
+      <c r="G74" s="64"/>
       <c r="H74" s="47"/>
       <c r="I74" s="12"/>
       <c r="J74" s="12"/>
@@ -15001,23 +15010,23 @@
       <c r="GH74" s="32"/>
       <c r="GI74" s="32"/>
     </row>
-    <row r="75" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A75" s="118" t="s">
+    <row r="75" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A75" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="B75" s="88"/>
+      <c r="B75" s="65"/>
       <c r="C75" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D75" s="65">
+      <c r="D75" s="62">
         <v>16</v>
       </c>
-      <c r="E75" s="66"/>
-      <c r="F75" s="65">
+      <c r="E75" s="63"/>
+      <c r="F75" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G75" s="80"/>
+      <c r="G75" s="64"/>
       <c r="H75" s="47"/>
       <c r="I75" s="12"/>
       <c r="J75" s="12"/>
@@ -15203,23 +15212,23 @@
       <c r="GH75" s="32"/>
       <c r="GI75" s="36"/>
     </row>
-    <row r="76" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A76" s="118" t="s">
+    <row r="76" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A76" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="B76" s="119"/>
+      <c r="B76" s="61"/>
       <c r="C76" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="D76" s="65">
+      <c r="D76" s="62">
         <v>5</v>
       </c>
-      <c r="E76" s="66"/>
-      <c r="F76" s="65">
+      <c r="E76" s="63"/>
+      <c r="F76" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G76" s="80"/>
+      <c r="G76" s="64"/>
       <c r="H76" s="47"/>
       <c r="I76" s="12"/>
       <c r="J76" s="12"/>
@@ -15405,23 +15414,23 @@
       <c r="GH76" s="32"/>
       <c r="GI76" s="32"/>
     </row>
-    <row r="77" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A77" s="118" t="s">
+    <row r="77" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A77" s="60" t="s">
         <v>146</v>
       </c>
-      <c r="B77" s="119"/>
+      <c r="B77" s="61"/>
       <c r="C77" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="D77" s="65">
+      <c r="D77" s="62">
         <v>4</v>
       </c>
-      <c r="E77" s="66"/>
-      <c r="F77" s="65">
+      <c r="E77" s="63"/>
+      <c r="F77" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G77" s="80"/>
+      <c r="G77" s="64"/>
       <c r="H77" s="47"/>
       <c r="I77" s="12"/>
       <c r="J77" s="12"/>
@@ -15607,23 +15616,23 @@
       <c r="GH77" s="32"/>
       <c r="GI77" s="32"/>
     </row>
-    <row r="78" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A78" s="118" t="s">
+    <row r="78" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A78" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="B78" s="119"/>
+      <c r="B78" s="61"/>
       <c r="C78" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="D78" s="65">
+      <c r="D78" s="62">
         <v>16</v>
       </c>
-      <c r="E78" s="66"/>
-      <c r="F78" s="65">
+      <c r="E78" s="63"/>
+      <c r="F78" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G78" s="80"/>
+      <c r="G78" s="64"/>
       <c r="H78" s="47"/>
       <c r="I78" s="12"/>
       <c r="J78" s="12"/>
@@ -15809,23 +15818,23 @@
       <c r="GH78" s="32"/>
       <c r="GI78" s="32"/>
     </row>
-    <row r="79" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A79" s="73" t="s">
+    <row r="79" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A79" s="82" t="s">
         <v>150</v>
       </c>
-      <c r="B79" s="74"/>
+      <c r="B79" s="83"/>
       <c r="C79" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="D79" s="65">
+      <c r="D79" s="62">
         <v>6</v>
       </c>
-      <c r="E79" s="66"/>
-      <c r="F79" s="65">
+      <c r="E79" s="63"/>
+      <c r="F79" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G79" s="80"/>
+      <c r="G79" s="64"/>
       <c r="H79" s="47"/>
       <c r="I79" s="12"/>
       <c r="J79" s="12"/>
@@ -16011,23 +16020,23 @@
       <c r="GH79" s="32"/>
       <c r="GI79" s="36"/>
     </row>
-    <row r="80" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A80" s="73" t="s">
+    <row r="80" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A80" s="82" t="s">
         <v>152</v>
       </c>
-      <c r="B80" s="74"/>
+      <c r="B80" s="83"/>
       <c r="C80" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D80" s="65">
+      <c r="D80" s="62">
         <v>6</v>
       </c>
-      <c r="E80" s="66"/>
-      <c r="F80" s="65">
+      <c r="E80" s="63"/>
+      <c r="F80" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G80" s="80"/>
+      <c r="G80" s="64"/>
       <c r="H80" s="47"/>
       <c r="I80" s="12"/>
       <c r="J80" s="12"/>
@@ -16213,22 +16222,22 @@
       <c r="GH80" s="32"/>
       <c r="GI80" s="36"/>
     </row>
-    <row r="81" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A81" s="115" t="s">
+    <row r="81" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A81" s="76" t="s">
         <v>153</v>
       </c>
-      <c r="B81" s="116"/>
+      <c r="B81" s="77"/>
       <c r="C81" s="39"/>
-      <c r="D81" s="71">
+      <c r="D81" s="78">
         <f>SUM(D82:E82)</f>
         <v>16</v>
       </c>
-      <c r="E81" s="72"/>
-      <c r="F81" s="71">
+      <c r="E81" s="88"/>
+      <c r="F81" s="78">
         <f>SUM(F82:G82)</f>
         <v>0</v>
       </c>
-      <c r="G81" s="75"/>
+      <c r="G81" s="80"/>
       <c r="H81" s="29"/>
       <c r="I81" s="8"/>
       <c r="J81" s="8"/>
@@ -16414,21 +16423,21 @@
       <c r="GH81" s="8"/>
       <c r="GI81" s="29"/>
     </row>
-    <row r="82" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A82" s="93" t="s">
+    <row r="82" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A82" s="86" t="s">
         <v>153</v>
       </c>
-      <c r="B82" s="94"/>
+      <c r="B82" s="87"/>
       <c r="C82" s="40"/>
-      <c r="D82" s="91">
+      <c r="D82" s="84">
         <v>16</v>
       </c>
-      <c r="E82" s="92"/>
-      <c r="F82" s="65">
+      <c r="E82" s="85"/>
+      <c r="F82" s="62">
         <f>SUM(H82:GI82)</f>
         <v>0</v>
       </c>
-      <c r="G82" s="80"/>
+      <c r="G82" s="64"/>
       <c r="H82" s="26"/>
       <c r="I82" s="12"/>
       <c r="J82" s="12"/>
@@ -16614,22 +16623,22 @@
       <c r="GH82" s="32"/>
       <c r="GI82" s="32"/>
     </row>
-    <row r="83" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A83" s="110" t="s">
+    <row r="83" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A83" s="104" t="s">
         <v>154</v>
       </c>
-      <c r="B83" s="111"/>
+      <c r="B83" s="105"/>
       <c r="C83" s="41"/>
-      <c r="D83" s="71">
+      <c r="D83" s="78">
         <f>SUM(D84:E84)</f>
         <v>32</v>
       </c>
-      <c r="E83" s="72"/>
-      <c r="F83" s="71">
+      <c r="E83" s="88"/>
+      <c r="F83" s="78">
         <f>SUM(F84:G84)</f>
         <v>0</v>
       </c>
-      <c r="G83" s="75"/>
+      <c r="G83" s="80"/>
       <c r="H83" s="29"/>
       <c r="I83" s="8"/>
       <c r="J83" s="8"/>
@@ -16815,21 +16824,21 @@
       <c r="GH83" s="8"/>
       <c r="GI83" s="29"/>
     </row>
-    <row r="84" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A84" s="85" t="s">
+    <row r="84" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A84" s="108" t="s">
         <v>154</v>
       </c>
-      <c r="B84" s="86"/>
+      <c r="B84" s="109"/>
       <c r="C84" s="42"/>
-      <c r="D84" s="65">
+      <c r="D84" s="62">
         <v>32</v>
       </c>
-      <c r="E84" s="66"/>
-      <c r="F84" s="65">
+      <c r="E84" s="63"/>
+      <c r="F84" s="62">
         <f>SUM(H84:GI84)</f>
         <v>0</v>
       </c>
-      <c r="G84" s="80"/>
+      <c r="G84" s="64"/>
       <c r="H84" s="26"/>
       <c r="I84" s="12"/>
       <c r="J84" s="12"/>
@@ -17015,22 +17024,22 @@
       <c r="GH84" s="32"/>
       <c r="GI84" s="32"/>
     </row>
-    <row r="85" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A85" s="89" t="s">
+    <row r="85" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A85" s="111" t="s">
         <v>155</v>
       </c>
-      <c r="B85" s="90"/>
+      <c r="B85" s="112"/>
       <c r="C85" s="43"/>
-      <c r="D85" s="71">
+      <c r="D85" s="78">
         <f>SUM(D86:E86)</f>
         <v>8</v>
       </c>
-      <c r="E85" s="72"/>
-      <c r="F85" s="95">
+      <c r="E85" s="88"/>
+      <c r="F85" s="89">
         <f>SUM(F86:G86)</f>
         <v>0</v>
       </c>
-      <c r="G85" s="96"/>
+      <c r="G85" s="90"/>
       <c r="H85" s="29"/>
       <c r="I85" s="8"/>
       <c r="J85" s="8"/>
@@ -17216,21 +17225,21 @@
       <c r="GH85" s="8"/>
       <c r="GI85" s="29"/>
     </row>
-    <row r="86" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A86" s="87" t="s">
+    <row r="86" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A86" s="110" t="s">
         <v>156</v>
       </c>
-      <c r="B86" s="88"/>
+      <c r="B86" s="65"/>
       <c r="C86" s="27"/>
-      <c r="D86" s="65">
+      <c r="D86" s="62">
         <v>8</v>
       </c>
-      <c r="E86" s="66"/>
-      <c r="F86" s="65">
+      <c r="E86" s="63"/>
+      <c r="F86" s="62">
         <f>SUM(H86:GI86)</f>
         <v>0</v>
       </c>
-      <c r="G86" s="80"/>
+      <c r="G86" s="64"/>
       <c r="H86" s="26"/>
       <c r="I86" s="12"/>
       <c r="J86" s="12"/>
@@ -17416,21 +17425,21 @@
       <c r="GH86" s="32"/>
       <c r="GI86" s="32"/>
     </row>
-    <row r="87" spans="1:191" ht="18" x14ac:dyDescent="0.25">
-      <c r="A87" s="83" t="s">
+    <row r="87" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A87" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="84"/>
+      <c r="B87" s="107"/>
       <c r="C87" s="43"/>
-      <c r="D87" s="71">
+      <c r="D87" s="78">
         <f>232-D90</f>
         <v>36.349999999999994</v>
       </c>
-      <c r="E87" s="72"/>
-      <c r="F87" s="71">
+      <c r="E87" s="88"/>
+      <c r="F87" s="78">
         <v>0</v>
       </c>
-      <c r="G87" s="75"/>
+      <c r="G87" s="80"/>
       <c r="H87" s="29"/>
       <c r="I87" s="8"/>
       <c r="J87" s="8"/>
@@ -17616,16 +17625,16 @@
       <c r="GH87" s="8"/>
       <c r="GI87" s="29"/>
     </row>
-    <row r="88" spans="1:191" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="107" t="s">
+    <row r="88" spans="1:191" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="B88" s="108"/>
+      <c r="B88" s="102"/>
       <c r="C88" s="44"/>
-      <c r="D88" s="104"/>
-      <c r="E88" s="105"/>
-      <c r="F88" s="104"/>
-      <c r="G88" s="106"/>
+      <c r="D88" s="98"/>
+      <c r="E88" s="99"/>
+      <c r="F88" s="98"/>
+      <c r="G88" s="100"/>
       <c r="H88" s="28"/>
       <c r="I88" s="17"/>
       <c r="J88" s="17"/>
@@ -17811,7 +17820,7 @@
       <c r="GH88" s="17"/>
       <c r="GI88" s="17"/>
     </row>
-    <row r="89" spans="1:191" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:191" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -17863,22 +17872,22 @@
       <c r="AW89" s="3"/>
       <c r="AX89" s="3"/>
     </row>
-    <row r="90" spans="1:191" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="102" t="s">
+    <row r="90" spans="1:191" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="103"/>
+      <c r="B90" s="97"/>
       <c r="C90" s="45"/>
-      <c r="D90" s="100">
+      <c r="D90" s="94">
         <f>SUM(D85,D83,D81,D62,D14)</f>
         <v>195.65</v>
       </c>
-      <c r="E90" s="101"/>
-      <c r="F90" s="100">
+      <c r="E90" s="95"/>
+      <c r="F90" s="94">
         <f>SUM(F85,F83,F81,F62,F14)</f>
-        <v>22.900000000000002</v>
-      </c>
-      <c r="G90" s="109"/>
+        <v>30.650000000000002</v>
+      </c>
+      <c r="G90" s="103"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
@@ -17925,132 +17934,190 @@
     </row>
   </sheetData>
   <mergeCells count="334">
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="BR13:BS13"/>
+    <mergeCell ref="BL13:BM13"/>
+    <mergeCell ref="BN13:BO13"/>
+    <mergeCell ref="BR12:DY12"/>
+    <mergeCell ref="DZ13:EA13"/>
+    <mergeCell ref="CL13:CM13"/>
+    <mergeCell ref="CN13:CO13"/>
+    <mergeCell ref="BT13:BU13"/>
+    <mergeCell ref="BV13:BW13"/>
+    <mergeCell ref="BX13:BY13"/>
+    <mergeCell ref="BZ13:CA13"/>
+    <mergeCell ref="CB13:CC13"/>
+    <mergeCell ref="CD13:CE13"/>
+    <mergeCell ref="CF13:CG13"/>
+    <mergeCell ref="CH13:CI13"/>
+    <mergeCell ref="CJ13:CK13"/>
+    <mergeCell ref="CP13:CQ13"/>
+    <mergeCell ref="CR13:CS13"/>
+    <mergeCell ref="CT13:CU13"/>
+    <mergeCell ref="CV13:CW13"/>
+    <mergeCell ref="CX13:CY13"/>
+    <mergeCell ref="CZ13:DA13"/>
+    <mergeCell ref="DB13:DC13"/>
+    <mergeCell ref="DD13:DE13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="P6:X6"/>
+    <mergeCell ref="P5:X5"/>
+    <mergeCell ref="P4:X4"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="H12:BQ12"/>
+    <mergeCell ref="BB13:BC13"/>
+    <mergeCell ref="BD13:BE13"/>
+    <mergeCell ref="BF13:BG13"/>
+    <mergeCell ref="BP13:BQ13"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="AF13:AG13"/>
+    <mergeCell ref="AH13:AI13"/>
+    <mergeCell ref="AJ13:AK13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="AL13:AM13"/>
+    <mergeCell ref="AN13:AO13"/>
+    <mergeCell ref="AP13:AQ13"/>
+    <mergeCell ref="AR13:AS13"/>
+    <mergeCell ref="AT13:AU13"/>
+    <mergeCell ref="AV13:AW13"/>
+    <mergeCell ref="AX13:AY13"/>
+    <mergeCell ref="AZ13:BA13"/>
+    <mergeCell ref="BH13:BI13"/>
+    <mergeCell ref="BJ13:BK13"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="P9:X9"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F11:G13"/>
+    <mergeCell ref="D11:E13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="DF13:DG13"/>
+    <mergeCell ref="DH13:DI13"/>
+    <mergeCell ref="DJ13:DK13"/>
+    <mergeCell ref="DL13:DM13"/>
+    <mergeCell ref="DN13:DO13"/>
+    <mergeCell ref="DP13:DQ13"/>
+    <mergeCell ref="DR13:DS13"/>
+    <mergeCell ref="DT13:DU13"/>
+    <mergeCell ref="DV13:DW13"/>
+    <mergeCell ref="FF13:FG13"/>
+    <mergeCell ref="DX13:DY13"/>
+    <mergeCell ref="FH13:FI13"/>
+    <mergeCell ref="FJ13:FK13"/>
+    <mergeCell ref="EB13:EC13"/>
+    <mergeCell ref="ED13:EE13"/>
+    <mergeCell ref="EF13:EG13"/>
+    <mergeCell ref="EH13:EI13"/>
+    <mergeCell ref="EJ13:EK13"/>
+    <mergeCell ref="EL13:EM13"/>
+    <mergeCell ref="EN13:EO13"/>
+    <mergeCell ref="EP13:EQ13"/>
+    <mergeCell ref="ER13:ES13"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="GD13:GE13"/>
+    <mergeCell ref="GF13:GG13"/>
+    <mergeCell ref="GH13:GI13"/>
+    <mergeCell ref="DZ12:GI12"/>
+    <mergeCell ref="FL13:FM13"/>
+    <mergeCell ref="FN13:FO13"/>
+    <mergeCell ref="FP13:FQ13"/>
+    <mergeCell ref="FR13:FS13"/>
+    <mergeCell ref="FT13:FU13"/>
+    <mergeCell ref="FV13:FW13"/>
+    <mergeCell ref="FX13:FY13"/>
+    <mergeCell ref="FZ13:GA13"/>
+    <mergeCell ref="GB13:GC13"/>
+    <mergeCell ref="ET13:EU13"/>
+    <mergeCell ref="EV13:EW13"/>
+    <mergeCell ref="EX13:EY13"/>
+    <mergeCell ref="EZ13:FA13"/>
+    <mergeCell ref="FB13:FC13"/>
+    <mergeCell ref="FD13:FE13"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="D32:E32"/>
@@ -18075,190 +18142,132 @@
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="GD13:GE13"/>
-    <mergeCell ref="GF13:GG13"/>
-    <mergeCell ref="GH13:GI13"/>
-    <mergeCell ref="DZ12:GI12"/>
-    <mergeCell ref="FL13:FM13"/>
-    <mergeCell ref="FN13:FO13"/>
-    <mergeCell ref="FP13:FQ13"/>
-    <mergeCell ref="FR13:FS13"/>
-    <mergeCell ref="FT13:FU13"/>
-    <mergeCell ref="FV13:FW13"/>
-    <mergeCell ref="FX13:FY13"/>
-    <mergeCell ref="FZ13:GA13"/>
-    <mergeCell ref="GB13:GC13"/>
-    <mergeCell ref="ET13:EU13"/>
-    <mergeCell ref="EV13:EW13"/>
-    <mergeCell ref="EX13:EY13"/>
-    <mergeCell ref="EZ13:FA13"/>
-    <mergeCell ref="FB13:FC13"/>
-    <mergeCell ref="FD13:FE13"/>
-    <mergeCell ref="FF13:FG13"/>
-    <mergeCell ref="DX13:DY13"/>
-    <mergeCell ref="FH13:FI13"/>
-    <mergeCell ref="FJ13:FK13"/>
-    <mergeCell ref="EB13:EC13"/>
-    <mergeCell ref="ED13:EE13"/>
-    <mergeCell ref="EF13:EG13"/>
-    <mergeCell ref="EH13:EI13"/>
-    <mergeCell ref="EJ13:EK13"/>
-    <mergeCell ref="EL13:EM13"/>
-    <mergeCell ref="EN13:EO13"/>
-    <mergeCell ref="EP13:EQ13"/>
-    <mergeCell ref="ER13:ES13"/>
-    <mergeCell ref="DF13:DG13"/>
-    <mergeCell ref="DH13:DI13"/>
-    <mergeCell ref="DJ13:DK13"/>
-    <mergeCell ref="DL13:DM13"/>
-    <mergeCell ref="DN13:DO13"/>
-    <mergeCell ref="DP13:DQ13"/>
-    <mergeCell ref="DR13:DS13"/>
-    <mergeCell ref="DT13:DU13"/>
-    <mergeCell ref="DV13:DW13"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="F90:G90"/>
-    <mergeCell ref="F87:G87"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="BH13:BI13"/>
-    <mergeCell ref="BJ13:BK13"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="P9:X9"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F11:G13"/>
-    <mergeCell ref="D11:E13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="AL13:AM13"/>
-    <mergeCell ref="AN13:AO13"/>
-    <mergeCell ref="AP13:AQ13"/>
-    <mergeCell ref="AR13:AS13"/>
-    <mergeCell ref="AT13:AU13"/>
-    <mergeCell ref="AV13:AW13"/>
-    <mergeCell ref="AX13:AY13"/>
-    <mergeCell ref="AZ13:BA13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="P6:X6"/>
-    <mergeCell ref="P5:X5"/>
-    <mergeCell ref="P4:X4"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="H12:BQ12"/>
-    <mergeCell ref="BB13:BC13"/>
-    <mergeCell ref="BD13:BE13"/>
-    <mergeCell ref="BF13:BG13"/>
-    <mergeCell ref="BP13:BQ13"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="AF13:AG13"/>
-    <mergeCell ref="AH13:AI13"/>
-    <mergeCell ref="AJ13:AK13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="BR13:BS13"/>
-    <mergeCell ref="BL13:BM13"/>
-    <mergeCell ref="BN13:BO13"/>
-    <mergeCell ref="BR12:DY12"/>
-    <mergeCell ref="DZ13:EA13"/>
-    <mergeCell ref="CL13:CM13"/>
-    <mergeCell ref="CN13:CO13"/>
-    <mergeCell ref="BT13:BU13"/>
-    <mergeCell ref="BV13:BW13"/>
-    <mergeCell ref="BX13:BY13"/>
-    <mergeCell ref="BZ13:CA13"/>
-    <mergeCell ref="CB13:CC13"/>
-    <mergeCell ref="CD13:CE13"/>
-    <mergeCell ref="CF13:CG13"/>
-    <mergeCell ref="CH13:CI13"/>
-    <mergeCell ref="CJ13:CK13"/>
-    <mergeCell ref="CP13:CQ13"/>
-    <mergeCell ref="CR13:CS13"/>
-    <mergeCell ref="CT13:CU13"/>
-    <mergeCell ref="CV13:CW13"/>
-    <mergeCell ref="CX13:CY13"/>
-    <mergeCell ref="CZ13:DA13"/>
-    <mergeCell ref="DB13:DC13"/>
-    <mergeCell ref="DD13:DE13"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Created Model for Issue #49
</commit_message>
<xml_diff>
--- a/Documents/Zeitplan.xlsx
+++ b/Documents/Zeitplan.xlsx
@@ -1164,24 +1164,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1194,31 +1176,32 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1226,6 +1209,42 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1234,9 +1253,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1284,40 +1300,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1787,8 +1787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GI90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AL44" sqref="AL44"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AN27" sqref="AN27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1796,35 +1796,35 @@
     <col min="1" max="35" width="5.77734375" style="1" customWidth="1"/>
     <col min="36" max="36" width="7.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="37" max="38" width="5.77734375" style="1" customWidth="1"/>
-    <col min="39" max="39" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="40" max="191" width="5.77734375" style="1" customWidth="1"/>
     <col min="192" max="256" width="3.33203125" style="1" customWidth="1"/>
     <col min="257" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:191" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
     </row>
     <row r="2" spans="1:191" x14ac:dyDescent="0.25">
       <c r="T2" s="9"/>
@@ -1857,17 +1857,17 @@
         <v>160</v>
       </c>
       <c r="N4" s="57"/>
-      <c r="P4" s="81" t="s">
+      <c r="P4" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="81"/>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="67"/>
+      <c r="V4" s="67"/>
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
     </row>
     <row r="5" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -1884,17 +1884,17 @@
       <c r="F5" s="5"/>
       <c r="G5" s="7"/>
       <c r="N5" s="24"/>
-      <c r="P5" s="81" t="s">
+      <c r="P5" s="67" t="s">
         <v>158</v>
       </c>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81"/>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="81"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
+      <c r="S5" s="67"/>
+      <c r="T5" s="67"/>
+      <c r="U5" s="67"/>
+      <c r="V5" s="67"/>
+      <c r="W5" s="67"/>
+      <c r="X5" s="67"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
@@ -1918,17 +1918,17 @@
         <v>15</v>
       </c>
       <c r="N6" s="16"/>
-      <c r="P6" s="81" t="s">
+      <c r="P6" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="81"/>
-      <c r="T6" s="81"/>
-      <c r="U6" s="81"/>
-      <c r="V6" s="81"/>
-      <c r="W6" s="81"/>
-      <c r="X6" s="81"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="67"/>
+      <c r="V6" s="67"/>
+      <c r="W6" s="67"/>
+      <c r="X6" s="67"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
@@ -1946,17 +1946,17 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="N7" s="21"/>
-      <c r="P7" s="81" t="s">
+      <c r="P7" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="81"/>
-      <c r="S7" s="81"/>
-      <c r="T7" s="81"/>
-      <c r="U7" s="81"/>
-      <c r="V7" s="81"/>
-      <c r="W7" s="81"/>
-      <c r="X7" s="81"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="67"/>
+      <c r="S7" s="67"/>
+      <c r="T7" s="67"/>
+      <c r="U7" s="67"/>
+      <c r="V7" s="67"/>
+      <c r="W7" s="67"/>
+      <c r="X7" s="67"/>
     </row>
     <row r="8" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1971,17 +1971,17 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="N8" s="20"/>
-      <c r="P8" s="113" t="s">
+      <c r="P8" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="113"/>
-      <c r="R8" s="113"/>
-      <c r="S8" s="113"/>
-      <c r="T8" s="113"/>
-      <c r="U8" s="113"/>
-      <c r="V8" s="113"/>
-      <c r="W8" s="113"/>
-      <c r="X8" s="113"/>
+      <c r="Q8" s="70"/>
+      <c r="R8" s="70"/>
+      <c r="S8" s="70"/>
+      <c r="T8" s="70"/>
+      <c r="U8" s="70"/>
+      <c r="V8" s="70"/>
+      <c r="W8" s="70"/>
+      <c r="X8" s="70"/>
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
@@ -1989,23 +1989,23 @@
       <c r="AC8" s="5"/>
     </row>
     <row r="9" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="118"/>
+      <c r="A9" s="68"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="12"/>
       <c r="N9" s="49"/>
-      <c r="P9" s="113" t="s">
+      <c r="P9" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="Q9" s="113"/>
-      <c r="R9" s="113"/>
-      <c r="S9" s="113"/>
-      <c r="T9" s="113"/>
-      <c r="U9" s="113"/>
-      <c r="V9" s="113"/>
-      <c r="W9" s="113"/>
-      <c r="X9" s="113"/>
+      <c r="Q9" s="70"/>
+      <c r="R9" s="70"/>
+      <c r="S9" s="70"/>
+      <c r="T9" s="70"/>
+      <c r="U9" s="70"/>
+      <c r="V9" s="70"/>
+      <c r="W9" s="70"/>
+      <c r="X9" s="70"/>
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
@@ -2015,7 +2015,7 @@
       <c r="AJ9" s="13"/>
     </row>
     <row r="10" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="118"/>
+      <c r="A10" s="68"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -2032,18 +2032,18 @@
       <c r="AC10" s="5"/>
     </row>
     <row r="11" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="118"/>
-      <c r="C11" s="116" t="s">
+      <c r="A11" s="68"/>
+      <c r="C11" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="114" t="s">
+      <c r="D11" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="114"/>
-      <c r="F11" s="114" t="s">
+      <c r="E11" s="76"/>
+      <c r="F11" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="114"/>
+      <c r="G11" s="76"/>
       <c r="T11" s="9"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
@@ -2056,596 +2056,596 @@
       <c r="AC11" s="5"/>
     </row>
     <row r="12" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="118"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="114"/>
-      <c r="G12" s="114"/>
-      <c r="H12" s="70" t="s">
+      <c r="A12" s="68"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="71"/>
-      <c r="N12" s="71"/>
-      <c r="O12" s="71"/>
-      <c r="P12" s="71"/>
-      <c r="Q12" s="71"/>
-      <c r="R12" s="71"/>
-      <c r="S12" s="71"/>
-      <c r="T12" s="71"/>
-      <c r="U12" s="71"/>
-      <c r="V12" s="71"/>
-      <c r="W12" s="71"/>
-      <c r="X12" s="71"/>
-      <c r="Y12" s="71"/>
-      <c r="Z12" s="71"/>
-      <c r="AA12" s="71"/>
-      <c r="AB12" s="71"/>
-      <c r="AC12" s="71"/>
-      <c r="AD12" s="71"/>
-      <c r="AE12" s="71"/>
-      <c r="AF12" s="71"/>
-      <c r="AG12" s="71"/>
-      <c r="AH12" s="71"/>
-      <c r="AI12" s="71"/>
-      <c r="AJ12" s="71"/>
-      <c r="AK12" s="71"/>
-      <c r="AL12" s="71"/>
-      <c r="AM12" s="71"/>
-      <c r="AN12" s="71"/>
-      <c r="AO12" s="71"/>
-      <c r="AP12" s="71"/>
-      <c r="AQ12" s="71"/>
-      <c r="AR12" s="71"/>
-      <c r="AS12" s="71"/>
-      <c r="AT12" s="71"/>
-      <c r="AU12" s="71"/>
-      <c r="AV12" s="71"/>
-      <c r="AW12" s="71"/>
-      <c r="AX12" s="71"/>
-      <c r="AY12" s="71"/>
-      <c r="AZ12" s="71"/>
-      <c r="BA12" s="71"/>
-      <c r="BB12" s="71"/>
-      <c r="BC12" s="71"/>
-      <c r="BD12" s="71"/>
-      <c r="BE12" s="71"/>
-      <c r="BF12" s="71"/>
-      <c r="BG12" s="71"/>
-      <c r="BH12" s="71"/>
-      <c r="BI12" s="71"/>
-      <c r="BJ12" s="71"/>
-      <c r="BK12" s="71"/>
-      <c r="BL12" s="71"/>
-      <c r="BM12" s="71"/>
-      <c r="BN12" s="71"/>
-      <c r="BO12" s="71"/>
-      <c r="BP12" s="71"/>
-      <c r="BQ12" s="119"/>
-      <c r="BR12" s="70" t="s">
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="63"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="63"/>
+      <c r="W12" s="63"/>
+      <c r="X12" s="63"/>
+      <c r="Y12" s="63"/>
+      <c r="Z12" s="63"/>
+      <c r="AA12" s="63"/>
+      <c r="AB12" s="63"/>
+      <c r="AC12" s="63"/>
+      <c r="AD12" s="63"/>
+      <c r="AE12" s="63"/>
+      <c r="AF12" s="63"/>
+      <c r="AG12" s="63"/>
+      <c r="AH12" s="63"/>
+      <c r="AI12" s="63"/>
+      <c r="AJ12" s="63"/>
+      <c r="AK12" s="63"/>
+      <c r="AL12" s="63"/>
+      <c r="AM12" s="63"/>
+      <c r="AN12" s="63"/>
+      <c r="AO12" s="63"/>
+      <c r="AP12" s="63"/>
+      <c r="AQ12" s="63"/>
+      <c r="AR12" s="63"/>
+      <c r="AS12" s="63"/>
+      <c r="AT12" s="63"/>
+      <c r="AU12" s="63"/>
+      <c r="AV12" s="63"/>
+      <c r="AW12" s="63"/>
+      <c r="AX12" s="63"/>
+      <c r="AY12" s="63"/>
+      <c r="AZ12" s="63"/>
+      <c r="BA12" s="63"/>
+      <c r="BB12" s="63"/>
+      <c r="BC12" s="63"/>
+      <c r="BD12" s="63"/>
+      <c r="BE12" s="63"/>
+      <c r="BF12" s="63"/>
+      <c r="BG12" s="63"/>
+      <c r="BH12" s="63"/>
+      <c r="BI12" s="63"/>
+      <c r="BJ12" s="63"/>
+      <c r="BK12" s="63"/>
+      <c r="BL12" s="63"/>
+      <c r="BM12" s="63"/>
+      <c r="BN12" s="63"/>
+      <c r="BO12" s="63"/>
+      <c r="BP12" s="63"/>
+      <c r="BQ12" s="64"/>
+      <c r="BR12" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="BS12" s="71"/>
-      <c r="BT12" s="71"/>
-      <c r="BU12" s="71"/>
-      <c r="BV12" s="71"/>
-      <c r="BW12" s="71"/>
-      <c r="BX12" s="71"/>
-      <c r="BY12" s="71"/>
-      <c r="BZ12" s="71"/>
-      <c r="CA12" s="71"/>
-      <c r="CB12" s="71"/>
-      <c r="CC12" s="71"/>
-      <c r="CD12" s="71"/>
-      <c r="CE12" s="71"/>
-      <c r="CF12" s="71"/>
-      <c r="CG12" s="71"/>
-      <c r="CH12" s="71"/>
-      <c r="CI12" s="71"/>
-      <c r="CJ12" s="71"/>
-      <c r="CK12" s="71"/>
-      <c r="CL12" s="71"/>
-      <c r="CM12" s="71"/>
-      <c r="CN12" s="71"/>
-      <c r="CO12" s="71"/>
-      <c r="CP12" s="71"/>
-      <c r="CQ12" s="71"/>
-      <c r="CR12" s="71"/>
-      <c r="CS12" s="71"/>
-      <c r="CT12" s="71"/>
-      <c r="CU12" s="71"/>
-      <c r="CV12" s="71"/>
-      <c r="CW12" s="71"/>
-      <c r="CX12" s="71"/>
-      <c r="CY12" s="71"/>
-      <c r="CZ12" s="71"/>
-      <c r="DA12" s="71"/>
-      <c r="DB12" s="71"/>
-      <c r="DC12" s="71"/>
-      <c r="DD12" s="71"/>
-      <c r="DE12" s="71"/>
-      <c r="DF12" s="71"/>
-      <c r="DG12" s="71"/>
-      <c r="DH12" s="71"/>
-      <c r="DI12" s="71"/>
-      <c r="DJ12" s="71"/>
-      <c r="DK12" s="71"/>
-      <c r="DL12" s="71"/>
-      <c r="DM12" s="71"/>
-      <c r="DN12" s="71"/>
-      <c r="DO12" s="71"/>
-      <c r="DP12" s="71"/>
-      <c r="DQ12" s="71"/>
-      <c r="DR12" s="71"/>
-      <c r="DS12" s="71"/>
-      <c r="DT12" s="71"/>
-      <c r="DU12" s="71"/>
-      <c r="DV12" s="71"/>
-      <c r="DW12" s="71"/>
-      <c r="DX12" s="71"/>
-      <c r="DY12" s="119"/>
-      <c r="DZ12" s="70" t="s">
+      <c r="BS12" s="63"/>
+      <c r="BT12" s="63"/>
+      <c r="BU12" s="63"/>
+      <c r="BV12" s="63"/>
+      <c r="BW12" s="63"/>
+      <c r="BX12" s="63"/>
+      <c r="BY12" s="63"/>
+      <c r="BZ12" s="63"/>
+      <c r="CA12" s="63"/>
+      <c r="CB12" s="63"/>
+      <c r="CC12" s="63"/>
+      <c r="CD12" s="63"/>
+      <c r="CE12" s="63"/>
+      <c r="CF12" s="63"/>
+      <c r="CG12" s="63"/>
+      <c r="CH12" s="63"/>
+      <c r="CI12" s="63"/>
+      <c r="CJ12" s="63"/>
+      <c r="CK12" s="63"/>
+      <c r="CL12" s="63"/>
+      <c r="CM12" s="63"/>
+      <c r="CN12" s="63"/>
+      <c r="CO12" s="63"/>
+      <c r="CP12" s="63"/>
+      <c r="CQ12" s="63"/>
+      <c r="CR12" s="63"/>
+      <c r="CS12" s="63"/>
+      <c r="CT12" s="63"/>
+      <c r="CU12" s="63"/>
+      <c r="CV12" s="63"/>
+      <c r="CW12" s="63"/>
+      <c r="CX12" s="63"/>
+      <c r="CY12" s="63"/>
+      <c r="CZ12" s="63"/>
+      <c r="DA12" s="63"/>
+      <c r="DB12" s="63"/>
+      <c r="DC12" s="63"/>
+      <c r="DD12" s="63"/>
+      <c r="DE12" s="63"/>
+      <c r="DF12" s="63"/>
+      <c r="DG12" s="63"/>
+      <c r="DH12" s="63"/>
+      <c r="DI12" s="63"/>
+      <c r="DJ12" s="63"/>
+      <c r="DK12" s="63"/>
+      <c r="DL12" s="63"/>
+      <c r="DM12" s="63"/>
+      <c r="DN12" s="63"/>
+      <c r="DO12" s="63"/>
+      <c r="DP12" s="63"/>
+      <c r="DQ12" s="63"/>
+      <c r="DR12" s="63"/>
+      <c r="DS12" s="63"/>
+      <c r="DT12" s="63"/>
+      <c r="DU12" s="63"/>
+      <c r="DV12" s="63"/>
+      <c r="DW12" s="63"/>
+      <c r="DX12" s="63"/>
+      <c r="DY12" s="64"/>
+      <c r="DZ12" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="EA12" s="71"/>
-      <c r="EB12" s="71"/>
-      <c r="EC12" s="71"/>
-      <c r="ED12" s="71"/>
-      <c r="EE12" s="71"/>
-      <c r="EF12" s="71"/>
-      <c r="EG12" s="71"/>
-      <c r="EH12" s="71"/>
-      <c r="EI12" s="71"/>
-      <c r="EJ12" s="71"/>
-      <c r="EK12" s="71"/>
-      <c r="EL12" s="71"/>
-      <c r="EM12" s="71"/>
-      <c r="EN12" s="71"/>
-      <c r="EO12" s="71"/>
-      <c r="EP12" s="71"/>
-      <c r="EQ12" s="71"/>
-      <c r="ER12" s="71"/>
-      <c r="ES12" s="71"/>
-      <c r="ET12" s="71"/>
-      <c r="EU12" s="71"/>
-      <c r="EV12" s="71"/>
-      <c r="EW12" s="71"/>
-      <c r="EX12" s="71"/>
-      <c r="EY12" s="71"/>
-      <c r="EZ12" s="71"/>
-      <c r="FA12" s="71"/>
-      <c r="FB12" s="71"/>
-      <c r="FC12" s="71"/>
-      <c r="FD12" s="71"/>
-      <c r="FE12" s="71"/>
-      <c r="FF12" s="71"/>
-      <c r="FG12" s="71"/>
-      <c r="FH12" s="71"/>
-      <c r="FI12" s="71"/>
-      <c r="FJ12" s="71"/>
-      <c r="FK12" s="71"/>
-      <c r="FL12" s="71"/>
-      <c r="FM12" s="71"/>
-      <c r="FN12" s="71"/>
-      <c r="FO12" s="71"/>
-      <c r="FP12" s="71"/>
-      <c r="FQ12" s="71"/>
-      <c r="FR12" s="71"/>
-      <c r="FS12" s="71"/>
-      <c r="FT12" s="71"/>
-      <c r="FU12" s="71"/>
-      <c r="FV12" s="71"/>
-      <c r="FW12" s="71"/>
-      <c r="FX12" s="71"/>
-      <c r="FY12" s="71"/>
-      <c r="FZ12" s="71"/>
-      <c r="GA12" s="71"/>
-      <c r="GB12" s="71"/>
-      <c r="GC12" s="71"/>
-      <c r="GD12" s="71"/>
-      <c r="GE12" s="71"/>
-      <c r="GF12" s="71"/>
-      <c r="GG12" s="71"/>
-      <c r="GH12" s="71"/>
-      <c r="GI12" s="72"/>
+      <c r="EA12" s="63"/>
+      <c r="EB12" s="63"/>
+      <c r="EC12" s="63"/>
+      <c r="ED12" s="63"/>
+      <c r="EE12" s="63"/>
+      <c r="EF12" s="63"/>
+      <c r="EG12" s="63"/>
+      <c r="EH12" s="63"/>
+      <c r="EI12" s="63"/>
+      <c r="EJ12" s="63"/>
+      <c r="EK12" s="63"/>
+      <c r="EL12" s="63"/>
+      <c r="EM12" s="63"/>
+      <c r="EN12" s="63"/>
+      <c r="EO12" s="63"/>
+      <c r="EP12" s="63"/>
+      <c r="EQ12" s="63"/>
+      <c r="ER12" s="63"/>
+      <c r="ES12" s="63"/>
+      <c r="ET12" s="63"/>
+      <c r="EU12" s="63"/>
+      <c r="EV12" s="63"/>
+      <c r="EW12" s="63"/>
+      <c r="EX12" s="63"/>
+      <c r="EY12" s="63"/>
+      <c r="EZ12" s="63"/>
+      <c r="FA12" s="63"/>
+      <c r="FB12" s="63"/>
+      <c r="FC12" s="63"/>
+      <c r="FD12" s="63"/>
+      <c r="FE12" s="63"/>
+      <c r="FF12" s="63"/>
+      <c r="FG12" s="63"/>
+      <c r="FH12" s="63"/>
+      <c r="FI12" s="63"/>
+      <c r="FJ12" s="63"/>
+      <c r="FK12" s="63"/>
+      <c r="FL12" s="63"/>
+      <c r="FM12" s="63"/>
+      <c r="FN12" s="63"/>
+      <c r="FO12" s="63"/>
+      <c r="FP12" s="63"/>
+      <c r="FQ12" s="63"/>
+      <c r="FR12" s="63"/>
+      <c r="FS12" s="63"/>
+      <c r="FT12" s="63"/>
+      <c r="FU12" s="63"/>
+      <c r="FV12" s="63"/>
+      <c r="FW12" s="63"/>
+      <c r="FX12" s="63"/>
+      <c r="FY12" s="63"/>
+      <c r="FZ12" s="63"/>
+      <c r="GA12" s="63"/>
+      <c r="GB12" s="63"/>
+      <c r="GC12" s="63"/>
+      <c r="GD12" s="63"/>
+      <c r="GE12" s="63"/>
+      <c r="GF12" s="63"/>
+      <c r="GG12" s="63"/>
+      <c r="GH12" s="63"/>
+      <c r="GI12" s="120"/>
     </row>
     <row r="13" spans="1:191" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="117"/>
-      <c r="D13" s="115"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="115"/>
-      <c r="H13" s="68">
+      <c r="C13" s="79"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="60">
         <v>1</v>
       </c>
-      <c r="I13" s="69"/>
-      <c r="J13" s="68">
+      <c r="I13" s="61"/>
+      <c r="J13" s="60">
         <v>2</v>
       </c>
-      <c r="K13" s="69"/>
-      <c r="L13" s="68">
+      <c r="K13" s="61"/>
+      <c r="L13" s="60">
         <v>3</v>
       </c>
-      <c r="M13" s="69"/>
-      <c r="N13" s="68">
+      <c r="M13" s="61"/>
+      <c r="N13" s="60">
         <v>4</v>
       </c>
-      <c r="O13" s="69"/>
-      <c r="P13" s="68">
+      <c r="O13" s="61"/>
+      <c r="P13" s="60">
         <v>5</v>
       </c>
-      <c r="Q13" s="69"/>
-      <c r="R13" s="68">
+      <c r="Q13" s="61"/>
+      <c r="R13" s="60">
         <v>6</v>
       </c>
-      <c r="S13" s="69"/>
-      <c r="T13" s="68">
+      <c r="S13" s="61"/>
+      <c r="T13" s="60">
         <v>7</v>
       </c>
-      <c r="U13" s="69"/>
-      <c r="V13" s="68">
+      <c r="U13" s="61"/>
+      <c r="V13" s="60">
         <v>8</v>
       </c>
-      <c r="W13" s="69"/>
-      <c r="X13" s="68">
+      <c r="W13" s="61"/>
+      <c r="X13" s="60">
         <v>9</v>
       </c>
-      <c r="Y13" s="69"/>
-      <c r="Z13" s="68">
+      <c r="Y13" s="61"/>
+      <c r="Z13" s="60">
         <v>10</v>
       </c>
-      <c r="AA13" s="69"/>
-      <c r="AB13" s="68">
+      <c r="AA13" s="61"/>
+      <c r="AB13" s="60">
         <v>11</v>
       </c>
-      <c r="AC13" s="69"/>
-      <c r="AD13" s="68">
+      <c r="AC13" s="61"/>
+      <c r="AD13" s="60">
         <v>12</v>
       </c>
-      <c r="AE13" s="69"/>
-      <c r="AF13" s="68">
+      <c r="AE13" s="61"/>
+      <c r="AF13" s="60">
         <v>13</v>
       </c>
-      <c r="AG13" s="69"/>
-      <c r="AH13" s="68">
+      <c r="AG13" s="61"/>
+      <c r="AH13" s="60">
         <v>14</v>
       </c>
-      <c r="AI13" s="69"/>
-      <c r="AJ13" s="68">
+      <c r="AI13" s="61"/>
+      <c r="AJ13" s="60">
         <v>15</v>
       </c>
-      <c r="AK13" s="69"/>
-      <c r="AL13" s="68">
+      <c r="AK13" s="61"/>
+      <c r="AL13" s="60">
         <v>16</v>
       </c>
-      <c r="AM13" s="69"/>
-      <c r="AN13" s="68">
+      <c r="AM13" s="61"/>
+      <c r="AN13" s="60">
         <v>17</v>
       </c>
-      <c r="AO13" s="69"/>
-      <c r="AP13" s="68">
+      <c r="AO13" s="61"/>
+      <c r="AP13" s="60">
         <v>18</v>
       </c>
-      <c r="AQ13" s="69"/>
-      <c r="AR13" s="68">
+      <c r="AQ13" s="61"/>
+      <c r="AR13" s="60">
         <v>19</v>
       </c>
-      <c r="AS13" s="69"/>
-      <c r="AT13" s="68">
+      <c r="AS13" s="61"/>
+      <c r="AT13" s="60">
         <v>20</v>
       </c>
-      <c r="AU13" s="69"/>
-      <c r="AV13" s="68">
+      <c r="AU13" s="61"/>
+      <c r="AV13" s="60">
         <v>21</v>
       </c>
-      <c r="AW13" s="69"/>
-      <c r="AX13" s="68">
+      <c r="AW13" s="61"/>
+      <c r="AX13" s="60">
         <v>22</v>
       </c>
-      <c r="AY13" s="69"/>
-      <c r="AZ13" s="68">
+      <c r="AY13" s="61"/>
+      <c r="AZ13" s="60">
         <v>23</v>
       </c>
-      <c r="BA13" s="69"/>
-      <c r="BB13" s="68">
+      <c r="BA13" s="61"/>
+      <c r="BB13" s="60">
         <v>24</v>
       </c>
-      <c r="BC13" s="69"/>
-      <c r="BD13" s="68">
+      <c r="BC13" s="61"/>
+      <c r="BD13" s="60">
         <v>25</v>
       </c>
-      <c r="BE13" s="69"/>
-      <c r="BF13" s="68">
+      <c r="BE13" s="61"/>
+      <c r="BF13" s="60">
         <v>26</v>
       </c>
-      <c r="BG13" s="69"/>
-      <c r="BH13" s="68">
+      <c r="BG13" s="61"/>
+      <c r="BH13" s="60">
         <v>27</v>
       </c>
-      <c r="BI13" s="69"/>
-      <c r="BJ13" s="68">
+      <c r="BI13" s="61"/>
+      <c r="BJ13" s="60">
         <v>28</v>
       </c>
-      <c r="BK13" s="69"/>
-      <c r="BL13" s="68">
+      <c r="BK13" s="61"/>
+      <c r="BL13" s="60">
         <v>29</v>
       </c>
-      <c r="BM13" s="69"/>
-      <c r="BN13" s="68">
+      <c r="BM13" s="61"/>
+      <c r="BN13" s="60">
         <v>30</v>
       </c>
-      <c r="BO13" s="69"/>
-      <c r="BP13" s="68">
+      <c r="BO13" s="61"/>
+      <c r="BP13" s="60">
         <v>31</v>
       </c>
-      <c r="BQ13" s="120"/>
-      <c r="BR13" s="68">
+      <c r="BQ13" s="69"/>
+      <c r="BR13" s="60">
         <v>1</v>
       </c>
-      <c r="BS13" s="69"/>
-      <c r="BT13" s="68">
+      <c r="BS13" s="61"/>
+      <c r="BT13" s="60">
         <v>2</v>
       </c>
-      <c r="BU13" s="69"/>
-      <c r="BV13" s="68">
+      <c r="BU13" s="61"/>
+      <c r="BV13" s="60">
         <v>3</v>
       </c>
-      <c r="BW13" s="69"/>
-      <c r="BX13" s="68">
+      <c r="BW13" s="61"/>
+      <c r="BX13" s="60">
         <v>4</v>
       </c>
-      <c r="BY13" s="69"/>
-      <c r="BZ13" s="68">
+      <c r="BY13" s="61"/>
+      <c r="BZ13" s="60">
         <v>5</v>
       </c>
-      <c r="CA13" s="69"/>
-      <c r="CB13" s="68">
+      <c r="CA13" s="61"/>
+      <c r="CB13" s="60">
         <v>6</v>
       </c>
-      <c r="CC13" s="69"/>
-      <c r="CD13" s="68">
+      <c r="CC13" s="61"/>
+      <c r="CD13" s="60">
         <v>7</v>
       </c>
-      <c r="CE13" s="69"/>
-      <c r="CF13" s="68">
+      <c r="CE13" s="61"/>
+      <c r="CF13" s="60">
         <v>8</v>
       </c>
-      <c r="CG13" s="69"/>
-      <c r="CH13" s="68">
+      <c r="CG13" s="61"/>
+      <c r="CH13" s="60">
         <v>9</v>
       </c>
-      <c r="CI13" s="69"/>
-      <c r="CJ13" s="68">
+      <c r="CI13" s="61"/>
+      <c r="CJ13" s="60">
         <v>10</v>
       </c>
-      <c r="CK13" s="69"/>
-      <c r="CL13" s="68">
+      <c r="CK13" s="61"/>
+      <c r="CL13" s="60">
         <v>11</v>
       </c>
-      <c r="CM13" s="69"/>
-      <c r="CN13" s="68">
+      <c r="CM13" s="61"/>
+      <c r="CN13" s="60">
         <v>12</v>
       </c>
-      <c r="CO13" s="69"/>
-      <c r="CP13" s="68">
+      <c r="CO13" s="61"/>
+      <c r="CP13" s="60">
         <v>13</v>
       </c>
-      <c r="CQ13" s="69"/>
-      <c r="CR13" s="68">
+      <c r="CQ13" s="61"/>
+      <c r="CR13" s="60">
         <v>14</v>
       </c>
-      <c r="CS13" s="69"/>
-      <c r="CT13" s="68">
+      <c r="CS13" s="61"/>
+      <c r="CT13" s="60">
         <v>15</v>
       </c>
-      <c r="CU13" s="69"/>
-      <c r="CV13" s="68">
+      <c r="CU13" s="61"/>
+      <c r="CV13" s="60">
         <v>16</v>
       </c>
-      <c r="CW13" s="69"/>
-      <c r="CX13" s="68">
+      <c r="CW13" s="61"/>
+      <c r="CX13" s="60">
         <v>17</v>
       </c>
-      <c r="CY13" s="69"/>
-      <c r="CZ13" s="68">
+      <c r="CY13" s="61"/>
+      <c r="CZ13" s="60">
         <v>18</v>
       </c>
-      <c r="DA13" s="69"/>
-      <c r="DB13" s="68">
+      <c r="DA13" s="61"/>
+      <c r="DB13" s="60">
         <v>19</v>
       </c>
-      <c r="DC13" s="69"/>
-      <c r="DD13" s="68">
+      <c r="DC13" s="61"/>
+      <c r="DD13" s="60">
         <v>20</v>
       </c>
-      <c r="DE13" s="69"/>
-      <c r="DF13" s="68">
+      <c r="DE13" s="61"/>
+      <c r="DF13" s="60">
         <v>21</v>
       </c>
-      <c r="DG13" s="69"/>
-      <c r="DH13" s="68">
+      <c r="DG13" s="61"/>
+      <c r="DH13" s="60">
         <v>22</v>
       </c>
-      <c r="DI13" s="69"/>
-      <c r="DJ13" s="68">
+      <c r="DI13" s="61"/>
+      <c r="DJ13" s="60">
         <v>23</v>
       </c>
-      <c r="DK13" s="69"/>
-      <c r="DL13" s="68">
+      <c r="DK13" s="61"/>
+      <c r="DL13" s="60">
         <v>24</v>
       </c>
-      <c r="DM13" s="69"/>
-      <c r="DN13" s="68">
+      <c r="DM13" s="61"/>
+      <c r="DN13" s="60">
         <v>25</v>
       </c>
-      <c r="DO13" s="69"/>
-      <c r="DP13" s="68">
+      <c r="DO13" s="61"/>
+      <c r="DP13" s="60">
         <v>26</v>
       </c>
-      <c r="DQ13" s="69"/>
-      <c r="DR13" s="68">
+      <c r="DQ13" s="61"/>
+      <c r="DR13" s="60">
         <v>27</v>
       </c>
-      <c r="DS13" s="69"/>
-      <c r="DT13" s="68">
+      <c r="DS13" s="61"/>
+      <c r="DT13" s="60">
         <v>28</v>
       </c>
-      <c r="DU13" s="69"/>
-      <c r="DV13" s="68">
+      <c r="DU13" s="61"/>
+      <c r="DV13" s="60">
         <v>29</v>
       </c>
-      <c r="DW13" s="69"/>
-      <c r="DX13" s="68">
+      <c r="DW13" s="61"/>
+      <c r="DX13" s="60">
         <v>30</v>
       </c>
-      <c r="DY13" s="69"/>
-      <c r="DZ13" s="68">
+      <c r="DY13" s="61"/>
+      <c r="DZ13" s="60">
         <v>1</v>
       </c>
-      <c r="EA13" s="69"/>
-      <c r="EB13" s="68">
+      <c r="EA13" s="61"/>
+      <c r="EB13" s="60">
         <v>2</v>
       </c>
-      <c r="EC13" s="69"/>
-      <c r="ED13" s="68">
+      <c r="EC13" s="61"/>
+      <c r="ED13" s="60">
         <v>3</v>
       </c>
-      <c r="EE13" s="69"/>
-      <c r="EF13" s="68">
+      <c r="EE13" s="61"/>
+      <c r="EF13" s="60">
         <v>4</v>
       </c>
-      <c r="EG13" s="69"/>
-      <c r="EH13" s="68">
+      <c r="EG13" s="61"/>
+      <c r="EH13" s="60">
         <v>5</v>
       </c>
-      <c r="EI13" s="69"/>
-      <c r="EJ13" s="68">
+      <c r="EI13" s="61"/>
+      <c r="EJ13" s="60">
         <v>6</v>
       </c>
-      <c r="EK13" s="69"/>
-      <c r="EL13" s="68">
+      <c r="EK13" s="61"/>
+      <c r="EL13" s="60">
         <v>7</v>
       </c>
-      <c r="EM13" s="69"/>
-      <c r="EN13" s="68">
+      <c r="EM13" s="61"/>
+      <c r="EN13" s="60">
         <v>8</v>
       </c>
-      <c r="EO13" s="69"/>
-      <c r="EP13" s="68">
+      <c r="EO13" s="61"/>
+      <c r="EP13" s="60">
         <v>9</v>
       </c>
-      <c r="EQ13" s="69"/>
-      <c r="ER13" s="68">
+      <c r="EQ13" s="61"/>
+      <c r="ER13" s="60">
         <v>10</v>
       </c>
-      <c r="ES13" s="69"/>
-      <c r="ET13" s="68">
+      <c r="ES13" s="61"/>
+      <c r="ET13" s="60">
         <v>11</v>
       </c>
-      <c r="EU13" s="69"/>
-      <c r="EV13" s="68">
+      <c r="EU13" s="61"/>
+      <c r="EV13" s="60">
         <v>12</v>
       </c>
-      <c r="EW13" s="69"/>
-      <c r="EX13" s="68">
+      <c r="EW13" s="61"/>
+      <c r="EX13" s="60">
         <v>13</v>
       </c>
-      <c r="EY13" s="69"/>
-      <c r="EZ13" s="68">
+      <c r="EY13" s="61"/>
+      <c r="EZ13" s="60">
         <v>14</v>
       </c>
-      <c r="FA13" s="69"/>
-      <c r="FB13" s="68">
+      <c r="FA13" s="61"/>
+      <c r="FB13" s="60">
         <v>15</v>
       </c>
-      <c r="FC13" s="69"/>
-      <c r="FD13" s="68">
+      <c r="FC13" s="61"/>
+      <c r="FD13" s="60">
         <v>16</v>
       </c>
-      <c r="FE13" s="69"/>
-      <c r="FF13" s="68">
+      <c r="FE13" s="61"/>
+      <c r="FF13" s="60">
         <v>17</v>
       </c>
-      <c r="FG13" s="69"/>
-      <c r="FH13" s="68">
+      <c r="FG13" s="61"/>
+      <c r="FH13" s="60">
         <v>18</v>
       </c>
-      <c r="FI13" s="69"/>
-      <c r="FJ13" s="68">
+      <c r="FI13" s="61"/>
+      <c r="FJ13" s="60">
         <v>19</v>
       </c>
-      <c r="FK13" s="69"/>
-      <c r="FL13" s="68">
+      <c r="FK13" s="61"/>
+      <c r="FL13" s="60">
         <v>20</v>
       </c>
-      <c r="FM13" s="69"/>
-      <c r="FN13" s="68">
+      <c r="FM13" s="61"/>
+      <c r="FN13" s="60">
         <v>21</v>
       </c>
-      <c r="FO13" s="69"/>
-      <c r="FP13" s="68">
+      <c r="FO13" s="61"/>
+      <c r="FP13" s="60">
         <v>22</v>
       </c>
-      <c r="FQ13" s="69"/>
-      <c r="FR13" s="68">
+      <c r="FQ13" s="61"/>
+      <c r="FR13" s="60">
         <v>23</v>
       </c>
-      <c r="FS13" s="69"/>
-      <c r="FT13" s="68">
+      <c r="FS13" s="61"/>
+      <c r="FT13" s="60">
         <v>24</v>
       </c>
-      <c r="FU13" s="69"/>
-      <c r="FV13" s="68">
+      <c r="FU13" s="61"/>
+      <c r="FV13" s="60">
         <v>25</v>
       </c>
-      <c r="FW13" s="69"/>
-      <c r="FX13" s="68">
+      <c r="FW13" s="61"/>
+      <c r="FX13" s="60">
         <v>26</v>
       </c>
-      <c r="FY13" s="69"/>
-      <c r="FZ13" s="68">
+      <c r="FY13" s="61"/>
+      <c r="FZ13" s="60">
         <v>27</v>
       </c>
-      <c r="GA13" s="69"/>
-      <c r="GB13" s="68">
+      <c r="GA13" s="61"/>
+      <c r="GB13" s="60">
         <v>28</v>
       </c>
-      <c r="GC13" s="69"/>
-      <c r="GD13" s="68">
+      <c r="GC13" s="61"/>
+      <c r="GD13" s="60">
         <v>29</v>
       </c>
-      <c r="GE13" s="69"/>
-      <c r="GF13" s="68">
+      <c r="GE13" s="61"/>
+      <c r="GF13" s="60">
         <v>30</v>
       </c>
-      <c r="GG13" s="69"/>
-      <c r="GH13" s="68">
+      <c r="GG13" s="61"/>
+      <c r="GH13" s="60">
         <v>31</v>
       </c>
-      <c r="GI13" s="69"/>
+      <c r="GI13" s="61"/>
     </row>
     <row r="14" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="113" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="75"/>
+      <c r="B14" s="114"/>
       <c r="C14" s="37"/>
-      <c r="D14" s="91">
+      <c r="D14" s="97">
         <f>SUM(D15:E61)</f>
         <v>51.050000000000011</v>
       </c>
-      <c r="E14" s="93"/>
-      <c r="F14" s="91">
+      <c r="E14" s="99"/>
+      <c r="F14" s="97">
         <f>SUM(F15:G61)</f>
-        <v>33.25</v>
-      </c>
-      <c r="G14" s="92"/>
+        <v>33.416000000000004</v>
+      </c>
+      <c r="G14" s="98"/>
       <c r="H14" s="18"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -2832,22 +2832,22 @@
       <c r="GI14" s="14"/>
     </row>
     <row r="15" spans="1:191" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="82" t="s">
+      <c r="A15" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="83"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="62">
+      <c r="D15" s="65">
         <v>1.5</v>
       </c>
-      <c r="E15" s="63"/>
-      <c r="F15" s="62">
+      <c r="E15" s="66"/>
+      <c r="F15" s="65">
         <f>SUM(H15:GI15)</f>
         <v>0.5</v>
       </c>
-      <c r="G15" s="64"/>
+      <c r="G15" s="80"/>
       <c r="H15" s="47"/>
       <c r="I15" s="12"/>
       <c r="J15" s="24">
@@ -3036,22 +3036,22 @@
       <c r="GI15" s="34"/>
     </row>
     <row r="16" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="67"/>
+      <c r="B16" s="82"/>
       <c r="C16" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="62">
+      <c r="D16" s="65">
         <v>0.6</v>
       </c>
-      <c r="E16" s="63"/>
-      <c r="F16" s="62">
+      <c r="E16" s="66"/>
+      <c r="F16" s="65">
         <f>SUM(H16:GI16)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="64"/>
+      <c r="G16" s="80"/>
       <c r="H16" s="47"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
@@ -3238,22 +3238,22 @@
       <c r="GI16" s="32"/>
     </row>
     <row r="17" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="67"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="62">
+      <c r="D17" s="65">
         <v>1</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="62">
+      <c r="E17" s="66"/>
+      <c r="F17" s="65">
         <f>SUM(H17:GI17)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="64"/>
+      <c r="G17" s="80"/>
       <c r="H17" s="47"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
@@ -3444,22 +3444,22 @@
       <c r="GI17" s="32"/>
     </row>
     <row r="18" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="67"/>
+      <c r="B18" s="82"/>
       <c r="C18" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="62">
+      <c r="D18" s="65">
         <v>0.8</v>
       </c>
-      <c r="E18" s="63"/>
-      <c r="F18" s="62">
+      <c r="E18" s="66"/>
+      <c r="F18" s="65">
         <f t="shared" ref="F18:F60" si="0">SUM(H18:GI18)</f>
         <v>0.75</v>
       </c>
-      <c r="G18" s="64"/>
+      <c r="G18" s="80"/>
       <c r="H18" s="26"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
@@ -3648,22 +3648,22 @@
       <c r="GI18" s="32"/>
     </row>
     <row r="19" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="67"/>
+      <c r="B19" s="82"/>
       <c r="C19" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="62">
+      <c r="D19" s="65">
         <v>0.5</v>
       </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="62">
+      <c r="E19" s="66"/>
+      <c r="F19" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="64"/>
+      <c r="G19" s="80"/>
       <c r="H19" s="26"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
@@ -3850,22 +3850,22 @@
       <c r="GI19" s="36"/>
     </row>
     <row r="20" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="67"/>
+      <c r="B20" s="82"/>
       <c r="C20" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="62">
+      <c r="D20" s="65">
         <v>0.3</v>
       </c>
-      <c r="E20" s="63"/>
-      <c r="F20" s="62">
+      <c r="E20" s="66"/>
+      <c r="F20" s="65">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="64"/>
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="G20" s="80"/>
       <c r="H20" s="26"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -3897,7 +3897,9 @@
       <c r="AJ20" s="32"/>
       <c r="AK20" s="32"/>
       <c r="AL20" s="32"/>
-      <c r="AM20" s="32"/>
+      <c r="AM20" s="24">
+        <v>0.16600000000000001</v>
+      </c>
       <c r="AN20" s="49"/>
       <c r="AO20" s="52"/>
       <c r="AP20" s="51"/>
@@ -4052,22 +4054,22 @@
       <c r="GI20" s="36"/>
     </row>
     <row r="21" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="67"/>
+      <c r="B21" s="82"/>
       <c r="C21" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="62">
+      <c r="D21" s="65">
         <v>1</v>
       </c>
-      <c r="E21" s="63"/>
-      <c r="F21" s="62">
+      <c r="E21" s="66"/>
+      <c r="F21" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="64"/>
+      <c r="G21" s="80"/>
       <c r="H21" s="26"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
@@ -4254,22 +4256,22 @@
       <c r="GI21" s="36"/>
     </row>
     <row r="22" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="67"/>
+      <c r="B22" s="82"/>
       <c r="C22" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="62">
+      <c r="D22" s="65">
         <v>0.6</v>
       </c>
-      <c r="E22" s="63"/>
-      <c r="F22" s="62">
+      <c r="E22" s="66"/>
+      <c r="F22" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="64"/>
+      <c r="G22" s="80"/>
       <c r="H22" s="26"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
@@ -4456,22 +4458,22 @@
       <c r="GI22" s="36"/>
     </row>
     <row r="23" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="67"/>
+      <c r="B23" s="82"/>
       <c r="C23" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="62">
+      <c r="D23" s="65">
         <v>0.6</v>
       </c>
-      <c r="E23" s="63"/>
-      <c r="F23" s="62">
+      <c r="E23" s="66"/>
+      <c r="F23" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="64"/>
+      <c r="G23" s="80"/>
       <c r="H23" s="26"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
@@ -4658,22 +4660,22 @@
       <c r="GI23" s="36"/>
     </row>
     <row r="24" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="67"/>
+      <c r="B24" s="82"/>
       <c r="C24" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="62">
+      <c r="D24" s="65">
         <v>3</v>
       </c>
-      <c r="E24" s="63"/>
-      <c r="F24" s="62">
+      <c r="E24" s="66"/>
+      <c r="F24" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="64"/>
+      <c r="G24" s="80"/>
       <c r="H24" s="26"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
@@ -4860,22 +4862,22 @@
       <c r="GI24" s="36"/>
     </row>
     <row r="25" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="67"/>
+      <c r="B25" s="82"/>
       <c r="C25" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="62">
+      <c r="D25" s="65">
         <v>1.5</v>
       </c>
-      <c r="E25" s="63"/>
-      <c r="F25" s="62">
+      <c r="E25" s="66"/>
+      <c r="F25" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="64"/>
+      <c r="G25" s="80"/>
       <c r="H25" s="26"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
@@ -5062,22 +5064,22 @@
       <c r="GI25" s="36"/>
     </row>
     <row r="26" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A26" s="66" t="s">
+      <c r="A26" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="67"/>
+      <c r="B26" s="82"/>
       <c r="C26" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="62">
+      <c r="D26" s="65">
         <v>1</v>
       </c>
-      <c r="E26" s="63"/>
-      <c r="F26" s="62">
+      <c r="E26" s="66"/>
+      <c r="F26" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="64"/>
+      <c r="G26" s="80"/>
       <c r="H26" s="26"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
@@ -5264,22 +5266,22 @@
       <c r="GI26" s="36"/>
     </row>
     <row r="27" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="67"/>
+      <c r="B27" s="82"/>
       <c r="C27" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="62">
+      <c r="D27" s="65">
         <v>1</v>
       </c>
-      <c r="E27" s="63"/>
-      <c r="F27" s="62">
+      <c r="E27" s="66"/>
+      <c r="F27" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G27" s="64"/>
+      <c r="G27" s="80"/>
       <c r="H27" s="26"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
@@ -5466,22 +5468,22 @@
       <c r="GI27" s="36"/>
     </row>
     <row r="28" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A28" s="66" t="s">
+      <c r="A28" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="67"/>
+      <c r="B28" s="82"/>
       <c r="C28" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="62">
+      <c r="D28" s="65">
         <v>1</v>
       </c>
-      <c r="E28" s="63"/>
-      <c r="F28" s="62">
+      <c r="E28" s="66"/>
+      <c r="F28" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G28" s="64"/>
+      <c r="G28" s="80"/>
       <c r="H28" s="26"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
@@ -5668,22 +5670,22 @@
       <c r="GI28" s="36"/>
     </row>
     <row r="29" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="67"/>
+      <c r="B29" s="82"/>
       <c r="C29" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="62">
+      <c r="D29" s="65">
         <v>1</v>
       </c>
-      <c r="E29" s="63"/>
-      <c r="F29" s="62">
+      <c r="E29" s="66"/>
+      <c r="F29" s="65">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G29" s="64"/>
+      <c r="G29" s="80"/>
       <c r="H29" s="26"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
@@ -5872,22 +5874,22 @@
       <c r="GI29" s="36"/>
     </row>
     <row r="30" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A30" s="66" t="s">
+      <c r="A30" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="67"/>
+      <c r="B30" s="82"/>
       <c r="C30" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="62">
+      <c r="D30" s="65">
         <v>1</v>
       </c>
-      <c r="E30" s="63"/>
-      <c r="F30" s="62">
+      <c r="E30" s="66"/>
+      <c r="F30" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G30" s="64"/>
+      <c r="G30" s="80"/>
       <c r="H30" s="26"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
@@ -6076,22 +6078,22 @@
       <c r="GI30" s="36"/>
     </row>
     <row r="31" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A31" s="66" t="s">
+      <c r="A31" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="67"/>
+      <c r="B31" s="82"/>
       <c r="C31" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="62">
+      <c r="D31" s="65">
         <v>4</v>
       </c>
-      <c r="E31" s="63"/>
-      <c r="F31" s="62">
+      <c r="E31" s="66"/>
+      <c r="F31" s="65">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G31" s="64"/>
+      <c r="G31" s="80"/>
       <c r="H31" s="26"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
@@ -6282,22 +6284,22 @@
       <c r="GI31" s="36"/>
     </row>
     <row r="32" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A32" s="66" t="s">
+      <c r="A32" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="67"/>
+      <c r="B32" s="82"/>
       <c r="C32" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="62">
+      <c r="D32" s="65">
         <v>0.6</v>
       </c>
-      <c r="E32" s="63"/>
-      <c r="F32" s="62">
+      <c r="E32" s="66"/>
+      <c r="F32" s="65">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G32" s="64"/>
+      <c r="G32" s="80"/>
       <c r="H32" s="26"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
@@ -6486,22 +6488,22 @@
       <c r="GI32" s="36"/>
     </row>
     <row r="33" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="67"/>
+      <c r="B33" s="82"/>
       <c r="C33" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="62">
+      <c r="D33" s="65">
         <v>0.5</v>
       </c>
-      <c r="E33" s="63"/>
-      <c r="F33" s="62">
+      <c r="E33" s="66"/>
+      <c r="F33" s="65">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G33" s="64"/>
+      <c r="G33" s="80"/>
       <c r="H33" s="26"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
@@ -6690,22 +6692,22 @@
       <c r="GI33" s="36"/>
     </row>
     <row r="34" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A34" s="66" t="s">
+      <c r="A34" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="67"/>
+      <c r="B34" s="82"/>
       <c r="C34" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="62">
+      <c r="D34" s="65">
         <v>0.3</v>
       </c>
-      <c r="E34" s="63"/>
-      <c r="F34" s="62">
+      <c r="E34" s="66"/>
+      <c r="F34" s="65">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G34" s="64"/>
+      <c r="G34" s="80"/>
       <c r="H34" s="26"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
@@ -6894,22 +6896,22 @@
       <c r="GI34" s="36"/>
     </row>
     <row r="35" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A35" s="66" t="s">
+      <c r="A35" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="67"/>
+      <c r="B35" s="82"/>
       <c r="C35" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="62">
+      <c r="D35" s="65">
         <v>0.3</v>
       </c>
-      <c r="E35" s="63"/>
-      <c r="F35" s="62">
+      <c r="E35" s="66"/>
+      <c r="F35" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G35" s="64"/>
+      <c r="G35" s="80"/>
       <c r="H35" s="26"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
@@ -7096,22 +7098,22 @@
       <c r="GI35" s="36"/>
     </row>
     <row r="36" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A36" s="66" t="s">
+      <c r="A36" s="81" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="67"/>
+      <c r="B36" s="82"/>
       <c r="C36" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="62">
+      <c r="D36" s="65">
         <v>1.5</v>
       </c>
-      <c r="E36" s="63"/>
-      <c r="F36" s="62">
+      <c r="E36" s="66"/>
+      <c r="F36" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G36" s="64"/>
+      <c r="G36" s="80"/>
       <c r="H36" s="26"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
@@ -7298,22 +7300,22 @@
       <c r="GI36" s="36"/>
     </row>
     <row r="37" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A37" s="66" t="s">
+      <c r="A37" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="67"/>
+      <c r="B37" s="82"/>
       <c r="C37" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="62">
+      <c r="D37" s="65">
         <v>0.5</v>
       </c>
-      <c r="E37" s="63"/>
-      <c r="F37" s="62">
+      <c r="E37" s="66"/>
+      <c r="F37" s="65">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G37" s="64"/>
+      <c r="G37" s="80"/>
       <c r="H37" s="26"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
@@ -7502,22 +7504,22 @@
       <c r="GI37" s="36"/>
     </row>
     <row r="38" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A38" s="66" t="s">
+      <c r="A38" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="67"/>
+      <c r="B38" s="82"/>
       <c r="C38" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="62">
+      <c r="D38" s="65">
         <v>0.25</v>
       </c>
-      <c r="E38" s="63"/>
-      <c r="F38" s="62">
+      <c r="E38" s="66"/>
+      <c r="F38" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G38" s="64"/>
+      <c r="G38" s="80"/>
       <c r="H38" s="26"/>
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
@@ -7706,22 +7708,22 @@
       <c r="GI38" s="36"/>
     </row>
     <row r="39" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="67"/>
+      <c r="B39" s="82"/>
       <c r="C39" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="62">
+      <c r="D39" s="65">
         <v>0.5</v>
       </c>
-      <c r="E39" s="63"/>
-      <c r="F39" s="62">
+      <c r="E39" s="66"/>
+      <c r="F39" s="65">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="G39" s="64"/>
+      <c r="G39" s="80"/>
       <c r="H39" s="26"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
@@ -7910,22 +7912,22 @@
       <c r="GI39" s="36"/>
     </row>
     <row r="40" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A40" s="66" t="s">
+      <c r="A40" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="67"/>
+      <c r="B40" s="82"/>
       <c r="C40" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="62">
+      <c r="D40" s="65">
         <v>0.5</v>
       </c>
-      <c r="E40" s="63"/>
-      <c r="F40" s="62">
+      <c r="E40" s="66"/>
+      <c r="F40" s="65">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G40" s="64"/>
+      <c r="G40" s="80"/>
       <c r="H40" s="26"/>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
@@ -8114,22 +8116,22 @@
       <c r="GI40" s="36"/>
     </row>
     <row r="41" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="67"/>
+      <c r="B41" s="82"/>
       <c r="C41" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="62">
+      <c r="D41" s="65">
         <v>0.3</v>
       </c>
-      <c r="E41" s="63"/>
-      <c r="F41" s="62">
+      <c r="E41" s="66"/>
+      <c r="F41" s="65">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G41" s="64"/>
+      <c r="G41" s="80"/>
       <c r="H41" s="26"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
@@ -8318,22 +8320,22 @@
       <c r="GI41" s="36"/>
     </row>
     <row r="42" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A42" s="66" t="s">
+      <c r="A42" s="81" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="67"/>
+      <c r="B42" s="82"/>
       <c r="C42" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="62">
+      <c r="D42" s="65">
         <v>0.5</v>
       </c>
-      <c r="E42" s="63"/>
-      <c r="F42" s="62">
+      <c r="E42" s="66"/>
+      <c r="F42" s="65">
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-      <c r="G42" s="64"/>
+      <c r="G42" s="80"/>
       <c r="H42" s="26"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
@@ -8522,22 +8524,22 @@
       <c r="GI42" s="36"/>
     </row>
     <row r="43" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A43" s="66" t="s">
+      <c r="A43" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="67"/>
+      <c r="B43" s="82"/>
       <c r="C43" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D43" s="62">
+      <c r="D43" s="65">
         <v>1.3</v>
       </c>
-      <c r="E43" s="63"/>
-      <c r="F43" s="62">
+      <c r="E43" s="66"/>
+      <c r="F43" s="65">
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
-      <c r="G43" s="64"/>
+      <c r="G43" s="80"/>
       <c r="H43" s="26"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
@@ -8728,22 +8730,22 @@
       <c r="GI43" s="36"/>
     </row>
     <row r="44" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="66" t="s">
+      <c r="A44" s="81" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="67"/>
+      <c r="B44" s="82"/>
       <c r="C44" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="62">
+      <c r="D44" s="65">
         <v>1.3</v>
       </c>
-      <c r="E44" s="63"/>
-      <c r="F44" s="62">
+      <c r="E44" s="66"/>
+      <c r="F44" s="65">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G44" s="64"/>
+      <c r="G44" s="80"/>
       <c r="H44" s="26"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
@@ -8932,22 +8934,22 @@
       <c r="GI44" s="36"/>
     </row>
     <row r="45" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A45" s="66" t="s">
+      <c r="A45" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="67"/>
+      <c r="B45" s="82"/>
       <c r="C45" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="62">
+      <c r="D45" s="65">
         <v>1</v>
       </c>
-      <c r="E45" s="63"/>
-      <c r="F45" s="62">
+      <c r="E45" s="66"/>
+      <c r="F45" s="65">
         <f t="shared" si="0"/>
         <v>1.05</v>
       </c>
-      <c r="G45" s="64"/>
+      <c r="G45" s="80"/>
       <c r="H45" s="26"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
@@ -9138,22 +9140,22 @@
       <c r="GI45" s="36"/>
     </row>
     <row r="46" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A46" s="66" t="s">
+      <c r="A46" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="67"/>
+      <c r="B46" s="82"/>
       <c r="C46" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="D46" s="62">
+      <c r="D46" s="65">
         <v>1</v>
       </c>
-      <c r="E46" s="63"/>
-      <c r="F46" s="62">
+      <c r="E46" s="66"/>
+      <c r="F46" s="65">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="G46" s="64"/>
+      <c r="G46" s="80"/>
       <c r="H46" s="26"/>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
@@ -9342,22 +9344,22 @@
       <c r="GI46" s="36"/>
     </row>
     <row r="47" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A47" s="66" t="s">
+      <c r="A47" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="67"/>
+      <c r="B47" s="82"/>
       <c r="C47" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="D47" s="62">
+      <c r="D47" s="65">
         <v>1</v>
       </c>
-      <c r="E47" s="63"/>
-      <c r="F47" s="62">
+      <c r="E47" s="66"/>
+      <c r="F47" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G47" s="64"/>
+      <c r="G47" s="80"/>
       <c r="H47" s="26"/>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
@@ -9544,22 +9546,22 @@
       <c r="GI47" s="36"/>
     </row>
     <row r="48" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A48" s="66" t="s">
+      <c r="A48" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="B48" s="67"/>
+      <c r="B48" s="82"/>
       <c r="C48" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D48" s="62">
+      <c r="D48" s="65">
         <v>0.3</v>
       </c>
-      <c r="E48" s="63"/>
-      <c r="F48" s="62">
+      <c r="E48" s="66"/>
+      <c r="F48" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G48" s="64"/>
+      <c r="G48" s="80"/>
       <c r="H48" s="26"/>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
@@ -9746,22 +9748,22 @@
       <c r="GI48" s="36"/>
     </row>
     <row r="49" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A49" s="66" t="s">
+      <c r="A49" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="67"/>
+      <c r="B49" s="82"/>
       <c r="C49" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="62">
+      <c r="D49" s="65">
         <v>2</v>
       </c>
-      <c r="E49" s="63"/>
-      <c r="F49" s="62">
+      <c r="E49" s="66"/>
+      <c r="F49" s="65">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G49" s="64"/>
+      <c r="G49" s="80"/>
       <c r="H49" s="26"/>
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
@@ -9952,22 +9954,22 @@
       <c r="GI49" s="36"/>
     </row>
     <row r="50" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A50" s="66" t="s">
+      <c r="A50" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="67"/>
+      <c r="B50" s="82"/>
       <c r="C50" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="D50" s="62">
+      <c r="D50" s="65">
         <v>2</v>
       </c>
-      <c r="E50" s="63"/>
-      <c r="F50" s="62">
+      <c r="E50" s="66"/>
+      <c r="F50" s="65">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G50" s="64"/>
+      <c r="G50" s="80"/>
       <c r="H50" s="26"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
@@ -10158,22 +10160,22 @@
       <c r="GI50" s="36"/>
     </row>
     <row r="51" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A51" s="66" t="s">
+      <c r="A51" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="67"/>
+      <c r="B51" s="82"/>
       <c r="C51" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D51" s="62">
+      <c r="D51" s="65">
         <v>2</v>
       </c>
-      <c r="E51" s="63"/>
-      <c r="F51" s="62">
+      <c r="E51" s="66"/>
+      <c r="F51" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G51" s="64"/>
+      <c r="G51" s="80"/>
       <c r="H51" s="26"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
@@ -10360,22 +10362,22 @@
       <c r="GI51" s="36"/>
     </row>
     <row r="52" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A52" s="66" t="s">
+      <c r="A52" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="67"/>
+      <c r="B52" s="82"/>
       <c r="C52" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="62">
+      <c r="D52" s="65">
         <v>2</v>
       </c>
-      <c r="E52" s="63"/>
-      <c r="F52" s="62">
+      <c r="E52" s="66"/>
+      <c r="F52" s="65">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G52" s="64"/>
+      <c r="G52" s="80"/>
       <c r="H52" s="26"/>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
@@ -10566,22 +10568,22 @@
       <c r="GI52" s="36"/>
     </row>
     <row r="53" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A53" s="66" t="s">
+      <c r="A53" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="67"/>
+      <c r="B53" s="82"/>
       <c r="C53" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D53" s="62">
+      <c r="D53" s="65">
         <v>2</v>
       </c>
-      <c r="E53" s="63"/>
-      <c r="F53" s="62">
+      <c r="E53" s="66"/>
+      <c r="F53" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G53" s="64"/>
+      <c r="G53" s="80"/>
       <c r="H53" s="26"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
@@ -10768,22 +10770,22 @@
       <c r="GI53" s="36"/>
     </row>
     <row r="54" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A54" s="66" t="s">
+      <c r="A54" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="67"/>
+      <c r="B54" s="82"/>
       <c r="C54" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="D54" s="62">
+      <c r="D54" s="65">
         <v>0.25</v>
       </c>
-      <c r="E54" s="63"/>
-      <c r="F54" s="62">
+      <c r="E54" s="66"/>
+      <c r="F54" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G54" s="64"/>
+      <c r="G54" s="80"/>
       <c r="H54" s="26"/>
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
@@ -10970,22 +10972,22 @@
       <c r="GI54" s="36"/>
     </row>
     <row r="55" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A55" s="66" t="s">
+      <c r="A55" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="67"/>
+      <c r="B55" s="82"/>
       <c r="C55" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="D55" s="62">
+      <c r="D55" s="65">
         <v>1</v>
       </c>
-      <c r="E55" s="63"/>
-      <c r="F55" s="62">
+      <c r="E55" s="66"/>
+      <c r="F55" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G55" s="64"/>
+      <c r="G55" s="80"/>
       <c r="H55" s="26"/>
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
@@ -11172,22 +11174,22 @@
       <c r="GI55" s="36"/>
     </row>
     <row r="56" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A56" s="66" t="s">
+      <c r="A56" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="67"/>
+      <c r="B56" s="82"/>
       <c r="C56" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="D56" s="62">
+      <c r="D56" s="65">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E56" s="63"/>
-      <c r="F56" s="62">
+      <c r="E56" s="66"/>
+      <c r="F56" s="65">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G56" s="64"/>
+      <c r="G56" s="80"/>
       <c r="H56" s="26"/>
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
@@ -11378,22 +11380,22 @@
       <c r="GI56" s="36"/>
     </row>
     <row r="57" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A57" s="66" t="s">
+      <c r="A57" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="67"/>
+      <c r="B57" s="82"/>
       <c r="C57" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="D57" s="62">
+      <c r="D57" s="65">
         <v>1.75</v>
       </c>
-      <c r="E57" s="63"/>
-      <c r="F57" s="62">
+      <c r="E57" s="66"/>
+      <c r="F57" s="65">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G57" s="64"/>
+      <c r="G57" s="80"/>
       <c r="H57" s="26"/>
       <c r="I57" s="12"/>
       <c r="J57" s="12"/>
@@ -11582,22 +11584,22 @@
       <c r="GI57" s="36"/>
     </row>
     <row r="58" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A58" s="66" t="s">
+      <c r="A58" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="B58" s="67"/>
+      <c r="B58" s="82"/>
       <c r="C58" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="D58" s="62">
+      <c r="D58" s="65">
         <v>0.6</v>
       </c>
-      <c r="E58" s="63"/>
-      <c r="F58" s="62">
+      <c r="E58" s="66"/>
+      <c r="F58" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G58" s="64"/>
+      <c r="G58" s="80"/>
       <c r="H58" s="26"/>
       <c r="I58" s="12"/>
       <c r="J58" s="12"/>
@@ -11784,22 +11786,22 @@
       <c r="GI58" s="36"/>
     </row>
     <row r="59" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="66" t="s">
+      <c r="A59" s="81" t="s">
         <v>111</v>
       </c>
-      <c r="B59" s="67"/>
+      <c r="B59" s="82"/>
       <c r="C59" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="62">
+      <c r="D59" s="65">
         <v>1</v>
       </c>
-      <c r="E59" s="63"/>
-      <c r="F59" s="62">
+      <c r="E59" s="66"/>
+      <c r="F59" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G59" s="64"/>
+      <c r="G59" s="80"/>
       <c r="H59" s="26"/>
       <c r="I59" s="12"/>
       <c r="J59" s="12"/>
@@ -11986,22 +11988,22 @@
       <c r="GI59" s="36"/>
     </row>
     <row r="60" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A60" s="66" t="s">
+      <c r="A60" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="B60" s="67"/>
+      <c r="B60" s="82"/>
       <c r="C60" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="D60" s="62">
+      <c r="D60" s="65">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E60" s="63"/>
-      <c r="F60" s="62">
+      <c r="E60" s="66"/>
+      <c r="F60" s="65">
         <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
-      <c r="G60" s="64"/>
+      <c r="G60" s="80"/>
       <c r="H60" s="26"/>
       <c r="I60" s="12"/>
       <c r="J60" s="12"/>
@@ -12190,22 +12192,22 @@
       <c r="GI60" s="36"/>
     </row>
     <row r="61" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A61" s="66" t="s">
+      <c r="A61" s="81" t="s">
         <v>115</v>
       </c>
-      <c r="B61" s="67"/>
+      <c r="B61" s="82"/>
       <c r="C61" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="D61" s="62">
+      <c r="D61" s="65">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E61" s="63"/>
-      <c r="F61" s="62">
+      <c r="E61" s="66"/>
+      <c r="F61" s="65">
         <f>SUM(H61:GI61)</f>
         <v>1</v>
       </c>
-      <c r="G61" s="64"/>
+      <c r="G61" s="80"/>
       <c r="H61" s="26"/>
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
@@ -12394,21 +12396,21 @@
       <c r="GI61" s="36"/>
     </row>
     <row r="62" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A62" s="76" t="s">
+      <c r="A62" s="115" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="77"/>
+      <c r="B62" s="116"/>
       <c r="C62" s="39"/>
-      <c r="D62" s="78">
+      <c r="D62" s="71">
         <f>SUM(D63:E80)</f>
         <v>88.6</v>
       </c>
-      <c r="E62" s="79"/>
-      <c r="F62" s="78">
+      <c r="E62" s="117"/>
+      <c r="F62" s="71">
         <f>SUM(F63:G80)</f>
         <v>0</v>
       </c>
-      <c r="G62" s="80"/>
+      <c r="G62" s="75"/>
       <c r="H62" s="29"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
@@ -12595,22 +12597,22 @@
       <c r="GI62" s="29"/>
     </row>
     <row r="63" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="60" t="s">
+      <c r="A63" s="118" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="61"/>
+      <c r="B63" s="119"/>
       <c r="C63" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D63" s="62">
+      <c r="D63" s="65">
         <v>0.6</v>
       </c>
-      <c r="E63" s="63"/>
-      <c r="F63" s="62">
+      <c r="E63" s="66"/>
+      <c r="F63" s="65">
         <f>SUM(H63:GI63)</f>
         <v>0</v>
       </c>
-      <c r="G63" s="64"/>
+      <c r="G63" s="80"/>
       <c r="H63" s="47"/>
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
@@ -12797,22 +12799,22 @@
       <c r="GI63" s="32"/>
     </row>
     <row r="64" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="60" t="s">
+      <c r="A64" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="B64" s="61"/>
+      <c r="B64" s="119"/>
       <c r="C64" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D64" s="62">
+      <c r="D64" s="65">
         <v>1.5</v>
       </c>
-      <c r="E64" s="63"/>
-      <c r="F64" s="62">
+      <c r="E64" s="66"/>
+      <c r="F64" s="65">
         <f>SUM(H64:GI64)</f>
         <v>0</v>
       </c>
-      <c r="G64" s="64"/>
+      <c r="G64" s="80"/>
       <c r="H64" s="47"/>
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
@@ -12999,22 +13001,22 @@
       <c r="GI64" s="32"/>
     </row>
     <row r="65" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A65" s="60" t="s">
+      <c r="A65" s="118" t="s">
         <v>123</v>
       </c>
-      <c r="B65" s="61"/>
+      <c r="B65" s="119"/>
       <c r="C65" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D65" s="62">
+      <c r="D65" s="65">
         <v>1</v>
       </c>
-      <c r="E65" s="63"/>
-      <c r="F65" s="62">
+      <c r="E65" s="66"/>
+      <c r="F65" s="65">
         <f t="shared" ref="F65:F80" si="1">SUM(H65:GI65)</f>
         <v>0</v>
       </c>
-      <c r="G65" s="64"/>
+      <c r="G65" s="80"/>
       <c r="H65" s="47"/>
       <c r="I65" s="12"/>
       <c r="J65" s="12"/>
@@ -13201,22 +13203,22 @@
       <c r="GI65" s="32"/>
     </row>
     <row r="66" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A66" s="60" t="s">
+      <c r="A66" s="118" t="s">
         <v>125</v>
       </c>
-      <c r="B66" s="61"/>
+      <c r="B66" s="119"/>
       <c r="C66" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D66" s="62">
+      <c r="D66" s="65">
         <v>0.5</v>
       </c>
-      <c r="E66" s="63"/>
-      <c r="F66" s="62">
+      <c r="E66" s="66"/>
+      <c r="F66" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G66" s="64"/>
+      <c r="G66" s="80"/>
       <c r="H66" s="47"/>
       <c r="I66" s="12"/>
       <c r="J66" s="12"/>
@@ -13403,22 +13405,22 @@
       <c r="GI66" s="32"/>
     </row>
     <row r="67" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A67" s="60" t="s">
+      <c r="A67" s="118" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="61"/>
+      <c r="B67" s="119"/>
       <c r="C67" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D67" s="62">
+      <c r="D67" s="65">
         <v>1</v>
       </c>
-      <c r="E67" s="63"/>
-      <c r="F67" s="62">
+      <c r="E67" s="66"/>
+      <c r="F67" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G67" s="64"/>
+      <c r="G67" s="80"/>
       <c r="H67" s="47"/>
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
@@ -13605,22 +13607,22 @@
       <c r="GI67" s="32"/>
     </row>
     <row r="68" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A68" s="60" t="s">
+      <c r="A68" s="118" t="s">
         <v>129</v>
       </c>
-      <c r="B68" s="61"/>
+      <c r="B68" s="119"/>
       <c r="C68" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D68" s="62">
+      <c r="D68" s="65">
         <v>1</v>
       </c>
-      <c r="E68" s="63"/>
-      <c r="F68" s="62">
+      <c r="E68" s="66"/>
+      <c r="F68" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G68" s="64"/>
+      <c r="G68" s="80"/>
       <c r="H68" s="47"/>
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
@@ -13807,22 +13809,22 @@
       <c r="GI68" s="32"/>
     </row>
     <row r="69" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A69" s="60" t="s">
+      <c r="A69" s="118" t="s">
         <v>131</v>
       </c>
-      <c r="B69" s="61"/>
+      <c r="B69" s="119"/>
       <c r="C69" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="D69" s="62">
+      <c r="D69" s="65">
         <v>4</v>
       </c>
-      <c r="E69" s="63"/>
-      <c r="F69" s="62">
+      <c r="E69" s="66"/>
+      <c r="F69" s="65">
         <f>SUM(H69:GI69)</f>
         <v>0</v>
       </c>
-      <c r="G69" s="64"/>
+      <c r="G69" s="80"/>
       <c r="H69" s="47"/>
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
@@ -14009,22 +14011,22 @@
       <c r="GI69" s="32"/>
     </row>
     <row r="70" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A70" s="60" t="s">
+      <c r="A70" s="118" t="s">
         <v>133</v>
       </c>
-      <c r="B70" s="61"/>
+      <c r="B70" s="119"/>
       <c r="C70" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="D70" s="62">
+      <c r="D70" s="65">
         <v>8</v>
       </c>
-      <c r="E70" s="63"/>
-      <c r="F70" s="62">
+      <c r="E70" s="66"/>
+      <c r="F70" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G70" s="64"/>
+      <c r="G70" s="80"/>
       <c r="H70" s="47"/>
       <c r="I70" s="12"/>
       <c r="J70" s="12"/>
@@ -14211,22 +14213,22 @@
       <c r="GI70" s="32"/>
     </row>
     <row r="71" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A71" s="60" t="s">
+      <c r="A71" s="118" t="s">
         <v>135</v>
       </c>
-      <c r="B71" s="61"/>
+      <c r="B71" s="119"/>
       <c r="C71" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="D71" s="62">
+      <c r="D71" s="65">
         <v>1</v>
       </c>
-      <c r="E71" s="63"/>
-      <c r="F71" s="62">
+      <c r="E71" s="66"/>
+      <c r="F71" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G71" s="64"/>
+      <c r="G71" s="80"/>
       <c r="H71" s="47"/>
       <c r="I71" s="12"/>
       <c r="J71" s="12"/>
@@ -14413,22 +14415,22 @@
       <c r="GI71" s="32"/>
     </row>
     <row r="72" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A72" s="60" t="s">
+      <c r="A72" s="118" t="s">
         <v>137</v>
       </c>
-      <c r="B72" s="61"/>
+      <c r="B72" s="119"/>
       <c r="C72" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="D72" s="62">
+      <c r="D72" s="65">
         <v>1</v>
       </c>
-      <c r="E72" s="63"/>
-      <c r="F72" s="62">
+      <c r="E72" s="66"/>
+      <c r="F72" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G72" s="64"/>
+      <c r="G72" s="80"/>
       <c r="H72" s="47"/>
       <c r="I72" s="12"/>
       <c r="J72" s="12"/>
@@ -14615,22 +14617,22 @@
       <c r="GI72" s="32"/>
     </row>
     <row r="73" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A73" s="60" t="s">
+      <c r="A73" s="118" t="s">
         <v>47</v>
       </c>
-      <c r="B73" s="61"/>
+      <c r="B73" s="119"/>
       <c r="C73" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="D73" s="62">
+      <c r="D73" s="65">
         <v>4</v>
       </c>
-      <c r="E73" s="63"/>
-      <c r="F73" s="62">
+      <c r="E73" s="66"/>
+      <c r="F73" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G73" s="64"/>
+      <c r="G73" s="80"/>
       <c r="H73" s="47"/>
       <c r="I73" s="12"/>
       <c r="J73" s="12"/>
@@ -14817,22 +14819,22 @@
       <c r="GI73" s="32"/>
     </row>
     <row r="74" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A74" s="60" t="s">
+      <c r="A74" s="118" t="s">
         <v>140</v>
       </c>
-      <c r="B74" s="61"/>
+      <c r="B74" s="119"/>
       <c r="C74" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="D74" s="62">
+      <c r="D74" s="65">
         <v>12</v>
       </c>
-      <c r="E74" s="63"/>
-      <c r="F74" s="62">
+      <c r="E74" s="66"/>
+      <c r="F74" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G74" s="64"/>
+      <c r="G74" s="80"/>
       <c r="H74" s="47"/>
       <c r="I74" s="12"/>
       <c r="J74" s="12"/>
@@ -15019,22 +15021,22 @@
       <c r="GI74" s="32"/>
     </row>
     <row r="75" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A75" s="60" t="s">
+      <c r="A75" s="118" t="s">
         <v>142</v>
       </c>
-      <c r="B75" s="65"/>
+      <c r="B75" s="88"/>
       <c r="C75" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D75" s="62">
+      <c r="D75" s="65">
         <v>16</v>
       </c>
-      <c r="E75" s="63"/>
-      <c r="F75" s="62">
+      <c r="E75" s="66"/>
+      <c r="F75" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G75" s="64"/>
+      <c r="G75" s="80"/>
       <c r="H75" s="47"/>
       <c r="I75" s="12"/>
       <c r="J75" s="12"/>
@@ -15221,22 +15223,22 @@
       <c r="GI75" s="36"/>
     </row>
     <row r="76" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A76" s="60" t="s">
+      <c r="A76" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B76" s="61"/>
+      <c r="B76" s="119"/>
       <c r="C76" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="D76" s="62">
+      <c r="D76" s="65">
         <v>5</v>
       </c>
-      <c r="E76" s="63"/>
-      <c r="F76" s="62">
+      <c r="E76" s="66"/>
+      <c r="F76" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G76" s="64"/>
+      <c r="G76" s="80"/>
       <c r="H76" s="47"/>
       <c r="I76" s="12"/>
       <c r="J76" s="12"/>
@@ -15423,22 +15425,22 @@
       <c r="GI76" s="32"/>
     </row>
     <row r="77" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A77" s="60" t="s">
+      <c r="A77" s="118" t="s">
         <v>146</v>
       </c>
-      <c r="B77" s="61"/>
+      <c r="B77" s="119"/>
       <c r="C77" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="D77" s="62">
+      <c r="D77" s="65">
         <v>4</v>
       </c>
-      <c r="E77" s="63"/>
-      <c r="F77" s="62">
+      <c r="E77" s="66"/>
+      <c r="F77" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G77" s="64"/>
+      <c r="G77" s="80"/>
       <c r="H77" s="47"/>
       <c r="I77" s="12"/>
       <c r="J77" s="12"/>
@@ -15625,22 +15627,22 @@
       <c r="GI77" s="32"/>
     </row>
     <row r="78" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A78" s="60" t="s">
+      <c r="A78" s="118" t="s">
         <v>148</v>
       </c>
-      <c r="B78" s="61"/>
+      <c r="B78" s="119"/>
       <c r="C78" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="D78" s="62">
+      <c r="D78" s="65">
         <v>16</v>
       </c>
-      <c r="E78" s="63"/>
-      <c r="F78" s="62">
+      <c r="E78" s="66"/>
+      <c r="F78" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G78" s="64"/>
+      <c r="G78" s="80"/>
       <c r="H78" s="47"/>
       <c r="I78" s="12"/>
       <c r="J78" s="12"/>
@@ -15827,22 +15829,22 @@
       <c r="GI78" s="32"/>
     </row>
     <row r="79" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A79" s="82" t="s">
+      <c r="A79" s="73" t="s">
         <v>150</v>
       </c>
-      <c r="B79" s="83"/>
+      <c r="B79" s="74"/>
       <c r="C79" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="D79" s="62">
+      <c r="D79" s="65">
         <v>6</v>
       </c>
-      <c r="E79" s="63"/>
-      <c r="F79" s="62">
+      <c r="E79" s="66"/>
+      <c r="F79" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G79" s="64"/>
+      <c r="G79" s="80"/>
       <c r="H79" s="47"/>
       <c r="I79" s="12"/>
       <c r="J79" s="12"/>
@@ -16029,22 +16031,22 @@
       <c r="GI79" s="36"/>
     </row>
     <row r="80" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A80" s="82" t="s">
+      <c r="A80" s="73" t="s">
         <v>152</v>
       </c>
-      <c r="B80" s="83"/>
+      <c r="B80" s="74"/>
       <c r="C80" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D80" s="62">
+      <c r="D80" s="65">
         <v>6</v>
       </c>
-      <c r="E80" s="63"/>
-      <c r="F80" s="62">
+      <c r="E80" s="66"/>
+      <c r="F80" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G80" s="64"/>
+      <c r="G80" s="80"/>
       <c r="H80" s="47"/>
       <c r="I80" s="12"/>
       <c r="J80" s="12"/>
@@ -16231,21 +16233,21 @@
       <c r="GI80" s="36"/>
     </row>
     <row r="81" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A81" s="76" t="s">
+      <c r="A81" s="115" t="s">
         <v>153</v>
       </c>
-      <c r="B81" s="77"/>
+      <c r="B81" s="116"/>
       <c r="C81" s="39"/>
-      <c r="D81" s="78">
+      <c r="D81" s="71">
         <f>SUM(D82:E82)</f>
         <v>16</v>
       </c>
-      <c r="E81" s="88"/>
-      <c r="F81" s="78">
+      <c r="E81" s="72"/>
+      <c r="F81" s="71">
         <f>SUM(F82:G82)</f>
         <v>0</v>
       </c>
-      <c r="G81" s="80"/>
+      <c r="G81" s="75"/>
       <c r="H81" s="29"/>
       <c r="I81" s="8"/>
       <c r="J81" s="8"/>
@@ -16432,20 +16434,20 @@
       <c r="GI81" s="29"/>
     </row>
     <row r="82" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A82" s="86" t="s">
+      <c r="A82" s="93" t="s">
         <v>153</v>
       </c>
-      <c r="B82" s="87"/>
+      <c r="B82" s="94"/>
       <c r="C82" s="40"/>
-      <c r="D82" s="84">
+      <c r="D82" s="91">
         <v>16</v>
       </c>
-      <c r="E82" s="85"/>
-      <c r="F82" s="62">
+      <c r="E82" s="92"/>
+      <c r="F82" s="65">
         <f>SUM(H82:GI82)</f>
         <v>0</v>
       </c>
-      <c r="G82" s="64"/>
+      <c r="G82" s="80"/>
       <c r="H82" s="26"/>
       <c r="I82" s="12"/>
       <c r="J82" s="12"/>
@@ -16632,21 +16634,21 @@
       <c r="GI82" s="32"/>
     </row>
     <row r="83" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A83" s="104" t="s">
+      <c r="A83" s="110" t="s">
         <v>154</v>
       </c>
-      <c r="B83" s="105"/>
+      <c r="B83" s="111"/>
       <c r="C83" s="41"/>
-      <c r="D83" s="78">
+      <c r="D83" s="71">
         <f>SUM(D84:E84)</f>
         <v>32</v>
       </c>
-      <c r="E83" s="88"/>
-      <c r="F83" s="78">
+      <c r="E83" s="72"/>
+      <c r="F83" s="71">
         <f>SUM(F84:G84)</f>
         <v>0</v>
       </c>
-      <c r="G83" s="80"/>
+      <c r="G83" s="75"/>
       <c r="H83" s="29"/>
       <c r="I83" s="8"/>
       <c r="J83" s="8"/>
@@ -16833,20 +16835,20 @@
       <c r="GI83" s="29"/>
     </row>
     <row r="84" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A84" s="108" t="s">
+      <c r="A84" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="B84" s="109"/>
+      <c r="B84" s="86"/>
       <c r="C84" s="42"/>
-      <c r="D84" s="62">
+      <c r="D84" s="65">
         <v>32</v>
       </c>
-      <c r="E84" s="63"/>
-      <c r="F84" s="62">
+      <c r="E84" s="66"/>
+      <c r="F84" s="65">
         <f>SUM(H84:GI84)</f>
         <v>0</v>
       </c>
-      <c r="G84" s="64"/>
+      <c r="G84" s="80"/>
       <c r="H84" s="26"/>
       <c r="I84" s="12"/>
       <c r="J84" s="12"/>
@@ -17033,21 +17035,21 @@
       <c r="GI84" s="32"/>
     </row>
     <row r="85" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A85" s="111" t="s">
+      <c r="A85" s="89" t="s">
         <v>155</v>
       </c>
-      <c r="B85" s="112"/>
+      <c r="B85" s="90"/>
       <c r="C85" s="43"/>
-      <c r="D85" s="78">
+      <c r="D85" s="71">
         <f>SUM(D86:E86)</f>
         <v>8</v>
       </c>
-      <c r="E85" s="88"/>
-      <c r="F85" s="89">
+      <c r="E85" s="72"/>
+      <c r="F85" s="95">
         <f>SUM(F86:G86)</f>
         <v>0</v>
       </c>
-      <c r="G85" s="90"/>
+      <c r="G85" s="96"/>
       <c r="H85" s="29"/>
       <c r="I85" s="8"/>
       <c r="J85" s="8"/>
@@ -17234,20 +17236,20 @@
       <c r="GI85" s="29"/>
     </row>
     <row r="86" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A86" s="110" t="s">
+      <c r="A86" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="B86" s="65"/>
+      <c r="B86" s="88"/>
       <c r="C86" s="27"/>
-      <c r="D86" s="62">
+      <c r="D86" s="65">
         <v>8</v>
       </c>
-      <c r="E86" s="63"/>
-      <c r="F86" s="62">
+      <c r="E86" s="66"/>
+      <c r="F86" s="65">
         <f>SUM(H86:GI86)</f>
         <v>0</v>
       </c>
-      <c r="G86" s="64"/>
+      <c r="G86" s="80"/>
       <c r="H86" s="26"/>
       <c r="I86" s="12"/>
       <c r="J86" s="12"/>
@@ -17434,20 +17436,20 @@
       <c r="GI86" s="32"/>
     </row>
     <row r="87" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A87" s="106" t="s">
+      <c r="A87" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="107"/>
+      <c r="B87" s="84"/>
       <c r="C87" s="43"/>
-      <c r="D87" s="78">
+      <c r="D87" s="71">
         <f>232-D90</f>
         <v>36.349999999999994</v>
       </c>
-      <c r="E87" s="88"/>
-      <c r="F87" s="78">
+      <c r="E87" s="72"/>
+      <c r="F87" s="71">
         <v>0</v>
       </c>
-      <c r="G87" s="80"/>
+      <c r="G87" s="75"/>
       <c r="H87" s="29"/>
       <c r="I87" s="8"/>
       <c r="J87" s="8"/>
@@ -17634,15 +17636,15 @@
       <c r="GI87" s="29"/>
     </row>
     <row r="88" spans="1:191" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="101" t="s">
+      <c r="A88" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="B88" s="102"/>
+      <c r="B88" s="108"/>
       <c r="C88" s="44"/>
-      <c r="D88" s="98"/>
-      <c r="E88" s="99"/>
-      <c r="F88" s="98"/>
-      <c r="G88" s="100"/>
+      <c r="D88" s="104"/>
+      <c r="E88" s="105"/>
+      <c r="F88" s="104"/>
+      <c r="G88" s="106"/>
       <c r="H88" s="28"/>
       <c r="I88" s="17"/>
       <c r="J88" s="17"/>
@@ -17881,21 +17883,21 @@
       <c r="AX89" s="3"/>
     </row>
     <row r="90" spans="1:191" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="96" t="s">
+      <c r="A90" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="97"/>
+      <c r="B90" s="103"/>
       <c r="C90" s="45"/>
-      <c r="D90" s="94">
+      <c r="D90" s="100">
         <f>SUM(D85,D83,D81,D62,D14)</f>
         <v>195.65</v>
       </c>
-      <c r="E90" s="95"/>
-      <c r="F90" s="94">
+      <c r="E90" s="101"/>
+      <c r="F90" s="100">
         <f>SUM(F85,F83,F81,F62,F14)</f>
-        <v>33.25</v>
-      </c>
-      <c r="G90" s="103"/>
+        <v>33.416000000000004</v>
+      </c>
+      <c r="G90" s="109"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
@@ -17942,6 +17944,316 @@
     </row>
   </sheetData>
   <mergeCells count="334">
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="GD13:GE13"/>
+    <mergeCell ref="GF13:GG13"/>
+    <mergeCell ref="GH13:GI13"/>
+    <mergeCell ref="DZ12:GI12"/>
+    <mergeCell ref="FL13:FM13"/>
+    <mergeCell ref="FN13:FO13"/>
+    <mergeCell ref="FP13:FQ13"/>
+    <mergeCell ref="FR13:FS13"/>
+    <mergeCell ref="FT13:FU13"/>
+    <mergeCell ref="FV13:FW13"/>
+    <mergeCell ref="FX13:FY13"/>
+    <mergeCell ref="FZ13:GA13"/>
+    <mergeCell ref="GB13:GC13"/>
+    <mergeCell ref="ET13:EU13"/>
+    <mergeCell ref="EV13:EW13"/>
+    <mergeCell ref="EX13:EY13"/>
+    <mergeCell ref="EZ13:FA13"/>
+    <mergeCell ref="FB13:FC13"/>
+    <mergeCell ref="FD13:FE13"/>
+    <mergeCell ref="FF13:FG13"/>
+    <mergeCell ref="DX13:DY13"/>
+    <mergeCell ref="FH13:FI13"/>
+    <mergeCell ref="FJ13:FK13"/>
+    <mergeCell ref="EB13:EC13"/>
+    <mergeCell ref="ED13:EE13"/>
+    <mergeCell ref="EF13:EG13"/>
+    <mergeCell ref="EH13:EI13"/>
+    <mergeCell ref="EJ13:EK13"/>
+    <mergeCell ref="EL13:EM13"/>
+    <mergeCell ref="EN13:EO13"/>
+    <mergeCell ref="EP13:EQ13"/>
+    <mergeCell ref="ER13:ES13"/>
+    <mergeCell ref="DF13:DG13"/>
+    <mergeCell ref="DH13:DI13"/>
+    <mergeCell ref="DJ13:DK13"/>
+    <mergeCell ref="DL13:DM13"/>
+    <mergeCell ref="DN13:DO13"/>
+    <mergeCell ref="DP13:DQ13"/>
+    <mergeCell ref="DR13:DS13"/>
+    <mergeCell ref="DT13:DU13"/>
+    <mergeCell ref="DV13:DW13"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="BH13:BI13"/>
+    <mergeCell ref="BJ13:BK13"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="P9:X9"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F11:G13"/>
+    <mergeCell ref="D11:E13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="AL13:AM13"/>
+    <mergeCell ref="AN13:AO13"/>
+    <mergeCell ref="AP13:AQ13"/>
+    <mergeCell ref="AR13:AS13"/>
+    <mergeCell ref="AT13:AU13"/>
+    <mergeCell ref="AV13:AW13"/>
+    <mergeCell ref="AX13:AY13"/>
+    <mergeCell ref="AZ13:BA13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="P6:X6"/>
+    <mergeCell ref="P5:X5"/>
+    <mergeCell ref="P4:X4"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="H12:BQ12"/>
+    <mergeCell ref="BB13:BC13"/>
+    <mergeCell ref="BD13:BE13"/>
+    <mergeCell ref="BF13:BG13"/>
+    <mergeCell ref="BP13:BQ13"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="AF13:AG13"/>
+    <mergeCell ref="AH13:AI13"/>
+    <mergeCell ref="AJ13:AK13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
     <mergeCell ref="BR13:BS13"/>
     <mergeCell ref="BL13:BM13"/>
     <mergeCell ref="BN13:BO13"/>
@@ -17966,316 +18278,6 @@
     <mergeCell ref="CZ13:DA13"/>
     <mergeCell ref="DB13:DC13"/>
     <mergeCell ref="DD13:DE13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="P6:X6"/>
-    <mergeCell ref="P5:X5"/>
-    <mergeCell ref="P4:X4"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="H12:BQ12"/>
-    <mergeCell ref="BB13:BC13"/>
-    <mergeCell ref="BD13:BE13"/>
-    <mergeCell ref="BF13:BG13"/>
-    <mergeCell ref="BP13:BQ13"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="AF13:AG13"/>
-    <mergeCell ref="AH13:AI13"/>
-    <mergeCell ref="AJ13:AK13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="AL13:AM13"/>
-    <mergeCell ref="AN13:AO13"/>
-    <mergeCell ref="AP13:AQ13"/>
-    <mergeCell ref="AR13:AS13"/>
-    <mergeCell ref="AT13:AU13"/>
-    <mergeCell ref="AV13:AW13"/>
-    <mergeCell ref="AX13:AY13"/>
-    <mergeCell ref="AZ13:BA13"/>
-    <mergeCell ref="BH13:BI13"/>
-    <mergeCell ref="BJ13:BK13"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="P9:X9"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F11:G13"/>
-    <mergeCell ref="D11:E13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="F90:G90"/>
-    <mergeCell ref="F87:G87"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="DF13:DG13"/>
-    <mergeCell ref="DH13:DI13"/>
-    <mergeCell ref="DJ13:DK13"/>
-    <mergeCell ref="DL13:DM13"/>
-    <mergeCell ref="DN13:DO13"/>
-    <mergeCell ref="DP13:DQ13"/>
-    <mergeCell ref="DR13:DS13"/>
-    <mergeCell ref="DT13:DU13"/>
-    <mergeCell ref="DV13:DW13"/>
-    <mergeCell ref="FF13:FG13"/>
-    <mergeCell ref="DX13:DY13"/>
-    <mergeCell ref="FH13:FI13"/>
-    <mergeCell ref="FJ13:FK13"/>
-    <mergeCell ref="EB13:EC13"/>
-    <mergeCell ref="ED13:EE13"/>
-    <mergeCell ref="EF13:EG13"/>
-    <mergeCell ref="EH13:EI13"/>
-    <mergeCell ref="EJ13:EK13"/>
-    <mergeCell ref="EL13:EM13"/>
-    <mergeCell ref="EN13:EO13"/>
-    <mergeCell ref="EP13:EQ13"/>
-    <mergeCell ref="ER13:ES13"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="GD13:GE13"/>
-    <mergeCell ref="GF13:GG13"/>
-    <mergeCell ref="GH13:GI13"/>
-    <mergeCell ref="DZ12:GI12"/>
-    <mergeCell ref="FL13:FM13"/>
-    <mergeCell ref="FN13:FO13"/>
-    <mergeCell ref="FP13:FQ13"/>
-    <mergeCell ref="FR13:FS13"/>
-    <mergeCell ref="FT13:FU13"/>
-    <mergeCell ref="FV13:FW13"/>
-    <mergeCell ref="FX13:FY13"/>
-    <mergeCell ref="FZ13:GA13"/>
-    <mergeCell ref="GB13:GC13"/>
-    <mergeCell ref="ET13:EU13"/>
-    <mergeCell ref="EV13:EW13"/>
-    <mergeCell ref="EX13:EY13"/>
-    <mergeCell ref="EZ13:FA13"/>
-    <mergeCell ref="FB13:FC13"/>
-    <mergeCell ref="FD13:FE13"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Created Model for Issue #41
</commit_message>
<xml_diff>
--- a/Documents/Zeitplan.xlsx
+++ b/Documents/Zeitplan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VirtualReality\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VirtualReality\Documents\SiemensVR\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1164,6 +1164,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1176,32 +1194,31 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1209,42 +1226,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1253,6 +1234,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1300,24 +1284,40 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1787,40 +1787,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GI90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AM21" sqref="AM21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AM25" sqref="AM25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="191" width="5.77734375" style="1" customWidth="1"/>
+    <col min="1" max="38" width="5.77734375" style="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="191" width="5.77734375" style="1" customWidth="1"/>
     <col min="192" max="256" width="3.33203125" style="1" customWidth="1"/>
     <col min="257" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:191" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="112"/>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="112"/>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
     </row>
     <row r="2" spans="1:191" x14ac:dyDescent="0.25">
       <c r="T2" s="9"/>
@@ -1853,17 +1855,17 @@
         <v>160</v>
       </c>
       <c r="N4" s="57"/>
-      <c r="P4" s="67" t="s">
+      <c r="P4" s="81" t="s">
         <v>157</v>
       </c>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="67"/>
-      <c r="W4" s="67"/>
-      <c r="X4" s="67"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="81"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
     </row>
     <row r="5" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -1880,17 +1882,17 @@
       <c r="F5" s="5"/>
       <c r="G5" s="7"/>
       <c r="N5" s="24"/>
-      <c r="P5" s="67" t="s">
+      <c r="P5" s="81" t="s">
         <v>158</v>
       </c>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="67"/>
-      <c r="S5" s="67"/>
-      <c r="T5" s="67"/>
-      <c r="U5" s="67"/>
-      <c r="V5" s="67"/>
-      <c r="W5" s="67"/>
-      <c r="X5" s="67"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="81"/>
+      <c r="S5" s="81"/>
+      <c r="T5" s="81"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
+      <c r="W5" s="81"/>
+      <c r="X5" s="81"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
@@ -1914,17 +1916,17 @@
         <v>15</v>
       </c>
       <c r="N6" s="16"/>
-      <c r="P6" s="67" t="s">
+      <c r="P6" s="81" t="s">
         <v>159</v>
       </c>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="67"/>
-      <c r="V6" s="67"/>
-      <c r="W6" s="67"/>
-      <c r="X6" s="67"/>
+      <c r="Q6" s="81"/>
+      <c r="R6" s="81"/>
+      <c r="S6" s="81"/>
+      <c r="T6" s="81"/>
+      <c r="U6" s="81"/>
+      <c r="V6" s="81"/>
+      <c r="W6" s="81"/>
+      <c r="X6" s="81"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
@@ -1942,17 +1944,17 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="N7" s="21"/>
-      <c r="P7" s="67" t="s">
+      <c r="P7" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="67"/>
-      <c r="R7" s="67"/>
-      <c r="S7" s="67"/>
-      <c r="T7" s="67"/>
-      <c r="U7" s="67"/>
-      <c r="V7" s="67"/>
-      <c r="W7" s="67"/>
-      <c r="X7" s="67"/>
+      <c r="Q7" s="81"/>
+      <c r="R7" s="81"/>
+      <c r="S7" s="81"/>
+      <c r="T7" s="81"/>
+      <c r="U7" s="81"/>
+      <c r="V7" s="81"/>
+      <c r="W7" s="81"/>
+      <c r="X7" s="81"/>
     </row>
     <row r="8" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1967,17 +1969,17 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="N8" s="20"/>
-      <c r="P8" s="70" t="s">
+      <c r="P8" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="70"/>
-      <c r="R8" s="70"/>
-      <c r="S8" s="70"/>
-      <c r="T8" s="70"/>
-      <c r="U8" s="70"/>
-      <c r="V8" s="70"/>
-      <c r="W8" s="70"/>
-      <c r="X8" s="70"/>
+      <c r="Q8" s="113"/>
+      <c r="R8" s="113"/>
+      <c r="S8" s="113"/>
+      <c r="T8" s="113"/>
+      <c r="U8" s="113"/>
+      <c r="V8" s="113"/>
+      <c r="W8" s="113"/>
+      <c r="X8" s="113"/>
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
@@ -1985,23 +1987,23 @@
       <c r="AC8" s="5"/>
     </row>
     <row r="9" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="68"/>
+      <c r="A9" s="118"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="12"/>
       <c r="N9" s="49"/>
-      <c r="P9" s="70" t="s">
+      <c r="P9" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="Q9" s="70"/>
-      <c r="R9" s="70"/>
-      <c r="S9" s="70"/>
-      <c r="T9" s="70"/>
-      <c r="U9" s="70"/>
-      <c r="V9" s="70"/>
-      <c r="W9" s="70"/>
-      <c r="X9" s="70"/>
+      <c r="Q9" s="113"/>
+      <c r="R9" s="113"/>
+      <c r="S9" s="113"/>
+      <c r="T9" s="113"/>
+      <c r="U9" s="113"/>
+      <c r="V9" s="113"/>
+      <c r="W9" s="113"/>
+      <c r="X9" s="113"/>
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
@@ -2011,7 +2013,7 @@
       <c r="AJ9" s="13"/>
     </row>
     <row r="10" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="68"/>
+      <c r="A10" s="118"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -2028,18 +2030,18 @@
       <c r="AC10" s="5"/>
     </row>
     <row r="11" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="68"/>
-      <c r="C11" s="78" t="s">
+      <c r="A11" s="118"/>
+      <c r="C11" s="116" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="76" t="s">
+      <c r="D11" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76" t="s">
+      <c r="E11" s="114"/>
+      <c r="F11" s="114" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="76"/>
+      <c r="G11" s="114"/>
       <c r="T11" s="9"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
@@ -2052,596 +2054,596 @@
       <c r="AC11" s="5"/>
     </row>
     <row r="12" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="68"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="62" t="s">
+      <c r="A12" s="118"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="114"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="114"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="63"/>
-      <c r="J12" s="63"/>
-      <c r="K12" s="63"/>
-      <c r="L12" s="63"/>
-      <c r="M12" s="63"/>
-      <c r="N12" s="63"/>
-      <c r="O12" s="63"/>
-      <c r="P12" s="63"/>
-      <c r="Q12" s="63"/>
-      <c r="R12" s="63"/>
-      <c r="S12" s="63"/>
-      <c r="T12" s="63"/>
-      <c r="U12" s="63"/>
-      <c r="V12" s="63"/>
-      <c r="W12" s="63"/>
-      <c r="X12" s="63"/>
-      <c r="Y12" s="63"/>
-      <c r="Z12" s="63"/>
-      <c r="AA12" s="63"/>
-      <c r="AB12" s="63"/>
-      <c r="AC12" s="63"/>
-      <c r="AD12" s="63"/>
-      <c r="AE12" s="63"/>
-      <c r="AF12" s="63"/>
-      <c r="AG12" s="63"/>
-      <c r="AH12" s="63"/>
-      <c r="AI12" s="63"/>
-      <c r="AJ12" s="63"/>
-      <c r="AK12" s="63"/>
-      <c r="AL12" s="63"/>
-      <c r="AM12" s="63"/>
-      <c r="AN12" s="63"/>
-      <c r="AO12" s="63"/>
-      <c r="AP12" s="63"/>
-      <c r="AQ12" s="63"/>
-      <c r="AR12" s="63"/>
-      <c r="AS12" s="63"/>
-      <c r="AT12" s="63"/>
-      <c r="AU12" s="63"/>
-      <c r="AV12" s="63"/>
-      <c r="AW12" s="63"/>
-      <c r="AX12" s="63"/>
-      <c r="AY12" s="63"/>
-      <c r="AZ12" s="63"/>
-      <c r="BA12" s="63"/>
-      <c r="BB12" s="63"/>
-      <c r="BC12" s="63"/>
-      <c r="BD12" s="63"/>
-      <c r="BE12" s="63"/>
-      <c r="BF12" s="63"/>
-      <c r="BG12" s="63"/>
-      <c r="BH12" s="63"/>
-      <c r="BI12" s="63"/>
-      <c r="BJ12" s="63"/>
-      <c r="BK12" s="63"/>
-      <c r="BL12" s="63"/>
-      <c r="BM12" s="63"/>
-      <c r="BN12" s="63"/>
-      <c r="BO12" s="63"/>
-      <c r="BP12" s="63"/>
-      <c r="BQ12" s="64"/>
-      <c r="BR12" s="62" t="s">
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="71"/>
+      <c r="O12" s="71"/>
+      <c r="P12" s="71"/>
+      <c r="Q12" s="71"/>
+      <c r="R12" s="71"/>
+      <c r="S12" s="71"/>
+      <c r="T12" s="71"/>
+      <c r="U12" s="71"/>
+      <c r="V12" s="71"/>
+      <c r="W12" s="71"/>
+      <c r="X12" s="71"/>
+      <c r="Y12" s="71"/>
+      <c r="Z12" s="71"/>
+      <c r="AA12" s="71"/>
+      <c r="AB12" s="71"/>
+      <c r="AC12" s="71"/>
+      <c r="AD12" s="71"/>
+      <c r="AE12" s="71"/>
+      <c r="AF12" s="71"/>
+      <c r="AG12" s="71"/>
+      <c r="AH12" s="71"/>
+      <c r="AI12" s="71"/>
+      <c r="AJ12" s="71"/>
+      <c r="AK12" s="71"/>
+      <c r="AL12" s="71"/>
+      <c r="AM12" s="71"/>
+      <c r="AN12" s="71"/>
+      <c r="AO12" s="71"/>
+      <c r="AP12" s="71"/>
+      <c r="AQ12" s="71"/>
+      <c r="AR12" s="71"/>
+      <c r="AS12" s="71"/>
+      <c r="AT12" s="71"/>
+      <c r="AU12" s="71"/>
+      <c r="AV12" s="71"/>
+      <c r="AW12" s="71"/>
+      <c r="AX12" s="71"/>
+      <c r="AY12" s="71"/>
+      <c r="AZ12" s="71"/>
+      <c r="BA12" s="71"/>
+      <c r="BB12" s="71"/>
+      <c r="BC12" s="71"/>
+      <c r="BD12" s="71"/>
+      <c r="BE12" s="71"/>
+      <c r="BF12" s="71"/>
+      <c r="BG12" s="71"/>
+      <c r="BH12" s="71"/>
+      <c r="BI12" s="71"/>
+      <c r="BJ12" s="71"/>
+      <c r="BK12" s="71"/>
+      <c r="BL12" s="71"/>
+      <c r="BM12" s="71"/>
+      <c r="BN12" s="71"/>
+      <c r="BO12" s="71"/>
+      <c r="BP12" s="71"/>
+      <c r="BQ12" s="119"/>
+      <c r="BR12" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="BS12" s="63"/>
-      <c r="BT12" s="63"/>
-      <c r="BU12" s="63"/>
-      <c r="BV12" s="63"/>
-      <c r="BW12" s="63"/>
-      <c r="BX12" s="63"/>
-      <c r="BY12" s="63"/>
-      <c r="BZ12" s="63"/>
-      <c r="CA12" s="63"/>
-      <c r="CB12" s="63"/>
-      <c r="CC12" s="63"/>
-      <c r="CD12" s="63"/>
-      <c r="CE12" s="63"/>
-      <c r="CF12" s="63"/>
-      <c r="CG12" s="63"/>
-      <c r="CH12" s="63"/>
-      <c r="CI12" s="63"/>
-      <c r="CJ12" s="63"/>
-      <c r="CK12" s="63"/>
-      <c r="CL12" s="63"/>
-      <c r="CM12" s="63"/>
-      <c r="CN12" s="63"/>
-      <c r="CO12" s="63"/>
-      <c r="CP12" s="63"/>
-      <c r="CQ12" s="63"/>
-      <c r="CR12" s="63"/>
-      <c r="CS12" s="63"/>
-      <c r="CT12" s="63"/>
-      <c r="CU12" s="63"/>
-      <c r="CV12" s="63"/>
-      <c r="CW12" s="63"/>
-      <c r="CX12" s="63"/>
-      <c r="CY12" s="63"/>
-      <c r="CZ12" s="63"/>
-      <c r="DA12" s="63"/>
-      <c r="DB12" s="63"/>
-      <c r="DC12" s="63"/>
-      <c r="DD12" s="63"/>
-      <c r="DE12" s="63"/>
-      <c r="DF12" s="63"/>
-      <c r="DG12" s="63"/>
-      <c r="DH12" s="63"/>
-      <c r="DI12" s="63"/>
-      <c r="DJ12" s="63"/>
-      <c r="DK12" s="63"/>
-      <c r="DL12" s="63"/>
-      <c r="DM12" s="63"/>
-      <c r="DN12" s="63"/>
-      <c r="DO12" s="63"/>
-      <c r="DP12" s="63"/>
-      <c r="DQ12" s="63"/>
-      <c r="DR12" s="63"/>
-      <c r="DS12" s="63"/>
-      <c r="DT12" s="63"/>
-      <c r="DU12" s="63"/>
-      <c r="DV12" s="63"/>
-      <c r="DW12" s="63"/>
-      <c r="DX12" s="63"/>
-      <c r="DY12" s="64"/>
-      <c r="DZ12" s="62" t="s">
+      <c r="BS12" s="71"/>
+      <c r="BT12" s="71"/>
+      <c r="BU12" s="71"/>
+      <c r="BV12" s="71"/>
+      <c r="BW12" s="71"/>
+      <c r="BX12" s="71"/>
+      <c r="BY12" s="71"/>
+      <c r="BZ12" s="71"/>
+      <c r="CA12" s="71"/>
+      <c r="CB12" s="71"/>
+      <c r="CC12" s="71"/>
+      <c r="CD12" s="71"/>
+      <c r="CE12" s="71"/>
+      <c r="CF12" s="71"/>
+      <c r="CG12" s="71"/>
+      <c r="CH12" s="71"/>
+      <c r="CI12" s="71"/>
+      <c r="CJ12" s="71"/>
+      <c r="CK12" s="71"/>
+      <c r="CL12" s="71"/>
+      <c r="CM12" s="71"/>
+      <c r="CN12" s="71"/>
+      <c r="CO12" s="71"/>
+      <c r="CP12" s="71"/>
+      <c r="CQ12" s="71"/>
+      <c r="CR12" s="71"/>
+      <c r="CS12" s="71"/>
+      <c r="CT12" s="71"/>
+      <c r="CU12" s="71"/>
+      <c r="CV12" s="71"/>
+      <c r="CW12" s="71"/>
+      <c r="CX12" s="71"/>
+      <c r="CY12" s="71"/>
+      <c r="CZ12" s="71"/>
+      <c r="DA12" s="71"/>
+      <c r="DB12" s="71"/>
+      <c r="DC12" s="71"/>
+      <c r="DD12" s="71"/>
+      <c r="DE12" s="71"/>
+      <c r="DF12" s="71"/>
+      <c r="DG12" s="71"/>
+      <c r="DH12" s="71"/>
+      <c r="DI12" s="71"/>
+      <c r="DJ12" s="71"/>
+      <c r="DK12" s="71"/>
+      <c r="DL12" s="71"/>
+      <c r="DM12" s="71"/>
+      <c r="DN12" s="71"/>
+      <c r="DO12" s="71"/>
+      <c r="DP12" s="71"/>
+      <c r="DQ12" s="71"/>
+      <c r="DR12" s="71"/>
+      <c r="DS12" s="71"/>
+      <c r="DT12" s="71"/>
+      <c r="DU12" s="71"/>
+      <c r="DV12" s="71"/>
+      <c r="DW12" s="71"/>
+      <c r="DX12" s="71"/>
+      <c r="DY12" s="119"/>
+      <c r="DZ12" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="EA12" s="63"/>
-      <c r="EB12" s="63"/>
-      <c r="EC12" s="63"/>
-      <c r="ED12" s="63"/>
-      <c r="EE12" s="63"/>
-      <c r="EF12" s="63"/>
-      <c r="EG12" s="63"/>
-      <c r="EH12" s="63"/>
-      <c r="EI12" s="63"/>
-      <c r="EJ12" s="63"/>
-      <c r="EK12" s="63"/>
-      <c r="EL12" s="63"/>
-      <c r="EM12" s="63"/>
-      <c r="EN12" s="63"/>
-      <c r="EO12" s="63"/>
-      <c r="EP12" s="63"/>
-      <c r="EQ12" s="63"/>
-      <c r="ER12" s="63"/>
-      <c r="ES12" s="63"/>
-      <c r="ET12" s="63"/>
-      <c r="EU12" s="63"/>
-      <c r="EV12" s="63"/>
-      <c r="EW12" s="63"/>
-      <c r="EX12" s="63"/>
-      <c r="EY12" s="63"/>
-      <c r="EZ12" s="63"/>
-      <c r="FA12" s="63"/>
-      <c r="FB12" s="63"/>
-      <c r="FC12" s="63"/>
-      <c r="FD12" s="63"/>
-      <c r="FE12" s="63"/>
-      <c r="FF12" s="63"/>
-      <c r="FG12" s="63"/>
-      <c r="FH12" s="63"/>
-      <c r="FI12" s="63"/>
-      <c r="FJ12" s="63"/>
-      <c r="FK12" s="63"/>
-      <c r="FL12" s="63"/>
-      <c r="FM12" s="63"/>
-      <c r="FN12" s="63"/>
-      <c r="FO12" s="63"/>
-      <c r="FP12" s="63"/>
-      <c r="FQ12" s="63"/>
-      <c r="FR12" s="63"/>
-      <c r="FS12" s="63"/>
-      <c r="FT12" s="63"/>
-      <c r="FU12" s="63"/>
-      <c r="FV12" s="63"/>
-      <c r="FW12" s="63"/>
-      <c r="FX12" s="63"/>
-      <c r="FY12" s="63"/>
-      <c r="FZ12" s="63"/>
-      <c r="GA12" s="63"/>
-      <c r="GB12" s="63"/>
-      <c r="GC12" s="63"/>
-      <c r="GD12" s="63"/>
-      <c r="GE12" s="63"/>
-      <c r="GF12" s="63"/>
-      <c r="GG12" s="63"/>
-      <c r="GH12" s="63"/>
-      <c r="GI12" s="120"/>
+      <c r="EA12" s="71"/>
+      <c r="EB12" s="71"/>
+      <c r="EC12" s="71"/>
+      <c r="ED12" s="71"/>
+      <c r="EE12" s="71"/>
+      <c r="EF12" s="71"/>
+      <c r="EG12" s="71"/>
+      <c r="EH12" s="71"/>
+      <c r="EI12" s="71"/>
+      <c r="EJ12" s="71"/>
+      <c r="EK12" s="71"/>
+      <c r="EL12" s="71"/>
+      <c r="EM12" s="71"/>
+      <c r="EN12" s="71"/>
+      <c r="EO12" s="71"/>
+      <c r="EP12" s="71"/>
+      <c r="EQ12" s="71"/>
+      <c r="ER12" s="71"/>
+      <c r="ES12" s="71"/>
+      <c r="ET12" s="71"/>
+      <c r="EU12" s="71"/>
+      <c r="EV12" s="71"/>
+      <c r="EW12" s="71"/>
+      <c r="EX12" s="71"/>
+      <c r="EY12" s="71"/>
+      <c r="EZ12" s="71"/>
+      <c r="FA12" s="71"/>
+      <c r="FB12" s="71"/>
+      <c r="FC12" s="71"/>
+      <c r="FD12" s="71"/>
+      <c r="FE12" s="71"/>
+      <c r="FF12" s="71"/>
+      <c r="FG12" s="71"/>
+      <c r="FH12" s="71"/>
+      <c r="FI12" s="71"/>
+      <c r="FJ12" s="71"/>
+      <c r="FK12" s="71"/>
+      <c r="FL12" s="71"/>
+      <c r="FM12" s="71"/>
+      <c r="FN12" s="71"/>
+      <c r="FO12" s="71"/>
+      <c r="FP12" s="71"/>
+      <c r="FQ12" s="71"/>
+      <c r="FR12" s="71"/>
+      <c r="FS12" s="71"/>
+      <c r="FT12" s="71"/>
+      <c r="FU12" s="71"/>
+      <c r="FV12" s="71"/>
+      <c r="FW12" s="71"/>
+      <c r="FX12" s="71"/>
+      <c r="FY12" s="71"/>
+      <c r="FZ12" s="71"/>
+      <c r="GA12" s="71"/>
+      <c r="GB12" s="71"/>
+      <c r="GC12" s="71"/>
+      <c r="GD12" s="71"/>
+      <c r="GE12" s="71"/>
+      <c r="GF12" s="71"/>
+      <c r="GG12" s="71"/>
+      <c r="GH12" s="71"/>
+      <c r="GI12" s="72"/>
     </row>
     <row r="13" spans="1:191" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="60">
+      <c r="C13" s="117"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="68">
         <v>1</v>
       </c>
-      <c r="I13" s="61"/>
-      <c r="J13" s="60">
+      <c r="I13" s="69"/>
+      <c r="J13" s="68">
         <v>2</v>
       </c>
-      <c r="K13" s="61"/>
-      <c r="L13" s="60">
+      <c r="K13" s="69"/>
+      <c r="L13" s="68">
         <v>3</v>
       </c>
-      <c r="M13" s="61"/>
-      <c r="N13" s="60">
+      <c r="M13" s="69"/>
+      <c r="N13" s="68">
         <v>4</v>
       </c>
-      <c r="O13" s="61"/>
-      <c r="P13" s="60">
+      <c r="O13" s="69"/>
+      <c r="P13" s="68">
         <v>5</v>
       </c>
-      <c r="Q13" s="61"/>
-      <c r="R13" s="60">
+      <c r="Q13" s="69"/>
+      <c r="R13" s="68">
         <v>6</v>
       </c>
-      <c r="S13" s="61"/>
-      <c r="T13" s="60">
+      <c r="S13" s="69"/>
+      <c r="T13" s="68">
         <v>7</v>
       </c>
-      <c r="U13" s="61"/>
-      <c r="V13" s="60">
+      <c r="U13" s="69"/>
+      <c r="V13" s="68">
         <v>8</v>
       </c>
-      <c r="W13" s="61"/>
-      <c r="X13" s="60">
+      <c r="W13" s="69"/>
+      <c r="X13" s="68">
         <v>9</v>
       </c>
-      <c r="Y13" s="61"/>
-      <c r="Z13" s="60">
+      <c r="Y13" s="69"/>
+      <c r="Z13" s="68">
         <v>10</v>
       </c>
-      <c r="AA13" s="61"/>
-      <c r="AB13" s="60">
+      <c r="AA13" s="69"/>
+      <c r="AB13" s="68">
         <v>11</v>
       </c>
-      <c r="AC13" s="61"/>
-      <c r="AD13" s="60">
+      <c r="AC13" s="69"/>
+      <c r="AD13" s="68">
         <v>12</v>
       </c>
-      <c r="AE13" s="61"/>
-      <c r="AF13" s="60">
+      <c r="AE13" s="69"/>
+      <c r="AF13" s="68">
         <v>13</v>
       </c>
-      <c r="AG13" s="61"/>
-      <c r="AH13" s="60">
+      <c r="AG13" s="69"/>
+      <c r="AH13" s="68">
         <v>14</v>
       </c>
-      <c r="AI13" s="61"/>
-      <c r="AJ13" s="60">
+      <c r="AI13" s="69"/>
+      <c r="AJ13" s="68">
         <v>15</v>
       </c>
-      <c r="AK13" s="61"/>
-      <c r="AL13" s="60">
+      <c r="AK13" s="69"/>
+      <c r="AL13" s="68">
         <v>16</v>
       </c>
-      <c r="AM13" s="61"/>
-      <c r="AN13" s="60">
+      <c r="AM13" s="69"/>
+      <c r="AN13" s="68">
         <v>17</v>
       </c>
-      <c r="AO13" s="61"/>
-      <c r="AP13" s="60">
+      <c r="AO13" s="69"/>
+      <c r="AP13" s="68">
         <v>18</v>
       </c>
-      <c r="AQ13" s="61"/>
-      <c r="AR13" s="60">
+      <c r="AQ13" s="69"/>
+      <c r="AR13" s="68">
         <v>19</v>
       </c>
-      <c r="AS13" s="61"/>
-      <c r="AT13" s="60">
+      <c r="AS13" s="69"/>
+      <c r="AT13" s="68">
         <v>20</v>
       </c>
-      <c r="AU13" s="61"/>
-      <c r="AV13" s="60">
+      <c r="AU13" s="69"/>
+      <c r="AV13" s="68">
         <v>21</v>
       </c>
-      <c r="AW13" s="61"/>
-      <c r="AX13" s="60">
+      <c r="AW13" s="69"/>
+      <c r="AX13" s="68">
         <v>22</v>
       </c>
-      <c r="AY13" s="61"/>
-      <c r="AZ13" s="60">
+      <c r="AY13" s="69"/>
+      <c r="AZ13" s="68">
         <v>23</v>
       </c>
-      <c r="BA13" s="61"/>
-      <c r="BB13" s="60">
+      <c r="BA13" s="69"/>
+      <c r="BB13" s="68">
         <v>24</v>
       </c>
-      <c r="BC13" s="61"/>
-      <c r="BD13" s="60">
+      <c r="BC13" s="69"/>
+      <c r="BD13" s="68">
         <v>25</v>
       </c>
-      <c r="BE13" s="61"/>
-      <c r="BF13" s="60">
+      <c r="BE13" s="69"/>
+      <c r="BF13" s="68">
         <v>26</v>
       </c>
-      <c r="BG13" s="61"/>
-      <c r="BH13" s="60">
+      <c r="BG13" s="69"/>
+      <c r="BH13" s="68">
         <v>27</v>
       </c>
-      <c r="BI13" s="61"/>
-      <c r="BJ13" s="60">
+      <c r="BI13" s="69"/>
+      <c r="BJ13" s="68">
         <v>28</v>
       </c>
-      <c r="BK13" s="61"/>
-      <c r="BL13" s="60">
+      <c r="BK13" s="69"/>
+      <c r="BL13" s="68">
         <v>29</v>
       </c>
-      <c r="BM13" s="61"/>
-      <c r="BN13" s="60">
+      <c r="BM13" s="69"/>
+      <c r="BN13" s="68">
         <v>30</v>
       </c>
-      <c r="BO13" s="61"/>
-      <c r="BP13" s="60">
+      <c r="BO13" s="69"/>
+      <c r="BP13" s="68">
         <v>31</v>
       </c>
-      <c r="BQ13" s="69"/>
-      <c r="BR13" s="60">
+      <c r="BQ13" s="120"/>
+      <c r="BR13" s="68">
         <v>1</v>
       </c>
-      <c r="BS13" s="61"/>
-      <c r="BT13" s="60">
+      <c r="BS13" s="69"/>
+      <c r="BT13" s="68">
         <v>2</v>
       </c>
-      <c r="BU13" s="61"/>
-      <c r="BV13" s="60">
+      <c r="BU13" s="69"/>
+      <c r="BV13" s="68">
         <v>3</v>
       </c>
-      <c r="BW13" s="61"/>
-      <c r="BX13" s="60">
+      <c r="BW13" s="69"/>
+      <c r="BX13" s="68">
         <v>4</v>
       </c>
-      <c r="BY13" s="61"/>
-      <c r="BZ13" s="60">
+      <c r="BY13" s="69"/>
+      <c r="BZ13" s="68">
         <v>5</v>
       </c>
-      <c r="CA13" s="61"/>
-      <c r="CB13" s="60">
+      <c r="CA13" s="69"/>
+      <c r="CB13" s="68">
         <v>6</v>
       </c>
-      <c r="CC13" s="61"/>
-      <c r="CD13" s="60">
+      <c r="CC13" s="69"/>
+      <c r="CD13" s="68">
         <v>7</v>
       </c>
-      <c r="CE13" s="61"/>
-      <c r="CF13" s="60">
+      <c r="CE13" s="69"/>
+      <c r="CF13" s="68">
         <v>8</v>
       </c>
-      <c r="CG13" s="61"/>
-      <c r="CH13" s="60">
+      <c r="CG13" s="69"/>
+      <c r="CH13" s="68">
         <v>9</v>
       </c>
-      <c r="CI13" s="61"/>
-      <c r="CJ13" s="60">
+      <c r="CI13" s="69"/>
+      <c r="CJ13" s="68">
         <v>10</v>
       </c>
-      <c r="CK13" s="61"/>
-      <c r="CL13" s="60">
+      <c r="CK13" s="69"/>
+      <c r="CL13" s="68">
         <v>11</v>
       </c>
-      <c r="CM13" s="61"/>
-      <c r="CN13" s="60">
+      <c r="CM13" s="69"/>
+      <c r="CN13" s="68">
         <v>12</v>
       </c>
-      <c r="CO13" s="61"/>
-      <c r="CP13" s="60">
+      <c r="CO13" s="69"/>
+      <c r="CP13" s="68">
         <v>13</v>
       </c>
-      <c r="CQ13" s="61"/>
-      <c r="CR13" s="60">
+      <c r="CQ13" s="69"/>
+      <c r="CR13" s="68">
         <v>14</v>
       </c>
-      <c r="CS13" s="61"/>
-      <c r="CT13" s="60">
+      <c r="CS13" s="69"/>
+      <c r="CT13" s="68">
         <v>15</v>
       </c>
-      <c r="CU13" s="61"/>
-      <c r="CV13" s="60">
+      <c r="CU13" s="69"/>
+      <c r="CV13" s="68">
         <v>16</v>
       </c>
-      <c r="CW13" s="61"/>
-      <c r="CX13" s="60">
+      <c r="CW13" s="69"/>
+      <c r="CX13" s="68">
         <v>17</v>
       </c>
-      <c r="CY13" s="61"/>
-      <c r="CZ13" s="60">
+      <c r="CY13" s="69"/>
+      <c r="CZ13" s="68">
         <v>18</v>
       </c>
-      <c r="DA13" s="61"/>
-      <c r="DB13" s="60">
+      <c r="DA13" s="69"/>
+      <c r="DB13" s="68">
         <v>19</v>
       </c>
-      <c r="DC13" s="61"/>
-      <c r="DD13" s="60">
+      <c r="DC13" s="69"/>
+      <c r="DD13" s="68">
         <v>20</v>
       </c>
-      <c r="DE13" s="61"/>
-      <c r="DF13" s="60">
+      <c r="DE13" s="69"/>
+      <c r="DF13" s="68">
         <v>21</v>
       </c>
-      <c r="DG13" s="61"/>
-      <c r="DH13" s="60">
+      <c r="DG13" s="69"/>
+      <c r="DH13" s="68">
         <v>22</v>
       </c>
-      <c r="DI13" s="61"/>
-      <c r="DJ13" s="60">
+      <c r="DI13" s="69"/>
+      <c r="DJ13" s="68">
         <v>23</v>
       </c>
-      <c r="DK13" s="61"/>
-      <c r="DL13" s="60">
+      <c r="DK13" s="69"/>
+      <c r="DL13" s="68">
         <v>24</v>
       </c>
-      <c r="DM13" s="61"/>
-      <c r="DN13" s="60">
+      <c r="DM13" s="69"/>
+      <c r="DN13" s="68">
         <v>25</v>
       </c>
-      <c r="DO13" s="61"/>
-      <c r="DP13" s="60">
+      <c r="DO13" s="69"/>
+      <c r="DP13" s="68">
         <v>26</v>
       </c>
-      <c r="DQ13" s="61"/>
-      <c r="DR13" s="60">
+      <c r="DQ13" s="69"/>
+      <c r="DR13" s="68">
         <v>27</v>
       </c>
-      <c r="DS13" s="61"/>
-      <c r="DT13" s="60">
+      <c r="DS13" s="69"/>
+      <c r="DT13" s="68">
         <v>28</v>
       </c>
-      <c r="DU13" s="61"/>
-      <c r="DV13" s="60">
+      <c r="DU13" s="69"/>
+      <c r="DV13" s="68">
         <v>29</v>
       </c>
-      <c r="DW13" s="61"/>
-      <c r="DX13" s="60">
+      <c r="DW13" s="69"/>
+      <c r="DX13" s="68">
         <v>30</v>
       </c>
-      <c r="DY13" s="61"/>
-      <c r="DZ13" s="60">
+      <c r="DY13" s="69"/>
+      <c r="DZ13" s="68">
         <v>1</v>
       </c>
-      <c r="EA13" s="61"/>
-      <c r="EB13" s="60">
+      <c r="EA13" s="69"/>
+      <c r="EB13" s="68">
         <v>2</v>
       </c>
-      <c r="EC13" s="61"/>
-      <c r="ED13" s="60">
+      <c r="EC13" s="69"/>
+      <c r="ED13" s="68">
         <v>3</v>
       </c>
-      <c r="EE13" s="61"/>
-      <c r="EF13" s="60">
+      <c r="EE13" s="69"/>
+      <c r="EF13" s="68">
         <v>4</v>
       </c>
-      <c r="EG13" s="61"/>
-      <c r="EH13" s="60">
+      <c r="EG13" s="69"/>
+      <c r="EH13" s="68">
         <v>5</v>
       </c>
-      <c r="EI13" s="61"/>
-      <c r="EJ13" s="60">
+      <c r="EI13" s="69"/>
+      <c r="EJ13" s="68">
         <v>6</v>
       </c>
-      <c r="EK13" s="61"/>
-      <c r="EL13" s="60">
+      <c r="EK13" s="69"/>
+      <c r="EL13" s="68">
         <v>7</v>
       </c>
-      <c r="EM13" s="61"/>
-      <c r="EN13" s="60">
+      <c r="EM13" s="69"/>
+      <c r="EN13" s="68">
         <v>8</v>
       </c>
-      <c r="EO13" s="61"/>
-      <c r="EP13" s="60">
+      <c r="EO13" s="69"/>
+      <c r="EP13" s="68">
         <v>9</v>
       </c>
-      <c r="EQ13" s="61"/>
-      <c r="ER13" s="60">
+      <c r="EQ13" s="69"/>
+      <c r="ER13" s="68">
         <v>10</v>
       </c>
-      <c r="ES13" s="61"/>
-      <c r="ET13" s="60">
+      <c r="ES13" s="69"/>
+      <c r="ET13" s="68">
         <v>11</v>
       </c>
-      <c r="EU13" s="61"/>
-      <c r="EV13" s="60">
+      <c r="EU13" s="69"/>
+      <c r="EV13" s="68">
         <v>12</v>
       </c>
-      <c r="EW13" s="61"/>
-      <c r="EX13" s="60">
+      <c r="EW13" s="69"/>
+      <c r="EX13" s="68">
         <v>13</v>
       </c>
-      <c r="EY13" s="61"/>
-      <c r="EZ13" s="60">
+      <c r="EY13" s="69"/>
+      <c r="EZ13" s="68">
         <v>14</v>
       </c>
-      <c r="FA13" s="61"/>
-      <c r="FB13" s="60">
+      <c r="FA13" s="69"/>
+      <c r="FB13" s="68">
         <v>15</v>
       </c>
-      <c r="FC13" s="61"/>
-      <c r="FD13" s="60">
+      <c r="FC13" s="69"/>
+      <c r="FD13" s="68">
         <v>16</v>
       </c>
-      <c r="FE13" s="61"/>
-      <c r="FF13" s="60">
+      <c r="FE13" s="69"/>
+      <c r="FF13" s="68">
         <v>17</v>
       </c>
-      <c r="FG13" s="61"/>
-      <c r="FH13" s="60">
+      <c r="FG13" s="69"/>
+      <c r="FH13" s="68">
         <v>18</v>
       </c>
-      <c r="FI13" s="61"/>
-      <c r="FJ13" s="60">
+      <c r="FI13" s="69"/>
+      <c r="FJ13" s="68">
         <v>19</v>
       </c>
-      <c r="FK13" s="61"/>
-      <c r="FL13" s="60">
+      <c r="FK13" s="69"/>
+      <c r="FL13" s="68">
         <v>20</v>
       </c>
-      <c r="FM13" s="61"/>
-      <c r="FN13" s="60">
+      <c r="FM13" s="69"/>
+      <c r="FN13" s="68">
         <v>21</v>
       </c>
-      <c r="FO13" s="61"/>
-      <c r="FP13" s="60">
+      <c r="FO13" s="69"/>
+      <c r="FP13" s="68">
         <v>22</v>
       </c>
-      <c r="FQ13" s="61"/>
-      <c r="FR13" s="60">
+      <c r="FQ13" s="69"/>
+      <c r="FR13" s="68">
         <v>23</v>
       </c>
-      <c r="FS13" s="61"/>
-      <c r="FT13" s="60">
+      <c r="FS13" s="69"/>
+      <c r="FT13" s="68">
         <v>24</v>
       </c>
-      <c r="FU13" s="61"/>
-      <c r="FV13" s="60">
+      <c r="FU13" s="69"/>
+      <c r="FV13" s="68">
         <v>25</v>
       </c>
-      <c r="FW13" s="61"/>
-      <c r="FX13" s="60">
+      <c r="FW13" s="69"/>
+      <c r="FX13" s="68">
         <v>26</v>
       </c>
-      <c r="FY13" s="61"/>
-      <c r="FZ13" s="60">
+      <c r="FY13" s="69"/>
+      <c r="FZ13" s="68">
         <v>27</v>
       </c>
-      <c r="GA13" s="61"/>
-      <c r="GB13" s="60">
+      <c r="GA13" s="69"/>
+      <c r="GB13" s="68">
         <v>28</v>
       </c>
-      <c r="GC13" s="61"/>
-      <c r="GD13" s="60">
+      <c r="GC13" s="69"/>
+      <c r="GD13" s="68">
         <v>29</v>
       </c>
-      <c r="GE13" s="61"/>
-      <c r="GF13" s="60">
+      <c r="GE13" s="69"/>
+      <c r="GF13" s="68">
         <v>30</v>
       </c>
-      <c r="GG13" s="61"/>
-      <c r="GH13" s="60">
+      <c r="GG13" s="69"/>
+      <c r="GH13" s="68">
         <v>31</v>
       </c>
-      <c r="GI13" s="61"/>
+      <c r="GI13" s="69"/>
     </row>
     <row r="14" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A14" s="113" t="s">
+      <c r="A14" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="114"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="37"/>
-      <c r="D14" s="97">
+      <c r="D14" s="91">
         <f>SUM(D15:E61)</f>
         <v>51.050000000000011</v>
       </c>
-      <c r="E14" s="99"/>
-      <c r="F14" s="97">
+      <c r="E14" s="93"/>
+      <c r="F14" s="91">
         <f>SUM(F15:G61)</f>
-        <v>33.916000000000004</v>
-      </c>
-      <c r="G14" s="98"/>
+        <v>34.249000000000002</v>
+      </c>
+      <c r="G14" s="92"/>
       <c r="H14" s="18"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -2828,22 +2830,22 @@
       <c r="GI14" s="14"/>
     </row>
     <row r="15" spans="1:191" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="74"/>
+      <c r="B15" s="83"/>
       <c r="C15" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="65">
+      <c r="D15" s="62">
         <v>1.5</v>
       </c>
-      <c r="E15" s="66"/>
-      <c r="F15" s="65">
+      <c r="E15" s="63"/>
+      <c r="F15" s="62">
         <f>SUM(H15:GI15)</f>
         <v>0.5</v>
       </c>
-      <c r="G15" s="80"/>
+      <c r="G15" s="64"/>
       <c r="H15" s="47"/>
       <c r="I15" s="12"/>
       <c r="J15" s="24">
@@ -3032,22 +3034,22 @@
       <c r="GI15" s="34"/>
     </row>
     <row r="16" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A16" s="81" t="s">
+      <c r="A16" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="82"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="62">
         <v>0.6</v>
       </c>
-      <c r="E16" s="66"/>
-      <c r="F16" s="65">
+      <c r="E16" s="63"/>
+      <c r="F16" s="62">
         <f>SUM(H16:GI16)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="80"/>
+      <c r="G16" s="64"/>
       <c r="H16" s="47"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
@@ -3234,22 +3236,22 @@
       <c r="GI16" s="32"/>
     </row>
     <row r="17" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A17" s="81" t="s">
+      <c r="A17" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="82"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="65">
+      <c r="D17" s="62">
         <v>1</v>
       </c>
-      <c r="E17" s="66"/>
-      <c r="F17" s="65">
+      <c r="E17" s="63"/>
+      <c r="F17" s="62">
         <f>SUM(H17:GI17)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="80"/>
+      <c r="G17" s="64"/>
       <c r="H17" s="47"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
@@ -3440,22 +3442,22 @@
       <c r="GI17" s="32"/>
     </row>
     <row r="18" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A18" s="81" t="s">
+      <c r="A18" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="82"/>
+      <c r="B18" s="67"/>
       <c r="C18" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="65">
+      <c r="D18" s="62">
         <v>0.8</v>
       </c>
-      <c r="E18" s="66"/>
-      <c r="F18" s="65">
+      <c r="E18" s="63"/>
+      <c r="F18" s="62">
         <f t="shared" ref="F18:F60" si="0">SUM(H18:GI18)</f>
         <v>0.75</v>
       </c>
-      <c r="G18" s="80"/>
+      <c r="G18" s="64"/>
       <c r="H18" s="26"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
@@ -3644,22 +3646,22 @@
       <c r="GI18" s="32"/>
     </row>
     <row r="19" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="82"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="65">
+      <c r="D19" s="62">
         <v>0.5</v>
       </c>
-      <c r="E19" s="66"/>
-      <c r="F19" s="65">
+      <c r="E19" s="63"/>
+      <c r="F19" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="80"/>
+      <c r="G19" s="64"/>
       <c r="H19" s="26"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
@@ -3846,22 +3848,22 @@
       <c r="GI19" s="36"/>
     </row>
     <row r="20" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="82"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="65">
+      <c r="D20" s="62">
         <v>0.3</v>
       </c>
-      <c r="E20" s="66"/>
-      <c r="F20" s="65">
+      <c r="E20" s="63"/>
+      <c r="F20" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="80"/>
+      <c r="G20" s="64"/>
       <c r="H20" s="26"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -4048,22 +4050,22 @@
       <c r="GI20" s="36"/>
     </row>
     <row r="21" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="82"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="65">
+      <c r="D21" s="62">
         <v>1</v>
       </c>
-      <c r="E21" s="66"/>
-      <c r="F21" s="65">
+      <c r="E21" s="63"/>
+      <c r="F21" s="62">
         <f t="shared" si="0"/>
         <v>0.16600000000000001</v>
       </c>
-      <c r="G21" s="80"/>
+      <c r="G21" s="64"/>
       <c r="H21" s="26"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
@@ -4252,22 +4254,22 @@
       <c r="GI21" s="36"/>
     </row>
     <row r="22" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A22" s="81" t="s">
+      <c r="A22" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="82"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="65">
+      <c r="D22" s="62">
         <v>0.6</v>
       </c>
-      <c r="E22" s="66"/>
-      <c r="F22" s="65">
+      <c r="E22" s="63"/>
+      <c r="F22" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="80"/>
+      <c r="G22" s="64"/>
       <c r="H22" s="26"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
@@ -4454,22 +4456,22 @@
       <c r="GI22" s="36"/>
     </row>
     <row r="23" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A23" s="81" t="s">
+      <c r="A23" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="82"/>
+      <c r="B23" s="67"/>
       <c r="C23" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="65">
+      <c r="D23" s="62">
         <v>0.6</v>
       </c>
-      <c r="E23" s="66"/>
-      <c r="F23" s="65">
+      <c r="E23" s="63"/>
+      <c r="F23" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="80"/>
+      <c r="G23" s="64"/>
       <c r="H23" s="26"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
@@ -4656,22 +4658,22 @@
       <c r="GI23" s="36"/>
     </row>
     <row r="24" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A24" s="81" t="s">
+      <c r="A24" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="82"/>
+      <c r="B24" s="67"/>
       <c r="C24" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="65">
+      <c r="D24" s="62">
         <v>3</v>
       </c>
-      <c r="E24" s="66"/>
-      <c r="F24" s="65">
+      <c r="E24" s="63"/>
+      <c r="F24" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="80"/>
+      <c r="G24" s="64"/>
       <c r="H24" s="26"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
@@ -4858,22 +4860,22 @@
       <c r="GI24" s="36"/>
     </row>
     <row r="25" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A25" s="81" t="s">
+      <c r="A25" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="82"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="65">
+      <c r="D25" s="62">
         <v>1.5</v>
       </c>
-      <c r="E25" s="66"/>
-      <c r="F25" s="65">
+      <c r="E25" s="63"/>
+      <c r="F25" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="80"/>
+      <c r="G25" s="64"/>
       <c r="H25" s="26"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
@@ -5060,22 +5062,22 @@
       <c r="GI25" s="36"/>
     </row>
     <row r="26" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A26" s="81" t="s">
+      <c r="A26" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="82"/>
+      <c r="B26" s="67"/>
       <c r="C26" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="65">
+      <c r="D26" s="62">
         <v>1</v>
       </c>
-      <c r="E26" s="66"/>
-      <c r="F26" s="65">
+      <c r="E26" s="63"/>
+      <c r="F26" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="80"/>
+      <c r="G26" s="64"/>
       <c r="H26" s="26"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
@@ -5262,22 +5264,22 @@
       <c r="GI26" s="36"/>
     </row>
     <row r="27" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="81" t="s">
+      <c r="A27" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="82"/>
+      <c r="B27" s="67"/>
       <c r="C27" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="65">
+      <c r="D27" s="62">
         <v>1</v>
       </c>
-      <c r="E27" s="66"/>
-      <c r="F27" s="65">
+      <c r="E27" s="63"/>
+      <c r="F27" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G27" s="80"/>
+      <c r="G27" s="64"/>
       <c r="H27" s="26"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
@@ -5464,22 +5466,22 @@
       <c r="GI27" s="36"/>
     </row>
     <row r="28" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A28" s="81" t="s">
+      <c r="A28" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="82"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="65">
+      <c r="D28" s="62">
         <v>1</v>
       </c>
-      <c r="E28" s="66"/>
-      <c r="F28" s="65">
+      <c r="E28" s="63"/>
+      <c r="F28" s="62">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G28" s="80"/>
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="G28" s="64"/>
       <c r="H28" s="26"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
@@ -5511,7 +5513,9 @@
       <c r="AJ28" s="32"/>
       <c r="AK28" s="32"/>
       <c r="AL28" s="32"/>
-      <c r="AM28" s="32"/>
+      <c r="AM28" s="24">
+        <v>0.33300000000000002</v>
+      </c>
       <c r="AN28" s="49"/>
       <c r="AO28" s="52"/>
       <c r="AP28" s="51"/>
@@ -5666,22 +5670,22 @@
       <c r="GI28" s="36"/>
     </row>
     <row r="29" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A29" s="81" t="s">
+      <c r="A29" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="82"/>
+      <c r="B29" s="67"/>
       <c r="C29" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="65">
+      <c r="D29" s="62">
         <v>1</v>
       </c>
-      <c r="E29" s="66"/>
-      <c r="F29" s="65">
+      <c r="E29" s="63"/>
+      <c r="F29" s="62">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G29" s="80"/>
+      <c r="G29" s="64"/>
       <c r="H29" s="26"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
@@ -5870,22 +5874,22 @@
       <c r="GI29" s="36"/>
     </row>
     <row r="30" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A30" s="81" t="s">
+      <c r="A30" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="82"/>
+      <c r="B30" s="67"/>
       <c r="C30" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="65">
+      <c r="D30" s="62">
         <v>1</v>
       </c>
-      <c r="E30" s="66"/>
-      <c r="F30" s="65">
+      <c r="E30" s="63"/>
+      <c r="F30" s="62">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G30" s="80"/>
+      <c r="G30" s="64"/>
       <c r="H30" s="26"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
@@ -6074,22 +6078,22 @@
       <c r="GI30" s="36"/>
     </row>
     <row r="31" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A31" s="81" t="s">
+      <c r="A31" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="82"/>
+      <c r="B31" s="67"/>
       <c r="C31" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="65">
+      <c r="D31" s="62">
         <v>4</v>
       </c>
-      <c r="E31" s="66"/>
-      <c r="F31" s="65">
+      <c r="E31" s="63"/>
+      <c r="F31" s="62">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G31" s="80"/>
+      <c r="G31" s="64"/>
       <c r="H31" s="26"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
@@ -6280,22 +6284,22 @@
       <c r="GI31" s="36"/>
     </row>
     <row r="32" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A32" s="81" t="s">
+      <c r="A32" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="82"/>
+      <c r="B32" s="67"/>
       <c r="C32" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="65">
+      <c r="D32" s="62">
         <v>0.6</v>
       </c>
-      <c r="E32" s="66"/>
-      <c r="F32" s="65">
+      <c r="E32" s="63"/>
+      <c r="F32" s="62">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G32" s="80"/>
+      <c r="G32" s="64"/>
       <c r="H32" s="26"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
@@ -6484,22 +6488,22 @@
       <c r="GI32" s="36"/>
     </row>
     <row r="33" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="81" t="s">
+      <c r="A33" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="82"/>
+      <c r="B33" s="67"/>
       <c r="C33" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="65">
+      <c r="D33" s="62">
         <v>0.5</v>
       </c>
-      <c r="E33" s="66"/>
-      <c r="F33" s="65">
+      <c r="E33" s="63"/>
+      <c r="F33" s="62">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G33" s="80"/>
+      <c r="G33" s="64"/>
       <c r="H33" s="26"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
@@ -6688,22 +6692,22 @@
       <c r="GI33" s="36"/>
     </row>
     <row r="34" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A34" s="81" t="s">
+      <c r="A34" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="82"/>
+      <c r="B34" s="67"/>
       <c r="C34" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="65">
+      <c r="D34" s="62">
         <v>0.3</v>
       </c>
-      <c r="E34" s="66"/>
-      <c r="F34" s="65">
+      <c r="E34" s="63"/>
+      <c r="F34" s="62">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G34" s="80"/>
+      <c r="G34" s="64"/>
       <c r="H34" s="26"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
@@ -6892,22 +6896,22 @@
       <c r="GI34" s="36"/>
     </row>
     <row r="35" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A35" s="81" t="s">
+      <c r="A35" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="82"/>
+      <c r="B35" s="67"/>
       <c r="C35" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="65">
+      <c r="D35" s="62">
         <v>0.3</v>
       </c>
-      <c r="E35" s="66"/>
-      <c r="F35" s="65">
+      <c r="E35" s="63"/>
+      <c r="F35" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G35" s="80"/>
+      <c r="G35" s="64"/>
       <c r="H35" s="26"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
@@ -7094,22 +7098,22 @@
       <c r="GI35" s="36"/>
     </row>
     <row r="36" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A36" s="81" t="s">
+      <c r="A36" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="82"/>
+      <c r="B36" s="67"/>
       <c r="C36" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="65">
+      <c r="D36" s="62">
         <v>1.5</v>
       </c>
-      <c r="E36" s="66"/>
-      <c r="F36" s="65">
+      <c r="E36" s="63"/>
+      <c r="F36" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G36" s="80"/>
+      <c r="G36" s="64"/>
       <c r="H36" s="26"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
@@ -7296,22 +7300,22 @@
       <c r="GI36" s="36"/>
     </row>
     <row r="37" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A37" s="81" t="s">
+      <c r="A37" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="82"/>
+      <c r="B37" s="67"/>
       <c r="C37" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="65">
+      <c r="D37" s="62">
         <v>0.5</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="65">
+      <c r="E37" s="63"/>
+      <c r="F37" s="62">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G37" s="80"/>
+      <c r="G37" s="64"/>
       <c r="H37" s="26"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
@@ -7500,22 +7504,22 @@
       <c r="GI37" s="36"/>
     </row>
     <row r="38" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A38" s="81" t="s">
+      <c r="A38" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="82"/>
+      <c r="B38" s="67"/>
       <c r="C38" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="65">
+      <c r="D38" s="62">
         <v>0.25</v>
       </c>
-      <c r="E38" s="66"/>
-      <c r="F38" s="65">
+      <c r="E38" s="63"/>
+      <c r="F38" s="62">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G38" s="80"/>
+      <c r="G38" s="64"/>
       <c r="H38" s="26"/>
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
@@ -7704,22 +7708,22 @@
       <c r="GI38" s="36"/>
     </row>
     <row r="39" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A39" s="81" t="s">
+      <c r="A39" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="82"/>
+      <c r="B39" s="67"/>
       <c r="C39" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="65">
+      <c r="D39" s="62">
         <v>0.5</v>
       </c>
-      <c r="E39" s="66"/>
-      <c r="F39" s="65">
+      <c r="E39" s="63"/>
+      <c r="F39" s="62">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="G39" s="80"/>
+      <c r="G39" s="64"/>
       <c r="H39" s="26"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
@@ -7908,22 +7912,22 @@
       <c r="GI39" s="36"/>
     </row>
     <row r="40" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A40" s="81" t="s">
+      <c r="A40" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="82"/>
+      <c r="B40" s="67"/>
       <c r="C40" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="65">
+      <c r="D40" s="62">
         <v>0.5</v>
       </c>
-      <c r="E40" s="66"/>
-      <c r="F40" s="65">
+      <c r="E40" s="63"/>
+      <c r="F40" s="62">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G40" s="80"/>
+      <c r="G40" s="64"/>
       <c r="H40" s="26"/>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
@@ -8112,22 +8116,22 @@
       <c r="GI40" s="36"/>
     </row>
     <row r="41" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A41" s="81" t="s">
+      <c r="A41" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="82"/>
+      <c r="B41" s="67"/>
       <c r="C41" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="65">
+      <c r="D41" s="62">
         <v>0.3</v>
       </c>
-      <c r="E41" s="66"/>
-      <c r="F41" s="65">
+      <c r="E41" s="63"/>
+      <c r="F41" s="62">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G41" s="80"/>
+      <c r="G41" s="64"/>
       <c r="H41" s="26"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
@@ -8316,22 +8320,22 @@
       <c r="GI41" s="36"/>
     </row>
     <row r="42" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A42" s="81" t="s">
+      <c r="A42" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="82"/>
+      <c r="B42" s="67"/>
       <c r="C42" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="65">
+      <c r="D42" s="62">
         <v>0.5</v>
       </c>
-      <c r="E42" s="66"/>
-      <c r="F42" s="65">
+      <c r="E42" s="63"/>
+      <c r="F42" s="62">
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-      <c r="G42" s="80"/>
+      <c r="G42" s="64"/>
       <c r="H42" s="26"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
@@ -8520,22 +8524,22 @@
       <c r="GI42" s="36"/>
     </row>
     <row r="43" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A43" s="81" t="s">
+      <c r="A43" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="82"/>
+      <c r="B43" s="67"/>
       <c r="C43" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D43" s="65">
+      <c r="D43" s="62">
         <v>1.3</v>
       </c>
-      <c r="E43" s="66"/>
-      <c r="F43" s="65">
+      <c r="E43" s="63"/>
+      <c r="F43" s="62">
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
-      <c r="G43" s="80"/>
+      <c r="G43" s="64"/>
       <c r="H43" s="26"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
@@ -8726,22 +8730,22 @@
       <c r="GI43" s="36"/>
     </row>
     <row r="44" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="81" t="s">
+      <c r="A44" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="82"/>
+      <c r="B44" s="67"/>
       <c r="C44" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="65">
+      <c r="D44" s="62">
         <v>1.3</v>
       </c>
-      <c r="E44" s="66"/>
-      <c r="F44" s="65">
+      <c r="E44" s="63"/>
+      <c r="F44" s="62">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G44" s="80"/>
+      <c r="G44" s="64"/>
       <c r="H44" s="26"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
@@ -8930,22 +8934,22 @@
       <c r="GI44" s="36"/>
     </row>
     <row r="45" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A45" s="81" t="s">
+      <c r="A45" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="82"/>
+      <c r="B45" s="67"/>
       <c r="C45" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="65">
+      <c r="D45" s="62">
         <v>1</v>
       </c>
-      <c r="E45" s="66"/>
-      <c r="F45" s="65">
+      <c r="E45" s="63"/>
+      <c r="F45" s="62">
         <f t="shared" si="0"/>
         <v>1.05</v>
       </c>
-      <c r="G45" s="80"/>
+      <c r="G45" s="64"/>
       <c r="H45" s="26"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
@@ -9136,22 +9140,22 @@
       <c r="GI45" s="36"/>
     </row>
     <row r="46" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A46" s="81" t="s">
+      <c r="A46" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="82"/>
+      <c r="B46" s="67"/>
       <c r="C46" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="D46" s="65">
+      <c r="D46" s="62">
         <v>1</v>
       </c>
-      <c r="E46" s="66"/>
-      <c r="F46" s="65">
+      <c r="E46" s="63"/>
+      <c r="F46" s="62">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="G46" s="80"/>
+      <c r="G46" s="64"/>
       <c r="H46" s="26"/>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
@@ -9340,22 +9344,22 @@
       <c r="GI46" s="36"/>
     </row>
     <row r="47" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A47" s="81" t="s">
+      <c r="A47" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="82"/>
+      <c r="B47" s="67"/>
       <c r="C47" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="D47" s="65">
+      <c r="D47" s="62">
         <v>1</v>
       </c>
-      <c r="E47" s="66"/>
-      <c r="F47" s="65">
+      <c r="E47" s="63"/>
+      <c r="F47" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G47" s="80"/>
+      <c r="G47" s="64"/>
       <c r="H47" s="26"/>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
@@ -9542,22 +9546,22 @@
       <c r="GI47" s="36"/>
     </row>
     <row r="48" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A48" s="81" t="s">
+      <c r="A48" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="B48" s="82"/>
+      <c r="B48" s="67"/>
       <c r="C48" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D48" s="65">
+      <c r="D48" s="62">
         <v>0.3</v>
       </c>
-      <c r="E48" s="66"/>
-      <c r="F48" s="65">
+      <c r="E48" s="63"/>
+      <c r="F48" s="62">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G48" s="80"/>
+      <c r="G48" s="64"/>
       <c r="H48" s="26"/>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
@@ -9746,22 +9750,22 @@
       <c r="GI48" s="36"/>
     </row>
     <row r="49" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A49" s="81" t="s">
+      <c r="A49" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="82"/>
+      <c r="B49" s="67"/>
       <c r="C49" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="65">
+      <c r="D49" s="62">
         <v>2</v>
       </c>
-      <c r="E49" s="66"/>
-      <c r="F49" s="65">
+      <c r="E49" s="63"/>
+      <c r="F49" s="62">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G49" s="80"/>
+      <c r="G49" s="64"/>
       <c r="H49" s="26"/>
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
@@ -9952,22 +9956,22 @@
       <c r="GI49" s="36"/>
     </row>
     <row r="50" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A50" s="81" t="s">
+      <c r="A50" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="82"/>
+      <c r="B50" s="67"/>
       <c r="C50" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="D50" s="65">
+      <c r="D50" s="62">
         <v>2</v>
       </c>
-      <c r="E50" s="66"/>
-      <c r="F50" s="65">
+      <c r="E50" s="63"/>
+      <c r="F50" s="62">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G50" s="80"/>
+      <c r="G50" s="64"/>
       <c r="H50" s="26"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
@@ -10158,22 +10162,22 @@
       <c r="GI50" s="36"/>
     </row>
     <row r="51" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A51" s="81" t="s">
+      <c r="A51" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="82"/>
+      <c r="B51" s="67"/>
       <c r="C51" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D51" s="65">
+      <c r="D51" s="62">
         <v>2</v>
       </c>
-      <c r="E51" s="66"/>
-      <c r="F51" s="65">
+      <c r="E51" s="63"/>
+      <c r="F51" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G51" s="80"/>
+      <c r="G51" s="64"/>
       <c r="H51" s="26"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
@@ -10360,22 +10364,22 @@
       <c r="GI51" s="36"/>
     </row>
     <row r="52" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A52" s="81" t="s">
+      <c r="A52" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="82"/>
+      <c r="B52" s="67"/>
       <c r="C52" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="65">
+      <c r="D52" s="62">
         <v>2</v>
       </c>
-      <c r="E52" s="66"/>
-      <c r="F52" s="65">
+      <c r="E52" s="63"/>
+      <c r="F52" s="62">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G52" s="80"/>
+      <c r="G52" s="64"/>
       <c r="H52" s="26"/>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
@@ -10566,22 +10570,22 @@
       <c r="GI52" s="36"/>
     </row>
     <row r="53" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A53" s="81" t="s">
+      <c r="A53" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="82"/>
+      <c r="B53" s="67"/>
       <c r="C53" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D53" s="65">
+      <c r="D53" s="62">
         <v>2</v>
       </c>
-      <c r="E53" s="66"/>
-      <c r="F53" s="65">
+      <c r="E53" s="63"/>
+      <c r="F53" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G53" s="80"/>
+      <c r="G53" s="64"/>
       <c r="H53" s="26"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
@@ -10768,22 +10772,22 @@
       <c r="GI53" s="36"/>
     </row>
     <row r="54" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A54" s="81" t="s">
+      <c r="A54" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="82"/>
+      <c r="B54" s="67"/>
       <c r="C54" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="D54" s="65">
+      <c r="D54" s="62">
         <v>0.25</v>
       </c>
-      <c r="E54" s="66"/>
-      <c r="F54" s="65">
+      <c r="E54" s="63"/>
+      <c r="F54" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G54" s="80"/>
+      <c r="G54" s="64"/>
       <c r="H54" s="26"/>
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
@@ -10970,22 +10974,22 @@
       <c r="GI54" s="36"/>
     </row>
     <row r="55" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A55" s="81" t="s">
+      <c r="A55" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="82"/>
+      <c r="B55" s="67"/>
       <c r="C55" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="D55" s="65">
+      <c r="D55" s="62">
         <v>1</v>
       </c>
-      <c r="E55" s="66"/>
-      <c r="F55" s="65">
+      <c r="E55" s="63"/>
+      <c r="F55" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G55" s="80"/>
+      <c r="G55" s="64"/>
       <c r="H55" s="26"/>
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
@@ -11172,22 +11176,22 @@
       <c r="GI55" s="36"/>
     </row>
     <row r="56" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A56" s="81" t="s">
+      <c r="A56" s="66" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="82"/>
+      <c r="B56" s="67"/>
       <c r="C56" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="D56" s="65">
+      <c r="D56" s="62">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E56" s="66"/>
-      <c r="F56" s="65">
+      <c r="E56" s="63"/>
+      <c r="F56" s="62">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G56" s="80"/>
+      <c r="G56" s="64"/>
       <c r="H56" s="26"/>
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
@@ -11378,22 +11382,22 @@
       <c r="GI56" s="36"/>
     </row>
     <row r="57" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A57" s="81" t="s">
+      <c r="A57" s="66" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="82"/>
+      <c r="B57" s="67"/>
       <c r="C57" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="D57" s="65">
+      <c r="D57" s="62">
         <v>1.75</v>
       </c>
-      <c r="E57" s="66"/>
-      <c r="F57" s="65">
+      <c r="E57" s="63"/>
+      <c r="F57" s="62">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G57" s="80"/>
+      <c r="G57" s="64"/>
       <c r="H57" s="26"/>
       <c r="I57" s="12"/>
       <c r="J57" s="12"/>
@@ -11582,22 +11586,22 @@
       <c r="GI57" s="36"/>
     </row>
     <row r="58" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A58" s="81" t="s">
+      <c r="A58" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="B58" s="82"/>
+      <c r="B58" s="67"/>
       <c r="C58" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="D58" s="65">
+      <c r="D58" s="62">
         <v>0.6</v>
       </c>
-      <c r="E58" s="66"/>
-      <c r="F58" s="65">
+      <c r="E58" s="63"/>
+      <c r="F58" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G58" s="80"/>
+      <c r="G58" s="64"/>
       <c r="H58" s="26"/>
       <c r="I58" s="12"/>
       <c r="J58" s="12"/>
@@ -11784,22 +11788,22 @@
       <c r="GI58" s="36"/>
     </row>
     <row r="59" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="81" t="s">
+      <c r="A59" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="B59" s="82"/>
+      <c r="B59" s="67"/>
       <c r="C59" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="65">
+      <c r="D59" s="62">
         <v>1</v>
       </c>
-      <c r="E59" s="66"/>
-      <c r="F59" s="65">
+      <c r="E59" s="63"/>
+      <c r="F59" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G59" s="80"/>
+      <c r="G59" s="64"/>
       <c r="H59" s="26"/>
       <c r="I59" s="12"/>
       <c r="J59" s="12"/>
@@ -11986,22 +11990,22 @@
       <c r="GI59" s="36"/>
     </row>
     <row r="60" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A60" s="81" t="s">
+      <c r="A60" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="B60" s="82"/>
+      <c r="B60" s="67"/>
       <c r="C60" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="D60" s="65">
+      <c r="D60" s="62">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E60" s="66"/>
-      <c r="F60" s="65">
+      <c r="E60" s="63"/>
+      <c r="F60" s="62">
         <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
-      <c r="G60" s="80"/>
+      <c r="G60" s="64"/>
       <c r="H60" s="26"/>
       <c r="I60" s="12"/>
       <c r="J60" s="12"/>
@@ -12190,22 +12194,22 @@
       <c r="GI60" s="36"/>
     </row>
     <row r="61" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A61" s="81" t="s">
+      <c r="A61" s="66" t="s">
         <v>115</v>
       </c>
-      <c r="B61" s="82"/>
+      <c r="B61" s="67"/>
       <c r="C61" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="D61" s="65">
+      <c r="D61" s="62">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E61" s="66"/>
-      <c r="F61" s="65">
+      <c r="E61" s="63"/>
+      <c r="F61" s="62">
         <f>SUM(H61:GI61)</f>
         <v>1</v>
       </c>
-      <c r="G61" s="80"/>
+      <c r="G61" s="64"/>
       <c r="H61" s="26"/>
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
@@ -12394,21 +12398,21 @@
       <c r="GI61" s="36"/>
     </row>
     <row r="62" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A62" s="115" t="s">
+      <c r="A62" s="76" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="116"/>
+      <c r="B62" s="77"/>
       <c r="C62" s="39"/>
-      <c r="D62" s="71">
+      <c r="D62" s="78">
         <f>SUM(D63:E80)</f>
         <v>88.6</v>
       </c>
-      <c r="E62" s="117"/>
-      <c r="F62" s="71">
+      <c r="E62" s="79"/>
+      <c r="F62" s="78">
         <f>SUM(F63:G80)</f>
         <v>0</v>
       </c>
-      <c r="G62" s="75"/>
+      <c r="G62" s="80"/>
       <c r="H62" s="29"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
@@ -12595,22 +12599,22 @@
       <c r="GI62" s="29"/>
     </row>
     <row r="63" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="118" t="s">
+      <c r="A63" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="119"/>
+      <c r="B63" s="61"/>
       <c r="C63" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D63" s="65">
+      <c r="D63" s="62">
         <v>0.6</v>
       </c>
-      <c r="E63" s="66"/>
-      <c r="F63" s="65">
+      <c r="E63" s="63"/>
+      <c r="F63" s="62">
         <f>SUM(H63:GI63)</f>
         <v>0</v>
       </c>
-      <c r="G63" s="80"/>
+      <c r="G63" s="64"/>
       <c r="H63" s="47"/>
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
@@ -12797,22 +12801,22 @@
       <c r="GI63" s="32"/>
     </row>
     <row r="64" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="118" t="s">
+      <c r="A64" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="B64" s="119"/>
+      <c r="B64" s="61"/>
       <c r="C64" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D64" s="65">
+      <c r="D64" s="62">
         <v>1.5</v>
       </c>
-      <c r="E64" s="66"/>
-      <c r="F64" s="65">
+      <c r="E64" s="63"/>
+      <c r="F64" s="62">
         <f>SUM(H64:GI64)</f>
         <v>0</v>
       </c>
-      <c r="G64" s="80"/>
+      <c r="G64" s="64"/>
       <c r="H64" s="47"/>
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
@@ -12999,22 +13003,22 @@
       <c r="GI64" s="32"/>
     </row>
     <row r="65" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A65" s="118" t="s">
+      <c r="A65" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="B65" s="119"/>
+      <c r="B65" s="61"/>
       <c r="C65" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D65" s="65">
+      <c r="D65" s="62">
         <v>1</v>
       </c>
-      <c r="E65" s="66"/>
-      <c r="F65" s="65">
+      <c r="E65" s="63"/>
+      <c r="F65" s="62">
         <f t="shared" ref="F65:F80" si="1">SUM(H65:GI65)</f>
         <v>0</v>
       </c>
-      <c r="G65" s="80"/>
+      <c r="G65" s="64"/>
       <c r="H65" s="47"/>
       <c r="I65" s="12"/>
       <c r="J65" s="12"/>
@@ -13201,22 +13205,22 @@
       <c r="GI65" s="32"/>
     </row>
     <row r="66" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A66" s="118" t="s">
+      <c r="A66" s="60" t="s">
         <v>125</v>
       </c>
-      <c r="B66" s="119"/>
+      <c r="B66" s="61"/>
       <c r="C66" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D66" s="65">
+      <c r="D66" s="62">
         <v>0.5</v>
       </c>
-      <c r="E66" s="66"/>
-      <c r="F66" s="65">
+      <c r="E66" s="63"/>
+      <c r="F66" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G66" s="80"/>
+      <c r="G66" s="64"/>
       <c r="H66" s="47"/>
       <c r="I66" s="12"/>
       <c r="J66" s="12"/>
@@ -13403,22 +13407,22 @@
       <c r="GI66" s="32"/>
     </row>
     <row r="67" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A67" s="118" t="s">
+      <c r="A67" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="119"/>
+      <c r="B67" s="61"/>
       <c r="C67" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D67" s="65">
+      <c r="D67" s="62">
         <v>1</v>
       </c>
-      <c r="E67" s="66"/>
-      <c r="F67" s="65">
+      <c r="E67" s="63"/>
+      <c r="F67" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G67" s="80"/>
+      <c r="G67" s="64"/>
       <c r="H67" s="47"/>
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
@@ -13605,22 +13609,22 @@
       <c r="GI67" s="32"/>
     </row>
     <row r="68" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A68" s="118" t="s">
+      <c r="A68" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="B68" s="119"/>
+      <c r="B68" s="61"/>
       <c r="C68" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D68" s="65">
+      <c r="D68" s="62">
         <v>1</v>
       </c>
-      <c r="E68" s="66"/>
-      <c r="F68" s="65">
+      <c r="E68" s="63"/>
+      <c r="F68" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G68" s="80"/>
+      <c r="G68" s="64"/>
       <c r="H68" s="47"/>
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
@@ -13807,22 +13811,22 @@
       <c r="GI68" s="32"/>
     </row>
     <row r="69" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A69" s="118" t="s">
+      <c r="A69" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="B69" s="119"/>
+      <c r="B69" s="61"/>
       <c r="C69" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="D69" s="65">
+      <c r="D69" s="62">
         <v>4</v>
       </c>
-      <c r="E69" s="66"/>
-      <c r="F69" s="65">
+      <c r="E69" s="63"/>
+      <c r="F69" s="62">
         <f>SUM(H69:GI69)</f>
         <v>0</v>
       </c>
-      <c r="G69" s="80"/>
+      <c r="G69" s="64"/>
       <c r="H69" s="47"/>
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
@@ -14009,22 +14013,22 @@
       <c r="GI69" s="32"/>
     </row>
     <row r="70" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A70" s="118" t="s">
+      <c r="A70" s="60" t="s">
         <v>133</v>
       </c>
-      <c r="B70" s="119"/>
+      <c r="B70" s="61"/>
       <c r="C70" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="D70" s="65">
+      <c r="D70" s="62">
         <v>8</v>
       </c>
-      <c r="E70" s="66"/>
-      <c r="F70" s="65">
+      <c r="E70" s="63"/>
+      <c r="F70" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G70" s="80"/>
+      <c r="G70" s="64"/>
       <c r="H70" s="47"/>
       <c r="I70" s="12"/>
       <c r="J70" s="12"/>
@@ -14211,22 +14215,22 @@
       <c r="GI70" s="32"/>
     </row>
     <row r="71" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A71" s="118" t="s">
+      <c r="A71" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="B71" s="119"/>
+      <c r="B71" s="61"/>
       <c r="C71" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="D71" s="65">
+      <c r="D71" s="62">
         <v>1</v>
       </c>
-      <c r="E71" s="66"/>
-      <c r="F71" s="65">
+      <c r="E71" s="63"/>
+      <c r="F71" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G71" s="80"/>
+      <c r="G71" s="64"/>
       <c r="H71" s="47"/>
       <c r="I71" s="12"/>
       <c r="J71" s="12"/>
@@ -14413,22 +14417,22 @@
       <c r="GI71" s="32"/>
     </row>
     <row r="72" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A72" s="118" t="s">
+      <c r="A72" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="B72" s="119"/>
+      <c r="B72" s="61"/>
       <c r="C72" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="D72" s="65">
+      <c r="D72" s="62">
         <v>1</v>
       </c>
-      <c r="E72" s="66"/>
-      <c r="F72" s="65">
+      <c r="E72" s="63"/>
+      <c r="F72" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G72" s="80"/>
+      <c r="G72" s="64"/>
       <c r="H72" s="47"/>
       <c r="I72" s="12"/>
       <c r="J72" s="12"/>
@@ -14615,22 +14619,22 @@
       <c r="GI72" s="32"/>
     </row>
     <row r="73" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A73" s="118" t="s">
+      <c r="A73" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="B73" s="119"/>
+      <c r="B73" s="61"/>
       <c r="C73" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="D73" s="65">
+      <c r="D73" s="62">
         <v>4</v>
       </c>
-      <c r="E73" s="66"/>
-      <c r="F73" s="65">
+      <c r="E73" s="63"/>
+      <c r="F73" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G73" s="80"/>
+      <c r="G73" s="64"/>
       <c r="H73" s="47"/>
       <c r="I73" s="12"/>
       <c r="J73" s="12"/>
@@ -14817,22 +14821,22 @@
       <c r="GI73" s="32"/>
     </row>
     <row r="74" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A74" s="118" t="s">
+      <c r="A74" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="B74" s="119"/>
+      <c r="B74" s="61"/>
       <c r="C74" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="D74" s="65">
+      <c r="D74" s="62">
         <v>12</v>
       </c>
-      <c r="E74" s="66"/>
-      <c r="F74" s="65">
+      <c r="E74" s="63"/>
+      <c r="F74" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G74" s="80"/>
+      <c r="G74" s="64"/>
       <c r="H74" s="47"/>
       <c r="I74" s="12"/>
       <c r="J74" s="12"/>
@@ -15019,22 +15023,22 @@
       <c r="GI74" s="32"/>
     </row>
     <row r="75" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A75" s="118" t="s">
+      <c r="A75" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="B75" s="88"/>
+      <c r="B75" s="65"/>
       <c r="C75" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D75" s="65">
+      <c r="D75" s="62">
         <v>16</v>
       </c>
-      <c r="E75" s="66"/>
-      <c r="F75" s="65">
+      <c r="E75" s="63"/>
+      <c r="F75" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G75" s="80"/>
+      <c r="G75" s="64"/>
       <c r="H75" s="47"/>
       <c r="I75" s="12"/>
       <c r="J75" s="12"/>
@@ -15221,22 +15225,22 @@
       <c r="GI75" s="36"/>
     </row>
     <row r="76" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A76" s="118" t="s">
+      <c r="A76" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="B76" s="119"/>
+      <c r="B76" s="61"/>
       <c r="C76" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="D76" s="65">
+      <c r="D76" s="62">
         <v>5</v>
       </c>
-      <c r="E76" s="66"/>
-      <c r="F76" s="65">
+      <c r="E76" s="63"/>
+      <c r="F76" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G76" s="80"/>
+      <c r="G76" s="64"/>
       <c r="H76" s="47"/>
       <c r="I76" s="12"/>
       <c r="J76" s="12"/>
@@ -15423,22 +15427,22 @@
       <c r="GI76" s="32"/>
     </row>
     <row r="77" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A77" s="118" t="s">
+      <c r="A77" s="60" t="s">
         <v>146</v>
       </c>
-      <c r="B77" s="119"/>
+      <c r="B77" s="61"/>
       <c r="C77" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="D77" s="65">
+      <c r="D77" s="62">
         <v>4</v>
       </c>
-      <c r="E77" s="66"/>
-      <c r="F77" s="65">
+      <c r="E77" s="63"/>
+      <c r="F77" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G77" s="80"/>
+      <c r="G77" s="64"/>
       <c r="H77" s="47"/>
       <c r="I77" s="12"/>
       <c r="J77" s="12"/>
@@ -15625,22 +15629,22 @@
       <c r="GI77" s="32"/>
     </row>
     <row r="78" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A78" s="118" t="s">
+      <c r="A78" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="B78" s="119"/>
+      <c r="B78" s="61"/>
       <c r="C78" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="D78" s="65">
+      <c r="D78" s="62">
         <v>16</v>
       </c>
-      <c r="E78" s="66"/>
-      <c r="F78" s="65">
+      <c r="E78" s="63"/>
+      <c r="F78" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G78" s="80"/>
+      <c r="G78" s="64"/>
       <c r="H78" s="47"/>
       <c r="I78" s="12"/>
       <c r="J78" s="12"/>
@@ -15827,22 +15831,22 @@
       <c r="GI78" s="32"/>
     </row>
     <row r="79" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A79" s="73" t="s">
+      <c r="A79" s="82" t="s">
         <v>150</v>
       </c>
-      <c r="B79" s="74"/>
+      <c r="B79" s="83"/>
       <c r="C79" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="D79" s="65">
+      <c r="D79" s="62">
         <v>6</v>
       </c>
-      <c r="E79" s="66"/>
-      <c r="F79" s="65">
+      <c r="E79" s="63"/>
+      <c r="F79" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G79" s="80"/>
+      <c r="G79" s="64"/>
       <c r="H79" s="47"/>
       <c r="I79" s="12"/>
       <c r="J79" s="12"/>
@@ -16029,22 +16033,22 @@
       <c r="GI79" s="36"/>
     </row>
     <row r="80" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A80" s="73" t="s">
+      <c r="A80" s="82" t="s">
         <v>152</v>
       </c>
-      <c r="B80" s="74"/>
+      <c r="B80" s="83"/>
       <c r="C80" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D80" s="65">
+      <c r="D80" s="62">
         <v>6</v>
       </c>
-      <c r="E80" s="66"/>
-      <c r="F80" s="65">
+      <c r="E80" s="63"/>
+      <c r="F80" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G80" s="80"/>
+      <c r="G80" s="64"/>
       <c r="H80" s="47"/>
       <c r="I80" s="12"/>
       <c r="J80" s="12"/>
@@ -16231,21 +16235,21 @@
       <c r="GI80" s="36"/>
     </row>
     <row r="81" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A81" s="115" t="s">
+      <c r="A81" s="76" t="s">
         <v>153</v>
       </c>
-      <c r="B81" s="116"/>
+      <c r="B81" s="77"/>
       <c r="C81" s="39"/>
-      <c r="D81" s="71">
+      <c r="D81" s="78">
         <f>SUM(D82:E82)</f>
         <v>16</v>
       </c>
-      <c r="E81" s="72"/>
-      <c r="F81" s="71">
+      <c r="E81" s="88"/>
+      <c r="F81" s="78">
         <f>SUM(F82:G82)</f>
         <v>0</v>
       </c>
-      <c r="G81" s="75"/>
+      <c r="G81" s="80"/>
       <c r="H81" s="29"/>
       <c r="I81" s="8"/>
       <c r="J81" s="8"/>
@@ -16432,20 +16436,20 @@
       <c r="GI81" s="29"/>
     </row>
     <row r="82" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A82" s="93" t="s">
+      <c r="A82" s="86" t="s">
         <v>153</v>
       </c>
-      <c r="B82" s="94"/>
+      <c r="B82" s="87"/>
       <c r="C82" s="40"/>
-      <c r="D82" s="91">
+      <c r="D82" s="84">
         <v>16</v>
       </c>
-      <c r="E82" s="92"/>
-      <c r="F82" s="65">
+      <c r="E82" s="85"/>
+      <c r="F82" s="62">
         <f>SUM(H82:GI82)</f>
         <v>0</v>
       </c>
-      <c r="G82" s="80"/>
+      <c r="G82" s="64"/>
       <c r="H82" s="26"/>
       <c r="I82" s="12"/>
       <c r="J82" s="12"/>
@@ -16632,21 +16636,21 @@
       <c r="GI82" s="32"/>
     </row>
     <row r="83" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A83" s="110" t="s">
+      <c r="A83" s="104" t="s">
         <v>154</v>
       </c>
-      <c r="B83" s="111"/>
+      <c r="B83" s="105"/>
       <c r="C83" s="41"/>
-      <c r="D83" s="71">
+      <c r="D83" s="78">
         <f>SUM(D84:E84)</f>
         <v>32</v>
       </c>
-      <c r="E83" s="72"/>
-      <c r="F83" s="71">
+      <c r="E83" s="88"/>
+      <c r="F83" s="78">
         <f>SUM(F84:G84)</f>
         <v>0</v>
       </c>
-      <c r="G83" s="75"/>
+      <c r="G83" s="80"/>
       <c r="H83" s="29"/>
       <c r="I83" s="8"/>
       <c r="J83" s="8"/>
@@ -16833,20 +16837,20 @@
       <c r="GI83" s="29"/>
     </row>
     <row r="84" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A84" s="85" t="s">
+      <c r="A84" s="108" t="s">
         <v>154</v>
       </c>
-      <c r="B84" s="86"/>
+      <c r="B84" s="109"/>
       <c r="C84" s="42"/>
-      <c r="D84" s="65">
+      <c r="D84" s="62">
         <v>32</v>
       </c>
-      <c r="E84" s="66"/>
-      <c r="F84" s="65">
+      <c r="E84" s="63"/>
+      <c r="F84" s="62">
         <f>SUM(H84:GI84)</f>
         <v>0</v>
       </c>
-      <c r="G84" s="80"/>
+      <c r="G84" s="64"/>
       <c r="H84" s="26"/>
       <c r="I84" s="12"/>
       <c r="J84" s="12"/>
@@ -17033,21 +17037,21 @@
       <c r="GI84" s="32"/>
     </row>
     <row r="85" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A85" s="89" t="s">
+      <c r="A85" s="111" t="s">
         <v>155</v>
       </c>
-      <c r="B85" s="90"/>
+      <c r="B85" s="112"/>
       <c r="C85" s="43"/>
-      <c r="D85" s="71">
+      <c r="D85" s="78">
         <f>SUM(D86:E86)</f>
         <v>8</v>
       </c>
-      <c r="E85" s="72"/>
-      <c r="F85" s="95">
+      <c r="E85" s="88"/>
+      <c r="F85" s="89">
         <f>SUM(F86:G86)</f>
         <v>0</v>
       </c>
-      <c r="G85" s="96"/>
+      <c r="G85" s="90"/>
       <c r="H85" s="29"/>
       <c r="I85" s="8"/>
       <c r="J85" s="8"/>
@@ -17234,20 +17238,20 @@
       <c r="GI85" s="29"/>
     </row>
     <row r="86" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A86" s="87" t="s">
+      <c r="A86" s="110" t="s">
         <v>156</v>
       </c>
-      <c r="B86" s="88"/>
+      <c r="B86" s="65"/>
       <c r="C86" s="27"/>
-      <c r="D86" s="65">
+      <c r="D86" s="62">
         <v>8</v>
       </c>
-      <c r="E86" s="66"/>
-      <c r="F86" s="65">
+      <c r="E86" s="63"/>
+      <c r="F86" s="62">
         <f>SUM(H86:GI86)</f>
         <v>0</v>
       </c>
-      <c r="G86" s="80"/>
+      <c r="G86" s="64"/>
       <c r="H86" s="26"/>
       <c r="I86" s="12"/>
       <c r="J86" s="12"/>
@@ -17434,20 +17438,20 @@
       <c r="GI86" s="32"/>
     </row>
     <row r="87" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A87" s="83" t="s">
+      <c r="A87" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="84"/>
+      <c r="B87" s="107"/>
       <c r="C87" s="43"/>
-      <c r="D87" s="71">
+      <c r="D87" s="78">
         <f>232-D90</f>
         <v>36.349999999999994</v>
       </c>
-      <c r="E87" s="72"/>
-      <c r="F87" s="71">
+      <c r="E87" s="88"/>
+      <c r="F87" s="78">
         <v>0</v>
       </c>
-      <c r="G87" s="75"/>
+      <c r="G87" s="80"/>
       <c r="H87" s="29"/>
       <c r="I87" s="8"/>
       <c r="J87" s="8"/>
@@ -17634,15 +17638,15 @@
       <c r="GI87" s="29"/>
     </row>
     <row r="88" spans="1:191" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="107" t="s">
+      <c r="A88" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="B88" s="108"/>
+      <c r="B88" s="102"/>
       <c r="C88" s="44"/>
-      <c r="D88" s="104"/>
-      <c r="E88" s="105"/>
-      <c r="F88" s="104"/>
-      <c r="G88" s="106"/>
+      <c r="D88" s="98"/>
+      <c r="E88" s="99"/>
+      <c r="F88" s="98"/>
+      <c r="G88" s="100"/>
       <c r="H88" s="28"/>
       <c r="I88" s="17"/>
       <c r="J88" s="17"/>
@@ -17881,21 +17885,21 @@
       <c r="AX89" s="3"/>
     </row>
     <row r="90" spans="1:191" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="102" t="s">
+      <c r="A90" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="103"/>
+      <c r="B90" s="97"/>
       <c r="C90" s="45"/>
-      <c r="D90" s="100">
+      <c r="D90" s="94">
         <f>SUM(D85,D83,D81,D62,D14)</f>
         <v>195.65</v>
       </c>
-      <c r="E90" s="101"/>
-      <c r="F90" s="100">
+      <c r="E90" s="95"/>
+      <c r="F90" s="94">
         <f>SUM(F85,F83,F81,F62,F14)</f>
-        <v>33.916000000000004</v>
-      </c>
-      <c r="G90" s="109"/>
+        <v>34.249000000000002</v>
+      </c>
+      <c r="G90" s="103"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
@@ -17942,132 +17946,190 @@
     </row>
   </sheetData>
   <mergeCells count="334">
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="BR13:BS13"/>
+    <mergeCell ref="BL13:BM13"/>
+    <mergeCell ref="BN13:BO13"/>
+    <mergeCell ref="BR12:DY12"/>
+    <mergeCell ref="DZ13:EA13"/>
+    <mergeCell ref="CL13:CM13"/>
+    <mergeCell ref="CN13:CO13"/>
+    <mergeCell ref="BT13:BU13"/>
+    <mergeCell ref="BV13:BW13"/>
+    <mergeCell ref="BX13:BY13"/>
+    <mergeCell ref="BZ13:CA13"/>
+    <mergeCell ref="CB13:CC13"/>
+    <mergeCell ref="CD13:CE13"/>
+    <mergeCell ref="CF13:CG13"/>
+    <mergeCell ref="CH13:CI13"/>
+    <mergeCell ref="CJ13:CK13"/>
+    <mergeCell ref="CP13:CQ13"/>
+    <mergeCell ref="CR13:CS13"/>
+    <mergeCell ref="CT13:CU13"/>
+    <mergeCell ref="CV13:CW13"/>
+    <mergeCell ref="CX13:CY13"/>
+    <mergeCell ref="CZ13:DA13"/>
+    <mergeCell ref="DB13:DC13"/>
+    <mergeCell ref="DD13:DE13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="P6:X6"/>
+    <mergeCell ref="P5:X5"/>
+    <mergeCell ref="P4:X4"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="H12:BQ12"/>
+    <mergeCell ref="BB13:BC13"/>
+    <mergeCell ref="BD13:BE13"/>
+    <mergeCell ref="BF13:BG13"/>
+    <mergeCell ref="BP13:BQ13"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="AF13:AG13"/>
+    <mergeCell ref="AH13:AI13"/>
+    <mergeCell ref="AJ13:AK13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="AL13:AM13"/>
+    <mergeCell ref="AN13:AO13"/>
+    <mergeCell ref="AP13:AQ13"/>
+    <mergeCell ref="AR13:AS13"/>
+    <mergeCell ref="AT13:AU13"/>
+    <mergeCell ref="AV13:AW13"/>
+    <mergeCell ref="AX13:AY13"/>
+    <mergeCell ref="AZ13:BA13"/>
+    <mergeCell ref="BH13:BI13"/>
+    <mergeCell ref="BJ13:BK13"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="P9:X9"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F11:G13"/>
+    <mergeCell ref="D11:E13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="DF13:DG13"/>
+    <mergeCell ref="DH13:DI13"/>
+    <mergeCell ref="DJ13:DK13"/>
+    <mergeCell ref="DL13:DM13"/>
+    <mergeCell ref="DN13:DO13"/>
+    <mergeCell ref="DP13:DQ13"/>
+    <mergeCell ref="DR13:DS13"/>
+    <mergeCell ref="DT13:DU13"/>
+    <mergeCell ref="DV13:DW13"/>
+    <mergeCell ref="FF13:FG13"/>
+    <mergeCell ref="DX13:DY13"/>
+    <mergeCell ref="FH13:FI13"/>
+    <mergeCell ref="FJ13:FK13"/>
+    <mergeCell ref="EB13:EC13"/>
+    <mergeCell ref="ED13:EE13"/>
+    <mergeCell ref="EF13:EG13"/>
+    <mergeCell ref="EH13:EI13"/>
+    <mergeCell ref="EJ13:EK13"/>
+    <mergeCell ref="EL13:EM13"/>
+    <mergeCell ref="EN13:EO13"/>
+    <mergeCell ref="EP13:EQ13"/>
+    <mergeCell ref="ER13:ES13"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="GD13:GE13"/>
+    <mergeCell ref="GF13:GG13"/>
+    <mergeCell ref="GH13:GI13"/>
+    <mergeCell ref="DZ12:GI12"/>
+    <mergeCell ref="FL13:FM13"/>
+    <mergeCell ref="FN13:FO13"/>
+    <mergeCell ref="FP13:FQ13"/>
+    <mergeCell ref="FR13:FS13"/>
+    <mergeCell ref="FT13:FU13"/>
+    <mergeCell ref="FV13:FW13"/>
+    <mergeCell ref="FX13:FY13"/>
+    <mergeCell ref="FZ13:GA13"/>
+    <mergeCell ref="GB13:GC13"/>
+    <mergeCell ref="ET13:EU13"/>
+    <mergeCell ref="EV13:EW13"/>
+    <mergeCell ref="EX13:EY13"/>
+    <mergeCell ref="EZ13:FA13"/>
+    <mergeCell ref="FB13:FC13"/>
+    <mergeCell ref="FD13:FE13"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="D32:E32"/>
@@ -18092,190 +18154,132 @@
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="GD13:GE13"/>
-    <mergeCell ref="GF13:GG13"/>
-    <mergeCell ref="GH13:GI13"/>
-    <mergeCell ref="DZ12:GI12"/>
-    <mergeCell ref="FL13:FM13"/>
-    <mergeCell ref="FN13:FO13"/>
-    <mergeCell ref="FP13:FQ13"/>
-    <mergeCell ref="FR13:FS13"/>
-    <mergeCell ref="FT13:FU13"/>
-    <mergeCell ref="FV13:FW13"/>
-    <mergeCell ref="FX13:FY13"/>
-    <mergeCell ref="FZ13:GA13"/>
-    <mergeCell ref="GB13:GC13"/>
-    <mergeCell ref="ET13:EU13"/>
-    <mergeCell ref="EV13:EW13"/>
-    <mergeCell ref="EX13:EY13"/>
-    <mergeCell ref="EZ13:FA13"/>
-    <mergeCell ref="FB13:FC13"/>
-    <mergeCell ref="FD13:FE13"/>
-    <mergeCell ref="FF13:FG13"/>
-    <mergeCell ref="DX13:DY13"/>
-    <mergeCell ref="FH13:FI13"/>
-    <mergeCell ref="FJ13:FK13"/>
-    <mergeCell ref="EB13:EC13"/>
-    <mergeCell ref="ED13:EE13"/>
-    <mergeCell ref="EF13:EG13"/>
-    <mergeCell ref="EH13:EI13"/>
-    <mergeCell ref="EJ13:EK13"/>
-    <mergeCell ref="EL13:EM13"/>
-    <mergeCell ref="EN13:EO13"/>
-    <mergeCell ref="EP13:EQ13"/>
-    <mergeCell ref="ER13:ES13"/>
-    <mergeCell ref="DF13:DG13"/>
-    <mergeCell ref="DH13:DI13"/>
-    <mergeCell ref="DJ13:DK13"/>
-    <mergeCell ref="DL13:DM13"/>
-    <mergeCell ref="DN13:DO13"/>
-    <mergeCell ref="DP13:DQ13"/>
-    <mergeCell ref="DR13:DS13"/>
-    <mergeCell ref="DT13:DU13"/>
-    <mergeCell ref="DV13:DW13"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="F90:G90"/>
-    <mergeCell ref="F87:G87"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="BH13:BI13"/>
-    <mergeCell ref="BJ13:BK13"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="P9:X9"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F11:G13"/>
-    <mergeCell ref="D11:E13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="AL13:AM13"/>
-    <mergeCell ref="AN13:AO13"/>
-    <mergeCell ref="AP13:AQ13"/>
-    <mergeCell ref="AR13:AS13"/>
-    <mergeCell ref="AT13:AU13"/>
-    <mergeCell ref="AV13:AW13"/>
-    <mergeCell ref="AX13:AY13"/>
-    <mergeCell ref="AZ13:BA13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="P6:X6"/>
-    <mergeCell ref="P5:X5"/>
-    <mergeCell ref="P4:X4"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="H12:BQ12"/>
-    <mergeCell ref="BB13:BC13"/>
-    <mergeCell ref="BD13:BE13"/>
-    <mergeCell ref="BF13:BG13"/>
-    <mergeCell ref="BP13:BQ13"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="AF13:AG13"/>
-    <mergeCell ref="AH13:AI13"/>
-    <mergeCell ref="AJ13:AK13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="BR13:BS13"/>
-    <mergeCell ref="BL13:BM13"/>
-    <mergeCell ref="BN13:BO13"/>
-    <mergeCell ref="BR12:DY12"/>
-    <mergeCell ref="DZ13:EA13"/>
-    <mergeCell ref="CL13:CM13"/>
-    <mergeCell ref="CN13:CO13"/>
-    <mergeCell ref="BT13:BU13"/>
-    <mergeCell ref="BV13:BW13"/>
-    <mergeCell ref="BX13:BY13"/>
-    <mergeCell ref="BZ13:CA13"/>
-    <mergeCell ref="CB13:CC13"/>
-    <mergeCell ref="CD13:CE13"/>
-    <mergeCell ref="CF13:CG13"/>
-    <mergeCell ref="CH13:CI13"/>
-    <mergeCell ref="CJ13:CK13"/>
-    <mergeCell ref="CP13:CQ13"/>
-    <mergeCell ref="CR13:CS13"/>
-    <mergeCell ref="CT13:CU13"/>
-    <mergeCell ref="CV13:CW13"/>
-    <mergeCell ref="CX13:CY13"/>
-    <mergeCell ref="CZ13:DA13"/>
-    <mergeCell ref="DB13:DC13"/>
-    <mergeCell ref="DD13:DE13"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Created Model for Issue #42 Didn't make a Watertower -> Water Diplay instead
</commit_message>
<xml_diff>
--- a/Documents/Zeitplan.xlsx
+++ b/Documents/Zeitplan.xlsx
@@ -1164,24 +1164,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1194,31 +1176,32 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1226,6 +1209,42 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1234,9 +1253,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1284,40 +1300,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1787,8 +1787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GI90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AM25" sqref="AM25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AM30" sqref="AM30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1801,28 +1801,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:191" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
     </row>
     <row r="2" spans="1:191" x14ac:dyDescent="0.25">
       <c r="T2" s="9"/>
@@ -1855,17 +1855,17 @@
         <v>160</v>
       </c>
       <c r="N4" s="57"/>
-      <c r="P4" s="81" t="s">
+      <c r="P4" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="81"/>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="67"/>
+      <c r="V4" s="67"/>
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
     </row>
     <row r="5" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -1882,17 +1882,17 @@
       <c r="F5" s="5"/>
       <c r="G5" s="7"/>
       <c r="N5" s="24"/>
-      <c r="P5" s="81" t="s">
+      <c r="P5" s="67" t="s">
         <v>158</v>
       </c>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81"/>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="81"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
+      <c r="S5" s="67"/>
+      <c r="T5" s="67"/>
+      <c r="U5" s="67"/>
+      <c r="V5" s="67"/>
+      <c r="W5" s="67"/>
+      <c r="X5" s="67"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
@@ -1916,17 +1916,17 @@
         <v>15</v>
       </c>
       <c r="N6" s="16"/>
-      <c r="P6" s="81" t="s">
+      <c r="P6" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="81"/>
-      <c r="T6" s="81"/>
-      <c r="U6" s="81"/>
-      <c r="V6" s="81"/>
-      <c r="W6" s="81"/>
-      <c r="X6" s="81"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="67"/>
+      <c r="V6" s="67"/>
+      <c r="W6" s="67"/>
+      <c r="X6" s="67"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
@@ -1944,17 +1944,17 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="N7" s="21"/>
-      <c r="P7" s="81" t="s">
+      <c r="P7" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="81"/>
-      <c r="S7" s="81"/>
-      <c r="T7" s="81"/>
-      <c r="U7" s="81"/>
-      <c r="V7" s="81"/>
-      <c r="W7" s="81"/>
-      <c r="X7" s="81"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="67"/>
+      <c r="S7" s="67"/>
+      <c r="T7" s="67"/>
+      <c r="U7" s="67"/>
+      <c r="V7" s="67"/>
+      <c r="W7" s="67"/>
+      <c r="X7" s="67"/>
     </row>
     <row r="8" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1969,17 +1969,17 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="N8" s="20"/>
-      <c r="P8" s="113" t="s">
+      <c r="P8" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="113"/>
-      <c r="R8" s="113"/>
-      <c r="S8" s="113"/>
-      <c r="T8" s="113"/>
-      <c r="U8" s="113"/>
-      <c r="V8" s="113"/>
-      <c r="W8" s="113"/>
-      <c r="X8" s="113"/>
+      <c r="Q8" s="70"/>
+      <c r="R8" s="70"/>
+      <c r="S8" s="70"/>
+      <c r="T8" s="70"/>
+      <c r="U8" s="70"/>
+      <c r="V8" s="70"/>
+      <c r="W8" s="70"/>
+      <c r="X8" s="70"/>
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
@@ -1987,23 +1987,23 @@
       <c r="AC8" s="5"/>
     </row>
     <row r="9" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="118"/>
+      <c r="A9" s="68"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="12"/>
       <c r="N9" s="49"/>
-      <c r="P9" s="113" t="s">
+      <c r="P9" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="Q9" s="113"/>
-      <c r="R9" s="113"/>
-      <c r="S9" s="113"/>
-      <c r="T9" s="113"/>
-      <c r="U9" s="113"/>
-      <c r="V9" s="113"/>
-      <c r="W9" s="113"/>
-      <c r="X9" s="113"/>
+      <c r="Q9" s="70"/>
+      <c r="R9" s="70"/>
+      <c r="S9" s="70"/>
+      <c r="T9" s="70"/>
+      <c r="U9" s="70"/>
+      <c r="V9" s="70"/>
+      <c r="W9" s="70"/>
+      <c r="X9" s="70"/>
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
@@ -2013,7 +2013,7 @@
       <c r="AJ9" s="13"/>
     </row>
     <row r="10" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="118"/>
+      <c r="A10" s="68"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -2030,18 +2030,18 @@
       <c r="AC10" s="5"/>
     </row>
     <row r="11" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="118"/>
-      <c r="C11" s="116" t="s">
+      <c r="A11" s="68"/>
+      <c r="C11" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="114" t="s">
+      <c r="D11" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="114"/>
-      <c r="F11" s="114" t="s">
+      <c r="E11" s="76"/>
+      <c r="F11" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="114"/>
+      <c r="G11" s="76"/>
       <c r="T11" s="9"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
@@ -2054,596 +2054,596 @@
       <c r="AC11" s="5"/>
     </row>
     <row r="12" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="118"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="114"/>
-      <c r="G12" s="114"/>
-      <c r="H12" s="70" t="s">
+      <c r="A12" s="68"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="71"/>
-      <c r="N12" s="71"/>
-      <c r="O12" s="71"/>
-      <c r="P12" s="71"/>
-      <c r="Q12" s="71"/>
-      <c r="R12" s="71"/>
-      <c r="S12" s="71"/>
-      <c r="T12" s="71"/>
-      <c r="U12" s="71"/>
-      <c r="V12" s="71"/>
-      <c r="W12" s="71"/>
-      <c r="X12" s="71"/>
-      <c r="Y12" s="71"/>
-      <c r="Z12" s="71"/>
-      <c r="AA12" s="71"/>
-      <c r="AB12" s="71"/>
-      <c r="AC12" s="71"/>
-      <c r="AD12" s="71"/>
-      <c r="AE12" s="71"/>
-      <c r="AF12" s="71"/>
-      <c r="AG12" s="71"/>
-      <c r="AH12" s="71"/>
-      <c r="AI12" s="71"/>
-      <c r="AJ12" s="71"/>
-      <c r="AK12" s="71"/>
-      <c r="AL12" s="71"/>
-      <c r="AM12" s="71"/>
-      <c r="AN12" s="71"/>
-      <c r="AO12" s="71"/>
-      <c r="AP12" s="71"/>
-      <c r="AQ12" s="71"/>
-      <c r="AR12" s="71"/>
-      <c r="AS12" s="71"/>
-      <c r="AT12" s="71"/>
-      <c r="AU12" s="71"/>
-      <c r="AV12" s="71"/>
-      <c r="AW12" s="71"/>
-      <c r="AX12" s="71"/>
-      <c r="AY12" s="71"/>
-      <c r="AZ12" s="71"/>
-      <c r="BA12" s="71"/>
-      <c r="BB12" s="71"/>
-      <c r="BC12" s="71"/>
-      <c r="BD12" s="71"/>
-      <c r="BE12" s="71"/>
-      <c r="BF12" s="71"/>
-      <c r="BG12" s="71"/>
-      <c r="BH12" s="71"/>
-      <c r="BI12" s="71"/>
-      <c r="BJ12" s="71"/>
-      <c r="BK12" s="71"/>
-      <c r="BL12" s="71"/>
-      <c r="BM12" s="71"/>
-      <c r="BN12" s="71"/>
-      <c r="BO12" s="71"/>
-      <c r="BP12" s="71"/>
-      <c r="BQ12" s="119"/>
-      <c r="BR12" s="70" t="s">
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="63"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="63"/>
+      <c r="W12" s="63"/>
+      <c r="X12" s="63"/>
+      <c r="Y12" s="63"/>
+      <c r="Z12" s="63"/>
+      <c r="AA12" s="63"/>
+      <c r="AB12" s="63"/>
+      <c r="AC12" s="63"/>
+      <c r="AD12" s="63"/>
+      <c r="AE12" s="63"/>
+      <c r="AF12" s="63"/>
+      <c r="AG12" s="63"/>
+      <c r="AH12" s="63"/>
+      <c r="AI12" s="63"/>
+      <c r="AJ12" s="63"/>
+      <c r="AK12" s="63"/>
+      <c r="AL12" s="63"/>
+      <c r="AM12" s="63"/>
+      <c r="AN12" s="63"/>
+      <c r="AO12" s="63"/>
+      <c r="AP12" s="63"/>
+      <c r="AQ12" s="63"/>
+      <c r="AR12" s="63"/>
+      <c r="AS12" s="63"/>
+      <c r="AT12" s="63"/>
+      <c r="AU12" s="63"/>
+      <c r="AV12" s="63"/>
+      <c r="AW12" s="63"/>
+      <c r="AX12" s="63"/>
+      <c r="AY12" s="63"/>
+      <c r="AZ12" s="63"/>
+      <c r="BA12" s="63"/>
+      <c r="BB12" s="63"/>
+      <c r="BC12" s="63"/>
+      <c r="BD12" s="63"/>
+      <c r="BE12" s="63"/>
+      <c r="BF12" s="63"/>
+      <c r="BG12" s="63"/>
+      <c r="BH12" s="63"/>
+      <c r="BI12" s="63"/>
+      <c r="BJ12" s="63"/>
+      <c r="BK12" s="63"/>
+      <c r="BL12" s="63"/>
+      <c r="BM12" s="63"/>
+      <c r="BN12" s="63"/>
+      <c r="BO12" s="63"/>
+      <c r="BP12" s="63"/>
+      <c r="BQ12" s="64"/>
+      <c r="BR12" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="BS12" s="71"/>
-      <c r="BT12" s="71"/>
-      <c r="BU12" s="71"/>
-      <c r="BV12" s="71"/>
-      <c r="BW12" s="71"/>
-      <c r="BX12" s="71"/>
-      <c r="BY12" s="71"/>
-      <c r="BZ12" s="71"/>
-      <c r="CA12" s="71"/>
-      <c r="CB12" s="71"/>
-      <c r="CC12" s="71"/>
-      <c r="CD12" s="71"/>
-      <c r="CE12" s="71"/>
-      <c r="CF12" s="71"/>
-      <c r="CG12" s="71"/>
-      <c r="CH12" s="71"/>
-      <c r="CI12" s="71"/>
-      <c r="CJ12" s="71"/>
-      <c r="CK12" s="71"/>
-      <c r="CL12" s="71"/>
-      <c r="CM12" s="71"/>
-      <c r="CN12" s="71"/>
-      <c r="CO12" s="71"/>
-      <c r="CP12" s="71"/>
-      <c r="CQ12" s="71"/>
-      <c r="CR12" s="71"/>
-      <c r="CS12" s="71"/>
-      <c r="CT12" s="71"/>
-      <c r="CU12" s="71"/>
-      <c r="CV12" s="71"/>
-      <c r="CW12" s="71"/>
-      <c r="CX12" s="71"/>
-      <c r="CY12" s="71"/>
-      <c r="CZ12" s="71"/>
-      <c r="DA12" s="71"/>
-      <c r="DB12" s="71"/>
-      <c r="DC12" s="71"/>
-      <c r="DD12" s="71"/>
-      <c r="DE12" s="71"/>
-      <c r="DF12" s="71"/>
-      <c r="DG12" s="71"/>
-      <c r="DH12" s="71"/>
-      <c r="DI12" s="71"/>
-      <c r="DJ12" s="71"/>
-      <c r="DK12" s="71"/>
-      <c r="DL12" s="71"/>
-      <c r="DM12" s="71"/>
-      <c r="DN12" s="71"/>
-      <c r="DO12" s="71"/>
-      <c r="DP12" s="71"/>
-      <c r="DQ12" s="71"/>
-      <c r="DR12" s="71"/>
-      <c r="DS12" s="71"/>
-      <c r="DT12" s="71"/>
-      <c r="DU12" s="71"/>
-      <c r="DV12" s="71"/>
-      <c r="DW12" s="71"/>
-      <c r="DX12" s="71"/>
-      <c r="DY12" s="119"/>
-      <c r="DZ12" s="70" t="s">
+      <c r="BS12" s="63"/>
+      <c r="BT12" s="63"/>
+      <c r="BU12" s="63"/>
+      <c r="BV12" s="63"/>
+      <c r="BW12" s="63"/>
+      <c r="BX12" s="63"/>
+      <c r="BY12" s="63"/>
+      <c r="BZ12" s="63"/>
+      <c r="CA12" s="63"/>
+      <c r="CB12" s="63"/>
+      <c r="CC12" s="63"/>
+      <c r="CD12" s="63"/>
+      <c r="CE12" s="63"/>
+      <c r="CF12" s="63"/>
+      <c r="CG12" s="63"/>
+      <c r="CH12" s="63"/>
+      <c r="CI12" s="63"/>
+      <c r="CJ12" s="63"/>
+      <c r="CK12" s="63"/>
+      <c r="CL12" s="63"/>
+      <c r="CM12" s="63"/>
+      <c r="CN12" s="63"/>
+      <c r="CO12" s="63"/>
+      <c r="CP12" s="63"/>
+      <c r="CQ12" s="63"/>
+      <c r="CR12" s="63"/>
+      <c r="CS12" s="63"/>
+      <c r="CT12" s="63"/>
+      <c r="CU12" s="63"/>
+      <c r="CV12" s="63"/>
+      <c r="CW12" s="63"/>
+      <c r="CX12" s="63"/>
+      <c r="CY12" s="63"/>
+      <c r="CZ12" s="63"/>
+      <c r="DA12" s="63"/>
+      <c r="DB12" s="63"/>
+      <c r="DC12" s="63"/>
+      <c r="DD12" s="63"/>
+      <c r="DE12" s="63"/>
+      <c r="DF12" s="63"/>
+      <c r="DG12" s="63"/>
+      <c r="DH12" s="63"/>
+      <c r="DI12" s="63"/>
+      <c r="DJ12" s="63"/>
+      <c r="DK12" s="63"/>
+      <c r="DL12" s="63"/>
+      <c r="DM12" s="63"/>
+      <c r="DN12" s="63"/>
+      <c r="DO12" s="63"/>
+      <c r="DP12" s="63"/>
+      <c r="DQ12" s="63"/>
+      <c r="DR12" s="63"/>
+      <c r="DS12" s="63"/>
+      <c r="DT12" s="63"/>
+      <c r="DU12" s="63"/>
+      <c r="DV12" s="63"/>
+      <c r="DW12" s="63"/>
+      <c r="DX12" s="63"/>
+      <c r="DY12" s="64"/>
+      <c r="DZ12" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="EA12" s="71"/>
-      <c r="EB12" s="71"/>
-      <c r="EC12" s="71"/>
-      <c r="ED12" s="71"/>
-      <c r="EE12" s="71"/>
-      <c r="EF12" s="71"/>
-      <c r="EG12" s="71"/>
-      <c r="EH12" s="71"/>
-      <c r="EI12" s="71"/>
-      <c r="EJ12" s="71"/>
-      <c r="EK12" s="71"/>
-      <c r="EL12" s="71"/>
-      <c r="EM12" s="71"/>
-      <c r="EN12" s="71"/>
-      <c r="EO12" s="71"/>
-      <c r="EP12" s="71"/>
-      <c r="EQ12" s="71"/>
-      <c r="ER12" s="71"/>
-      <c r="ES12" s="71"/>
-      <c r="ET12" s="71"/>
-      <c r="EU12" s="71"/>
-      <c r="EV12" s="71"/>
-      <c r="EW12" s="71"/>
-      <c r="EX12" s="71"/>
-      <c r="EY12" s="71"/>
-      <c r="EZ12" s="71"/>
-      <c r="FA12" s="71"/>
-      <c r="FB12" s="71"/>
-      <c r="FC12" s="71"/>
-      <c r="FD12" s="71"/>
-      <c r="FE12" s="71"/>
-      <c r="FF12" s="71"/>
-      <c r="FG12" s="71"/>
-      <c r="FH12" s="71"/>
-      <c r="FI12" s="71"/>
-      <c r="FJ12" s="71"/>
-      <c r="FK12" s="71"/>
-      <c r="FL12" s="71"/>
-      <c r="FM12" s="71"/>
-      <c r="FN12" s="71"/>
-      <c r="FO12" s="71"/>
-      <c r="FP12" s="71"/>
-      <c r="FQ12" s="71"/>
-      <c r="FR12" s="71"/>
-      <c r="FS12" s="71"/>
-      <c r="FT12" s="71"/>
-      <c r="FU12" s="71"/>
-      <c r="FV12" s="71"/>
-      <c r="FW12" s="71"/>
-      <c r="FX12" s="71"/>
-      <c r="FY12" s="71"/>
-      <c r="FZ12" s="71"/>
-      <c r="GA12" s="71"/>
-      <c r="GB12" s="71"/>
-      <c r="GC12" s="71"/>
-      <c r="GD12" s="71"/>
-      <c r="GE12" s="71"/>
-      <c r="GF12" s="71"/>
-      <c r="GG12" s="71"/>
-      <c r="GH12" s="71"/>
-      <c r="GI12" s="72"/>
+      <c r="EA12" s="63"/>
+      <c r="EB12" s="63"/>
+      <c r="EC12" s="63"/>
+      <c r="ED12" s="63"/>
+      <c r="EE12" s="63"/>
+      <c r="EF12" s="63"/>
+      <c r="EG12" s="63"/>
+      <c r="EH12" s="63"/>
+      <c r="EI12" s="63"/>
+      <c r="EJ12" s="63"/>
+      <c r="EK12" s="63"/>
+      <c r="EL12" s="63"/>
+      <c r="EM12" s="63"/>
+      <c r="EN12" s="63"/>
+      <c r="EO12" s="63"/>
+      <c r="EP12" s="63"/>
+      <c r="EQ12" s="63"/>
+      <c r="ER12" s="63"/>
+      <c r="ES12" s="63"/>
+      <c r="ET12" s="63"/>
+      <c r="EU12" s="63"/>
+      <c r="EV12" s="63"/>
+      <c r="EW12" s="63"/>
+      <c r="EX12" s="63"/>
+      <c r="EY12" s="63"/>
+      <c r="EZ12" s="63"/>
+      <c r="FA12" s="63"/>
+      <c r="FB12" s="63"/>
+      <c r="FC12" s="63"/>
+      <c r="FD12" s="63"/>
+      <c r="FE12" s="63"/>
+      <c r="FF12" s="63"/>
+      <c r="FG12" s="63"/>
+      <c r="FH12" s="63"/>
+      <c r="FI12" s="63"/>
+      <c r="FJ12" s="63"/>
+      <c r="FK12" s="63"/>
+      <c r="FL12" s="63"/>
+      <c r="FM12" s="63"/>
+      <c r="FN12" s="63"/>
+      <c r="FO12" s="63"/>
+      <c r="FP12" s="63"/>
+      <c r="FQ12" s="63"/>
+      <c r="FR12" s="63"/>
+      <c r="FS12" s="63"/>
+      <c r="FT12" s="63"/>
+      <c r="FU12" s="63"/>
+      <c r="FV12" s="63"/>
+      <c r="FW12" s="63"/>
+      <c r="FX12" s="63"/>
+      <c r="FY12" s="63"/>
+      <c r="FZ12" s="63"/>
+      <c r="GA12" s="63"/>
+      <c r="GB12" s="63"/>
+      <c r="GC12" s="63"/>
+      <c r="GD12" s="63"/>
+      <c r="GE12" s="63"/>
+      <c r="GF12" s="63"/>
+      <c r="GG12" s="63"/>
+      <c r="GH12" s="63"/>
+      <c r="GI12" s="120"/>
     </row>
     <row r="13" spans="1:191" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="117"/>
-      <c r="D13" s="115"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="115"/>
-      <c r="H13" s="68">
+      <c r="C13" s="79"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="60">
         <v>1</v>
       </c>
-      <c r="I13" s="69"/>
-      <c r="J13" s="68">
+      <c r="I13" s="61"/>
+      <c r="J13" s="60">
         <v>2</v>
       </c>
-      <c r="K13" s="69"/>
-      <c r="L13" s="68">
+      <c r="K13" s="61"/>
+      <c r="L13" s="60">
         <v>3</v>
       </c>
-      <c r="M13" s="69"/>
-      <c r="N13" s="68">
+      <c r="M13" s="61"/>
+      <c r="N13" s="60">
         <v>4</v>
       </c>
-      <c r="O13" s="69"/>
-      <c r="P13" s="68">
+      <c r="O13" s="61"/>
+      <c r="P13" s="60">
         <v>5</v>
       </c>
-      <c r="Q13" s="69"/>
-      <c r="R13" s="68">
+      <c r="Q13" s="61"/>
+      <c r="R13" s="60">
         <v>6</v>
       </c>
-      <c r="S13" s="69"/>
-      <c r="T13" s="68">
+      <c r="S13" s="61"/>
+      <c r="T13" s="60">
         <v>7</v>
       </c>
-      <c r="U13" s="69"/>
-      <c r="V13" s="68">
+      <c r="U13" s="61"/>
+      <c r="V13" s="60">
         <v>8</v>
       </c>
-      <c r="W13" s="69"/>
-      <c r="X13" s="68">
+      <c r="W13" s="61"/>
+      <c r="X13" s="60">
         <v>9</v>
       </c>
-      <c r="Y13" s="69"/>
-      <c r="Z13" s="68">
+      <c r="Y13" s="61"/>
+      <c r="Z13" s="60">
         <v>10</v>
       </c>
-      <c r="AA13" s="69"/>
-      <c r="AB13" s="68">
+      <c r="AA13" s="61"/>
+      <c r="AB13" s="60">
         <v>11</v>
       </c>
-      <c r="AC13" s="69"/>
-      <c r="AD13" s="68">
+      <c r="AC13" s="61"/>
+      <c r="AD13" s="60">
         <v>12</v>
       </c>
-      <c r="AE13" s="69"/>
-      <c r="AF13" s="68">
+      <c r="AE13" s="61"/>
+      <c r="AF13" s="60">
         <v>13</v>
       </c>
-      <c r="AG13" s="69"/>
-      <c r="AH13" s="68">
+      <c r="AG13" s="61"/>
+      <c r="AH13" s="60">
         <v>14</v>
       </c>
-      <c r="AI13" s="69"/>
-      <c r="AJ13" s="68">
+      <c r="AI13" s="61"/>
+      <c r="AJ13" s="60">
         <v>15</v>
       </c>
-      <c r="AK13" s="69"/>
-      <c r="AL13" s="68">
+      <c r="AK13" s="61"/>
+      <c r="AL13" s="60">
         <v>16</v>
       </c>
-      <c r="AM13" s="69"/>
-      <c r="AN13" s="68">
+      <c r="AM13" s="61"/>
+      <c r="AN13" s="60">
         <v>17</v>
       </c>
-      <c r="AO13" s="69"/>
-      <c r="AP13" s="68">
+      <c r="AO13" s="61"/>
+      <c r="AP13" s="60">
         <v>18</v>
       </c>
-      <c r="AQ13" s="69"/>
-      <c r="AR13" s="68">
+      <c r="AQ13" s="61"/>
+      <c r="AR13" s="60">
         <v>19</v>
       </c>
-      <c r="AS13" s="69"/>
-      <c r="AT13" s="68">
+      <c r="AS13" s="61"/>
+      <c r="AT13" s="60">
         <v>20</v>
       </c>
-      <c r="AU13" s="69"/>
-      <c r="AV13" s="68">
+      <c r="AU13" s="61"/>
+      <c r="AV13" s="60">
         <v>21</v>
       </c>
-      <c r="AW13" s="69"/>
-      <c r="AX13" s="68">
+      <c r="AW13" s="61"/>
+      <c r="AX13" s="60">
         <v>22</v>
       </c>
-      <c r="AY13" s="69"/>
-      <c r="AZ13" s="68">
+      <c r="AY13" s="61"/>
+      <c r="AZ13" s="60">
         <v>23</v>
       </c>
-      <c r="BA13" s="69"/>
-      <c r="BB13" s="68">
+      <c r="BA13" s="61"/>
+      <c r="BB13" s="60">
         <v>24</v>
       </c>
-      <c r="BC13" s="69"/>
-      <c r="BD13" s="68">
+      <c r="BC13" s="61"/>
+      <c r="BD13" s="60">
         <v>25</v>
       </c>
-      <c r="BE13" s="69"/>
-      <c r="BF13" s="68">
+      <c r="BE13" s="61"/>
+      <c r="BF13" s="60">
         <v>26</v>
       </c>
-      <c r="BG13" s="69"/>
-      <c r="BH13" s="68">
+      <c r="BG13" s="61"/>
+      <c r="BH13" s="60">
         <v>27</v>
       </c>
-      <c r="BI13" s="69"/>
-      <c r="BJ13" s="68">
+      <c r="BI13" s="61"/>
+      <c r="BJ13" s="60">
         <v>28</v>
       </c>
-      <c r="BK13" s="69"/>
-      <c r="BL13" s="68">
+      <c r="BK13" s="61"/>
+      <c r="BL13" s="60">
         <v>29</v>
       </c>
-      <c r="BM13" s="69"/>
-      <c r="BN13" s="68">
+      <c r="BM13" s="61"/>
+      <c r="BN13" s="60">
         <v>30</v>
       </c>
-      <c r="BO13" s="69"/>
-      <c r="BP13" s="68">
+      <c r="BO13" s="61"/>
+      <c r="BP13" s="60">
         <v>31</v>
       </c>
-      <c r="BQ13" s="120"/>
-      <c r="BR13" s="68">
+      <c r="BQ13" s="69"/>
+      <c r="BR13" s="60">
         <v>1</v>
       </c>
-      <c r="BS13" s="69"/>
-      <c r="BT13" s="68">
+      <c r="BS13" s="61"/>
+      <c r="BT13" s="60">
         <v>2</v>
       </c>
-      <c r="BU13" s="69"/>
-      <c r="BV13" s="68">
+      <c r="BU13" s="61"/>
+      <c r="BV13" s="60">
         <v>3</v>
       </c>
-      <c r="BW13" s="69"/>
-      <c r="BX13" s="68">
+      <c r="BW13" s="61"/>
+      <c r="BX13" s="60">
         <v>4</v>
       </c>
-      <c r="BY13" s="69"/>
-      <c r="BZ13" s="68">
+      <c r="BY13" s="61"/>
+      <c r="BZ13" s="60">
         <v>5</v>
       </c>
-      <c r="CA13" s="69"/>
-      <c r="CB13" s="68">
+      <c r="CA13" s="61"/>
+      <c r="CB13" s="60">
         <v>6</v>
       </c>
-      <c r="CC13" s="69"/>
-      <c r="CD13" s="68">
+      <c r="CC13" s="61"/>
+      <c r="CD13" s="60">
         <v>7</v>
       </c>
-      <c r="CE13" s="69"/>
-      <c r="CF13" s="68">
+      <c r="CE13" s="61"/>
+      <c r="CF13" s="60">
         <v>8</v>
       </c>
-      <c r="CG13" s="69"/>
-      <c r="CH13" s="68">
+      <c r="CG13" s="61"/>
+      <c r="CH13" s="60">
         <v>9</v>
       </c>
-      <c r="CI13" s="69"/>
-      <c r="CJ13" s="68">
+      <c r="CI13" s="61"/>
+      <c r="CJ13" s="60">
         <v>10</v>
       </c>
-      <c r="CK13" s="69"/>
-      <c r="CL13" s="68">
+      <c r="CK13" s="61"/>
+      <c r="CL13" s="60">
         <v>11</v>
       </c>
-      <c r="CM13" s="69"/>
-      <c r="CN13" s="68">
+      <c r="CM13" s="61"/>
+      <c r="CN13" s="60">
         <v>12</v>
       </c>
-      <c r="CO13" s="69"/>
-      <c r="CP13" s="68">
+      <c r="CO13" s="61"/>
+      <c r="CP13" s="60">
         <v>13</v>
       </c>
-      <c r="CQ13" s="69"/>
-      <c r="CR13" s="68">
+      <c r="CQ13" s="61"/>
+      <c r="CR13" s="60">
         <v>14</v>
       </c>
-      <c r="CS13" s="69"/>
-      <c r="CT13" s="68">
+      <c r="CS13" s="61"/>
+      <c r="CT13" s="60">
         <v>15</v>
       </c>
-      <c r="CU13" s="69"/>
-      <c r="CV13" s="68">
+      <c r="CU13" s="61"/>
+      <c r="CV13" s="60">
         <v>16</v>
       </c>
-      <c r="CW13" s="69"/>
-      <c r="CX13" s="68">
+      <c r="CW13" s="61"/>
+      <c r="CX13" s="60">
         <v>17</v>
       </c>
-      <c r="CY13" s="69"/>
-      <c r="CZ13" s="68">
+      <c r="CY13" s="61"/>
+      <c r="CZ13" s="60">
         <v>18</v>
       </c>
-      <c r="DA13" s="69"/>
-      <c r="DB13" s="68">
+      <c r="DA13" s="61"/>
+      <c r="DB13" s="60">
         <v>19</v>
       </c>
-      <c r="DC13" s="69"/>
-      <c r="DD13" s="68">
+      <c r="DC13" s="61"/>
+      <c r="DD13" s="60">
         <v>20</v>
       </c>
-      <c r="DE13" s="69"/>
-      <c r="DF13" s="68">
+      <c r="DE13" s="61"/>
+      <c r="DF13" s="60">
         <v>21</v>
       </c>
-      <c r="DG13" s="69"/>
-      <c r="DH13" s="68">
+      <c r="DG13" s="61"/>
+      <c r="DH13" s="60">
         <v>22</v>
       </c>
-      <c r="DI13" s="69"/>
-      <c r="DJ13" s="68">
+      <c r="DI13" s="61"/>
+      <c r="DJ13" s="60">
         <v>23</v>
       </c>
-      <c r="DK13" s="69"/>
-      <c r="DL13" s="68">
+      <c r="DK13" s="61"/>
+      <c r="DL13" s="60">
         <v>24</v>
       </c>
-      <c r="DM13" s="69"/>
-      <c r="DN13" s="68">
+      <c r="DM13" s="61"/>
+      <c r="DN13" s="60">
         <v>25</v>
       </c>
-      <c r="DO13" s="69"/>
-      <c r="DP13" s="68">
+      <c r="DO13" s="61"/>
+      <c r="DP13" s="60">
         <v>26</v>
       </c>
-      <c r="DQ13" s="69"/>
-      <c r="DR13" s="68">
+      <c r="DQ13" s="61"/>
+      <c r="DR13" s="60">
         <v>27</v>
       </c>
-      <c r="DS13" s="69"/>
-      <c r="DT13" s="68">
+      <c r="DS13" s="61"/>
+      <c r="DT13" s="60">
         <v>28</v>
       </c>
-      <c r="DU13" s="69"/>
-      <c r="DV13" s="68">
+      <c r="DU13" s="61"/>
+      <c r="DV13" s="60">
         <v>29</v>
       </c>
-      <c r="DW13" s="69"/>
-      <c r="DX13" s="68">
+      <c r="DW13" s="61"/>
+      <c r="DX13" s="60">
         <v>30</v>
       </c>
-      <c r="DY13" s="69"/>
-      <c r="DZ13" s="68">
+      <c r="DY13" s="61"/>
+      <c r="DZ13" s="60">
         <v>1</v>
       </c>
-      <c r="EA13" s="69"/>
-      <c r="EB13" s="68">
+      <c r="EA13" s="61"/>
+      <c r="EB13" s="60">
         <v>2</v>
       </c>
-      <c r="EC13" s="69"/>
-      <c r="ED13" s="68">
+      <c r="EC13" s="61"/>
+      <c r="ED13" s="60">
         <v>3</v>
       </c>
-      <c r="EE13" s="69"/>
-      <c r="EF13" s="68">
+      <c r="EE13" s="61"/>
+      <c r="EF13" s="60">
         <v>4</v>
       </c>
-      <c r="EG13" s="69"/>
-      <c r="EH13" s="68">
+      <c r="EG13" s="61"/>
+      <c r="EH13" s="60">
         <v>5</v>
       </c>
-      <c r="EI13" s="69"/>
-      <c r="EJ13" s="68">
+      <c r="EI13" s="61"/>
+      <c r="EJ13" s="60">
         <v>6</v>
       </c>
-      <c r="EK13" s="69"/>
-      <c r="EL13" s="68">
+      <c r="EK13" s="61"/>
+      <c r="EL13" s="60">
         <v>7</v>
       </c>
-      <c r="EM13" s="69"/>
-      <c r="EN13" s="68">
+      <c r="EM13" s="61"/>
+      <c r="EN13" s="60">
         <v>8</v>
       </c>
-      <c r="EO13" s="69"/>
-      <c r="EP13" s="68">
+      <c r="EO13" s="61"/>
+      <c r="EP13" s="60">
         <v>9</v>
       </c>
-      <c r="EQ13" s="69"/>
-      <c r="ER13" s="68">
+      <c r="EQ13" s="61"/>
+      <c r="ER13" s="60">
         <v>10</v>
       </c>
-      <c r="ES13" s="69"/>
-      <c r="ET13" s="68">
+      <c r="ES13" s="61"/>
+      <c r="ET13" s="60">
         <v>11</v>
       </c>
-      <c r="EU13" s="69"/>
-      <c r="EV13" s="68">
+      <c r="EU13" s="61"/>
+      <c r="EV13" s="60">
         <v>12</v>
       </c>
-      <c r="EW13" s="69"/>
-      <c r="EX13" s="68">
+      <c r="EW13" s="61"/>
+      <c r="EX13" s="60">
         <v>13</v>
       </c>
-      <c r="EY13" s="69"/>
-      <c r="EZ13" s="68">
+      <c r="EY13" s="61"/>
+      <c r="EZ13" s="60">
         <v>14</v>
       </c>
-      <c r="FA13" s="69"/>
-      <c r="FB13" s="68">
+      <c r="FA13" s="61"/>
+      <c r="FB13" s="60">
         <v>15</v>
       </c>
-      <c r="FC13" s="69"/>
-      <c r="FD13" s="68">
+      <c r="FC13" s="61"/>
+      <c r="FD13" s="60">
         <v>16</v>
       </c>
-      <c r="FE13" s="69"/>
-      <c r="FF13" s="68">
+      <c r="FE13" s="61"/>
+      <c r="FF13" s="60">
         <v>17</v>
       </c>
-      <c r="FG13" s="69"/>
-      <c r="FH13" s="68">
+      <c r="FG13" s="61"/>
+      <c r="FH13" s="60">
         <v>18</v>
       </c>
-      <c r="FI13" s="69"/>
-      <c r="FJ13" s="68">
+      <c r="FI13" s="61"/>
+      <c r="FJ13" s="60">
         <v>19</v>
       </c>
-      <c r="FK13" s="69"/>
-      <c r="FL13" s="68">
+      <c r="FK13" s="61"/>
+      <c r="FL13" s="60">
         <v>20</v>
       </c>
-      <c r="FM13" s="69"/>
-      <c r="FN13" s="68">
+      <c r="FM13" s="61"/>
+      <c r="FN13" s="60">
         <v>21</v>
       </c>
-      <c r="FO13" s="69"/>
-      <c r="FP13" s="68">
+      <c r="FO13" s="61"/>
+      <c r="FP13" s="60">
         <v>22</v>
       </c>
-      <c r="FQ13" s="69"/>
-      <c r="FR13" s="68">
+      <c r="FQ13" s="61"/>
+      <c r="FR13" s="60">
         <v>23</v>
       </c>
-      <c r="FS13" s="69"/>
-      <c r="FT13" s="68">
+      <c r="FS13" s="61"/>
+      <c r="FT13" s="60">
         <v>24</v>
       </c>
-      <c r="FU13" s="69"/>
-      <c r="FV13" s="68">
+      <c r="FU13" s="61"/>
+      <c r="FV13" s="60">
         <v>25</v>
       </c>
-      <c r="FW13" s="69"/>
-      <c r="FX13" s="68">
+      <c r="FW13" s="61"/>
+      <c r="FX13" s="60">
         <v>26</v>
       </c>
-      <c r="FY13" s="69"/>
-      <c r="FZ13" s="68">
+      <c r="FY13" s="61"/>
+      <c r="FZ13" s="60">
         <v>27</v>
       </c>
-      <c r="GA13" s="69"/>
-      <c r="GB13" s="68">
+      <c r="GA13" s="61"/>
+      <c r="GB13" s="60">
         <v>28</v>
       </c>
-      <c r="GC13" s="69"/>
-      <c r="GD13" s="68">
+      <c r="GC13" s="61"/>
+      <c r="GD13" s="60">
         <v>29</v>
       </c>
-      <c r="GE13" s="69"/>
-      <c r="GF13" s="68">
+      <c r="GE13" s="61"/>
+      <c r="GF13" s="60">
         <v>30</v>
       </c>
-      <c r="GG13" s="69"/>
-      <c r="GH13" s="68">
+      <c r="GG13" s="61"/>
+      <c r="GH13" s="60">
         <v>31</v>
       </c>
-      <c r="GI13" s="69"/>
+      <c r="GI13" s="61"/>
     </row>
     <row r="14" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="113" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="75"/>
+      <c r="B14" s="114"/>
       <c r="C14" s="37"/>
-      <c r="D14" s="91">
+      <c r="D14" s="97">
         <f>SUM(D15:E61)</f>
         <v>51.050000000000011</v>
       </c>
-      <c r="E14" s="93"/>
-      <c r="F14" s="91">
+      <c r="E14" s="99"/>
+      <c r="F14" s="97">
         <f>SUM(F15:G61)</f>
-        <v>34.249000000000002</v>
-      </c>
-      <c r="G14" s="92"/>
+        <v>36.249000000000002</v>
+      </c>
+      <c r="G14" s="98"/>
       <c r="H14" s="18"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -2830,22 +2830,22 @@
       <c r="GI14" s="14"/>
     </row>
     <row r="15" spans="1:191" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="82" t="s">
+      <c r="A15" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="83"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="62">
+      <c r="D15" s="65">
         <v>1.5</v>
       </c>
-      <c r="E15" s="63"/>
-      <c r="F15" s="62">
+      <c r="E15" s="66"/>
+      <c r="F15" s="65">
         <f>SUM(H15:GI15)</f>
         <v>0.5</v>
       </c>
-      <c r="G15" s="64"/>
+      <c r="G15" s="80"/>
       <c r="H15" s="47"/>
       <c r="I15" s="12"/>
       <c r="J15" s="24">
@@ -3034,22 +3034,22 @@
       <c r="GI15" s="34"/>
     </row>
     <row r="16" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="67"/>
+      <c r="B16" s="82"/>
       <c r="C16" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="62">
+      <c r="D16" s="65">
         <v>0.6</v>
       </c>
-      <c r="E16" s="63"/>
-      <c r="F16" s="62">
+      <c r="E16" s="66"/>
+      <c r="F16" s="65">
         <f>SUM(H16:GI16)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="64"/>
+      <c r="G16" s="80"/>
       <c r="H16" s="47"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
@@ -3236,22 +3236,22 @@
       <c r="GI16" s="32"/>
     </row>
     <row r="17" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="67"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="62">
+      <c r="D17" s="65">
         <v>1</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="62">
+      <c r="E17" s="66"/>
+      <c r="F17" s="65">
         <f>SUM(H17:GI17)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="64"/>
+      <c r="G17" s="80"/>
       <c r="H17" s="47"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
@@ -3442,22 +3442,22 @@
       <c r="GI17" s="32"/>
     </row>
     <row r="18" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="67"/>
+      <c r="B18" s="82"/>
       <c r="C18" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="62">
+      <c r="D18" s="65">
         <v>0.8</v>
       </c>
-      <c r="E18" s="63"/>
-      <c r="F18" s="62">
+      <c r="E18" s="66"/>
+      <c r="F18" s="65">
         <f t="shared" ref="F18:F60" si="0">SUM(H18:GI18)</f>
         <v>0.75</v>
       </c>
-      <c r="G18" s="64"/>
+      <c r="G18" s="80"/>
       <c r="H18" s="26"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
@@ -3646,22 +3646,22 @@
       <c r="GI18" s="32"/>
     </row>
     <row r="19" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="67"/>
+      <c r="B19" s="82"/>
       <c r="C19" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="62">
+      <c r="D19" s="65">
         <v>0.5</v>
       </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="62">
+      <c r="E19" s="66"/>
+      <c r="F19" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="64"/>
+      <c r="G19" s="80"/>
       <c r="H19" s="26"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
@@ -3848,22 +3848,22 @@
       <c r="GI19" s="36"/>
     </row>
     <row r="20" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="67"/>
+      <c r="B20" s="82"/>
       <c r="C20" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="62">
+      <c r="D20" s="65">
         <v>0.3</v>
       </c>
-      <c r="E20" s="63"/>
-      <c r="F20" s="62">
+      <c r="E20" s="66"/>
+      <c r="F20" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="64"/>
+      <c r="G20" s="80"/>
       <c r="H20" s="26"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -4050,22 +4050,22 @@
       <c r="GI20" s="36"/>
     </row>
     <row r="21" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="67"/>
+      <c r="B21" s="82"/>
       <c r="C21" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="62">
+      <c r="D21" s="65">
         <v>1</v>
       </c>
-      <c r="E21" s="63"/>
-      <c r="F21" s="62">
+      <c r="E21" s="66"/>
+      <c r="F21" s="65">
         <f t="shared" si="0"/>
         <v>0.16600000000000001</v>
       </c>
-      <c r="G21" s="64"/>
+      <c r="G21" s="80"/>
       <c r="H21" s="26"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
@@ -4254,22 +4254,22 @@
       <c r="GI21" s="36"/>
     </row>
     <row r="22" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="67"/>
+      <c r="B22" s="82"/>
       <c r="C22" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="62">
+      <c r="D22" s="65">
         <v>0.6</v>
       </c>
-      <c r="E22" s="63"/>
-      <c r="F22" s="62">
+      <c r="E22" s="66"/>
+      <c r="F22" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="64"/>
+      <c r="G22" s="80"/>
       <c r="H22" s="26"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
@@ -4456,22 +4456,22 @@
       <c r="GI22" s="36"/>
     </row>
     <row r="23" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="67"/>
+      <c r="B23" s="82"/>
       <c r="C23" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="62">
+      <c r="D23" s="65">
         <v>0.6</v>
       </c>
-      <c r="E23" s="63"/>
-      <c r="F23" s="62">
+      <c r="E23" s="66"/>
+      <c r="F23" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="64"/>
+      <c r="G23" s="80"/>
       <c r="H23" s="26"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
@@ -4658,22 +4658,22 @@
       <c r="GI23" s="36"/>
     </row>
     <row r="24" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="67"/>
+      <c r="B24" s="82"/>
       <c r="C24" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="62">
+      <c r="D24" s="65">
         <v>3</v>
       </c>
-      <c r="E24" s="63"/>
-      <c r="F24" s="62">
+      <c r="E24" s="66"/>
+      <c r="F24" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="64"/>
+      <c r="G24" s="80"/>
       <c r="H24" s="26"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
@@ -4860,22 +4860,22 @@
       <c r="GI24" s="36"/>
     </row>
     <row r="25" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="67"/>
+      <c r="B25" s="82"/>
       <c r="C25" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="62">
+      <c r="D25" s="65">
         <v>1.5</v>
       </c>
-      <c r="E25" s="63"/>
-      <c r="F25" s="62">
+      <c r="E25" s="66"/>
+      <c r="F25" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="64"/>
+      <c r="G25" s="80"/>
       <c r="H25" s="26"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
@@ -5062,22 +5062,22 @@
       <c r="GI25" s="36"/>
     </row>
     <row r="26" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A26" s="66" t="s">
+      <c r="A26" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="67"/>
+      <c r="B26" s="82"/>
       <c r="C26" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="62">
+      <c r="D26" s="65">
         <v>1</v>
       </c>
-      <c r="E26" s="63"/>
-      <c r="F26" s="62">
+      <c r="E26" s="66"/>
+      <c r="F26" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="64"/>
+      <c r="G26" s="80"/>
       <c r="H26" s="26"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
@@ -5264,22 +5264,22 @@
       <c r="GI26" s="36"/>
     </row>
     <row r="27" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="67"/>
+      <c r="B27" s="82"/>
       <c r="C27" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="62">
+      <c r="D27" s="65">
         <v>1</v>
       </c>
-      <c r="E27" s="63"/>
-      <c r="F27" s="62">
+      <c r="E27" s="66"/>
+      <c r="F27" s="65">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="64"/>
+        <v>2</v>
+      </c>
+      <c r="G27" s="80"/>
       <c r="H27" s="26"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
@@ -5297,7 +5297,9 @@
       <c r="V27" s="32"/>
       <c r="W27" s="32"/>
       <c r="X27" s="32"/>
-      <c r="Y27" s="32"/>
+      <c r="Y27" s="58">
+        <v>1</v>
+      </c>
       <c r="Z27" s="50"/>
       <c r="AA27" s="50"/>
       <c r="AB27" s="49"/>
@@ -5311,7 +5313,9 @@
       <c r="AJ27" s="32"/>
       <c r="AK27" s="32"/>
       <c r="AL27" s="32"/>
-      <c r="AM27" s="32"/>
+      <c r="AM27" s="24">
+        <v>1</v>
+      </c>
       <c r="AN27" s="49"/>
       <c r="AO27" s="52"/>
       <c r="AP27" s="51"/>
@@ -5466,22 +5470,22 @@
       <c r="GI27" s="36"/>
     </row>
     <row r="28" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A28" s="66" t="s">
+      <c r="A28" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="67"/>
+      <c r="B28" s="82"/>
       <c r="C28" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="62">
+      <c r="D28" s="65">
         <v>1</v>
       </c>
-      <c r="E28" s="63"/>
-      <c r="F28" s="62">
+      <c r="E28" s="66"/>
+      <c r="F28" s="65">
         <f t="shared" si="0"/>
         <v>0.33300000000000002</v>
       </c>
-      <c r="G28" s="64"/>
+      <c r="G28" s="80"/>
       <c r="H28" s="26"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
@@ -5670,22 +5674,22 @@
       <c r="GI28" s="36"/>
     </row>
     <row r="29" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="67"/>
+      <c r="B29" s="82"/>
       <c r="C29" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="62">
+      <c r="D29" s="65">
         <v>1</v>
       </c>
-      <c r="E29" s="63"/>
-      <c r="F29" s="62">
+      <c r="E29" s="66"/>
+      <c r="F29" s="65">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G29" s="64"/>
+      <c r="G29" s="80"/>
       <c r="H29" s="26"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
@@ -5874,22 +5878,22 @@
       <c r="GI29" s="36"/>
     </row>
     <row r="30" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A30" s="66" t="s">
+      <c r="A30" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="67"/>
+      <c r="B30" s="82"/>
       <c r="C30" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="62">
+      <c r="D30" s="65">
         <v>1</v>
       </c>
-      <c r="E30" s="63"/>
-      <c r="F30" s="62">
+      <c r="E30" s="66"/>
+      <c r="F30" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G30" s="64"/>
+      <c r="G30" s="80"/>
       <c r="H30" s="26"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
@@ -6078,22 +6082,22 @@
       <c r="GI30" s="36"/>
     </row>
     <row r="31" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A31" s="66" t="s">
+      <c r="A31" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="67"/>
+      <c r="B31" s="82"/>
       <c r="C31" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="62">
+      <c r="D31" s="65">
         <v>4</v>
       </c>
-      <c r="E31" s="63"/>
-      <c r="F31" s="62">
+      <c r="E31" s="66"/>
+      <c r="F31" s="65">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G31" s="64"/>
+      <c r="G31" s="80"/>
       <c r="H31" s="26"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
@@ -6284,22 +6288,22 @@
       <c r="GI31" s="36"/>
     </row>
     <row r="32" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A32" s="66" t="s">
+      <c r="A32" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="67"/>
+      <c r="B32" s="82"/>
       <c r="C32" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="62">
+      <c r="D32" s="65">
         <v>0.6</v>
       </c>
-      <c r="E32" s="63"/>
-      <c r="F32" s="62">
+      <c r="E32" s="66"/>
+      <c r="F32" s="65">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G32" s="64"/>
+      <c r="G32" s="80"/>
       <c r="H32" s="26"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
@@ -6488,22 +6492,22 @@
       <c r="GI32" s="36"/>
     </row>
     <row r="33" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="67"/>
+      <c r="B33" s="82"/>
       <c r="C33" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="62">
+      <c r="D33" s="65">
         <v>0.5</v>
       </c>
-      <c r="E33" s="63"/>
-      <c r="F33" s="62">
+      <c r="E33" s="66"/>
+      <c r="F33" s="65">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G33" s="64"/>
+      <c r="G33" s="80"/>
       <c r="H33" s="26"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
@@ -6692,22 +6696,22 @@
       <c r="GI33" s="36"/>
     </row>
     <row r="34" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A34" s="66" t="s">
+      <c r="A34" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="67"/>
+      <c r="B34" s="82"/>
       <c r="C34" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="62">
+      <c r="D34" s="65">
         <v>0.3</v>
       </c>
-      <c r="E34" s="63"/>
-      <c r="F34" s="62">
+      <c r="E34" s="66"/>
+      <c r="F34" s="65">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G34" s="64"/>
+      <c r="G34" s="80"/>
       <c r="H34" s="26"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
@@ -6896,22 +6900,22 @@
       <c r="GI34" s="36"/>
     </row>
     <row r="35" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A35" s="66" t="s">
+      <c r="A35" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="67"/>
+      <c r="B35" s="82"/>
       <c r="C35" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="62">
+      <c r="D35" s="65">
         <v>0.3</v>
       </c>
-      <c r="E35" s="63"/>
-      <c r="F35" s="62">
+      <c r="E35" s="66"/>
+      <c r="F35" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G35" s="64"/>
+      <c r="G35" s="80"/>
       <c r="H35" s="26"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
@@ -7098,22 +7102,22 @@
       <c r="GI35" s="36"/>
     </row>
     <row r="36" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A36" s="66" t="s">
+      <c r="A36" s="81" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="67"/>
+      <c r="B36" s="82"/>
       <c r="C36" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="62">
+      <c r="D36" s="65">
         <v>1.5</v>
       </c>
-      <c r="E36" s="63"/>
-      <c r="F36" s="62">
+      <c r="E36" s="66"/>
+      <c r="F36" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G36" s="64"/>
+      <c r="G36" s="80"/>
       <c r="H36" s="26"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
@@ -7300,22 +7304,22 @@
       <c r="GI36" s="36"/>
     </row>
     <row r="37" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A37" s="66" t="s">
+      <c r="A37" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="67"/>
+      <c r="B37" s="82"/>
       <c r="C37" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="62">
+      <c r="D37" s="65">
         <v>0.5</v>
       </c>
-      <c r="E37" s="63"/>
-      <c r="F37" s="62">
+      <c r="E37" s="66"/>
+      <c r="F37" s="65">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G37" s="64"/>
+      <c r="G37" s="80"/>
       <c r="H37" s="26"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
@@ -7504,22 +7508,22 @@
       <c r="GI37" s="36"/>
     </row>
     <row r="38" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A38" s="66" t="s">
+      <c r="A38" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="67"/>
+      <c r="B38" s="82"/>
       <c r="C38" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="62">
+      <c r="D38" s="65">
         <v>0.25</v>
       </c>
-      <c r="E38" s="63"/>
-      <c r="F38" s="62">
+      <c r="E38" s="66"/>
+      <c r="F38" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G38" s="64"/>
+      <c r="G38" s="80"/>
       <c r="H38" s="26"/>
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
@@ -7708,22 +7712,22 @@
       <c r="GI38" s="36"/>
     </row>
     <row r="39" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="67"/>
+      <c r="B39" s="82"/>
       <c r="C39" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="62">
+      <c r="D39" s="65">
         <v>0.5</v>
       </c>
-      <c r="E39" s="63"/>
-      <c r="F39" s="62">
+      <c r="E39" s="66"/>
+      <c r="F39" s="65">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="G39" s="64"/>
+      <c r="G39" s="80"/>
       <c r="H39" s="26"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
@@ -7912,22 +7916,22 @@
       <c r="GI39" s="36"/>
     </row>
     <row r="40" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A40" s="66" t="s">
+      <c r="A40" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="67"/>
+      <c r="B40" s="82"/>
       <c r="C40" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="62">
+      <c r="D40" s="65">
         <v>0.5</v>
       </c>
-      <c r="E40" s="63"/>
-      <c r="F40" s="62">
+      <c r="E40" s="66"/>
+      <c r="F40" s="65">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G40" s="64"/>
+      <c r="G40" s="80"/>
       <c r="H40" s="26"/>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
@@ -8116,22 +8120,22 @@
       <c r="GI40" s="36"/>
     </row>
     <row r="41" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="67"/>
+      <c r="B41" s="82"/>
       <c r="C41" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="62">
+      <c r="D41" s="65">
         <v>0.3</v>
       </c>
-      <c r="E41" s="63"/>
-      <c r="F41" s="62">
+      <c r="E41" s="66"/>
+      <c r="F41" s="65">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G41" s="64"/>
+      <c r="G41" s="80"/>
       <c r="H41" s="26"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
@@ -8320,22 +8324,22 @@
       <c r="GI41" s="36"/>
     </row>
     <row r="42" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A42" s="66" t="s">
+      <c r="A42" s="81" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="67"/>
+      <c r="B42" s="82"/>
       <c r="C42" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="62">
+      <c r="D42" s="65">
         <v>0.5</v>
       </c>
-      <c r="E42" s="63"/>
-      <c r="F42" s="62">
+      <c r="E42" s="66"/>
+      <c r="F42" s="65">
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-      <c r="G42" s="64"/>
+      <c r="G42" s="80"/>
       <c r="H42" s="26"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
@@ -8524,22 +8528,22 @@
       <c r="GI42" s="36"/>
     </row>
     <row r="43" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A43" s="66" t="s">
+      <c r="A43" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="67"/>
+      <c r="B43" s="82"/>
       <c r="C43" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D43" s="62">
+      <c r="D43" s="65">
         <v>1.3</v>
       </c>
-      <c r="E43" s="63"/>
-      <c r="F43" s="62">
+      <c r="E43" s="66"/>
+      <c r="F43" s="65">
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
-      <c r="G43" s="64"/>
+      <c r="G43" s="80"/>
       <c r="H43" s="26"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
@@ -8730,22 +8734,22 @@
       <c r="GI43" s="36"/>
     </row>
     <row r="44" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="66" t="s">
+      <c r="A44" s="81" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="67"/>
+      <c r="B44" s="82"/>
       <c r="C44" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="62">
+      <c r="D44" s="65">
         <v>1.3</v>
       </c>
-      <c r="E44" s="63"/>
-      <c r="F44" s="62">
+      <c r="E44" s="66"/>
+      <c r="F44" s="65">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G44" s="64"/>
+      <c r="G44" s="80"/>
       <c r="H44" s="26"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
@@ -8934,22 +8938,22 @@
       <c r="GI44" s="36"/>
     </row>
     <row r="45" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A45" s="66" t="s">
+      <c r="A45" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="67"/>
+      <c r="B45" s="82"/>
       <c r="C45" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="62">
+      <c r="D45" s="65">
         <v>1</v>
       </c>
-      <c r="E45" s="63"/>
-      <c r="F45" s="62">
+      <c r="E45" s="66"/>
+      <c r="F45" s="65">
         <f t="shared" si="0"/>
         <v>1.05</v>
       </c>
-      <c r="G45" s="64"/>
+      <c r="G45" s="80"/>
       <c r="H45" s="26"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
@@ -9140,22 +9144,22 @@
       <c r="GI45" s="36"/>
     </row>
     <row r="46" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A46" s="66" t="s">
+      <c r="A46" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="67"/>
+      <c r="B46" s="82"/>
       <c r="C46" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="D46" s="62">
+      <c r="D46" s="65">
         <v>1</v>
       </c>
-      <c r="E46" s="63"/>
-      <c r="F46" s="62">
+      <c r="E46" s="66"/>
+      <c r="F46" s="65">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="G46" s="64"/>
+      <c r="G46" s="80"/>
       <c r="H46" s="26"/>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
@@ -9344,22 +9348,22 @@
       <c r="GI46" s="36"/>
     </row>
     <row r="47" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A47" s="66" t="s">
+      <c r="A47" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="67"/>
+      <c r="B47" s="82"/>
       <c r="C47" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="D47" s="62">
+      <c r="D47" s="65">
         <v>1</v>
       </c>
-      <c r="E47" s="63"/>
-      <c r="F47" s="62">
+      <c r="E47" s="66"/>
+      <c r="F47" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G47" s="64"/>
+      <c r="G47" s="80"/>
       <c r="H47" s="26"/>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
@@ -9546,22 +9550,22 @@
       <c r="GI47" s="36"/>
     </row>
     <row r="48" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A48" s="66" t="s">
+      <c r="A48" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="B48" s="67"/>
+      <c r="B48" s="82"/>
       <c r="C48" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D48" s="62">
+      <c r="D48" s="65">
         <v>0.3</v>
       </c>
-      <c r="E48" s="63"/>
-      <c r="F48" s="62">
+      <c r="E48" s="66"/>
+      <c r="F48" s="65">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G48" s="64"/>
+      <c r="G48" s="80"/>
       <c r="H48" s="26"/>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
@@ -9750,22 +9754,22 @@
       <c r="GI48" s="36"/>
     </row>
     <row r="49" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A49" s="66" t="s">
+      <c r="A49" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="67"/>
+      <c r="B49" s="82"/>
       <c r="C49" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="62">
+      <c r="D49" s="65">
         <v>2</v>
       </c>
-      <c r="E49" s="63"/>
-      <c r="F49" s="62">
+      <c r="E49" s="66"/>
+      <c r="F49" s="65">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G49" s="64"/>
+      <c r="G49" s="80"/>
       <c r="H49" s="26"/>
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
@@ -9956,22 +9960,22 @@
       <c r="GI49" s="36"/>
     </row>
     <row r="50" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A50" s="66" t="s">
+      <c r="A50" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="67"/>
+      <c r="B50" s="82"/>
       <c r="C50" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="D50" s="62">
+      <c r="D50" s="65">
         <v>2</v>
       </c>
-      <c r="E50" s="63"/>
-      <c r="F50" s="62">
+      <c r="E50" s="66"/>
+      <c r="F50" s="65">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G50" s="64"/>
+      <c r="G50" s="80"/>
       <c r="H50" s="26"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
@@ -10162,22 +10166,22 @@
       <c r="GI50" s="36"/>
     </row>
     <row r="51" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A51" s="66" t="s">
+      <c r="A51" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="67"/>
+      <c r="B51" s="82"/>
       <c r="C51" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D51" s="62">
+      <c r="D51" s="65">
         <v>2</v>
       </c>
-      <c r="E51" s="63"/>
-      <c r="F51" s="62">
+      <c r="E51" s="66"/>
+      <c r="F51" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G51" s="64"/>
+      <c r="G51" s="80"/>
       <c r="H51" s="26"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
@@ -10364,22 +10368,22 @@
       <c r="GI51" s="36"/>
     </row>
     <row r="52" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A52" s="66" t="s">
+      <c r="A52" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="67"/>
+      <c r="B52" s="82"/>
       <c r="C52" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="62">
+      <c r="D52" s="65">
         <v>2</v>
       </c>
-      <c r="E52" s="63"/>
-      <c r="F52" s="62">
+      <c r="E52" s="66"/>
+      <c r="F52" s="65">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G52" s="64"/>
+      <c r="G52" s="80"/>
       <c r="H52" s="26"/>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
@@ -10570,22 +10574,22 @@
       <c r="GI52" s="36"/>
     </row>
     <row r="53" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A53" s="66" t="s">
+      <c r="A53" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="67"/>
+      <c r="B53" s="82"/>
       <c r="C53" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D53" s="62">
+      <c r="D53" s="65">
         <v>2</v>
       </c>
-      <c r="E53" s="63"/>
-      <c r="F53" s="62">
+      <c r="E53" s="66"/>
+      <c r="F53" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G53" s="64"/>
+      <c r="G53" s="80"/>
       <c r="H53" s="26"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
@@ -10772,22 +10776,22 @@
       <c r="GI53" s="36"/>
     </row>
     <row r="54" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A54" s="66" t="s">
+      <c r="A54" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="67"/>
+      <c r="B54" s="82"/>
       <c r="C54" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="D54" s="62">
+      <c r="D54" s="65">
         <v>0.25</v>
       </c>
-      <c r="E54" s="63"/>
-      <c r="F54" s="62">
+      <c r="E54" s="66"/>
+      <c r="F54" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G54" s="64"/>
+      <c r="G54" s="80"/>
       <c r="H54" s="26"/>
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
@@ -10974,22 +10978,22 @@
       <c r="GI54" s="36"/>
     </row>
     <row r="55" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A55" s="66" t="s">
+      <c r="A55" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="67"/>
+      <c r="B55" s="82"/>
       <c r="C55" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="D55" s="62">
+      <c r="D55" s="65">
         <v>1</v>
       </c>
-      <c r="E55" s="63"/>
-      <c r="F55" s="62">
+      <c r="E55" s="66"/>
+      <c r="F55" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G55" s="64"/>
+      <c r="G55" s="80"/>
       <c r="H55" s="26"/>
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
@@ -11176,22 +11180,22 @@
       <c r="GI55" s="36"/>
     </row>
     <row r="56" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A56" s="66" t="s">
+      <c r="A56" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="67"/>
+      <c r="B56" s="82"/>
       <c r="C56" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="D56" s="62">
+      <c r="D56" s="65">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E56" s="63"/>
-      <c r="F56" s="62">
+      <c r="E56" s="66"/>
+      <c r="F56" s="65">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G56" s="64"/>
+      <c r="G56" s="80"/>
       <c r="H56" s="26"/>
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
@@ -11382,22 +11386,22 @@
       <c r="GI56" s="36"/>
     </row>
     <row r="57" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A57" s="66" t="s">
+      <c r="A57" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="67"/>
+      <c r="B57" s="82"/>
       <c r="C57" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="D57" s="62">
+      <c r="D57" s="65">
         <v>1.75</v>
       </c>
-      <c r="E57" s="63"/>
-      <c r="F57" s="62">
+      <c r="E57" s="66"/>
+      <c r="F57" s="65">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G57" s="64"/>
+      <c r="G57" s="80"/>
       <c r="H57" s="26"/>
       <c r="I57" s="12"/>
       <c r="J57" s="12"/>
@@ -11586,22 +11590,22 @@
       <c r="GI57" s="36"/>
     </row>
     <row r="58" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A58" s="66" t="s">
+      <c r="A58" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="B58" s="67"/>
+      <c r="B58" s="82"/>
       <c r="C58" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="D58" s="62">
+      <c r="D58" s="65">
         <v>0.6</v>
       </c>
-      <c r="E58" s="63"/>
-      <c r="F58" s="62">
+      <c r="E58" s="66"/>
+      <c r="F58" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G58" s="64"/>
+      <c r="G58" s="80"/>
       <c r="H58" s="26"/>
       <c r="I58" s="12"/>
       <c r="J58" s="12"/>
@@ -11788,22 +11792,22 @@
       <c r="GI58" s="36"/>
     </row>
     <row r="59" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="66" t="s">
+      <c r="A59" s="81" t="s">
         <v>111</v>
       </c>
-      <c r="B59" s="67"/>
+      <c r="B59" s="82"/>
       <c r="C59" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="62">
+      <c r="D59" s="65">
         <v>1</v>
       </c>
-      <c r="E59" s="63"/>
-      <c r="F59" s="62">
+      <c r="E59" s="66"/>
+      <c r="F59" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G59" s="64"/>
+      <c r="G59" s="80"/>
       <c r="H59" s="26"/>
       <c r="I59" s="12"/>
       <c r="J59" s="12"/>
@@ -11990,22 +11994,22 @@
       <c r="GI59" s="36"/>
     </row>
     <row r="60" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A60" s="66" t="s">
+      <c r="A60" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="B60" s="67"/>
+      <c r="B60" s="82"/>
       <c r="C60" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="D60" s="62">
+      <c r="D60" s="65">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E60" s="63"/>
-      <c r="F60" s="62">
+      <c r="E60" s="66"/>
+      <c r="F60" s="65">
         <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
-      <c r="G60" s="64"/>
+      <c r="G60" s="80"/>
       <c r="H60" s="26"/>
       <c r="I60" s="12"/>
       <c r="J60" s="12"/>
@@ -12194,22 +12198,22 @@
       <c r="GI60" s="36"/>
     </row>
     <row r="61" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A61" s="66" t="s">
+      <c r="A61" s="81" t="s">
         <v>115</v>
       </c>
-      <c r="B61" s="67"/>
+      <c r="B61" s="82"/>
       <c r="C61" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="D61" s="62">
+      <c r="D61" s="65">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E61" s="63"/>
-      <c r="F61" s="62">
+      <c r="E61" s="66"/>
+      <c r="F61" s="65">
         <f>SUM(H61:GI61)</f>
         <v>1</v>
       </c>
-      <c r="G61" s="64"/>
+      <c r="G61" s="80"/>
       <c r="H61" s="26"/>
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
@@ -12398,21 +12402,21 @@
       <c r="GI61" s="36"/>
     </row>
     <row r="62" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A62" s="76" t="s">
+      <c r="A62" s="115" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="77"/>
+      <c r="B62" s="116"/>
       <c r="C62" s="39"/>
-      <c r="D62" s="78">
+      <c r="D62" s="71">
         <f>SUM(D63:E80)</f>
         <v>88.6</v>
       </c>
-      <c r="E62" s="79"/>
-      <c r="F62" s="78">
+      <c r="E62" s="117"/>
+      <c r="F62" s="71">
         <f>SUM(F63:G80)</f>
         <v>0</v>
       </c>
-      <c r="G62" s="80"/>
+      <c r="G62" s="75"/>
       <c r="H62" s="29"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
@@ -12599,22 +12603,22 @@
       <c r="GI62" s="29"/>
     </row>
     <row r="63" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="60" t="s">
+      <c r="A63" s="118" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="61"/>
+      <c r="B63" s="119"/>
       <c r="C63" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D63" s="62">
+      <c r="D63" s="65">
         <v>0.6</v>
       </c>
-      <c r="E63" s="63"/>
-      <c r="F63" s="62">
+      <c r="E63" s="66"/>
+      <c r="F63" s="65">
         <f>SUM(H63:GI63)</f>
         <v>0</v>
       </c>
-      <c r="G63" s="64"/>
+      <c r="G63" s="80"/>
       <c r="H63" s="47"/>
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
@@ -12801,22 +12805,22 @@
       <c r="GI63" s="32"/>
     </row>
     <row r="64" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="60" t="s">
+      <c r="A64" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="B64" s="61"/>
+      <c r="B64" s="119"/>
       <c r="C64" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D64" s="62">
+      <c r="D64" s="65">
         <v>1.5</v>
       </c>
-      <c r="E64" s="63"/>
-      <c r="F64" s="62">
+      <c r="E64" s="66"/>
+      <c r="F64" s="65">
         <f>SUM(H64:GI64)</f>
         <v>0</v>
       </c>
-      <c r="G64" s="64"/>
+      <c r="G64" s="80"/>
       <c r="H64" s="47"/>
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
@@ -13003,22 +13007,22 @@
       <c r="GI64" s="32"/>
     </row>
     <row r="65" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A65" s="60" t="s">
+      <c r="A65" s="118" t="s">
         <v>123</v>
       </c>
-      <c r="B65" s="61"/>
+      <c r="B65" s="119"/>
       <c r="C65" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D65" s="62">
+      <c r="D65" s="65">
         <v>1</v>
       </c>
-      <c r="E65" s="63"/>
-      <c r="F65" s="62">
+      <c r="E65" s="66"/>
+      <c r="F65" s="65">
         <f t="shared" ref="F65:F80" si="1">SUM(H65:GI65)</f>
         <v>0</v>
       </c>
-      <c r="G65" s="64"/>
+      <c r="G65" s="80"/>
       <c r="H65" s="47"/>
       <c r="I65" s="12"/>
       <c r="J65" s="12"/>
@@ -13205,22 +13209,22 @@
       <c r="GI65" s="32"/>
     </row>
     <row r="66" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A66" s="60" t="s">
+      <c r="A66" s="118" t="s">
         <v>125</v>
       </c>
-      <c r="B66" s="61"/>
+      <c r="B66" s="119"/>
       <c r="C66" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D66" s="62">
+      <c r="D66" s="65">
         <v>0.5</v>
       </c>
-      <c r="E66" s="63"/>
-      <c r="F66" s="62">
+      <c r="E66" s="66"/>
+      <c r="F66" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G66" s="64"/>
+      <c r="G66" s="80"/>
       <c r="H66" s="47"/>
       <c r="I66" s="12"/>
       <c r="J66" s="12"/>
@@ -13407,22 +13411,22 @@
       <c r="GI66" s="32"/>
     </row>
     <row r="67" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A67" s="60" t="s">
+      <c r="A67" s="118" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="61"/>
+      <c r="B67" s="119"/>
       <c r="C67" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D67" s="62">
+      <c r="D67" s="65">
         <v>1</v>
       </c>
-      <c r="E67" s="63"/>
-      <c r="F67" s="62">
+      <c r="E67" s="66"/>
+      <c r="F67" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G67" s="64"/>
+      <c r="G67" s="80"/>
       <c r="H67" s="47"/>
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
@@ -13609,22 +13613,22 @@
       <c r="GI67" s="32"/>
     </row>
     <row r="68" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A68" s="60" t="s">
+      <c r="A68" s="118" t="s">
         <v>129</v>
       </c>
-      <c r="B68" s="61"/>
+      <c r="B68" s="119"/>
       <c r="C68" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D68" s="62">
+      <c r="D68" s="65">
         <v>1</v>
       </c>
-      <c r="E68" s="63"/>
-      <c r="F68" s="62">
+      <c r="E68" s="66"/>
+      <c r="F68" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G68" s="64"/>
+      <c r="G68" s="80"/>
       <c r="H68" s="47"/>
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
@@ -13811,22 +13815,22 @@
       <c r="GI68" s="32"/>
     </row>
     <row r="69" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A69" s="60" t="s">
+      <c r="A69" s="118" t="s">
         <v>131</v>
       </c>
-      <c r="B69" s="61"/>
+      <c r="B69" s="119"/>
       <c r="C69" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="D69" s="62">
+      <c r="D69" s="65">
         <v>4</v>
       </c>
-      <c r="E69" s="63"/>
-      <c r="F69" s="62">
+      <c r="E69" s="66"/>
+      <c r="F69" s="65">
         <f>SUM(H69:GI69)</f>
         <v>0</v>
       </c>
-      <c r="G69" s="64"/>
+      <c r="G69" s="80"/>
       <c r="H69" s="47"/>
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
@@ -14013,22 +14017,22 @@
       <c r="GI69" s="32"/>
     </row>
     <row r="70" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A70" s="60" t="s">
+      <c r="A70" s="118" t="s">
         <v>133</v>
       </c>
-      <c r="B70" s="61"/>
+      <c r="B70" s="119"/>
       <c r="C70" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="D70" s="62">
+      <c r="D70" s="65">
         <v>8</v>
       </c>
-      <c r="E70" s="63"/>
-      <c r="F70" s="62">
+      <c r="E70" s="66"/>
+      <c r="F70" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G70" s="64"/>
+      <c r="G70" s="80"/>
       <c r="H70" s="47"/>
       <c r="I70" s="12"/>
       <c r="J70" s="12"/>
@@ -14215,22 +14219,22 @@
       <c r="GI70" s="32"/>
     </row>
     <row r="71" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A71" s="60" t="s">
+      <c r="A71" s="118" t="s">
         <v>135</v>
       </c>
-      <c r="B71" s="61"/>
+      <c r="B71" s="119"/>
       <c r="C71" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="D71" s="62">
+      <c r="D71" s="65">
         <v>1</v>
       </c>
-      <c r="E71" s="63"/>
-      <c r="F71" s="62">
+      <c r="E71" s="66"/>
+      <c r="F71" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G71" s="64"/>
+      <c r="G71" s="80"/>
       <c r="H71" s="47"/>
       <c r="I71" s="12"/>
       <c r="J71" s="12"/>
@@ -14417,22 +14421,22 @@
       <c r="GI71" s="32"/>
     </row>
     <row r="72" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A72" s="60" t="s">
+      <c r="A72" s="118" t="s">
         <v>137</v>
       </c>
-      <c r="B72" s="61"/>
+      <c r="B72" s="119"/>
       <c r="C72" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="D72" s="62">
+      <c r="D72" s="65">
         <v>1</v>
       </c>
-      <c r="E72" s="63"/>
-      <c r="F72" s="62">
+      <c r="E72" s="66"/>
+      <c r="F72" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G72" s="64"/>
+      <c r="G72" s="80"/>
       <c r="H72" s="47"/>
       <c r="I72" s="12"/>
       <c r="J72" s="12"/>
@@ -14619,22 +14623,22 @@
       <c r="GI72" s="32"/>
     </row>
     <row r="73" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A73" s="60" t="s">
+      <c r="A73" s="118" t="s">
         <v>47</v>
       </c>
-      <c r="B73" s="61"/>
+      <c r="B73" s="119"/>
       <c r="C73" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="D73" s="62">
+      <c r="D73" s="65">
         <v>4</v>
       </c>
-      <c r="E73" s="63"/>
-      <c r="F73" s="62">
+      <c r="E73" s="66"/>
+      <c r="F73" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G73" s="64"/>
+      <c r="G73" s="80"/>
       <c r="H73" s="47"/>
       <c r="I73" s="12"/>
       <c r="J73" s="12"/>
@@ -14821,22 +14825,22 @@
       <c r="GI73" s="32"/>
     </row>
     <row r="74" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A74" s="60" t="s">
+      <c r="A74" s="118" t="s">
         <v>140</v>
       </c>
-      <c r="B74" s="61"/>
+      <c r="B74" s="119"/>
       <c r="C74" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="D74" s="62">
+      <c r="D74" s="65">
         <v>12</v>
       </c>
-      <c r="E74" s="63"/>
-      <c r="F74" s="62">
+      <c r="E74" s="66"/>
+      <c r="F74" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G74" s="64"/>
+      <c r="G74" s="80"/>
       <c r="H74" s="47"/>
       <c r="I74" s="12"/>
       <c r="J74" s="12"/>
@@ -15023,22 +15027,22 @@
       <c r="GI74" s="32"/>
     </row>
     <row r="75" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A75" s="60" t="s">
+      <c r="A75" s="118" t="s">
         <v>142</v>
       </c>
-      <c r="B75" s="65"/>
+      <c r="B75" s="88"/>
       <c r="C75" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D75" s="62">
+      <c r="D75" s="65">
         <v>16</v>
       </c>
-      <c r="E75" s="63"/>
-      <c r="F75" s="62">
+      <c r="E75" s="66"/>
+      <c r="F75" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G75" s="64"/>
+      <c r="G75" s="80"/>
       <c r="H75" s="47"/>
       <c r="I75" s="12"/>
       <c r="J75" s="12"/>
@@ -15225,22 +15229,22 @@
       <c r="GI75" s="36"/>
     </row>
     <row r="76" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A76" s="60" t="s">
+      <c r="A76" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B76" s="61"/>
+      <c r="B76" s="119"/>
       <c r="C76" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="D76" s="62">
+      <c r="D76" s="65">
         <v>5</v>
       </c>
-      <c r="E76" s="63"/>
-      <c r="F76" s="62">
+      <c r="E76" s="66"/>
+      <c r="F76" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G76" s="64"/>
+      <c r="G76" s="80"/>
       <c r="H76" s="47"/>
       <c r="I76" s="12"/>
       <c r="J76" s="12"/>
@@ -15427,22 +15431,22 @@
       <c r="GI76" s="32"/>
     </row>
     <row r="77" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A77" s="60" t="s">
+      <c r="A77" s="118" t="s">
         <v>146</v>
       </c>
-      <c r="B77" s="61"/>
+      <c r="B77" s="119"/>
       <c r="C77" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="D77" s="62">
+      <c r="D77" s="65">
         <v>4</v>
       </c>
-      <c r="E77" s="63"/>
-      <c r="F77" s="62">
+      <c r="E77" s="66"/>
+      <c r="F77" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G77" s="64"/>
+      <c r="G77" s="80"/>
       <c r="H77" s="47"/>
       <c r="I77" s="12"/>
       <c r="J77" s="12"/>
@@ -15629,22 +15633,22 @@
       <c r="GI77" s="32"/>
     </row>
     <row r="78" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A78" s="60" t="s">
+      <c r="A78" s="118" t="s">
         <v>148</v>
       </c>
-      <c r="B78" s="61"/>
+      <c r="B78" s="119"/>
       <c r="C78" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="D78" s="62">
+      <c r="D78" s="65">
         <v>16</v>
       </c>
-      <c r="E78" s="63"/>
-      <c r="F78" s="62">
+      <c r="E78" s="66"/>
+      <c r="F78" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G78" s="64"/>
+      <c r="G78" s="80"/>
       <c r="H78" s="47"/>
       <c r="I78" s="12"/>
       <c r="J78" s="12"/>
@@ -15831,22 +15835,22 @@
       <c r="GI78" s="32"/>
     </row>
     <row r="79" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A79" s="82" t="s">
+      <c r="A79" s="73" t="s">
         <v>150</v>
       </c>
-      <c r="B79" s="83"/>
+      <c r="B79" s="74"/>
       <c r="C79" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="D79" s="62">
+      <c r="D79" s="65">
         <v>6</v>
       </c>
-      <c r="E79" s="63"/>
-      <c r="F79" s="62">
+      <c r="E79" s="66"/>
+      <c r="F79" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G79" s="64"/>
+      <c r="G79" s="80"/>
       <c r="H79" s="47"/>
       <c r="I79" s="12"/>
       <c r="J79" s="12"/>
@@ -16033,22 +16037,22 @@
       <c r="GI79" s="36"/>
     </row>
     <row r="80" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A80" s="82" t="s">
+      <c r="A80" s="73" t="s">
         <v>152</v>
       </c>
-      <c r="B80" s="83"/>
+      <c r="B80" s="74"/>
       <c r="C80" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D80" s="62">
+      <c r="D80" s="65">
         <v>6</v>
       </c>
-      <c r="E80" s="63"/>
-      <c r="F80" s="62">
+      <c r="E80" s="66"/>
+      <c r="F80" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G80" s="64"/>
+      <c r="G80" s="80"/>
       <c r="H80" s="47"/>
       <c r="I80" s="12"/>
       <c r="J80" s="12"/>
@@ -16235,21 +16239,21 @@
       <c r="GI80" s="36"/>
     </row>
     <row r="81" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A81" s="76" t="s">
+      <c r="A81" s="115" t="s">
         <v>153</v>
       </c>
-      <c r="B81" s="77"/>
+      <c r="B81" s="116"/>
       <c r="C81" s="39"/>
-      <c r="D81" s="78">
+      <c r="D81" s="71">
         <f>SUM(D82:E82)</f>
         <v>16</v>
       </c>
-      <c r="E81" s="88"/>
-      <c r="F81" s="78">
+      <c r="E81" s="72"/>
+      <c r="F81" s="71">
         <f>SUM(F82:G82)</f>
         <v>0</v>
       </c>
-      <c r="G81" s="80"/>
+      <c r="G81" s="75"/>
       <c r="H81" s="29"/>
       <c r="I81" s="8"/>
       <c r="J81" s="8"/>
@@ -16436,20 +16440,20 @@
       <c r="GI81" s="29"/>
     </row>
     <row r="82" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A82" s="86" t="s">
+      <c r="A82" s="93" t="s">
         <v>153</v>
       </c>
-      <c r="B82" s="87"/>
+      <c r="B82" s="94"/>
       <c r="C82" s="40"/>
-      <c r="D82" s="84">
+      <c r="D82" s="91">
         <v>16</v>
       </c>
-      <c r="E82" s="85"/>
-      <c r="F82" s="62">
+      <c r="E82" s="92"/>
+      <c r="F82" s="65">
         <f>SUM(H82:GI82)</f>
         <v>0</v>
       </c>
-      <c r="G82" s="64"/>
+      <c r="G82" s="80"/>
       <c r="H82" s="26"/>
       <c r="I82" s="12"/>
       <c r="J82" s="12"/>
@@ -16636,21 +16640,21 @@
       <c r="GI82" s="32"/>
     </row>
     <row r="83" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A83" s="104" t="s">
+      <c r="A83" s="110" t="s">
         <v>154</v>
       </c>
-      <c r="B83" s="105"/>
+      <c r="B83" s="111"/>
       <c r="C83" s="41"/>
-      <c r="D83" s="78">
+      <c r="D83" s="71">
         <f>SUM(D84:E84)</f>
         <v>32</v>
       </c>
-      <c r="E83" s="88"/>
-      <c r="F83" s="78">
+      <c r="E83" s="72"/>
+      <c r="F83" s="71">
         <f>SUM(F84:G84)</f>
         <v>0</v>
       </c>
-      <c r="G83" s="80"/>
+      <c r="G83" s="75"/>
       <c r="H83" s="29"/>
       <c r="I83" s="8"/>
       <c r="J83" s="8"/>
@@ -16837,20 +16841,20 @@
       <c r="GI83" s="29"/>
     </row>
     <row r="84" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A84" s="108" t="s">
+      <c r="A84" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="B84" s="109"/>
+      <c r="B84" s="86"/>
       <c r="C84" s="42"/>
-      <c r="D84" s="62">
+      <c r="D84" s="65">
         <v>32</v>
       </c>
-      <c r="E84" s="63"/>
-      <c r="F84" s="62">
+      <c r="E84" s="66"/>
+      <c r="F84" s="65">
         <f>SUM(H84:GI84)</f>
         <v>0</v>
       </c>
-      <c r="G84" s="64"/>
+      <c r="G84" s="80"/>
       <c r="H84" s="26"/>
       <c r="I84" s="12"/>
       <c r="J84" s="12"/>
@@ -17037,21 +17041,21 @@
       <c r="GI84" s="32"/>
     </row>
     <row r="85" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A85" s="111" t="s">
+      <c r="A85" s="89" t="s">
         <v>155</v>
       </c>
-      <c r="B85" s="112"/>
+      <c r="B85" s="90"/>
       <c r="C85" s="43"/>
-      <c r="D85" s="78">
+      <c r="D85" s="71">
         <f>SUM(D86:E86)</f>
         <v>8</v>
       </c>
-      <c r="E85" s="88"/>
-      <c r="F85" s="89">
+      <c r="E85" s="72"/>
+      <c r="F85" s="95">
         <f>SUM(F86:G86)</f>
         <v>0</v>
       </c>
-      <c r="G85" s="90"/>
+      <c r="G85" s="96"/>
       <c r="H85" s="29"/>
       <c r="I85" s="8"/>
       <c r="J85" s="8"/>
@@ -17238,20 +17242,20 @@
       <c r="GI85" s="29"/>
     </row>
     <row r="86" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A86" s="110" t="s">
+      <c r="A86" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="B86" s="65"/>
+      <c r="B86" s="88"/>
       <c r="C86" s="27"/>
-      <c r="D86" s="62">
+      <c r="D86" s="65">
         <v>8</v>
       </c>
-      <c r="E86" s="63"/>
-      <c r="F86" s="62">
+      <c r="E86" s="66"/>
+      <c r="F86" s="65">
         <f>SUM(H86:GI86)</f>
         <v>0</v>
       </c>
-      <c r="G86" s="64"/>
+      <c r="G86" s="80"/>
       <c r="H86" s="26"/>
       <c r="I86" s="12"/>
       <c r="J86" s="12"/>
@@ -17438,20 +17442,20 @@
       <c r="GI86" s="32"/>
     </row>
     <row r="87" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A87" s="106" t="s">
+      <c r="A87" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="107"/>
+      <c r="B87" s="84"/>
       <c r="C87" s="43"/>
-      <c r="D87" s="78">
+      <c r="D87" s="71">
         <f>232-D90</f>
         <v>36.349999999999994</v>
       </c>
-      <c r="E87" s="88"/>
-      <c r="F87" s="78">
+      <c r="E87" s="72"/>
+      <c r="F87" s="71">
         <v>0</v>
       </c>
-      <c r="G87" s="80"/>
+      <c r="G87" s="75"/>
       <c r="H87" s="29"/>
       <c r="I87" s="8"/>
       <c r="J87" s="8"/>
@@ -17638,15 +17642,15 @@
       <c r="GI87" s="29"/>
     </row>
     <row r="88" spans="1:191" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="101" t="s">
+      <c r="A88" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="B88" s="102"/>
+      <c r="B88" s="108"/>
       <c r="C88" s="44"/>
-      <c r="D88" s="98"/>
-      <c r="E88" s="99"/>
-      <c r="F88" s="98"/>
-      <c r="G88" s="100"/>
+      <c r="D88" s="104"/>
+      <c r="E88" s="105"/>
+      <c r="F88" s="104"/>
+      <c r="G88" s="106"/>
       <c r="H88" s="28"/>
       <c r="I88" s="17"/>
       <c r="J88" s="17"/>
@@ -17885,21 +17889,21 @@
       <c r="AX89" s="3"/>
     </row>
     <row r="90" spans="1:191" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="96" t="s">
+      <c r="A90" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="97"/>
+      <c r="B90" s="103"/>
       <c r="C90" s="45"/>
-      <c r="D90" s="94">
+      <c r="D90" s="100">
         <f>SUM(D85,D83,D81,D62,D14)</f>
         <v>195.65</v>
       </c>
-      <c r="E90" s="95"/>
-      <c r="F90" s="94">
+      <c r="E90" s="101"/>
+      <c r="F90" s="100">
         <f>SUM(F85,F83,F81,F62,F14)</f>
-        <v>34.249000000000002</v>
-      </c>
-      <c r="G90" s="103"/>
+        <v>36.249000000000002</v>
+      </c>
+      <c r="G90" s="109"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
@@ -17946,6 +17950,316 @@
     </row>
   </sheetData>
   <mergeCells count="334">
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="GD13:GE13"/>
+    <mergeCell ref="GF13:GG13"/>
+    <mergeCell ref="GH13:GI13"/>
+    <mergeCell ref="DZ12:GI12"/>
+    <mergeCell ref="FL13:FM13"/>
+    <mergeCell ref="FN13:FO13"/>
+    <mergeCell ref="FP13:FQ13"/>
+    <mergeCell ref="FR13:FS13"/>
+    <mergeCell ref="FT13:FU13"/>
+    <mergeCell ref="FV13:FW13"/>
+    <mergeCell ref="FX13:FY13"/>
+    <mergeCell ref="FZ13:GA13"/>
+    <mergeCell ref="GB13:GC13"/>
+    <mergeCell ref="ET13:EU13"/>
+    <mergeCell ref="EV13:EW13"/>
+    <mergeCell ref="EX13:EY13"/>
+    <mergeCell ref="EZ13:FA13"/>
+    <mergeCell ref="FB13:FC13"/>
+    <mergeCell ref="FD13:FE13"/>
+    <mergeCell ref="FF13:FG13"/>
+    <mergeCell ref="DX13:DY13"/>
+    <mergeCell ref="FH13:FI13"/>
+    <mergeCell ref="FJ13:FK13"/>
+    <mergeCell ref="EB13:EC13"/>
+    <mergeCell ref="ED13:EE13"/>
+    <mergeCell ref="EF13:EG13"/>
+    <mergeCell ref="EH13:EI13"/>
+    <mergeCell ref="EJ13:EK13"/>
+    <mergeCell ref="EL13:EM13"/>
+    <mergeCell ref="EN13:EO13"/>
+    <mergeCell ref="EP13:EQ13"/>
+    <mergeCell ref="ER13:ES13"/>
+    <mergeCell ref="DF13:DG13"/>
+    <mergeCell ref="DH13:DI13"/>
+    <mergeCell ref="DJ13:DK13"/>
+    <mergeCell ref="DL13:DM13"/>
+    <mergeCell ref="DN13:DO13"/>
+    <mergeCell ref="DP13:DQ13"/>
+    <mergeCell ref="DR13:DS13"/>
+    <mergeCell ref="DT13:DU13"/>
+    <mergeCell ref="DV13:DW13"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="BH13:BI13"/>
+    <mergeCell ref="BJ13:BK13"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="P9:X9"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F11:G13"/>
+    <mergeCell ref="D11:E13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="AL13:AM13"/>
+    <mergeCell ref="AN13:AO13"/>
+    <mergeCell ref="AP13:AQ13"/>
+    <mergeCell ref="AR13:AS13"/>
+    <mergeCell ref="AT13:AU13"/>
+    <mergeCell ref="AV13:AW13"/>
+    <mergeCell ref="AX13:AY13"/>
+    <mergeCell ref="AZ13:BA13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="P6:X6"/>
+    <mergeCell ref="P5:X5"/>
+    <mergeCell ref="P4:X4"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="H12:BQ12"/>
+    <mergeCell ref="BB13:BC13"/>
+    <mergeCell ref="BD13:BE13"/>
+    <mergeCell ref="BF13:BG13"/>
+    <mergeCell ref="BP13:BQ13"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="AF13:AG13"/>
+    <mergeCell ref="AH13:AI13"/>
+    <mergeCell ref="AJ13:AK13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
     <mergeCell ref="BR13:BS13"/>
     <mergeCell ref="BL13:BM13"/>
     <mergeCell ref="BN13:BO13"/>
@@ -17970,316 +18284,6 @@
     <mergeCell ref="CZ13:DA13"/>
     <mergeCell ref="DB13:DC13"/>
     <mergeCell ref="DD13:DE13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="P6:X6"/>
-    <mergeCell ref="P5:X5"/>
-    <mergeCell ref="P4:X4"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="H12:BQ12"/>
-    <mergeCell ref="BB13:BC13"/>
-    <mergeCell ref="BD13:BE13"/>
-    <mergeCell ref="BF13:BG13"/>
-    <mergeCell ref="BP13:BQ13"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="AF13:AG13"/>
-    <mergeCell ref="AH13:AI13"/>
-    <mergeCell ref="AJ13:AK13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="AL13:AM13"/>
-    <mergeCell ref="AN13:AO13"/>
-    <mergeCell ref="AP13:AQ13"/>
-    <mergeCell ref="AR13:AS13"/>
-    <mergeCell ref="AT13:AU13"/>
-    <mergeCell ref="AV13:AW13"/>
-    <mergeCell ref="AX13:AY13"/>
-    <mergeCell ref="AZ13:BA13"/>
-    <mergeCell ref="BH13:BI13"/>
-    <mergeCell ref="BJ13:BK13"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="P9:X9"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F11:G13"/>
-    <mergeCell ref="D11:E13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="F90:G90"/>
-    <mergeCell ref="F87:G87"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="DF13:DG13"/>
-    <mergeCell ref="DH13:DI13"/>
-    <mergeCell ref="DJ13:DK13"/>
-    <mergeCell ref="DL13:DM13"/>
-    <mergeCell ref="DN13:DO13"/>
-    <mergeCell ref="DP13:DQ13"/>
-    <mergeCell ref="DR13:DS13"/>
-    <mergeCell ref="DT13:DU13"/>
-    <mergeCell ref="DV13:DW13"/>
-    <mergeCell ref="FF13:FG13"/>
-    <mergeCell ref="DX13:DY13"/>
-    <mergeCell ref="FH13:FI13"/>
-    <mergeCell ref="FJ13:FK13"/>
-    <mergeCell ref="EB13:EC13"/>
-    <mergeCell ref="ED13:EE13"/>
-    <mergeCell ref="EF13:EG13"/>
-    <mergeCell ref="EH13:EI13"/>
-    <mergeCell ref="EJ13:EK13"/>
-    <mergeCell ref="EL13:EM13"/>
-    <mergeCell ref="EN13:EO13"/>
-    <mergeCell ref="EP13:EQ13"/>
-    <mergeCell ref="ER13:ES13"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="GD13:GE13"/>
-    <mergeCell ref="GF13:GG13"/>
-    <mergeCell ref="GH13:GI13"/>
-    <mergeCell ref="DZ12:GI12"/>
-    <mergeCell ref="FL13:FM13"/>
-    <mergeCell ref="FN13:FO13"/>
-    <mergeCell ref="FP13:FQ13"/>
-    <mergeCell ref="FR13:FS13"/>
-    <mergeCell ref="FT13:FU13"/>
-    <mergeCell ref="FV13:FW13"/>
-    <mergeCell ref="FX13:FY13"/>
-    <mergeCell ref="FZ13:GA13"/>
-    <mergeCell ref="GB13:GC13"/>
-    <mergeCell ref="ET13:EU13"/>
-    <mergeCell ref="EV13:EW13"/>
-    <mergeCell ref="EX13:EY13"/>
-    <mergeCell ref="EZ13:FA13"/>
-    <mergeCell ref="FB13:FC13"/>
-    <mergeCell ref="FD13:FE13"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Created Model for Issue #53
</commit_message>
<xml_diff>
--- a/Documents/Zeitplan.xlsx
+++ b/Documents/Zeitplan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VirtualReality\Documents\SiemensVR\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VirtualReality\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1164,24 +1164,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1194,31 +1176,32 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1226,6 +1209,42 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1234,9 +1253,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1284,40 +1300,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1418,8 +1418,8 @@
       <xdr:rowOff>51955</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>212420</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>386592</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>34638</xdr:rowOff>
     </xdr:to>
@@ -1787,13 +1787,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GI90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AL20" sqref="AL20"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AM20" sqref="AM20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="38" width="5.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="38" width="5.77734375" style="1" customWidth="1"/>
     <col min="39" max="39" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="40" max="191" width="5.77734375" style="1" customWidth="1"/>
     <col min="192" max="256" width="3.33203125" style="1" customWidth="1"/>
@@ -1801,28 +1803,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:191" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
     </row>
     <row r="2" spans="1:191" x14ac:dyDescent="0.25">
       <c r="T2" s="9"/>
@@ -1855,17 +1857,17 @@
         <v>160</v>
       </c>
       <c r="N4" s="57"/>
-      <c r="P4" s="81" t="s">
+      <c r="P4" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="81"/>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="67"/>
+      <c r="V4" s="67"/>
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
     </row>
     <row r="5" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -1882,17 +1884,17 @@
       <c r="F5" s="5"/>
       <c r="G5" s="7"/>
       <c r="N5" s="24"/>
-      <c r="P5" s="81" t="s">
+      <c r="P5" s="67" t="s">
         <v>158</v>
       </c>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81"/>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="81"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
+      <c r="S5" s="67"/>
+      <c r="T5" s="67"/>
+      <c r="U5" s="67"/>
+      <c r="V5" s="67"/>
+      <c r="W5" s="67"/>
+      <c r="X5" s="67"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
@@ -1916,17 +1918,17 @@
         <v>15</v>
       </c>
       <c r="N6" s="16"/>
-      <c r="P6" s="81" t="s">
+      <c r="P6" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="81"/>
-      <c r="T6" s="81"/>
-      <c r="U6" s="81"/>
-      <c r="V6" s="81"/>
-      <c r="W6" s="81"/>
-      <c r="X6" s="81"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="67"/>
+      <c r="V6" s="67"/>
+      <c r="W6" s="67"/>
+      <c r="X6" s="67"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
@@ -1944,17 +1946,17 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="N7" s="21"/>
-      <c r="P7" s="81" t="s">
+      <c r="P7" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="81"/>
-      <c r="S7" s="81"/>
-      <c r="T7" s="81"/>
-      <c r="U7" s="81"/>
-      <c r="V7" s="81"/>
-      <c r="W7" s="81"/>
-      <c r="X7" s="81"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="67"/>
+      <c r="S7" s="67"/>
+      <c r="T7" s="67"/>
+      <c r="U7" s="67"/>
+      <c r="V7" s="67"/>
+      <c r="W7" s="67"/>
+      <c r="X7" s="67"/>
     </row>
     <row r="8" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1969,17 +1971,17 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="N8" s="20"/>
-      <c r="P8" s="113" t="s">
+      <c r="P8" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="113"/>
-      <c r="R8" s="113"/>
-      <c r="S8" s="113"/>
-      <c r="T8" s="113"/>
-      <c r="U8" s="113"/>
-      <c r="V8" s="113"/>
-      <c r="W8" s="113"/>
-      <c r="X8" s="113"/>
+      <c r="Q8" s="70"/>
+      <c r="R8" s="70"/>
+      <c r="S8" s="70"/>
+      <c r="T8" s="70"/>
+      <c r="U8" s="70"/>
+      <c r="V8" s="70"/>
+      <c r="W8" s="70"/>
+      <c r="X8" s="70"/>
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
@@ -1987,23 +1989,23 @@
       <c r="AC8" s="5"/>
     </row>
     <row r="9" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="118"/>
+      <c r="A9" s="68"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="12"/>
       <c r="N9" s="49"/>
-      <c r="P9" s="113" t="s">
+      <c r="P9" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="Q9" s="113"/>
-      <c r="R9" s="113"/>
-      <c r="S9" s="113"/>
-      <c r="T9" s="113"/>
-      <c r="U9" s="113"/>
-      <c r="V9" s="113"/>
-      <c r="W9" s="113"/>
-      <c r="X9" s="113"/>
+      <c r="Q9" s="70"/>
+      <c r="R9" s="70"/>
+      <c r="S9" s="70"/>
+      <c r="T9" s="70"/>
+      <c r="U9" s="70"/>
+      <c r="V9" s="70"/>
+      <c r="W9" s="70"/>
+      <c r="X9" s="70"/>
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
@@ -2013,7 +2015,7 @@
       <c r="AJ9" s="13"/>
     </row>
     <row r="10" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="118"/>
+      <c r="A10" s="68"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -2030,18 +2032,18 @@
       <c r="AC10" s="5"/>
     </row>
     <row r="11" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="118"/>
-      <c r="C11" s="116" t="s">
+      <c r="A11" s="68"/>
+      <c r="C11" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="114" t="s">
+      <c r="D11" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="114"/>
-      <c r="F11" s="114" t="s">
+      <c r="E11" s="76"/>
+      <c r="F11" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="114"/>
+      <c r="G11" s="76"/>
       <c r="T11" s="9"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
@@ -2054,596 +2056,596 @@
       <c r="AC11" s="5"/>
     </row>
     <row r="12" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="118"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="114"/>
-      <c r="G12" s="114"/>
-      <c r="H12" s="70" t="s">
+      <c r="A12" s="68"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="71"/>
-      <c r="N12" s="71"/>
-      <c r="O12" s="71"/>
-      <c r="P12" s="71"/>
-      <c r="Q12" s="71"/>
-      <c r="R12" s="71"/>
-      <c r="S12" s="71"/>
-      <c r="T12" s="71"/>
-      <c r="U12" s="71"/>
-      <c r="V12" s="71"/>
-      <c r="W12" s="71"/>
-      <c r="X12" s="71"/>
-      <c r="Y12" s="71"/>
-      <c r="Z12" s="71"/>
-      <c r="AA12" s="71"/>
-      <c r="AB12" s="71"/>
-      <c r="AC12" s="71"/>
-      <c r="AD12" s="71"/>
-      <c r="AE12" s="71"/>
-      <c r="AF12" s="71"/>
-      <c r="AG12" s="71"/>
-      <c r="AH12" s="71"/>
-      <c r="AI12" s="71"/>
-      <c r="AJ12" s="71"/>
-      <c r="AK12" s="71"/>
-      <c r="AL12" s="71"/>
-      <c r="AM12" s="71"/>
-      <c r="AN12" s="71"/>
-      <c r="AO12" s="71"/>
-      <c r="AP12" s="71"/>
-      <c r="AQ12" s="71"/>
-      <c r="AR12" s="71"/>
-      <c r="AS12" s="71"/>
-      <c r="AT12" s="71"/>
-      <c r="AU12" s="71"/>
-      <c r="AV12" s="71"/>
-      <c r="AW12" s="71"/>
-      <c r="AX12" s="71"/>
-      <c r="AY12" s="71"/>
-      <c r="AZ12" s="71"/>
-      <c r="BA12" s="71"/>
-      <c r="BB12" s="71"/>
-      <c r="BC12" s="71"/>
-      <c r="BD12" s="71"/>
-      <c r="BE12" s="71"/>
-      <c r="BF12" s="71"/>
-      <c r="BG12" s="71"/>
-      <c r="BH12" s="71"/>
-      <c r="BI12" s="71"/>
-      <c r="BJ12" s="71"/>
-      <c r="BK12" s="71"/>
-      <c r="BL12" s="71"/>
-      <c r="BM12" s="71"/>
-      <c r="BN12" s="71"/>
-      <c r="BO12" s="71"/>
-      <c r="BP12" s="71"/>
-      <c r="BQ12" s="119"/>
-      <c r="BR12" s="70" t="s">
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="63"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="63"/>
+      <c r="W12" s="63"/>
+      <c r="X12" s="63"/>
+      <c r="Y12" s="63"/>
+      <c r="Z12" s="63"/>
+      <c r="AA12" s="63"/>
+      <c r="AB12" s="63"/>
+      <c r="AC12" s="63"/>
+      <c r="AD12" s="63"/>
+      <c r="AE12" s="63"/>
+      <c r="AF12" s="63"/>
+      <c r="AG12" s="63"/>
+      <c r="AH12" s="63"/>
+      <c r="AI12" s="63"/>
+      <c r="AJ12" s="63"/>
+      <c r="AK12" s="63"/>
+      <c r="AL12" s="63"/>
+      <c r="AM12" s="63"/>
+      <c r="AN12" s="63"/>
+      <c r="AO12" s="63"/>
+      <c r="AP12" s="63"/>
+      <c r="AQ12" s="63"/>
+      <c r="AR12" s="63"/>
+      <c r="AS12" s="63"/>
+      <c r="AT12" s="63"/>
+      <c r="AU12" s="63"/>
+      <c r="AV12" s="63"/>
+      <c r="AW12" s="63"/>
+      <c r="AX12" s="63"/>
+      <c r="AY12" s="63"/>
+      <c r="AZ12" s="63"/>
+      <c r="BA12" s="63"/>
+      <c r="BB12" s="63"/>
+      <c r="BC12" s="63"/>
+      <c r="BD12" s="63"/>
+      <c r="BE12" s="63"/>
+      <c r="BF12" s="63"/>
+      <c r="BG12" s="63"/>
+      <c r="BH12" s="63"/>
+      <c r="BI12" s="63"/>
+      <c r="BJ12" s="63"/>
+      <c r="BK12" s="63"/>
+      <c r="BL12" s="63"/>
+      <c r="BM12" s="63"/>
+      <c r="BN12" s="63"/>
+      <c r="BO12" s="63"/>
+      <c r="BP12" s="63"/>
+      <c r="BQ12" s="64"/>
+      <c r="BR12" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="BS12" s="71"/>
-      <c r="BT12" s="71"/>
-      <c r="BU12" s="71"/>
-      <c r="BV12" s="71"/>
-      <c r="BW12" s="71"/>
-      <c r="BX12" s="71"/>
-      <c r="BY12" s="71"/>
-      <c r="BZ12" s="71"/>
-      <c r="CA12" s="71"/>
-      <c r="CB12" s="71"/>
-      <c r="CC12" s="71"/>
-      <c r="CD12" s="71"/>
-      <c r="CE12" s="71"/>
-      <c r="CF12" s="71"/>
-      <c r="CG12" s="71"/>
-      <c r="CH12" s="71"/>
-      <c r="CI12" s="71"/>
-      <c r="CJ12" s="71"/>
-      <c r="CK12" s="71"/>
-      <c r="CL12" s="71"/>
-      <c r="CM12" s="71"/>
-      <c r="CN12" s="71"/>
-      <c r="CO12" s="71"/>
-      <c r="CP12" s="71"/>
-      <c r="CQ12" s="71"/>
-      <c r="CR12" s="71"/>
-      <c r="CS12" s="71"/>
-      <c r="CT12" s="71"/>
-      <c r="CU12" s="71"/>
-      <c r="CV12" s="71"/>
-      <c r="CW12" s="71"/>
-      <c r="CX12" s="71"/>
-      <c r="CY12" s="71"/>
-      <c r="CZ12" s="71"/>
-      <c r="DA12" s="71"/>
-      <c r="DB12" s="71"/>
-      <c r="DC12" s="71"/>
-      <c r="DD12" s="71"/>
-      <c r="DE12" s="71"/>
-      <c r="DF12" s="71"/>
-      <c r="DG12" s="71"/>
-      <c r="DH12" s="71"/>
-      <c r="DI12" s="71"/>
-      <c r="DJ12" s="71"/>
-      <c r="DK12" s="71"/>
-      <c r="DL12" s="71"/>
-      <c r="DM12" s="71"/>
-      <c r="DN12" s="71"/>
-      <c r="DO12" s="71"/>
-      <c r="DP12" s="71"/>
-      <c r="DQ12" s="71"/>
-      <c r="DR12" s="71"/>
-      <c r="DS12" s="71"/>
-      <c r="DT12" s="71"/>
-      <c r="DU12" s="71"/>
-      <c r="DV12" s="71"/>
-      <c r="DW12" s="71"/>
-      <c r="DX12" s="71"/>
-      <c r="DY12" s="119"/>
-      <c r="DZ12" s="70" t="s">
+      <c r="BS12" s="63"/>
+      <c r="BT12" s="63"/>
+      <c r="BU12" s="63"/>
+      <c r="BV12" s="63"/>
+      <c r="BW12" s="63"/>
+      <c r="BX12" s="63"/>
+      <c r="BY12" s="63"/>
+      <c r="BZ12" s="63"/>
+      <c r="CA12" s="63"/>
+      <c r="CB12" s="63"/>
+      <c r="CC12" s="63"/>
+      <c r="CD12" s="63"/>
+      <c r="CE12" s="63"/>
+      <c r="CF12" s="63"/>
+      <c r="CG12" s="63"/>
+      <c r="CH12" s="63"/>
+      <c r="CI12" s="63"/>
+      <c r="CJ12" s="63"/>
+      <c r="CK12" s="63"/>
+      <c r="CL12" s="63"/>
+      <c r="CM12" s="63"/>
+      <c r="CN12" s="63"/>
+      <c r="CO12" s="63"/>
+      <c r="CP12" s="63"/>
+      <c r="CQ12" s="63"/>
+      <c r="CR12" s="63"/>
+      <c r="CS12" s="63"/>
+      <c r="CT12" s="63"/>
+      <c r="CU12" s="63"/>
+      <c r="CV12" s="63"/>
+      <c r="CW12" s="63"/>
+      <c r="CX12" s="63"/>
+      <c r="CY12" s="63"/>
+      <c r="CZ12" s="63"/>
+      <c r="DA12" s="63"/>
+      <c r="DB12" s="63"/>
+      <c r="DC12" s="63"/>
+      <c r="DD12" s="63"/>
+      <c r="DE12" s="63"/>
+      <c r="DF12" s="63"/>
+      <c r="DG12" s="63"/>
+      <c r="DH12" s="63"/>
+      <c r="DI12" s="63"/>
+      <c r="DJ12" s="63"/>
+      <c r="DK12" s="63"/>
+      <c r="DL12" s="63"/>
+      <c r="DM12" s="63"/>
+      <c r="DN12" s="63"/>
+      <c r="DO12" s="63"/>
+      <c r="DP12" s="63"/>
+      <c r="DQ12" s="63"/>
+      <c r="DR12" s="63"/>
+      <c r="DS12" s="63"/>
+      <c r="DT12" s="63"/>
+      <c r="DU12" s="63"/>
+      <c r="DV12" s="63"/>
+      <c r="DW12" s="63"/>
+      <c r="DX12" s="63"/>
+      <c r="DY12" s="64"/>
+      <c r="DZ12" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="EA12" s="71"/>
-      <c r="EB12" s="71"/>
-      <c r="EC12" s="71"/>
-      <c r="ED12" s="71"/>
-      <c r="EE12" s="71"/>
-      <c r="EF12" s="71"/>
-      <c r="EG12" s="71"/>
-      <c r="EH12" s="71"/>
-      <c r="EI12" s="71"/>
-      <c r="EJ12" s="71"/>
-      <c r="EK12" s="71"/>
-      <c r="EL12" s="71"/>
-      <c r="EM12" s="71"/>
-      <c r="EN12" s="71"/>
-      <c r="EO12" s="71"/>
-      <c r="EP12" s="71"/>
-      <c r="EQ12" s="71"/>
-      <c r="ER12" s="71"/>
-      <c r="ES12" s="71"/>
-      <c r="ET12" s="71"/>
-      <c r="EU12" s="71"/>
-      <c r="EV12" s="71"/>
-      <c r="EW12" s="71"/>
-      <c r="EX12" s="71"/>
-      <c r="EY12" s="71"/>
-      <c r="EZ12" s="71"/>
-      <c r="FA12" s="71"/>
-      <c r="FB12" s="71"/>
-      <c r="FC12" s="71"/>
-      <c r="FD12" s="71"/>
-      <c r="FE12" s="71"/>
-      <c r="FF12" s="71"/>
-      <c r="FG12" s="71"/>
-      <c r="FH12" s="71"/>
-      <c r="FI12" s="71"/>
-      <c r="FJ12" s="71"/>
-      <c r="FK12" s="71"/>
-      <c r="FL12" s="71"/>
-      <c r="FM12" s="71"/>
-      <c r="FN12" s="71"/>
-      <c r="FO12" s="71"/>
-      <c r="FP12" s="71"/>
-      <c r="FQ12" s="71"/>
-      <c r="FR12" s="71"/>
-      <c r="FS12" s="71"/>
-      <c r="FT12" s="71"/>
-      <c r="FU12" s="71"/>
-      <c r="FV12" s="71"/>
-      <c r="FW12" s="71"/>
-      <c r="FX12" s="71"/>
-      <c r="FY12" s="71"/>
-      <c r="FZ12" s="71"/>
-      <c r="GA12" s="71"/>
-      <c r="GB12" s="71"/>
-      <c r="GC12" s="71"/>
-      <c r="GD12" s="71"/>
-      <c r="GE12" s="71"/>
-      <c r="GF12" s="71"/>
-      <c r="GG12" s="71"/>
-      <c r="GH12" s="71"/>
-      <c r="GI12" s="72"/>
+      <c r="EA12" s="63"/>
+      <c r="EB12" s="63"/>
+      <c r="EC12" s="63"/>
+      <c r="ED12" s="63"/>
+      <c r="EE12" s="63"/>
+      <c r="EF12" s="63"/>
+      <c r="EG12" s="63"/>
+      <c r="EH12" s="63"/>
+      <c r="EI12" s="63"/>
+      <c r="EJ12" s="63"/>
+      <c r="EK12" s="63"/>
+      <c r="EL12" s="63"/>
+      <c r="EM12" s="63"/>
+      <c r="EN12" s="63"/>
+      <c r="EO12" s="63"/>
+      <c r="EP12" s="63"/>
+      <c r="EQ12" s="63"/>
+      <c r="ER12" s="63"/>
+      <c r="ES12" s="63"/>
+      <c r="ET12" s="63"/>
+      <c r="EU12" s="63"/>
+      <c r="EV12" s="63"/>
+      <c r="EW12" s="63"/>
+      <c r="EX12" s="63"/>
+      <c r="EY12" s="63"/>
+      <c r="EZ12" s="63"/>
+      <c r="FA12" s="63"/>
+      <c r="FB12" s="63"/>
+      <c r="FC12" s="63"/>
+      <c r="FD12" s="63"/>
+      <c r="FE12" s="63"/>
+      <c r="FF12" s="63"/>
+      <c r="FG12" s="63"/>
+      <c r="FH12" s="63"/>
+      <c r="FI12" s="63"/>
+      <c r="FJ12" s="63"/>
+      <c r="FK12" s="63"/>
+      <c r="FL12" s="63"/>
+      <c r="FM12" s="63"/>
+      <c r="FN12" s="63"/>
+      <c r="FO12" s="63"/>
+      <c r="FP12" s="63"/>
+      <c r="FQ12" s="63"/>
+      <c r="FR12" s="63"/>
+      <c r="FS12" s="63"/>
+      <c r="FT12" s="63"/>
+      <c r="FU12" s="63"/>
+      <c r="FV12" s="63"/>
+      <c r="FW12" s="63"/>
+      <c r="FX12" s="63"/>
+      <c r="FY12" s="63"/>
+      <c r="FZ12" s="63"/>
+      <c r="GA12" s="63"/>
+      <c r="GB12" s="63"/>
+      <c r="GC12" s="63"/>
+      <c r="GD12" s="63"/>
+      <c r="GE12" s="63"/>
+      <c r="GF12" s="63"/>
+      <c r="GG12" s="63"/>
+      <c r="GH12" s="63"/>
+      <c r="GI12" s="120"/>
     </row>
     <row r="13" spans="1:191" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="117"/>
-      <c r="D13" s="115"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="115"/>
-      <c r="H13" s="68">
+      <c r="C13" s="79"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="60">
         <v>1</v>
       </c>
-      <c r="I13" s="69"/>
-      <c r="J13" s="68">
+      <c r="I13" s="61"/>
+      <c r="J13" s="60">
         <v>2</v>
       </c>
-      <c r="K13" s="69"/>
-      <c r="L13" s="68">
+      <c r="K13" s="61"/>
+      <c r="L13" s="60">
         <v>3</v>
       </c>
-      <c r="M13" s="69"/>
-      <c r="N13" s="68">
+      <c r="M13" s="61"/>
+      <c r="N13" s="60">
         <v>4</v>
       </c>
-      <c r="O13" s="69"/>
-      <c r="P13" s="68">
+      <c r="O13" s="61"/>
+      <c r="P13" s="60">
         <v>5</v>
       </c>
-      <c r="Q13" s="69"/>
-      <c r="R13" s="68">
+      <c r="Q13" s="61"/>
+      <c r="R13" s="60">
         <v>6</v>
       </c>
-      <c r="S13" s="69"/>
-      <c r="T13" s="68">
+      <c r="S13" s="61"/>
+      <c r="T13" s="60">
         <v>7</v>
       </c>
-      <c r="U13" s="69"/>
-      <c r="V13" s="68">
+      <c r="U13" s="61"/>
+      <c r="V13" s="60">
         <v>8</v>
       </c>
-      <c r="W13" s="69"/>
-      <c r="X13" s="68">
+      <c r="W13" s="61"/>
+      <c r="X13" s="60">
         <v>9</v>
       </c>
-      <c r="Y13" s="69"/>
-      <c r="Z13" s="68">
+      <c r="Y13" s="61"/>
+      <c r="Z13" s="60">
         <v>10</v>
       </c>
-      <c r="AA13" s="69"/>
-      <c r="AB13" s="68">
+      <c r="AA13" s="61"/>
+      <c r="AB13" s="60">
         <v>11</v>
       </c>
-      <c r="AC13" s="69"/>
-      <c r="AD13" s="68">
+      <c r="AC13" s="61"/>
+      <c r="AD13" s="60">
         <v>12</v>
       </c>
-      <c r="AE13" s="69"/>
-      <c r="AF13" s="68">
+      <c r="AE13" s="61"/>
+      <c r="AF13" s="60">
         <v>13</v>
       </c>
-      <c r="AG13" s="69"/>
-      <c r="AH13" s="68">
+      <c r="AG13" s="61"/>
+      <c r="AH13" s="60">
         <v>14</v>
       </c>
-      <c r="AI13" s="69"/>
-      <c r="AJ13" s="68">
+      <c r="AI13" s="61"/>
+      <c r="AJ13" s="60">
         <v>15</v>
       </c>
-      <c r="AK13" s="69"/>
-      <c r="AL13" s="68">
+      <c r="AK13" s="61"/>
+      <c r="AL13" s="60">
         <v>16</v>
       </c>
-      <c r="AM13" s="69"/>
-      <c r="AN13" s="68">
+      <c r="AM13" s="61"/>
+      <c r="AN13" s="60">
         <v>17</v>
       </c>
-      <c r="AO13" s="69"/>
-      <c r="AP13" s="68">
+      <c r="AO13" s="61"/>
+      <c r="AP13" s="60">
         <v>18</v>
       </c>
-      <c r="AQ13" s="69"/>
-      <c r="AR13" s="68">
+      <c r="AQ13" s="61"/>
+      <c r="AR13" s="60">
         <v>19</v>
       </c>
-      <c r="AS13" s="69"/>
-      <c r="AT13" s="68">
+      <c r="AS13" s="61"/>
+      <c r="AT13" s="60">
         <v>20</v>
       </c>
-      <c r="AU13" s="69"/>
-      <c r="AV13" s="68">
+      <c r="AU13" s="61"/>
+      <c r="AV13" s="60">
         <v>21</v>
       </c>
-      <c r="AW13" s="69"/>
-      <c r="AX13" s="68">
+      <c r="AW13" s="61"/>
+      <c r="AX13" s="60">
         <v>22</v>
       </c>
-      <c r="AY13" s="69"/>
-      <c r="AZ13" s="68">
+      <c r="AY13" s="61"/>
+      <c r="AZ13" s="60">
         <v>23</v>
       </c>
-      <c r="BA13" s="69"/>
-      <c r="BB13" s="68">
+      <c r="BA13" s="61"/>
+      <c r="BB13" s="60">
         <v>24</v>
       </c>
-      <c r="BC13" s="69"/>
-      <c r="BD13" s="68">
+      <c r="BC13" s="61"/>
+      <c r="BD13" s="60">
         <v>25</v>
       </c>
-      <c r="BE13" s="69"/>
-      <c r="BF13" s="68">
+      <c r="BE13" s="61"/>
+      <c r="BF13" s="60">
         <v>26</v>
       </c>
-      <c r="BG13" s="69"/>
-      <c r="BH13" s="68">
+      <c r="BG13" s="61"/>
+      <c r="BH13" s="60">
         <v>27</v>
       </c>
-      <c r="BI13" s="69"/>
-      <c r="BJ13" s="68">
+      <c r="BI13" s="61"/>
+      <c r="BJ13" s="60">
         <v>28</v>
       </c>
-      <c r="BK13" s="69"/>
-      <c r="BL13" s="68">
+      <c r="BK13" s="61"/>
+      <c r="BL13" s="60">
         <v>29</v>
       </c>
-      <c r="BM13" s="69"/>
-      <c r="BN13" s="68">
+      <c r="BM13" s="61"/>
+      <c r="BN13" s="60">
         <v>30</v>
       </c>
-      <c r="BO13" s="69"/>
-      <c r="BP13" s="68">
+      <c r="BO13" s="61"/>
+      <c r="BP13" s="60">
         <v>31</v>
       </c>
-      <c r="BQ13" s="120"/>
-      <c r="BR13" s="68">
+      <c r="BQ13" s="69"/>
+      <c r="BR13" s="60">
         <v>1</v>
       </c>
-      <c r="BS13" s="69"/>
-      <c r="BT13" s="68">
+      <c r="BS13" s="61"/>
+      <c r="BT13" s="60">
         <v>2</v>
       </c>
-      <c r="BU13" s="69"/>
-      <c r="BV13" s="68">
+      <c r="BU13" s="61"/>
+      <c r="BV13" s="60">
         <v>3</v>
       </c>
-      <c r="BW13" s="69"/>
-      <c r="BX13" s="68">
+      <c r="BW13" s="61"/>
+      <c r="BX13" s="60">
         <v>4</v>
       </c>
-      <c r="BY13" s="69"/>
-      <c r="BZ13" s="68">
+      <c r="BY13" s="61"/>
+      <c r="BZ13" s="60">
         <v>5</v>
       </c>
-      <c r="CA13" s="69"/>
-      <c r="CB13" s="68">
+      <c r="CA13" s="61"/>
+      <c r="CB13" s="60">
         <v>6</v>
       </c>
-      <c r="CC13" s="69"/>
-      <c r="CD13" s="68">
+      <c r="CC13" s="61"/>
+      <c r="CD13" s="60">
         <v>7</v>
       </c>
-      <c r="CE13" s="69"/>
-      <c r="CF13" s="68">
+      <c r="CE13" s="61"/>
+      <c r="CF13" s="60">
         <v>8</v>
       </c>
-      <c r="CG13" s="69"/>
-      <c r="CH13" s="68">
+      <c r="CG13" s="61"/>
+      <c r="CH13" s="60">
         <v>9</v>
       </c>
-      <c r="CI13" s="69"/>
-      <c r="CJ13" s="68">
+      <c r="CI13" s="61"/>
+      <c r="CJ13" s="60">
         <v>10</v>
       </c>
-      <c r="CK13" s="69"/>
-      <c r="CL13" s="68">
+      <c r="CK13" s="61"/>
+      <c r="CL13" s="60">
         <v>11</v>
       </c>
-      <c r="CM13" s="69"/>
-      <c r="CN13" s="68">
+      <c r="CM13" s="61"/>
+      <c r="CN13" s="60">
         <v>12</v>
       </c>
-      <c r="CO13" s="69"/>
-      <c r="CP13" s="68">
+      <c r="CO13" s="61"/>
+      <c r="CP13" s="60">
         <v>13</v>
       </c>
-      <c r="CQ13" s="69"/>
-      <c r="CR13" s="68">
+      <c r="CQ13" s="61"/>
+      <c r="CR13" s="60">
         <v>14</v>
       </c>
-      <c r="CS13" s="69"/>
-      <c r="CT13" s="68">
+      <c r="CS13" s="61"/>
+      <c r="CT13" s="60">
         <v>15</v>
       </c>
-      <c r="CU13" s="69"/>
-      <c r="CV13" s="68">
+      <c r="CU13" s="61"/>
+      <c r="CV13" s="60">
         <v>16</v>
       </c>
-      <c r="CW13" s="69"/>
-      <c r="CX13" s="68">
+      <c r="CW13" s="61"/>
+      <c r="CX13" s="60">
         <v>17</v>
       </c>
-      <c r="CY13" s="69"/>
-      <c r="CZ13" s="68">
+      <c r="CY13" s="61"/>
+      <c r="CZ13" s="60">
         <v>18</v>
       </c>
-      <c r="DA13" s="69"/>
-      <c r="DB13" s="68">
+      <c r="DA13" s="61"/>
+      <c r="DB13" s="60">
         <v>19</v>
       </c>
-      <c r="DC13" s="69"/>
-      <c r="DD13" s="68">
+      <c r="DC13" s="61"/>
+      <c r="DD13" s="60">
         <v>20</v>
       </c>
-      <c r="DE13" s="69"/>
-      <c r="DF13" s="68">
+      <c r="DE13" s="61"/>
+      <c r="DF13" s="60">
         <v>21</v>
       </c>
-      <c r="DG13" s="69"/>
-      <c r="DH13" s="68">
+      <c r="DG13" s="61"/>
+      <c r="DH13" s="60">
         <v>22</v>
       </c>
-      <c r="DI13" s="69"/>
-      <c r="DJ13" s="68">
+      <c r="DI13" s="61"/>
+      <c r="DJ13" s="60">
         <v>23</v>
       </c>
-      <c r="DK13" s="69"/>
-      <c r="DL13" s="68">
+      <c r="DK13" s="61"/>
+      <c r="DL13" s="60">
         <v>24</v>
       </c>
-      <c r="DM13" s="69"/>
-      <c r="DN13" s="68">
+      <c r="DM13" s="61"/>
+      <c r="DN13" s="60">
         <v>25</v>
       </c>
-      <c r="DO13" s="69"/>
-      <c r="DP13" s="68">
+      <c r="DO13" s="61"/>
+      <c r="DP13" s="60">
         <v>26</v>
       </c>
-      <c r="DQ13" s="69"/>
-      <c r="DR13" s="68">
+      <c r="DQ13" s="61"/>
+      <c r="DR13" s="60">
         <v>27</v>
       </c>
-      <c r="DS13" s="69"/>
-      <c r="DT13" s="68">
+      <c r="DS13" s="61"/>
+      <c r="DT13" s="60">
         <v>28</v>
       </c>
-      <c r="DU13" s="69"/>
-      <c r="DV13" s="68">
+      <c r="DU13" s="61"/>
+      <c r="DV13" s="60">
         <v>29</v>
       </c>
-      <c r="DW13" s="69"/>
-      <c r="DX13" s="68">
+      <c r="DW13" s="61"/>
+      <c r="DX13" s="60">
         <v>30</v>
       </c>
-      <c r="DY13" s="69"/>
-      <c r="DZ13" s="68">
+      <c r="DY13" s="61"/>
+      <c r="DZ13" s="60">
         <v>1</v>
       </c>
-      <c r="EA13" s="69"/>
-      <c r="EB13" s="68">
+      <c r="EA13" s="61"/>
+      <c r="EB13" s="60">
         <v>2</v>
       </c>
-      <c r="EC13" s="69"/>
-      <c r="ED13" s="68">
+      <c r="EC13" s="61"/>
+      <c r="ED13" s="60">
         <v>3</v>
       </c>
-      <c r="EE13" s="69"/>
-      <c r="EF13" s="68">
+      <c r="EE13" s="61"/>
+      <c r="EF13" s="60">
         <v>4</v>
       </c>
-      <c r="EG13" s="69"/>
-      <c r="EH13" s="68">
+      <c r="EG13" s="61"/>
+      <c r="EH13" s="60">
         <v>5</v>
       </c>
-      <c r="EI13" s="69"/>
-      <c r="EJ13" s="68">
+      <c r="EI13" s="61"/>
+      <c r="EJ13" s="60">
         <v>6</v>
       </c>
-      <c r="EK13" s="69"/>
-      <c r="EL13" s="68">
+      <c r="EK13" s="61"/>
+      <c r="EL13" s="60">
         <v>7</v>
       </c>
-      <c r="EM13" s="69"/>
-      <c r="EN13" s="68">
+      <c r="EM13" s="61"/>
+      <c r="EN13" s="60">
         <v>8</v>
       </c>
-      <c r="EO13" s="69"/>
-      <c r="EP13" s="68">
+      <c r="EO13" s="61"/>
+      <c r="EP13" s="60">
         <v>9</v>
       </c>
-      <c r="EQ13" s="69"/>
-      <c r="ER13" s="68">
+      <c r="EQ13" s="61"/>
+      <c r="ER13" s="60">
         <v>10</v>
       </c>
-      <c r="ES13" s="69"/>
-      <c r="ET13" s="68">
+      <c r="ES13" s="61"/>
+      <c r="ET13" s="60">
         <v>11</v>
       </c>
-      <c r="EU13" s="69"/>
-      <c r="EV13" s="68">
+      <c r="EU13" s="61"/>
+      <c r="EV13" s="60">
         <v>12</v>
       </c>
-      <c r="EW13" s="69"/>
-      <c r="EX13" s="68">
+      <c r="EW13" s="61"/>
+      <c r="EX13" s="60">
         <v>13</v>
       </c>
-      <c r="EY13" s="69"/>
-      <c r="EZ13" s="68">
+      <c r="EY13" s="61"/>
+      <c r="EZ13" s="60">
         <v>14</v>
       </c>
-      <c r="FA13" s="69"/>
-      <c r="FB13" s="68">
+      <c r="FA13" s="61"/>
+      <c r="FB13" s="60">
         <v>15</v>
       </c>
-      <c r="FC13" s="69"/>
-      <c r="FD13" s="68">
+      <c r="FC13" s="61"/>
+      <c r="FD13" s="60">
         <v>16</v>
       </c>
-      <c r="FE13" s="69"/>
-      <c r="FF13" s="68">
+      <c r="FE13" s="61"/>
+      <c r="FF13" s="60">
         <v>17</v>
       </c>
-      <c r="FG13" s="69"/>
-      <c r="FH13" s="68">
+      <c r="FG13" s="61"/>
+      <c r="FH13" s="60">
         <v>18</v>
       </c>
-      <c r="FI13" s="69"/>
-      <c r="FJ13" s="68">
+      <c r="FI13" s="61"/>
+      <c r="FJ13" s="60">
         <v>19</v>
       </c>
-      <c r="FK13" s="69"/>
-      <c r="FL13" s="68">
+      <c r="FK13" s="61"/>
+      <c r="FL13" s="60">
         <v>20</v>
       </c>
-      <c r="FM13" s="69"/>
-      <c r="FN13" s="68">
+      <c r="FM13" s="61"/>
+      <c r="FN13" s="60">
         <v>21</v>
       </c>
-      <c r="FO13" s="69"/>
-      <c r="FP13" s="68">
+      <c r="FO13" s="61"/>
+      <c r="FP13" s="60">
         <v>22</v>
       </c>
-      <c r="FQ13" s="69"/>
-      <c r="FR13" s="68">
+      <c r="FQ13" s="61"/>
+      <c r="FR13" s="60">
         <v>23</v>
       </c>
-      <c r="FS13" s="69"/>
-      <c r="FT13" s="68">
+      <c r="FS13" s="61"/>
+      <c r="FT13" s="60">
         <v>24</v>
       </c>
-      <c r="FU13" s="69"/>
-      <c r="FV13" s="68">
+      <c r="FU13" s="61"/>
+      <c r="FV13" s="60">
         <v>25</v>
       </c>
-      <c r="FW13" s="69"/>
-      <c r="FX13" s="68">
+      <c r="FW13" s="61"/>
+      <c r="FX13" s="60">
         <v>26</v>
       </c>
-      <c r="FY13" s="69"/>
-      <c r="FZ13" s="68">
+      <c r="FY13" s="61"/>
+      <c r="FZ13" s="60">
         <v>27</v>
       </c>
-      <c r="GA13" s="69"/>
-      <c r="GB13" s="68">
+      <c r="GA13" s="61"/>
+      <c r="GB13" s="60">
         <v>28</v>
       </c>
-      <c r="GC13" s="69"/>
-      <c r="GD13" s="68">
+      <c r="GC13" s="61"/>
+      <c r="GD13" s="60">
         <v>29</v>
       </c>
-      <c r="GE13" s="69"/>
-      <c r="GF13" s="68">
+      <c r="GE13" s="61"/>
+      <c r="GF13" s="60">
         <v>30</v>
       </c>
-      <c r="GG13" s="69"/>
-      <c r="GH13" s="68">
+      <c r="GG13" s="61"/>
+      <c r="GH13" s="60">
         <v>31</v>
       </c>
-      <c r="GI13" s="69"/>
+      <c r="GI13" s="61"/>
     </row>
     <row r="14" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="113" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="75"/>
+      <c r="B14" s="114"/>
       <c r="C14" s="37"/>
-      <c r="D14" s="91">
+      <c r="D14" s="97">
         <f>SUM(D15:E61)</f>
         <v>51.050000000000011</v>
       </c>
-      <c r="E14" s="93"/>
-      <c r="F14" s="91">
+      <c r="E14" s="99"/>
+      <c r="F14" s="97">
         <f>SUM(F15:G61)</f>
-        <v>36.448999999999998</v>
-      </c>
-      <c r="G14" s="92"/>
+        <v>36.948999999999998</v>
+      </c>
+      <c r="G14" s="98"/>
       <c r="H14" s="18"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -2830,22 +2832,22 @@
       <c r="GI14" s="14"/>
     </row>
     <row r="15" spans="1:191" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="82" t="s">
+      <c r="A15" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="83"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="62">
+      <c r="D15" s="65">
         <v>1.5</v>
       </c>
-      <c r="E15" s="63"/>
-      <c r="F15" s="62">
+      <c r="E15" s="66"/>
+      <c r="F15" s="65">
         <f>SUM(H15:GI15)</f>
         <v>0.5</v>
       </c>
-      <c r="G15" s="64"/>
+      <c r="G15" s="80"/>
       <c r="H15" s="47"/>
       <c r="I15" s="12"/>
       <c r="J15" s="24">
@@ -3034,22 +3036,22 @@
       <c r="GI15" s="34"/>
     </row>
     <row r="16" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="67"/>
+      <c r="B16" s="82"/>
       <c r="C16" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="62">
+      <c r="D16" s="65">
         <v>0.6</v>
       </c>
-      <c r="E16" s="63"/>
-      <c r="F16" s="62">
+      <c r="E16" s="66"/>
+      <c r="F16" s="65">
         <f>SUM(H16:GI16)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="64"/>
+      <c r="G16" s="80"/>
       <c r="H16" s="47"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
@@ -3236,22 +3238,22 @@
       <c r="GI16" s="32"/>
     </row>
     <row r="17" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="67"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="62">
+      <c r="D17" s="65">
         <v>1</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="62">
+      <c r="E17" s="66"/>
+      <c r="F17" s="65">
         <f>SUM(H17:GI17)</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="64"/>
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="80"/>
       <c r="H17" s="47"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
@@ -3294,7 +3296,9 @@
       <c r="AU17" s="52"/>
       <c r="AV17" s="51"/>
       <c r="AW17" s="51"/>
-      <c r="AX17" s="32"/>
+      <c r="AX17" s="24">
+        <v>0.5</v>
+      </c>
       <c r="AY17" s="32"/>
       <c r="AZ17" s="32"/>
       <c r="BA17" s="32"/>
@@ -3442,22 +3446,22 @@
       <c r="GI17" s="32"/>
     </row>
     <row r="18" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="67"/>
+      <c r="B18" s="82"/>
       <c r="C18" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="62">
+      <c r="D18" s="65">
         <v>0.8</v>
       </c>
-      <c r="E18" s="63"/>
-      <c r="F18" s="62">
+      <c r="E18" s="66"/>
+      <c r="F18" s="65">
         <f t="shared" ref="F18:F60" si="0">SUM(H18:GI18)</f>
         <v>0.75</v>
       </c>
-      <c r="G18" s="64"/>
+      <c r="G18" s="80"/>
       <c r="H18" s="26"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
@@ -3646,22 +3650,22 @@
       <c r="GI18" s="32"/>
     </row>
     <row r="19" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="67"/>
+      <c r="B19" s="82"/>
       <c r="C19" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="62">
+      <c r="D19" s="65">
         <v>0.5</v>
       </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="62">
+      <c r="E19" s="66"/>
+      <c r="F19" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="64"/>
+      <c r="G19" s="80"/>
       <c r="H19" s="26"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
@@ -3848,22 +3852,22 @@
       <c r="GI19" s="36"/>
     </row>
     <row r="20" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="67"/>
+      <c r="B20" s="82"/>
       <c r="C20" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="62">
+      <c r="D20" s="65">
         <v>0.3</v>
       </c>
-      <c r="E20" s="63"/>
-      <c r="F20" s="62">
+      <c r="E20" s="66"/>
+      <c r="F20" s="65">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="G20" s="64"/>
+      <c r="G20" s="80"/>
       <c r="H20" s="26"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -3894,10 +3898,10 @@
       <c r="AI20" s="51"/>
       <c r="AJ20" s="32"/>
       <c r="AK20" s="32"/>
-      <c r="AL20" s="58">
+      <c r="AL20" s="32"/>
+      <c r="AM20" s="24">
         <v>0.2</v>
       </c>
-      <c r="AM20" s="32"/>
       <c r="AN20" s="49"/>
       <c r="AO20" s="52"/>
       <c r="AP20" s="51"/>
@@ -4052,22 +4056,22 @@
       <c r="GI20" s="36"/>
     </row>
     <row r="21" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="67"/>
+      <c r="B21" s="82"/>
       <c r="C21" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="62">
+      <c r="D21" s="65">
         <v>1</v>
       </c>
-      <c r="E21" s="63"/>
-      <c r="F21" s="62">
+      <c r="E21" s="66"/>
+      <c r="F21" s="65">
         <f t="shared" si="0"/>
         <v>0.16600000000000001</v>
       </c>
-      <c r="G21" s="64"/>
+      <c r="G21" s="80"/>
       <c r="H21" s="26"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
@@ -4256,22 +4260,22 @@
       <c r="GI21" s="36"/>
     </row>
     <row r="22" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="67"/>
+      <c r="B22" s="82"/>
       <c r="C22" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="62">
+      <c r="D22" s="65">
         <v>0.6</v>
       </c>
-      <c r="E22" s="63"/>
-      <c r="F22" s="62">
+      <c r="E22" s="66"/>
+      <c r="F22" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="64"/>
+      <c r="G22" s="80"/>
       <c r="H22" s="26"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
@@ -4458,22 +4462,22 @@
       <c r="GI22" s="36"/>
     </row>
     <row r="23" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="67"/>
+      <c r="B23" s="82"/>
       <c r="C23" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="62">
+      <c r="D23" s="65">
         <v>0.6</v>
       </c>
-      <c r="E23" s="63"/>
-      <c r="F23" s="62">
+      <c r="E23" s="66"/>
+      <c r="F23" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="64"/>
+      <c r="G23" s="80"/>
       <c r="H23" s="26"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
@@ -4660,22 +4664,22 @@
       <c r="GI23" s="36"/>
     </row>
     <row r="24" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="67"/>
+      <c r="B24" s="82"/>
       <c r="C24" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="62">
+      <c r="D24" s="65">
         <v>3</v>
       </c>
-      <c r="E24" s="63"/>
-      <c r="F24" s="62">
+      <c r="E24" s="66"/>
+      <c r="F24" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="64"/>
+      <c r="G24" s="80"/>
       <c r="H24" s="26"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
@@ -4862,22 +4866,22 @@
       <c r="GI24" s="36"/>
     </row>
     <row r="25" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="67"/>
+      <c r="B25" s="82"/>
       <c r="C25" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="62">
+      <c r="D25" s="65">
         <v>1.5</v>
       </c>
-      <c r="E25" s="63"/>
-      <c r="F25" s="62">
+      <c r="E25" s="66"/>
+      <c r="F25" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="64"/>
+      <c r="G25" s="80"/>
       <c r="H25" s="26"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
@@ -5064,22 +5068,22 @@
       <c r="GI25" s="36"/>
     </row>
     <row r="26" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A26" s="66" t="s">
+      <c r="A26" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="67"/>
+      <c r="B26" s="82"/>
       <c r="C26" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="62">
+      <c r="D26" s="65">
         <v>1</v>
       </c>
-      <c r="E26" s="63"/>
-      <c r="F26" s="62">
+      <c r="E26" s="66"/>
+      <c r="F26" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="64"/>
+      <c r="G26" s="80"/>
       <c r="H26" s="26"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
@@ -5266,22 +5270,22 @@
       <c r="GI26" s="36"/>
     </row>
     <row r="27" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="67"/>
+      <c r="B27" s="82"/>
       <c r="C27" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="62">
+      <c r="D27" s="65">
         <v>1</v>
       </c>
-      <c r="E27" s="63"/>
-      <c r="F27" s="62">
+      <c r="E27" s="66"/>
+      <c r="F27" s="65">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G27" s="64"/>
+      <c r="G27" s="80"/>
       <c r="H27" s="26"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
@@ -5472,22 +5476,22 @@
       <c r="GI27" s="36"/>
     </row>
     <row r="28" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A28" s="66" t="s">
+      <c r="A28" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="67"/>
+      <c r="B28" s="82"/>
       <c r="C28" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="62">
+      <c r="D28" s="65">
         <v>1</v>
       </c>
-      <c r="E28" s="63"/>
-      <c r="F28" s="62">
+      <c r="E28" s="66"/>
+      <c r="F28" s="65">
         <f t="shared" si="0"/>
         <v>0.33300000000000002</v>
       </c>
-      <c r="G28" s="64"/>
+      <c r="G28" s="80"/>
       <c r="H28" s="26"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
@@ -5676,22 +5680,22 @@
       <c r="GI28" s="36"/>
     </row>
     <row r="29" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="67"/>
+      <c r="B29" s="82"/>
       <c r="C29" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="62">
+      <c r="D29" s="65">
         <v>1</v>
       </c>
-      <c r="E29" s="63"/>
-      <c r="F29" s="62">
+      <c r="E29" s="66"/>
+      <c r="F29" s="65">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G29" s="64"/>
+      <c r="G29" s="80"/>
       <c r="H29" s="26"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
@@ -5880,22 +5884,22 @@
       <c r="GI29" s="36"/>
     </row>
     <row r="30" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A30" s="66" t="s">
+      <c r="A30" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="67"/>
+      <c r="B30" s="82"/>
       <c r="C30" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="62">
+      <c r="D30" s="65">
         <v>1</v>
       </c>
-      <c r="E30" s="63"/>
-      <c r="F30" s="62">
+      <c r="E30" s="66"/>
+      <c r="F30" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G30" s="64"/>
+      <c r="G30" s="80"/>
       <c r="H30" s="26"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
@@ -6084,22 +6088,22 @@
       <c r="GI30" s="36"/>
     </row>
     <row r="31" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A31" s="66" t="s">
+      <c r="A31" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="67"/>
+      <c r="B31" s="82"/>
       <c r="C31" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="62">
+      <c r="D31" s="65">
         <v>4</v>
       </c>
-      <c r="E31" s="63"/>
-      <c r="F31" s="62">
+      <c r="E31" s="66"/>
+      <c r="F31" s="65">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G31" s="64"/>
+      <c r="G31" s="80"/>
       <c r="H31" s="26"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
@@ -6290,22 +6294,22 @@
       <c r="GI31" s="36"/>
     </row>
     <row r="32" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A32" s="66" t="s">
+      <c r="A32" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="67"/>
+      <c r="B32" s="82"/>
       <c r="C32" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="62">
+      <c r="D32" s="65">
         <v>0.6</v>
       </c>
-      <c r="E32" s="63"/>
-      <c r="F32" s="62">
+      <c r="E32" s="66"/>
+      <c r="F32" s="65">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G32" s="64"/>
+      <c r="G32" s="80"/>
       <c r="H32" s="26"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
@@ -6494,22 +6498,22 @@
       <c r="GI32" s="36"/>
     </row>
     <row r="33" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="67"/>
+      <c r="B33" s="82"/>
       <c r="C33" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="62">
+      <c r="D33" s="65">
         <v>0.5</v>
       </c>
-      <c r="E33" s="63"/>
-      <c r="F33" s="62">
+      <c r="E33" s="66"/>
+      <c r="F33" s="65">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G33" s="64"/>
+      <c r="G33" s="80"/>
       <c r="H33" s="26"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
@@ -6698,22 +6702,22 @@
       <c r="GI33" s="36"/>
     </row>
     <row r="34" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A34" s="66" t="s">
+      <c r="A34" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="67"/>
+      <c r="B34" s="82"/>
       <c r="C34" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="62">
+      <c r="D34" s="65">
         <v>0.3</v>
       </c>
-      <c r="E34" s="63"/>
-      <c r="F34" s="62">
+      <c r="E34" s="66"/>
+      <c r="F34" s="65">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G34" s="64"/>
+      <c r="G34" s="80"/>
       <c r="H34" s="26"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
@@ -6902,22 +6906,22 @@
       <c r="GI34" s="36"/>
     </row>
     <row r="35" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A35" s="66" t="s">
+      <c r="A35" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="67"/>
+      <c r="B35" s="82"/>
       <c r="C35" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="62">
+      <c r="D35" s="65">
         <v>0.3</v>
       </c>
-      <c r="E35" s="63"/>
-      <c r="F35" s="62">
+      <c r="E35" s="66"/>
+      <c r="F35" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G35" s="64"/>
+      <c r="G35" s="80"/>
       <c r="H35" s="26"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
@@ -7104,22 +7108,22 @@
       <c r="GI35" s="36"/>
     </row>
     <row r="36" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A36" s="66" t="s">
+      <c r="A36" s="81" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="67"/>
+      <c r="B36" s="82"/>
       <c r="C36" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="62">
+      <c r="D36" s="65">
         <v>1.5</v>
       </c>
-      <c r="E36" s="63"/>
-      <c r="F36" s="62">
+      <c r="E36" s="66"/>
+      <c r="F36" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G36" s="64"/>
+      <c r="G36" s="80"/>
       <c r="H36" s="26"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
@@ -7306,22 +7310,22 @@
       <c r="GI36" s="36"/>
     </row>
     <row r="37" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A37" s="66" t="s">
+      <c r="A37" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="67"/>
+      <c r="B37" s="82"/>
       <c r="C37" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="62">
+      <c r="D37" s="65">
         <v>0.5</v>
       </c>
-      <c r="E37" s="63"/>
-      <c r="F37" s="62">
+      <c r="E37" s="66"/>
+      <c r="F37" s="65">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G37" s="64"/>
+      <c r="G37" s="80"/>
       <c r="H37" s="26"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
@@ -7510,22 +7514,22 @@
       <c r="GI37" s="36"/>
     </row>
     <row r="38" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A38" s="66" t="s">
+      <c r="A38" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="67"/>
+      <c r="B38" s="82"/>
       <c r="C38" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="62">
+      <c r="D38" s="65">
         <v>0.25</v>
       </c>
-      <c r="E38" s="63"/>
-      <c r="F38" s="62">
+      <c r="E38" s="66"/>
+      <c r="F38" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G38" s="64"/>
+      <c r="G38" s="80"/>
       <c r="H38" s="26"/>
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
@@ -7714,22 +7718,22 @@
       <c r="GI38" s="36"/>
     </row>
     <row r="39" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="67"/>
+      <c r="B39" s="82"/>
       <c r="C39" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="62">
+      <c r="D39" s="65">
         <v>0.5</v>
       </c>
-      <c r="E39" s="63"/>
-      <c r="F39" s="62">
+      <c r="E39" s="66"/>
+      <c r="F39" s="65">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="G39" s="64"/>
+      <c r="G39" s="80"/>
       <c r="H39" s="26"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
@@ -7918,22 +7922,22 @@
       <c r="GI39" s="36"/>
     </row>
     <row r="40" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A40" s="66" t="s">
+      <c r="A40" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="67"/>
+      <c r="B40" s="82"/>
       <c r="C40" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="62">
+      <c r="D40" s="65">
         <v>0.5</v>
       </c>
-      <c r="E40" s="63"/>
-      <c r="F40" s="62">
+      <c r="E40" s="66"/>
+      <c r="F40" s="65">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G40" s="64"/>
+      <c r="G40" s="80"/>
       <c r="H40" s="26"/>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
@@ -8122,22 +8126,22 @@
       <c r="GI40" s="36"/>
     </row>
     <row r="41" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="67"/>
+      <c r="B41" s="82"/>
       <c r="C41" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="62">
+      <c r="D41" s="65">
         <v>0.3</v>
       </c>
-      <c r="E41" s="63"/>
-      <c r="F41" s="62">
+      <c r="E41" s="66"/>
+      <c r="F41" s="65">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G41" s="64"/>
+      <c r="G41" s="80"/>
       <c r="H41" s="26"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
@@ -8326,22 +8330,22 @@
       <c r="GI41" s="36"/>
     </row>
     <row r="42" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A42" s="66" t="s">
+      <c r="A42" s="81" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="67"/>
+      <c r="B42" s="82"/>
       <c r="C42" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="62">
+      <c r="D42" s="65">
         <v>0.5</v>
       </c>
-      <c r="E42" s="63"/>
-      <c r="F42" s="62">
+      <c r="E42" s="66"/>
+      <c r="F42" s="65">
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-      <c r="G42" s="64"/>
+      <c r="G42" s="80"/>
       <c r="H42" s="26"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
@@ -8530,22 +8534,22 @@
       <c r="GI42" s="36"/>
     </row>
     <row r="43" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A43" s="66" t="s">
+      <c r="A43" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="67"/>
+      <c r="B43" s="82"/>
       <c r="C43" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D43" s="62">
+      <c r="D43" s="65">
         <v>1.3</v>
       </c>
-      <c r="E43" s="63"/>
-      <c r="F43" s="62">
+      <c r="E43" s="66"/>
+      <c r="F43" s="65">
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
-      <c r="G43" s="64"/>
+      <c r="G43" s="80"/>
       <c r="H43" s="26"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
@@ -8736,22 +8740,22 @@
       <c r="GI43" s="36"/>
     </row>
     <row r="44" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="66" t="s">
+      <c r="A44" s="81" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="67"/>
+      <c r="B44" s="82"/>
       <c r="C44" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="62">
+      <c r="D44" s="65">
         <v>1.3</v>
       </c>
-      <c r="E44" s="63"/>
-      <c r="F44" s="62">
+      <c r="E44" s="66"/>
+      <c r="F44" s="65">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G44" s="64"/>
+      <c r="G44" s="80"/>
       <c r="H44" s="26"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
@@ -8940,22 +8944,22 @@
       <c r="GI44" s="36"/>
     </row>
     <row r="45" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A45" s="66" t="s">
+      <c r="A45" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="67"/>
+      <c r="B45" s="82"/>
       <c r="C45" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="62">
+      <c r="D45" s="65">
         <v>1</v>
       </c>
-      <c r="E45" s="63"/>
-      <c r="F45" s="62">
+      <c r="E45" s="66"/>
+      <c r="F45" s="65">
         <f t="shared" si="0"/>
         <v>1.05</v>
       </c>
-      <c r="G45" s="64"/>
+      <c r="G45" s="80"/>
       <c r="H45" s="26"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
@@ -9146,22 +9150,22 @@
       <c r="GI45" s="36"/>
     </row>
     <row r="46" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A46" s="66" t="s">
+      <c r="A46" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="67"/>
+      <c r="B46" s="82"/>
       <c r="C46" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="D46" s="62">
+      <c r="D46" s="65">
         <v>1</v>
       </c>
-      <c r="E46" s="63"/>
-      <c r="F46" s="62">
+      <c r="E46" s="66"/>
+      <c r="F46" s="65">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="G46" s="64"/>
+      <c r="G46" s="80"/>
       <c r="H46" s="26"/>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
@@ -9350,22 +9354,22 @@
       <c r="GI46" s="36"/>
     </row>
     <row r="47" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A47" s="66" t="s">
+      <c r="A47" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="67"/>
+      <c r="B47" s="82"/>
       <c r="C47" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="D47" s="62">
+      <c r="D47" s="65">
         <v>1</v>
       </c>
-      <c r="E47" s="63"/>
-      <c r="F47" s="62">
+      <c r="E47" s="66"/>
+      <c r="F47" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G47" s="64"/>
+      <c r="G47" s="80"/>
       <c r="H47" s="26"/>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
@@ -9552,22 +9556,22 @@
       <c r="GI47" s="36"/>
     </row>
     <row r="48" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A48" s="66" t="s">
+      <c r="A48" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="B48" s="67"/>
+      <c r="B48" s="82"/>
       <c r="C48" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D48" s="62">
+      <c r="D48" s="65">
         <v>0.3</v>
       </c>
-      <c r="E48" s="63"/>
-      <c r="F48" s="62">
+      <c r="E48" s="66"/>
+      <c r="F48" s="65">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G48" s="64"/>
+      <c r="G48" s="80"/>
       <c r="H48" s="26"/>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
@@ -9756,22 +9760,22 @@
       <c r="GI48" s="36"/>
     </row>
     <row r="49" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A49" s="66" t="s">
+      <c r="A49" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="67"/>
+      <c r="B49" s="82"/>
       <c r="C49" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="62">
+      <c r="D49" s="65">
         <v>2</v>
       </c>
-      <c r="E49" s="63"/>
-      <c r="F49" s="62">
+      <c r="E49" s="66"/>
+      <c r="F49" s="65">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G49" s="64"/>
+      <c r="G49" s="80"/>
       <c r="H49" s="26"/>
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
@@ -9962,22 +9966,22 @@
       <c r="GI49" s="36"/>
     </row>
     <row r="50" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A50" s="66" t="s">
+      <c r="A50" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="67"/>
+      <c r="B50" s="82"/>
       <c r="C50" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="D50" s="62">
+      <c r="D50" s="65">
         <v>2</v>
       </c>
-      <c r="E50" s="63"/>
-      <c r="F50" s="62">
+      <c r="E50" s="66"/>
+      <c r="F50" s="65">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G50" s="64"/>
+      <c r="G50" s="80"/>
       <c r="H50" s="26"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
@@ -10168,22 +10172,22 @@
       <c r="GI50" s="36"/>
     </row>
     <row r="51" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A51" s="66" t="s">
+      <c r="A51" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="67"/>
+      <c r="B51" s="82"/>
       <c r="C51" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D51" s="62">
+      <c r="D51" s="65">
         <v>2</v>
       </c>
-      <c r="E51" s="63"/>
-      <c r="F51" s="62">
+      <c r="E51" s="66"/>
+      <c r="F51" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G51" s="64"/>
+      <c r="G51" s="80"/>
       <c r="H51" s="26"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
@@ -10370,22 +10374,22 @@
       <c r="GI51" s="36"/>
     </row>
     <row r="52" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A52" s="66" t="s">
+      <c r="A52" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="67"/>
+      <c r="B52" s="82"/>
       <c r="C52" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="62">
+      <c r="D52" s="65">
         <v>2</v>
       </c>
-      <c r="E52" s="63"/>
-      <c r="F52" s="62">
+      <c r="E52" s="66"/>
+      <c r="F52" s="65">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G52" s="64"/>
+      <c r="G52" s="80"/>
       <c r="H52" s="26"/>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
@@ -10576,22 +10580,22 @@
       <c r="GI52" s="36"/>
     </row>
     <row r="53" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A53" s="66" t="s">
+      <c r="A53" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="67"/>
+      <c r="B53" s="82"/>
       <c r="C53" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D53" s="62">
+      <c r="D53" s="65">
         <v>2</v>
       </c>
-      <c r="E53" s="63"/>
-      <c r="F53" s="62">
+      <c r="E53" s="66"/>
+      <c r="F53" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G53" s="64"/>
+      <c r="G53" s="80"/>
       <c r="H53" s="26"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
@@ -10778,22 +10782,22 @@
       <c r="GI53" s="36"/>
     </row>
     <row r="54" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A54" s="66" t="s">
+      <c r="A54" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="67"/>
+      <c r="B54" s="82"/>
       <c r="C54" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="D54" s="62">
+      <c r="D54" s="65">
         <v>0.25</v>
       </c>
-      <c r="E54" s="63"/>
-      <c r="F54" s="62">
+      <c r="E54" s="66"/>
+      <c r="F54" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G54" s="64"/>
+      <c r="G54" s="80"/>
       <c r="H54" s="26"/>
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
@@ -10980,22 +10984,22 @@
       <c r="GI54" s="36"/>
     </row>
     <row r="55" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A55" s="66" t="s">
+      <c r="A55" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="67"/>
+      <c r="B55" s="82"/>
       <c r="C55" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="D55" s="62">
+      <c r="D55" s="65">
         <v>1</v>
       </c>
-      <c r="E55" s="63"/>
-      <c r="F55" s="62">
+      <c r="E55" s="66"/>
+      <c r="F55" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G55" s="64"/>
+      <c r="G55" s="80"/>
       <c r="H55" s="26"/>
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
@@ -11182,22 +11186,22 @@
       <c r="GI55" s="36"/>
     </row>
     <row r="56" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A56" s="66" t="s">
+      <c r="A56" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="67"/>
+      <c r="B56" s="82"/>
       <c r="C56" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="D56" s="62">
+      <c r="D56" s="65">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E56" s="63"/>
-      <c r="F56" s="62">
+      <c r="E56" s="66"/>
+      <c r="F56" s="65">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G56" s="64"/>
+      <c r="G56" s="80"/>
       <c r="H56" s="26"/>
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
@@ -11388,22 +11392,22 @@
       <c r="GI56" s="36"/>
     </row>
     <row r="57" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A57" s="66" t="s">
+      <c r="A57" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="67"/>
+      <c r="B57" s="82"/>
       <c r="C57" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="D57" s="62">
+      <c r="D57" s="65">
         <v>1.75</v>
       </c>
-      <c r="E57" s="63"/>
-      <c r="F57" s="62">
+      <c r="E57" s="66"/>
+      <c r="F57" s="65">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G57" s="64"/>
+      <c r="G57" s="80"/>
       <c r="H57" s="26"/>
       <c r="I57" s="12"/>
       <c r="J57" s="12"/>
@@ -11592,22 +11596,22 @@
       <c r="GI57" s="36"/>
     </row>
     <row r="58" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A58" s="66" t="s">
+      <c r="A58" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="B58" s="67"/>
+      <c r="B58" s="82"/>
       <c r="C58" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="D58" s="62">
+      <c r="D58" s="65">
         <v>0.6</v>
       </c>
-      <c r="E58" s="63"/>
-      <c r="F58" s="62">
+      <c r="E58" s="66"/>
+      <c r="F58" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G58" s="64"/>
+      <c r="G58" s="80"/>
       <c r="H58" s="26"/>
       <c r="I58" s="12"/>
       <c r="J58" s="12"/>
@@ -11794,22 +11798,22 @@
       <c r="GI58" s="36"/>
     </row>
     <row r="59" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="66" t="s">
+      <c r="A59" s="81" t="s">
         <v>111</v>
       </c>
-      <c r="B59" s="67"/>
+      <c r="B59" s="82"/>
       <c r="C59" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="62">
+      <c r="D59" s="65">
         <v>1</v>
       </c>
-      <c r="E59" s="63"/>
-      <c r="F59" s="62">
+      <c r="E59" s="66"/>
+      <c r="F59" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G59" s="64"/>
+      <c r="G59" s="80"/>
       <c r="H59" s="26"/>
       <c r="I59" s="12"/>
       <c r="J59" s="12"/>
@@ -11996,22 +12000,22 @@
       <c r="GI59" s="36"/>
     </row>
     <row r="60" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A60" s="66" t="s">
+      <c r="A60" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="B60" s="67"/>
+      <c r="B60" s="82"/>
       <c r="C60" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="D60" s="62">
+      <c r="D60" s="65">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E60" s="63"/>
-      <c r="F60" s="62">
+      <c r="E60" s="66"/>
+      <c r="F60" s="65">
         <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
-      <c r="G60" s="64"/>
+      <c r="G60" s="80"/>
       <c r="H60" s="26"/>
       <c r="I60" s="12"/>
       <c r="J60" s="12"/>
@@ -12200,22 +12204,22 @@
       <c r="GI60" s="36"/>
     </row>
     <row r="61" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A61" s="66" t="s">
+      <c r="A61" s="81" t="s">
         <v>115</v>
       </c>
-      <c r="B61" s="67"/>
+      <c r="B61" s="82"/>
       <c r="C61" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="D61" s="62">
+      <c r="D61" s="65">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E61" s="63"/>
-      <c r="F61" s="62">
+      <c r="E61" s="66"/>
+      <c r="F61" s="65">
         <f>SUM(H61:GI61)</f>
         <v>1</v>
       </c>
-      <c r="G61" s="64"/>
+      <c r="G61" s="80"/>
       <c r="H61" s="26"/>
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
@@ -12404,21 +12408,21 @@
       <c r="GI61" s="36"/>
     </row>
     <row r="62" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A62" s="76" t="s">
+      <c r="A62" s="115" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="77"/>
+      <c r="B62" s="116"/>
       <c r="C62" s="39"/>
-      <c r="D62" s="78">
+      <c r="D62" s="71">
         <f>SUM(D63:E80)</f>
         <v>88.6</v>
       </c>
-      <c r="E62" s="79"/>
-      <c r="F62" s="78">
+      <c r="E62" s="117"/>
+      <c r="F62" s="71">
         <f>SUM(F63:G80)</f>
         <v>0</v>
       </c>
-      <c r="G62" s="80"/>
+      <c r="G62" s="75"/>
       <c r="H62" s="29"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
@@ -12605,22 +12609,22 @@
       <c r="GI62" s="29"/>
     </row>
     <row r="63" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="60" t="s">
+      <c r="A63" s="118" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="61"/>
+      <c r="B63" s="119"/>
       <c r="C63" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D63" s="62">
+      <c r="D63" s="65">
         <v>0.6</v>
       </c>
-      <c r="E63" s="63"/>
-      <c r="F63" s="62">
+      <c r="E63" s="66"/>
+      <c r="F63" s="65">
         <f>SUM(H63:GI63)</f>
         <v>0</v>
       </c>
-      <c r="G63" s="64"/>
+      <c r="G63" s="80"/>
       <c r="H63" s="47"/>
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
@@ -12807,22 +12811,22 @@
       <c r="GI63" s="32"/>
     </row>
     <row r="64" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="60" t="s">
+      <c r="A64" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="B64" s="61"/>
+      <c r="B64" s="119"/>
       <c r="C64" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D64" s="62">
+      <c r="D64" s="65">
         <v>1.5</v>
       </c>
-      <c r="E64" s="63"/>
-      <c r="F64" s="62">
+      <c r="E64" s="66"/>
+      <c r="F64" s="65">
         <f>SUM(H64:GI64)</f>
         <v>0</v>
       </c>
-      <c r="G64" s="64"/>
+      <c r="G64" s="80"/>
       <c r="H64" s="47"/>
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
@@ -13009,22 +13013,22 @@
       <c r="GI64" s="32"/>
     </row>
     <row r="65" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A65" s="60" t="s">
+      <c r="A65" s="118" t="s">
         <v>123</v>
       </c>
-      <c r="B65" s="61"/>
+      <c r="B65" s="119"/>
       <c r="C65" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D65" s="62">
+      <c r="D65" s="65">
         <v>1</v>
       </c>
-      <c r="E65" s="63"/>
-      <c r="F65" s="62">
+      <c r="E65" s="66"/>
+      <c r="F65" s="65">
         <f t="shared" ref="F65:F80" si="1">SUM(H65:GI65)</f>
         <v>0</v>
       </c>
-      <c r="G65" s="64"/>
+      <c r="G65" s="80"/>
       <c r="H65" s="47"/>
       <c r="I65" s="12"/>
       <c r="J65" s="12"/>
@@ -13211,22 +13215,22 @@
       <c r="GI65" s="32"/>
     </row>
     <row r="66" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A66" s="60" t="s">
+      <c r="A66" s="118" t="s">
         <v>125</v>
       </c>
-      <c r="B66" s="61"/>
+      <c r="B66" s="119"/>
       <c r="C66" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D66" s="62">
+      <c r="D66" s="65">
         <v>0.5</v>
       </c>
-      <c r="E66" s="63"/>
-      <c r="F66" s="62">
+      <c r="E66" s="66"/>
+      <c r="F66" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G66" s="64"/>
+      <c r="G66" s="80"/>
       <c r="H66" s="47"/>
       <c r="I66" s="12"/>
       <c r="J66" s="12"/>
@@ -13413,22 +13417,22 @@
       <c r="GI66" s="32"/>
     </row>
     <row r="67" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A67" s="60" t="s">
+      <c r="A67" s="118" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="61"/>
+      <c r="B67" s="119"/>
       <c r="C67" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D67" s="62">
+      <c r="D67" s="65">
         <v>1</v>
       </c>
-      <c r="E67" s="63"/>
-      <c r="F67" s="62">
+      <c r="E67" s="66"/>
+      <c r="F67" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G67" s="64"/>
+      <c r="G67" s="80"/>
       <c r="H67" s="47"/>
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
@@ -13615,22 +13619,22 @@
       <c r="GI67" s="32"/>
     </row>
     <row r="68" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A68" s="60" t="s">
+      <c r="A68" s="118" t="s">
         <v>129</v>
       </c>
-      <c r="B68" s="61"/>
+      <c r="B68" s="119"/>
       <c r="C68" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D68" s="62">
+      <c r="D68" s="65">
         <v>1</v>
       </c>
-      <c r="E68" s="63"/>
-      <c r="F68" s="62">
+      <c r="E68" s="66"/>
+      <c r="F68" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G68" s="64"/>
+      <c r="G68" s="80"/>
       <c r="H68" s="47"/>
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
@@ -13817,22 +13821,22 @@
       <c r="GI68" s="32"/>
     </row>
     <row r="69" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A69" s="60" t="s">
+      <c r="A69" s="118" t="s">
         <v>131</v>
       </c>
-      <c r="B69" s="61"/>
+      <c r="B69" s="119"/>
       <c r="C69" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="D69" s="62">
+      <c r="D69" s="65">
         <v>4</v>
       </c>
-      <c r="E69" s="63"/>
-      <c r="F69" s="62">
+      <c r="E69" s="66"/>
+      <c r="F69" s="65">
         <f>SUM(H69:GI69)</f>
         <v>0</v>
       </c>
-      <c r="G69" s="64"/>
+      <c r="G69" s="80"/>
       <c r="H69" s="47"/>
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
@@ -14019,22 +14023,22 @@
       <c r="GI69" s="32"/>
     </row>
     <row r="70" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A70" s="60" t="s">
+      <c r="A70" s="118" t="s">
         <v>133</v>
       </c>
-      <c r="B70" s="61"/>
+      <c r="B70" s="119"/>
       <c r="C70" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="D70" s="62">
+      <c r="D70" s="65">
         <v>8</v>
       </c>
-      <c r="E70" s="63"/>
-      <c r="F70" s="62">
+      <c r="E70" s="66"/>
+      <c r="F70" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G70" s="64"/>
+      <c r="G70" s="80"/>
       <c r="H70" s="47"/>
       <c r="I70" s="12"/>
       <c r="J70" s="12"/>
@@ -14221,22 +14225,22 @@
       <c r="GI70" s="32"/>
     </row>
     <row r="71" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A71" s="60" t="s">
+      <c r="A71" s="118" t="s">
         <v>135</v>
       </c>
-      <c r="B71" s="61"/>
+      <c r="B71" s="119"/>
       <c r="C71" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="D71" s="62">
+      <c r="D71" s="65">
         <v>1</v>
       </c>
-      <c r="E71" s="63"/>
-      <c r="F71" s="62">
+      <c r="E71" s="66"/>
+      <c r="F71" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G71" s="64"/>
+      <c r="G71" s="80"/>
       <c r="H71" s="47"/>
       <c r="I71" s="12"/>
       <c r="J71" s="12"/>
@@ -14423,22 +14427,22 @@
       <c r="GI71" s="32"/>
     </row>
     <row r="72" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A72" s="60" t="s">
+      <c r="A72" s="118" t="s">
         <v>137</v>
       </c>
-      <c r="B72" s="61"/>
+      <c r="B72" s="119"/>
       <c r="C72" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="D72" s="62">
+      <c r="D72" s="65">
         <v>1</v>
       </c>
-      <c r="E72" s="63"/>
-      <c r="F72" s="62">
+      <c r="E72" s="66"/>
+      <c r="F72" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G72" s="64"/>
+      <c r="G72" s="80"/>
       <c r="H72" s="47"/>
       <c r="I72" s="12"/>
       <c r="J72" s="12"/>
@@ -14625,22 +14629,22 @@
       <c r="GI72" s="32"/>
     </row>
     <row r="73" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A73" s="60" t="s">
+      <c r="A73" s="118" t="s">
         <v>47</v>
       </c>
-      <c r="B73" s="61"/>
+      <c r="B73" s="119"/>
       <c r="C73" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="D73" s="62">
+      <c r="D73" s="65">
         <v>4</v>
       </c>
-      <c r="E73" s="63"/>
-      <c r="F73" s="62">
+      <c r="E73" s="66"/>
+      <c r="F73" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G73" s="64"/>
+      <c r="G73" s="80"/>
       <c r="H73" s="47"/>
       <c r="I73" s="12"/>
       <c r="J73" s="12"/>
@@ -14827,22 +14831,22 @@
       <c r="GI73" s="32"/>
     </row>
     <row r="74" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A74" s="60" t="s">
+      <c r="A74" s="118" t="s">
         <v>140</v>
       </c>
-      <c r="B74" s="61"/>
+      <c r="B74" s="119"/>
       <c r="C74" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="D74" s="62">
+      <c r="D74" s="65">
         <v>12</v>
       </c>
-      <c r="E74" s="63"/>
-      <c r="F74" s="62">
+      <c r="E74" s="66"/>
+      <c r="F74" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G74" s="64"/>
+      <c r="G74" s="80"/>
       <c r="H74" s="47"/>
       <c r="I74" s="12"/>
       <c r="J74" s="12"/>
@@ -15029,22 +15033,22 @@
       <c r="GI74" s="32"/>
     </row>
     <row r="75" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A75" s="60" t="s">
+      <c r="A75" s="118" t="s">
         <v>142</v>
       </c>
-      <c r="B75" s="65"/>
+      <c r="B75" s="88"/>
       <c r="C75" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D75" s="62">
+      <c r="D75" s="65">
         <v>16</v>
       </c>
-      <c r="E75" s="63"/>
-      <c r="F75" s="62">
+      <c r="E75" s="66"/>
+      <c r="F75" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G75" s="64"/>
+      <c r="G75" s="80"/>
       <c r="H75" s="47"/>
       <c r="I75" s="12"/>
       <c r="J75" s="12"/>
@@ -15231,22 +15235,22 @@
       <c r="GI75" s="36"/>
     </row>
     <row r="76" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A76" s="60" t="s">
+      <c r="A76" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B76" s="61"/>
+      <c r="B76" s="119"/>
       <c r="C76" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="D76" s="62">
+      <c r="D76" s="65">
         <v>5</v>
       </c>
-      <c r="E76" s="63"/>
-      <c r="F76" s="62">
+      <c r="E76" s="66"/>
+      <c r="F76" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G76" s="64"/>
+      <c r="G76" s="80"/>
       <c r="H76" s="47"/>
       <c r="I76" s="12"/>
       <c r="J76" s="12"/>
@@ -15433,22 +15437,22 @@
       <c r="GI76" s="32"/>
     </row>
     <row r="77" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A77" s="60" t="s">
+      <c r="A77" s="118" t="s">
         <v>146</v>
       </c>
-      <c r="B77" s="61"/>
+      <c r="B77" s="119"/>
       <c r="C77" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="D77" s="62">
+      <c r="D77" s="65">
         <v>4</v>
       </c>
-      <c r="E77" s="63"/>
-      <c r="F77" s="62">
+      <c r="E77" s="66"/>
+      <c r="F77" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G77" s="64"/>
+      <c r="G77" s="80"/>
       <c r="H77" s="47"/>
       <c r="I77" s="12"/>
       <c r="J77" s="12"/>
@@ -15635,22 +15639,22 @@
       <c r="GI77" s="32"/>
     </row>
     <row r="78" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A78" s="60" t="s">
+      <c r="A78" s="118" t="s">
         <v>148</v>
       </c>
-      <c r="B78" s="61"/>
+      <c r="B78" s="119"/>
       <c r="C78" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="D78" s="62">
+      <c r="D78" s="65">
         <v>16</v>
       </c>
-      <c r="E78" s="63"/>
-      <c r="F78" s="62">
+      <c r="E78" s="66"/>
+      <c r="F78" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G78" s="64"/>
+      <c r="G78" s="80"/>
       <c r="H78" s="47"/>
       <c r="I78" s="12"/>
       <c r="J78" s="12"/>
@@ -15837,22 +15841,22 @@
       <c r="GI78" s="32"/>
     </row>
     <row r="79" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A79" s="82" t="s">
+      <c r="A79" s="73" t="s">
         <v>150</v>
       </c>
-      <c r="B79" s="83"/>
+      <c r="B79" s="74"/>
       <c r="C79" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="D79" s="62">
+      <c r="D79" s="65">
         <v>6</v>
       </c>
-      <c r="E79" s="63"/>
-      <c r="F79" s="62">
+      <c r="E79" s="66"/>
+      <c r="F79" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G79" s="64"/>
+      <c r="G79" s="80"/>
       <c r="H79" s="47"/>
       <c r="I79" s="12"/>
       <c r="J79" s="12"/>
@@ -16039,22 +16043,22 @@
       <c r="GI79" s="36"/>
     </row>
     <row r="80" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A80" s="82" t="s">
+      <c r="A80" s="73" t="s">
         <v>152</v>
       </c>
-      <c r="B80" s="83"/>
+      <c r="B80" s="74"/>
       <c r="C80" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D80" s="62">
+      <c r="D80" s="65">
         <v>6</v>
       </c>
-      <c r="E80" s="63"/>
-      <c r="F80" s="62">
+      <c r="E80" s="66"/>
+      <c r="F80" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G80" s="64"/>
+      <c r="G80" s="80"/>
       <c r="H80" s="47"/>
       <c r="I80" s="12"/>
       <c r="J80" s="12"/>
@@ -16241,21 +16245,21 @@
       <c r="GI80" s="36"/>
     </row>
     <row r="81" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A81" s="76" t="s">
+      <c r="A81" s="115" t="s">
         <v>153</v>
       </c>
-      <c r="B81" s="77"/>
+      <c r="B81" s="116"/>
       <c r="C81" s="39"/>
-      <c r="D81" s="78">
+      <c r="D81" s="71">
         <f>SUM(D82:E82)</f>
         <v>16</v>
       </c>
-      <c r="E81" s="88"/>
-      <c r="F81" s="78">
+      <c r="E81" s="72"/>
+      <c r="F81" s="71">
         <f>SUM(F82:G82)</f>
         <v>0</v>
       </c>
-      <c r="G81" s="80"/>
+      <c r="G81" s="75"/>
       <c r="H81" s="29"/>
       <c r="I81" s="8"/>
       <c r="J81" s="8"/>
@@ -16442,20 +16446,20 @@
       <c r="GI81" s="29"/>
     </row>
     <row r="82" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A82" s="86" t="s">
+      <c r="A82" s="93" t="s">
         <v>153</v>
       </c>
-      <c r="B82" s="87"/>
+      <c r="B82" s="94"/>
       <c r="C82" s="40"/>
-      <c r="D82" s="84">
+      <c r="D82" s="91">
         <v>16</v>
       </c>
-      <c r="E82" s="85"/>
-      <c r="F82" s="62">
+      <c r="E82" s="92"/>
+      <c r="F82" s="65">
         <f>SUM(H82:GI82)</f>
         <v>0</v>
       </c>
-      <c r="G82" s="64"/>
+      <c r="G82" s="80"/>
       <c r="H82" s="26"/>
       <c r="I82" s="12"/>
       <c r="J82" s="12"/>
@@ -16642,21 +16646,21 @@
       <c r="GI82" s="32"/>
     </row>
     <row r="83" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A83" s="104" t="s">
+      <c r="A83" s="110" t="s">
         <v>154</v>
       </c>
-      <c r="B83" s="105"/>
+      <c r="B83" s="111"/>
       <c r="C83" s="41"/>
-      <c r="D83" s="78">
+      <c r="D83" s="71">
         <f>SUM(D84:E84)</f>
         <v>32</v>
       </c>
-      <c r="E83" s="88"/>
-      <c r="F83" s="78">
+      <c r="E83" s="72"/>
+      <c r="F83" s="71">
         <f>SUM(F84:G84)</f>
         <v>0</v>
       </c>
-      <c r="G83" s="80"/>
+      <c r="G83" s="75"/>
       <c r="H83" s="29"/>
       <c r="I83" s="8"/>
       <c r="J83" s="8"/>
@@ -16843,20 +16847,20 @@
       <c r="GI83" s="29"/>
     </row>
     <row r="84" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A84" s="108" t="s">
+      <c r="A84" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="B84" s="109"/>
+      <c r="B84" s="86"/>
       <c r="C84" s="42"/>
-      <c r="D84" s="62">
+      <c r="D84" s="65">
         <v>32</v>
       </c>
-      <c r="E84" s="63"/>
-      <c r="F84" s="62">
+      <c r="E84" s="66"/>
+      <c r="F84" s="65">
         <f>SUM(H84:GI84)</f>
         <v>0</v>
       </c>
-      <c r="G84" s="64"/>
+      <c r="G84" s="80"/>
       <c r="H84" s="26"/>
       <c r="I84" s="12"/>
       <c r="J84" s="12"/>
@@ -17043,21 +17047,21 @@
       <c r="GI84" s="32"/>
     </row>
     <row r="85" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A85" s="111" t="s">
+      <c r="A85" s="89" t="s">
         <v>155</v>
       </c>
-      <c r="B85" s="112"/>
+      <c r="B85" s="90"/>
       <c r="C85" s="43"/>
-      <c r="D85" s="78">
+      <c r="D85" s="71">
         <f>SUM(D86:E86)</f>
         <v>8</v>
       </c>
-      <c r="E85" s="88"/>
-      <c r="F85" s="89">
+      <c r="E85" s="72"/>
+      <c r="F85" s="95">
         <f>SUM(F86:G86)</f>
         <v>0</v>
       </c>
-      <c r="G85" s="90"/>
+      <c r="G85" s="96"/>
       <c r="H85" s="29"/>
       <c r="I85" s="8"/>
       <c r="J85" s="8"/>
@@ -17244,20 +17248,20 @@
       <c r="GI85" s="29"/>
     </row>
     <row r="86" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A86" s="110" t="s">
+      <c r="A86" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="B86" s="65"/>
+      <c r="B86" s="88"/>
       <c r="C86" s="27"/>
-      <c r="D86" s="62">
+      <c r="D86" s="65">
         <v>8</v>
       </c>
-      <c r="E86" s="63"/>
-      <c r="F86" s="62">
+      <c r="E86" s="66"/>
+      <c r="F86" s="65">
         <f>SUM(H86:GI86)</f>
         <v>0</v>
       </c>
-      <c r="G86" s="64"/>
+      <c r="G86" s="80"/>
       <c r="H86" s="26"/>
       <c r="I86" s="12"/>
       <c r="J86" s="12"/>
@@ -17444,20 +17448,20 @@
       <c r="GI86" s="32"/>
     </row>
     <row r="87" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A87" s="106" t="s">
+      <c r="A87" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="107"/>
+      <c r="B87" s="84"/>
       <c r="C87" s="43"/>
-      <c r="D87" s="78">
+      <c r="D87" s="71">
         <f>232-D90</f>
         <v>36.349999999999994</v>
       </c>
-      <c r="E87" s="88"/>
-      <c r="F87" s="78">
+      <c r="E87" s="72"/>
+      <c r="F87" s="71">
         <v>0</v>
       </c>
-      <c r="G87" s="80"/>
+      <c r="G87" s="75"/>
       <c r="H87" s="29"/>
       <c r="I87" s="8"/>
       <c r="J87" s="8"/>
@@ -17644,15 +17648,15 @@
       <c r="GI87" s="29"/>
     </row>
     <row r="88" spans="1:191" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="101" t="s">
+      <c r="A88" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="B88" s="102"/>
+      <c r="B88" s="108"/>
       <c r="C88" s="44"/>
-      <c r="D88" s="98"/>
-      <c r="E88" s="99"/>
-      <c r="F88" s="98"/>
-      <c r="G88" s="100"/>
+      <c r="D88" s="104"/>
+      <c r="E88" s="105"/>
+      <c r="F88" s="104"/>
+      <c r="G88" s="106"/>
       <c r="H88" s="28"/>
       <c r="I88" s="17"/>
       <c r="J88" s="17"/>
@@ -17891,21 +17895,21 @@
       <c r="AX89" s="3"/>
     </row>
     <row r="90" spans="1:191" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="96" t="s">
+      <c r="A90" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="97"/>
+      <c r="B90" s="103"/>
       <c r="C90" s="45"/>
-      <c r="D90" s="94">
+      <c r="D90" s="100">
         <f>SUM(D85,D83,D81,D62,D14)</f>
         <v>195.65</v>
       </c>
-      <c r="E90" s="95"/>
-      <c r="F90" s="94">
+      <c r="E90" s="101"/>
+      <c r="F90" s="100">
         <f>SUM(F85,F83,F81,F62,F14)</f>
-        <v>36.448999999999998</v>
-      </c>
-      <c r="G90" s="103"/>
+        <v>36.948999999999998</v>
+      </c>
+      <c r="G90" s="109"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
@@ -17952,6 +17956,316 @@
     </row>
   </sheetData>
   <mergeCells count="334">
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="GD13:GE13"/>
+    <mergeCell ref="GF13:GG13"/>
+    <mergeCell ref="GH13:GI13"/>
+    <mergeCell ref="DZ12:GI12"/>
+    <mergeCell ref="FL13:FM13"/>
+    <mergeCell ref="FN13:FO13"/>
+    <mergeCell ref="FP13:FQ13"/>
+    <mergeCell ref="FR13:FS13"/>
+    <mergeCell ref="FT13:FU13"/>
+    <mergeCell ref="FV13:FW13"/>
+    <mergeCell ref="FX13:FY13"/>
+    <mergeCell ref="FZ13:GA13"/>
+    <mergeCell ref="GB13:GC13"/>
+    <mergeCell ref="ET13:EU13"/>
+    <mergeCell ref="EV13:EW13"/>
+    <mergeCell ref="EX13:EY13"/>
+    <mergeCell ref="EZ13:FA13"/>
+    <mergeCell ref="FB13:FC13"/>
+    <mergeCell ref="FD13:FE13"/>
+    <mergeCell ref="FF13:FG13"/>
+    <mergeCell ref="DX13:DY13"/>
+    <mergeCell ref="FH13:FI13"/>
+    <mergeCell ref="FJ13:FK13"/>
+    <mergeCell ref="EB13:EC13"/>
+    <mergeCell ref="ED13:EE13"/>
+    <mergeCell ref="EF13:EG13"/>
+    <mergeCell ref="EH13:EI13"/>
+    <mergeCell ref="EJ13:EK13"/>
+    <mergeCell ref="EL13:EM13"/>
+    <mergeCell ref="EN13:EO13"/>
+    <mergeCell ref="EP13:EQ13"/>
+    <mergeCell ref="ER13:ES13"/>
+    <mergeCell ref="DF13:DG13"/>
+    <mergeCell ref="DH13:DI13"/>
+    <mergeCell ref="DJ13:DK13"/>
+    <mergeCell ref="DL13:DM13"/>
+    <mergeCell ref="DN13:DO13"/>
+    <mergeCell ref="DP13:DQ13"/>
+    <mergeCell ref="DR13:DS13"/>
+    <mergeCell ref="DT13:DU13"/>
+    <mergeCell ref="DV13:DW13"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="BH13:BI13"/>
+    <mergeCell ref="BJ13:BK13"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="P9:X9"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F11:G13"/>
+    <mergeCell ref="D11:E13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="AL13:AM13"/>
+    <mergeCell ref="AN13:AO13"/>
+    <mergeCell ref="AP13:AQ13"/>
+    <mergeCell ref="AR13:AS13"/>
+    <mergeCell ref="AT13:AU13"/>
+    <mergeCell ref="AV13:AW13"/>
+    <mergeCell ref="AX13:AY13"/>
+    <mergeCell ref="AZ13:BA13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="P6:X6"/>
+    <mergeCell ref="P5:X5"/>
+    <mergeCell ref="P4:X4"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="H12:BQ12"/>
+    <mergeCell ref="BB13:BC13"/>
+    <mergeCell ref="BD13:BE13"/>
+    <mergeCell ref="BF13:BG13"/>
+    <mergeCell ref="BP13:BQ13"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="AF13:AG13"/>
+    <mergeCell ref="AH13:AI13"/>
+    <mergeCell ref="AJ13:AK13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
     <mergeCell ref="BR13:BS13"/>
     <mergeCell ref="BL13:BM13"/>
     <mergeCell ref="BN13:BO13"/>
@@ -17976,316 +18290,6 @@
     <mergeCell ref="CZ13:DA13"/>
     <mergeCell ref="DB13:DC13"/>
     <mergeCell ref="DD13:DE13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="P6:X6"/>
-    <mergeCell ref="P5:X5"/>
-    <mergeCell ref="P4:X4"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="H12:BQ12"/>
-    <mergeCell ref="BB13:BC13"/>
-    <mergeCell ref="BD13:BE13"/>
-    <mergeCell ref="BF13:BG13"/>
-    <mergeCell ref="BP13:BQ13"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="AF13:AG13"/>
-    <mergeCell ref="AH13:AI13"/>
-    <mergeCell ref="AJ13:AK13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="AL13:AM13"/>
-    <mergeCell ref="AN13:AO13"/>
-    <mergeCell ref="AP13:AQ13"/>
-    <mergeCell ref="AR13:AS13"/>
-    <mergeCell ref="AT13:AU13"/>
-    <mergeCell ref="AV13:AW13"/>
-    <mergeCell ref="AX13:AY13"/>
-    <mergeCell ref="AZ13:BA13"/>
-    <mergeCell ref="BH13:BI13"/>
-    <mergeCell ref="BJ13:BK13"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="P9:X9"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F11:G13"/>
-    <mergeCell ref="D11:E13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="F90:G90"/>
-    <mergeCell ref="F87:G87"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="DF13:DG13"/>
-    <mergeCell ref="DH13:DI13"/>
-    <mergeCell ref="DJ13:DK13"/>
-    <mergeCell ref="DL13:DM13"/>
-    <mergeCell ref="DN13:DO13"/>
-    <mergeCell ref="DP13:DQ13"/>
-    <mergeCell ref="DR13:DS13"/>
-    <mergeCell ref="DT13:DU13"/>
-    <mergeCell ref="DV13:DW13"/>
-    <mergeCell ref="FF13:FG13"/>
-    <mergeCell ref="DX13:DY13"/>
-    <mergeCell ref="FH13:FI13"/>
-    <mergeCell ref="FJ13:FK13"/>
-    <mergeCell ref="EB13:EC13"/>
-    <mergeCell ref="ED13:EE13"/>
-    <mergeCell ref="EF13:EG13"/>
-    <mergeCell ref="EH13:EI13"/>
-    <mergeCell ref="EJ13:EK13"/>
-    <mergeCell ref="EL13:EM13"/>
-    <mergeCell ref="EN13:EO13"/>
-    <mergeCell ref="EP13:EQ13"/>
-    <mergeCell ref="ER13:ES13"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="GD13:GE13"/>
-    <mergeCell ref="GF13:GG13"/>
-    <mergeCell ref="GH13:GI13"/>
-    <mergeCell ref="DZ12:GI12"/>
-    <mergeCell ref="FL13:FM13"/>
-    <mergeCell ref="FN13:FO13"/>
-    <mergeCell ref="FP13:FQ13"/>
-    <mergeCell ref="FR13:FS13"/>
-    <mergeCell ref="FT13:FU13"/>
-    <mergeCell ref="FV13:FW13"/>
-    <mergeCell ref="FX13:FY13"/>
-    <mergeCell ref="FZ13:GA13"/>
-    <mergeCell ref="GB13:GC13"/>
-    <mergeCell ref="ET13:EU13"/>
-    <mergeCell ref="EV13:EW13"/>
-    <mergeCell ref="EX13:EY13"/>
-    <mergeCell ref="EZ13:FA13"/>
-    <mergeCell ref="FB13:FC13"/>
-    <mergeCell ref="FD13:FE13"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Created Models for Issue #3
</commit_message>
<xml_diff>
--- a/Documents/Zeitplan.xlsx
+++ b/Documents/Zeitplan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VirtualReality\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VirtualReality\Documents\SiemensVR\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1164,24 +1164,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1194,31 +1176,32 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1226,6 +1209,42 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1234,9 +1253,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1284,40 +1300,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1787,8 +1787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GI90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AX22" sqref="AX22"/>
+    <sheetView tabSelected="1" topLeftCell="Y31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BA59" sqref="BA59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1799,28 +1799,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:191" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
     </row>
     <row r="2" spans="1:191" x14ac:dyDescent="0.25">
       <c r="T2" s="9"/>
@@ -1853,17 +1853,17 @@
         <v>160</v>
       </c>
       <c r="N4" s="57"/>
-      <c r="P4" s="81" t="s">
+      <c r="P4" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="81"/>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="67"/>
+      <c r="V4" s="67"/>
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
     </row>
     <row r="5" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -1880,17 +1880,17 @@
       <c r="F5" s="5"/>
       <c r="G5" s="7"/>
       <c r="N5" s="24"/>
-      <c r="P5" s="81" t="s">
+      <c r="P5" s="67" t="s">
         <v>158</v>
       </c>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81"/>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="81"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
+      <c r="S5" s="67"/>
+      <c r="T5" s="67"/>
+      <c r="U5" s="67"/>
+      <c r="V5" s="67"/>
+      <c r="W5" s="67"/>
+      <c r="X5" s="67"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
@@ -1914,17 +1914,17 @@
         <v>15</v>
       </c>
       <c r="N6" s="16"/>
-      <c r="P6" s="81" t="s">
+      <c r="P6" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="81"/>
-      <c r="T6" s="81"/>
-      <c r="U6" s="81"/>
-      <c r="V6" s="81"/>
-      <c r="W6" s="81"/>
-      <c r="X6" s="81"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="67"/>
+      <c r="V6" s="67"/>
+      <c r="W6" s="67"/>
+      <c r="X6" s="67"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
@@ -1942,17 +1942,17 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="N7" s="21"/>
-      <c r="P7" s="81" t="s">
+      <c r="P7" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="81"/>
-      <c r="S7" s="81"/>
-      <c r="T7" s="81"/>
-      <c r="U7" s="81"/>
-      <c r="V7" s="81"/>
-      <c r="W7" s="81"/>
-      <c r="X7" s="81"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="67"/>
+      <c r="S7" s="67"/>
+      <c r="T7" s="67"/>
+      <c r="U7" s="67"/>
+      <c r="V7" s="67"/>
+      <c r="W7" s="67"/>
+      <c r="X7" s="67"/>
     </row>
     <row r="8" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1967,17 +1967,17 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="N8" s="20"/>
-      <c r="P8" s="113" t="s">
+      <c r="P8" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="113"/>
-      <c r="R8" s="113"/>
-      <c r="S8" s="113"/>
-      <c r="T8" s="113"/>
-      <c r="U8" s="113"/>
-      <c r="V8" s="113"/>
-      <c r="W8" s="113"/>
-      <c r="X8" s="113"/>
+      <c r="Q8" s="70"/>
+      <c r="R8" s="70"/>
+      <c r="S8" s="70"/>
+      <c r="T8" s="70"/>
+      <c r="U8" s="70"/>
+      <c r="V8" s="70"/>
+      <c r="W8" s="70"/>
+      <c r="X8" s="70"/>
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
@@ -1985,23 +1985,23 @@
       <c r="AC8" s="5"/>
     </row>
     <row r="9" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="118"/>
+      <c r="A9" s="68"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="12"/>
       <c r="N9" s="49"/>
-      <c r="P9" s="113" t="s">
+      <c r="P9" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="Q9" s="113"/>
-      <c r="R9" s="113"/>
-      <c r="S9" s="113"/>
-      <c r="T9" s="113"/>
-      <c r="U9" s="113"/>
-      <c r="V9" s="113"/>
-      <c r="W9" s="113"/>
-      <c r="X9" s="113"/>
+      <c r="Q9" s="70"/>
+      <c r="R9" s="70"/>
+      <c r="S9" s="70"/>
+      <c r="T9" s="70"/>
+      <c r="U9" s="70"/>
+      <c r="V9" s="70"/>
+      <c r="W9" s="70"/>
+      <c r="X9" s="70"/>
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
@@ -2011,7 +2011,7 @@
       <c r="AJ9" s="13"/>
     </row>
     <row r="10" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="118"/>
+      <c r="A10" s="68"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -2028,18 +2028,18 @@
       <c r="AC10" s="5"/>
     </row>
     <row r="11" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="118"/>
-      <c r="C11" s="116" t="s">
+      <c r="A11" s="68"/>
+      <c r="C11" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="114" t="s">
+      <c r="D11" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="114"/>
-      <c r="F11" s="114" t="s">
+      <c r="E11" s="76"/>
+      <c r="F11" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="114"/>
+      <c r="G11" s="76"/>
       <c r="T11" s="9"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
@@ -2052,596 +2052,596 @@
       <c r="AC11" s="5"/>
     </row>
     <row r="12" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="118"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="114"/>
-      <c r="G12" s="114"/>
-      <c r="H12" s="70" t="s">
+      <c r="A12" s="68"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="71"/>
-      <c r="N12" s="71"/>
-      <c r="O12" s="71"/>
-      <c r="P12" s="71"/>
-      <c r="Q12" s="71"/>
-      <c r="R12" s="71"/>
-      <c r="S12" s="71"/>
-      <c r="T12" s="71"/>
-      <c r="U12" s="71"/>
-      <c r="V12" s="71"/>
-      <c r="W12" s="71"/>
-      <c r="X12" s="71"/>
-      <c r="Y12" s="71"/>
-      <c r="Z12" s="71"/>
-      <c r="AA12" s="71"/>
-      <c r="AB12" s="71"/>
-      <c r="AC12" s="71"/>
-      <c r="AD12" s="71"/>
-      <c r="AE12" s="71"/>
-      <c r="AF12" s="71"/>
-      <c r="AG12" s="71"/>
-      <c r="AH12" s="71"/>
-      <c r="AI12" s="71"/>
-      <c r="AJ12" s="71"/>
-      <c r="AK12" s="71"/>
-      <c r="AL12" s="71"/>
-      <c r="AM12" s="71"/>
-      <c r="AN12" s="71"/>
-      <c r="AO12" s="71"/>
-      <c r="AP12" s="71"/>
-      <c r="AQ12" s="71"/>
-      <c r="AR12" s="71"/>
-      <c r="AS12" s="71"/>
-      <c r="AT12" s="71"/>
-      <c r="AU12" s="71"/>
-      <c r="AV12" s="71"/>
-      <c r="AW12" s="71"/>
-      <c r="AX12" s="71"/>
-      <c r="AY12" s="71"/>
-      <c r="AZ12" s="71"/>
-      <c r="BA12" s="71"/>
-      <c r="BB12" s="71"/>
-      <c r="BC12" s="71"/>
-      <c r="BD12" s="71"/>
-      <c r="BE12" s="71"/>
-      <c r="BF12" s="71"/>
-      <c r="BG12" s="71"/>
-      <c r="BH12" s="71"/>
-      <c r="BI12" s="71"/>
-      <c r="BJ12" s="71"/>
-      <c r="BK12" s="71"/>
-      <c r="BL12" s="71"/>
-      <c r="BM12" s="71"/>
-      <c r="BN12" s="71"/>
-      <c r="BO12" s="71"/>
-      <c r="BP12" s="71"/>
-      <c r="BQ12" s="119"/>
-      <c r="BR12" s="70" t="s">
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="63"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="63"/>
+      <c r="W12" s="63"/>
+      <c r="X12" s="63"/>
+      <c r="Y12" s="63"/>
+      <c r="Z12" s="63"/>
+      <c r="AA12" s="63"/>
+      <c r="AB12" s="63"/>
+      <c r="AC12" s="63"/>
+      <c r="AD12" s="63"/>
+      <c r="AE12" s="63"/>
+      <c r="AF12" s="63"/>
+      <c r="AG12" s="63"/>
+      <c r="AH12" s="63"/>
+      <c r="AI12" s="63"/>
+      <c r="AJ12" s="63"/>
+      <c r="AK12" s="63"/>
+      <c r="AL12" s="63"/>
+      <c r="AM12" s="63"/>
+      <c r="AN12" s="63"/>
+      <c r="AO12" s="63"/>
+      <c r="AP12" s="63"/>
+      <c r="AQ12" s="63"/>
+      <c r="AR12" s="63"/>
+      <c r="AS12" s="63"/>
+      <c r="AT12" s="63"/>
+      <c r="AU12" s="63"/>
+      <c r="AV12" s="63"/>
+      <c r="AW12" s="63"/>
+      <c r="AX12" s="63"/>
+      <c r="AY12" s="63"/>
+      <c r="AZ12" s="63"/>
+      <c r="BA12" s="63"/>
+      <c r="BB12" s="63"/>
+      <c r="BC12" s="63"/>
+      <c r="BD12" s="63"/>
+      <c r="BE12" s="63"/>
+      <c r="BF12" s="63"/>
+      <c r="BG12" s="63"/>
+      <c r="BH12" s="63"/>
+      <c r="BI12" s="63"/>
+      <c r="BJ12" s="63"/>
+      <c r="BK12" s="63"/>
+      <c r="BL12" s="63"/>
+      <c r="BM12" s="63"/>
+      <c r="BN12" s="63"/>
+      <c r="BO12" s="63"/>
+      <c r="BP12" s="63"/>
+      <c r="BQ12" s="64"/>
+      <c r="BR12" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="BS12" s="71"/>
-      <c r="BT12" s="71"/>
-      <c r="BU12" s="71"/>
-      <c r="BV12" s="71"/>
-      <c r="BW12" s="71"/>
-      <c r="BX12" s="71"/>
-      <c r="BY12" s="71"/>
-      <c r="BZ12" s="71"/>
-      <c r="CA12" s="71"/>
-      <c r="CB12" s="71"/>
-      <c r="CC12" s="71"/>
-      <c r="CD12" s="71"/>
-      <c r="CE12" s="71"/>
-      <c r="CF12" s="71"/>
-      <c r="CG12" s="71"/>
-      <c r="CH12" s="71"/>
-      <c r="CI12" s="71"/>
-      <c r="CJ12" s="71"/>
-      <c r="CK12" s="71"/>
-      <c r="CL12" s="71"/>
-      <c r="CM12" s="71"/>
-      <c r="CN12" s="71"/>
-      <c r="CO12" s="71"/>
-      <c r="CP12" s="71"/>
-      <c r="CQ12" s="71"/>
-      <c r="CR12" s="71"/>
-      <c r="CS12" s="71"/>
-      <c r="CT12" s="71"/>
-      <c r="CU12" s="71"/>
-      <c r="CV12" s="71"/>
-      <c r="CW12" s="71"/>
-      <c r="CX12" s="71"/>
-      <c r="CY12" s="71"/>
-      <c r="CZ12" s="71"/>
-      <c r="DA12" s="71"/>
-      <c r="DB12" s="71"/>
-      <c r="DC12" s="71"/>
-      <c r="DD12" s="71"/>
-      <c r="DE12" s="71"/>
-      <c r="DF12" s="71"/>
-      <c r="DG12" s="71"/>
-      <c r="DH12" s="71"/>
-      <c r="DI12" s="71"/>
-      <c r="DJ12" s="71"/>
-      <c r="DK12" s="71"/>
-      <c r="DL12" s="71"/>
-      <c r="DM12" s="71"/>
-      <c r="DN12" s="71"/>
-      <c r="DO12" s="71"/>
-      <c r="DP12" s="71"/>
-      <c r="DQ12" s="71"/>
-      <c r="DR12" s="71"/>
-      <c r="DS12" s="71"/>
-      <c r="DT12" s="71"/>
-      <c r="DU12" s="71"/>
-      <c r="DV12" s="71"/>
-      <c r="DW12" s="71"/>
-      <c r="DX12" s="71"/>
-      <c r="DY12" s="119"/>
-      <c r="DZ12" s="70" t="s">
+      <c r="BS12" s="63"/>
+      <c r="BT12" s="63"/>
+      <c r="BU12" s="63"/>
+      <c r="BV12" s="63"/>
+      <c r="BW12" s="63"/>
+      <c r="BX12" s="63"/>
+      <c r="BY12" s="63"/>
+      <c r="BZ12" s="63"/>
+      <c r="CA12" s="63"/>
+      <c r="CB12" s="63"/>
+      <c r="CC12" s="63"/>
+      <c r="CD12" s="63"/>
+      <c r="CE12" s="63"/>
+      <c r="CF12" s="63"/>
+      <c r="CG12" s="63"/>
+      <c r="CH12" s="63"/>
+      <c r="CI12" s="63"/>
+      <c r="CJ12" s="63"/>
+      <c r="CK12" s="63"/>
+      <c r="CL12" s="63"/>
+      <c r="CM12" s="63"/>
+      <c r="CN12" s="63"/>
+      <c r="CO12" s="63"/>
+      <c r="CP12" s="63"/>
+      <c r="CQ12" s="63"/>
+      <c r="CR12" s="63"/>
+      <c r="CS12" s="63"/>
+      <c r="CT12" s="63"/>
+      <c r="CU12" s="63"/>
+      <c r="CV12" s="63"/>
+      <c r="CW12" s="63"/>
+      <c r="CX12" s="63"/>
+      <c r="CY12" s="63"/>
+      <c r="CZ12" s="63"/>
+      <c r="DA12" s="63"/>
+      <c r="DB12" s="63"/>
+      <c r="DC12" s="63"/>
+      <c r="DD12" s="63"/>
+      <c r="DE12" s="63"/>
+      <c r="DF12" s="63"/>
+      <c r="DG12" s="63"/>
+      <c r="DH12" s="63"/>
+      <c r="DI12" s="63"/>
+      <c r="DJ12" s="63"/>
+      <c r="DK12" s="63"/>
+      <c r="DL12" s="63"/>
+      <c r="DM12" s="63"/>
+      <c r="DN12" s="63"/>
+      <c r="DO12" s="63"/>
+      <c r="DP12" s="63"/>
+      <c r="DQ12" s="63"/>
+      <c r="DR12" s="63"/>
+      <c r="DS12" s="63"/>
+      <c r="DT12" s="63"/>
+      <c r="DU12" s="63"/>
+      <c r="DV12" s="63"/>
+      <c r="DW12" s="63"/>
+      <c r="DX12" s="63"/>
+      <c r="DY12" s="64"/>
+      <c r="DZ12" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="EA12" s="71"/>
-      <c r="EB12" s="71"/>
-      <c r="EC12" s="71"/>
-      <c r="ED12" s="71"/>
-      <c r="EE12" s="71"/>
-      <c r="EF12" s="71"/>
-      <c r="EG12" s="71"/>
-      <c r="EH12" s="71"/>
-      <c r="EI12" s="71"/>
-      <c r="EJ12" s="71"/>
-      <c r="EK12" s="71"/>
-      <c r="EL12" s="71"/>
-      <c r="EM12" s="71"/>
-      <c r="EN12" s="71"/>
-      <c r="EO12" s="71"/>
-      <c r="EP12" s="71"/>
-      <c r="EQ12" s="71"/>
-      <c r="ER12" s="71"/>
-      <c r="ES12" s="71"/>
-      <c r="ET12" s="71"/>
-      <c r="EU12" s="71"/>
-      <c r="EV12" s="71"/>
-      <c r="EW12" s="71"/>
-      <c r="EX12" s="71"/>
-      <c r="EY12" s="71"/>
-      <c r="EZ12" s="71"/>
-      <c r="FA12" s="71"/>
-      <c r="FB12" s="71"/>
-      <c r="FC12" s="71"/>
-      <c r="FD12" s="71"/>
-      <c r="FE12" s="71"/>
-      <c r="FF12" s="71"/>
-      <c r="FG12" s="71"/>
-      <c r="FH12" s="71"/>
-      <c r="FI12" s="71"/>
-      <c r="FJ12" s="71"/>
-      <c r="FK12" s="71"/>
-      <c r="FL12" s="71"/>
-      <c r="FM12" s="71"/>
-      <c r="FN12" s="71"/>
-      <c r="FO12" s="71"/>
-      <c r="FP12" s="71"/>
-      <c r="FQ12" s="71"/>
-      <c r="FR12" s="71"/>
-      <c r="FS12" s="71"/>
-      <c r="FT12" s="71"/>
-      <c r="FU12" s="71"/>
-      <c r="FV12" s="71"/>
-      <c r="FW12" s="71"/>
-      <c r="FX12" s="71"/>
-      <c r="FY12" s="71"/>
-      <c r="FZ12" s="71"/>
-      <c r="GA12" s="71"/>
-      <c r="GB12" s="71"/>
-      <c r="GC12" s="71"/>
-      <c r="GD12" s="71"/>
-      <c r="GE12" s="71"/>
-      <c r="GF12" s="71"/>
-      <c r="GG12" s="71"/>
-      <c r="GH12" s="71"/>
-      <c r="GI12" s="72"/>
+      <c r="EA12" s="63"/>
+      <c r="EB12" s="63"/>
+      <c r="EC12" s="63"/>
+      <c r="ED12" s="63"/>
+      <c r="EE12" s="63"/>
+      <c r="EF12" s="63"/>
+      <c r="EG12" s="63"/>
+      <c r="EH12" s="63"/>
+      <c r="EI12" s="63"/>
+      <c r="EJ12" s="63"/>
+      <c r="EK12" s="63"/>
+      <c r="EL12" s="63"/>
+      <c r="EM12" s="63"/>
+      <c r="EN12" s="63"/>
+      <c r="EO12" s="63"/>
+      <c r="EP12" s="63"/>
+      <c r="EQ12" s="63"/>
+      <c r="ER12" s="63"/>
+      <c r="ES12" s="63"/>
+      <c r="ET12" s="63"/>
+      <c r="EU12" s="63"/>
+      <c r="EV12" s="63"/>
+      <c r="EW12" s="63"/>
+      <c r="EX12" s="63"/>
+      <c r="EY12" s="63"/>
+      <c r="EZ12" s="63"/>
+      <c r="FA12" s="63"/>
+      <c r="FB12" s="63"/>
+      <c r="FC12" s="63"/>
+      <c r="FD12" s="63"/>
+      <c r="FE12" s="63"/>
+      <c r="FF12" s="63"/>
+      <c r="FG12" s="63"/>
+      <c r="FH12" s="63"/>
+      <c r="FI12" s="63"/>
+      <c r="FJ12" s="63"/>
+      <c r="FK12" s="63"/>
+      <c r="FL12" s="63"/>
+      <c r="FM12" s="63"/>
+      <c r="FN12" s="63"/>
+      <c r="FO12" s="63"/>
+      <c r="FP12" s="63"/>
+      <c r="FQ12" s="63"/>
+      <c r="FR12" s="63"/>
+      <c r="FS12" s="63"/>
+      <c r="FT12" s="63"/>
+      <c r="FU12" s="63"/>
+      <c r="FV12" s="63"/>
+      <c r="FW12" s="63"/>
+      <c r="FX12" s="63"/>
+      <c r="FY12" s="63"/>
+      <c r="FZ12" s="63"/>
+      <c r="GA12" s="63"/>
+      <c r="GB12" s="63"/>
+      <c r="GC12" s="63"/>
+      <c r="GD12" s="63"/>
+      <c r="GE12" s="63"/>
+      <c r="GF12" s="63"/>
+      <c r="GG12" s="63"/>
+      <c r="GH12" s="63"/>
+      <c r="GI12" s="120"/>
     </row>
     <row r="13" spans="1:191" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="117"/>
-      <c r="D13" s="115"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="115"/>
-      <c r="H13" s="68">
+      <c r="C13" s="79"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="60">
         <v>1</v>
       </c>
-      <c r="I13" s="69"/>
-      <c r="J13" s="68">
+      <c r="I13" s="61"/>
+      <c r="J13" s="60">
         <v>2</v>
       </c>
-      <c r="K13" s="69"/>
-      <c r="L13" s="68">
+      <c r="K13" s="61"/>
+      <c r="L13" s="60">
         <v>3</v>
       </c>
-      <c r="M13" s="69"/>
-      <c r="N13" s="68">
+      <c r="M13" s="61"/>
+      <c r="N13" s="60">
         <v>4</v>
       </c>
-      <c r="O13" s="69"/>
-      <c r="P13" s="68">
+      <c r="O13" s="61"/>
+      <c r="P13" s="60">
         <v>5</v>
       </c>
-      <c r="Q13" s="69"/>
-      <c r="R13" s="68">
+      <c r="Q13" s="61"/>
+      <c r="R13" s="60">
         <v>6</v>
       </c>
-      <c r="S13" s="69"/>
-      <c r="T13" s="68">
+      <c r="S13" s="61"/>
+      <c r="T13" s="60">
         <v>7</v>
       </c>
-      <c r="U13" s="69"/>
-      <c r="V13" s="68">
+      <c r="U13" s="61"/>
+      <c r="V13" s="60">
         <v>8</v>
       </c>
-      <c r="W13" s="69"/>
-      <c r="X13" s="68">
+      <c r="W13" s="61"/>
+      <c r="X13" s="60">
         <v>9</v>
       </c>
-      <c r="Y13" s="69"/>
-      <c r="Z13" s="68">
+      <c r="Y13" s="61"/>
+      <c r="Z13" s="60">
         <v>10</v>
       </c>
-      <c r="AA13" s="69"/>
-      <c r="AB13" s="68">
+      <c r="AA13" s="61"/>
+      <c r="AB13" s="60">
         <v>11</v>
       </c>
-      <c r="AC13" s="69"/>
-      <c r="AD13" s="68">
+      <c r="AC13" s="61"/>
+      <c r="AD13" s="60">
         <v>12</v>
       </c>
-      <c r="AE13" s="69"/>
-      <c r="AF13" s="68">
+      <c r="AE13" s="61"/>
+      <c r="AF13" s="60">
         <v>13</v>
       </c>
-      <c r="AG13" s="69"/>
-      <c r="AH13" s="68">
+      <c r="AG13" s="61"/>
+      <c r="AH13" s="60">
         <v>14</v>
       </c>
-      <c r="AI13" s="69"/>
-      <c r="AJ13" s="68">
+      <c r="AI13" s="61"/>
+      <c r="AJ13" s="60">
         <v>15</v>
       </c>
-      <c r="AK13" s="69"/>
-      <c r="AL13" s="68">
+      <c r="AK13" s="61"/>
+      <c r="AL13" s="60">
         <v>16</v>
       </c>
-      <c r="AM13" s="69"/>
-      <c r="AN13" s="68">
+      <c r="AM13" s="61"/>
+      <c r="AN13" s="60">
         <v>17</v>
       </c>
-      <c r="AO13" s="69"/>
-      <c r="AP13" s="68">
+      <c r="AO13" s="61"/>
+      <c r="AP13" s="60">
         <v>18</v>
       </c>
-      <c r="AQ13" s="69"/>
-      <c r="AR13" s="68">
+      <c r="AQ13" s="61"/>
+      <c r="AR13" s="60">
         <v>19</v>
       </c>
-      <c r="AS13" s="69"/>
-      <c r="AT13" s="68">
+      <c r="AS13" s="61"/>
+      <c r="AT13" s="60">
         <v>20</v>
       </c>
-      <c r="AU13" s="69"/>
-      <c r="AV13" s="68">
+      <c r="AU13" s="61"/>
+      <c r="AV13" s="60">
         <v>21</v>
       </c>
-      <c r="AW13" s="69"/>
-      <c r="AX13" s="68">
+      <c r="AW13" s="61"/>
+      <c r="AX13" s="60">
         <v>22</v>
       </c>
-      <c r="AY13" s="69"/>
-      <c r="AZ13" s="68">
+      <c r="AY13" s="61"/>
+      <c r="AZ13" s="60">
         <v>23</v>
       </c>
-      <c r="BA13" s="69"/>
-      <c r="BB13" s="68">
+      <c r="BA13" s="61"/>
+      <c r="BB13" s="60">
         <v>24</v>
       </c>
-      <c r="BC13" s="69"/>
-      <c r="BD13" s="68">
+      <c r="BC13" s="61"/>
+      <c r="BD13" s="60">
         <v>25</v>
       </c>
-      <c r="BE13" s="69"/>
-      <c r="BF13" s="68">
+      <c r="BE13" s="61"/>
+      <c r="BF13" s="60">
         <v>26</v>
       </c>
-      <c r="BG13" s="69"/>
-      <c r="BH13" s="68">
+      <c r="BG13" s="61"/>
+      <c r="BH13" s="60">
         <v>27</v>
       </c>
-      <c r="BI13" s="69"/>
-      <c r="BJ13" s="68">
+      <c r="BI13" s="61"/>
+      <c r="BJ13" s="60">
         <v>28</v>
       </c>
-      <c r="BK13" s="69"/>
-      <c r="BL13" s="68">
+      <c r="BK13" s="61"/>
+      <c r="BL13" s="60">
         <v>29</v>
       </c>
-      <c r="BM13" s="69"/>
-      <c r="BN13" s="68">
+      <c r="BM13" s="61"/>
+      <c r="BN13" s="60">
         <v>30</v>
       </c>
-      <c r="BO13" s="69"/>
-      <c r="BP13" s="68">
+      <c r="BO13" s="61"/>
+      <c r="BP13" s="60">
         <v>31</v>
       </c>
-      <c r="BQ13" s="120"/>
-      <c r="BR13" s="68">
+      <c r="BQ13" s="69"/>
+      <c r="BR13" s="60">
         <v>1</v>
       </c>
-      <c r="BS13" s="69"/>
-      <c r="BT13" s="68">
+      <c r="BS13" s="61"/>
+      <c r="BT13" s="60">
         <v>2</v>
       </c>
-      <c r="BU13" s="69"/>
-      <c r="BV13" s="68">
+      <c r="BU13" s="61"/>
+      <c r="BV13" s="60">
         <v>3</v>
       </c>
-      <c r="BW13" s="69"/>
-      <c r="BX13" s="68">
+      <c r="BW13" s="61"/>
+      <c r="BX13" s="60">
         <v>4</v>
       </c>
-      <c r="BY13" s="69"/>
-      <c r="BZ13" s="68">
+      <c r="BY13" s="61"/>
+      <c r="BZ13" s="60">
         <v>5</v>
       </c>
-      <c r="CA13" s="69"/>
-      <c r="CB13" s="68">
+      <c r="CA13" s="61"/>
+      <c r="CB13" s="60">
         <v>6</v>
       </c>
-      <c r="CC13" s="69"/>
-      <c r="CD13" s="68">
+      <c r="CC13" s="61"/>
+      <c r="CD13" s="60">
         <v>7</v>
       </c>
-      <c r="CE13" s="69"/>
-      <c r="CF13" s="68">
+      <c r="CE13" s="61"/>
+      <c r="CF13" s="60">
         <v>8</v>
       </c>
-      <c r="CG13" s="69"/>
-      <c r="CH13" s="68">
+      <c r="CG13" s="61"/>
+      <c r="CH13" s="60">
         <v>9</v>
       </c>
-      <c r="CI13" s="69"/>
-      <c r="CJ13" s="68">
+      <c r="CI13" s="61"/>
+      <c r="CJ13" s="60">
         <v>10</v>
       </c>
-      <c r="CK13" s="69"/>
-      <c r="CL13" s="68">
+      <c r="CK13" s="61"/>
+      <c r="CL13" s="60">
         <v>11</v>
       </c>
-      <c r="CM13" s="69"/>
-      <c r="CN13" s="68">
+      <c r="CM13" s="61"/>
+      <c r="CN13" s="60">
         <v>12</v>
       </c>
-      <c r="CO13" s="69"/>
-      <c r="CP13" s="68">
+      <c r="CO13" s="61"/>
+      <c r="CP13" s="60">
         <v>13</v>
       </c>
-      <c r="CQ13" s="69"/>
-      <c r="CR13" s="68">
+      <c r="CQ13" s="61"/>
+      <c r="CR13" s="60">
         <v>14</v>
       </c>
-      <c r="CS13" s="69"/>
-      <c r="CT13" s="68">
+      <c r="CS13" s="61"/>
+      <c r="CT13" s="60">
         <v>15</v>
       </c>
-      <c r="CU13" s="69"/>
-      <c r="CV13" s="68">
+      <c r="CU13" s="61"/>
+      <c r="CV13" s="60">
         <v>16</v>
       </c>
-      <c r="CW13" s="69"/>
-      <c r="CX13" s="68">
+      <c r="CW13" s="61"/>
+      <c r="CX13" s="60">
         <v>17</v>
       </c>
-      <c r="CY13" s="69"/>
-      <c r="CZ13" s="68">
+      <c r="CY13" s="61"/>
+      <c r="CZ13" s="60">
         <v>18</v>
       </c>
-      <c r="DA13" s="69"/>
-      <c r="DB13" s="68">
+      <c r="DA13" s="61"/>
+      <c r="DB13" s="60">
         <v>19</v>
       </c>
-      <c r="DC13" s="69"/>
-      <c r="DD13" s="68">
+      <c r="DC13" s="61"/>
+      <c r="DD13" s="60">
         <v>20</v>
       </c>
-      <c r="DE13" s="69"/>
-      <c r="DF13" s="68">
+      <c r="DE13" s="61"/>
+      <c r="DF13" s="60">
         <v>21</v>
       </c>
-      <c r="DG13" s="69"/>
-      <c r="DH13" s="68">
+      <c r="DG13" s="61"/>
+      <c r="DH13" s="60">
         <v>22</v>
       </c>
-      <c r="DI13" s="69"/>
-      <c r="DJ13" s="68">
+      <c r="DI13" s="61"/>
+      <c r="DJ13" s="60">
         <v>23</v>
       </c>
-      <c r="DK13" s="69"/>
-      <c r="DL13" s="68">
+      <c r="DK13" s="61"/>
+      <c r="DL13" s="60">
         <v>24</v>
       </c>
-      <c r="DM13" s="69"/>
-      <c r="DN13" s="68">
+      <c r="DM13" s="61"/>
+      <c r="DN13" s="60">
         <v>25</v>
       </c>
-      <c r="DO13" s="69"/>
-      <c r="DP13" s="68">
+      <c r="DO13" s="61"/>
+      <c r="DP13" s="60">
         <v>26</v>
       </c>
-      <c r="DQ13" s="69"/>
-      <c r="DR13" s="68">
+      <c r="DQ13" s="61"/>
+      <c r="DR13" s="60">
         <v>27</v>
       </c>
-      <c r="DS13" s="69"/>
-      <c r="DT13" s="68">
+      <c r="DS13" s="61"/>
+      <c r="DT13" s="60">
         <v>28</v>
       </c>
-      <c r="DU13" s="69"/>
-      <c r="DV13" s="68">
+      <c r="DU13" s="61"/>
+      <c r="DV13" s="60">
         <v>29</v>
       </c>
-      <c r="DW13" s="69"/>
-      <c r="DX13" s="68">
+      <c r="DW13" s="61"/>
+      <c r="DX13" s="60">
         <v>30</v>
       </c>
-      <c r="DY13" s="69"/>
-      <c r="DZ13" s="68">
+      <c r="DY13" s="61"/>
+      <c r="DZ13" s="60">
         <v>1</v>
       </c>
-      <c r="EA13" s="69"/>
-      <c r="EB13" s="68">
+      <c r="EA13" s="61"/>
+      <c r="EB13" s="60">
         <v>2</v>
       </c>
-      <c r="EC13" s="69"/>
-      <c r="ED13" s="68">
+      <c r="EC13" s="61"/>
+      <c r="ED13" s="60">
         <v>3</v>
       </c>
-      <c r="EE13" s="69"/>
-      <c r="EF13" s="68">
+      <c r="EE13" s="61"/>
+      <c r="EF13" s="60">
         <v>4</v>
       </c>
-      <c r="EG13" s="69"/>
-      <c r="EH13" s="68">
+      <c r="EG13" s="61"/>
+      <c r="EH13" s="60">
         <v>5</v>
       </c>
-      <c r="EI13" s="69"/>
-      <c r="EJ13" s="68">
+      <c r="EI13" s="61"/>
+      <c r="EJ13" s="60">
         <v>6</v>
       </c>
-      <c r="EK13" s="69"/>
-      <c r="EL13" s="68">
+      <c r="EK13" s="61"/>
+      <c r="EL13" s="60">
         <v>7</v>
       </c>
-      <c r="EM13" s="69"/>
-      <c r="EN13" s="68">
+      <c r="EM13" s="61"/>
+      <c r="EN13" s="60">
         <v>8</v>
       </c>
-      <c r="EO13" s="69"/>
-      <c r="EP13" s="68">
+      <c r="EO13" s="61"/>
+      <c r="EP13" s="60">
         <v>9</v>
       </c>
-      <c r="EQ13" s="69"/>
-      <c r="ER13" s="68">
+      <c r="EQ13" s="61"/>
+      <c r="ER13" s="60">
         <v>10</v>
       </c>
-      <c r="ES13" s="69"/>
-      <c r="ET13" s="68">
+      <c r="ES13" s="61"/>
+      <c r="ET13" s="60">
         <v>11</v>
       </c>
-      <c r="EU13" s="69"/>
-      <c r="EV13" s="68">
+      <c r="EU13" s="61"/>
+      <c r="EV13" s="60">
         <v>12</v>
       </c>
-      <c r="EW13" s="69"/>
-      <c r="EX13" s="68">
+      <c r="EW13" s="61"/>
+      <c r="EX13" s="60">
         <v>13</v>
       </c>
-      <c r="EY13" s="69"/>
-      <c r="EZ13" s="68">
+      <c r="EY13" s="61"/>
+      <c r="EZ13" s="60">
         <v>14</v>
       </c>
-      <c r="FA13" s="69"/>
-      <c r="FB13" s="68">
+      <c r="FA13" s="61"/>
+      <c r="FB13" s="60">
         <v>15</v>
       </c>
-      <c r="FC13" s="69"/>
-      <c r="FD13" s="68">
+      <c r="FC13" s="61"/>
+      <c r="FD13" s="60">
         <v>16</v>
       </c>
-      <c r="FE13" s="69"/>
-      <c r="FF13" s="68">
+      <c r="FE13" s="61"/>
+      <c r="FF13" s="60">
         <v>17</v>
       </c>
-      <c r="FG13" s="69"/>
-      <c r="FH13" s="68">
+      <c r="FG13" s="61"/>
+      <c r="FH13" s="60">
         <v>18</v>
       </c>
-      <c r="FI13" s="69"/>
-      <c r="FJ13" s="68">
+      <c r="FI13" s="61"/>
+      <c r="FJ13" s="60">
         <v>19</v>
       </c>
-      <c r="FK13" s="69"/>
-      <c r="FL13" s="68">
+      <c r="FK13" s="61"/>
+      <c r="FL13" s="60">
         <v>20</v>
       </c>
-      <c r="FM13" s="69"/>
-      <c r="FN13" s="68">
+      <c r="FM13" s="61"/>
+      <c r="FN13" s="60">
         <v>21</v>
       </c>
-      <c r="FO13" s="69"/>
-      <c r="FP13" s="68">
+      <c r="FO13" s="61"/>
+      <c r="FP13" s="60">
         <v>22</v>
       </c>
-      <c r="FQ13" s="69"/>
-      <c r="FR13" s="68">
+      <c r="FQ13" s="61"/>
+      <c r="FR13" s="60">
         <v>23</v>
       </c>
-      <c r="FS13" s="69"/>
-      <c r="FT13" s="68">
+      <c r="FS13" s="61"/>
+      <c r="FT13" s="60">
         <v>24</v>
       </c>
-      <c r="FU13" s="69"/>
-      <c r="FV13" s="68">
+      <c r="FU13" s="61"/>
+      <c r="FV13" s="60">
         <v>25</v>
       </c>
-      <c r="FW13" s="69"/>
-      <c r="FX13" s="68">
+      <c r="FW13" s="61"/>
+      <c r="FX13" s="60">
         <v>26</v>
       </c>
-      <c r="FY13" s="69"/>
-      <c r="FZ13" s="68">
+      <c r="FY13" s="61"/>
+      <c r="FZ13" s="60">
         <v>27</v>
       </c>
-      <c r="GA13" s="69"/>
-      <c r="GB13" s="68">
+      <c r="GA13" s="61"/>
+      <c r="GB13" s="60">
         <v>28</v>
       </c>
-      <c r="GC13" s="69"/>
-      <c r="GD13" s="68">
+      <c r="GC13" s="61"/>
+      <c r="GD13" s="60">
         <v>29</v>
       </c>
-      <c r="GE13" s="69"/>
-      <c r="GF13" s="68">
+      <c r="GE13" s="61"/>
+      <c r="GF13" s="60">
         <v>30</v>
       </c>
-      <c r="GG13" s="69"/>
-      <c r="GH13" s="68">
+      <c r="GG13" s="61"/>
+      <c r="GH13" s="60">
         <v>31</v>
       </c>
-      <c r="GI13" s="69"/>
+      <c r="GI13" s="61"/>
     </row>
     <row r="14" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="113" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="75"/>
+      <c r="B14" s="114"/>
       <c r="C14" s="37"/>
-      <c r="D14" s="91">
+      <c r="D14" s="97">
         <f>SUM(D15:E61)</f>
         <v>51.050000000000011</v>
       </c>
-      <c r="E14" s="93"/>
-      <c r="F14" s="91">
+      <c r="E14" s="99"/>
+      <c r="F14" s="97">
         <f>SUM(F15:G61)</f>
-        <v>40.625999999999998</v>
-      </c>
-      <c r="G14" s="92"/>
+        <v>42.125999999999998</v>
+      </c>
+      <c r="G14" s="98"/>
       <c r="H14" s="18"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -2828,22 +2828,22 @@
       <c r="GI14" s="14"/>
     </row>
     <row r="15" spans="1:191" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="82" t="s">
+      <c r="A15" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="83"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="62">
+      <c r="D15" s="65">
         <v>1.5</v>
       </c>
-      <c r="E15" s="63"/>
-      <c r="F15" s="62">
+      <c r="E15" s="66"/>
+      <c r="F15" s="65">
         <f>SUM(H15:GI15)</f>
         <v>0.5</v>
       </c>
-      <c r="G15" s="64"/>
+      <c r="G15" s="80"/>
       <c r="H15" s="47"/>
       <c r="I15" s="12"/>
       <c r="J15" s="24">
@@ -3032,22 +3032,22 @@
       <c r="GI15" s="34"/>
     </row>
     <row r="16" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="67"/>
+      <c r="B16" s="82"/>
       <c r="C16" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="62">
+      <c r="D16" s="65">
         <v>0.6</v>
       </c>
-      <c r="E16" s="63"/>
-      <c r="F16" s="62">
+      <c r="E16" s="66"/>
+      <c r="F16" s="65">
         <f>SUM(H16:GI16)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="64"/>
+      <c r="G16" s="80"/>
       <c r="H16" s="47"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
@@ -3234,22 +3234,22 @@
       <c r="GI16" s="32"/>
     </row>
     <row r="17" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="67"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="62">
+      <c r="D17" s="65">
         <v>1</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="62">
+      <c r="E17" s="66"/>
+      <c r="F17" s="65">
         <f>SUM(H17:GI17)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="64"/>
+      <c r="G17" s="80"/>
       <c r="H17" s="47"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
@@ -3440,22 +3440,22 @@
       <c r="GI17" s="32"/>
     </row>
     <row r="18" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="67"/>
+      <c r="B18" s="82"/>
       <c r="C18" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="62">
+      <c r="D18" s="65">
         <v>0.8</v>
       </c>
-      <c r="E18" s="63"/>
-      <c r="F18" s="62">
+      <c r="E18" s="66"/>
+      <c r="F18" s="65">
         <f t="shared" ref="F18:F60" si="0">SUM(H18:GI18)</f>
         <v>1.25</v>
       </c>
-      <c r="G18" s="64"/>
+      <c r="G18" s="80"/>
       <c r="H18" s="26"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
@@ -3646,22 +3646,22 @@
       <c r="GI18" s="32"/>
     </row>
     <row r="19" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="67"/>
+      <c r="B19" s="82"/>
       <c r="C19" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="62">
+      <c r="D19" s="65">
         <v>0.5</v>
       </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="62">
+      <c r="E19" s="66"/>
+      <c r="F19" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="64"/>
+      <c r="G19" s="80"/>
       <c r="H19" s="26"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
@@ -3848,22 +3848,22 @@
       <c r="GI19" s="36"/>
     </row>
     <row r="20" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="67"/>
+      <c r="B20" s="82"/>
       <c r="C20" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="62">
+      <c r="D20" s="65">
         <v>0.3</v>
       </c>
-      <c r="E20" s="63"/>
-      <c r="F20" s="62">
+      <c r="E20" s="66"/>
+      <c r="F20" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="64"/>
+      <c r="G20" s="80"/>
       <c r="H20" s="26"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -4050,22 +4050,22 @@
       <c r="GI20" s="36"/>
     </row>
     <row r="21" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="67"/>
+      <c r="B21" s="82"/>
       <c r="C21" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="62">
+      <c r="D21" s="65">
         <v>1</v>
       </c>
-      <c r="E21" s="63"/>
-      <c r="F21" s="62">
+      <c r="E21" s="66"/>
+      <c r="F21" s="65">
         <f t="shared" si="0"/>
         <v>0.16600000000000001</v>
       </c>
-      <c r="G21" s="64"/>
+      <c r="G21" s="80"/>
       <c r="H21" s="26"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
@@ -4254,22 +4254,22 @@
       <c r="GI21" s="36"/>
     </row>
     <row r="22" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="67"/>
+      <c r="B22" s="82"/>
       <c r="C22" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="62">
+      <c r="D22" s="65">
         <v>0.6</v>
       </c>
-      <c r="E22" s="63"/>
-      <c r="F22" s="62">
+      <c r="E22" s="66"/>
+      <c r="F22" s="65">
         <f t="shared" si="0"/>
         <v>0.66</v>
       </c>
-      <c r="G22" s="64"/>
+      <c r="G22" s="80"/>
       <c r="H22" s="26"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
@@ -4458,22 +4458,22 @@
       <c r="GI22" s="36"/>
     </row>
     <row r="23" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="67"/>
+      <c r="B23" s="82"/>
       <c r="C23" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="62">
+      <c r="D23" s="65">
         <v>0.6</v>
       </c>
-      <c r="E23" s="63"/>
-      <c r="F23" s="62">
+      <c r="E23" s="66"/>
+      <c r="F23" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="64"/>
+      <c r="G23" s="80"/>
       <c r="H23" s="26"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
@@ -4660,22 +4660,22 @@
       <c r="GI23" s="36"/>
     </row>
     <row r="24" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="67"/>
+      <c r="B24" s="82"/>
       <c r="C24" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="62">
+      <c r="D24" s="65">
         <v>3</v>
       </c>
-      <c r="E24" s="63"/>
-      <c r="F24" s="62">
+      <c r="E24" s="66"/>
+      <c r="F24" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="64"/>
+      <c r="G24" s="80"/>
       <c r="H24" s="26"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
@@ -4862,22 +4862,22 @@
       <c r="GI24" s="36"/>
     </row>
     <row r="25" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="67"/>
+      <c r="B25" s="82"/>
       <c r="C25" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="62">
+      <c r="D25" s="65">
         <v>1.5</v>
       </c>
-      <c r="E25" s="63"/>
-      <c r="F25" s="62">
+      <c r="E25" s="66"/>
+      <c r="F25" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="64"/>
+      <c r="G25" s="80"/>
       <c r="H25" s="26"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
@@ -5064,22 +5064,22 @@
       <c r="GI25" s="36"/>
     </row>
     <row r="26" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A26" s="66" t="s">
+      <c r="A26" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="67"/>
+      <c r="B26" s="82"/>
       <c r="C26" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="62">
+      <c r="D26" s="65">
         <v>1</v>
       </c>
-      <c r="E26" s="63"/>
-      <c r="F26" s="62">
+      <c r="E26" s="66"/>
+      <c r="F26" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="64"/>
+      <c r="G26" s="80"/>
       <c r="H26" s="26"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
@@ -5266,22 +5266,22 @@
       <c r="GI26" s="36"/>
     </row>
     <row r="27" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="67"/>
+      <c r="B27" s="82"/>
       <c r="C27" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="62">
+      <c r="D27" s="65">
         <v>1</v>
       </c>
-      <c r="E27" s="63"/>
-      <c r="F27" s="62">
+      <c r="E27" s="66"/>
+      <c r="F27" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G27" s="64"/>
+      <c r="G27" s="80"/>
       <c r="H27" s="26"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
@@ -5468,22 +5468,22 @@
       <c r="GI27" s="36"/>
     </row>
     <row r="28" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A28" s="66" t="s">
+      <c r="A28" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="67"/>
+      <c r="B28" s="82"/>
       <c r="C28" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="62">
+      <c r="D28" s="65">
         <v>1</v>
       </c>
-      <c r="E28" s="63"/>
-      <c r="F28" s="62">
+      <c r="E28" s="66"/>
+      <c r="F28" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G28" s="64"/>
+      <c r="G28" s="80"/>
       <c r="H28" s="26"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
@@ -5672,22 +5672,22 @@
       <c r="GI28" s="36"/>
     </row>
     <row r="29" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="67"/>
+      <c r="B29" s="82"/>
       <c r="C29" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="62">
+      <c r="D29" s="65">
         <v>1</v>
       </c>
-      <c r="E29" s="63"/>
-      <c r="F29" s="62">
+      <c r="E29" s="66"/>
+      <c r="F29" s="65">
         <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
-      <c r="G29" s="64"/>
+      <c r="G29" s="80"/>
       <c r="H29" s="26"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
@@ -5878,22 +5878,22 @@
       <c r="GI29" s="36"/>
     </row>
     <row r="30" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A30" s="66" t="s">
+      <c r="A30" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="67"/>
+      <c r="B30" s="82"/>
       <c r="C30" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="62">
+      <c r="D30" s="65">
         <v>1</v>
       </c>
-      <c r="E30" s="63"/>
-      <c r="F30" s="62">
+      <c r="E30" s="66"/>
+      <c r="F30" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G30" s="64"/>
+      <c r="G30" s="80"/>
       <c r="H30" s="26"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
@@ -6082,22 +6082,22 @@
       <c r="GI30" s="36"/>
     </row>
     <row r="31" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A31" s="66" t="s">
+      <c r="A31" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="67"/>
+      <c r="B31" s="82"/>
       <c r="C31" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="62">
+      <c r="D31" s="65">
         <v>4</v>
       </c>
-      <c r="E31" s="63"/>
-      <c r="F31" s="62">
+      <c r="E31" s="66"/>
+      <c r="F31" s="65">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G31" s="64"/>
+      <c r="G31" s="80"/>
       <c r="H31" s="26"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
@@ -6288,22 +6288,22 @@
       <c r="GI31" s="36"/>
     </row>
     <row r="32" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A32" s="66" t="s">
+      <c r="A32" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="67"/>
+      <c r="B32" s="82"/>
       <c r="C32" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="62">
+      <c r="D32" s="65">
         <v>0.6</v>
       </c>
-      <c r="E32" s="63"/>
-      <c r="F32" s="62">
+      <c r="E32" s="66"/>
+      <c r="F32" s="65">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G32" s="64"/>
+      <c r="G32" s="80"/>
       <c r="H32" s="26"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
@@ -6492,22 +6492,22 @@
       <c r="GI32" s="36"/>
     </row>
     <row r="33" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="67"/>
+      <c r="B33" s="82"/>
       <c r="C33" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="62">
+      <c r="D33" s="65">
         <v>0.5</v>
       </c>
-      <c r="E33" s="63"/>
-      <c r="F33" s="62">
+      <c r="E33" s="66"/>
+      <c r="F33" s="65">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G33" s="64"/>
+      <c r="G33" s="80"/>
       <c r="H33" s="26"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
@@ -6696,22 +6696,22 @@
       <c r="GI33" s="36"/>
     </row>
     <row r="34" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A34" s="66" t="s">
+      <c r="A34" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="67"/>
+      <c r="B34" s="82"/>
       <c r="C34" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="62">
+      <c r="D34" s="65">
         <v>0.3</v>
       </c>
-      <c r="E34" s="63"/>
-      <c r="F34" s="62">
+      <c r="E34" s="66"/>
+      <c r="F34" s="65">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G34" s="64"/>
+      <c r="G34" s="80"/>
       <c r="H34" s="26"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
@@ -6900,22 +6900,22 @@
       <c r="GI34" s="36"/>
     </row>
     <row r="35" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A35" s="66" t="s">
+      <c r="A35" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="67"/>
+      <c r="B35" s="82"/>
       <c r="C35" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="62">
+      <c r="D35" s="65">
         <v>0.3</v>
       </c>
-      <c r="E35" s="63"/>
-      <c r="F35" s="62">
+      <c r="E35" s="66"/>
+      <c r="F35" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G35" s="64"/>
+      <c r="G35" s="80"/>
       <c r="H35" s="26"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
@@ -7102,22 +7102,22 @@
       <c r="GI35" s="36"/>
     </row>
     <row r="36" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A36" s="66" t="s">
+      <c r="A36" s="81" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="67"/>
+      <c r="B36" s="82"/>
       <c r="C36" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="62">
+      <c r="D36" s="65">
         <v>1.5</v>
       </c>
-      <c r="E36" s="63"/>
-      <c r="F36" s="62">
+      <c r="E36" s="66"/>
+      <c r="F36" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G36" s="64"/>
+      <c r="G36" s="80"/>
       <c r="H36" s="26"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
@@ -7304,22 +7304,22 @@
       <c r="GI36" s="36"/>
     </row>
     <row r="37" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A37" s="66" t="s">
+      <c r="A37" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="67"/>
+      <c r="B37" s="82"/>
       <c r="C37" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="62">
+      <c r="D37" s="65">
         <v>0.5</v>
       </c>
-      <c r="E37" s="63"/>
-      <c r="F37" s="62">
+      <c r="E37" s="66"/>
+      <c r="F37" s="65">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G37" s="64"/>
+      <c r="G37" s="80"/>
       <c r="H37" s="26"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
@@ -7508,22 +7508,22 @@
       <c r="GI37" s="36"/>
     </row>
     <row r="38" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A38" s="66" t="s">
+      <c r="A38" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="67"/>
+      <c r="B38" s="82"/>
       <c r="C38" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="62">
+      <c r="D38" s="65">
         <v>0.25</v>
       </c>
-      <c r="E38" s="63"/>
-      <c r="F38" s="62">
+      <c r="E38" s="66"/>
+      <c r="F38" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G38" s="64"/>
+      <c r="G38" s="80"/>
       <c r="H38" s="26"/>
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
@@ -7712,22 +7712,22 @@
       <c r="GI38" s="36"/>
     </row>
     <row r="39" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="67"/>
+      <c r="B39" s="82"/>
       <c r="C39" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="62">
+      <c r="D39" s="65">
         <v>0.5</v>
       </c>
-      <c r="E39" s="63"/>
-      <c r="F39" s="62">
+      <c r="E39" s="66"/>
+      <c r="F39" s="65">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="G39" s="64"/>
+      <c r="G39" s="80"/>
       <c r="H39" s="26"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
@@ -7916,22 +7916,22 @@
       <c r="GI39" s="36"/>
     </row>
     <row r="40" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A40" s="66" t="s">
+      <c r="A40" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="67"/>
+      <c r="B40" s="82"/>
       <c r="C40" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="62">
+      <c r="D40" s="65">
         <v>0.5</v>
       </c>
-      <c r="E40" s="63"/>
-      <c r="F40" s="62">
+      <c r="E40" s="66"/>
+      <c r="F40" s="65">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G40" s="64"/>
+      <c r="G40" s="80"/>
       <c r="H40" s="26"/>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
@@ -8120,22 +8120,22 @@
       <c r="GI40" s="36"/>
     </row>
     <row r="41" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="67"/>
+      <c r="B41" s="82"/>
       <c r="C41" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="62">
+      <c r="D41" s="65">
         <v>0.3</v>
       </c>
-      <c r="E41" s="63"/>
-      <c r="F41" s="62">
+      <c r="E41" s="66"/>
+      <c r="F41" s="65">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G41" s="64"/>
+      <c r="G41" s="80"/>
       <c r="H41" s="26"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
@@ -8324,22 +8324,22 @@
       <c r="GI41" s="36"/>
     </row>
     <row r="42" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A42" s="66" t="s">
+      <c r="A42" s="81" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="67"/>
+      <c r="B42" s="82"/>
       <c r="C42" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="62">
+      <c r="D42" s="65">
         <v>0.5</v>
       </c>
-      <c r="E42" s="63"/>
-      <c r="F42" s="62">
+      <c r="E42" s="66"/>
+      <c r="F42" s="65">
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-      <c r="G42" s="64"/>
+      <c r="G42" s="80"/>
       <c r="H42" s="26"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
@@ -8528,22 +8528,22 @@
       <c r="GI42" s="36"/>
     </row>
     <row r="43" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A43" s="66" t="s">
+      <c r="A43" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="67"/>
+      <c r="B43" s="82"/>
       <c r="C43" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D43" s="62">
+      <c r="D43" s="65">
         <v>1.3</v>
       </c>
-      <c r="E43" s="63"/>
-      <c r="F43" s="62">
+      <c r="E43" s="66"/>
+      <c r="F43" s="65">
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
-      <c r="G43" s="64"/>
+      <c r="G43" s="80"/>
       <c r="H43" s="26"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
@@ -8734,22 +8734,22 @@
       <c r="GI43" s="36"/>
     </row>
     <row r="44" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="66" t="s">
+      <c r="A44" s="81" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="67"/>
+      <c r="B44" s="82"/>
       <c r="C44" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="62">
+      <c r="D44" s="65">
         <v>1.3</v>
       </c>
-      <c r="E44" s="63"/>
-      <c r="F44" s="62">
+      <c r="E44" s="66"/>
+      <c r="F44" s="65">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G44" s="64"/>
+      <c r="G44" s="80"/>
       <c r="H44" s="26"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
@@ -8938,22 +8938,22 @@
       <c r="GI44" s="36"/>
     </row>
     <row r="45" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A45" s="66" t="s">
+      <c r="A45" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="67"/>
+      <c r="B45" s="82"/>
       <c r="C45" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="62">
+      <c r="D45" s="65">
         <v>1</v>
       </c>
-      <c r="E45" s="63"/>
-      <c r="F45" s="62">
+      <c r="E45" s="66"/>
+      <c r="F45" s="65">
         <f t="shared" si="0"/>
         <v>1.05</v>
       </c>
-      <c r="G45" s="64"/>
+      <c r="G45" s="80"/>
       <c r="H45" s="26"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
@@ -9144,22 +9144,22 @@
       <c r="GI45" s="36"/>
     </row>
     <row r="46" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A46" s="66" t="s">
+      <c r="A46" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="67"/>
+      <c r="B46" s="82"/>
       <c r="C46" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="D46" s="62">
+      <c r="D46" s="65">
         <v>1</v>
       </c>
-      <c r="E46" s="63"/>
-      <c r="F46" s="62">
+      <c r="E46" s="66"/>
+      <c r="F46" s="65">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="G46" s="64"/>
+      <c r="G46" s="80"/>
       <c r="H46" s="26"/>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
@@ -9348,22 +9348,22 @@
       <c r="GI46" s="36"/>
     </row>
     <row r="47" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A47" s="66" t="s">
+      <c r="A47" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="67"/>
+      <c r="B47" s="82"/>
       <c r="C47" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="D47" s="62">
+      <c r="D47" s="65">
         <v>1</v>
       </c>
-      <c r="E47" s="63"/>
-      <c r="F47" s="62">
+      <c r="E47" s="66"/>
+      <c r="F47" s="65">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="G47" s="64"/>
+      <c r="G47" s="80"/>
       <c r="H47" s="26"/>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
@@ -9552,22 +9552,22 @@
       <c r="GI47" s="36"/>
     </row>
     <row r="48" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A48" s="66" t="s">
+      <c r="A48" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="B48" s="67"/>
+      <c r="B48" s="82"/>
       <c r="C48" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D48" s="62">
+      <c r="D48" s="65">
         <v>0.3</v>
       </c>
-      <c r="E48" s="63"/>
-      <c r="F48" s="62">
+      <c r="E48" s="66"/>
+      <c r="F48" s="65">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G48" s="64"/>
+      <c r="G48" s="80"/>
       <c r="H48" s="26"/>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
@@ -9756,22 +9756,22 @@
       <c r="GI48" s="36"/>
     </row>
     <row r="49" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A49" s="66" t="s">
+      <c r="A49" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="67"/>
+      <c r="B49" s="82"/>
       <c r="C49" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="62">
+      <c r="D49" s="65">
         <v>2</v>
       </c>
-      <c r="E49" s="63"/>
-      <c r="F49" s="62">
+      <c r="E49" s="66"/>
+      <c r="F49" s="65">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G49" s="64"/>
+      <c r="G49" s="80"/>
       <c r="H49" s="26"/>
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
@@ -9962,22 +9962,22 @@
       <c r="GI49" s="36"/>
     </row>
     <row r="50" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A50" s="66" t="s">
+      <c r="A50" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="67"/>
+      <c r="B50" s="82"/>
       <c r="C50" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="D50" s="62">
+      <c r="D50" s="65">
         <v>2</v>
       </c>
-      <c r="E50" s="63"/>
-      <c r="F50" s="62">
+      <c r="E50" s="66"/>
+      <c r="F50" s="65">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G50" s="64"/>
+      <c r="G50" s="80"/>
       <c r="H50" s="26"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
@@ -10168,22 +10168,22 @@
       <c r="GI50" s="36"/>
     </row>
     <row r="51" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A51" s="66" t="s">
+      <c r="A51" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="67"/>
+      <c r="B51" s="82"/>
       <c r="C51" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D51" s="62">
+      <c r="D51" s="65">
         <v>2</v>
       </c>
-      <c r="E51" s="63"/>
-      <c r="F51" s="62">
+      <c r="E51" s="66"/>
+      <c r="F51" s="65">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G51" s="64"/>
+      <c r="G51" s="80"/>
       <c r="H51" s="26"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
@@ -10374,22 +10374,22 @@
       <c r="GI51" s="36"/>
     </row>
     <row r="52" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A52" s="66" t="s">
+      <c r="A52" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="67"/>
+      <c r="B52" s="82"/>
       <c r="C52" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="62">
+      <c r="D52" s="65">
         <v>2</v>
       </c>
-      <c r="E52" s="63"/>
-      <c r="F52" s="62">
+      <c r="E52" s="66"/>
+      <c r="F52" s="65">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G52" s="64"/>
+      <c r="G52" s="80"/>
       <c r="H52" s="26"/>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
@@ -10580,22 +10580,22 @@
       <c r="GI52" s="36"/>
     </row>
     <row r="53" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A53" s="66" t="s">
+      <c r="A53" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="67"/>
+      <c r="B53" s="82"/>
       <c r="C53" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D53" s="62">
+      <c r="D53" s="65">
         <v>2</v>
       </c>
-      <c r="E53" s="63"/>
-      <c r="F53" s="62">
+      <c r="E53" s="66"/>
+      <c r="F53" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G53" s="64"/>
+      <c r="G53" s="80"/>
       <c r="H53" s="26"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
@@ -10782,22 +10782,22 @@
       <c r="GI53" s="36"/>
     </row>
     <row r="54" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A54" s="66" t="s">
+      <c r="A54" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="67"/>
+      <c r="B54" s="82"/>
       <c r="C54" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="D54" s="62">
+      <c r="D54" s="65">
         <v>0.25</v>
       </c>
-      <c r="E54" s="63"/>
-      <c r="F54" s="62">
+      <c r="E54" s="66"/>
+      <c r="F54" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G54" s="64"/>
+      <c r="G54" s="80"/>
       <c r="H54" s="26"/>
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
@@ -10984,22 +10984,22 @@
       <c r="GI54" s="36"/>
     </row>
     <row r="55" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A55" s="66" t="s">
+      <c r="A55" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="67"/>
+      <c r="B55" s="82"/>
       <c r="C55" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="D55" s="62">
+      <c r="D55" s="65">
         <v>1</v>
       </c>
-      <c r="E55" s="63"/>
-      <c r="F55" s="62">
+      <c r="E55" s="66"/>
+      <c r="F55" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G55" s="64"/>
+      <c r="G55" s="80"/>
       <c r="H55" s="26"/>
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
@@ -11186,22 +11186,22 @@
       <c r="GI55" s="36"/>
     </row>
     <row r="56" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A56" s="66" t="s">
+      <c r="A56" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="67"/>
+      <c r="B56" s="82"/>
       <c r="C56" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="D56" s="62">
+      <c r="D56" s="65">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E56" s="63"/>
-      <c r="F56" s="62">
+      <c r="E56" s="66"/>
+      <c r="F56" s="65">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G56" s="64"/>
+      <c r="G56" s="80"/>
       <c r="H56" s="26"/>
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
@@ -11392,22 +11392,22 @@
       <c r="GI56" s="36"/>
     </row>
     <row r="57" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A57" s="66" t="s">
+      <c r="A57" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="67"/>
+      <c r="B57" s="82"/>
       <c r="C57" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="D57" s="62">
+      <c r="D57" s="65">
         <v>1.75</v>
       </c>
-      <c r="E57" s="63"/>
-      <c r="F57" s="62">
+      <c r="E57" s="66"/>
+      <c r="F57" s="65">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G57" s="64"/>
+      <c r="G57" s="80"/>
       <c r="H57" s="26"/>
       <c r="I57" s="12"/>
       <c r="J57" s="12"/>
@@ -11596,22 +11596,22 @@
       <c r="GI57" s="36"/>
     </row>
     <row r="58" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A58" s="66" t="s">
+      <c r="A58" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="B58" s="67"/>
+      <c r="B58" s="82"/>
       <c r="C58" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="D58" s="62">
+      <c r="D58" s="65">
         <v>0.6</v>
       </c>
-      <c r="E58" s="63"/>
-      <c r="F58" s="62">
+      <c r="E58" s="66"/>
+      <c r="F58" s="65">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G58" s="64"/>
+      <c r="G58" s="80"/>
       <c r="H58" s="26"/>
       <c r="I58" s="12"/>
       <c r="J58" s="12"/>
@@ -11800,22 +11800,22 @@
       <c r="GI58" s="36"/>
     </row>
     <row r="59" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="66" t="s">
+      <c r="A59" s="81" t="s">
         <v>111</v>
       </c>
-      <c r="B59" s="67"/>
+      <c r="B59" s="82"/>
       <c r="C59" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="62">
+      <c r="D59" s="65">
         <v>1</v>
       </c>
-      <c r="E59" s="63"/>
-      <c r="F59" s="62">
+      <c r="E59" s="66"/>
+      <c r="F59" s="65">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G59" s="64"/>
+        <v>1.5</v>
+      </c>
+      <c r="G59" s="80"/>
       <c r="H59" s="26"/>
       <c r="I59" s="12"/>
       <c r="J59" s="12"/>
@@ -11859,9 +11859,13 @@
       <c r="AV59" s="51"/>
       <c r="AW59" s="51"/>
       <c r="AX59" s="32"/>
-      <c r="AY59" s="32"/>
+      <c r="AY59" s="24">
+        <v>1</v>
+      </c>
       <c r="AZ59" s="32"/>
-      <c r="BA59" s="32"/>
+      <c r="BA59" s="24">
+        <v>0.5</v>
+      </c>
       <c r="BB59" s="49"/>
       <c r="BC59" s="52"/>
       <c r="BD59" s="51"/>
@@ -12002,22 +12006,22 @@
       <c r="GI59" s="36"/>
     </row>
     <row r="60" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A60" s="66" t="s">
+      <c r="A60" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="B60" s="67"/>
+      <c r="B60" s="82"/>
       <c r="C60" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="D60" s="62">
+      <c r="D60" s="65">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E60" s="63"/>
-      <c r="F60" s="62">
+      <c r="E60" s="66"/>
+      <c r="F60" s="65">
         <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
-      <c r="G60" s="64"/>
+      <c r="G60" s="80"/>
       <c r="H60" s="26"/>
       <c r="I60" s="12"/>
       <c r="J60" s="12"/>
@@ -12206,22 +12210,22 @@
       <c r="GI60" s="36"/>
     </row>
     <row r="61" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A61" s="66" t="s">
+      <c r="A61" s="81" t="s">
         <v>115</v>
       </c>
-      <c r="B61" s="67"/>
+      <c r="B61" s="82"/>
       <c r="C61" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="D61" s="62">
+      <c r="D61" s="65">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E61" s="63"/>
-      <c r="F61" s="62">
+      <c r="E61" s="66"/>
+      <c r="F61" s="65">
         <f>SUM(H61:GI61)</f>
         <v>1</v>
       </c>
-      <c r="G61" s="64"/>
+      <c r="G61" s="80"/>
       <c r="H61" s="26"/>
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
@@ -12410,21 +12414,21 @@
       <c r="GI61" s="36"/>
     </row>
     <row r="62" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A62" s="76" t="s">
+      <c r="A62" s="115" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="77"/>
+      <c r="B62" s="116"/>
       <c r="C62" s="39"/>
-      <c r="D62" s="78">
+      <c r="D62" s="71">
         <f>SUM(D63:E80)</f>
         <v>88.6</v>
       </c>
-      <c r="E62" s="79"/>
-      <c r="F62" s="78">
+      <c r="E62" s="117"/>
+      <c r="F62" s="71">
         <f>SUM(F63:G80)</f>
         <v>0</v>
       </c>
-      <c r="G62" s="80"/>
+      <c r="G62" s="75"/>
       <c r="H62" s="29"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
@@ -12611,22 +12615,22 @@
       <c r="GI62" s="29"/>
     </row>
     <row r="63" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="60" t="s">
+      <c r="A63" s="118" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="61"/>
+      <c r="B63" s="119"/>
       <c r="C63" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D63" s="62">
+      <c r="D63" s="65">
         <v>0.6</v>
       </c>
-      <c r="E63" s="63"/>
-      <c r="F63" s="62">
+      <c r="E63" s="66"/>
+      <c r="F63" s="65">
         <f>SUM(H63:GI63)</f>
         <v>0</v>
       </c>
-      <c r="G63" s="64"/>
+      <c r="G63" s="80"/>
       <c r="H63" s="47"/>
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
@@ -12813,22 +12817,22 @@
       <c r="GI63" s="32"/>
     </row>
     <row r="64" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="60" t="s">
+      <c r="A64" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="B64" s="61"/>
+      <c r="B64" s="119"/>
       <c r="C64" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D64" s="62">
+      <c r="D64" s="65">
         <v>1.5</v>
       </c>
-      <c r="E64" s="63"/>
-      <c r="F64" s="62">
+      <c r="E64" s="66"/>
+      <c r="F64" s="65">
         <f>SUM(H64:GI64)</f>
         <v>0</v>
       </c>
-      <c r="G64" s="64"/>
+      <c r="G64" s="80"/>
       <c r="H64" s="47"/>
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
@@ -13015,22 +13019,22 @@
       <c r="GI64" s="32"/>
     </row>
     <row r="65" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A65" s="60" t="s">
+      <c r="A65" s="118" t="s">
         <v>123</v>
       </c>
-      <c r="B65" s="61"/>
+      <c r="B65" s="119"/>
       <c r="C65" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D65" s="62">
+      <c r="D65" s="65">
         <v>1</v>
       </c>
-      <c r="E65" s="63"/>
-      <c r="F65" s="62">
+      <c r="E65" s="66"/>
+      <c r="F65" s="65">
         <f t="shared" ref="F65:F80" si="1">SUM(H65:GI65)</f>
         <v>0</v>
       </c>
-      <c r="G65" s="64"/>
+      <c r="G65" s="80"/>
       <c r="H65" s="47"/>
       <c r="I65" s="12"/>
       <c r="J65" s="12"/>
@@ -13217,22 +13221,22 @@
       <c r="GI65" s="32"/>
     </row>
     <row r="66" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A66" s="60" t="s">
+      <c r="A66" s="118" t="s">
         <v>125</v>
       </c>
-      <c r="B66" s="61"/>
+      <c r="B66" s="119"/>
       <c r="C66" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D66" s="62">
+      <c r="D66" s="65">
         <v>0.5</v>
       </c>
-      <c r="E66" s="63"/>
-      <c r="F66" s="62">
+      <c r="E66" s="66"/>
+      <c r="F66" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G66" s="64"/>
+      <c r="G66" s="80"/>
       <c r="H66" s="47"/>
       <c r="I66" s="12"/>
       <c r="J66" s="12"/>
@@ -13419,22 +13423,22 @@
       <c r="GI66" s="32"/>
     </row>
     <row r="67" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A67" s="60" t="s">
+      <c r="A67" s="118" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="61"/>
+      <c r="B67" s="119"/>
       <c r="C67" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D67" s="62">
+      <c r="D67" s="65">
         <v>1</v>
       </c>
-      <c r="E67" s="63"/>
-      <c r="F67" s="62">
+      <c r="E67" s="66"/>
+      <c r="F67" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G67" s="64"/>
+      <c r="G67" s="80"/>
       <c r="H67" s="47"/>
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
@@ -13621,22 +13625,22 @@
       <c r="GI67" s="32"/>
     </row>
     <row r="68" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A68" s="60" t="s">
+      <c r="A68" s="118" t="s">
         <v>129</v>
       </c>
-      <c r="B68" s="61"/>
+      <c r="B68" s="119"/>
       <c r="C68" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D68" s="62">
+      <c r="D68" s="65">
         <v>1</v>
       </c>
-      <c r="E68" s="63"/>
-      <c r="F68" s="62">
+      <c r="E68" s="66"/>
+      <c r="F68" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G68" s="64"/>
+      <c r="G68" s="80"/>
       <c r="H68" s="47"/>
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
@@ -13823,22 +13827,22 @@
       <c r="GI68" s="32"/>
     </row>
     <row r="69" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A69" s="60" t="s">
+      <c r="A69" s="118" t="s">
         <v>131</v>
       </c>
-      <c r="B69" s="61"/>
+      <c r="B69" s="119"/>
       <c r="C69" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="D69" s="62">
+      <c r="D69" s="65">
         <v>4</v>
       </c>
-      <c r="E69" s="63"/>
-      <c r="F69" s="62">
+      <c r="E69" s="66"/>
+      <c r="F69" s="65">
         <f>SUM(H69:GI69)</f>
         <v>0</v>
       </c>
-      <c r="G69" s="64"/>
+      <c r="G69" s="80"/>
       <c r="H69" s="47"/>
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
@@ -14025,22 +14029,22 @@
       <c r="GI69" s="32"/>
     </row>
     <row r="70" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A70" s="60" t="s">
+      <c r="A70" s="118" t="s">
         <v>133</v>
       </c>
-      <c r="B70" s="61"/>
+      <c r="B70" s="119"/>
       <c r="C70" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="D70" s="62">
+      <c r="D70" s="65">
         <v>8</v>
       </c>
-      <c r="E70" s="63"/>
-      <c r="F70" s="62">
+      <c r="E70" s="66"/>
+      <c r="F70" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G70" s="64"/>
+      <c r="G70" s="80"/>
       <c r="H70" s="47"/>
       <c r="I70" s="12"/>
       <c r="J70" s="12"/>
@@ -14227,22 +14231,22 @@
       <c r="GI70" s="32"/>
     </row>
     <row r="71" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A71" s="60" t="s">
+      <c r="A71" s="118" t="s">
         <v>135</v>
       </c>
-      <c r="B71" s="61"/>
+      <c r="B71" s="119"/>
       <c r="C71" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="D71" s="62">
+      <c r="D71" s="65">
         <v>1</v>
       </c>
-      <c r="E71" s="63"/>
-      <c r="F71" s="62">
+      <c r="E71" s="66"/>
+      <c r="F71" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G71" s="64"/>
+      <c r="G71" s="80"/>
       <c r="H71" s="47"/>
       <c r="I71" s="12"/>
       <c r="J71" s="12"/>
@@ -14429,22 +14433,22 @@
       <c r="GI71" s="32"/>
     </row>
     <row r="72" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A72" s="60" t="s">
+      <c r="A72" s="118" t="s">
         <v>137</v>
       </c>
-      <c r="B72" s="61"/>
+      <c r="B72" s="119"/>
       <c r="C72" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="D72" s="62">
+      <c r="D72" s="65">
         <v>1</v>
       </c>
-      <c r="E72" s="63"/>
-      <c r="F72" s="62">
+      <c r="E72" s="66"/>
+      <c r="F72" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G72" s="64"/>
+      <c r="G72" s="80"/>
       <c r="H72" s="47"/>
       <c r="I72" s="12"/>
       <c r="J72" s="12"/>
@@ -14631,22 +14635,22 @@
       <c r="GI72" s="32"/>
     </row>
     <row r="73" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A73" s="60" t="s">
+      <c r="A73" s="118" t="s">
         <v>47</v>
       </c>
-      <c r="B73" s="61"/>
+      <c r="B73" s="119"/>
       <c r="C73" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="D73" s="62">
+      <c r="D73" s="65">
         <v>4</v>
       </c>
-      <c r="E73" s="63"/>
-      <c r="F73" s="62">
+      <c r="E73" s="66"/>
+      <c r="F73" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G73" s="64"/>
+      <c r="G73" s="80"/>
       <c r="H73" s="47"/>
       <c r="I73" s="12"/>
       <c r="J73" s="12"/>
@@ -14833,22 +14837,22 @@
       <c r="GI73" s="32"/>
     </row>
     <row r="74" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A74" s="60" t="s">
+      <c r="A74" s="118" t="s">
         <v>140</v>
       </c>
-      <c r="B74" s="61"/>
+      <c r="B74" s="119"/>
       <c r="C74" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="D74" s="62">
+      <c r="D74" s="65">
         <v>12</v>
       </c>
-      <c r="E74" s="63"/>
-      <c r="F74" s="62">
+      <c r="E74" s="66"/>
+      <c r="F74" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G74" s="64"/>
+      <c r="G74" s="80"/>
       <c r="H74" s="47"/>
       <c r="I74" s="12"/>
       <c r="J74" s="12"/>
@@ -15035,22 +15039,22 @@
       <c r="GI74" s="32"/>
     </row>
     <row r="75" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A75" s="60" t="s">
+      <c r="A75" s="118" t="s">
         <v>142</v>
       </c>
-      <c r="B75" s="65"/>
+      <c r="B75" s="88"/>
       <c r="C75" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D75" s="62">
+      <c r="D75" s="65">
         <v>16</v>
       </c>
-      <c r="E75" s="63"/>
-      <c r="F75" s="62">
+      <c r="E75" s="66"/>
+      <c r="F75" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G75" s="64"/>
+      <c r="G75" s="80"/>
       <c r="H75" s="47"/>
       <c r="I75" s="12"/>
       <c r="J75" s="12"/>
@@ -15237,22 +15241,22 @@
       <c r="GI75" s="36"/>
     </row>
     <row r="76" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A76" s="60" t="s">
+      <c r="A76" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B76" s="61"/>
+      <c r="B76" s="119"/>
       <c r="C76" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="D76" s="62">
+      <c r="D76" s="65">
         <v>5</v>
       </c>
-      <c r="E76" s="63"/>
-      <c r="F76" s="62">
+      <c r="E76" s="66"/>
+      <c r="F76" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G76" s="64"/>
+      <c r="G76" s="80"/>
       <c r="H76" s="47"/>
       <c r="I76" s="12"/>
       <c r="J76" s="12"/>
@@ -15439,22 +15443,22 @@
       <c r="GI76" s="32"/>
     </row>
     <row r="77" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A77" s="60" t="s">
+      <c r="A77" s="118" t="s">
         <v>146</v>
       </c>
-      <c r="B77" s="61"/>
+      <c r="B77" s="119"/>
       <c r="C77" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="D77" s="62">
+      <c r="D77" s="65">
         <v>4</v>
       </c>
-      <c r="E77" s="63"/>
-      <c r="F77" s="62">
+      <c r="E77" s="66"/>
+      <c r="F77" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G77" s="64"/>
+      <c r="G77" s="80"/>
       <c r="H77" s="47"/>
       <c r="I77" s="12"/>
       <c r="J77" s="12"/>
@@ -15641,22 +15645,22 @@
       <c r="GI77" s="32"/>
     </row>
     <row r="78" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A78" s="60" t="s">
+      <c r="A78" s="118" t="s">
         <v>148</v>
       </c>
-      <c r="B78" s="61"/>
+      <c r="B78" s="119"/>
       <c r="C78" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="D78" s="62">
+      <c r="D78" s="65">
         <v>16</v>
       </c>
-      <c r="E78" s="63"/>
-      <c r="F78" s="62">
+      <c r="E78" s="66"/>
+      <c r="F78" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G78" s="64"/>
+      <c r="G78" s="80"/>
       <c r="H78" s="47"/>
       <c r="I78" s="12"/>
       <c r="J78" s="12"/>
@@ -15843,22 +15847,22 @@
       <c r="GI78" s="32"/>
     </row>
     <row r="79" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A79" s="82" t="s">
+      <c r="A79" s="73" t="s">
         <v>150</v>
       </c>
-      <c r="B79" s="83"/>
+      <c r="B79" s="74"/>
       <c r="C79" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="D79" s="62">
+      <c r="D79" s="65">
         <v>6</v>
       </c>
-      <c r="E79" s="63"/>
-      <c r="F79" s="62">
+      <c r="E79" s="66"/>
+      <c r="F79" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G79" s="64"/>
+      <c r="G79" s="80"/>
       <c r="H79" s="47"/>
       <c r="I79" s="12"/>
       <c r="J79" s="12"/>
@@ -16045,22 +16049,22 @@
       <c r="GI79" s="36"/>
     </row>
     <row r="80" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A80" s="82" t="s">
+      <c r="A80" s="73" t="s">
         <v>152</v>
       </c>
-      <c r="B80" s="83"/>
+      <c r="B80" s="74"/>
       <c r="C80" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D80" s="62">
+      <c r="D80" s="65">
         <v>6</v>
       </c>
-      <c r="E80" s="63"/>
-      <c r="F80" s="62">
+      <c r="E80" s="66"/>
+      <c r="F80" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G80" s="64"/>
+      <c r="G80" s="80"/>
       <c r="H80" s="47"/>
       <c r="I80" s="12"/>
       <c r="J80" s="12"/>
@@ -16247,21 +16251,21 @@
       <c r="GI80" s="36"/>
     </row>
     <row r="81" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A81" s="76" t="s">
+      <c r="A81" s="115" t="s">
         <v>153</v>
       </c>
-      <c r="B81" s="77"/>
+      <c r="B81" s="116"/>
       <c r="C81" s="39"/>
-      <c r="D81" s="78">
+      <c r="D81" s="71">
         <f>SUM(D82:E82)</f>
         <v>16</v>
       </c>
-      <c r="E81" s="88"/>
-      <c r="F81" s="78">
+      <c r="E81" s="72"/>
+      <c r="F81" s="71">
         <f>SUM(F82:G82)</f>
         <v>0</v>
       </c>
-      <c r="G81" s="80"/>
+      <c r="G81" s="75"/>
       <c r="H81" s="29"/>
       <c r="I81" s="8"/>
       <c r="J81" s="8"/>
@@ -16448,20 +16452,20 @@
       <c r="GI81" s="29"/>
     </row>
     <row r="82" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A82" s="86" t="s">
+      <c r="A82" s="93" t="s">
         <v>153</v>
       </c>
-      <c r="B82" s="87"/>
+      <c r="B82" s="94"/>
       <c r="C82" s="40"/>
-      <c r="D82" s="84">
+      <c r="D82" s="91">
         <v>16</v>
       </c>
-      <c r="E82" s="85"/>
-      <c r="F82" s="62">
+      <c r="E82" s="92"/>
+      <c r="F82" s="65">
         <f>SUM(H82:GI82)</f>
         <v>0</v>
       </c>
-      <c r="G82" s="64"/>
+      <c r="G82" s="80"/>
       <c r="H82" s="26"/>
       <c r="I82" s="12"/>
       <c r="J82" s="12"/>
@@ -16648,21 +16652,21 @@
       <c r="GI82" s="32"/>
     </row>
     <row r="83" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A83" s="104" t="s">
+      <c r="A83" s="110" t="s">
         <v>154</v>
       </c>
-      <c r="B83" s="105"/>
+      <c r="B83" s="111"/>
       <c r="C83" s="41"/>
-      <c r="D83" s="78">
+      <c r="D83" s="71">
         <f>SUM(D84:E84)</f>
         <v>32</v>
       </c>
-      <c r="E83" s="88"/>
-      <c r="F83" s="78">
+      <c r="E83" s="72"/>
+      <c r="F83" s="71">
         <f>SUM(F84:G84)</f>
         <v>0</v>
       </c>
-      <c r="G83" s="80"/>
+      <c r="G83" s="75"/>
       <c r="H83" s="29"/>
       <c r="I83" s="8"/>
       <c r="J83" s="8"/>
@@ -16849,20 +16853,20 @@
       <c r="GI83" s="29"/>
     </row>
     <row r="84" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A84" s="108" t="s">
+      <c r="A84" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="B84" s="109"/>
+      <c r="B84" s="86"/>
       <c r="C84" s="42"/>
-      <c r="D84" s="62">
+      <c r="D84" s="65">
         <v>32</v>
       </c>
-      <c r="E84" s="63"/>
-      <c r="F84" s="62">
+      <c r="E84" s="66"/>
+      <c r="F84" s="65">
         <f>SUM(H84:GI84)</f>
         <v>0</v>
       </c>
-      <c r="G84" s="64"/>
+      <c r="G84" s="80"/>
       <c r="H84" s="26"/>
       <c r="I84" s="12"/>
       <c r="J84" s="12"/>
@@ -17049,21 +17053,21 @@
       <c r="GI84" s="32"/>
     </row>
     <row r="85" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A85" s="111" t="s">
+      <c r="A85" s="89" t="s">
         <v>155</v>
       </c>
-      <c r="B85" s="112"/>
+      <c r="B85" s="90"/>
       <c r="C85" s="43"/>
-      <c r="D85" s="78">
+      <c r="D85" s="71">
         <f>SUM(D86:E86)</f>
         <v>8</v>
       </c>
-      <c r="E85" s="88"/>
-      <c r="F85" s="89">
+      <c r="E85" s="72"/>
+      <c r="F85" s="95">
         <f>SUM(F86:G86)</f>
         <v>0</v>
       </c>
-      <c r="G85" s="90"/>
+      <c r="G85" s="96"/>
       <c r="H85" s="29"/>
       <c r="I85" s="8"/>
       <c r="J85" s="8"/>
@@ -17250,20 +17254,20 @@
       <c r="GI85" s="29"/>
     </row>
     <row r="86" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A86" s="110" t="s">
+      <c r="A86" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="B86" s="65"/>
+      <c r="B86" s="88"/>
       <c r="C86" s="27"/>
-      <c r="D86" s="62">
+      <c r="D86" s="65">
         <v>8</v>
       </c>
-      <c r="E86" s="63"/>
-      <c r="F86" s="62">
+      <c r="E86" s="66"/>
+      <c r="F86" s="65">
         <f>SUM(H86:GI86)</f>
         <v>0</v>
       </c>
-      <c r="G86" s="64"/>
+      <c r="G86" s="80"/>
       <c r="H86" s="26"/>
       <c r="I86" s="12"/>
       <c r="J86" s="12"/>
@@ -17450,20 +17454,20 @@
       <c r="GI86" s="32"/>
     </row>
     <row r="87" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A87" s="106" t="s">
+      <c r="A87" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="107"/>
+      <c r="B87" s="84"/>
       <c r="C87" s="43"/>
-      <c r="D87" s="78">
+      <c r="D87" s="71">
         <f>232-D90</f>
         <v>36.349999999999994</v>
       </c>
-      <c r="E87" s="88"/>
-      <c r="F87" s="78">
+      <c r="E87" s="72"/>
+      <c r="F87" s="71">
         <v>0</v>
       </c>
-      <c r="G87" s="80"/>
+      <c r="G87" s="75"/>
       <c r="H87" s="29"/>
       <c r="I87" s="8"/>
       <c r="J87" s="8"/>
@@ -17650,15 +17654,15 @@
       <c r="GI87" s="29"/>
     </row>
     <row r="88" spans="1:191" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="101" t="s">
+      <c r="A88" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="B88" s="102"/>
+      <c r="B88" s="108"/>
       <c r="C88" s="44"/>
-      <c r="D88" s="98"/>
-      <c r="E88" s="99"/>
-      <c r="F88" s="98"/>
-      <c r="G88" s="100"/>
+      <c r="D88" s="104"/>
+      <c r="E88" s="105"/>
+      <c r="F88" s="104"/>
+      <c r="G88" s="106"/>
       <c r="H88" s="28"/>
       <c r="I88" s="17"/>
       <c r="J88" s="17"/>
@@ -17897,21 +17901,21 @@
       <c r="AX89" s="3"/>
     </row>
     <row r="90" spans="1:191" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="96" t="s">
+      <c r="A90" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="97"/>
+      <c r="B90" s="103"/>
       <c r="C90" s="45"/>
-      <c r="D90" s="94">
+      <c r="D90" s="100">
         <f>SUM(D85,D83,D81,D62,D14)</f>
         <v>195.65</v>
       </c>
-      <c r="E90" s="95"/>
-      <c r="F90" s="94">
+      <c r="E90" s="101"/>
+      <c r="F90" s="100">
         <f>SUM(F85,F83,F81,F62,F14)</f>
-        <v>40.625999999999998</v>
-      </c>
-      <c r="G90" s="103"/>
+        <v>42.125999999999998</v>
+      </c>
+      <c r="G90" s="109"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
@@ -17958,6 +17962,316 @@
     </row>
   </sheetData>
   <mergeCells count="334">
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="GD13:GE13"/>
+    <mergeCell ref="GF13:GG13"/>
+    <mergeCell ref="GH13:GI13"/>
+    <mergeCell ref="DZ12:GI12"/>
+    <mergeCell ref="FL13:FM13"/>
+    <mergeCell ref="FN13:FO13"/>
+    <mergeCell ref="FP13:FQ13"/>
+    <mergeCell ref="FR13:FS13"/>
+    <mergeCell ref="FT13:FU13"/>
+    <mergeCell ref="FV13:FW13"/>
+    <mergeCell ref="FX13:FY13"/>
+    <mergeCell ref="FZ13:GA13"/>
+    <mergeCell ref="GB13:GC13"/>
+    <mergeCell ref="ET13:EU13"/>
+    <mergeCell ref="EV13:EW13"/>
+    <mergeCell ref="EX13:EY13"/>
+    <mergeCell ref="EZ13:FA13"/>
+    <mergeCell ref="FB13:FC13"/>
+    <mergeCell ref="FD13:FE13"/>
+    <mergeCell ref="FF13:FG13"/>
+    <mergeCell ref="DX13:DY13"/>
+    <mergeCell ref="FH13:FI13"/>
+    <mergeCell ref="FJ13:FK13"/>
+    <mergeCell ref="EB13:EC13"/>
+    <mergeCell ref="ED13:EE13"/>
+    <mergeCell ref="EF13:EG13"/>
+    <mergeCell ref="EH13:EI13"/>
+    <mergeCell ref="EJ13:EK13"/>
+    <mergeCell ref="EL13:EM13"/>
+    <mergeCell ref="EN13:EO13"/>
+    <mergeCell ref="EP13:EQ13"/>
+    <mergeCell ref="ER13:ES13"/>
+    <mergeCell ref="DF13:DG13"/>
+    <mergeCell ref="DH13:DI13"/>
+    <mergeCell ref="DJ13:DK13"/>
+    <mergeCell ref="DL13:DM13"/>
+    <mergeCell ref="DN13:DO13"/>
+    <mergeCell ref="DP13:DQ13"/>
+    <mergeCell ref="DR13:DS13"/>
+    <mergeCell ref="DT13:DU13"/>
+    <mergeCell ref="DV13:DW13"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="BH13:BI13"/>
+    <mergeCell ref="BJ13:BK13"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="P9:X9"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F11:G13"/>
+    <mergeCell ref="D11:E13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="AL13:AM13"/>
+    <mergeCell ref="AN13:AO13"/>
+    <mergeCell ref="AP13:AQ13"/>
+    <mergeCell ref="AR13:AS13"/>
+    <mergeCell ref="AT13:AU13"/>
+    <mergeCell ref="AV13:AW13"/>
+    <mergeCell ref="AX13:AY13"/>
+    <mergeCell ref="AZ13:BA13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="P6:X6"/>
+    <mergeCell ref="P5:X5"/>
+    <mergeCell ref="P4:X4"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="H12:BQ12"/>
+    <mergeCell ref="BB13:BC13"/>
+    <mergeCell ref="BD13:BE13"/>
+    <mergeCell ref="BF13:BG13"/>
+    <mergeCell ref="BP13:BQ13"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="AF13:AG13"/>
+    <mergeCell ref="AH13:AI13"/>
+    <mergeCell ref="AJ13:AK13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
     <mergeCell ref="BR13:BS13"/>
     <mergeCell ref="BL13:BM13"/>
     <mergeCell ref="BN13:BO13"/>
@@ -17982,316 +18296,6 @@
     <mergeCell ref="CZ13:DA13"/>
     <mergeCell ref="DB13:DC13"/>
     <mergeCell ref="DD13:DE13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="P6:X6"/>
-    <mergeCell ref="P5:X5"/>
-    <mergeCell ref="P4:X4"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="H12:BQ12"/>
-    <mergeCell ref="BB13:BC13"/>
-    <mergeCell ref="BD13:BE13"/>
-    <mergeCell ref="BF13:BG13"/>
-    <mergeCell ref="BP13:BQ13"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="AF13:AG13"/>
-    <mergeCell ref="AH13:AI13"/>
-    <mergeCell ref="AJ13:AK13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="AL13:AM13"/>
-    <mergeCell ref="AN13:AO13"/>
-    <mergeCell ref="AP13:AQ13"/>
-    <mergeCell ref="AR13:AS13"/>
-    <mergeCell ref="AT13:AU13"/>
-    <mergeCell ref="AV13:AW13"/>
-    <mergeCell ref="AX13:AY13"/>
-    <mergeCell ref="AZ13:BA13"/>
-    <mergeCell ref="BH13:BI13"/>
-    <mergeCell ref="BJ13:BK13"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="P9:X9"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F11:G13"/>
-    <mergeCell ref="D11:E13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="F90:G90"/>
-    <mergeCell ref="F87:G87"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="DF13:DG13"/>
-    <mergeCell ref="DH13:DI13"/>
-    <mergeCell ref="DJ13:DK13"/>
-    <mergeCell ref="DL13:DM13"/>
-    <mergeCell ref="DN13:DO13"/>
-    <mergeCell ref="DP13:DQ13"/>
-    <mergeCell ref="DR13:DS13"/>
-    <mergeCell ref="DT13:DU13"/>
-    <mergeCell ref="DV13:DW13"/>
-    <mergeCell ref="FF13:FG13"/>
-    <mergeCell ref="DX13:DY13"/>
-    <mergeCell ref="FH13:FI13"/>
-    <mergeCell ref="FJ13:FK13"/>
-    <mergeCell ref="EB13:EC13"/>
-    <mergeCell ref="ED13:EE13"/>
-    <mergeCell ref="EF13:EG13"/>
-    <mergeCell ref="EH13:EI13"/>
-    <mergeCell ref="EJ13:EK13"/>
-    <mergeCell ref="EL13:EM13"/>
-    <mergeCell ref="EN13:EO13"/>
-    <mergeCell ref="EP13:EQ13"/>
-    <mergeCell ref="ER13:ES13"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="GD13:GE13"/>
-    <mergeCell ref="GF13:GG13"/>
-    <mergeCell ref="GH13:GI13"/>
-    <mergeCell ref="DZ12:GI12"/>
-    <mergeCell ref="FL13:FM13"/>
-    <mergeCell ref="FN13:FO13"/>
-    <mergeCell ref="FP13:FQ13"/>
-    <mergeCell ref="FR13:FS13"/>
-    <mergeCell ref="FT13:FU13"/>
-    <mergeCell ref="FV13:FW13"/>
-    <mergeCell ref="FX13:FY13"/>
-    <mergeCell ref="FZ13:GA13"/>
-    <mergeCell ref="GB13:GC13"/>
-    <mergeCell ref="ET13:EU13"/>
-    <mergeCell ref="EV13:EW13"/>
-    <mergeCell ref="EX13:EY13"/>
-    <mergeCell ref="EZ13:FA13"/>
-    <mergeCell ref="FB13:FC13"/>
-    <mergeCell ref="FD13:FE13"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Created Models for Issue #54
</commit_message>
<xml_diff>
--- a/Documents/Zeitplan.xlsx
+++ b/Documents/Zeitplan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VirtualReality\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VirtualReality\Documents\SiemensVR\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1164,6 +1164,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1176,32 +1194,31 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1209,42 +1226,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1253,6 +1234,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1300,24 +1284,40 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1787,8 +1787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GI90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="BA59" sqref="BA59"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BA20" sqref="BA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1799,28 +1799,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:191" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="112"/>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="112"/>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
     </row>
     <row r="2" spans="1:191" x14ac:dyDescent="0.25">
       <c r="T2" s="9"/>
@@ -1853,17 +1853,17 @@
         <v>160</v>
       </c>
       <c r="N4" s="57"/>
-      <c r="P4" s="67" t="s">
+      <c r="P4" s="81" t="s">
         <v>157</v>
       </c>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="67"/>
-      <c r="W4" s="67"/>
-      <c r="X4" s="67"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="81"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
     </row>
     <row r="5" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -1880,17 +1880,17 @@
       <c r="F5" s="5"/>
       <c r="G5" s="7"/>
       <c r="N5" s="24"/>
-      <c r="P5" s="67" t="s">
+      <c r="P5" s="81" t="s">
         <v>158</v>
       </c>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="67"/>
-      <c r="S5" s="67"/>
-      <c r="T5" s="67"/>
-      <c r="U5" s="67"/>
-      <c r="V5" s="67"/>
-      <c r="W5" s="67"/>
-      <c r="X5" s="67"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="81"/>
+      <c r="S5" s="81"/>
+      <c r="T5" s="81"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
+      <c r="W5" s="81"/>
+      <c r="X5" s="81"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
@@ -1914,17 +1914,17 @@
         <v>15</v>
       </c>
       <c r="N6" s="16"/>
-      <c r="P6" s="67" t="s">
+      <c r="P6" s="81" t="s">
         <v>159</v>
       </c>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="67"/>
-      <c r="V6" s="67"/>
-      <c r="W6" s="67"/>
-      <c r="X6" s="67"/>
+      <c r="Q6" s="81"/>
+      <c r="R6" s="81"/>
+      <c r="S6" s="81"/>
+      <c r="T6" s="81"/>
+      <c r="U6" s="81"/>
+      <c r="V6" s="81"/>
+      <c r="W6" s="81"/>
+      <c r="X6" s="81"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
@@ -1942,17 +1942,17 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="N7" s="21"/>
-      <c r="P7" s="67" t="s">
+      <c r="P7" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="67"/>
-      <c r="R7" s="67"/>
-      <c r="S7" s="67"/>
-      <c r="T7" s="67"/>
-      <c r="U7" s="67"/>
-      <c r="V7" s="67"/>
-      <c r="W7" s="67"/>
-      <c r="X7" s="67"/>
+      <c r="Q7" s="81"/>
+      <c r="R7" s="81"/>
+      <c r="S7" s="81"/>
+      <c r="T7" s="81"/>
+      <c r="U7" s="81"/>
+      <c r="V7" s="81"/>
+      <c r="W7" s="81"/>
+      <c r="X7" s="81"/>
     </row>
     <row r="8" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1967,17 +1967,17 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="N8" s="20"/>
-      <c r="P8" s="70" t="s">
+      <c r="P8" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="70"/>
-      <c r="R8" s="70"/>
-      <c r="S8" s="70"/>
-      <c r="T8" s="70"/>
-      <c r="U8" s="70"/>
-      <c r="V8" s="70"/>
-      <c r="W8" s="70"/>
-      <c r="X8" s="70"/>
+      <c r="Q8" s="113"/>
+      <c r="R8" s="113"/>
+      <c r="S8" s="113"/>
+      <c r="T8" s="113"/>
+      <c r="U8" s="113"/>
+      <c r="V8" s="113"/>
+      <c r="W8" s="113"/>
+      <c r="X8" s="113"/>
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
@@ -1985,23 +1985,23 @@
       <c r="AC8" s="5"/>
     </row>
     <row r="9" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="68"/>
+      <c r="A9" s="118"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="12"/>
       <c r="N9" s="49"/>
-      <c r="P9" s="70" t="s">
+      <c r="P9" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="Q9" s="70"/>
-      <c r="R9" s="70"/>
-      <c r="S9" s="70"/>
-      <c r="T9" s="70"/>
-      <c r="U9" s="70"/>
-      <c r="V9" s="70"/>
-      <c r="W9" s="70"/>
-      <c r="X9" s="70"/>
+      <c r="Q9" s="113"/>
+      <c r="R9" s="113"/>
+      <c r="S9" s="113"/>
+      <c r="T9" s="113"/>
+      <c r="U9" s="113"/>
+      <c r="V9" s="113"/>
+      <c r="W9" s="113"/>
+      <c r="X9" s="113"/>
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
@@ -2011,7 +2011,7 @@
       <c r="AJ9" s="13"/>
     </row>
     <row r="10" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="68"/>
+      <c r="A10" s="118"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -2028,18 +2028,18 @@
       <c r="AC10" s="5"/>
     </row>
     <row r="11" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="68"/>
-      <c r="C11" s="78" t="s">
+      <c r="A11" s="118"/>
+      <c r="C11" s="116" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="76" t="s">
+      <c r="D11" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76" t="s">
+      <c r="E11" s="114"/>
+      <c r="F11" s="114" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="76"/>
+      <c r="G11" s="114"/>
       <c r="T11" s="9"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
@@ -2052,596 +2052,596 @@
       <c r="AC11" s="5"/>
     </row>
     <row r="12" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="68"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="62" t="s">
+      <c r="A12" s="118"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="114"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="114"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="63"/>
-      <c r="J12" s="63"/>
-      <c r="K12" s="63"/>
-      <c r="L12" s="63"/>
-      <c r="M12" s="63"/>
-      <c r="N12" s="63"/>
-      <c r="O12" s="63"/>
-      <c r="P12" s="63"/>
-      <c r="Q12" s="63"/>
-      <c r="R12" s="63"/>
-      <c r="S12" s="63"/>
-      <c r="T12" s="63"/>
-      <c r="U12" s="63"/>
-      <c r="V12" s="63"/>
-      <c r="W12" s="63"/>
-      <c r="X12" s="63"/>
-      <c r="Y12" s="63"/>
-      <c r="Z12" s="63"/>
-      <c r="AA12" s="63"/>
-      <c r="AB12" s="63"/>
-      <c r="AC12" s="63"/>
-      <c r="AD12" s="63"/>
-      <c r="AE12" s="63"/>
-      <c r="AF12" s="63"/>
-      <c r="AG12" s="63"/>
-      <c r="AH12" s="63"/>
-      <c r="AI12" s="63"/>
-      <c r="AJ12" s="63"/>
-      <c r="AK12" s="63"/>
-      <c r="AL12" s="63"/>
-      <c r="AM12" s="63"/>
-      <c r="AN12" s="63"/>
-      <c r="AO12" s="63"/>
-      <c r="AP12" s="63"/>
-      <c r="AQ12" s="63"/>
-      <c r="AR12" s="63"/>
-      <c r="AS12" s="63"/>
-      <c r="AT12" s="63"/>
-      <c r="AU12" s="63"/>
-      <c r="AV12" s="63"/>
-      <c r="AW12" s="63"/>
-      <c r="AX12" s="63"/>
-      <c r="AY12" s="63"/>
-      <c r="AZ12" s="63"/>
-      <c r="BA12" s="63"/>
-      <c r="BB12" s="63"/>
-      <c r="BC12" s="63"/>
-      <c r="BD12" s="63"/>
-      <c r="BE12" s="63"/>
-      <c r="BF12" s="63"/>
-      <c r="BG12" s="63"/>
-      <c r="BH12" s="63"/>
-      <c r="BI12" s="63"/>
-      <c r="BJ12" s="63"/>
-      <c r="BK12" s="63"/>
-      <c r="BL12" s="63"/>
-      <c r="BM12" s="63"/>
-      <c r="BN12" s="63"/>
-      <c r="BO12" s="63"/>
-      <c r="BP12" s="63"/>
-      <c r="BQ12" s="64"/>
-      <c r="BR12" s="62" t="s">
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="71"/>
+      <c r="O12" s="71"/>
+      <c r="P12" s="71"/>
+      <c r="Q12" s="71"/>
+      <c r="R12" s="71"/>
+      <c r="S12" s="71"/>
+      <c r="T12" s="71"/>
+      <c r="U12" s="71"/>
+      <c r="V12" s="71"/>
+      <c r="W12" s="71"/>
+      <c r="X12" s="71"/>
+      <c r="Y12" s="71"/>
+      <c r="Z12" s="71"/>
+      <c r="AA12" s="71"/>
+      <c r="AB12" s="71"/>
+      <c r="AC12" s="71"/>
+      <c r="AD12" s="71"/>
+      <c r="AE12" s="71"/>
+      <c r="AF12" s="71"/>
+      <c r="AG12" s="71"/>
+      <c r="AH12" s="71"/>
+      <c r="AI12" s="71"/>
+      <c r="AJ12" s="71"/>
+      <c r="AK12" s="71"/>
+      <c r="AL12" s="71"/>
+      <c r="AM12" s="71"/>
+      <c r="AN12" s="71"/>
+      <c r="AO12" s="71"/>
+      <c r="AP12" s="71"/>
+      <c r="AQ12" s="71"/>
+      <c r="AR12" s="71"/>
+      <c r="AS12" s="71"/>
+      <c r="AT12" s="71"/>
+      <c r="AU12" s="71"/>
+      <c r="AV12" s="71"/>
+      <c r="AW12" s="71"/>
+      <c r="AX12" s="71"/>
+      <c r="AY12" s="71"/>
+      <c r="AZ12" s="71"/>
+      <c r="BA12" s="71"/>
+      <c r="BB12" s="71"/>
+      <c r="BC12" s="71"/>
+      <c r="BD12" s="71"/>
+      <c r="BE12" s="71"/>
+      <c r="BF12" s="71"/>
+      <c r="BG12" s="71"/>
+      <c r="BH12" s="71"/>
+      <c r="BI12" s="71"/>
+      <c r="BJ12" s="71"/>
+      <c r="BK12" s="71"/>
+      <c r="BL12" s="71"/>
+      <c r="BM12" s="71"/>
+      <c r="BN12" s="71"/>
+      <c r="BO12" s="71"/>
+      <c r="BP12" s="71"/>
+      <c r="BQ12" s="119"/>
+      <c r="BR12" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="BS12" s="63"/>
-      <c r="BT12" s="63"/>
-      <c r="BU12" s="63"/>
-      <c r="BV12" s="63"/>
-      <c r="BW12" s="63"/>
-      <c r="BX12" s="63"/>
-      <c r="BY12" s="63"/>
-      <c r="BZ12" s="63"/>
-      <c r="CA12" s="63"/>
-      <c r="CB12" s="63"/>
-      <c r="CC12" s="63"/>
-      <c r="CD12" s="63"/>
-      <c r="CE12" s="63"/>
-      <c r="CF12" s="63"/>
-      <c r="CG12" s="63"/>
-      <c r="CH12" s="63"/>
-      <c r="CI12" s="63"/>
-      <c r="CJ12" s="63"/>
-      <c r="CK12" s="63"/>
-      <c r="CL12" s="63"/>
-      <c r="CM12" s="63"/>
-      <c r="CN12" s="63"/>
-      <c r="CO12" s="63"/>
-      <c r="CP12" s="63"/>
-      <c r="CQ12" s="63"/>
-      <c r="CR12" s="63"/>
-      <c r="CS12" s="63"/>
-      <c r="CT12" s="63"/>
-      <c r="CU12" s="63"/>
-      <c r="CV12" s="63"/>
-      <c r="CW12" s="63"/>
-      <c r="CX12" s="63"/>
-      <c r="CY12" s="63"/>
-      <c r="CZ12" s="63"/>
-      <c r="DA12" s="63"/>
-      <c r="DB12" s="63"/>
-      <c r="DC12" s="63"/>
-      <c r="DD12" s="63"/>
-      <c r="DE12" s="63"/>
-      <c r="DF12" s="63"/>
-      <c r="DG12" s="63"/>
-      <c r="DH12" s="63"/>
-      <c r="DI12" s="63"/>
-      <c r="DJ12" s="63"/>
-      <c r="DK12" s="63"/>
-      <c r="DL12" s="63"/>
-      <c r="DM12" s="63"/>
-      <c r="DN12" s="63"/>
-      <c r="DO12" s="63"/>
-      <c r="DP12" s="63"/>
-      <c r="DQ12" s="63"/>
-      <c r="DR12" s="63"/>
-      <c r="DS12" s="63"/>
-      <c r="DT12" s="63"/>
-      <c r="DU12" s="63"/>
-      <c r="DV12" s="63"/>
-      <c r="DW12" s="63"/>
-      <c r="DX12" s="63"/>
-      <c r="DY12" s="64"/>
-      <c r="DZ12" s="62" t="s">
+      <c r="BS12" s="71"/>
+      <c r="BT12" s="71"/>
+      <c r="BU12" s="71"/>
+      <c r="BV12" s="71"/>
+      <c r="BW12" s="71"/>
+      <c r="BX12" s="71"/>
+      <c r="BY12" s="71"/>
+      <c r="BZ12" s="71"/>
+      <c r="CA12" s="71"/>
+      <c r="CB12" s="71"/>
+      <c r="CC12" s="71"/>
+      <c r="CD12" s="71"/>
+      <c r="CE12" s="71"/>
+      <c r="CF12" s="71"/>
+      <c r="CG12" s="71"/>
+      <c r="CH12" s="71"/>
+      <c r="CI12" s="71"/>
+      <c r="CJ12" s="71"/>
+      <c r="CK12" s="71"/>
+      <c r="CL12" s="71"/>
+      <c r="CM12" s="71"/>
+      <c r="CN12" s="71"/>
+      <c r="CO12" s="71"/>
+      <c r="CP12" s="71"/>
+      <c r="CQ12" s="71"/>
+      <c r="CR12" s="71"/>
+      <c r="CS12" s="71"/>
+      <c r="CT12" s="71"/>
+      <c r="CU12" s="71"/>
+      <c r="CV12" s="71"/>
+      <c r="CW12" s="71"/>
+      <c r="CX12" s="71"/>
+      <c r="CY12" s="71"/>
+      <c r="CZ12" s="71"/>
+      <c r="DA12" s="71"/>
+      <c r="DB12" s="71"/>
+      <c r="DC12" s="71"/>
+      <c r="DD12" s="71"/>
+      <c r="DE12" s="71"/>
+      <c r="DF12" s="71"/>
+      <c r="DG12" s="71"/>
+      <c r="DH12" s="71"/>
+      <c r="DI12" s="71"/>
+      <c r="DJ12" s="71"/>
+      <c r="DK12" s="71"/>
+      <c r="DL12" s="71"/>
+      <c r="DM12" s="71"/>
+      <c r="DN12" s="71"/>
+      <c r="DO12" s="71"/>
+      <c r="DP12" s="71"/>
+      <c r="DQ12" s="71"/>
+      <c r="DR12" s="71"/>
+      <c r="DS12" s="71"/>
+      <c r="DT12" s="71"/>
+      <c r="DU12" s="71"/>
+      <c r="DV12" s="71"/>
+      <c r="DW12" s="71"/>
+      <c r="DX12" s="71"/>
+      <c r="DY12" s="119"/>
+      <c r="DZ12" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="EA12" s="63"/>
-      <c r="EB12" s="63"/>
-      <c r="EC12" s="63"/>
-      <c r="ED12" s="63"/>
-      <c r="EE12" s="63"/>
-      <c r="EF12" s="63"/>
-      <c r="EG12" s="63"/>
-      <c r="EH12" s="63"/>
-      <c r="EI12" s="63"/>
-      <c r="EJ12" s="63"/>
-      <c r="EK12" s="63"/>
-      <c r="EL12" s="63"/>
-      <c r="EM12" s="63"/>
-      <c r="EN12" s="63"/>
-      <c r="EO12" s="63"/>
-      <c r="EP12" s="63"/>
-      <c r="EQ12" s="63"/>
-      <c r="ER12" s="63"/>
-      <c r="ES12" s="63"/>
-      <c r="ET12" s="63"/>
-      <c r="EU12" s="63"/>
-      <c r="EV12" s="63"/>
-      <c r="EW12" s="63"/>
-      <c r="EX12" s="63"/>
-      <c r="EY12" s="63"/>
-      <c r="EZ12" s="63"/>
-      <c r="FA12" s="63"/>
-      <c r="FB12" s="63"/>
-      <c r="FC12" s="63"/>
-      <c r="FD12" s="63"/>
-      <c r="FE12" s="63"/>
-      <c r="FF12" s="63"/>
-      <c r="FG12" s="63"/>
-      <c r="FH12" s="63"/>
-      <c r="FI12" s="63"/>
-      <c r="FJ12" s="63"/>
-      <c r="FK12" s="63"/>
-      <c r="FL12" s="63"/>
-      <c r="FM12" s="63"/>
-      <c r="FN12" s="63"/>
-      <c r="FO12" s="63"/>
-      <c r="FP12" s="63"/>
-      <c r="FQ12" s="63"/>
-      <c r="FR12" s="63"/>
-      <c r="FS12" s="63"/>
-      <c r="FT12" s="63"/>
-      <c r="FU12" s="63"/>
-      <c r="FV12" s="63"/>
-      <c r="FW12" s="63"/>
-      <c r="FX12" s="63"/>
-      <c r="FY12" s="63"/>
-      <c r="FZ12" s="63"/>
-      <c r="GA12" s="63"/>
-      <c r="GB12" s="63"/>
-      <c r="GC12" s="63"/>
-      <c r="GD12" s="63"/>
-      <c r="GE12" s="63"/>
-      <c r="GF12" s="63"/>
-      <c r="GG12" s="63"/>
-      <c r="GH12" s="63"/>
-      <c r="GI12" s="120"/>
+      <c r="EA12" s="71"/>
+      <c r="EB12" s="71"/>
+      <c r="EC12" s="71"/>
+      <c r="ED12" s="71"/>
+      <c r="EE12" s="71"/>
+      <c r="EF12" s="71"/>
+      <c r="EG12" s="71"/>
+      <c r="EH12" s="71"/>
+      <c r="EI12" s="71"/>
+      <c r="EJ12" s="71"/>
+      <c r="EK12" s="71"/>
+      <c r="EL12" s="71"/>
+      <c r="EM12" s="71"/>
+      <c r="EN12" s="71"/>
+      <c r="EO12" s="71"/>
+      <c r="EP12" s="71"/>
+      <c r="EQ12" s="71"/>
+      <c r="ER12" s="71"/>
+      <c r="ES12" s="71"/>
+      <c r="ET12" s="71"/>
+      <c r="EU12" s="71"/>
+      <c r="EV12" s="71"/>
+      <c r="EW12" s="71"/>
+      <c r="EX12" s="71"/>
+      <c r="EY12" s="71"/>
+      <c r="EZ12" s="71"/>
+      <c r="FA12" s="71"/>
+      <c r="FB12" s="71"/>
+      <c r="FC12" s="71"/>
+      <c r="FD12" s="71"/>
+      <c r="FE12" s="71"/>
+      <c r="FF12" s="71"/>
+      <c r="FG12" s="71"/>
+      <c r="FH12" s="71"/>
+      <c r="FI12" s="71"/>
+      <c r="FJ12" s="71"/>
+      <c r="FK12" s="71"/>
+      <c r="FL12" s="71"/>
+      <c r="FM12" s="71"/>
+      <c r="FN12" s="71"/>
+      <c r="FO12" s="71"/>
+      <c r="FP12" s="71"/>
+      <c r="FQ12" s="71"/>
+      <c r="FR12" s="71"/>
+      <c r="FS12" s="71"/>
+      <c r="FT12" s="71"/>
+      <c r="FU12" s="71"/>
+      <c r="FV12" s="71"/>
+      <c r="FW12" s="71"/>
+      <c r="FX12" s="71"/>
+      <c r="FY12" s="71"/>
+      <c r="FZ12" s="71"/>
+      <c r="GA12" s="71"/>
+      <c r="GB12" s="71"/>
+      <c r="GC12" s="71"/>
+      <c r="GD12" s="71"/>
+      <c r="GE12" s="71"/>
+      <c r="GF12" s="71"/>
+      <c r="GG12" s="71"/>
+      <c r="GH12" s="71"/>
+      <c r="GI12" s="72"/>
     </row>
     <row r="13" spans="1:191" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="60">
+      <c r="C13" s="117"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="68">
         <v>1</v>
       </c>
-      <c r="I13" s="61"/>
-      <c r="J13" s="60">
+      <c r="I13" s="69"/>
+      <c r="J13" s="68">
         <v>2</v>
       </c>
-      <c r="K13" s="61"/>
-      <c r="L13" s="60">
+      <c r="K13" s="69"/>
+      <c r="L13" s="68">
         <v>3</v>
       </c>
-      <c r="M13" s="61"/>
-      <c r="N13" s="60">
+      <c r="M13" s="69"/>
+      <c r="N13" s="68">
         <v>4</v>
       </c>
-      <c r="O13" s="61"/>
-      <c r="P13" s="60">
+      <c r="O13" s="69"/>
+      <c r="P13" s="68">
         <v>5</v>
       </c>
-      <c r="Q13" s="61"/>
-      <c r="R13" s="60">
+      <c r="Q13" s="69"/>
+      <c r="R13" s="68">
         <v>6</v>
       </c>
-      <c r="S13" s="61"/>
-      <c r="T13" s="60">
+      <c r="S13" s="69"/>
+      <c r="T13" s="68">
         <v>7</v>
       </c>
-      <c r="U13" s="61"/>
-      <c r="V13" s="60">
+      <c r="U13" s="69"/>
+      <c r="V13" s="68">
         <v>8</v>
       </c>
-      <c r="W13" s="61"/>
-      <c r="X13" s="60">
+      <c r="W13" s="69"/>
+      <c r="X13" s="68">
         <v>9</v>
       </c>
-      <c r="Y13" s="61"/>
-      <c r="Z13" s="60">
+      <c r="Y13" s="69"/>
+      <c r="Z13" s="68">
         <v>10</v>
       </c>
-      <c r="AA13" s="61"/>
-      <c r="AB13" s="60">
+      <c r="AA13" s="69"/>
+      <c r="AB13" s="68">
         <v>11</v>
       </c>
-      <c r="AC13" s="61"/>
-      <c r="AD13" s="60">
+      <c r="AC13" s="69"/>
+      <c r="AD13" s="68">
         <v>12</v>
       </c>
-      <c r="AE13" s="61"/>
-      <c r="AF13" s="60">
+      <c r="AE13" s="69"/>
+      <c r="AF13" s="68">
         <v>13</v>
       </c>
-      <c r="AG13" s="61"/>
-      <c r="AH13" s="60">
+      <c r="AG13" s="69"/>
+      <c r="AH13" s="68">
         <v>14</v>
       </c>
-      <c r="AI13" s="61"/>
-      <c r="AJ13" s="60">
+      <c r="AI13" s="69"/>
+      <c r="AJ13" s="68">
         <v>15</v>
       </c>
-      <c r="AK13" s="61"/>
-      <c r="AL13" s="60">
+      <c r="AK13" s="69"/>
+      <c r="AL13" s="68">
         <v>16</v>
       </c>
-      <c r="AM13" s="61"/>
-      <c r="AN13" s="60">
+      <c r="AM13" s="69"/>
+      <c r="AN13" s="68">
         <v>17</v>
       </c>
-      <c r="AO13" s="61"/>
-      <c r="AP13" s="60">
+      <c r="AO13" s="69"/>
+      <c r="AP13" s="68">
         <v>18</v>
       </c>
-      <c r="AQ13" s="61"/>
-      <c r="AR13" s="60">
+      <c r="AQ13" s="69"/>
+      <c r="AR13" s="68">
         <v>19</v>
       </c>
-      <c r="AS13" s="61"/>
-      <c r="AT13" s="60">
+      <c r="AS13" s="69"/>
+      <c r="AT13" s="68">
         <v>20</v>
       </c>
-      <c r="AU13" s="61"/>
-      <c r="AV13" s="60">
+      <c r="AU13" s="69"/>
+      <c r="AV13" s="68">
         <v>21</v>
       </c>
-      <c r="AW13" s="61"/>
-      <c r="AX13" s="60">
+      <c r="AW13" s="69"/>
+      <c r="AX13" s="68">
         <v>22</v>
       </c>
-      <c r="AY13" s="61"/>
-      <c r="AZ13" s="60">
+      <c r="AY13" s="69"/>
+      <c r="AZ13" s="68">
         <v>23</v>
       </c>
-      <c r="BA13" s="61"/>
-      <c r="BB13" s="60">
+      <c r="BA13" s="69"/>
+      <c r="BB13" s="68">
         <v>24</v>
       </c>
-      <c r="BC13" s="61"/>
-      <c r="BD13" s="60">
+      <c r="BC13" s="69"/>
+      <c r="BD13" s="68">
         <v>25</v>
       </c>
-      <c r="BE13" s="61"/>
-      <c r="BF13" s="60">
+      <c r="BE13" s="69"/>
+      <c r="BF13" s="68">
         <v>26</v>
       </c>
-      <c r="BG13" s="61"/>
-      <c r="BH13" s="60">
+      <c r="BG13" s="69"/>
+      <c r="BH13" s="68">
         <v>27</v>
       </c>
-      <c r="BI13" s="61"/>
-      <c r="BJ13" s="60">
+      <c r="BI13" s="69"/>
+      <c r="BJ13" s="68">
         <v>28</v>
       </c>
-      <c r="BK13" s="61"/>
-      <c r="BL13" s="60">
+      <c r="BK13" s="69"/>
+      <c r="BL13" s="68">
         <v>29</v>
       </c>
-      <c r="BM13" s="61"/>
-      <c r="BN13" s="60">
+      <c r="BM13" s="69"/>
+      <c r="BN13" s="68">
         <v>30</v>
       </c>
-      <c r="BO13" s="61"/>
-      <c r="BP13" s="60">
+      <c r="BO13" s="69"/>
+      <c r="BP13" s="68">
         <v>31</v>
       </c>
-      <c r="BQ13" s="69"/>
-      <c r="BR13" s="60">
+      <c r="BQ13" s="120"/>
+      <c r="BR13" s="68">
         <v>1</v>
       </c>
-      <c r="BS13" s="61"/>
-      <c r="BT13" s="60">
+      <c r="BS13" s="69"/>
+      <c r="BT13" s="68">
         <v>2</v>
       </c>
-      <c r="BU13" s="61"/>
-      <c r="BV13" s="60">
+      <c r="BU13" s="69"/>
+      <c r="BV13" s="68">
         <v>3</v>
       </c>
-      <c r="BW13" s="61"/>
-      <c r="BX13" s="60">
+      <c r="BW13" s="69"/>
+      <c r="BX13" s="68">
         <v>4</v>
       </c>
-      <c r="BY13" s="61"/>
-      <c r="BZ13" s="60">
+      <c r="BY13" s="69"/>
+      <c r="BZ13" s="68">
         <v>5</v>
       </c>
-      <c r="CA13" s="61"/>
-      <c r="CB13" s="60">
+      <c r="CA13" s="69"/>
+      <c r="CB13" s="68">
         <v>6</v>
       </c>
-      <c r="CC13" s="61"/>
-      <c r="CD13" s="60">
+      <c r="CC13" s="69"/>
+      <c r="CD13" s="68">
         <v>7</v>
       </c>
-      <c r="CE13" s="61"/>
-      <c r="CF13" s="60">
+      <c r="CE13" s="69"/>
+      <c r="CF13" s="68">
         <v>8</v>
       </c>
-      <c r="CG13" s="61"/>
-      <c r="CH13" s="60">
+      <c r="CG13" s="69"/>
+      <c r="CH13" s="68">
         <v>9</v>
       </c>
-      <c r="CI13" s="61"/>
-      <c r="CJ13" s="60">
+      <c r="CI13" s="69"/>
+      <c r="CJ13" s="68">
         <v>10</v>
       </c>
-      <c r="CK13" s="61"/>
-      <c r="CL13" s="60">
+      <c r="CK13" s="69"/>
+      <c r="CL13" s="68">
         <v>11</v>
       </c>
-      <c r="CM13" s="61"/>
-      <c r="CN13" s="60">
+      <c r="CM13" s="69"/>
+      <c r="CN13" s="68">
         <v>12</v>
       </c>
-      <c r="CO13" s="61"/>
-      <c r="CP13" s="60">
+      <c r="CO13" s="69"/>
+      <c r="CP13" s="68">
         <v>13</v>
       </c>
-      <c r="CQ13" s="61"/>
-      <c r="CR13" s="60">
+      <c r="CQ13" s="69"/>
+      <c r="CR13" s="68">
         <v>14</v>
       </c>
-      <c r="CS13" s="61"/>
-      <c r="CT13" s="60">
+      <c r="CS13" s="69"/>
+      <c r="CT13" s="68">
         <v>15</v>
       </c>
-      <c r="CU13" s="61"/>
-      <c r="CV13" s="60">
+      <c r="CU13" s="69"/>
+      <c r="CV13" s="68">
         <v>16</v>
       </c>
-      <c r="CW13" s="61"/>
-      <c r="CX13" s="60">
+      <c r="CW13" s="69"/>
+      <c r="CX13" s="68">
         <v>17</v>
       </c>
-      <c r="CY13" s="61"/>
-      <c r="CZ13" s="60">
+      <c r="CY13" s="69"/>
+      <c r="CZ13" s="68">
         <v>18</v>
       </c>
-      <c r="DA13" s="61"/>
-      <c r="DB13" s="60">
+      <c r="DA13" s="69"/>
+      <c r="DB13" s="68">
         <v>19</v>
       </c>
-      <c r="DC13" s="61"/>
-      <c r="DD13" s="60">
+      <c r="DC13" s="69"/>
+      <c r="DD13" s="68">
         <v>20</v>
       </c>
-      <c r="DE13" s="61"/>
-      <c r="DF13" s="60">
+      <c r="DE13" s="69"/>
+      <c r="DF13" s="68">
         <v>21</v>
       </c>
-      <c r="DG13" s="61"/>
-      <c r="DH13" s="60">
+      <c r="DG13" s="69"/>
+      <c r="DH13" s="68">
         <v>22</v>
       </c>
-      <c r="DI13" s="61"/>
-      <c r="DJ13" s="60">
+      <c r="DI13" s="69"/>
+      <c r="DJ13" s="68">
         <v>23</v>
       </c>
-      <c r="DK13" s="61"/>
-      <c r="DL13" s="60">
+      <c r="DK13" s="69"/>
+      <c r="DL13" s="68">
         <v>24</v>
       </c>
-      <c r="DM13" s="61"/>
-      <c r="DN13" s="60">
+      <c r="DM13" s="69"/>
+      <c r="DN13" s="68">
         <v>25</v>
       </c>
-      <c r="DO13" s="61"/>
-      <c r="DP13" s="60">
+      <c r="DO13" s="69"/>
+      <c r="DP13" s="68">
         <v>26</v>
       </c>
-      <c r="DQ13" s="61"/>
-      <c r="DR13" s="60">
+      <c r="DQ13" s="69"/>
+      <c r="DR13" s="68">
         <v>27</v>
       </c>
-      <c r="DS13" s="61"/>
-      <c r="DT13" s="60">
+      <c r="DS13" s="69"/>
+      <c r="DT13" s="68">
         <v>28</v>
       </c>
-      <c r="DU13" s="61"/>
-      <c r="DV13" s="60">
+      <c r="DU13" s="69"/>
+      <c r="DV13" s="68">
         <v>29</v>
       </c>
-      <c r="DW13" s="61"/>
-      <c r="DX13" s="60">
+      <c r="DW13" s="69"/>
+      <c r="DX13" s="68">
         <v>30</v>
       </c>
-      <c r="DY13" s="61"/>
-      <c r="DZ13" s="60">
+      <c r="DY13" s="69"/>
+      <c r="DZ13" s="68">
         <v>1</v>
       </c>
-      <c r="EA13" s="61"/>
-      <c r="EB13" s="60">
+      <c r="EA13" s="69"/>
+      <c r="EB13" s="68">
         <v>2</v>
       </c>
-      <c r="EC13" s="61"/>
-      <c r="ED13" s="60">
+      <c r="EC13" s="69"/>
+      <c r="ED13" s="68">
         <v>3</v>
       </c>
-      <c r="EE13" s="61"/>
-      <c r="EF13" s="60">
+      <c r="EE13" s="69"/>
+      <c r="EF13" s="68">
         <v>4</v>
       </c>
-      <c r="EG13" s="61"/>
-      <c r="EH13" s="60">
+      <c r="EG13" s="69"/>
+      <c r="EH13" s="68">
         <v>5</v>
       </c>
-      <c r="EI13" s="61"/>
-      <c r="EJ13" s="60">
+      <c r="EI13" s="69"/>
+      <c r="EJ13" s="68">
         <v>6</v>
       </c>
-      <c r="EK13" s="61"/>
-      <c r="EL13" s="60">
+      <c r="EK13" s="69"/>
+      <c r="EL13" s="68">
         <v>7</v>
       </c>
-      <c r="EM13" s="61"/>
-      <c r="EN13" s="60">
+      <c r="EM13" s="69"/>
+      <c r="EN13" s="68">
         <v>8</v>
       </c>
-      <c r="EO13" s="61"/>
-      <c r="EP13" s="60">
+      <c r="EO13" s="69"/>
+      <c r="EP13" s="68">
         <v>9</v>
       </c>
-      <c r="EQ13" s="61"/>
-      <c r="ER13" s="60">
+      <c r="EQ13" s="69"/>
+      <c r="ER13" s="68">
         <v>10</v>
       </c>
-      <c r="ES13" s="61"/>
-      <c r="ET13" s="60">
+      <c r="ES13" s="69"/>
+      <c r="ET13" s="68">
         <v>11</v>
       </c>
-      <c r="EU13" s="61"/>
-      <c r="EV13" s="60">
+      <c r="EU13" s="69"/>
+      <c r="EV13" s="68">
         <v>12</v>
       </c>
-      <c r="EW13" s="61"/>
-      <c r="EX13" s="60">
+      <c r="EW13" s="69"/>
+      <c r="EX13" s="68">
         <v>13</v>
       </c>
-      <c r="EY13" s="61"/>
-      <c r="EZ13" s="60">
+      <c r="EY13" s="69"/>
+      <c r="EZ13" s="68">
         <v>14</v>
       </c>
-      <c r="FA13" s="61"/>
-      <c r="FB13" s="60">
+      <c r="FA13" s="69"/>
+      <c r="FB13" s="68">
         <v>15</v>
       </c>
-      <c r="FC13" s="61"/>
-      <c r="FD13" s="60">
+      <c r="FC13" s="69"/>
+      <c r="FD13" s="68">
         <v>16</v>
       </c>
-      <c r="FE13" s="61"/>
-      <c r="FF13" s="60">
+      <c r="FE13" s="69"/>
+      <c r="FF13" s="68">
         <v>17</v>
       </c>
-      <c r="FG13" s="61"/>
-      <c r="FH13" s="60">
+      <c r="FG13" s="69"/>
+      <c r="FH13" s="68">
         <v>18</v>
       </c>
-      <c r="FI13" s="61"/>
-      <c r="FJ13" s="60">
+      <c r="FI13" s="69"/>
+      <c r="FJ13" s="68">
         <v>19</v>
       </c>
-      <c r="FK13" s="61"/>
-      <c r="FL13" s="60">
+      <c r="FK13" s="69"/>
+      <c r="FL13" s="68">
         <v>20</v>
       </c>
-      <c r="FM13" s="61"/>
-      <c r="FN13" s="60">
+      <c r="FM13" s="69"/>
+      <c r="FN13" s="68">
         <v>21</v>
       </c>
-      <c r="FO13" s="61"/>
-      <c r="FP13" s="60">
+      <c r="FO13" s="69"/>
+      <c r="FP13" s="68">
         <v>22</v>
       </c>
-      <c r="FQ13" s="61"/>
-      <c r="FR13" s="60">
+      <c r="FQ13" s="69"/>
+      <c r="FR13" s="68">
         <v>23</v>
       </c>
-      <c r="FS13" s="61"/>
-      <c r="FT13" s="60">
+      <c r="FS13" s="69"/>
+      <c r="FT13" s="68">
         <v>24</v>
       </c>
-      <c r="FU13" s="61"/>
-      <c r="FV13" s="60">
+      <c r="FU13" s="69"/>
+      <c r="FV13" s="68">
         <v>25</v>
       </c>
-      <c r="FW13" s="61"/>
-      <c r="FX13" s="60">
+      <c r="FW13" s="69"/>
+      <c r="FX13" s="68">
         <v>26</v>
       </c>
-      <c r="FY13" s="61"/>
-      <c r="FZ13" s="60">
+      <c r="FY13" s="69"/>
+      <c r="FZ13" s="68">
         <v>27</v>
       </c>
-      <c r="GA13" s="61"/>
-      <c r="GB13" s="60">
+      <c r="GA13" s="69"/>
+      <c r="GB13" s="68">
         <v>28</v>
       </c>
-      <c r="GC13" s="61"/>
-      <c r="GD13" s="60">
+      <c r="GC13" s="69"/>
+      <c r="GD13" s="68">
         <v>29</v>
       </c>
-      <c r="GE13" s="61"/>
-      <c r="GF13" s="60">
+      <c r="GE13" s="69"/>
+      <c r="GF13" s="68">
         <v>30</v>
       </c>
-      <c r="GG13" s="61"/>
-      <c r="GH13" s="60">
+      <c r="GG13" s="69"/>
+      <c r="GH13" s="68">
         <v>31</v>
       </c>
-      <c r="GI13" s="61"/>
+      <c r="GI13" s="69"/>
     </row>
     <row r="14" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A14" s="113" t="s">
+      <c r="A14" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="114"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="37"/>
-      <c r="D14" s="97">
+      <c r="D14" s="91">
         <f>SUM(D15:E61)</f>
         <v>51.050000000000011</v>
       </c>
-      <c r="E14" s="99"/>
-      <c r="F14" s="97">
+      <c r="E14" s="93"/>
+      <c r="F14" s="91">
         <f>SUM(F15:G61)</f>
-        <v>44.125999999999998</v>
-      </c>
-      <c r="G14" s="98"/>
+        <v>44.725999999999999</v>
+      </c>
+      <c r="G14" s="92"/>
       <c r="H14" s="18"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -2828,22 +2828,22 @@
       <c r="GI14" s="14"/>
     </row>
     <row r="15" spans="1:191" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="74"/>
+      <c r="B15" s="83"/>
       <c r="C15" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="65">
+      <c r="D15" s="62">
         <v>1.5</v>
       </c>
-      <c r="E15" s="66"/>
-      <c r="F15" s="65">
+      <c r="E15" s="63"/>
+      <c r="F15" s="62">
         <f>SUM(H15:GI15)</f>
         <v>0.5</v>
       </c>
-      <c r="G15" s="80"/>
+      <c r="G15" s="64"/>
       <c r="H15" s="47"/>
       <c r="I15" s="12"/>
       <c r="J15" s="24">
@@ -3032,22 +3032,22 @@
       <c r="GI15" s="34"/>
     </row>
     <row r="16" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A16" s="81" t="s">
+      <c r="A16" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="82"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="62">
         <v>0.6</v>
       </c>
-      <c r="E16" s="66"/>
-      <c r="F16" s="65">
+      <c r="E16" s="63"/>
+      <c r="F16" s="62">
         <f>SUM(H16:GI16)</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="80"/>
+        <v>0.6</v>
+      </c>
+      <c r="G16" s="64"/>
       <c r="H16" s="47"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
@@ -3093,7 +3093,9 @@
       <c r="AX16" s="32"/>
       <c r="AY16" s="32"/>
       <c r="AZ16" s="32"/>
-      <c r="BA16" s="32"/>
+      <c r="BA16" s="24">
+        <v>0.6</v>
+      </c>
       <c r="BB16" s="49"/>
       <c r="BC16" s="52"/>
       <c r="BD16" s="51"/>
@@ -3234,22 +3236,22 @@
       <c r="GI16" s="32"/>
     </row>
     <row r="17" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A17" s="81" t="s">
+      <c r="A17" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="82"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="65">
+      <c r="D17" s="62">
         <v>1</v>
       </c>
-      <c r="E17" s="66"/>
-      <c r="F17" s="65">
+      <c r="E17" s="63"/>
+      <c r="F17" s="62">
         <f>SUM(H17:GI17)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="80"/>
+      <c r="G17" s="64"/>
       <c r="H17" s="47"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
@@ -3440,22 +3442,22 @@
       <c r="GI17" s="32"/>
     </row>
     <row r="18" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A18" s="81" t="s">
+      <c r="A18" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="82"/>
+      <c r="B18" s="67"/>
       <c r="C18" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="65">
+      <c r="D18" s="62">
         <v>0.8</v>
       </c>
-      <c r="E18" s="66"/>
-      <c r="F18" s="65">
+      <c r="E18" s="63"/>
+      <c r="F18" s="62">
         <f t="shared" ref="F18:F60" si="0">SUM(H18:GI18)</f>
         <v>1.25</v>
       </c>
-      <c r="G18" s="80"/>
+      <c r="G18" s="64"/>
       <c r="H18" s="26"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
@@ -3646,22 +3648,22 @@
       <c r="GI18" s="32"/>
     </row>
     <row r="19" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="82"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="65">
+      <c r="D19" s="62">
         <v>0.5</v>
       </c>
-      <c r="E19" s="66"/>
-      <c r="F19" s="65">
+      <c r="E19" s="63"/>
+      <c r="F19" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="80"/>
+      <c r="G19" s="64"/>
       <c r="H19" s="26"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
@@ -3848,22 +3850,22 @@
       <c r="GI19" s="36"/>
     </row>
     <row r="20" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="82"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="65">
+      <c r="D20" s="62">
         <v>0.3</v>
       </c>
-      <c r="E20" s="66"/>
-      <c r="F20" s="65">
+      <c r="E20" s="63"/>
+      <c r="F20" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="80"/>
+      <c r="G20" s="64"/>
       <c r="H20" s="26"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -4050,22 +4052,22 @@
       <c r="GI20" s="36"/>
     </row>
     <row r="21" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="82"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="65">
+      <c r="D21" s="62">
         <v>1</v>
       </c>
-      <c r="E21" s="66"/>
-      <c r="F21" s="65">
+      <c r="E21" s="63"/>
+      <c r="F21" s="62">
         <f t="shared" si="0"/>
         <v>0.16600000000000001</v>
       </c>
-      <c r="G21" s="80"/>
+      <c r="G21" s="64"/>
       <c r="H21" s="26"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
@@ -4254,22 +4256,22 @@
       <c r="GI21" s="36"/>
     </row>
     <row r="22" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A22" s="81" t="s">
+      <c r="A22" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="82"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="65">
+      <c r="D22" s="62">
         <v>0.6</v>
       </c>
-      <c r="E22" s="66"/>
-      <c r="F22" s="65">
+      <c r="E22" s="63"/>
+      <c r="F22" s="62">
         <f t="shared" si="0"/>
         <v>0.66</v>
       </c>
-      <c r="G22" s="80"/>
+      <c r="G22" s="64"/>
       <c r="H22" s="26"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
@@ -4458,22 +4460,22 @@
       <c r="GI22" s="36"/>
     </row>
     <row r="23" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A23" s="81" t="s">
+      <c r="A23" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="82"/>
+      <c r="B23" s="67"/>
       <c r="C23" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="65">
+      <c r="D23" s="62">
         <v>0.6</v>
       </c>
-      <c r="E23" s="66"/>
-      <c r="F23" s="65">
+      <c r="E23" s="63"/>
+      <c r="F23" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="80"/>
+      <c r="G23" s="64"/>
       <c r="H23" s="26"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
@@ -4660,22 +4662,22 @@
       <c r="GI23" s="36"/>
     </row>
     <row r="24" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A24" s="81" t="s">
+      <c r="A24" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="82"/>
+      <c r="B24" s="67"/>
       <c r="C24" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="65">
+      <c r="D24" s="62">
         <v>3</v>
       </c>
-      <c r="E24" s="66"/>
-      <c r="F24" s="65">
+      <c r="E24" s="63"/>
+      <c r="F24" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="80"/>
+      <c r="G24" s="64"/>
       <c r="H24" s="26"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
@@ -4862,22 +4864,22 @@
       <c r="GI24" s="36"/>
     </row>
     <row r="25" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A25" s="81" t="s">
+      <c r="A25" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="82"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="65">
+      <c r="D25" s="62">
         <v>1.5</v>
       </c>
-      <c r="E25" s="66"/>
-      <c r="F25" s="65">
+      <c r="E25" s="63"/>
+      <c r="F25" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="80"/>
+      <c r="G25" s="64"/>
       <c r="H25" s="26"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
@@ -5064,22 +5066,22 @@
       <c r="GI25" s="36"/>
     </row>
     <row r="26" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A26" s="81" t="s">
+      <c r="A26" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="82"/>
+      <c r="B26" s="67"/>
       <c r="C26" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="65">
+      <c r="D26" s="62">
         <v>1</v>
       </c>
-      <c r="E26" s="66"/>
-      <c r="F26" s="65">
+      <c r="E26" s="63"/>
+      <c r="F26" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="80"/>
+      <c r="G26" s="64"/>
       <c r="H26" s="26"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
@@ -5266,22 +5268,22 @@
       <c r="GI26" s="36"/>
     </row>
     <row r="27" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="81" t="s">
+      <c r="A27" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="82"/>
+      <c r="B27" s="67"/>
       <c r="C27" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="65">
+      <c r="D27" s="62">
         <v>1</v>
       </c>
-      <c r="E27" s="66"/>
-      <c r="F27" s="65">
+      <c r="E27" s="63"/>
+      <c r="F27" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G27" s="80"/>
+      <c r="G27" s="64"/>
       <c r="H27" s="26"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
@@ -5468,22 +5470,22 @@
       <c r="GI27" s="36"/>
     </row>
     <row r="28" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A28" s="81" t="s">
+      <c r="A28" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="82"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="65">
+      <c r="D28" s="62">
         <v>1</v>
       </c>
-      <c r="E28" s="66"/>
-      <c r="F28" s="65">
+      <c r="E28" s="63"/>
+      <c r="F28" s="62">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G28" s="80"/>
+      <c r="G28" s="64"/>
       <c r="H28" s="26"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
@@ -5672,22 +5674,22 @@
       <c r="GI28" s="36"/>
     </row>
     <row r="29" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A29" s="81" t="s">
+      <c r="A29" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="82"/>
+      <c r="B29" s="67"/>
       <c r="C29" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="65">
+      <c r="D29" s="62">
         <v>1</v>
       </c>
-      <c r="E29" s="66"/>
-      <c r="F29" s="65">
+      <c r="E29" s="63"/>
+      <c r="F29" s="62">
         <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
-      <c r="G29" s="80"/>
+      <c r="G29" s="64"/>
       <c r="H29" s="26"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
@@ -5878,22 +5880,22 @@
       <c r="GI29" s="36"/>
     </row>
     <row r="30" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A30" s="81" t="s">
+      <c r="A30" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="82"/>
+      <c r="B30" s="67"/>
       <c r="C30" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="65">
+      <c r="D30" s="62">
         <v>1</v>
       </c>
-      <c r="E30" s="66"/>
-      <c r="F30" s="65">
+      <c r="E30" s="63"/>
+      <c r="F30" s="62">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G30" s="80"/>
+      <c r="G30" s="64"/>
       <c r="H30" s="26"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
@@ -6082,22 +6084,22 @@
       <c r="GI30" s="36"/>
     </row>
     <row r="31" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A31" s="81" t="s">
+      <c r="A31" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="82"/>
+      <c r="B31" s="67"/>
       <c r="C31" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="65">
+      <c r="D31" s="62">
         <v>4</v>
       </c>
-      <c r="E31" s="66"/>
-      <c r="F31" s="65">
+      <c r="E31" s="63"/>
+      <c r="F31" s="62">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G31" s="80"/>
+      <c r="G31" s="64"/>
       <c r="H31" s="26"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
@@ -6288,22 +6290,22 @@
       <c r="GI31" s="36"/>
     </row>
     <row r="32" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A32" s="81" t="s">
+      <c r="A32" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="82"/>
+      <c r="B32" s="67"/>
       <c r="C32" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="65">
+      <c r="D32" s="62">
         <v>0.6</v>
       </c>
-      <c r="E32" s="66"/>
-      <c r="F32" s="65">
+      <c r="E32" s="63"/>
+      <c r="F32" s="62">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G32" s="80"/>
+      <c r="G32" s="64"/>
       <c r="H32" s="26"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
@@ -6492,22 +6494,22 @@
       <c r="GI32" s="36"/>
     </row>
     <row r="33" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="81" t="s">
+      <c r="A33" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="82"/>
+      <c r="B33" s="67"/>
       <c r="C33" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="65">
+      <c r="D33" s="62">
         <v>0.5</v>
       </c>
-      <c r="E33" s="66"/>
-      <c r="F33" s="65">
+      <c r="E33" s="63"/>
+      <c r="F33" s="62">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G33" s="80"/>
+      <c r="G33" s="64"/>
       <c r="H33" s="26"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
@@ -6696,22 +6698,22 @@
       <c r="GI33" s="36"/>
     </row>
     <row r="34" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A34" s="81" t="s">
+      <c r="A34" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="82"/>
+      <c r="B34" s="67"/>
       <c r="C34" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="65">
+      <c r="D34" s="62">
         <v>0.3</v>
       </c>
-      <c r="E34" s="66"/>
-      <c r="F34" s="65">
+      <c r="E34" s="63"/>
+      <c r="F34" s="62">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G34" s="80"/>
+      <c r="G34" s="64"/>
       <c r="H34" s="26"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
@@ -6900,22 +6902,22 @@
       <c r="GI34" s="36"/>
     </row>
     <row r="35" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A35" s="81" t="s">
+      <c r="A35" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="82"/>
+      <c r="B35" s="67"/>
       <c r="C35" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="65">
+      <c r="D35" s="62">
         <v>0.3</v>
       </c>
-      <c r="E35" s="66"/>
-      <c r="F35" s="65">
+      <c r="E35" s="63"/>
+      <c r="F35" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G35" s="80"/>
+      <c r="G35" s="64"/>
       <c r="H35" s="26"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
@@ -7102,22 +7104,22 @@
       <c r="GI35" s="36"/>
     </row>
     <row r="36" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A36" s="81" t="s">
+      <c r="A36" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="82"/>
+      <c r="B36" s="67"/>
       <c r="C36" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="65">
+      <c r="D36" s="62">
         <v>1.5</v>
       </c>
-      <c r="E36" s="66"/>
-      <c r="F36" s="65">
+      <c r="E36" s="63"/>
+      <c r="F36" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G36" s="80"/>
+      <c r="G36" s="64"/>
       <c r="H36" s="26"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
@@ -7304,22 +7306,22 @@
       <c r="GI36" s="36"/>
     </row>
     <row r="37" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A37" s="81" t="s">
+      <c r="A37" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="82"/>
+      <c r="B37" s="67"/>
       <c r="C37" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="65">
+      <c r="D37" s="62">
         <v>0.5</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="65">
+      <c r="E37" s="63"/>
+      <c r="F37" s="62">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G37" s="80"/>
+      <c r="G37" s="64"/>
       <c r="H37" s="26"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
@@ -7508,22 +7510,22 @@
       <c r="GI37" s="36"/>
     </row>
     <row r="38" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A38" s="81" t="s">
+      <c r="A38" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="82"/>
+      <c r="B38" s="67"/>
       <c r="C38" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="65">
+      <c r="D38" s="62">
         <v>0.25</v>
       </c>
-      <c r="E38" s="66"/>
-      <c r="F38" s="65">
+      <c r="E38" s="63"/>
+      <c r="F38" s="62">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G38" s="80"/>
+      <c r="G38" s="64"/>
       <c r="H38" s="26"/>
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
@@ -7712,22 +7714,22 @@
       <c r="GI38" s="36"/>
     </row>
     <row r="39" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A39" s="81" t="s">
+      <c r="A39" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="82"/>
+      <c r="B39" s="67"/>
       <c r="C39" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="65">
+      <c r="D39" s="62">
         <v>0.5</v>
       </c>
-      <c r="E39" s="66"/>
-      <c r="F39" s="65">
+      <c r="E39" s="63"/>
+      <c r="F39" s="62">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="G39" s="80"/>
+      <c r="G39" s="64"/>
       <c r="H39" s="26"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
@@ -7916,22 +7918,22 @@
       <c r="GI39" s="36"/>
     </row>
     <row r="40" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A40" s="81" t="s">
+      <c r="A40" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="82"/>
+      <c r="B40" s="67"/>
       <c r="C40" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="65">
+      <c r="D40" s="62">
         <v>0.5</v>
       </c>
-      <c r="E40" s="66"/>
-      <c r="F40" s="65">
+      <c r="E40" s="63"/>
+      <c r="F40" s="62">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G40" s="80"/>
+      <c r="G40" s="64"/>
       <c r="H40" s="26"/>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
@@ -8120,22 +8122,22 @@
       <c r="GI40" s="36"/>
     </row>
     <row r="41" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A41" s="81" t="s">
+      <c r="A41" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="82"/>
+      <c r="B41" s="67"/>
       <c r="C41" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="65">
+      <c r="D41" s="62">
         <v>0.3</v>
       </c>
-      <c r="E41" s="66"/>
-      <c r="F41" s="65">
+      <c r="E41" s="63"/>
+      <c r="F41" s="62">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G41" s="80"/>
+      <c r="G41" s="64"/>
       <c r="H41" s="26"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
@@ -8324,22 +8326,22 @@
       <c r="GI41" s="36"/>
     </row>
     <row r="42" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A42" s="81" t="s">
+      <c r="A42" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="82"/>
+      <c r="B42" s="67"/>
       <c r="C42" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="65">
+      <c r="D42" s="62">
         <v>0.5</v>
       </c>
-      <c r="E42" s="66"/>
-      <c r="F42" s="65">
+      <c r="E42" s="63"/>
+      <c r="F42" s="62">
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-      <c r="G42" s="80"/>
+      <c r="G42" s="64"/>
       <c r="H42" s="26"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
@@ -8528,22 +8530,22 @@
       <c r="GI42" s="36"/>
     </row>
     <row r="43" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A43" s="81" t="s">
+      <c r="A43" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="82"/>
+      <c r="B43" s="67"/>
       <c r="C43" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D43" s="65">
+      <c r="D43" s="62">
         <v>1.3</v>
       </c>
-      <c r="E43" s="66"/>
-      <c r="F43" s="65">
+      <c r="E43" s="63"/>
+      <c r="F43" s="62">
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
-      <c r="G43" s="80"/>
+      <c r="G43" s="64"/>
       <c r="H43" s="26"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
@@ -8734,22 +8736,22 @@
       <c r="GI43" s="36"/>
     </row>
     <row r="44" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="81" t="s">
+      <c r="A44" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="82"/>
+      <c r="B44" s="67"/>
       <c r="C44" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="65">
+      <c r="D44" s="62">
         <v>1.3</v>
       </c>
-      <c r="E44" s="66"/>
-      <c r="F44" s="65">
+      <c r="E44" s="63"/>
+      <c r="F44" s="62">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G44" s="80"/>
+      <c r="G44" s="64"/>
       <c r="H44" s="26"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
@@ -8938,22 +8940,22 @@
       <c r="GI44" s="36"/>
     </row>
     <row r="45" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A45" s="81" t="s">
+      <c r="A45" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="82"/>
+      <c r="B45" s="67"/>
       <c r="C45" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="65">
+      <c r="D45" s="62">
         <v>1</v>
       </c>
-      <c r="E45" s="66"/>
-      <c r="F45" s="65">
+      <c r="E45" s="63"/>
+      <c r="F45" s="62">
         <f t="shared" si="0"/>
         <v>1.05</v>
       </c>
-      <c r="G45" s="80"/>
+      <c r="G45" s="64"/>
       <c r="H45" s="26"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
@@ -9144,22 +9146,22 @@
       <c r="GI45" s="36"/>
     </row>
     <row r="46" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A46" s="81" t="s">
+      <c r="A46" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="82"/>
+      <c r="B46" s="67"/>
       <c r="C46" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="D46" s="65">
+      <c r="D46" s="62">
         <v>1</v>
       </c>
-      <c r="E46" s="66"/>
-      <c r="F46" s="65">
+      <c r="E46" s="63"/>
+      <c r="F46" s="62">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="G46" s="80"/>
+      <c r="G46" s="64"/>
       <c r="H46" s="26"/>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
@@ -9348,22 +9350,22 @@
       <c r="GI46" s="36"/>
     </row>
     <row r="47" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A47" s="81" t="s">
+      <c r="A47" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="82"/>
+      <c r="B47" s="67"/>
       <c r="C47" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="D47" s="65">
+      <c r="D47" s="62">
         <v>1</v>
       </c>
-      <c r="E47" s="66"/>
-      <c r="F47" s="65">
+      <c r="E47" s="63"/>
+      <c r="F47" s="62">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="G47" s="80"/>
+      <c r="G47" s="64"/>
       <c r="H47" s="26"/>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
@@ -9552,22 +9554,22 @@
       <c r="GI47" s="36"/>
     </row>
     <row r="48" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A48" s="81" t="s">
+      <c r="A48" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="B48" s="82"/>
+      <c r="B48" s="67"/>
       <c r="C48" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D48" s="65">
+      <c r="D48" s="62">
         <v>0.3</v>
       </c>
-      <c r="E48" s="66"/>
-      <c r="F48" s="65">
+      <c r="E48" s="63"/>
+      <c r="F48" s="62">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G48" s="80"/>
+      <c r="G48" s="64"/>
       <c r="H48" s="26"/>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
@@ -9756,22 +9758,22 @@
       <c r="GI48" s="36"/>
     </row>
     <row r="49" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A49" s="81" t="s">
+      <c r="A49" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="82"/>
+      <c r="B49" s="67"/>
       <c r="C49" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="65">
+      <c r="D49" s="62">
         <v>2</v>
       </c>
-      <c r="E49" s="66"/>
-      <c r="F49" s="65">
+      <c r="E49" s="63"/>
+      <c r="F49" s="62">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G49" s="80"/>
+      <c r="G49" s="64"/>
       <c r="H49" s="26"/>
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
@@ -9962,22 +9964,22 @@
       <c r="GI49" s="36"/>
     </row>
     <row r="50" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A50" s="81" t="s">
+      <c r="A50" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="82"/>
+      <c r="B50" s="67"/>
       <c r="C50" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="D50" s="65">
+      <c r="D50" s="62">
         <v>2</v>
       </c>
-      <c r="E50" s="66"/>
-      <c r="F50" s="65">
+      <c r="E50" s="63"/>
+      <c r="F50" s="62">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G50" s="80"/>
+      <c r="G50" s="64"/>
       <c r="H50" s="26"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
@@ -10168,22 +10170,22 @@
       <c r="GI50" s="36"/>
     </row>
     <row r="51" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A51" s="81" t="s">
+      <c r="A51" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="82"/>
+      <c r="B51" s="67"/>
       <c r="C51" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D51" s="65">
+      <c r="D51" s="62">
         <v>2</v>
       </c>
-      <c r="E51" s="66"/>
-      <c r="F51" s="65">
+      <c r="E51" s="63"/>
+      <c r="F51" s="62">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G51" s="80"/>
+      <c r="G51" s="64"/>
       <c r="H51" s="26"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
@@ -10374,22 +10376,22 @@
       <c r="GI51" s="36"/>
     </row>
     <row r="52" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A52" s="81" t="s">
+      <c r="A52" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="82"/>
+      <c r="B52" s="67"/>
       <c r="C52" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="65">
+      <c r="D52" s="62">
         <v>2</v>
       </c>
-      <c r="E52" s="66"/>
-      <c r="F52" s="65">
+      <c r="E52" s="63"/>
+      <c r="F52" s="62">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G52" s="80"/>
+      <c r="G52" s="64"/>
       <c r="H52" s="26"/>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
@@ -10580,22 +10582,22 @@
       <c r="GI52" s="36"/>
     </row>
     <row r="53" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A53" s="81" t="s">
+      <c r="A53" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="82"/>
+      <c r="B53" s="67"/>
       <c r="C53" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D53" s="65">
+      <c r="D53" s="62">
         <v>2</v>
       </c>
-      <c r="E53" s="66"/>
-      <c r="F53" s="65">
+      <c r="E53" s="63"/>
+      <c r="F53" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G53" s="80"/>
+      <c r="G53" s="64"/>
       <c r="H53" s="26"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
@@ -10782,22 +10784,22 @@
       <c r="GI53" s="36"/>
     </row>
     <row r="54" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A54" s="81" t="s">
+      <c r="A54" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="82"/>
+      <c r="B54" s="67"/>
       <c r="C54" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="D54" s="65">
+      <c r="D54" s="62">
         <v>0.25</v>
       </c>
-      <c r="E54" s="66"/>
-      <c r="F54" s="65">
+      <c r="E54" s="63"/>
+      <c r="F54" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G54" s="80"/>
+      <c r="G54" s="64"/>
       <c r="H54" s="26"/>
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
@@ -10984,22 +10986,22 @@
       <c r="GI54" s="36"/>
     </row>
     <row r="55" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A55" s="81" t="s">
+      <c r="A55" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="82"/>
+      <c r="B55" s="67"/>
       <c r="C55" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="D55" s="65">
+      <c r="D55" s="62">
         <v>1</v>
       </c>
-      <c r="E55" s="66"/>
-      <c r="F55" s="65">
+      <c r="E55" s="63"/>
+      <c r="F55" s="62">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G55" s="80"/>
+      <c r="G55" s="64"/>
       <c r="H55" s="26"/>
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
@@ -11190,22 +11192,22 @@
       <c r="GI55" s="36"/>
     </row>
     <row r="56" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A56" s="81" t="s">
+      <c r="A56" s="66" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="82"/>
+      <c r="B56" s="67"/>
       <c r="C56" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="D56" s="65">
+      <c r="D56" s="62">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E56" s="66"/>
-      <c r="F56" s="65">
+      <c r="E56" s="63"/>
+      <c r="F56" s="62">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G56" s="80"/>
+      <c r="G56" s="64"/>
       <c r="H56" s="26"/>
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
@@ -11396,22 +11398,22 @@
       <c r="GI56" s="36"/>
     </row>
     <row r="57" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A57" s="81" t="s">
+      <c r="A57" s="66" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="82"/>
+      <c r="B57" s="67"/>
       <c r="C57" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="D57" s="65">
+      <c r="D57" s="62">
         <v>1.75</v>
       </c>
-      <c r="E57" s="66"/>
-      <c r="F57" s="65">
+      <c r="E57" s="63"/>
+      <c r="F57" s="62">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G57" s="80"/>
+      <c r="G57" s="64"/>
       <c r="H57" s="26"/>
       <c r="I57" s="12"/>
       <c r="J57" s="12"/>
@@ -11600,22 +11602,22 @@
       <c r="GI57" s="36"/>
     </row>
     <row r="58" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A58" s="81" t="s">
+      <c r="A58" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="B58" s="82"/>
+      <c r="B58" s="67"/>
       <c r="C58" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="D58" s="65">
+      <c r="D58" s="62">
         <v>0.6</v>
       </c>
-      <c r="E58" s="66"/>
-      <c r="F58" s="65">
+      <c r="E58" s="63"/>
+      <c r="F58" s="62">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G58" s="80"/>
+      <c r="G58" s="64"/>
       <c r="H58" s="26"/>
       <c r="I58" s="12"/>
       <c r="J58" s="12"/>
@@ -11804,22 +11806,22 @@
       <c r="GI58" s="36"/>
     </row>
     <row r="59" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="81" t="s">
+      <c r="A59" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="B59" s="82"/>
+      <c r="B59" s="67"/>
       <c r="C59" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="65">
+      <c r="D59" s="62">
         <v>1</v>
       </c>
-      <c r="E59" s="66"/>
-      <c r="F59" s="65">
+      <c r="E59" s="63"/>
+      <c r="F59" s="62">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G59" s="80"/>
+      <c r="G59" s="64"/>
       <c r="H59" s="26"/>
       <c r="I59" s="12"/>
       <c r="J59" s="12"/>
@@ -12010,22 +12012,22 @@
       <c r="GI59" s="36"/>
     </row>
     <row r="60" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A60" s="81" t="s">
+      <c r="A60" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="B60" s="82"/>
+      <c r="B60" s="67"/>
       <c r="C60" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="D60" s="65">
+      <c r="D60" s="62">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E60" s="66"/>
-      <c r="F60" s="65">
+      <c r="E60" s="63"/>
+      <c r="F60" s="62">
         <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
-      <c r="G60" s="80"/>
+      <c r="G60" s="64"/>
       <c r="H60" s="26"/>
       <c r="I60" s="12"/>
       <c r="J60" s="12"/>
@@ -12214,22 +12216,22 @@
       <c r="GI60" s="36"/>
     </row>
     <row r="61" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A61" s="81" t="s">
+      <c r="A61" s="66" t="s">
         <v>115</v>
       </c>
-      <c r="B61" s="82"/>
+      <c r="B61" s="67"/>
       <c r="C61" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="D61" s="65">
+      <c r="D61" s="62">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E61" s="66"/>
-      <c r="F61" s="65">
+      <c r="E61" s="63"/>
+      <c r="F61" s="62">
         <f>SUM(H61:GI61)</f>
         <v>1</v>
       </c>
-      <c r="G61" s="80"/>
+      <c r="G61" s="64"/>
       <c r="H61" s="26"/>
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
@@ -12418,21 +12420,21 @@
       <c r="GI61" s="36"/>
     </row>
     <row r="62" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A62" s="115" t="s">
+      <c r="A62" s="76" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="116"/>
+      <c r="B62" s="77"/>
       <c r="C62" s="39"/>
-      <c r="D62" s="71">
+      <c r="D62" s="78">
         <f>SUM(D63:E80)</f>
         <v>88.6</v>
       </c>
-      <c r="E62" s="117"/>
-      <c r="F62" s="71">
+      <c r="E62" s="79"/>
+      <c r="F62" s="78">
         <f>SUM(F63:G80)</f>
         <v>0</v>
       </c>
-      <c r="G62" s="75"/>
+      <c r="G62" s="80"/>
       <c r="H62" s="29"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
@@ -12619,22 +12621,22 @@
       <c r="GI62" s="29"/>
     </row>
     <row r="63" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="118" t="s">
+      <c r="A63" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="119"/>
+      <c r="B63" s="61"/>
       <c r="C63" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D63" s="65">
+      <c r="D63" s="62">
         <v>0.6</v>
       </c>
-      <c r="E63" s="66"/>
-      <c r="F63" s="65">
+      <c r="E63" s="63"/>
+      <c r="F63" s="62">
         <f>SUM(H63:GI63)</f>
         <v>0</v>
       </c>
-      <c r="G63" s="80"/>
+      <c r="G63" s="64"/>
       <c r="H63" s="47"/>
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
@@ -12821,22 +12823,22 @@
       <c r="GI63" s="32"/>
     </row>
     <row r="64" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="118" t="s">
+      <c r="A64" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="B64" s="119"/>
+      <c r="B64" s="61"/>
       <c r="C64" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D64" s="65">
+      <c r="D64" s="62">
         <v>1.5</v>
       </c>
-      <c r="E64" s="66"/>
-      <c r="F64" s="65">
+      <c r="E64" s="63"/>
+      <c r="F64" s="62">
         <f>SUM(H64:GI64)</f>
         <v>0</v>
       </c>
-      <c r="G64" s="80"/>
+      <c r="G64" s="64"/>
       <c r="H64" s="47"/>
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
@@ -13023,22 +13025,22 @@
       <c r="GI64" s="32"/>
     </row>
     <row r="65" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A65" s="118" t="s">
+      <c r="A65" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="B65" s="119"/>
+      <c r="B65" s="61"/>
       <c r="C65" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D65" s="65">
+      <c r="D65" s="62">
         <v>1</v>
       </c>
-      <c r="E65" s="66"/>
-      <c r="F65" s="65">
+      <c r="E65" s="63"/>
+      <c r="F65" s="62">
         <f t="shared" ref="F65:F80" si="1">SUM(H65:GI65)</f>
         <v>0</v>
       </c>
-      <c r="G65" s="80"/>
+      <c r="G65" s="64"/>
       <c r="H65" s="47"/>
       <c r="I65" s="12"/>
       <c r="J65" s="12"/>
@@ -13225,22 +13227,22 @@
       <c r="GI65" s="32"/>
     </row>
     <row r="66" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A66" s="118" t="s">
+      <c r="A66" s="60" t="s">
         <v>125</v>
       </c>
-      <c r="B66" s="119"/>
+      <c r="B66" s="61"/>
       <c r="C66" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D66" s="65">
+      <c r="D66" s="62">
         <v>0.5</v>
       </c>
-      <c r="E66" s="66"/>
-      <c r="F66" s="65">
+      <c r="E66" s="63"/>
+      <c r="F66" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G66" s="80"/>
+      <c r="G66" s="64"/>
       <c r="H66" s="47"/>
       <c r="I66" s="12"/>
       <c r="J66" s="12"/>
@@ -13427,22 +13429,22 @@
       <c r="GI66" s="32"/>
     </row>
     <row r="67" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A67" s="118" t="s">
+      <c r="A67" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="119"/>
+      <c r="B67" s="61"/>
       <c r="C67" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D67" s="65">
+      <c r="D67" s="62">
         <v>1</v>
       </c>
-      <c r="E67" s="66"/>
-      <c r="F67" s="65">
+      <c r="E67" s="63"/>
+      <c r="F67" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G67" s="80"/>
+      <c r="G67" s="64"/>
       <c r="H67" s="47"/>
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
@@ -13629,22 +13631,22 @@
       <c r="GI67" s="32"/>
     </row>
     <row r="68" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A68" s="118" t="s">
+      <c r="A68" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="B68" s="119"/>
+      <c r="B68" s="61"/>
       <c r="C68" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D68" s="65">
+      <c r="D68" s="62">
         <v>1</v>
       </c>
-      <c r="E68" s="66"/>
-      <c r="F68" s="65">
+      <c r="E68" s="63"/>
+      <c r="F68" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G68" s="80"/>
+      <c r="G68" s="64"/>
       <c r="H68" s="47"/>
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
@@ -13831,22 +13833,22 @@
       <c r="GI68" s="32"/>
     </row>
     <row r="69" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A69" s="118" t="s">
+      <c r="A69" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="B69" s="119"/>
+      <c r="B69" s="61"/>
       <c r="C69" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="D69" s="65">
+      <c r="D69" s="62">
         <v>4</v>
       </c>
-      <c r="E69" s="66"/>
-      <c r="F69" s="65">
+      <c r="E69" s="63"/>
+      <c r="F69" s="62">
         <f>SUM(H69:GI69)</f>
         <v>0</v>
       </c>
-      <c r="G69" s="80"/>
+      <c r="G69" s="64"/>
       <c r="H69" s="47"/>
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
@@ -14033,22 +14035,22 @@
       <c r="GI69" s="32"/>
     </row>
     <row r="70" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A70" s="118" t="s">
+      <c r="A70" s="60" t="s">
         <v>133</v>
       </c>
-      <c r="B70" s="119"/>
+      <c r="B70" s="61"/>
       <c r="C70" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="D70" s="65">
+      <c r="D70" s="62">
         <v>8</v>
       </c>
-      <c r="E70" s="66"/>
-      <c r="F70" s="65">
+      <c r="E70" s="63"/>
+      <c r="F70" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G70" s="80"/>
+      <c r="G70" s="64"/>
       <c r="H70" s="47"/>
       <c r="I70" s="12"/>
       <c r="J70" s="12"/>
@@ -14235,22 +14237,22 @@
       <c r="GI70" s="32"/>
     </row>
     <row r="71" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A71" s="118" t="s">
+      <c r="A71" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="B71" s="119"/>
+      <c r="B71" s="61"/>
       <c r="C71" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="D71" s="65">
+      <c r="D71" s="62">
         <v>1</v>
       </c>
-      <c r="E71" s="66"/>
-      <c r="F71" s="65">
+      <c r="E71" s="63"/>
+      <c r="F71" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G71" s="80"/>
+      <c r="G71" s="64"/>
       <c r="H71" s="47"/>
       <c r="I71" s="12"/>
       <c r="J71" s="12"/>
@@ -14437,22 +14439,22 @@
       <c r="GI71" s="32"/>
     </row>
     <row r="72" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A72" s="118" t="s">
+      <c r="A72" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="B72" s="119"/>
+      <c r="B72" s="61"/>
       <c r="C72" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="D72" s="65">
+      <c r="D72" s="62">
         <v>1</v>
       </c>
-      <c r="E72" s="66"/>
-      <c r="F72" s="65">
+      <c r="E72" s="63"/>
+      <c r="F72" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G72" s="80"/>
+      <c r="G72" s="64"/>
       <c r="H72" s="47"/>
       <c r="I72" s="12"/>
       <c r="J72" s="12"/>
@@ -14639,22 +14641,22 @@
       <c r="GI72" s="32"/>
     </row>
     <row r="73" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A73" s="118" t="s">
+      <c r="A73" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="B73" s="119"/>
+      <c r="B73" s="61"/>
       <c r="C73" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="D73" s="65">
+      <c r="D73" s="62">
         <v>4</v>
       </c>
-      <c r="E73" s="66"/>
-      <c r="F73" s="65">
+      <c r="E73" s="63"/>
+      <c r="F73" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G73" s="80"/>
+      <c r="G73" s="64"/>
       <c r="H73" s="47"/>
       <c r="I73" s="12"/>
       <c r="J73" s="12"/>
@@ -14841,22 +14843,22 @@
       <c r="GI73" s="32"/>
     </row>
     <row r="74" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A74" s="118" t="s">
+      <c r="A74" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="B74" s="119"/>
+      <c r="B74" s="61"/>
       <c r="C74" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="D74" s="65">
+      <c r="D74" s="62">
         <v>12</v>
       </c>
-      <c r="E74" s="66"/>
-      <c r="F74" s="65">
+      <c r="E74" s="63"/>
+      <c r="F74" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G74" s="80"/>
+      <c r="G74" s="64"/>
       <c r="H74" s="47"/>
       <c r="I74" s="12"/>
       <c r="J74" s="12"/>
@@ -15043,22 +15045,22 @@
       <c r="GI74" s="32"/>
     </row>
     <row r="75" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A75" s="118" t="s">
+      <c r="A75" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="B75" s="88"/>
+      <c r="B75" s="65"/>
       <c r="C75" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D75" s="65">
+      <c r="D75" s="62">
         <v>16</v>
       </c>
-      <c r="E75" s="66"/>
-      <c r="F75" s="65">
+      <c r="E75" s="63"/>
+      <c r="F75" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G75" s="80"/>
+      <c r="G75" s="64"/>
       <c r="H75" s="47"/>
       <c r="I75" s="12"/>
       <c r="J75" s="12"/>
@@ -15245,22 +15247,22 @@
       <c r="GI75" s="36"/>
     </row>
     <row r="76" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A76" s="118" t="s">
+      <c r="A76" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="B76" s="119"/>
+      <c r="B76" s="61"/>
       <c r="C76" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="D76" s="65">
+      <c r="D76" s="62">
         <v>5</v>
       </c>
-      <c r="E76" s="66"/>
-      <c r="F76" s="65">
+      <c r="E76" s="63"/>
+      <c r="F76" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G76" s="80"/>
+      <c r="G76" s="64"/>
       <c r="H76" s="47"/>
       <c r="I76" s="12"/>
       <c r="J76" s="12"/>
@@ -15447,22 +15449,22 @@
       <c r="GI76" s="32"/>
     </row>
     <row r="77" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A77" s="118" t="s">
+      <c r="A77" s="60" t="s">
         <v>146</v>
       </c>
-      <c r="B77" s="119"/>
+      <c r="B77" s="61"/>
       <c r="C77" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="D77" s="65">
+      <c r="D77" s="62">
         <v>4</v>
       </c>
-      <c r="E77" s="66"/>
-      <c r="F77" s="65">
+      <c r="E77" s="63"/>
+      <c r="F77" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G77" s="80"/>
+      <c r="G77" s="64"/>
       <c r="H77" s="47"/>
       <c r="I77" s="12"/>
       <c r="J77" s="12"/>
@@ -15649,22 +15651,22 @@
       <c r="GI77" s="32"/>
     </row>
     <row r="78" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A78" s="118" t="s">
+      <c r="A78" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="B78" s="119"/>
+      <c r="B78" s="61"/>
       <c r="C78" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="D78" s="65">
+      <c r="D78" s="62">
         <v>16</v>
       </c>
-      <c r="E78" s="66"/>
-      <c r="F78" s="65">
+      <c r="E78" s="63"/>
+      <c r="F78" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G78" s="80"/>
+      <c r="G78" s="64"/>
       <c r="H78" s="47"/>
       <c r="I78" s="12"/>
       <c r="J78" s="12"/>
@@ -15851,22 +15853,22 @@
       <c r="GI78" s="32"/>
     </row>
     <row r="79" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A79" s="73" t="s">
+      <c r="A79" s="82" t="s">
         <v>150</v>
       </c>
-      <c r="B79" s="74"/>
+      <c r="B79" s="83"/>
       <c r="C79" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="D79" s="65">
+      <c r="D79" s="62">
         <v>6</v>
       </c>
-      <c r="E79" s="66"/>
-      <c r="F79" s="65">
+      <c r="E79" s="63"/>
+      <c r="F79" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G79" s="80"/>
+      <c r="G79" s="64"/>
       <c r="H79" s="47"/>
       <c r="I79" s="12"/>
       <c r="J79" s="12"/>
@@ -16053,22 +16055,22 @@
       <c r="GI79" s="36"/>
     </row>
     <row r="80" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A80" s="73" t="s">
+      <c r="A80" s="82" t="s">
         <v>152</v>
       </c>
-      <c r="B80" s="74"/>
+      <c r="B80" s="83"/>
       <c r="C80" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D80" s="65">
+      <c r="D80" s="62">
         <v>6</v>
       </c>
-      <c r="E80" s="66"/>
-      <c r="F80" s="65">
+      <c r="E80" s="63"/>
+      <c r="F80" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G80" s="80"/>
+      <c r="G80" s="64"/>
       <c r="H80" s="47"/>
       <c r="I80" s="12"/>
       <c r="J80" s="12"/>
@@ -16255,21 +16257,21 @@
       <c r="GI80" s="36"/>
     </row>
     <row r="81" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A81" s="115" t="s">
+      <c r="A81" s="76" t="s">
         <v>153</v>
       </c>
-      <c r="B81" s="116"/>
+      <c r="B81" s="77"/>
       <c r="C81" s="39"/>
-      <c r="D81" s="71">
+      <c r="D81" s="78">
         <f>SUM(D82:E82)</f>
         <v>16</v>
       </c>
-      <c r="E81" s="72"/>
-      <c r="F81" s="71">
+      <c r="E81" s="88"/>
+      <c r="F81" s="78">
         <f>SUM(F82:G82)</f>
         <v>0</v>
       </c>
-      <c r="G81" s="75"/>
+      <c r="G81" s="80"/>
       <c r="H81" s="29"/>
       <c r="I81" s="8"/>
       <c r="J81" s="8"/>
@@ -16456,20 +16458,20 @@
       <c r="GI81" s="29"/>
     </row>
     <row r="82" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A82" s="93" t="s">
+      <c r="A82" s="86" t="s">
         <v>153</v>
       </c>
-      <c r="B82" s="94"/>
+      <c r="B82" s="87"/>
       <c r="C82" s="40"/>
-      <c r="D82" s="91">
+      <c r="D82" s="84">
         <v>16</v>
       </c>
-      <c r="E82" s="92"/>
-      <c r="F82" s="65">
+      <c r="E82" s="85"/>
+      <c r="F82" s="62">
         <f>SUM(H82:GI82)</f>
         <v>0</v>
       </c>
-      <c r="G82" s="80"/>
+      <c r="G82" s="64"/>
       <c r="H82" s="26"/>
       <c r="I82" s="12"/>
       <c r="J82" s="12"/>
@@ -16656,21 +16658,21 @@
       <c r="GI82" s="32"/>
     </row>
     <row r="83" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A83" s="110" t="s">
+      <c r="A83" s="104" t="s">
         <v>154</v>
       </c>
-      <c r="B83" s="111"/>
+      <c r="B83" s="105"/>
       <c r="C83" s="41"/>
-      <c r="D83" s="71">
+      <c r="D83" s="78">
         <f>SUM(D84:E84)</f>
         <v>32</v>
       </c>
-      <c r="E83" s="72"/>
-      <c r="F83" s="71">
+      <c r="E83" s="88"/>
+      <c r="F83" s="78">
         <f>SUM(F84:G84)</f>
         <v>0</v>
       </c>
-      <c r="G83" s="75"/>
+      <c r="G83" s="80"/>
       <c r="H83" s="29"/>
       <c r="I83" s="8"/>
       <c r="J83" s="8"/>
@@ -16857,20 +16859,20 @@
       <c r="GI83" s="29"/>
     </row>
     <row r="84" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A84" s="85" t="s">
+      <c r="A84" s="108" t="s">
         <v>154</v>
       </c>
-      <c r="B84" s="86"/>
+      <c r="B84" s="109"/>
       <c r="C84" s="42"/>
-      <c r="D84" s="65">
+      <c r="D84" s="62">
         <v>32</v>
       </c>
-      <c r="E84" s="66"/>
-      <c r="F84" s="65">
+      <c r="E84" s="63"/>
+      <c r="F84" s="62">
         <f>SUM(H84:GI84)</f>
         <v>0</v>
       </c>
-      <c r="G84" s="80"/>
+      <c r="G84" s="64"/>
       <c r="H84" s="26"/>
       <c r="I84" s="12"/>
       <c r="J84" s="12"/>
@@ -17057,21 +17059,21 @@
       <c r="GI84" s="32"/>
     </row>
     <row r="85" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A85" s="89" t="s">
+      <c r="A85" s="111" t="s">
         <v>155</v>
       </c>
-      <c r="B85" s="90"/>
+      <c r="B85" s="112"/>
       <c r="C85" s="43"/>
-      <c r="D85" s="71">
+      <c r="D85" s="78">
         <f>SUM(D86:E86)</f>
         <v>8</v>
       </c>
-      <c r="E85" s="72"/>
-      <c r="F85" s="95">
+      <c r="E85" s="88"/>
+      <c r="F85" s="89">
         <f>SUM(F86:G86)</f>
         <v>0</v>
       </c>
-      <c r="G85" s="96"/>
+      <c r="G85" s="90"/>
       <c r="H85" s="29"/>
       <c r="I85" s="8"/>
       <c r="J85" s="8"/>
@@ -17258,20 +17260,20 @@
       <c r="GI85" s="29"/>
     </row>
     <row r="86" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A86" s="87" t="s">
+      <c r="A86" s="110" t="s">
         <v>156</v>
       </c>
-      <c r="B86" s="88"/>
+      <c r="B86" s="65"/>
       <c r="C86" s="27"/>
-      <c r="D86" s="65">
+      <c r="D86" s="62">
         <v>8</v>
       </c>
-      <c r="E86" s="66"/>
-      <c r="F86" s="65">
+      <c r="E86" s="63"/>
+      <c r="F86" s="62">
         <f>SUM(H86:GI86)</f>
         <v>0</v>
       </c>
-      <c r="G86" s="80"/>
+      <c r="G86" s="64"/>
       <c r="H86" s="26"/>
       <c r="I86" s="12"/>
       <c r="J86" s="12"/>
@@ -17458,20 +17460,20 @@
       <c r="GI86" s="32"/>
     </row>
     <row r="87" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A87" s="83" t="s">
+      <c r="A87" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="84"/>
+      <c r="B87" s="107"/>
       <c r="C87" s="43"/>
-      <c r="D87" s="71">
+      <c r="D87" s="78">
         <f>232-D90</f>
         <v>36.349999999999994</v>
       </c>
-      <c r="E87" s="72"/>
-      <c r="F87" s="71">
+      <c r="E87" s="88"/>
+      <c r="F87" s="78">
         <v>0</v>
       </c>
-      <c r="G87" s="75"/>
+      <c r="G87" s="80"/>
       <c r="H87" s="29"/>
       <c r="I87" s="8"/>
       <c r="J87" s="8"/>
@@ -17658,15 +17660,15 @@
       <c r="GI87" s="29"/>
     </row>
     <row r="88" spans="1:191" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="107" t="s">
+      <c r="A88" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="B88" s="108"/>
+      <c r="B88" s="102"/>
       <c r="C88" s="44"/>
-      <c r="D88" s="104"/>
-      <c r="E88" s="105"/>
-      <c r="F88" s="104"/>
-      <c r="G88" s="106"/>
+      <c r="D88" s="98"/>
+      <c r="E88" s="99"/>
+      <c r="F88" s="98"/>
+      <c r="G88" s="100"/>
       <c r="H88" s="28"/>
       <c r="I88" s="17"/>
       <c r="J88" s="17"/>
@@ -17905,21 +17907,21 @@
       <c r="AX89" s="3"/>
     </row>
     <row r="90" spans="1:191" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="102" t="s">
+      <c r="A90" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="103"/>
+      <c r="B90" s="97"/>
       <c r="C90" s="45"/>
-      <c r="D90" s="100">
+      <c r="D90" s="94">
         <f>SUM(D85,D83,D81,D62,D14)</f>
         <v>195.65</v>
       </c>
-      <c r="E90" s="101"/>
-      <c r="F90" s="100">
+      <c r="E90" s="95"/>
+      <c r="F90" s="94">
         <f>SUM(F85,F83,F81,F62,F14)</f>
-        <v>44.125999999999998</v>
-      </c>
-      <c r="G90" s="109"/>
+        <v>44.725999999999999</v>
+      </c>
+      <c r="G90" s="103"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
@@ -17966,132 +17968,190 @@
     </row>
   </sheetData>
   <mergeCells count="334">
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="BR13:BS13"/>
+    <mergeCell ref="BL13:BM13"/>
+    <mergeCell ref="BN13:BO13"/>
+    <mergeCell ref="BR12:DY12"/>
+    <mergeCell ref="DZ13:EA13"/>
+    <mergeCell ref="CL13:CM13"/>
+    <mergeCell ref="CN13:CO13"/>
+    <mergeCell ref="BT13:BU13"/>
+    <mergeCell ref="BV13:BW13"/>
+    <mergeCell ref="BX13:BY13"/>
+    <mergeCell ref="BZ13:CA13"/>
+    <mergeCell ref="CB13:CC13"/>
+    <mergeCell ref="CD13:CE13"/>
+    <mergeCell ref="CF13:CG13"/>
+    <mergeCell ref="CH13:CI13"/>
+    <mergeCell ref="CJ13:CK13"/>
+    <mergeCell ref="CP13:CQ13"/>
+    <mergeCell ref="CR13:CS13"/>
+    <mergeCell ref="CT13:CU13"/>
+    <mergeCell ref="CV13:CW13"/>
+    <mergeCell ref="CX13:CY13"/>
+    <mergeCell ref="CZ13:DA13"/>
+    <mergeCell ref="DB13:DC13"/>
+    <mergeCell ref="DD13:DE13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="P6:X6"/>
+    <mergeCell ref="P5:X5"/>
+    <mergeCell ref="P4:X4"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="H12:BQ12"/>
+    <mergeCell ref="BB13:BC13"/>
+    <mergeCell ref="BD13:BE13"/>
+    <mergeCell ref="BF13:BG13"/>
+    <mergeCell ref="BP13:BQ13"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="AF13:AG13"/>
+    <mergeCell ref="AH13:AI13"/>
+    <mergeCell ref="AJ13:AK13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="AL13:AM13"/>
+    <mergeCell ref="AN13:AO13"/>
+    <mergeCell ref="AP13:AQ13"/>
+    <mergeCell ref="AR13:AS13"/>
+    <mergeCell ref="AT13:AU13"/>
+    <mergeCell ref="AV13:AW13"/>
+    <mergeCell ref="AX13:AY13"/>
+    <mergeCell ref="AZ13:BA13"/>
+    <mergeCell ref="BH13:BI13"/>
+    <mergeCell ref="BJ13:BK13"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="P9:X9"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F11:G13"/>
+    <mergeCell ref="D11:E13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="DF13:DG13"/>
+    <mergeCell ref="DH13:DI13"/>
+    <mergeCell ref="DJ13:DK13"/>
+    <mergeCell ref="DL13:DM13"/>
+    <mergeCell ref="DN13:DO13"/>
+    <mergeCell ref="DP13:DQ13"/>
+    <mergeCell ref="DR13:DS13"/>
+    <mergeCell ref="DT13:DU13"/>
+    <mergeCell ref="DV13:DW13"/>
+    <mergeCell ref="FF13:FG13"/>
+    <mergeCell ref="DX13:DY13"/>
+    <mergeCell ref="FH13:FI13"/>
+    <mergeCell ref="FJ13:FK13"/>
+    <mergeCell ref="EB13:EC13"/>
+    <mergeCell ref="ED13:EE13"/>
+    <mergeCell ref="EF13:EG13"/>
+    <mergeCell ref="EH13:EI13"/>
+    <mergeCell ref="EJ13:EK13"/>
+    <mergeCell ref="EL13:EM13"/>
+    <mergeCell ref="EN13:EO13"/>
+    <mergeCell ref="EP13:EQ13"/>
+    <mergeCell ref="ER13:ES13"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="GD13:GE13"/>
+    <mergeCell ref="GF13:GG13"/>
+    <mergeCell ref="GH13:GI13"/>
+    <mergeCell ref="DZ12:GI12"/>
+    <mergeCell ref="FL13:FM13"/>
+    <mergeCell ref="FN13:FO13"/>
+    <mergeCell ref="FP13:FQ13"/>
+    <mergeCell ref="FR13:FS13"/>
+    <mergeCell ref="FT13:FU13"/>
+    <mergeCell ref="FV13:FW13"/>
+    <mergeCell ref="FX13:FY13"/>
+    <mergeCell ref="FZ13:GA13"/>
+    <mergeCell ref="GB13:GC13"/>
+    <mergeCell ref="ET13:EU13"/>
+    <mergeCell ref="EV13:EW13"/>
+    <mergeCell ref="EX13:EY13"/>
+    <mergeCell ref="EZ13:FA13"/>
+    <mergeCell ref="FB13:FC13"/>
+    <mergeCell ref="FD13:FE13"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="D32:E32"/>
@@ -18116,190 +18176,132 @@
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="GD13:GE13"/>
-    <mergeCell ref="GF13:GG13"/>
-    <mergeCell ref="GH13:GI13"/>
-    <mergeCell ref="DZ12:GI12"/>
-    <mergeCell ref="FL13:FM13"/>
-    <mergeCell ref="FN13:FO13"/>
-    <mergeCell ref="FP13:FQ13"/>
-    <mergeCell ref="FR13:FS13"/>
-    <mergeCell ref="FT13:FU13"/>
-    <mergeCell ref="FV13:FW13"/>
-    <mergeCell ref="FX13:FY13"/>
-    <mergeCell ref="FZ13:GA13"/>
-    <mergeCell ref="GB13:GC13"/>
-    <mergeCell ref="ET13:EU13"/>
-    <mergeCell ref="EV13:EW13"/>
-    <mergeCell ref="EX13:EY13"/>
-    <mergeCell ref="EZ13:FA13"/>
-    <mergeCell ref="FB13:FC13"/>
-    <mergeCell ref="FD13:FE13"/>
-    <mergeCell ref="FF13:FG13"/>
-    <mergeCell ref="DX13:DY13"/>
-    <mergeCell ref="FH13:FI13"/>
-    <mergeCell ref="FJ13:FK13"/>
-    <mergeCell ref="EB13:EC13"/>
-    <mergeCell ref="ED13:EE13"/>
-    <mergeCell ref="EF13:EG13"/>
-    <mergeCell ref="EH13:EI13"/>
-    <mergeCell ref="EJ13:EK13"/>
-    <mergeCell ref="EL13:EM13"/>
-    <mergeCell ref="EN13:EO13"/>
-    <mergeCell ref="EP13:EQ13"/>
-    <mergeCell ref="ER13:ES13"/>
-    <mergeCell ref="DF13:DG13"/>
-    <mergeCell ref="DH13:DI13"/>
-    <mergeCell ref="DJ13:DK13"/>
-    <mergeCell ref="DL13:DM13"/>
-    <mergeCell ref="DN13:DO13"/>
-    <mergeCell ref="DP13:DQ13"/>
-    <mergeCell ref="DR13:DS13"/>
-    <mergeCell ref="DT13:DU13"/>
-    <mergeCell ref="DV13:DW13"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="F90:G90"/>
-    <mergeCell ref="F87:G87"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="BH13:BI13"/>
-    <mergeCell ref="BJ13:BK13"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="P9:X9"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F11:G13"/>
-    <mergeCell ref="D11:E13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="AL13:AM13"/>
-    <mergeCell ref="AN13:AO13"/>
-    <mergeCell ref="AP13:AQ13"/>
-    <mergeCell ref="AR13:AS13"/>
-    <mergeCell ref="AT13:AU13"/>
-    <mergeCell ref="AV13:AW13"/>
-    <mergeCell ref="AX13:AY13"/>
-    <mergeCell ref="AZ13:BA13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="P6:X6"/>
-    <mergeCell ref="P5:X5"/>
-    <mergeCell ref="P4:X4"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="H12:BQ12"/>
-    <mergeCell ref="BB13:BC13"/>
-    <mergeCell ref="BD13:BE13"/>
-    <mergeCell ref="BF13:BG13"/>
-    <mergeCell ref="BP13:BQ13"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="AF13:AG13"/>
-    <mergeCell ref="AH13:AI13"/>
-    <mergeCell ref="AJ13:AK13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="BR13:BS13"/>
-    <mergeCell ref="BL13:BM13"/>
-    <mergeCell ref="BN13:BO13"/>
-    <mergeCell ref="BR12:DY12"/>
-    <mergeCell ref="DZ13:EA13"/>
-    <mergeCell ref="CL13:CM13"/>
-    <mergeCell ref="CN13:CO13"/>
-    <mergeCell ref="BT13:BU13"/>
-    <mergeCell ref="BV13:BW13"/>
-    <mergeCell ref="BX13:BY13"/>
-    <mergeCell ref="BZ13:CA13"/>
-    <mergeCell ref="CB13:CC13"/>
-    <mergeCell ref="CD13:CE13"/>
-    <mergeCell ref="CF13:CG13"/>
-    <mergeCell ref="CH13:CI13"/>
-    <mergeCell ref="CJ13:CK13"/>
-    <mergeCell ref="CP13:CQ13"/>
-    <mergeCell ref="CR13:CS13"/>
-    <mergeCell ref="CT13:CU13"/>
-    <mergeCell ref="CV13:CW13"/>
-    <mergeCell ref="CX13:CY13"/>
-    <mergeCell ref="CZ13:DA13"/>
-    <mergeCell ref="DB13:DC13"/>
-    <mergeCell ref="DD13:DE13"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Newest Version of Zeitplan
</commit_message>
<xml_diff>
--- a/Documents/Zeitplan.xlsx
+++ b/Documents/Zeitplan.xlsx
@@ -515,7 +515,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -578,6 +578,12 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="14"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -1049,7 +1055,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1164,24 +1170,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1194,31 +1182,32 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1226,6 +1215,42 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1234,9 +1259,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1284,40 +1306,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1418,8 +1430,8 @@
       <xdr:rowOff>51955</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>212420</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>528106</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>34638</xdr:rowOff>
     </xdr:to>
@@ -1788,39 +1800,48 @@
   <dimension ref="A1:GI90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BA20" sqref="BA20"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="191" width="5.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.77734375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="191" width="5.77734375" style="1" customWidth="1"/>
     <col min="192" max="256" width="3.33203125" style="1" customWidth="1"/>
     <col min="257" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:191" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
     </row>
     <row r="2" spans="1:191" x14ac:dyDescent="0.25">
       <c r="T2" s="9"/>
@@ -1853,17 +1874,17 @@
         <v>160</v>
       </c>
       <c r="N4" s="57"/>
-      <c r="P4" s="81" t="s">
+      <c r="P4" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="81"/>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="67"/>
+      <c r="V4" s="67"/>
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
     </row>
     <row r="5" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -1880,17 +1901,17 @@
       <c r="F5" s="5"/>
       <c r="G5" s="7"/>
       <c r="N5" s="24"/>
-      <c r="P5" s="81" t="s">
+      <c r="P5" s="67" t="s">
         <v>158</v>
       </c>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81"/>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="81"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
+      <c r="S5" s="67"/>
+      <c r="T5" s="67"/>
+      <c r="U5" s="67"/>
+      <c r="V5" s="67"/>
+      <c r="W5" s="67"/>
+      <c r="X5" s="67"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
@@ -1914,17 +1935,17 @@
         <v>15</v>
       </c>
       <c r="N6" s="16"/>
-      <c r="P6" s="81" t="s">
+      <c r="P6" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="81"/>
-      <c r="T6" s="81"/>
-      <c r="U6" s="81"/>
-      <c r="V6" s="81"/>
-      <c r="W6" s="81"/>
-      <c r="X6" s="81"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="67"/>
+      <c r="V6" s="67"/>
+      <c r="W6" s="67"/>
+      <c r="X6" s="67"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
@@ -1942,17 +1963,17 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="N7" s="21"/>
-      <c r="P7" s="81" t="s">
+      <c r="P7" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="81"/>
-      <c r="S7" s="81"/>
-      <c r="T7" s="81"/>
-      <c r="U7" s="81"/>
-      <c r="V7" s="81"/>
-      <c r="W7" s="81"/>
-      <c r="X7" s="81"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="67"/>
+      <c r="S7" s="67"/>
+      <c r="T7" s="67"/>
+      <c r="U7" s="67"/>
+      <c r="V7" s="67"/>
+      <c r="W7" s="67"/>
+      <c r="X7" s="67"/>
     </row>
     <row r="8" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1967,17 +1988,17 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="N8" s="20"/>
-      <c r="P8" s="113" t="s">
+      <c r="P8" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="113"/>
-      <c r="R8" s="113"/>
-      <c r="S8" s="113"/>
-      <c r="T8" s="113"/>
-      <c r="U8" s="113"/>
-      <c r="V8" s="113"/>
-      <c r="W8" s="113"/>
-      <c r="X8" s="113"/>
+      <c r="Q8" s="70"/>
+      <c r="R8" s="70"/>
+      <c r="S8" s="70"/>
+      <c r="T8" s="70"/>
+      <c r="U8" s="70"/>
+      <c r="V8" s="70"/>
+      <c r="W8" s="70"/>
+      <c r="X8" s="70"/>
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
@@ -1985,23 +2006,23 @@
       <c r="AC8" s="5"/>
     </row>
     <row r="9" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="118"/>
+      <c r="A9" s="68"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="12"/>
       <c r="N9" s="49"/>
-      <c r="P9" s="113" t="s">
+      <c r="P9" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="Q9" s="113"/>
-      <c r="R9" s="113"/>
-      <c r="S9" s="113"/>
-      <c r="T9" s="113"/>
-      <c r="U9" s="113"/>
-      <c r="V9" s="113"/>
-      <c r="W9" s="113"/>
-      <c r="X9" s="113"/>
+      <c r="Q9" s="70"/>
+      <c r="R9" s="70"/>
+      <c r="S9" s="70"/>
+      <c r="T9" s="70"/>
+      <c r="U9" s="70"/>
+      <c r="V9" s="70"/>
+      <c r="W9" s="70"/>
+      <c r="X9" s="70"/>
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
@@ -2011,7 +2032,7 @@
       <c r="AJ9" s="13"/>
     </row>
     <row r="10" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="118"/>
+      <c r="A10" s="68"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -2028,18 +2049,18 @@
       <c r="AC10" s="5"/>
     </row>
     <row r="11" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="118"/>
-      <c r="C11" s="116" t="s">
+      <c r="A11" s="68"/>
+      <c r="C11" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="114" t="s">
+      <c r="D11" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="114"/>
-      <c r="F11" s="114" t="s">
+      <c r="E11" s="76"/>
+      <c r="F11" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="114"/>
+      <c r="G11" s="76"/>
       <c r="T11" s="9"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
@@ -2052,596 +2073,596 @@
       <c r="AC11" s="5"/>
     </row>
     <row r="12" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="118"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="114"/>
-      <c r="G12" s="114"/>
-      <c r="H12" s="70" t="s">
+      <c r="A12" s="68"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="71"/>
-      <c r="N12" s="71"/>
-      <c r="O12" s="71"/>
-      <c r="P12" s="71"/>
-      <c r="Q12" s="71"/>
-      <c r="R12" s="71"/>
-      <c r="S12" s="71"/>
-      <c r="T12" s="71"/>
-      <c r="U12" s="71"/>
-      <c r="V12" s="71"/>
-      <c r="W12" s="71"/>
-      <c r="X12" s="71"/>
-      <c r="Y12" s="71"/>
-      <c r="Z12" s="71"/>
-      <c r="AA12" s="71"/>
-      <c r="AB12" s="71"/>
-      <c r="AC12" s="71"/>
-      <c r="AD12" s="71"/>
-      <c r="AE12" s="71"/>
-      <c r="AF12" s="71"/>
-      <c r="AG12" s="71"/>
-      <c r="AH12" s="71"/>
-      <c r="AI12" s="71"/>
-      <c r="AJ12" s="71"/>
-      <c r="AK12" s="71"/>
-      <c r="AL12" s="71"/>
-      <c r="AM12" s="71"/>
-      <c r="AN12" s="71"/>
-      <c r="AO12" s="71"/>
-      <c r="AP12" s="71"/>
-      <c r="AQ12" s="71"/>
-      <c r="AR12" s="71"/>
-      <c r="AS12" s="71"/>
-      <c r="AT12" s="71"/>
-      <c r="AU12" s="71"/>
-      <c r="AV12" s="71"/>
-      <c r="AW12" s="71"/>
-      <c r="AX12" s="71"/>
-      <c r="AY12" s="71"/>
-      <c r="AZ12" s="71"/>
-      <c r="BA12" s="71"/>
-      <c r="BB12" s="71"/>
-      <c r="BC12" s="71"/>
-      <c r="BD12" s="71"/>
-      <c r="BE12" s="71"/>
-      <c r="BF12" s="71"/>
-      <c r="BG12" s="71"/>
-      <c r="BH12" s="71"/>
-      <c r="BI12" s="71"/>
-      <c r="BJ12" s="71"/>
-      <c r="BK12" s="71"/>
-      <c r="BL12" s="71"/>
-      <c r="BM12" s="71"/>
-      <c r="BN12" s="71"/>
-      <c r="BO12" s="71"/>
-      <c r="BP12" s="71"/>
-      <c r="BQ12" s="119"/>
-      <c r="BR12" s="70" t="s">
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="63"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="63"/>
+      <c r="W12" s="63"/>
+      <c r="X12" s="63"/>
+      <c r="Y12" s="63"/>
+      <c r="Z12" s="63"/>
+      <c r="AA12" s="63"/>
+      <c r="AB12" s="63"/>
+      <c r="AC12" s="63"/>
+      <c r="AD12" s="63"/>
+      <c r="AE12" s="63"/>
+      <c r="AF12" s="63"/>
+      <c r="AG12" s="63"/>
+      <c r="AH12" s="63"/>
+      <c r="AI12" s="63"/>
+      <c r="AJ12" s="63"/>
+      <c r="AK12" s="63"/>
+      <c r="AL12" s="63"/>
+      <c r="AM12" s="63"/>
+      <c r="AN12" s="63"/>
+      <c r="AO12" s="63"/>
+      <c r="AP12" s="63"/>
+      <c r="AQ12" s="63"/>
+      <c r="AR12" s="63"/>
+      <c r="AS12" s="63"/>
+      <c r="AT12" s="63"/>
+      <c r="AU12" s="63"/>
+      <c r="AV12" s="63"/>
+      <c r="AW12" s="63"/>
+      <c r="AX12" s="63"/>
+      <c r="AY12" s="63"/>
+      <c r="AZ12" s="63"/>
+      <c r="BA12" s="63"/>
+      <c r="BB12" s="63"/>
+      <c r="BC12" s="63"/>
+      <c r="BD12" s="63"/>
+      <c r="BE12" s="63"/>
+      <c r="BF12" s="63"/>
+      <c r="BG12" s="63"/>
+      <c r="BH12" s="63"/>
+      <c r="BI12" s="63"/>
+      <c r="BJ12" s="63"/>
+      <c r="BK12" s="63"/>
+      <c r="BL12" s="63"/>
+      <c r="BM12" s="63"/>
+      <c r="BN12" s="63"/>
+      <c r="BO12" s="63"/>
+      <c r="BP12" s="63"/>
+      <c r="BQ12" s="64"/>
+      <c r="BR12" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="BS12" s="71"/>
-      <c r="BT12" s="71"/>
-      <c r="BU12" s="71"/>
-      <c r="BV12" s="71"/>
-      <c r="BW12" s="71"/>
-      <c r="BX12" s="71"/>
-      <c r="BY12" s="71"/>
-      <c r="BZ12" s="71"/>
-      <c r="CA12" s="71"/>
-      <c r="CB12" s="71"/>
-      <c r="CC12" s="71"/>
-      <c r="CD12" s="71"/>
-      <c r="CE12" s="71"/>
-      <c r="CF12" s="71"/>
-      <c r="CG12" s="71"/>
-      <c r="CH12" s="71"/>
-      <c r="CI12" s="71"/>
-      <c r="CJ12" s="71"/>
-      <c r="CK12" s="71"/>
-      <c r="CL12" s="71"/>
-      <c r="CM12" s="71"/>
-      <c r="CN12" s="71"/>
-      <c r="CO12" s="71"/>
-      <c r="CP12" s="71"/>
-      <c r="CQ12" s="71"/>
-      <c r="CR12" s="71"/>
-      <c r="CS12" s="71"/>
-      <c r="CT12" s="71"/>
-      <c r="CU12" s="71"/>
-      <c r="CV12" s="71"/>
-      <c r="CW12" s="71"/>
-      <c r="CX12" s="71"/>
-      <c r="CY12" s="71"/>
-      <c r="CZ12" s="71"/>
-      <c r="DA12" s="71"/>
-      <c r="DB12" s="71"/>
-      <c r="DC12" s="71"/>
-      <c r="DD12" s="71"/>
-      <c r="DE12" s="71"/>
-      <c r="DF12" s="71"/>
-      <c r="DG12" s="71"/>
-      <c r="DH12" s="71"/>
-      <c r="DI12" s="71"/>
-      <c r="DJ12" s="71"/>
-      <c r="DK12" s="71"/>
-      <c r="DL12" s="71"/>
-      <c r="DM12" s="71"/>
-      <c r="DN12" s="71"/>
-      <c r="DO12" s="71"/>
-      <c r="DP12" s="71"/>
-      <c r="DQ12" s="71"/>
-      <c r="DR12" s="71"/>
-      <c r="DS12" s="71"/>
-      <c r="DT12" s="71"/>
-      <c r="DU12" s="71"/>
-      <c r="DV12" s="71"/>
-      <c r="DW12" s="71"/>
-      <c r="DX12" s="71"/>
-      <c r="DY12" s="119"/>
-      <c r="DZ12" s="70" t="s">
+      <c r="BS12" s="63"/>
+      <c r="BT12" s="63"/>
+      <c r="BU12" s="63"/>
+      <c r="BV12" s="63"/>
+      <c r="BW12" s="63"/>
+      <c r="BX12" s="63"/>
+      <c r="BY12" s="63"/>
+      <c r="BZ12" s="63"/>
+      <c r="CA12" s="63"/>
+      <c r="CB12" s="63"/>
+      <c r="CC12" s="63"/>
+      <c r="CD12" s="63"/>
+      <c r="CE12" s="63"/>
+      <c r="CF12" s="63"/>
+      <c r="CG12" s="63"/>
+      <c r="CH12" s="63"/>
+      <c r="CI12" s="63"/>
+      <c r="CJ12" s="63"/>
+      <c r="CK12" s="63"/>
+      <c r="CL12" s="63"/>
+      <c r="CM12" s="63"/>
+      <c r="CN12" s="63"/>
+      <c r="CO12" s="63"/>
+      <c r="CP12" s="63"/>
+      <c r="CQ12" s="63"/>
+      <c r="CR12" s="63"/>
+      <c r="CS12" s="63"/>
+      <c r="CT12" s="63"/>
+      <c r="CU12" s="63"/>
+      <c r="CV12" s="63"/>
+      <c r="CW12" s="63"/>
+      <c r="CX12" s="63"/>
+      <c r="CY12" s="63"/>
+      <c r="CZ12" s="63"/>
+      <c r="DA12" s="63"/>
+      <c r="DB12" s="63"/>
+      <c r="DC12" s="63"/>
+      <c r="DD12" s="63"/>
+      <c r="DE12" s="63"/>
+      <c r="DF12" s="63"/>
+      <c r="DG12" s="63"/>
+      <c r="DH12" s="63"/>
+      <c r="DI12" s="63"/>
+      <c r="DJ12" s="63"/>
+      <c r="DK12" s="63"/>
+      <c r="DL12" s="63"/>
+      <c r="DM12" s="63"/>
+      <c r="DN12" s="63"/>
+      <c r="DO12" s="63"/>
+      <c r="DP12" s="63"/>
+      <c r="DQ12" s="63"/>
+      <c r="DR12" s="63"/>
+      <c r="DS12" s="63"/>
+      <c r="DT12" s="63"/>
+      <c r="DU12" s="63"/>
+      <c r="DV12" s="63"/>
+      <c r="DW12" s="63"/>
+      <c r="DX12" s="63"/>
+      <c r="DY12" s="64"/>
+      <c r="DZ12" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="EA12" s="71"/>
-      <c r="EB12" s="71"/>
-      <c r="EC12" s="71"/>
-      <c r="ED12" s="71"/>
-      <c r="EE12" s="71"/>
-      <c r="EF12" s="71"/>
-      <c r="EG12" s="71"/>
-      <c r="EH12" s="71"/>
-      <c r="EI12" s="71"/>
-      <c r="EJ12" s="71"/>
-      <c r="EK12" s="71"/>
-      <c r="EL12" s="71"/>
-      <c r="EM12" s="71"/>
-      <c r="EN12" s="71"/>
-      <c r="EO12" s="71"/>
-      <c r="EP12" s="71"/>
-      <c r="EQ12" s="71"/>
-      <c r="ER12" s="71"/>
-      <c r="ES12" s="71"/>
-      <c r="ET12" s="71"/>
-      <c r="EU12" s="71"/>
-      <c r="EV12" s="71"/>
-      <c r="EW12" s="71"/>
-      <c r="EX12" s="71"/>
-      <c r="EY12" s="71"/>
-      <c r="EZ12" s="71"/>
-      <c r="FA12" s="71"/>
-      <c r="FB12" s="71"/>
-      <c r="FC12" s="71"/>
-      <c r="FD12" s="71"/>
-      <c r="FE12" s="71"/>
-      <c r="FF12" s="71"/>
-      <c r="FG12" s="71"/>
-      <c r="FH12" s="71"/>
-      <c r="FI12" s="71"/>
-      <c r="FJ12" s="71"/>
-      <c r="FK12" s="71"/>
-      <c r="FL12" s="71"/>
-      <c r="FM12" s="71"/>
-      <c r="FN12" s="71"/>
-      <c r="FO12" s="71"/>
-      <c r="FP12" s="71"/>
-      <c r="FQ12" s="71"/>
-      <c r="FR12" s="71"/>
-      <c r="FS12" s="71"/>
-      <c r="FT12" s="71"/>
-      <c r="FU12" s="71"/>
-      <c r="FV12" s="71"/>
-      <c r="FW12" s="71"/>
-      <c r="FX12" s="71"/>
-      <c r="FY12" s="71"/>
-      <c r="FZ12" s="71"/>
-      <c r="GA12" s="71"/>
-      <c r="GB12" s="71"/>
-      <c r="GC12" s="71"/>
-      <c r="GD12" s="71"/>
-      <c r="GE12" s="71"/>
-      <c r="GF12" s="71"/>
-      <c r="GG12" s="71"/>
-      <c r="GH12" s="71"/>
-      <c r="GI12" s="72"/>
+      <c r="EA12" s="63"/>
+      <c r="EB12" s="63"/>
+      <c r="EC12" s="63"/>
+      <c r="ED12" s="63"/>
+      <c r="EE12" s="63"/>
+      <c r="EF12" s="63"/>
+      <c r="EG12" s="63"/>
+      <c r="EH12" s="63"/>
+      <c r="EI12" s="63"/>
+      <c r="EJ12" s="63"/>
+      <c r="EK12" s="63"/>
+      <c r="EL12" s="63"/>
+      <c r="EM12" s="63"/>
+      <c r="EN12" s="63"/>
+      <c r="EO12" s="63"/>
+      <c r="EP12" s="63"/>
+      <c r="EQ12" s="63"/>
+      <c r="ER12" s="63"/>
+      <c r="ES12" s="63"/>
+      <c r="ET12" s="63"/>
+      <c r="EU12" s="63"/>
+      <c r="EV12" s="63"/>
+      <c r="EW12" s="63"/>
+      <c r="EX12" s="63"/>
+      <c r="EY12" s="63"/>
+      <c r="EZ12" s="63"/>
+      <c r="FA12" s="63"/>
+      <c r="FB12" s="63"/>
+      <c r="FC12" s="63"/>
+      <c r="FD12" s="63"/>
+      <c r="FE12" s="63"/>
+      <c r="FF12" s="63"/>
+      <c r="FG12" s="63"/>
+      <c r="FH12" s="63"/>
+      <c r="FI12" s="63"/>
+      <c r="FJ12" s="63"/>
+      <c r="FK12" s="63"/>
+      <c r="FL12" s="63"/>
+      <c r="FM12" s="63"/>
+      <c r="FN12" s="63"/>
+      <c r="FO12" s="63"/>
+      <c r="FP12" s="63"/>
+      <c r="FQ12" s="63"/>
+      <c r="FR12" s="63"/>
+      <c r="FS12" s="63"/>
+      <c r="FT12" s="63"/>
+      <c r="FU12" s="63"/>
+      <c r="FV12" s="63"/>
+      <c r="FW12" s="63"/>
+      <c r="FX12" s="63"/>
+      <c r="FY12" s="63"/>
+      <c r="FZ12" s="63"/>
+      <c r="GA12" s="63"/>
+      <c r="GB12" s="63"/>
+      <c r="GC12" s="63"/>
+      <c r="GD12" s="63"/>
+      <c r="GE12" s="63"/>
+      <c r="GF12" s="63"/>
+      <c r="GG12" s="63"/>
+      <c r="GH12" s="63"/>
+      <c r="GI12" s="120"/>
     </row>
     <row r="13" spans="1:191" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="117"/>
-      <c r="D13" s="115"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="115"/>
-      <c r="H13" s="68">
+      <c r="C13" s="79"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="60">
         <v>1</v>
       </c>
-      <c r="I13" s="69"/>
-      <c r="J13" s="68">
+      <c r="I13" s="61"/>
+      <c r="J13" s="60">
         <v>2</v>
       </c>
-      <c r="K13" s="69"/>
-      <c r="L13" s="68">
+      <c r="K13" s="61"/>
+      <c r="L13" s="60">
         <v>3</v>
       </c>
-      <c r="M13" s="69"/>
-      <c r="N13" s="68">
+      <c r="M13" s="61"/>
+      <c r="N13" s="60">
         <v>4</v>
       </c>
-      <c r="O13" s="69"/>
-      <c r="P13" s="68">
+      <c r="O13" s="61"/>
+      <c r="P13" s="60">
         <v>5</v>
       </c>
-      <c r="Q13" s="69"/>
-      <c r="R13" s="68">
+      <c r="Q13" s="61"/>
+      <c r="R13" s="60">
         <v>6</v>
       </c>
-      <c r="S13" s="69"/>
-      <c r="T13" s="68">
+      <c r="S13" s="61"/>
+      <c r="T13" s="60">
         <v>7</v>
       </c>
-      <c r="U13" s="69"/>
-      <c r="V13" s="68">
+      <c r="U13" s="61"/>
+      <c r="V13" s="60">
         <v>8</v>
       </c>
-      <c r="W13" s="69"/>
-      <c r="X13" s="68">
+      <c r="W13" s="61"/>
+      <c r="X13" s="60">
         <v>9</v>
       </c>
-      <c r="Y13" s="69"/>
-      <c r="Z13" s="68">
+      <c r="Y13" s="61"/>
+      <c r="Z13" s="60">
         <v>10</v>
       </c>
-      <c r="AA13" s="69"/>
-      <c r="AB13" s="68">
+      <c r="AA13" s="61"/>
+      <c r="AB13" s="60">
         <v>11</v>
       </c>
-      <c r="AC13" s="69"/>
-      <c r="AD13" s="68">
+      <c r="AC13" s="61"/>
+      <c r="AD13" s="60">
         <v>12</v>
       </c>
-      <c r="AE13" s="69"/>
-      <c r="AF13" s="68">
+      <c r="AE13" s="61"/>
+      <c r="AF13" s="60">
         <v>13</v>
       </c>
-      <c r="AG13" s="69"/>
-      <c r="AH13" s="68">
+      <c r="AG13" s="61"/>
+      <c r="AH13" s="60">
         <v>14</v>
       </c>
-      <c r="AI13" s="69"/>
-      <c r="AJ13" s="68">
+      <c r="AI13" s="61"/>
+      <c r="AJ13" s="60">
         <v>15</v>
       </c>
-      <c r="AK13" s="69"/>
-      <c r="AL13" s="68">
+      <c r="AK13" s="61"/>
+      <c r="AL13" s="60">
         <v>16</v>
       </c>
-      <c r="AM13" s="69"/>
-      <c r="AN13" s="68">
+      <c r="AM13" s="61"/>
+      <c r="AN13" s="60">
         <v>17</v>
       </c>
-      <c r="AO13" s="69"/>
-      <c r="AP13" s="68">
+      <c r="AO13" s="61"/>
+      <c r="AP13" s="60">
         <v>18</v>
       </c>
-      <c r="AQ13" s="69"/>
-      <c r="AR13" s="68">
+      <c r="AQ13" s="61"/>
+      <c r="AR13" s="60">
         <v>19</v>
       </c>
-      <c r="AS13" s="69"/>
-      <c r="AT13" s="68">
+      <c r="AS13" s="61"/>
+      <c r="AT13" s="60">
         <v>20</v>
       </c>
-      <c r="AU13" s="69"/>
-      <c r="AV13" s="68">
+      <c r="AU13" s="61"/>
+      <c r="AV13" s="60">
         <v>21</v>
       </c>
-      <c r="AW13" s="69"/>
-      <c r="AX13" s="68">
+      <c r="AW13" s="61"/>
+      <c r="AX13" s="60">
         <v>22</v>
       </c>
-      <c r="AY13" s="69"/>
-      <c r="AZ13" s="68">
+      <c r="AY13" s="61"/>
+      <c r="AZ13" s="60">
         <v>23</v>
       </c>
-      <c r="BA13" s="69"/>
-      <c r="BB13" s="68">
+      <c r="BA13" s="61"/>
+      <c r="BB13" s="60">
         <v>24</v>
       </c>
-      <c r="BC13" s="69"/>
-      <c r="BD13" s="68">
+      <c r="BC13" s="61"/>
+      <c r="BD13" s="60">
         <v>25</v>
       </c>
-      <c r="BE13" s="69"/>
-      <c r="BF13" s="68">
+      <c r="BE13" s="61"/>
+      <c r="BF13" s="60">
         <v>26</v>
       </c>
-      <c r="BG13" s="69"/>
-      <c r="BH13" s="68">
+      <c r="BG13" s="61"/>
+      <c r="BH13" s="60">
         <v>27</v>
       </c>
-      <c r="BI13" s="69"/>
-      <c r="BJ13" s="68">
+      <c r="BI13" s="61"/>
+      <c r="BJ13" s="60">
         <v>28</v>
       </c>
-      <c r="BK13" s="69"/>
-      <c r="BL13" s="68">
+      <c r="BK13" s="61"/>
+      <c r="BL13" s="60">
         <v>29</v>
       </c>
-      <c r="BM13" s="69"/>
-      <c r="BN13" s="68">
+      <c r="BM13" s="61"/>
+      <c r="BN13" s="60">
         <v>30</v>
       </c>
-      <c r="BO13" s="69"/>
-      <c r="BP13" s="68">
+      <c r="BO13" s="61"/>
+      <c r="BP13" s="60">
         <v>31</v>
       </c>
-      <c r="BQ13" s="120"/>
-      <c r="BR13" s="68">
+      <c r="BQ13" s="69"/>
+      <c r="BR13" s="60">
         <v>1</v>
       </c>
-      <c r="BS13" s="69"/>
-      <c r="BT13" s="68">
+      <c r="BS13" s="61"/>
+      <c r="BT13" s="60">
         <v>2</v>
       </c>
-      <c r="BU13" s="69"/>
-      <c r="BV13" s="68">
+      <c r="BU13" s="61"/>
+      <c r="BV13" s="60">
         <v>3</v>
       </c>
-      <c r="BW13" s="69"/>
-      <c r="BX13" s="68">
+      <c r="BW13" s="61"/>
+      <c r="BX13" s="60">
         <v>4</v>
       </c>
-      <c r="BY13" s="69"/>
-      <c r="BZ13" s="68">
+      <c r="BY13" s="61"/>
+      <c r="BZ13" s="60">
         <v>5</v>
       </c>
-      <c r="CA13" s="69"/>
-      <c r="CB13" s="68">
+      <c r="CA13" s="61"/>
+      <c r="CB13" s="60">
         <v>6</v>
       </c>
-      <c r="CC13" s="69"/>
-      <c r="CD13" s="68">
+      <c r="CC13" s="61"/>
+      <c r="CD13" s="60">
         <v>7</v>
       </c>
-      <c r="CE13" s="69"/>
-      <c r="CF13" s="68">
+      <c r="CE13" s="61"/>
+      <c r="CF13" s="60">
         <v>8</v>
       </c>
-      <c r="CG13" s="69"/>
-      <c r="CH13" s="68">
+      <c r="CG13" s="61"/>
+      <c r="CH13" s="60">
         <v>9</v>
       </c>
-      <c r="CI13" s="69"/>
-      <c r="CJ13" s="68">
+      <c r="CI13" s="61"/>
+      <c r="CJ13" s="60">
         <v>10</v>
       </c>
-      <c r="CK13" s="69"/>
-      <c r="CL13" s="68">
+      <c r="CK13" s="61"/>
+      <c r="CL13" s="60">
         <v>11</v>
       </c>
-      <c r="CM13" s="69"/>
-      <c r="CN13" s="68">
+      <c r="CM13" s="61"/>
+      <c r="CN13" s="60">
         <v>12</v>
       </c>
-      <c r="CO13" s="69"/>
-      <c r="CP13" s="68">
+      <c r="CO13" s="61"/>
+      <c r="CP13" s="60">
         <v>13</v>
       </c>
-      <c r="CQ13" s="69"/>
-      <c r="CR13" s="68">
+      <c r="CQ13" s="61"/>
+      <c r="CR13" s="60">
         <v>14</v>
       </c>
-      <c r="CS13" s="69"/>
-      <c r="CT13" s="68">
+      <c r="CS13" s="61"/>
+      <c r="CT13" s="60">
         <v>15</v>
       </c>
-      <c r="CU13" s="69"/>
-      <c r="CV13" s="68">
+      <c r="CU13" s="61"/>
+      <c r="CV13" s="60">
         <v>16</v>
       </c>
-      <c r="CW13" s="69"/>
-      <c r="CX13" s="68">
+      <c r="CW13" s="61"/>
+      <c r="CX13" s="60">
         <v>17</v>
       </c>
-      <c r="CY13" s="69"/>
-      <c r="CZ13" s="68">
+      <c r="CY13" s="61"/>
+      <c r="CZ13" s="60">
         <v>18</v>
       </c>
-      <c r="DA13" s="69"/>
-      <c r="DB13" s="68">
+      <c r="DA13" s="61"/>
+      <c r="DB13" s="60">
         <v>19</v>
       </c>
-      <c r="DC13" s="69"/>
-      <c r="DD13" s="68">
+      <c r="DC13" s="61"/>
+      <c r="DD13" s="60">
         <v>20</v>
       </c>
-      <c r="DE13" s="69"/>
-      <c r="DF13" s="68">
+      <c r="DE13" s="61"/>
+      <c r="DF13" s="60">
         <v>21</v>
       </c>
-      <c r="DG13" s="69"/>
-      <c r="DH13" s="68">
+      <c r="DG13" s="61"/>
+      <c r="DH13" s="60">
         <v>22</v>
       </c>
-      <c r="DI13" s="69"/>
-      <c r="DJ13" s="68">
+      <c r="DI13" s="61"/>
+      <c r="DJ13" s="60">
         <v>23</v>
       </c>
-      <c r="DK13" s="69"/>
-      <c r="DL13" s="68">
+      <c r="DK13" s="61"/>
+      <c r="DL13" s="60">
         <v>24</v>
       </c>
-      <c r="DM13" s="69"/>
-      <c r="DN13" s="68">
+      <c r="DM13" s="61"/>
+      <c r="DN13" s="60">
         <v>25</v>
       </c>
-      <c r="DO13" s="69"/>
-      <c r="DP13" s="68">
+      <c r="DO13" s="61"/>
+      <c r="DP13" s="60">
         <v>26</v>
       </c>
-      <c r="DQ13" s="69"/>
-      <c r="DR13" s="68">
+      <c r="DQ13" s="61"/>
+      <c r="DR13" s="60">
         <v>27</v>
       </c>
-      <c r="DS13" s="69"/>
-      <c r="DT13" s="68">
+      <c r="DS13" s="61"/>
+      <c r="DT13" s="60">
         <v>28</v>
       </c>
-      <c r="DU13" s="69"/>
-      <c r="DV13" s="68">
+      <c r="DU13" s="61"/>
+      <c r="DV13" s="60">
         <v>29</v>
       </c>
-      <c r="DW13" s="69"/>
-      <c r="DX13" s="68">
+      <c r="DW13" s="61"/>
+      <c r="DX13" s="60">
         <v>30</v>
       </c>
-      <c r="DY13" s="69"/>
-      <c r="DZ13" s="68">
+      <c r="DY13" s="61"/>
+      <c r="DZ13" s="60">
         <v>1</v>
       </c>
-      <c r="EA13" s="69"/>
-      <c r="EB13" s="68">
+      <c r="EA13" s="61"/>
+      <c r="EB13" s="60">
         <v>2</v>
       </c>
-      <c r="EC13" s="69"/>
-      <c r="ED13" s="68">
+      <c r="EC13" s="61"/>
+      <c r="ED13" s="60">
         <v>3</v>
       </c>
-      <c r="EE13" s="69"/>
-      <c r="EF13" s="68">
+      <c r="EE13" s="61"/>
+      <c r="EF13" s="60">
         <v>4</v>
       </c>
-      <c r="EG13" s="69"/>
-      <c r="EH13" s="68">
+      <c r="EG13" s="61"/>
+      <c r="EH13" s="60">
         <v>5</v>
       </c>
-      <c r="EI13" s="69"/>
-      <c r="EJ13" s="68">
+      <c r="EI13" s="61"/>
+      <c r="EJ13" s="60">
         <v>6</v>
       </c>
-      <c r="EK13" s="69"/>
-      <c r="EL13" s="68">
+      <c r="EK13" s="61"/>
+      <c r="EL13" s="60">
         <v>7</v>
       </c>
-      <c r="EM13" s="69"/>
-      <c r="EN13" s="68">
+      <c r="EM13" s="61"/>
+      <c r="EN13" s="60">
         <v>8</v>
       </c>
-      <c r="EO13" s="69"/>
-      <c r="EP13" s="68">
+      <c r="EO13" s="61"/>
+      <c r="EP13" s="60">
         <v>9</v>
       </c>
-      <c r="EQ13" s="69"/>
-      <c r="ER13" s="68">
+      <c r="EQ13" s="61"/>
+      <c r="ER13" s="60">
         <v>10</v>
       </c>
-      <c r="ES13" s="69"/>
-      <c r="ET13" s="68">
+      <c r="ES13" s="61"/>
+      <c r="ET13" s="60">
         <v>11</v>
       </c>
-      <c r="EU13" s="69"/>
-      <c r="EV13" s="68">
+      <c r="EU13" s="61"/>
+      <c r="EV13" s="60">
         <v>12</v>
       </c>
-      <c r="EW13" s="69"/>
-      <c r="EX13" s="68">
+      <c r="EW13" s="61"/>
+      <c r="EX13" s="60">
         <v>13</v>
       </c>
-      <c r="EY13" s="69"/>
-      <c r="EZ13" s="68">
+      <c r="EY13" s="61"/>
+      <c r="EZ13" s="60">
         <v>14</v>
       </c>
-      <c r="FA13" s="69"/>
-      <c r="FB13" s="68">
+      <c r="FA13" s="61"/>
+      <c r="FB13" s="60">
         <v>15</v>
       </c>
-      <c r="FC13" s="69"/>
-      <c r="FD13" s="68">
+      <c r="FC13" s="61"/>
+      <c r="FD13" s="60">
         <v>16</v>
       </c>
-      <c r="FE13" s="69"/>
-      <c r="FF13" s="68">
+      <c r="FE13" s="61"/>
+      <c r="FF13" s="60">
         <v>17</v>
       </c>
-      <c r="FG13" s="69"/>
-      <c r="FH13" s="68">
+      <c r="FG13" s="61"/>
+      <c r="FH13" s="60">
         <v>18</v>
       </c>
-      <c r="FI13" s="69"/>
-      <c r="FJ13" s="68">
+      <c r="FI13" s="61"/>
+      <c r="FJ13" s="60">
         <v>19</v>
       </c>
-      <c r="FK13" s="69"/>
-      <c r="FL13" s="68">
+      <c r="FK13" s="61"/>
+      <c r="FL13" s="60">
         <v>20</v>
       </c>
-      <c r="FM13" s="69"/>
-      <c r="FN13" s="68">
+      <c r="FM13" s="61"/>
+      <c r="FN13" s="60">
         <v>21</v>
       </c>
-      <c r="FO13" s="69"/>
-      <c r="FP13" s="68">
+      <c r="FO13" s="61"/>
+      <c r="FP13" s="60">
         <v>22</v>
       </c>
-      <c r="FQ13" s="69"/>
-      <c r="FR13" s="68">
+      <c r="FQ13" s="61"/>
+      <c r="FR13" s="60">
         <v>23</v>
       </c>
-      <c r="FS13" s="69"/>
-      <c r="FT13" s="68">
+      <c r="FS13" s="61"/>
+      <c r="FT13" s="60">
         <v>24</v>
       </c>
-      <c r="FU13" s="69"/>
-      <c r="FV13" s="68">
+      <c r="FU13" s="61"/>
+      <c r="FV13" s="60">
         <v>25</v>
       </c>
-      <c r="FW13" s="69"/>
-      <c r="FX13" s="68">
+      <c r="FW13" s="61"/>
+      <c r="FX13" s="60">
         <v>26</v>
       </c>
-      <c r="FY13" s="69"/>
-      <c r="FZ13" s="68">
+      <c r="FY13" s="61"/>
+      <c r="FZ13" s="60">
         <v>27</v>
       </c>
-      <c r="GA13" s="69"/>
-      <c r="GB13" s="68">
+      <c r="GA13" s="61"/>
+      <c r="GB13" s="60">
         <v>28</v>
       </c>
-      <c r="GC13" s="69"/>
-      <c r="GD13" s="68">
+      <c r="GC13" s="61"/>
+      <c r="GD13" s="60">
         <v>29</v>
       </c>
-      <c r="GE13" s="69"/>
-      <c r="GF13" s="68">
+      <c r="GE13" s="61"/>
+      <c r="GF13" s="60">
         <v>30</v>
       </c>
-      <c r="GG13" s="69"/>
-      <c r="GH13" s="68">
+      <c r="GG13" s="61"/>
+      <c r="GH13" s="60">
         <v>31</v>
       </c>
-      <c r="GI13" s="69"/>
+      <c r="GI13" s="61"/>
     </row>
     <row r="14" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="113" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="75"/>
+      <c r="B14" s="114"/>
       <c r="C14" s="37"/>
-      <c r="D14" s="91">
+      <c r="D14" s="97">
         <f>SUM(D15:E61)</f>
         <v>51.050000000000011</v>
       </c>
-      <c r="E14" s="93"/>
-      <c r="F14" s="91">
+      <c r="E14" s="99"/>
+      <c r="F14" s="97">
         <f>SUM(F15:G61)</f>
         <v>44.725999999999999</v>
       </c>
-      <c r="G14" s="92"/>
+      <c r="G14" s="98"/>
       <c r="H14" s="18"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -2828,22 +2849,22 @@
       <c r="GI14" s="14"/>
     </row>
     <row r="15" spans="1:191" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="82" t="s">
+      <c r="A15" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="83"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="62">
+      <c r="D15" s="65">
         <v>1.5</v>
       </c>
-      <c r="E15" s="63"/>
-      <c r="F15" s="62">
+      <c r="E15" s="66"/>
+      <c r="F15" s="65">
         <f>SUM(H15:GI15)</f>
         <v>0.5</v>
       </c>
-      <c r="G15" s="64"/>
+      <c r="G15" s="80"/>
       <c r="H15" s="47"/>
       <c r="I15" s="12"/>
       <c r="J15" s="24">
@@ -3032,22 +3053,22 @@
       <c r="GI15" s="34"/>
     </row>
     <row r="16" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="67"/>
+      <c r="B16" s="82"/>
       <c r="C16" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="62">
+      <c r="D16" s="65">
         <v>0.6</v>
       </c>
-      <c r="E16" s="63"/>
-      <c r="F16" s="62">
+      <c r="E16" s="66"/>
+      <c r="F16" s="65">
         <f>SUM(H16:GI16)</f>
         <v>0.6</v>
       </c>
-      <c r="G16" s="64"/>
+      <c r="G16" s="80"/>
       <c r="H16" s="47"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
@@ -3236,22 +3257,22 @@
       <c r="GI16" s="32"/>
     </row>
     <row r="17" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="67"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="62">
+      <c r="D17" s="65">
         <v>1</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="62">
+      <c r="E17" s="66"/>
+      <c r="F17" s="65">
         <f>SUM(H17:GI17)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="64"/>
+      <c r="G17" s="80"/>
       <c r="H17" s="47"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
@@ -3442,22 +3463,22 @@
       <c r="GI17" s="32"/>
     </row>
     <row r="18" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="67"/>
+      <c r="B18" s="82"/>
       <c r="C18" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="62">
+      <c r="D18" s="65">
         <v>0.8</v>
       </c>
-      <c r="E18" s="63"/>
-      <c r="F18" s="62">
+      <c r="E18" s="66"/>
+      <c r="F18" s="65">
         <f t="shared" ref="F18:F60" si="0">SUM(H18:GI18)</f>
         <v>1.25</v>
       </c>
-      <c r="G18" s="64"/>
+      <c r="G18" s="80"/>
       <c r="H18" s="26"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
@@ -3648,22 +3669,22 @@
       <c r="GI18" s="32"/>
     </row>
     <row r="19" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="67"/>
+      <c r="B19" s="82"/>
       <c r="C19" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="62">
+      <c r="D19" s="65">
         <v>0.5</v>
       </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="62">
+      <c r="E19" s="66"/>
+      <c r="F19" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="64"/>
+      <c r="G19" s="80"/>
       <c r="H19" s="26"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
@@ -3850,22 +3871,22 @@
       <c r="GI19" s="36"/>
     </row>
     <row r="20" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="67"/>
+      <c r="B20" s="82"/>
       <c r="C20" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="62">
+      <c r="D20" s="65">
         <v>0.3</v>
       </c>
-      <c r="E20" s="63"/>
-      <c r="F20" s="62">
+      <c r="E20" s="66"/>
+      <c r="F20" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="64"/>
+      <c r="G20" s="80"/>
       <c r="H20" s="26"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -4052,22 +4073,22 @@
       <c r="GI20" s="36"/>
     </row>
     <row r="21" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="67"/>
+      <c r="B21" s="122"/>
       <c r="C21" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="62">
+      <c r="D21" s="65">
         <v>1</v>
       </c>
-      <c r="E21" s="63"/>
-      <c r="F21" s="62">
+      <c r="E21" s="66"/>
+      <c r="F21" s="65">
         <f t="shared" si="0"/>
         <v>0.16600000000000001</v>
       </c>
-      <c r="G21" s="64"/>
+      <c r="G21" s="80"/>
       <c r="H21" s="26"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
@@ -4256,22 +4277,22 @@
       <c r="GI21" s="36"/>
     </row>
     <row r="22" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="121" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="67"/>
+      <c r="B22" s="122"/>
       <c r="C22" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="62">
+      <c r="D22" s="65">
         <v>0.6</v>
       </c>
-      <c r="E22" s="63"/>
-      <c r="F22" s="62">
+      <c r="E22" s="66"/>
+      <c r="F22" s="65">
         <f t="shared" si="0"/>
         <v>0.66</v>
       </c>
-      <c r="G22" s="64"/>
+      <c r="G22" s="80"/>
       <c r="H22" s="26"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
@@ -4460,22 +4481,22 @@
       <c r="GI22" s="36"/>
     </row>
     <row r="23" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="67"/>
+      <c r="B23" s="122"/>
       <c r="C23" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="62">
+      <c r="D23" s="65">
         <v>0.6</v>
       </c>
-      <c r="E23" s="63"/>
-      <c r="F23" s="62">
+      <c r="E23" s="66"/>
+      <c r="F23" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="64"/>
+      <c r="G23" s="80"/>
       <c r="H23" s="26"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
@@ -4662,22 +4683,22 @@
       <c r="GI23" s="36"/>
     </row>
     <row r="24" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="67"/>
+      <c r="B24" s="122"/>
       <c r="C24" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="62">
+      <c r="D24" s="65">
         <v>3</v>
       </c>
-      <c r="E24" s="63"/>
-      <c r="F24" s="62">
+      <c r="E24" s="66"/>
+      <c r="F24" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="64"/>
+      <c r="G24" s="80"/>
       <c r="H24" s="26"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
@@ -4864,22 +4885,22 @@
       <c r="GI24" s="36"/>
     </row>
     <row r="25" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="67"/>
+      <c r="B25" s="122"/>
       <c r="C25" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="62">
+      <c r="D25" s="65">
         <v>1.5</v>
       </c>
-      <c r="E25" s="63"/>
-      <c r="F25" s="62">
+      <c r="E25" s="66"/>
+      <c r="F25" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="64"/>
+      <c r="G25" s="80"/>
       <c r="H25" s="26"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
@@ -5066,22 +5087,22 @@
       <c r="GI25" s="36"/>
     </row>
     <row r="26" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A26" s="66" t="s">
+      <c r="A26" s="121" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="67"/>
+      <c r="B26" s="122"/>
       <c r="C26" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="62">
+      <c r="D26" s="65">
         <v>1</v>
       </c>
-      <c r="E26" s="63"/>
-      <c r="F26" s="62">
+      <c r="E26" s="66"/>
+      <c r="F26" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="64"/>
+      <c r="G26" s="80"/>
       <c r="H26" s="26"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
@@ -5268,22 +5289,22 @@
       <c r="GI26" s="36"/>
     </row>
     <row r="27" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="67"/>
+      <c r="B27" s="82"/>
       <c r="C27" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="62">
+      <c r="D27" s="65">
         <v>1</v>
       </c>
-      <c r="E27" s="63"/>
-      <c r="F27" s="62">
+      <c r="E27" s="66"/>
+      <c r="F27" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G27" s="64"/>
+      <c r="G27" s="80"/>
       <c r="H27" s="26"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
@@ -5470,22 +5491,22 @@
       <c r="GI27" s="36"/>
     </row>
     <row r="28" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A28" s="66" t="s">
+      <c r="A28" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="67"/>
+      <c r="B28" s="82"/>
       <c r="C28" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="62">
+      <c r="D28" s="65">
         <v>1</v>
       </c>
-      <c r="E28" s="63"/>
-      <c r="F28" s="62">
+      <c r="E28" s="66"/>
+      <c r="F28" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G28" s="64"/>
+      <c r="G28" s="80"/>
       <c r="H28" s="26"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
@@ -5674,22 +5695,22 @@
       <c r="GI28" s="36"/>
     </row>
     <row r="29" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="67"/>
+      <c r="B29" s="82"/>
       <c r="C29" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="62">
+      <c r="D29" s="65">
         <v>1</v>
       </c>
-      <c r="E29" s="63"/>
-      <c r="F29" s="62">
+      <c r="E29" s="66"/>
+      <c r="F29" s="65">
         <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
-      <c r="G29" s="64"/>
+      <c r="G29" s="80"/>
       <c r="H29" s="26"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
@@ -5880,22 +5901,22 @@
       <c r="GI29" s="36"/>
     </row>
     <row r="30" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A30" s="66" t="s">
+      <c r="A30" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="67"/>
+      <c r="B30" s="82"/>
       <c r="C30" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="62">
+      <c r="D30" s="65">
         <v>1</v>
       </c>
-      <c r="E30" s="63"/>
-      <c r="F30" s="62">
+      <c r="E30" s="66"/>
+      <c r="F30" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G30" s="64"/>
+      <c r="G30" s="80"/>
       <c r="H30" s="26"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
@@ -6084,22 +6105,22 @@
       <c r="GI30" s="36"/>
     </row>
     <row r="31" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A31" s="66" t="s">
+      <c r="A31" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="67"/>
+      <c r="B31" s="82"/>
       <c r="C31" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="62">
+      <c r="D31" s="65">
         <v>4</v>
       </c>
-      <c r="E31" s="63"/>
-      <c r="F31" s="62">
+      <c r="E31" s="66"/>
+      <c r="F31" s="65">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G31" s="64"/>
+      <c r="G31" s="80"/>
       <c r="H31" s="26"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
@@ -6290,22 +6311,22 @@
       <c r="GI31" s="36"/>
     </row>
     <row r="32" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A32" s="66" t="s">
+      <c r="A32" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="67"/>
+      <c r="B32" s="82"/>
       <c r="C32" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="62">
+      <c r="D32" s="65">
         <v>0.6</v>
       </c>
-      <c r="E32" s="63"/>
-      <c r="F32" s="62">
+      <c r="E32" s="66"/>
+      <c r="F32" s="65">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G32" s="64"/>
+      <c r="G32" s="80"/>
       <c r="H32" s="26"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
@@ -6494,22 +6515,22 @@
       <c r="GI32" s="36"/>
     </row>
     <row r="33" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="67"/>
+      <c r="B33" s="82"/>
       <c r="C33" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="62">
+      <c r="D33" s="65">
         <v>0.5</v>
       </c>
-      <c r="E33" s="63"/>
-      <c r="F33" s="62">
+      <c r="E33" s="66"/>
+      <c r="F33" s="65">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G33" s="64"/>
+      <c r="G33" s="80"/>
       <c r="H33" s="26"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
@@ -6698,22 +6719,22 @@
       <c r="GI33" s="36"/>
     </row>
     <row r="34" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A34" s="66" t="s">
+      <c r="A34" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="67"/>
+      <c r="B34" s="82"/>
       <c r="C34" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="62">
+      <c r="D34" s="65">
         <v>0.3</v>
       </c>
-      <c r="E34" s="63"/>
-      <c r="F34" s="62">
+      <c r="E34" s="66"/>
+      <c r="F34" s="65">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G34" s="64"/>
+      <c r="G34" s="80"/>
       <c r="H34" s="26"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
@@ -6902,22 +6923,22 @@
       <c r="GI34" s="36"/>
     </row>
     <row r="35" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A35" s="66" t="s">
+      <c r="A35" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="67"/>
+      <c r="B35" s="82"/>
       <c r="C35" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="62">
+      <c r="D35" s="65">
         <v>0.3</v>
       </c>
-      <c r="E35" s="63"/>
-      <c r="F35" s="62">
+      <c r="E35" s="66"/>
+      <c r="F35" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G35" s="64"/>
+      <c r="G35" s="80"/>
       <c r="H35" s="26"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
@@ -7104,22 +7125,22 @@
       <c r="GI35" s="36"/>
     </row>
     <row r="36" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A36" s="66" t="s">
+      <c r="A36" s="81" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="67"/>
+      <c r="B36" s="82"/>
       <c r="C36" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="62">
+      <c r="D36" s="65">
         <v>1.5</v>
       </c>
-      <c r="E36" s="63"/>
-      <c r="F36" s="62">
+      <c r="E36" s="66"/>
+      <c r="F36" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G36" s="64"/>
+      <c r="G36" s="80"/>
       <c r="H36" s="26"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
@@ -7306,22 +7327,22 @@
       <c r="GI36" s="36"/>
     </row>
     <row r="37" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A37" s="66" t="s">
+      <c r="A37" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="67"/>
+      <c r="B37" s="82"/>
       <c r="C37" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="62">
+      <c r="D37" s="65">
         <v>0.5</v>
       </c>
-      <c r="E37" s="63"/>
-      <c r="F37" s="62">
+      <c r="E37" s="66"/>
+      <c r="F37" s="65">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G37" s="64"/>
+      <c r="G37" s="80"/>
       <c r="H37" s="26"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
@@ -7510,22 +7531,22 @@
       <c r="GI37" s="36"/>
     </row>
     <row r="38" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A38" s="66" t="s">
+      <c r="A38" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="67"/>
+      <c r="B38" s="82"/>
       <c r="C38" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="62">
+      <c r="D38" s="65">
         <v>0.25</v>
       </c>
-      <c r="E38" s="63"/>
-      <c r="F38" s="62">
+      <c r="E38" s="66"/>
+      <c r="F38" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G38" s="64"/>
+      <c r="G38" s="80"/>
       <c r="H38" s="26"/>
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
@@ -7714,22 +7735,22 @@
       <c r="GI38" s="36"/>
     </row>
     <row r="39" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="67"/>
+      <c r="B39" s="82"/>
       <c r="C39" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="62">
+      <c r="D39" s="65">
         <v>0.5</v>
       </c>
-      <c r="E39" s="63"/>
-      <c r="F39" s="62">
+      <c r="E39" s="66"/>
+      <c r="F39" s="65">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="G39" s="64"/>
+      <c r="G39" s="80"/>
       <c r="H39" s="26"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
@@ -7918,22 +7939,22 @@
       <c r="GI39" s="36"/>
     </row>
     <row r="40" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A40" s="66" t="s">
+      <c r="A40" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="67"/>
+      <c r="B40" s="82"/>
       <c r="C40" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="62">
+      <c r="D40" s="65">
         <v>0.5</v>
       </c>
-      <c r="E40" s="63"/>
-      <c r="F40" s="62">
+      <c r="E40" s="66"/>
+      <c r="F40" s="65">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G40" s="64"/>
+      <c r="G40" s="80"/>
       <c r="H40" s="26"/>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
@@ -8122,22 +8143,22 @@
       <c r="GI40" s="36"/>
     </row>
     <row r="41" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="67"/>
+      <c r="B41" s="82"/>
       <c r="C41" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="62">
+      <c r="D41" s="65">
         <v>0.3</v>
       </c>
-      <c r="E41" s="63"/>
-      <c r="F41" s="62">
+      <c r="E41" s="66"/>
+      <c r="F41" s="65">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G41" s="64"/>
+      <c r="G41" s="80"/>
       <c r="H41" s="26"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
@@ -8326,22 +8347,22 @@
       <c r="GI41" s="36"/>
     </row>
     <row r="42" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A42" s="66" t="s">
+      <c r="A42" s="81" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="67"/>
+      <c r="B42" s="82"/>
       <c r="C42" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="62">
+      <c r="D42" s="65">
         <v>0.5</v>
       </c>
-      <c r="E42" s="63"/>
-      <c r="F42" s="62">
+      <c r="E42" s="66"/>
+      <c r="F42" s="65">
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-      <c r="G42" s="64"/>
+      <c r="G42" s="80"/>
       <c r="H42" s="26"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
@@ -8530,22 +8551,22 @@
       <c r="GI42" s="36"/>
     </row>
     <row r="43" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A43" s="66" t="s">
+      <c r="A43" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="67"/>
+      <c r="B43" s="82"/>
       <c r="C43" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D43" s="62">
+      <c r="D43" s="65">
         <v>1.3</v>
       </c>
-      <c r="E43" s="63"/>
-      <c r="F43" s="62">
+      <c r="E43" s="66"/>
+      <c r="F43" s="65">
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
-      <c r="G43" s="64"/>
+      <c r="G43" s="80"/>
       <c r="H43" s="26"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
@@ -8736,22 +8757,22 @@
       <c r="GI43" s="36"/>
     </row>
     <row r="44" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="66" t="s">
+      <c r="A44" s="81" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="67"/>
+      <c r="B44" s="82"/>
       <c r="C44" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="62">
+      <c r="D44" s="65">
         <v>1.3</v>
       </c>
-      <c r="E44" s="63"/>
-      <c r="F44" s="62">
+      <c r="E44" s="66"/>
+      <c r="F44" s="65">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G44" s="64"/>
+      <c r="G44" s="80"/>
       <c r="H44" s="26"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
@@ -8940,22 +8961,22 @@
       <c r="GI44" s="36"/>
     </row>
     <row r="45" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A45" s="66" t="s">
+      <c r="A45" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="67"/>
+      <c r="B45" s="82"/>
       <c r="C45" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="62">
+      <c r="D45" s="65">
         <v>1</v>
       </c>
-      <c r="E45" s="63"/>
-      <c r="F45" s="62">
+      <c r="E45" s="66"/>
+      <c r="F45" s="65">
         <f t="shared" si="0"/>
         <v>1.05</v>
       </c>
-      <c r="G45" s="64"/>
+      <c r="G45" s="80"/>
       <c r="H45" s="26"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
@@ -9146,22 +9167,22 @@
       <c r="GI45" s="36"/>
     </row>
     <row r="46" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A46" s="66" t="s">
+      <c r="A46" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="67"/>
+      <c r="B46" s="82"/>
       <c r="C46" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="D46" s="62">
+      <c r="D46" s="65">
         <v>1</v>
       </c>
-      <c r="E46" s="63"/>
-      <c r="F46" s="62">
+      <c r="E46" s="66"/>
+      <c r="F46" s="65">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="G46" s="64"/>
+      <c r="G46" s="80"/>
       <c r="H46" s="26"/>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
@@ -9350,22 +9371,22 @@
       <c r="GI46" s="36"/>
     </row>
     <row r="47" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A47" s="66" t="s">
+      <c r="A47" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="67"/>
+      <c r="B47" s="82"/>
       <c r="C47" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="D47" s="62">
+      <c r="D47" s="65">
         <v>1</v>
       </c>
-      <c r="E47" s="63"/>
-      <c r="F47" s="62">
+      <c r="E47" s="66"/>
+      <c r="F47" s="65">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="G47" s="64"/>
+      <c r="G47" s="80"/>
       <c r="H47" s="26"/>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
@@ -9554,22 +9575,22 @@
       <c r="GI47" s="36"/>
     </row>
     <row r="48" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A48" s="66" t="s">
+      <c r="A48" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="B48" s="67"/>
+      <c r="B48" s="82"/>
       <c r="C48" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D48" s="62">
+      <c r="D48" s="65">
         <v>0.3</v>
       </c>
-      <c r="E48" s="63"/>
-      <c r="F48" s="62">
+      <c r="E48" s="66"/>
+      <c r="F48" s="65">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G48" s="64"/>
+      <c r="G48" s="80"/>
       <c r="H48" s="26"/>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
@@ -9758,22 +9779,22 @@
       <c r="GI48" s="36"/>
     </row>
     <row r="49" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A49" s="66" t="s">
+      <c r="A49" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="67"/>
+      <c r="B49" s="82"/>
       <c r="C49" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="62">
+      <c r="D49" s="65">
         <v>2</v>
       </c>
-      <c r="E49" s="63"/>
-      <c r="F49" s="62">
+      <c r="E49" s="66"/>
+      <c r="F49" s="65">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G49" s="64"/>
+      <c r="G49" s="80"/>
       <c r="H49" s="26"/>
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
@@ -9964,22 +9985,22 @@
       <c r="GI49" s="36"/>
     </row>
     <row r="50" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A50" s="66" t="s">
+      <c r="A50" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="67"/>
+      <c r="B50" s="82"/>
       <c r="C50" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="D50" s="62">
+      <c r="D50" s="65">
         <v>2</v>
       </c>
-      <c r="E50" s="63"/>
-      <c r="F50" s="62">
+      <c r="E50" s="66"/>
+      <c r="F50" s="65">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G50" s="64"/>
+      <c r="G50" s="80"/>
       <c r="H50" s="26"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
@@ -10170,22 +10191,22 @@
       <c r="GI50" s="36"/>
     </row>
     <row r="51" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A51" s="66" t="s">
+      <c r="A51" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="67"/>
+      <c r="B51" s="82"/>
       <c r="C51" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D51" s="62">
+      <c r="D51" s="65">
         <v>2</v>
       </c>
-      <c r="E51" s="63"/>
-      <c r="F51" s="62">
+      <c r="E51" s="66"/>
+      <c r="F51" s="65">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G51" s="64"/>
+      <c r="G51" s="80"/>
       <c r="H51" s="26"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
@@ -10376,22 +10397,22 @@
       <c r="GI51" s="36"/>
     </row>
     <row r="52" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A52" s="66" t="s">
+      <c r="A52" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="67"/>
+      <c r="B52" s="82"/>
       <c r="C52" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="62">
+      <c r="D52" s="65">
         <v>2</v>
       </c>
-      <c r="E52" s="63"/>
-      <c r="F52" s="62">
+      <c r="E52" s="66"/>
+      <c r="F52" s="65">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G52" s="64"/>
+      <c r="G52" s="80"/>
       <c r="H52" s="26"/>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
@@ -10582,22 +10603,22 @@
       <c r="GI52" s="36"/>
     </row>
     <row r="53" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A53" s="66" t="s">
+      <c r="A53" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="67"/>
+      <c r="B53" s="82"/>
       <c r="C53" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D53" s="62">
+      <c r="D53" s="65">
         <v>2</v>
       </c>
-      <c r="E53" s="63"/>
-      <c r="F53" s="62">
+      <c r="E53" s="66"/>
+      <c r="F53" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G53" s="64"/>
+      <c r="G53" s="80"/>
       <c r="H53" s="26"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
@@ -10784,22 +10805,22 @@
       <c r="GI53" s="36"/>
     </row>
     <row r="54" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A54" s="66" t="s">
+      <c r="A54" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="67"/>
+      <c r="B54" s="82"/>
       <c r="C54" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="D54" s="62">
+      <c r="D54" s="65">
         <v>0.25</v>
       </c>
-      <c r="E54" s="63"/>
-      <c r="F54" s="62">
+      <c r="E54" s="66"/>
+      <c r="F54" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G54" s="64"/>
+      <c r="G54" s="80"/>
       <c r="H54" s="26"/>
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
@@ -10986,22 +11007,22 @@
       <c r="GI54" s="36"/>
     </row>
     <row r="55" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A55" s="66" t="s">
+      <c r="A55" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="67"/>
+      <c r="B55" s="82"/>
       <c r="C55" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="D55" s="62">
+      <c r="D55" s="65">
         <v>1</v>
       </c>
-      <c r="E55" s="63"/>
-      <c r="F55" s="62">
+      <c r="E55" s="66"/>
+      <c r="F55" s="65">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G55" s="64"/>
+      <c r="G55" s="80"/>
       <c r="H55" s="26"/>
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
@@ -11192,22 +11213,22 @@
       <c r="GI55" s="36"/>
     </row>
     <row r="56" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A56" s="66" t="s">
+      <c r="A56" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="67"/>
+      <c r="B56" s="82"/>
       <c r="C56" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="D56" s="62">
+      <c r="D56" s="65">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E56" s="63"/>
-      <c r="F56" s="62">
+      <c r="E56" s="66"/>
+      <c r="F56" s="65">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G56" s="64"/>
+      <c r="G56" s="80"/>
       <c r="H56" s="26"/>
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
@@ -11398,22 +11419,22 @@
       <c r="GI56" s="36"/>
     </row>
     <row r="57" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A57" s="66" t="s">
+      <c r="A57" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="67"/>
+      <c r="B57" s="82"/>
       <c r="C57" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="D57" s="62">
+      <c r="D57" s="65">
         <v>1.75</v>
       </c>
-      <c r="E57" s="63"/>
-      <c r="F57" s="62">
+      <c r="E57" s="66"/>
+      <c r="F57" s="65">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G57" s="64"/>
+      <c r="G57" s="80"/>
       <c r="H57" s="26"/>
       <c r="I57" s="12"/>
       <c r="J57" s="12"/>
@@ -11602,22 +11623,22 @@
       <c r="GI57" s="36"/>
     </row>
     <row r="58" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A58" s="66" t="s">
+      <c r="A58" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="B58" s="67"/>
+      <c r="B58" s="82"/>
       <c r="C58" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="D58" s="62">
+      <c r="D58" s="65">
         <v>0.6</v>
       </c>
-      <c r="E58" s="63"/>
-      <c r="F58" s="62">
+      <c r="E58" s="66"/>
+      <c r="F58" s="65">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G58" s="64"/>
+      <c r="G58" s="80"/>
       <c r="H58" s="26"/>
       <c r="I58" s="12"/>
       <c r="J58" s="12"/>
@@ -11806,22 +11827,22 @@
       <c r="GI58" s="36"/>
     </row>
     <row r="59" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="66" t="s">
+      <c r="A59" s="81" t="s">
         <v>111</v>
       </c>
-      <c r="B59" s="67"/>
+      <c r="B59" s="82"/>
       <c r="C59" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="62">
+      <c r="D59" s="65">
         <v>1</v>
       </c>
-      <c r="E59" s="63"/>
-      <c r="F59" s="62">
+      <c r="E59" s="66"/>
+      <c r="F59" s="65">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G59" s="64"/>
+      <c r="G59" s="80"/>
       <c r="H59" s="26"/>
       <c r="I59" s="12"/>
       <c r="J59" s="12"/>
@@ -12012,22 +12033,22 @@
       <c r="GI59" s="36"/>
     </row>
     <row r="60" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A60" s="66" t="s">
+      <c r="A60" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="B60" s="67"/>
+      <c r="B60" s="82"/>
       <c r="C60" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="D60" s="62">
+      <c r="D60" s="65">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E60" s="63"/>
-      <c r="F60" s="62">
+      <c r="E60" s="66"/>
+      <c r="F60" s="65">
         <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
-      <c r="G60" s="64"/>
+      <c r="G60" s="80"/>
       <c r="H60" s="26"/>
       <c r="I60" s="12"/>
       <c r="J60" s="12"/>
@@ -12216,22 +12237,22 @@
       <c r="GI60" s="36"/>
     </row>
     <row r="61" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A61" s="66" t="s">
+      <c r="A61" s="81" t="s">
         <v>115</v>
       </c>
-      <c r="B61" s="67"/>
+      <c r="B61" s="82"/>
       <c r="C61" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="D61" s="62">
+      <c r="D61" s="65">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E61" s="63"/>
-      <c r="F61" s="62">
+      <c r="E61" s="66"/>
+      <c r="F61" s="65">
         <f>SUM(H61:GI61)</f>
         <v>1</v>
       </c>
-      <c r="G61" s="64"/>
+      <c r="G61" s="80"/>
       <c r="H61" s="26"/>
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
@@ -12420,21 +12441,21 @@
       <c r="GI61" s="36"/>
     </row>
     <row r="62" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A62" s="76" t="s">
+      <c r="A62" s="115" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="77"/>
+      <c r="B62" s="116"/>
       <c r="C62" s="39"/>
-      <c r="D62" s="78">
+      <c r="D62" s="71">
         <f>SUM(D63:E80)</f>
         <v>88.6</v>
       </c>
-      <c r="E62" s="79"/>
-      <c r="F62" s="78">
+      <c r="E62" s="117"/>
+      <c r="F62" s="71">
         <f>SUM(F63:G80)</f>
         <v>0</v>
       </c>
-      <c r="G62" s="80"/>
+      <c r="G62" s="75"/>
       <c r="H62" s="29"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
@@ -12621,22 +12642,22 @@
       <c r="GI62" s="29"/>
     </row>
     <row r="63" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="60" t="s">
+      <c r="A63" s="118" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="61"/>
+      <c r="B63" s="119"/>
       <c r="C63" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D63" s="62">
+      <c r="D63" s="65">
         <v>0.6</v>
       </c>
-      <c r="E63" s="63"/>
-      <c r="F63" s="62">
+      <c r="E63" s="66"/>
+      <c r="F63" s="65">
         <f>SUM(H63:GI63)</f>
         <v>0</v>
       </c>
-      <c r="G63" s="64"/>
+      <c r="G63" s="80"/>
       <c r="H63" s="47"/>
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
@@ -12823,22 +12844,22 @@
       <c r="GI63" s="32"/>
     </row>
     <row r="64" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="60" t="s">
+      <c r="A64" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="B64" s="61"/>
+      <c r="B64" s="119"/>
       <c r="C64" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D64" s="62">
+      <c r="D64" s="65">
         <v>1.5</v>
       </c>
-      <c r="E64" s="63"/>
-      <c r="F64" s="62">
+      <c r="E64" s="66"/>
+      <c r="F64" s="65">
         <f>SUM(H64:GI64)</f>
         <v>0</v>
       </c>
-      <c r="G64" s="64"/>
+      <c r="G64" s="80"/>
       <c r="H64" s="47"/>
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
@@ -13025,22 +13046,22 @@
       <c r="GI64" s="32"/>
     </row>
     <row r="65" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A65" s="60" t="s">
+      <c r="A65" s="118" t="s">
         <v>123</v>
       </c>
-      <c r="B65" s="61"/>
+      <c r="B65" s="119"/>
       <c r="C65" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D65" s="62">
+      <c r="D65" s="65">
         <v>1</v>
       </c>
-      <c r="E65" s="63"/>
-      <c r="F65" s="62">
+      <c r="E65" s="66"/>
+      <c r="F65" s="65">
         <f t="shared" ref="F65:F80" si="1">SUM(H65:GI65)</f>
         <v>0</v>
       </c>
-      <c r="G65" s="64"/>
+      <c r="G65" s="80"/>
       <c r="H65" s="47"/>
       <c r="I65" s="12"/>
       <c r="J65" s="12"/>
@@ -13227,22 +13248,22 @@
       <c r="GI65" s="32"/>
     </row>
     <row r="66" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A66" s="60" t="s">
+      <c r="A66" s="118" t="s">
         <v>125</v>
       </c>
-      <c r="B66" s="61"/>
+      <c r="B66" s="119"/>
       <c r="C66" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D66" s="62">
+      <c r="D66" s="65">
         <v>0.5</v>
       </c>
-      <c r="E66" s="63"/>
-      <c r="F66" s="62">
+      <c r="E66" s="66"/>
+      <c r="F66" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G66" s="64"/>
+      <c r="G66" s="80"/>
       <c r="H66" s="47"/>
       <c r="I66" s="12"/>
       <c r="J66" s="12"/>
@@ -13429,22 +13450,22 @@
       <c r="GI66" s="32"/>
     </row>
     <row r="67" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A67" s="60" t="s">
+      <c r="A67" s="118" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="61"/>
+      <c r="B67" s="119"/>
       <c r="C67" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D67" s="62">
+      <c r="D67" s="65">
         <v>1</v>
       </c>
-      <c r="E67" s="63"/>
-      <c r="F67" s="62">
+      <c r="E67" s="66"/>
+      <c r="F67" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G67" s="64"/>
+      <c r="G67" s="80"/>
       <c r="H67" s="47"/>
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
@@ -13631,22 +13652,22 @@
       <c r="GI67" s="32"/>
     </row>
     <row r="68" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A68" s="60" t="s">
+      <c r="A68" s="118" t="s">
         <v>129</v>
       </c>
-      <c r="B68" s="61"/>
+      <c r="B68" s="119"/>
       <c r="C68" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D68" s="62">
+      <c r="D68" s="65">
         <v>1</v>
       </c>
-      <c r="E68" s="63"/>
-      <c r="F68" s="62">
+      <c r="E68" s="66"/>
+      <c r="F68" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G68" s="64"/>
+      <c r="G68" s="80"/>
       <c r="H68" s="47"/>
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
@@ -13833,22 +13854,22 @@
       <c r="GI68" s="32"/>
     </row>
     <row r="69" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A69" s="60" t="s">
+      <c r="A69" s="118" t="s">
         <v>131</v>
       </c>
-      <c r="B69" s="61"/>
+      <c r="B69" s="119"/>
       <c r="C69" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="D69" s="62">
+      <c r="D69" s="65">
         <v>4</v>
       </c>
-      <c r="E69" s="63"/>
-      <c r="F69" s="62">
+      <c r="E69" s="66"/>
+      <c r="F69" s="65">
         <f>SUM(H69:GI69)</f>
         <v>0</v>
       </c>
-      <c r="G69" s="64"/>
+      <c r="G69" s="80"/>
       <c r="H69" s="47"/>
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
@@ -14035,22 +14056,22 @@
       <c r="GI69" s="32"/>
     </row>
     <row r="70" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A70" s="60" t="s">
+      <c r="A70" s="118" t="s">
         <v>133</v>
       </c>
-      <c r="B70" s="61"/>
+      <c r="B70" s="119"/>
       <c r="C70" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="D70" s="62">
+      <c r="D70" s="65">
         <v>8</v>
       </c>
-      <c r="E70" s="63"/>
-      <c r="F70" s="62">
+      <c r="E70" s="66"/>
+      <c r="F70" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G70" s="64"/>
+      <c r="G70" s="80"/>
       <c r="H70" s="47"/>
       <c r="I70" s="12"/>
       <c r="J70" s="12"/>
@@ -14237,22 +14258,22 @@
       <c r="GI70" s="32"/>
     </row>
     <row r="71" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A71" s="60" t="s">
+      <c r="A71" s="118" t="s">
         <v>135</v>
       </c>
-      <c r="B71" s="61"/>
+      <c r="B71" s="119"/>
       <c r="C71" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="D71" s="62">
+      <c r="D71" s="65">
         <v>1</v>
       </c>
-      <c r="E71" s="63"/>
-      <c r="F71" s="62">
+      <c r="E71" s="66"/>
+      <c r="F71" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G71" s="64"/>
+      <c r="G71" s="80"/>
       <c r="H71" s="47"/>
       <c r="I71" s="12"/>
       <c r="J71" s="12"/>
@@ -14439,22 +14460,22 @@
       <c r="GI71" s="32"/>
     </row>
     <row r="72" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A72" s="60" t="s">
+      <c r="A72" s="118" t="s">
         <v>137</v>
       </c>
-      <c r="B72" s="61"/>
+      <c r="B72" s="119"/>
       <c r="C72" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="D72" s="62">
+      <c r="D72" s="65">
         <v>1</v>
       </c>
-      <c r="E72" s="63"/>
-      <c r="F72" s="62">
+      <c r="E72" s="66"/>
+      <c r="F72" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G72" s="64"/>
+      <c r="G72" s="80"/>
       <c r="H72" s="47"/>
       <c r="I72" s="12"/>
       <c r="J72" s="12"/>
@@ -14641,22 +14662,22 @@
       <c r="GI72" s="32"/>
     </row>
     <row r="73" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A73" s="60" t="s">
+      <c r="A73" s="118" t="s">
         <v>47</v>
       </c>
-      <c r="B73" s="61"/>
+      <c r="B73" s="119"/>
       <c r="C73" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="D73" s="62">
+      <c r="D73" s="65">
         <v>4</v>
       </c>
-      <c r="E73" s="63"/>
-      <c r="F73" s="62">
+      <c r="E73" s="66"/>
+      <c r="F73" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G73" s="64"/>
+      <c r="G73" s="80"/>
       <c r="H73" s="47"/>
       <c r="I73" s="12"/>
       <c r="J73" s="12"/>
@@ -14843,22 +14864,22 @@
       <c r="GI73" s="32"/>
     </row>
     <row r="74" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A74" s="60" t="s">
+      <c r="A74" s="118" t="s">
         <v>140</v>
       </c>
-      <c r="B74" s="61"/>
+      <c r="B74" s="119"/>
       <c r="C74" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="D74" s="62">
+      <c r="D74" s="65">
         <v>12</v>
       </c>
-      <c r="E74" s="63"/>
-      <c r="F74" s="62">
+      <c r="E74" s="66"/>
+      <c r="F74" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G74" s="64"/>
+      <c r="G74" s="80"/>
       <c r="H74" s="47"/>
       <c r="I74" s="12"/>
       <c r="J74" s="12"/>
@@ -15045,22 +15066,22 @@
       <c r="GI74" s="32"/>
     </row>
     <row r="75" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A75" s="60" t="s">
+      <c r="A75" s="118" t="s">
         <v>142</v>
       </c>
-      <c r="B75" s="65"/>
+      <c r="B75" s="88"/>
       <c r="C75" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D75" s="62">
+      <c r="D75" s="65">
         <v>16</v>
       </c>
-      <c r="E75" s="63"/>
-      <c r="F75" s="62">
+      <c r="E75" s="66"/>
+      <c r="F75" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G75" s="64"/>
+      <c r="G75" s="80"/>
       <c r="H75" s="47"/>
       <c r="I75" s="12"/>
       <c r="J75" s="12"/>
@@ -15247,22 +15268,22 @@
       <c r="GI75" s="36"/>
     </row>
     <row r="76" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A76" s="60" t="s">
+      <c r="A76" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B76" s="61"/>
+      <c r="B76" s="119"/>
       <c r="C76" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="D76" s="62">
+      <c r="D76" s="65">
         <v>5</v>
       </c>
-      <c r="E76" s="63"/>
-      <c r="F76" s="62">
+      <c r="E76" s="66"/>
+      <c r="F76" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G76" s="64"/>
+      <c r="G76" s="80"/>
       <c r="H76" s="47"/>
       <c r="I76" s="12"/>
       <c r="J76" s="12"/>
@@ -15449,22 +15470,22 @@
       <c r="GI76" s="32"/>
     </row>
     <row r="77" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A77" s="60" t="s">
+      <c r="A77" s="118" t="s">
         <v>146</v>
       </c>
-      <c r="B77" s="61"/>
+      <c r="B77" s="119"/>
       <c r="C77" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="D77" s="62">
+      <c r="D77" s="65">
         <v>4</v>
       </c>
-      <c r="E77" s="63"/>
-      <c r="F77" s="62">
+      <c r="E77" s="66"/>
+      <c r="F77" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G77" s="64"/>
+      <c r="G77" s="80"/>
       <c r="H77" s="47"/>
       <c r="I77" s="12"/>
       <c r="J77" s="12"/>
@@ -15651,22 +15672,22 @@
       <c r="GI77" s="32"/>
     </row>
     <row r="78" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A78" s="60" t="s">
+      <c r="A78" s="118" t="s">
         <v>148</v>
       </c>
-      <c r="B78" s="61"/>
+      <c r="B78" s="119"/>
       <c r="C78" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="D78" s="62">
+      <c r="D78" s="65">
         <v>16</v>
       </c>
-      <c r="E78" s="63"/>
-      <c r="F78" s="62">
+      <c r="E78" s="66"/>
+      <c r="F78" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G78" s="64"/>
+      <c r="G78" s="80"/>
       <c r="H78" s="47"/>
       <c r="I78" s="12"/>
       <c r="J78" s="12"/>
@@ -15853,22 +15874,22 @@
       <c r="GI78" s="32"/>
     </row>
     <row r="79" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A79" s="82" t="s">
+      <c r="A79" s="73" t="s">
         <v>150</v>
       </c>
-      <c r="B79" s="83"/>
+      <c r="B79" s="74"/>
       <c r="C79" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="D79" s="62">
+      <c r="D79" s="65">
         <v>6</v>
       </c>
-      <c r="E79" s="63"/>
-      <c r="F79" s="62">
+      <c r="E79" s="66"/>
+      <c r="F79" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G79" s="64"/>
+      <c r="G79" s="80"/>
       <c r="H79" s="47"/>
       <c r="I79" s="12"/>
       <c r="J79" s="12"/>
@@ -16055,22 +16076,22 @@
       <c r="GI79" s="36"/>
     </row>
     <row r="80" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A80" s="82" t="s">
+      <c r="A80" s="73" t="s">
         <v>152</v>
       </c>
-      <c r="B80" s="83"/>
+      <c r="B80" s="74"/>
       <c r="C80" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D80" s="62">
+      <c r="D80" s="65">
         <v>6</v>
       </c>
-      <c r="E80" s="63"/>
-      <c r="F80" s="62">
+      <c r="E80" s="66"/>
+      <c r="F80" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G80" s="64"/>
+      <c r="G80" s="80"/>
       <c r="H80" s="47"/>
       <c r="I80" s="12"/>
       <c r="J80" s="12"/>
@@ -16257,21 +16278,21 @@
       <c r="GI80" s="36"/>
     </row>
     <row r="81" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A81" s="76" t="s">
+      <c r="A81" s="115" t="s">
         <v>153</v>
       </c>
-      <c r="B81" s="77"/>
+      <c r="B81" s="116"/>
       <c r="C81" s="39"/>
-      <c r="D81" s="78">
+      <c r="D81" s="71">
         <f>SUM(D82:E82)</f>
         <v>16</v>
       </c>
-      <c r="E81" s="88"/>
-      <c r="F81" s="78">
+      <c r="E81" s="72"/>
+      <c r="F81" s="71">
         <f>SUM(F82:G82)</f>
         <v>0</v>
       </c>
-      <c r="G81" s="80"/>
+      <c r="G81" s="75"/>
       <c r="H81" s="29"/>
       <c r="I81" s="8"/>
       <c r="J81" s="8"/>
@@ -16458,20 +16479,20 @@
       <c r="GI81" s="29"/>
     </row>
     <row r="82" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A82" s="86" t="s">
+      <c r="A82" s="93" t="s">
         <v>153</v>
       </c>
-      <c r="B82" s="87"/>
+      <c r="B82" s="94"/>
       <c r="C82" s="40"/>
-      <c r="D82" s="84">
+      <c r="D82" s="91">
         <v>16</v>
       </c>
-      <c r="E82" s="85"/>
-      <c r="F82" s="62">
+      <c r="E82" s="92"/>
+      <c r="F82" s="65">
         <f>SUM(H82:GI82)</f>
         <v>0</v>
       </c>
-      <c r="G82" s="64"/>
+      <c r="G82" s="80"/>
       <c r="H82" s="26"/>
       <c r="I82" s="12"/>
       <c r="J82" s="12"/>
@@ -16658,21 +16679,21 @@
       <c r="GI82" s="32"/>
     </row>
     <row r="83" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A83" s="104" t="s">
+      <c r="A83" s="110" t="s">
         <v>154</v>
       </c>
-      <c r="B83" s="105"/>
+      <c r="B83" s="111"/>
       <c r="C83" s="41"/>
-      <c r="D83" s="78">
+      <c r="D83" s="71">
         <f>SUM(D84:E84)</f>
         <v>32</v>
       </c>
-      <c r="E83" s="88"/>
-      <c r="F83" s="78">
+      <c r="E83" s="72"/>
+      <c r="F83" s="71">
         <f>SUM(F84:G84)</f>
         <v>0</v>
       </c>
-      <c r="G83" s="80"/>
+      <c r="G83" s="75"/>
       <c r="H83" s="29"/>
       <c r="I83" s="8"/>
       <c r="J83" s="8"/>
@@ -16859,20 +16880,20 @@
       <c r="GI83" s="29"/>
     </row>
     <row r="84" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A84" s="108" t="s">
+      <c r="A84" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="B84" s="109"/>
+      <c r="B84" s="86"/>
       <c r="C84" s="42"/>
-      <c r="D84" s="62">
+      <c r="D84" s="65">
         <v>32</v>
       </c>
-      <c r="E84" s="63"/>
-      <c r="F84" s="62">
+      <c r="E84" s="66"/>
+      <c r="F84" s="65">
         <f>SUM(H84:GI84)</f>
         <v>0</v>
       </c>
-      <c r="G84" s="64"/>
+      <c r="G84" s="80"/>
       <c r="H84" s="26"/>
       <c r="I84" s="12"/>
       <c r="J84" s="12"/>
@@ -17059,21 +17080,21 @@
       <c r="GI84" s="32"/>
     </row>
     <row r="85" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A85" s="111" t="s">
+      <c r="A85" s="89" t="s">
         <v>155</v>
       </c>
-      <c r="B85" s="112"/>
+      <c r="B85" s="90"/>
       <c r="C85" s="43"/>
-      <c r="D85" s="78">
+      <c r="D85" s="71">
         <f>SUM(D86:E86)</f>
         <v>8</v>
       </c>
-      <c r="E85" s="88"/>
-      <c r="F85" s="89">
+      <c r="E85" s="72"/>
+      <c r="F85" s="95">
         <f>SUM(F86:G86)</f>
         <v>0</v>
       </c>
-      <c r="G85" s="90"/>
+      <c r="G85" s="96"/>
       <c r="H85" s="29"/>
       <c r="I85" s="8"/>
       <c r="J85" s="8"/>
@@ -17260,20 +17281,20 @@
       <c r="GI85" s="29"/>
     </row>
     <row r="86" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A86" s="110" t="s">
+      <c r="A86" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="B86" s="65"/>
+      <c r="B86" s="88"/>
       <c r="C86" s="27"/>
-      <c r="D86" s="62">
+      <c r="D86" s="65">
         <v>8</v>
       </c>
-      <c r="E86" s="63"/>
-      <c r="F86" s="62">
+      <c r="E86" s="66"/>
+      <c r="F86" s="65">
         <f>SUM(H86:GI86)</f>
         <v>0</v>
       </c>
-      <c r="G86" s="64"/>
+      <c r="G86" s="80"/>
       <c r="H86" s="26"/>
       <c r="I86" s="12"/>
       <c r="J86" s="12"/>
@@ -17460,20 +17481,20 @@
       <c r="GI86" s="32"/>
     </row>
     <row r="87" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A87" s="106" t="s">
+      <c r="A87" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="107"/>
+      <c r="B87" s="84"/>
       <c r="C87" s="43"/>
-      <c r="D87" s="78">
+      <c r="D87" s="71">
         <f>232-D90</f>
         <v>36.349999999999994</v>
       </c>
-      <c r="E87" s="88"/>
-      <c r="F87" s="78">
+      <c r="E87" s="72"/>
+      <c r="F87" s="71">
         <v>0</v>
       </c>
-      <c r="G87" s="80"/>
+      <c r="G87" s="75"/>
       <c r="H87" s="29"/>
       <c r="I87" s="8"/>
       <c r="J87" s="8"/>
@@ -17660,15 +17681,15 @@
       <c r="GI87" s="29"/>
     </row>
     <row r="88" spans="1:191" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="101" t="s">
+      <c r="A88" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="B88" s="102"/>
+      <c r="B88" s="108"/>
       <c r="C88" s="44"/>
-      <c r="D88" s="98"/>
-      <c r="E88" s="99"/>
-      <c r="F88" s="98"/>
-      <c r="G88" s="100"/>
+      <c r="D88" s="104"/>
+      <c r="E88" s="105"/>
+      <c r="F88" s="104"/>
+      <c r="G88" s="106"/>
       <c r="H88" s="28"/>
       <c r="I88" s="17"/>
       <c r="J88" s="17"/>
@@ -17907,21 +17928,21 @@
       <c r="AX89" s="3"/>
     </row>
     <row r="90" spans="1:191" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="96" t="s">
+      <c r="A90" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="97"/>
+      <c r="B90" s="103"/>
       <c r="C90" s="45"/>
-      <c r="D90" s="94">
+      <c r="D90" s="100">
         <f>SUM(D85,D83,D81,D62,D14)</f>
         <v>195.65</v>
       </c>
-      <c r="E90" s="95"/>
-      <c r="F90" s="94">
+      <c r="E90" s="101"/>
+      <c r="F90" s="100">
         <f>SUM(F85,F83,F81,F62,F14)</f>
         <v>44.725999999999999</v>
       </c>
-      <c r="G90" s="103"/>
+      <c r="G90" s="109"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
@@ -17968,6 +17989,316 @@
     </row>
   </sheetData>
   <mergeCells count="334">
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="GD13:GE13"/>
+    <mergeCell ref="GF13:GG13"/>
+    <mergeCell ref="GH13:GI13"/>
+    <mergeCell ref="DZ12:GI12"/>
+    <mergeCell ref="FL13:FM13"/>
+    <mergeCell ref="FN13:FO13"/>
+    <mergeCell ref="FP13:FQ13"/>
+    <mergeCell ref="FR13:FS13"/>
+    <mergeCell ref="FT13:FU13"/>
+    <mergeCell ref="FV13:FW13"/>
+    <mergeCell ref="FX13:FY13"/>
+    <mergeCell ref="FZ13:GA13"/>
+    <mergeCell ref="GB13:GC13"/>
+    <mergeCell ref="ET13:EU13"/>
+    <mergeCell ref="EV13:EW13"/>
+    <mergeCell ref="EX13:EY13"/>
+    <mergeCell ref="EZ13:FA13"/>
+    <mergeCell ref="FB13:FC13"/>
+    <mergeCell ref="FD13:FE13"/>
+    <mergeCell ref="FF13:FG13"/>
+    <mergeCell ref="DX13:DY13"/>
+    <mergeCell ref="FH13:FI13"/>
+    <mergeCell ref="FJ13:FK13"/>
+    <mergeCell ref="EB13:EC13"/>
+    <mergeCell ref="ED13:EE13"/>
+    <mergeCell ref="EF13:EG13"/>
+    <mergeCell ref="EH13:EI13"/>
+    <mergeCell ref="EJ13:EK13"/>
+    <mergeCell ref="EL13:EM13"/>
+    <mergeCell ref="EN13:EO13"/>
+    <mergeCell ref="EP13:EQ13"/>
+    <mergeCell ref="ER13:ES13"/>
+    <mergeCell ref="DF13:DG13"/>
+    <mergeCell ref="DH13:DI13"/>
+    <mergeCell ref="DJ13:DK13"/>
+    <mergeCell ref="DL13:DM13"/>
+    <mergeCell ref="DN13:DO13"/>
+    <mergeCell ref="DP13:DQ13"/>
+    <mergeCell ref="DR13:DS13"/>
+    <mergeCell ref="DT13:DU13"/>
+    <mergeCell ref="DV13:DW13"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="BH13:BI13"/>
+    <mergeCell ref="BJ13:BK13"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="P9:X9"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F11:G13"/>
+    <mergeCell ref="D11:E13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="AL13:AM13"/>
+    <mergeCell ref="AN13:AO13"/>
+    <mergeCell ref="AP13:AQ13"/>
+    <mergeCell ref="AR13:AS13"/>
+    <mergeCell ref="AT13:AU13"/>
+    <mergeCell ref="AV13:AW13"/>
+    <mergeCell ref="AX13:AY13"/>
+    <mergeCell ref="AZ13:BA13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="P6:X6"/>
+    <mergeCell ref="P5:X5"/>
+    <mergeCell ref="P4:X4"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="H12:BQ12"/>
+    <mergeCell ref="BB13:BC13"/>
+    <mergeCell ref="BD13:BE13"/>
+    <mergeCell ref="BF13:BG13"/>
+    <mergeCell ref="BP13:BQ13"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="AF13:AG13"/>
+    <mergeCell ref="AH13:AI13"/>
+    <mergeCell ref="AJ13:AK13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
     <mergeCell ref="BR13:BS13"/>
     <mergeCell ref="BL13:BM13"/>
     <mergeCell ref="BN13:BO13"/>
@@ -17992,316 +18323,6 @@
     <mergeCell ref="CZ13:DA13"/>
     <mergeCell ref="DB13:DC13"/>
     <mergeCell ref="DD13:DE13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="P6:X6"/>
-    <mergeCell ref="P5:X5"/>
-    <mergeCell ref="P4:X4"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="H12:BQ12"/>
-    <mergeCell ref="BB13:BC13"/>
-    <mergeCell ref="BD13:BE13"/>
-    <mergeCell ref="BF13:BG13"/>
-    <mergeCell ref="BP13:BQ13"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="AF13:AG13"/>
-    <mergeCell ref="AH13:AI13"/>
-    <mergeCell ref="AJ13:AK13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="AL13:AM13"/>
-    <mergeCell ref="AN13:AO13"/>
-    <mergeCell ref="AP13:AQ13"/>
-    <mergeCell ref="AR13:AS13"/>
-    <mergeCell ref="AT13:AU13"/>
-    <mergeCell ref="AV13:AW13"/>
-    <mergeCell ref="AX13:AY13"/>
-    <mergeCell ref="AZ13:BA13"/>
-    <mergeCell ref="BH13:BI13"/>
-    <mergeCell ref="BJ13:BK13"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="P9:X9"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F11:G13"/>
-    <mergeCell ref="D11:E13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="F90:G90"/>
-    <mergeCell ref="F87:G87"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="DF13:DG13"/>
-    <mergeCell ref="DH13:DI13"/>
-    <mergeCell ref="DJ13:DK13"/>
-    <mergeCell ref="DL13:DM13"/>
-    <mergeCell ref="DN13:DO13"/>
-    <mergeCell ref="DP13:DQ13"/>
-    <mergeCell ref="DR13:DS13"/>
-    <mergeCell ref="DT13:DU13"/>
-    <mergeCell ref="DV13:DW13"/>
-    <mergeCell ref="FF13:FG13"/>
-    <mergeCell ref="DX13:DY13"/>
-    <mergeCell ref="FH13:FI13"/>
-    <mergeCell ref="FJ13:FK13"/>
-    <mergeCell ref="EB13:EC13"/>
-    <mergeCell ref="ED13:EE13"/>
-    <mergeCell ref="EF13:EG13"/>
-    <mergeCell ref="EH13:EI13"/>
-    <mergeCell ref="EJ13:EK13"/>
-    <mergeCell ref="EL13:EM13"/>
-    <mergeCell ref="EN13:EO13"/>
-    <mergeCell ref="EP13:EQ13"/>
-    <mergeCell ref="ER13:ES13"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="GD13:GE13"/>
-    <mergeCell ref="GF13:GG13"/>
-    <mergeCell ref="GH13:GI13"/>
-    <mergeCell ref="DZ12:GI12"/>
-    <mergeCell ref="FL13:FM13"/>
-    <mergeCell ref="FN13:FO13"/>
-    <mergeCell ref="FP13:FQ13"/>
-    <mergeCell ref="FR13:FS13"/>
-    <mergeCell ref="FT13:FU13"/>
-    <mergeCell ref="FV13:FW13"/>
-    <mergeCell ref="FX13:FY13"/>
-    <mergeCell ref="FZ13:GA13"/>
-    <mergeCell ref="GB13:GC13"/>
-    <mergeCell ref="ET13:EU13"/>
-    <mergeCell ref="EV13:EW13"/>
-    <mergeCell ref="EX13:EY13"/>
-    <mergeCell ref="EZ13:FA13"/>
-    <mergeCell ref="FB13:FC13"/>
-    <mergeCell ref="FD13:FE13"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Created Model for Issiue #33
</commit_message>
<xml_diff>
--- a/Documents/Zeitplan.xlsx
+++ b/Documents/Zeitplan.xlsx
@@ -1170,6 +1170,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1182,32 +1206,31 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1215,42 +1238,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1259,6 +1246,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1306,30 +1296,40 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1799,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GI90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AX31" sqref="AX31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1820,28 +1820,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:191" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="112"/>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="112"/>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="75"/>
     </row>
     <row r="2" spans="1:191" x14ac:dyDescent="0.25">
       <c r="T2" s="9"/>
@@ -1874,17 +1874,17 @@
         <v>160</v>
       </c>
       <c r="N4" s="57"/>
-      <c r="P4" s="67" t="s">
+      <c r="P4" s="83" t="s">
         <v>157</v>
       </c>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="67"/>
-      <c r="W4" s="67"/>
-      <c r="X4" s="67"/>
+      <c r="Q4" s="83"/>
+      <c r="R4" s="83"/>
+      <c r="S4" s="83"/>
+      <c r="T4" s="83"/>
+      <c r="U4" s="83"/>
+      <c r="V4" s="83"/>
+      <c r="W4" s="83"/>
+      <c r="X4" s="83"/>
     </row>
     <row r="5" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -1901,17 +1901,17 @@
       <c r="F5" s="5"/>
       <c r="G5" s="7"/>
       <c r="N5" s="24"/>
-      <c r="P5" s="67" t="s">
+      <c r="P5" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="67"/>
-      <c r="S5" s="67"/>
-      <c r="T5" s="67"/>
-      <c r="U5" s="67"/>
-      <c r="V5" s="67"/>
-      <c r="W5" s="67"/>
-      <c r="X5" s="67"/>
+      <c r="Q5" s="83"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="83"/>
+      <c r="T5" s="83"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
+      <c r="W5" s="83"/>
+      <c r="X5" s="83"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
@@ -1935,17 +1935,17 @@
         <v>15</v>
       </c>
       <c r="N6" s="16"/>
-      <c r="P6" s="67" t="s">
+      <c r="P6" s="83" t="s">
         <v>159</v>
       </c>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="67"/>
-      <c r="V6" s="67"/>
-      <c r="W6" s="67"/>
-      <c r="X6" s="67"/>
+      <c r="Q6" s="83"/>
+      <c r="R6" s="83"/>
+      <c r="S6" s="83"/>
+      <c r="T6" s="83"/>
+      <c r="U6" s="83"/>
+      <c r="V6" s="83"/>
+      <c r="W6" s="83"/>
+      <c r="X6" s="83"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
@@ -1963,17 +1963,17 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="N7" s="21"/>
-      <c r="P7" s="67" t="s">
+      <c r="P7" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="67"/>
-      <c r="R7" s="67"/>
-      <c r="S7" s="67"/>
-      <c r="T7" s="67"/>
-      <c r="U7" s="67"/>
-      <c r="V7" s="67"/>
-      <c r="W7" s="67"/>
-      <c r="X7" s="67"/>
+      <c r="Q7" s="83"/>
+      <c r="R7" s="83"/>
+      <c r="S7" s="83"/>
+      <c r="T7" s="83"/>
+      <c r="U7" s="83"/>
+      <c r="V7" s="83"/>
+      <c r="W7" s="83"/>
+      <c r="X7" s="83"/>
     </row>
     <row r="8" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1988,17 +1988,17 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="N8" s="20"/>
-      <c r="P8" s="70" t="s">
+      <c r="P8" s="115" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="70"/>
-      <c r="R8" s="70"/>
-      <c r="S8" s="70"/>
-      <c r="T8" s="70"/>
-      <c r="U8" s="70"/>
-      <c r="V8" s="70"/>
-      <c r="W8" s="70"/>
-      <c r="X8" s="70"/>
+      <c r="Q8" s="115"/>
+      <c r="R8" s="115"/>
+      <c r="S8" s="115"/>
+      <c r="T8" s="115"/>
+      <c r="U8" s="115"/>
+      <c r="V8" s="115"/>
+      <c r="W8" s="115"/>
+      <c r="X8" s="115"/>
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
@@ -2006,23 +2006,23 @@
       <c r="AC8" s="5"/>
     </row>
     <row r="9" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="68"/>
+      <c r="A9" s="120"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="12"/>
       <c r="N9" s="49"/>
-      <c r="P9" s="70" t="s">
+      <c r="P9" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="Q9" s="70"/>
-      <c r="R9" s="70"/>
-      <c r="S9" s="70"/>
-      <c r="T9" s="70"/>
-      <c r="U9" s="70"/>
-      <c r="V9" s="70"/>
-      <c r="W9" s="70"/>
-      <c r="X9" s="70"/>
+      <c r="Q9" s="115"/>
+      <c r="R9" s="115"/>
+      <c r="S9" s="115"/>
+      <c r="T9" s="115"/>
+      <c r="U9" s="115"/>
+      <c r="V9" s="115"/>
+      <c r="W9" s="115"/>
+      <c r="X9" s="115"/>
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
@@ -2032,7 +2032,7 @@
       <c r="AJ9" s="13"/>
     </row>
     <row r="10" spans="1:191" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="68"/>
+      <c r="A10" s="120"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -2049,18 +2049,18 @@
       <c r="AC10" s="5"/>
     </row>
     <row r="11" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="68"/>
-      <c r="C11" s="78" t="s">
+      <c r="A11" s="120"/>
+      <c r="C11" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="76" t="s">
+      <c r="D11" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76" t="s">
+      <c r="E11" s="116"/>
+      <c r="F11" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="76"/>
+      <c r="G11" s="116"/>
       <c r="T11" s="9"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
@@ -2073,596 +2073,596 @@
       <c r="AC11" s="5"/>
     </row>
     <row r="12" spans="1:191" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="68"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="62" t="s">
+      <c r="A12" s="120"/>
+      <c r="C12" s="118"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="63"/>
-      <c r="J12" s="63"/>
-      <c r="K12" s="63"/>
-      <c r="L12" s="63"/>
-      <c r="M12" s="63"/>
-      <c r="N12" s="63"/>
-      <c r="O12" s="63"/>
-      <c r="P12" s="63"/>
-      <c r="Q12" s="63"/>
-      <c r="R12" s="63"/>
-      <c r="S12" s="63"/>
-      <c r="T12" s="63"/>
-      <c r="U12" s="63"/>
-      <c r="V12" s="63"/>
-      <c r="W12" s="63"/>
-      <c r="X12" s="63"/>
-      <c r="Y12" s="63"/>
-      <c r="Z12" s="63"/>
-      <c r="AA12" s="63"/>
-      <c r="AB12" s="63"/>
-      <c r="AC12" s="63"/>
-      <c r="AD12" s="63"/>
-      <c r="AE12" s="63"/>
-      <c r="AF12" s="63"/>
-      <c r="AG12" s="63"/>
-      <c r="AH12" s="63"/>
-      <c r="AI12" s="63"/>
-      <c r="AJ12" s="63"/>
-      <c r="AK12" s="63"/>
-      <c r="AL12" s="63"/>
-      <c r="AM12" s="63"/>
-      <c r="AN12" s="63"/>
-      <c r="AO12" s="63"/>
-      <c r="AP12" s="63"/>
-      <c r="AQ12" s="63"/>
-      <c r="AR12" s="63"/>
-      <c r="AS12" s="63"/>
-      <c r="AT12" s="63"/>
-      <c r="AU12" s="63"/>
-      <c r="AV12" s="63"/>
-      <c r="AW12" s="63"/>
-      <c r="AX12" s="63"/>
-      <c r="AY12" s="63"/>
-      <c r="AZ12" s="63"/>
-      <c r="BA12" s="63"/>
-      <c r="BB12" s="63"/>
-      <c r="BC12" s="63"/>
-      <c r="BD12" s="63"/>
-      <c r="BE12" s="63"/>
-      <c r="BF12" s="63"/>
-      <c r="BG12" s="63"/>
-      <c r="BH12" s="63"/>
-      <c r="BI12" s="63"/>
-      <c r="BJ12" s="63"/>
-      <c r="BK12" s="63"/>
-      <c r="BL12" s="63"/>
-      <c r="BM12" s="63"/>
-      <c r="BN12" s="63"/>
-      <c r="BO12" s="63"/>
-      <c r="BP12" s="63"/>
-      <c r="BQ12" s="64"/>
-      <c r="BR12" s="62" t="s">
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="73"/>
+      <c r="M12" s="73"/>
+      <c r="N12" s="73"/>
+      <c r="O12" s="73"/>
+      <c r="P12" s="73"/>
+      <c r="Q12" s="73"/>
+      <c r="R12" s="73"/>
+      <c r="S12" s="73"/>
+      <c r="T12" s="73"/>
+      <c r="U12" s="73"/>
+      <c r="V12" s="73"/>
+      <c r="W12" s="73"/>
+      <c r="X12" s="73"/>
+      <c r="Y12" s="73"/>
+      <c r="Z12" s="73"/>
+      <c r="AA12" s="73"/>
+      <c r="AB12" s="73"/>
+      <c r="AC12" s="73"/>
+      <c r="AD12" s="73"/>
+      <c r="AE12" s="73"/>
+      <c r="AF12" s="73"/>
+      <c r="AG12" s="73"/>
+      <c r="AH12" s="73"/>
+      <c r="AI12" s="73"/>
+      <c r="AJ12" s="73"/>
+      <c r="AK12" s="73"/>
+      <c r="AL12" s="73"/>
+      <c r="AM12" s="73"/>
+      <c r="AN12" s="73"/>
+      <c r="AO12" s="73"/>
+      <c r="AP12" s="73"/>
+      <c r="AQ12" s="73"/>
+      <c r="AR12" s="73"/>
+      <c r="AS12" s="73"/>
+      <c r="AT12" s="73"/>
+      <c r="AU12" s="73"/>
+      <c r="AV12" s="73"/>
+      <c r="AW12" s="73"/>
+      <c r="AX12" s="73"/>
+      <c r="AY12" s="73"/>
+      <c r="AZ12" s="73"/>
+      <c r="BA12" s="73"/>
+      <c r="BB12" s="73"/>
+      <c r="BC12" s="73"/>
+      <c r="BD12" s="73"/>
+      <c r="BE12" s="73"/>
+      <c r="BF12" s="73"/>
+      <c r="BG12" s="73"/>
+      <c r="BH12" s="73"/>
+      <c r="BI12" s="73"/>
+      <c r="BJ12" s="73"/>
+      <c r="BK12" s="73"/>
+      <c r="BL12" s="73"/>
+      <c r="BM12" s="73"/>
+      <c r="BN12" s="73"/>
+      <c r="BO12" s="73"/>
+      <c r="BP12" s="73"/>
+      <c r="BQ12" s="121"/>
+      <c r="BR12" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="BS12" s="63"/>
-      <c r="BT12" s="63"/>
-      <c r="BU12" s="63"/>
-      <c r="BV12" s="63"/>
-      <c r="BW12" s="63"/>
-      <c r="BX12" s="63"/>
-      <c r="BY12" s="63"/>
-      <c r="BZ12" s="63"/>
-      <c r="CA12" s="63"/>
-      <c r="CB12" s="63"/>
-      <c r="CC12" s="63"/>
-      <c r="CD12" s="63"/>
-      <c r="CE12" s="63"/>
-      <c r="CF12" s="63"/>
-      <c r="CG12" s="63"/>
-      <c r="CH12" s="63"/>
-      <c r="CI12" s="63"/>
-      <c r="CJ12" s="63"/>
-      <c r="CK12" s="63"/>
-      <c r="CL12" s="63"/>
-      <c r="CM12" s="63"/>
-      <c r="CN12" s="63"/>
-      <c r="CO12" s="63"/>
-      <c r="CP12" s="63"/>
-      <c r="CQ12" s="63"/>
-      <c r="CR12" s="63"/>
-      <c r="CS12" s="63"/>
-      <c r="CT12" s="63"/>
-      <c r="CU12" s="63"/>
-      <c r="CV12" s="63"/>
-      <c r="CW12" s="63"/>
-      <c r="CX12" s="63"/>
-      <c r="CY12" s="63"/>
-      <c r="CZ12" s="63"/>
-      <c r="DA12" s="63"/>
-      <c r="DB12" s="63"/>
-      <c r="DC12" s="63"/>
-      <c r="DD12" s="63"/>
-      <c r="DE12" s="63"/>
-      <c r="DF12" s="63"/>
-      <c r="DG12" s="63"/>
-      <c r="DH12" s="63"/>
-      <c r="DI12" s="63"/>
-      <c r="DJ12" s="63"/>
-      <c r="DK12" s="63"/>
-      <c r="DL12" s="63"/>
-      <c r="DM12" s="63"/>
-      <c r="DN12" s="63"/>
-      <c r="DO12" s="63"/>
-      <c r="DP12" s="63"/>
-      <c r="DQ12" s="63"/>
-      <c r="DR12" s="63"/>
-      <c r="DS12" s="63"/>
-      <c r="DT12" s="63"/>
-      <c r="DU12" s="63"/>
-      <c r="DV12" s="63"/>
-      <c r="DW12" s="63"/>
-      <c r="DX12" s="63"/>
-      <c r="DY12" s="64"/>
-      <c r="DZ12" s="62" t="s">
+      <c r="BS12" s="73"/>
+      <c r="BT12" s="73"/>
+      <c r="BU12" s="73"/>
+      <c r="BV12" s="73"/>
+      <c r="BW12" s="73"/>
+      <c r="BX12" s="73"/>
+      <c r="BY12" s="73"/>
+      <c r="BZ12" s="73"/>
+      <c r="CA12" s="73"/>
+      <c r="CB12" s="73"/>
+      <c r="CC12" s="73"/>
+      <c r="CD12" s="73"/>
+      <c r="CE12" s="73"/>
+      <c r="CF12" s="73"/>
+      <c r="CG12" s="73"/>
+      <c r="CH12" s="73"/>
+      <c r="CI12" s="73"/>
+      <c r="CJ12" s="73"/>
+      <c r="CK12" s="73"/>
+      <c r="CL12" s="73"/>
+      <c r="CM12" s="73"/>
+      <c r="CN12" s="73"/>
+      <c r="CO12" s="73"/>
+      <c r="CP12" s="73"/>
+      <c r="CQ12" s="73"/>
+      <c r="CR12" s="73"/>
+      <c r="CS12" s="73"/>
+      <c r="CT12" s="73"/>
+      <c r="CU12" s="73"/>
+      <c r="CV12" s="73"/>
+      <c r="CW12" s="73"/>
+      <c r="CX12" s="73"/>
+      <c r="CY12" s="73"/>
+      <c r="CZ12" s="73"/>
+      <c r="DA12" s="73"/>
+      <c r="DB12" s="73"/>
+      <c r="DC12" s="73"/>
+      <c r="DD12" s="73"/>
+      <c r="DE12" s="73"/>
+      <c r="DF12" s="73"/>
+      <c r="DG12" s="73"/>
+      <c r="DH12" s="73"/>
+      <c r="DI12" s="73"/>
+      <c r="DJ12" s="73"/>
+      <c r="DK12" s="73"/>
+      <c r="DL12" s="73"/>
+      <c r="DM12" s="73"/>
+      <c r="DN12" s="73"/>
+      <c r="DO12" s="73"/>
+      <c r="DP12" s="73"/>
+      <c r="DQ12" s="73"/>
+      <c r="DR12" s="73"/>
+      <c r="DS12" s="73"/>
+      <c r="DT12" s="73"/>
+      <c r="DU12" s="73"/>
+      <c r="DV12" s="73"/>
+      <c r="DW12" s="73"/>
+      <c r="DX12" s="73"/>
+      <c r="DY12" s="121"/>
+      <c r="DZ12" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="EA12" s="63"/>
-      <c r="EB12" s="63"/>
-      <c r="EC12" s="63"/>
-      <c r="ED12" s="63"/>
-      <c r="EE12" s="63"/>
-      <c r="EF12" s="63"/>
-      <c r="EG12" s="63"/>
-      <c r="EH12" s="63"/>
-      <c r="EI12" s="63"/>
-      <c r="EJ12" s="63"/>
-      <c r="EK12" s="63"/>
-      <c r="EL12" s="63"/>
-      <c r="EM12" s="63"/>
-      <c r="EN12" s="63"/>
-      <c r="EO12" s="63"/>
-      <c r="EP12" s="63"/>
-      <c r="EQ12" s="63"/>
-      <c r="ER12" s="63"/>
-      <c r="ES12" s="63"/>
-      <c r="ET12" s="63"/>
-      <c r="EU12" s="63"/>
-      <c r="EV12" s="63"/>
-      <c r="EW12" s="63"/>
-      <c r="EX12" s="63"/>
-      <c r="EY12" s="63"/>
-      <c r="EZ12" s="63"/>
-      <c r="FA12" s="63"/>
-      <c r="FB12" s="63"/>
-      <c r="FC12" s="63"/>
-      <c r="FD12" s="63"/>
-      <c r="FE12" s="63"/>
-      <c r="FF12" s="63"/>
-      <c r="FG12" s="63"/>
-      <c r="FH12" s="63"/>
-      <c r="FI12" s="63"/>
-      <c r="FJ12" s="63"/>
-      <c r="FK12" s="63"/>
-      <c r="FL12" s="63"/>
-      <c r="FM12" s="63"/>
-      <c r="FN12" s="63"/>
-      <c r="FO12" s="63"/>
-      <c r="FP12" s="63"/>
-      <c r="FQ12" s="63"/>
-      <c r="FR12" s="63"/>
-      <c r="FS12" s="63"/>
-      <c r="FT12" s="63"/>
-      <c r="FU12" s="63"/>
-      <c r="FV12" s="63"/>
-      <c r="FW12" s="63"/>
-      <c r="FX12" s="63"/>
-      <c r="FY12" s="63"/>
-      <c r="FZ12" s="63"/>
-      <c r="GA12" s="63"/>
-      <c r="GB12" s="63"/>
-      <c r="GC12" s="63"/>
-      <c r="GD12" s="63"/>
-      <c r="GE12" s="63"/>
-      <c r="GF12" s="63"/>
-      <c r="GG12" s="63"/>
-      <c r="GH12" s="63"/>
-      <c r="GI12" s="120"/>
+      <c r="EA12" s="73"/>
+      <c r="EB12" s="73"/>
+      <c r="EC12" s="73"/>
+      <c r="ED12" s="73"/>
+      <c r="EE12" s="73"/>
+      <c r="EF12" s="73"/>
+      <c r="EG12" s="73"/>
+      <c r="EH12" s="73"/>
+      <c r="EI12" s="73"/>
+      <c r="EJ12" s="73"/>
+      <c r="EK12" s="73"/>
+      <c r="EL12" s="73"/>
+      <c r="EM12" s="73"/>
+      <c r="EN12" s="73"/>
+      <c r="EO12" s="73"/>
+      <c r="EP12" s="73"/>
+      <c r="EQ12" s="73"/>
+      <c r="ER12" s="73"/>
+      <c r="ES12" s="73"/>
+      <c r="ET12" s="73"/>
+      <c r="EU12" s="73"/>
+      <c r="EV12" s="73"/>
+      <c r="EW12" s="73"/>
+      <c r="EX12" s="73"/>
+      <c r="EY12" s="73"/>
+      <c r="EZ12" s="73"/>
+      <c r="FA12" s="73"/>
+      <c r="FB12" s="73"/>
+      <c r="FC12" s="73"/>
+      <c r="FD12" s="73"/>
+      <c r="FE12" s="73"/>
+      <c r="FF12" s="73"/>
+      <c r="FG12" s="73"/>
+      <c r="FH12" s="73"/>
+      <c r="FI12" s="73"/>
+      <c r="FJ12" s="73"/>
+      <c r="FK12" s="73"/>
+      <c r="FL12" s="73"/>
+      <c r="FM12" s="73"/>
+      <c r="FN12" s="73"/>
+      <c r="FO12" s="73"/>
+      <c r="FP12" s="73"/>
+      <c r="FQ12" s="73"/>
+      <c r="FR12" s="73"/>
+      <c r="FS12" s="73"/>
+      <c r="FT12" s="73"/>
+      <c r="FU12" s="73"/>
+      <c r="FV12" s="73"/>
+      <c r="FW12" s="73"/>
+      <c r="FX12" s="73"/>
+      <c r="FY12" s="73"/>
+      <c r="FZ12" s="73"/>
+      <c r="GA12" s="73"/>
+      <c r="GB12" s="73"/>
+      <c r="GC12" s="73"/>
+      <c r="GD12" s="73"/>
+      <c r="GE12" s="73"/>
+      <c r="GF12" s="73"/>
+      <c r="GG12" s="73"/>
+      <c r="GH12" s="73"/>
+      <c r="GI12" s="74"/>
     </row>
     <row r="13" spans="1:191" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="60">
+      <c r="C13" s="119"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="70">
         <v>1</v>
       </c>
-      <c r="I13" s="61"/>
-      <c r="J13" s="60">
+      <c r="I13" s="71"/>
+      <c r="J13" s="70">
         <v>2</v>
       </c>
-      <c r="K13" s="61"/>
-      <c r="L13" s="60">
+      <c r="K13" s="71"/>
+      <c r="L13" s="70">
         <v>3</v>
       </c>
-      <c r="M13" s="61"/>
-      <c r="N13" s="60">
+      <c r="M13" s="71"/>
+      <c r="N13" s="70">
         <v>4</v>
       </c>
-      <c r="O13" s="61"/>
-      <c r="P13" s="60">
+      <c r="O13" s="71"/>
+      <c r="P13" s="70">
         <v>5</v>
       </c>
-      <c r="Q13" s="61"/>
-      <c r="R13" s="60">
+      <c r="Q13" s="71"/>
+      <c r="R13" s="70">
         <v>6</v>
       </c>
-      <c r="S13" s="61"/>
-      <c r="T13" s="60">
+      <c r="S13" s="71"/>
+      <c r="T13" s="70">
         <v>7</v>
       </c>
-      <c r="U13" s="61"/>
-      <c r="V13" s="60">
+      <c r="U13" s="71"/>
+      <c r="V13" s="70">
         <v>8</v>
       </c>
-      <c r="W13" s="61"/>
-      <c r="X13" s="60">
+      <c r="W13" s="71"/>
+      <c r="X13" s="70">
         <v>9</v>
       </c>
-      <c r="Y13" s="61"/>
-      <c r="Z13" s="60">
+      <c r="Y13" s="71"/>
+      <c r="Z13" s="70">
         <v>10</v>
       </c>
-      <c r="AA13" s="61"/>
-      <c r="AB13" s="60">
+      <c r="AA13" s="71"/>
+      <c r="AB13" s="70">
         <v>11</v>
       </c>
-      <c r="AC13" s="61"/>
-      <c r="AD13" s="60">
+      <c r="AC13" s="71"/>
+      <c r="AD13" s="70">
         <v>12</v>
       </c>
-      <c r="AE13" s="61"/>
-      <c r="AF13" s="60">
+      <c r="AE13" s="71"/>
+      <c r="AF13" s="70">
         <v>13</v>
       </c>
-      <c r="AG13" s="61"/>
-      <c r="AH13" s="60">
+      <c r="AG13" s="71"/>
+      <c r="AH13" s="70">
         <v>14</v>
       </c>
-      <c r="AI13" s="61"/>
-      <c r="AJ13" s="60">
+      <c r="AI13" s="71"/>
+      <c r="AJ13" s="70">
         <v>15</v>
       </c>
-      <c r="AK13" s="61"/>
-      <c r="AL13" s="60">
+      <c r="AK13" s="71"/>
+      <c r="AL13" s="70">
         <v>16</v>
       </c>
-      <c r="AM13" s="61"/>
-      <c r="AN13" s="60">
+      <c r="AM13" s="71"/>
+      <c r="AN13" s="70">
         <v>17</v>
       </c>
-      <c r="AO13" s="61"/>
-      <c r="AP13" s="60">
+      <c r="AO13" s="71"/>
+      <c r="AP13" s="70">
         <v>18</v>
       </c>
-      <c r="AQ13" s="61"/>
-      <c r="AR13" s="60">
+      <c r="AQ13" s="71"/>
+      <c r="AR13" s="70">
         <v>19</v>
       </c>
-      <c r="AS13" s="61"/>
-      <c r="AT13" s="60">
+      <c r="AS13" s="71"/>
+      <c r="AT13" s="70">
         <v>20</v>
       </c>
-      <c r="AU13" s="61"/>
-      <c r="AV13" s="60">
+      <c r="AU13" s="71"/>
+      <c r="AV13" s="70">
         <v>21</v>
       </c>
-      <c r="AW13" s="61"/>
-      <c r="AX13" s="60">
+      <c r="AW13" s="71"/>
+      <c r="AX13" s="70">
         <v>22</v>
       </c>
-      <c r="AY13" s="61"/>
-      <c r="AZ13" s="60">
+      <c r="AY13" s="71"/>
+      <c r="AZ13" s="70">
         <v>23</v>
       </c>
-      <c r="BA13" s="61"/>
-      <c r="BB13" s="60">
+      <c r="BA13" s="71"/>
+      <c r="BB13" s="70">
         <v>24</v>
       </c>
-      <c r="BC13" s="61"/>
-      <c r="BD13" s="60">
+      <c r="BC13" s="71"/>
+      <c r="BD13" s="70">
         <v>25</v>
       </c>
-      <c r="BE13" s="61"/>
-      <c r="BF13" s="60">
+      <c r="BE13" s="71"/>
+      <c r="BF13" s="70">
         <v>26</v>
       </c>
-      <c r="BG13" s="61"/>
-      <c r="BH13" s="60">
+      <c r="BG13" s="71"/>
+      <c r="BH13" s="70">
         <v>27</v>
       </c>
-      <c r="BI13" s="61"/>
-      <c r="BJ13" s="60">
+      <c r="BI13" s="71"/>
+      <c r="BJ13" s="70">
         <v>28</v>
       </c>
-      <c r="BK13" s="61"/>
-      <c r="BL13" s="60">
+      <c r="BK13" s="71"/>
+      <c r="BL13" s="70">
         <v>29</v>
       </c>
-      <c r="BM13" s="61"/>
-      <c r="BN13" s="60">
+      <c r="BM13" s="71"/>
+      <c r="BN13" s="70">
         <v>30</v>
       </c>
-      <c r="BO13" s="61"/>
-      <c r="BP13" s="60">
+      <c r="BO13" s="71"/>
+      <c r="BP13" s="70">
         <v>31</v>
       </c>
-      <c r="BQ13" s="69"/>
-      <c r="BR13" s="60">
+      <c r="BQ13" s="122"/>
+      <c r="BR13" s="70">
         <v>1</v>
       </c>
-      <c r="BS13" s="61"/>
-      <c r="BT13" s="60">
+      <c r="BS13" s="71"/>
+      <c r="BT13" s="70">
         <v>2</v>
       </c>
-      <c r="BU13" s="61"/>
-      <c r="BV13" s="60">
+      <c r="BU13" s="71"/>
+      <c r="BV13" s="70">
         <v>3</v>
       </c>
-      <c r="BW13" s="61"/>
-      <c r="BX13" s="60">
+      <c r="BW13" s="71"/>
+      <c r="BX13" s="70">
         <v>4</v>
       </c>
-      <c r="BY13" s="61"/>
-      <c r="BZ13" s="60">
+      <c r="BY13" s="71"/>
+      <c r="BZ13" s="70">
         <v>5</v>
       </c>
-      <c r="CA13" s="61"/>
-      <c r="CB13" s="60">
+      <c r="CA13" s="71"/>
+      <c r="CB13" s="70">
         <v>6</v>
       </c>
-      <c r="CC13" s="61"/>
-      <c r="CD13" s="60">
+      <c r="CC13" s="71"/>
+      <c r="CD13" s="70">
         <v>7</v>
       </c>
-      <c r="CE13" s="61"/>
-      <c r="CF13" s="60">
+      <c r="CE13" s="71"/>
+      <c r="CF13" s="70">
         <v>8</v>
       </c>
-      <c r="CG13" s="61"/>
-      <c r="CH13" s="60">
+      <c r="CG13" s="71"/>
+      <c r="CH13" s="70">
         <v>9</v>
       </c>
-      <c r="CI13" s="61"/>
-      <c r="CJ13" s="60">
+      <c r="CI13" s="71"/>
+      <c r="CJ13" s="70">
         <v>10</v>
       </c>
-      <c r="CK13" s="61"/>
-      <c r="CL13" s="60">
+      <c r="CK13" s="71"/>
+      <c r="CL13" s="70">
         <v>11</v>
       </c>
-      <c r="CM13" s="61"/>
-      <c r="CN13" s="60">
+      <c r="CM13" s="71"/>
+      <c r="CN13" s="70">
         <v>12</v>
       </c>
-      <c r="CO13" s="61"/>
-      <c r="CP13" s="60">
+      <c r="CO13" s="71"/>
+      <c r="CP13" s="70">
         <v>13</v>
       </c>
-      <c r="CQ13" s="61"/>
-      <c r="CR13" s="60">
+      <c r="CQ13" s="71"/>
+      <c r="CR13" s="70">
         <v>14</v>
       </c>
-      <c r="CS13" s="61"/>
-      <c r="CT13" s="60">
+      <c r="CS13" s="71"/>
+      <c r="CT13" s="70">
         <v>15</v>
       </c>
-      <c r="CU13" s="61"/>
-      <c r="CV13" s="60">
+      <c r="CU13" s="71"/>
+      <c r="CV13" s="70">
         <v>16</v>
       </c>
-      <c r="CW13" s="61"/>
-      <c r="CX13" s="60">
+      <c r="CW13" s="71"/>
+      <c r="CX13" s="70">
         <v>17</v>
       </c>
-      <c r="CY13" s="61"/>
-      <c r="CZ13" s="60">
+      <c r="CY13" s="71"/>
+      <c r="CZ13" s="70">
         <v>18</v>
       </c>
-      <c r="DA13" s="61"/>
-      <c r="DB13" s="60">
+      <c r="DA13" s="71"/>
+      <c r="DB13" s="70">
         <v>19</v>
       </c>
-      <c r="DC13" s="61"/>
-      <c r="DD13" s="60">
+      <c r="DC13" s="71"/>
+      <c r="DD13" s="70">
         <v>20</v>
       </c>
-      <c r="DE13" s="61"/>
-      <c r="DF13" s="60">
+      <c r="DE13" s="71"/>
+      <c r="DF13" s="70">
         <v>21</v>
       </c>
-      <c r="DG13" s="61"/>
-      <c r="DH13" s="60">
+      <c r="DG13" s="71"/>
+      <c r="DH13" s="70">
         <v>22</v>
       </c>
-      <c r="DI13" s="61"/>
-      <c r="DJ13" s="60">
+      <c r="DI13" s="71"/>
+      <c r="DJ13" s="70">
         <v>23</v>
       </c>
-      <c r="DK13" s="61"/>
-      <c r="DL13" s="60">
+      <c r="DK13" s="71"/>
+      <c r="DL13" s="70">
         <v>24</v>
       </c>
-      <c r="DM13" s="61"/>
-      <c r="DN13" s="60">
+      <c r="DM13" s="71"/>
+      <c r="DN13" s="70">
         <v>25</v>
       </c>
-      <c r="DO13" s="61"/>
-      <c r="DP13" s="60">
+      <c r="DO13" s="71"/>
+      <c r="DP13" s="70">
         <v>26</v>
       </c>
-      <c r="DQ13" s="61"/>
-      <c r="DR13" s="60">
+      <c r="DQ13" s="71"/>
+      <c r="DR13" s="70">
         <v>27</v>
       </c>
-      <c r="DS13" s="61"/>
-      <c r="DT13" s="60">
+      <c r="DS13" s="71"/>
+      <c r="DT13" s="70">
         <v>28</v>
       </c>
-      <c r="DU13" s="61"/>
-      <c r="DV13" s="60">
+      <c r="DU13" s="71"/>
+      <c r="DV13" s="70">
         <v>29</v>
       </c>
-      <c r="DW13" s="61"/>
-      <c r="DX13" s="60">
+      <c r="DW13" s="71"/>
+      <c r="DX13" s="70">
         <v>30</v>
       </c>
-      <c r="DY13" s="61"/>
-      <c r="DZ13" s="60">
+      <c r="DY13" s="71"/>
+      <c r="DZ13" s="70">
         <v>1</v>
       </c>
-      <c r="EA13" s="61"/>
-      <c r="EB13" s="60">
+      <c r="EA13" s="71"/>
+      <c r="EB13" s="70">
         <v>2</v>
       </c>
-      <c r="EC13" s="61"/>
-      <c r="ED13" s="60">
+      <c r="EC13" s="71"/>
+      <c r="ED13" s="70">
         <v>3</v>
       </c>
-      <c r="EE13" s="61"/>
-      <c r="EF13" s="60">
+      <c r="EE13" s="71"/>
+      <c r="EF13" s="70">
         <v>4</v>
       </c>
-      <c r="EG13" s="61"/>
-      <c r="EH13" s="60">
+      <c r="EG13" s="71"/>
+      <c r="EH13" s="70">
         <v>5</v>
       </c>
-      <c r="EI13" s="61"/>
-      <c r="EJ13" s="60">
+      <c r="EI13" s="71"/>
+      <c r="EJ13" s="70">
         <v>6</v>
       </c>
-      <c r="EK13" s="61"/>
-      <c r="EL13" s="60">
+      <c r="EK13" s="71"/>
+      <c r="EL13" s="70">
         <v>7</v>
       </c>
-      <c r="EM13" s="61"/>
-      <c r="EN13" s="60">
+      <c r="EM13" s="71"/>
+      <c r="EN13" s="70">
         <v>8</v>
       </c>
-      <c r="EO13" s="61"/>
-      <c r="EP13" s="60">
+      <c r="EO13" s="71"/>
+      <c r="EP13" s="70">
         <v>9</v>
       </c>
-      <c r="EQ13" s="61"/>
-      <c r="ER13" s="60">
+      <c r="EQ13" s="71"/>
+      <c r="ER13" s="70">
         <v>10</v>
       </c>
-      <c r="ES13" s="61"/>
-      <c r="ET13" s="60">
+      <c r="ES13" s="71"/>
+      <c r="ET13" s="70">
         <v>11</v>
       </c>
-      <c r="EU13" s="61"/>
-      <c r="EV13" s="60">
+      <c r="EU13" s="71"/>
+      <c r="EV13" s="70">
         <v>12</v>
       </c>
-      <c r="EW13" s="61"/>
-      <c r="EX13" s="60">
+      <c r="EW13" s="71"/>
+      <c r="EX13" s="70">
         <v>13</v>
       </c>
-      <c r="EY13" s="61"/>
-      <c r="EZ13" s="60">
+      <c r="EY13" s="71"/>
+      <c r="EZ13" s="70">
         <v>14</v>
       </c>
-      <c r="FA13" s="61"/>
-      <c r="FB13" s="60">
+      <c r="FA13" s="71"/>
+      <c r="FB13" s="70">
         <v>15</v>
       </c>
-      <c r="FC13" s="61"/>
-      <c r="FD13" s="60">
+      <c r="FC13" s="71"/>
+      <c r="FD13" s="70">
         <v>16</v>
       </c>
-      <c r="FE13" s="61"/>
-      <c r="FF13" s="60">
+      <c r="FE13" s="71"/>
+      <c r="FF13" s="70">
         <v>17</v>
       </c>
-      <c r="FG13" s="61"/>
-      <c r="FH13" s="60">
+      <c r="FG13" s="71"/>
+      <c r="FH13" s="70">
         <v>18</v>
       </c>
-      <c r="FI13" s="61"/>
-      <c r="FJ13" s="60">
+      <c r="FI13" s="71"/>
+      <c r="FJ13" s="70">
         <v>19</v>
       </c>
-      <c r="FK13" s="61"/>
-      <c r="FL13" s="60">
+      <c r="FK13" s="71"/>
+      <c r="FL13" s="70">
         <v>20</v>
       </c>
-      <c r="FM13" s="61"/>
-      <c r="FN13" s="60">
+      <c r="FM13" s="71"/>
+      <c r="FN13" s="70">
         <v>21</v>
       </c>
-      <c r="FO13" s="61"/>
-      <c r="FP13" s="60">
+      <c r="FO13" s="71"/>
+      <c r="FP13" s="70">
         <v>22</v>
       </c>
-      <c r="FQ13" s="61"/>
-      <c r="FR13" s="60">
+      <c r="FQ13" s="71"/>
+      <c r="FR13" s="70">
         <v>23</v>
       </c>
-      <c r="FS13" s="61"/>
-      <c r="FT13" s="60">
+      <c r="FS13" s="71"/>
+      <c r="FT13" s="70">
         <v>24</v>
       </c>
-      <c r="FU13" s="61"/>
-      <c r="FV13" s="60">
+      <c r="FU13" s="71"/>
+      <c r="FV13" s="70">
         <v>25</v>
       </c>
-      <c r="FW13" s="61"/>
-      <c r="FX13" s="60">
+      <c r="FW13" s="71"/>
+      <c r="FX13" s="70">
         <v>26</v>
       </c>
-      <c r="FY13" s="61"/>
-      <c r="FZ13" s="60">
+      <c r="FY13" s="71"/>
+      <c r="FZ13" s="70">
         <v>27</v>
       </c>
-      <c r="GA13" s="61"/>
-      <c r="GB13" s="60">
+      <c r="GA13" s="71"/>
+      <c r="GB13" s="70">
         <v>28</v>
       </c>
-      <c r="GC13" s="61"/>
-      <c r="GD13" s="60">
+      <c r="GC13" s="71"/>
+      <c r="GD13" s="70">
         <v>29</v>
       </c>
-      <c r="GE13" s="61"/>
-      <c r="GF13" s="60">
+      <c r="GE13" s="71"/>
+      <c r="GF13" s="70">
         <v>30</v>
       </c>
-      <c r="GG13" s="61"/>
-      <c r="GH13" s="60">
+      <c r="GG13" s="71"/>
+      <c r="GH13" s="70">
         <v>31</v>
       </c>
-      <c r="GI13" s="61"/>
+      <c r="GI13" s="71"/>
     </row>
     <row r="14" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A14" s="113" t="s">
+      <c r="A14" s="76" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="114"/>
+      <c r="B14" s="77"/>
       <c r="C14" s="37"/>
-      <c r="D14" s="97">
+      <c r="D14" s="93">
         <f>SUM(D15:E61)</f>
         <v>51.050000000000011</v>
       </c>
-      <c r="E14" s="99"/>
-      <c r="F14" s="97">
+      <c r="E14" s="95"/>
+      <c r="F14" s="93">
         <f>SUM(F15:G61)</f>
-        <v>44.725999999999999</v>
-      </c>
-      <c r="G14" s="98"/>
+        <v>45.975999999999999</v>
+      </c>
+      <c r="G14" s="94"/>
       <c r="H14" s="18"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -2849,22 +2849,22 @@
       <c r="GI14" s="14"/>
     </row>
     <row r="15" spans="1:191" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="74"/>
+      <c r="B15" s="85"/>
       <c r="C15" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="65">
+      <c r="D15" s="62">
         <v>1.5</v>
       </c>
-      <c r="E15" s="66"/>
-      <c r="F15" s="65">
+      <c r="E15" s="63"/>
+      <c r="F15" s="62">
         <f>SUM(H15:GI15)</f>
         <v>0.5</v>
       </c>
-      <c r="G15" s="80"/>
+      <c r="G15" s="64"/>
       <c r="H15" s="47"/>
       <c r="I15" s="12"/>
       <c r="J15" s="24">
@@ -3053,22 +3053,22 @@
       <c r="GI15" s="34"/>
     </row>
     <row r="16" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A16" s="81" t="s">
+      <c r="A16" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="82"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="62">
         <v>0.6</v>
       </c>
-      <c r="E16" s="66"/>
-      <c r="F16" s="65">
+      <c r="E16" s="63"/>
+      <c r="F16" s="62">
         <f>SUM(H16:GI16)</f>
         <v>0.6</v>
       </c>
-      <c r="G16" s="80"/>
+      <c r="G16" s="64"/>
       <c r="H16" s="47"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
@@ -3257,22 +3257,22 @@
       <c r="GI16" s="32"/>
     </row>
     <row r="17" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A17" s="81" t="s">
+      <c r="A17" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="82"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="65">
+      <c r="D17" s="62">
         <v>1</v>
       </c>
-      <c r="E17" s="66"/>
-      <c r="F17" s="65">
+      <c r="E17" s="63"/>
+      <c r="F17" s="62">
         <f>SUM(H17:GI17)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="80"/>
+      <c r="G17" s="64"/>
       <c r="H17" s="47"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
@@ -3463,22 +3463,22 @@
       <c r="GI17" s="32"/>
     </row>
     <row r="18" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A18" s="81" t="s">
+      <c r="A18" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="82"/>
+      <c r="B18" s="67"/>
       <c r="C18" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="65">
+      <c r="D18" s="62">
         <v>0.8</v>
       </c>
-      <c r="E18" s="66"/>
-      <c r="F18" s="65">
+      <c r="E18" s="63"/>
+      <c r="F18" s="62">
         <f t="shared" ref="F18:F60" si="0">SUM(H18:GI18)</f>
         <v>1.25</v>
       </c>
-      <c r="G18" s="80"/>
+      <c r="G18" s="64"/>
       <c r="H18" s="26"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
@@ -3669,22 +3669,22 @@
       <c r="GI18" s="32"/>
     </row>
     <row r="19" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="82"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="65">
+      <c r="D19" s="62">
         <v>0.5</v>
       </c>
-      <c r="E19" s="66"/>
-      <c r="F19" s="65">
+      <c r="E19" s="63"/>
+      <c r="F19" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="80"/>
+      <c r="G19" s="64"/>
       <c r="H19" s="26"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
@@ -3871,22 +3871,22 @@
       <c r="GI19" s="36"/>
     </row>
     <row r="20" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="82"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="65">
+      <c r="D20" s="62">
         <v>0.3</v>
       </c>
-      <c r="E20" s="66"/>
-      <c r="F20" s="65">
+      <c r="E20" s="63"/>
+      <c r="F20" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="80"/>
+      <c r="G20" s="64"/>
       <c r="H20" s="26"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -4073,22 +4073,22 @@
       <c r="GI20" s="36"/>
     </row>
     <row r="21" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A21" s="121" t="s">
+      <c r="A21" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="122"/>
+      <c r="B21" s="69"/>
       <c r="C21" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="65">
+      <c r="D21" s="62">
         <v>1</v>
       </c>
-      <c r="E21" s="66"/>
-      <c r="F21" s="65">
+      <c r="E21" s="63"/>
+      <c r="F21" s="62">
         <f t="shared" si="0"/>
         <v>0.16600000000000001</v>
       </c>
-      <c r="G21" s="80"/>
+      <c r="G21" s="64"/>
       <c r="H21" s="26"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
@@ -4277,22 +4277,22 @@
       <c r="GI21" s="36"/>
     </row>
     <row r="22" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A22" s="121" t="s">
+      <c r="A22" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="122"/>
+      <c r="B22" s="69"/>
       <c r="C22" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="65">
+      <c r="D22" s="62">
         <v>0.6</v>
       </c>
-      <c r="E22" s="66"/>
-      <c r="F22" s="65">
+      <c r="E22" s="63"/>
+      <c r="F22" s="62">
         <f t="shared" si="0"/>
         <v>0.66</v>
       </c>
-      <c r="G22" s="80"/>
+      <c r="G22" s="64"/>
       <c r="H22" s="26"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
@@ -4481,22 +4481,22 @@
       <c r="GI22" s="36"/>
     </row>
     <row r="23" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A23" s="121" t="s">
+      <c r="A23" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="122"/>
+      <c r="B23" s="69"/>
       <c r="C23" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="65">
+      <c r="D23" s="62">
         <v>0.6</v>
       </c>
-      <c r="E23" s="66"/>
-      <c r="F23" s="65">
+      <c r="E23" s="63"/>
+      <c r="F23" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="80"/>
+      <c r="G23" s="64"/>
       <c r="H23" s="26"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
@@ -4683,22 +4683,22 @@
       <c r="GI23" s="36"/>
     </row>
     <row r="24" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A24" s="121" t="s">
+      <c r="A24" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="122"/>
+      <c r="B24" s="69"/>
       <c r="C24" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="65">
+      <c r="D24" s="62">
         <v>3</v>
       </c>
-      <c r="E24" s="66"/>
-      <c r="F24" s="65">
+      <c r="E24" s="63"/>
+      <c r="F24" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="80"/>
+      <c r="G24" s="64"/>
       <c r="H24" s="26"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
@@ -4885,22 +4885,22 @@
       <c r="GI24" s="36"/>
     </row>
     <row r="25" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A25" s="121" t="s">
+      <c r="A25" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="122"/>
+      <c r="B25" s="69"/>
       <c r="C25" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="65">
+      <c r="D25" s="62">
         <v>1.5</v>
       </c>
-      <c r="E25" s="66"/>
-      <c r="F25" s="65">
+      <c r="E25" s="63"/>
+      <c r="F25" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="80"/>
+      <c r="G25" s="64"/>
       <c r="H25" s="26"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
@@ -5087,22 +5087,22 @@
       <c r="GI25" s="36"/>
     </row>
     <row r="26" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A26" s="121" t="s">
+      <c r="A26" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="122"/>
+      <c r="B26" s="69"/>
       <c r="C26" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="65">
+      <c r="D26" s="62">
         <v>1</v>
       </c>
-      <c r="E26" s="66"/>
-      <c r="F26" s="65">
+      <c r="E26" s="63"/>
+      <c r="F26" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="80"/>
+      <c r="G26" s="64"/>
       <c r="H26" s="26"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
@@ -5289,22 +5289,22 @@
       <c r="GI26" s="36"/>
     </row>
     <row r="27" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="81" t="s">
+      <c r="A27" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="82"/>
+      <c r="B27" s="67"/>
       <c r="C27" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="65">
+      <c r="D27" s="62">
         <v>1</v>
       </c>
-      <c r="E27" s="66"/>
-      <c r="F27" s="65">
+      <c r="E27" s="63"/>
+      <c r="F27" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G27" s="80"/>
+      <c r="G27" s="64"/>
       <c r="H27" s="26"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
@@ -5491,22 +5491,22 @@
       <c r="GI27" s="36"/>
     </row>
     <row r="28" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A28" s="81" t="s">
+      <c r="A28" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="82"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="65">
+      <c r="D28" s="62">
         <v>1</v>
       </c>
-      <c r="E28" s="66"/>
-      <c r="F28" s="65">
+      <c r="E28" s="63"/>
+      <c r="F28" s="62">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G28" s="80"/>
+      <c r="G28" s="64"/>
       <c r="H28" s="26"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
@@ -5695,22 +5695,22 @@
       <c r="GI28" s="36"/>
     </row>
     <row r="29" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A29" s="81" t="s">
+      <c r="A29" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="82"/>
+      <c r="B29" s="67"/>
       <c r="C29" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="65">
+      <c r="D29" s="62">
         <v>1</v>
       </c>
-      <c r="E29" s="66"/>
-      <c r="F29" s="65">
+      <c r="E29" s="63"/>
+      <c r="F29" s="62">
         <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
-      <c r="G29" s="80"/>
+      <c r="G29" s="64"/>
       <c r="H29" s="26"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
@@ -5901,22 +5901,22 @@
       <c r="GI29" s="36"/>
     </row>
     <row r="30" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A30" s="81" t="s">
+      <c r="A30" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="82"/>
+      <c r="B30" s="67"/>
       <c r="C30" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="65">
+      <c r="D30" s="62">
         <v>1</v>
       </c>
-      <c r="E30" s="66"/>
-      <c r="F30" s="65">
+      <c r="E30" s="63"/>
+      <c r="F30" s="62">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G30" s="80"/>
+      <c r="G30" s="64"/>
       <c r="H30" s="26"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
@@ -6105,22 +6105,22 @@
       <c r="GI30" s="36"/>
     </row>
     <row r="31" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A31" s="81" t="s">
+      <c r="A31" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="82"/>
+      <c r="B31" s="67"/>
       <c r="C31" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="65">
+      <c r="D31" s="62">
         <v>4</v>
       </c>
-      <c r="E31" s="66"/>
-      <c r="F31" s="65">
+      <c r="E31" s="63"/>
+      <c r="F31" s="62">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G31" s="80"/>
+      <c r="G31" s="64"/>
       <c r="H31" s="26"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
@@ -6311,22 +6311,22 @@
       <c r="GI31" s="36"/>
     </row>
     <row r="32" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A32" s="81" t="s">
+      <c r="A32" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="82"/>
+      <c r="B32" s="67"/>
       <c r="C32" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="65">
+      <c r="D32" s="62">
         <v>0.6</v>
       </c>
-      <c r="E32" s="66"/>
-      <c r="F32" s="65">
+      <c r="E32" s="63"/>
+      <c r="F32" s="62">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G32" s="80"/>
+      <c r="G32" s="64"/>
       <c r="H32" s="26"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
@@ -6515,22 +6515,22 @@
       <c r="GI32" s="36"/>
     </row>
     <row r="33" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="81" t="s">
+      <c r="A33" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="82"/>
+      <c r="B33" s="67"/>
       <c r="C33" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="65">
+      <c r="D33" s="62">
         <v>0.5</v>
       </c>
-      <c r="E33" s="66"/>
-      <c r="F33" s="65">
+      <c r="E33" s="63"/>
+      <c r="F33" s="62">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G33" s="80"/>
+      <c r="G33" s="64"/>
       <c r="H33" s="26"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
@@ -6719,22 +6719,22 @@
       <c r="GI33" s="36"/>
     </row>
     <row r="34" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A34" s="81" t="s">
+      <c r="A34" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="82"/>
+      <c r="B34" s="67"/>
       <c r="C34" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="65">
+      <c r="D34" s="62">
         <v>0.3</v>
       </c>
-      <c r="E34" s="66"/>
-      <c r="F34" s="65">
+      <c r="E34" s="63"/>
+      <c r="F34" s="62">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G34" s="80"/>
+      <c r="G34" s="64"/>
       <c r="H34" s="26"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
@@ -6923,22 +6923,22 @@
       <c r="GI34" s="36"/>
     </row>
     <row r="35" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A35" s="81" t="s">
+      <c r="A35" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="82"/>
+      <c r="B35" s="67"/>
       <c r="C35" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="65">
+      <c r="D35" s="62">
         <v>0.3</v>
       </c>
-      <c r="E35" s="66"/>
-      <c r="F35" s="65">
+      <c r="E35" s="63"/>
+      <c r="F35" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G35" s="80"/>
+      <c r="G35" s="64"/>
       <c r="H35" s="26"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
@@ -7125,22 +7125,22 @@
       <c r="GI35" s="36"/>
     </row>
     <row r="36" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A36" s="81" t="s">
+      <c r="A36" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="82"/>
+      <c r="B36" s="67"/>
       <c r="C36" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="65">
+      <c r="D36" s="62">
         <v>1.5</v>
       </c>
-      <c r="E36" s="66"/>
-      <c r="F36" s="65">
+      <c r="E36" s="63"/>
+      <c r="F36" s="62">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G36" s="80"/>
+        <v>1.25</v>
+      </c>
+      <c r="G36" s="64"/>
       <c r="H36" s="26"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
@@ -7186,7 +7186,9 @@
       <c r="AX36" s="32"/>
       <c r="AY36" s="32"/>
       <c r="AZ36" s="32"/>
-      <c r="BA36" s="32"/>
+      <c r="BA36" s="24">
+        <v>1.25</v>
+      </c>
       <c r="BB36" s="49"/>
       <c r="BC36" s="52"/>
       <c r="BD36" s="51"/>
@@ -7327,22 +7329,22 @@
       <c r="GI36" s="36"/>
     </row>
     <row r="37" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A37" s="81" t="s">
+      <c r="A37" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="82"/>
+      <c r="B37" s="67"/>
       <c r="C37" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="65">
+      <c r="D37" s="62">
         <v>0.5</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="65">
+      <c r="E37" s="63"/>
+      <c r="F37" s="62">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G37" s="80"/>
+      <c r="G37" s="64"/>
       <c r="H37" s="26"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
@@ -7531,22 +7533,22 @@
       <c r="GI37" s="36"/>
     </row>
     <row r="38" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A38" s="81" t="s">
+      <c r="A38" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="82"/>
+      <c r="B38" s="67"/>
       <c r="C38" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="65">
+      <c r="D38" s="62">
         <v>0.25</v>
       </c>
-      <c r="E38" s="66"/>
-      <c r="F38" s="65">
+      <c r="E38" s="63"/>
+      <c r="F38" s="62">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G38" s="80"/>
+      <c r="G38" s="64"/>
       <c r="H38" s="26"/>
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
@@ -7735,22 +7737,22 @@
       <c r="GI38" s="36"/>
     </row>
     <row r="39" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A39" s="81" t="s">
+      <c r="A39" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="82"/>
+      <c r="B39" s="67"/>
       <c r="C39" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="65">
+      <c r="D39" s="62">
         <v>0.5</v>
       </c>
-      <c r="E39" s="66"/>
-      <c r="F39" s="65">
+      <c r="E39" s="63"/>
+      <c r="F39" s="62">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="G39" s="80"/>
+      <c r="G39" s="64"/>
       <c r="H39" s="26"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
@@ -7939,22 +7941,22 @@
       <c r="GI39" s="36"/>
     </row>
     <row r="40" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A40" s="81" t="s">
+      <c r="A40" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="82"/>
+      <c r="B40" s="67"/>
       <c r="C40" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="65">
+      <c r="D40" s="62">
         <v>0.5</v>
       </c>
-      <c r="E40" s="66"/>
-      <c r="F40" s="65">
+      <c r="E40" s="63"/>
+      <c r="F40" s="62">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G40" s="80"/>
+      <c r="G40" s="64"/>
       <c r="H40" s="26"/>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
@@ -8143,22 +8145,22 @@
       <c r="GI40" s="36"/>
     </row>
     <row r="41" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A41" s="81" t="s">
+      <c r="A41" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="82"/>
+      <c r="B41" s="67"/>
       <c r="C41" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="65">
+      <c r="D41" s="62">
         <v>0.3</v>
       </c>
-      <c r="E41" s="66"/>
-      <c r="F41" s="65">
+      <c r="E41" s="63"/>
+      <c r="F41" s="62">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G41" s="80"/>
+      <c r="G41" s="64"/>
       <c r="H41" s="26"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
@@ -8347,22 +8349,22 @@
       <c r="GI41" s="36"/>
     </row>
     <row r="42" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A42" s="81" t="s">
+      <c r="A42" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="82"/>
+      <c r="B42" s="67"/>
       <c r="C42" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="65">
+      <c r="D42" s="62">
         <v>0.5</v>
       </c>
-      <c r="E42" s="66"/>
-      <c r="F42" s="65">
+      <c r="E42" s="63"/>
+      <c r="F42" s="62">
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-      <c r="G42" s="80"/>
+      <c r="G42" s="64"/>
       <c r="H42" s="26"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
@@ -8551,22 +8553,22 @@
       <c r="GI42" s="36"/>
     </row>
     <row r="43" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A43" s="81" t="s">
+      <c r="A43" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="82"/>
+      <c r="B43" s="67"/>
       <c r="C43" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D43" s="65">
+      <c r="D43" s="62">
         <v>1.3</v>
       </c>
-      <c r="E43" s="66"/>
-      <c r="F43" s="65">
+      <c r="E43" s="63"/>
+      <c r="F43" s="62">
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
-      <c r="G43" s="80"/>
+      <c r="G43" s="64"/>
       <c r="H43" s="26"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
@@ -8757,22 +8759,22 @@
       <c r="GI43" s="36"/>
     </row>
     <row r="44" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="81" t="s">
+      <c r="A44" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="82"/>
+      <c r="B44" s="67"/>
       <c r="C44" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="65">
+      <c r="D44" s="62">
         <v>1.3</v>
       </c>
-      <c r="E44" s="66"/>
-      <c r="F44" s="65">
+      <c r="E44" s="63"/>
+      <c r="F44" s="62">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G44" s="80"/>
+      <c r="G44" s="64"/>
       <c r="H44" s="26"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
@@ -8961,22 +8963,22 @@
       <c r="GI44" s="36"/>
     </row>
     <row r="45" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A45" s="81" t="s">
+      <c r="A45" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="82"/>
+      <c r="B45" s="67"/>
       <c r="C45" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="65">
+      <c r="D45" s="62">
         <v>1</v>
       </c>
-      <c r="E45" s="66"/>
-      <c r="F45" s="65">
+      <c r="E45" s="63"/>
+      <c r="F45" s="62">
         <f t="shared" si="0"/>
         <v>1.05</v>
       </c>
-      <c r="G45" s="80"/>
+      <c r="G45" s="64"/>
       <c r="H45" s="26"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
@@ -9167,22 +9169,22 @@
       <c r="GI45" s="36"/>
     </row>
     <row r="46" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A46" s="81" t="s">
+      <c r="A46" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="82"/>
+      <c r="B46" s="67"/>
       <c r="C46" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="D46" s="65">
+      <c r="D46" s="62">
         <v>1</v>
       </c>
-      <c r="E46" s="66"/>
-      <c r="F46" s="65">
+      <c r="E46" s="63"/>
+      <c r="F46" s="62">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="G46" s="80"/>
+      <c r="G46" s="64"/>
       <c r="H46" s="26"/>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
@@ -9371,22 +9373,22 @@
       <c r="GI46" s="36"/>
     </row>
     <row r="47" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A47" s="81" t="s">
+      <c r="A47" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="82"/>
+      <c r="B47" s="67"/>
       <c r="C47" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="D47" s="65">
+      <c r="D47" s="62">
         <v>1</v>
       </c>
-      <c r="E47" s="66"/>
-      <c r="F47" s="65">
+      <c r="E47" s="63"/>
+      <c r="F47" s="62">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="G47" s="80"/>
+      <c r="G47" s="64"/>
       <c r="H47" s="26"/>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
@@ -9575,22 +9577,22 @@
       <c r="GI47" s="36"/>
     </row>
     <row r="48" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A48" s="81" t="s">
+      <c r="A48" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="B48" s="82"/>
+      <c r="B48" s="67"/>
       <c r="C48" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D48" s="65">
+      <c r="D48" s="62">
         <v>0.3</v>
       </c>
-      <c r="E48" s="66"/>
-      <c r="F48" s="65">
+      <c r="E48" s="63"/>
+      <c r="F48" s="62">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G48" s="80"/>
+      <c r="G48" s="64"/>
       <c r="H48" s="26"/>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
@@ -9779,22 +9781,22 @@
       <c r="GI48" s="36"/>
     </row>
     <row r="49" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A49" s="81" t="s">
+      <c r="A49" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="82"/>
+      <c r="B49" s="67"/>
       <c r="C49" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="65">
+      <c r="D49" s="62">
         <v>2</v>
       </c>
-      <c r="E49" s="66"/>
-      <c r="F49" s="65">
+      <c r="E49" s="63"/>
+      <c r="F49" s="62">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G49" s="80"/>
+      <c r="G49" s="64"/>
       <c r="H49" s="26"/>
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
@@ -9985,22 +9987,22 @@
       <c r="GI49" s="36"/>
     </row>
     <row r="50" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A50" s="81" t="s">
+      <c r="A50" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="82"/>
+      <c r="B50" s="67"/>
       <c r="C50" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="D50" s="65">
+      <c r="D50" s="62">
         <v>2</v>
       </c>
-      <c r="E50" s="66"/>
-      <c r="F50" s="65">
+      <c r="E50" s="63"/>
+      <c r="F50" s="62">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G50" s="80"/>
+      <c r="G50" s="64"/>
       <c r="H50" s="26"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
@@ -10191,22 +10193,22 @@
       <c r="GI50" s="36"/>
     </row>
     <row r="51" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A51" s="81" t="s">
+      <c r="A51" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="82"/>
+      <c r="B51" s="67"/>
       <c r="C51" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D51" s="65">
+      <c r="D51" s="62">
         <v>2</v>
       </c>
-      <c r="E51" s="66"/>
-      <c r="F51" s="65">
+      <c r="E51" s="63"/>
+      <c r="F51" s="62">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
-      <c r="G51" s="80"/>
+      <c r="G51" s="64"/>
       <c r="H51" s="26"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
@@ -10397,22 +10399,22 @@
       <c r="GI51" s="36"/>
     </row>
     <row r="52" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A52" s="81" t="s">
+      <c r="A52" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="82"/>
+      <c r="B52" s="67"/>
       <c r="C52" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="65">
+      <c r="D52" s="62">
         <v>2</v>
       </c>
-      <c r="E52" s="66"/>
-      <c r="F52" s="65">
+      <c r="E52" s="63"/>
+      <c r="F52" s="62">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G52" s="80"/>
+      <c r="G52" s="64"/>
       <c r="H52" s="26"/>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
@@ -10603,22 +10605,22 @@
       <c r="GI52" s="36"/>
     </row>
     <row r="53" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A53" s="81" t="s">
+      <c r="A53" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="82"/>
+      <c r="B53" s="67"/>
       <c r="C53" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D53" s="65">
+      <c r="D53" s="62">
         <v>2</v>
       </c>
-      <c r="E53" s="66"/>
-      <c r="F53" s="65">
+      <c r="E53" s="63"/>
+      <c r="F53" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G53" s="80"/>
+      <c r="G53" s="64"/>
       <c r="H53" s="26"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
@@ -10805,22 +10807,22 @@
       <c r="GI53" s="36"/>
     </row>
     <row r="54" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A54" s="81" t="s">
+      <c r="A54" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="82"/>
+      <c r="B54" s="67"/>
       <c r="C54" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="D54" s="65">
+      <c r="D54" s="62">
         <v>0.25</v>
       </c>
-      <c r="E54" s="66"/>
-      <c r="F54" s="65">
+      <c r="E54" s="63"/>
+      <c r="F54" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G54" s="80"/>
+      <c r="G54" s="64"/>
       <c r="H54" s="26"/>
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
@@ -11007,22 +11009,22 @@
       <c r="GI54" s="36"/>
     </row>
     <row r="55" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A55" s="81" t="s">
+      <c r="A55" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="82"/>
+      <c r="B55" s="67"/>
       <c r="C55" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="D55" s="65">
+      <c r="D55" s="62">
         <v>1</v>
       </c>
-      <c r="E55" s="66"/>
-      <c r="F55" s="65">
+      <c r="E55" s="63"/>
+      <c r="F55" s="62">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G55" s="80"/>
+      <c r="G55" s="64"/>
       <c r="H55" s="26"/>
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
@@ -11213,22 +11215,22 @@
       <c r="GI55" s="36"/>
     </row>
     <row r="56" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A56" s="81" t="s">
+      <c r="A56" s="66" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="82"/>
+      <c r="B56" s="67"/>
       <c r="C56" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="D56" s="65">
+      <c r="D56" s="62">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E56" s="66"/>
-      <c r="F56" s="65">
+      <c r="E56" s="63"/>
+      <c r="F56" s="62">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G56" s="80"/>
+      <c r="G56" s="64"/>
       <c r="H56" s="26"/>
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
@@ -11419,22 +11421,22 @@
       <c r="GI56" s="36"/>
     </row>
     <row r="57" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A57" s="81" t="s">
+      <c r="A57" s="66" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="82"/>
+      <c r="B57" s="67"/>
       <c r="C57" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="D57" s="65">
+      <c r="D57" s="62">
         <v>1.75</v>
       </c>
-      <c r="E57" s="66"/>
-      <c r="F57" s="65">
+      <c r="E57" s="63"/>
+      <c r="F57" s="62">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G57" s="80"/>
+      <c r="G57" s="64"/>
       <c r="H57" s="26"/>
       <c r="I57" s="12"/>
       <c r="J57" s="12"/>
@@ -11623,22 +11625,22 @@
       <c r="GI57" s="36"/>
     </row>
     <row r="58" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A58" s="81" t="s">
+      <c r="A58" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="B58" s="82"/>
+      <c r="B58" s="67"/>
       <c r="C58" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="D58" s="65">
+      <c r="D58" s="62">
         <v>0.6</v>
       </c>
-      <c r="E58" s="66"/>
-      <c r="F58" s="65">
+      <c r="E58" s="63"/>
+      <c r="F58" s="62">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G58" s="80"/>
+      <c r="G58" s="64"/>
       <c r="H58" s="26"/>
       <c r="I58" s="12"/>
       <c r="J58" s="12"/>
@@ -11827,22 +11829,22 @@
       <c r="GI58" s="36"/>
     </row>
     <row r="59" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="81" t="s">
+      <c r="A59" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="B59" s="82"/>
+      <c r="B59" s="67"/>
       <c r="C59" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="65">
+      <c r="D59" s="62">
         <v>1</v>
       </c>
-      <c r="E59" s="66"/>
-      <c r="F59" s="65">
+      <c r="E59" s="63"/>
+      <c r="F59" s="62">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G59" s="80"/>
+      <c r="G59" s="64"/>
       <c r="H59" s="26"/>
       <c r="I59" s="12"/>
       <c r="J59" s="12"/>
@@ -12033,22 +12035,22 @@
       <c r="GI59" s="36"/>
     </row>
     <row r="60" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A60" s="81" t="s">
+      <c r="A60" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="B60" s="82"/>
+      <c r="B60" s="67"/>
       <c r="C60" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="D60" s="65">
+      <c r="D60" s="62">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E60" s="66"/>
-      <c r="F60" s="65">
+      <c r="E60" s="63"/>
+      <c r="F60" s="62">
         <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
-      <c r="G60" s="80"/>
+      <c r="G60" s="64"/>
       <c r="H60" s="26"/>
       <c r="I60" s="12"/>
       <c r="J60" s="12"/>
@@ -12237,22 +12239,22 @@
       <c r="GI60" s="36"/>
     </row>
     <row r="61" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A61" s="81" t="s">
+      <c r="A61" s="66" t="s">
         <v>115</v>
       </c>
-      <c r="B61" s="82"/>
+      <c r="B61" s="67"/>
       <c r="C61" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="D61" s="65">
+      <c r="D61" s="62">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E61" s="66"/>
-      <c r="F61" s="65">
+      <c r="E61" s="63"/>
+      <c r="F61" s="62">
         <f>SUM(H61:GI61)</f>
         <v>1</v>
       </c>
-      <c r="G61" s="80"/>
+      <c r="G61" s="64"/>
       <c r="H61" s="26"/>
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
@@ -12441,21 +12443,21 @@
       <c r="GI61" s="36"/>
     </row>
     <row r="62" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A62" s="115" t="s">
+      <c r="A62" s="78" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="116"/>
+      <c r="B62" s="79"/>
       <c r="C62" s="39"/>
-      <c r="D62" s="71">
+      <c r="D62" s="80">
         <f>SUM(D63:E80)</f>
         <v>88.6</v>
       </c>
-      <c r="E62" s="117"/>
-      <c r="F62" s="71">
+      <c r="E62" s="81"/>
+      <c r="F62" s="80">
         <f>SUM(F63:G80)</f>
         <v>0</v>
       </c>
-      <c r="G62" s="75"/>
+      <c r="G62" s="82"/>
       <c r="H62" s="29"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
@@ -12642,22 +12644,22 @@
       <c r="GI62" s="29"/>
     </row>
     <row r="63" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="118" t="s">
+      <c r="A63" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="119"/>
+      <c r="B63" s="61"/>
       <c r="C63" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D63" s="65">
+      <c r="D63" s="62">
         <v>0.6</v>
       </c>
-      <c r="E63" s="66"/>
-      <c r="F63" s="65">
+      <c r="E63" s="63"/>
+      <c r="F63" s="62">
         <f>SUM(H63:GI63)</f>
         <v>0</v>
       </c>
-      <c r="G63" s="80"/>
+      <c r="G63" s="64"/>
       <c r="H63" s="47"/>
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
@@ -12844,22 +12846,22 @@
       <c r="GI63" s="32"/>
     </row>
     <row r="64" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="118" t="s">
+      <c r="A64" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="B64" s="119"/>
+      <c r="B64" s="61"/>
       <c r="C64" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D64" s="65">
+      <c r="D64" s="62">
         <v>1.5</v>
       </c>
-      <c r="E64" s="66"/>
-      <c r="F64" s="65">
+      <c r="E64" s="63"/>
+      <c r="F64" s="62">
         <f>SUM(H64:GI64)</f>
         <v>0</v>
       </c>
-      <c r="G64" s="80"/>
+      <c r="G64" s="64"/>
       <c r="H64" s="47"/>
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
@@ -13046,22 +13048,22 @@
       <c r="GI64" s="32"/>
     </row>
     <row r="65" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A65" s="118" t="s">
+      <c r="A65" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="B65" s="119"/>
+      <c r="B65" s="61"/>
       <c r="C65" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D65" s="65">
+      <c r="D65" s="62">
         <v>1</v>
       </c>
-      <c r="E65" s="66"/>
-      <c r="F65" s="65">
+      <c r="E65" s="63"/>
+      <c r="F65" s="62">
         <f t="shared" ref="F65:F80" si="1">SUM(H65:GI65)</f>
         <v>0</v>
       </c>
-      <c r="G65" s="80"/>
+      <c r="G65" s="64"/>
       <c r="H65" s="47"/>
       <c r="I65" s="12"/>
       <c r="J65" s="12"/>
@@ -13248,22 +13250,22 @@
       <c r="GI65" s="32"/>
     </row>
     <row r="66" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A66" s="118" t="s">
+      <c r="A66" s="60" t="s">
         <v>125</v>
       </c>
-      <c r="B66" s="119"/>
+      <c r="B66" s="61"/>
       <c r="C66" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D66" s="65">
+      <c r="D66" s="62">
         <v>0.5</v>
       </c>
-      <c r="E66" s="66"/>
-      <c r="F66" s="65">
+      <c r="E66" s="63"/>
+      <c r="F66" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G66" s="80"/>
+      <c r="G66" s="64"/>
       <c r="H66" s="47"/>
       <c r="I66" s="12"/>
       <c r="J66" s="12"/>
@@ -13450,22 +13452,22 @@
       <c r="GI66" s="32"/>
     </row>
     <row r="67" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A67" s="118" t="s">
+      <c r="A67" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="119"/>
+      <c r="B67" s="61"/>
       <c r="C67" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D67" s="65">
+      <c r="D67" s="62">
         <v>1</v>
       </c>
-      <c r="E67" s="66"/>
-      <c r="F67" s="65">
+      <c r="E67" s="63"/>
+      <c r="F67" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G67" s="80"/>
+      <c r="G67" s="64"/>
       <c r="H67" s="47"/>
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
@@ -13652,22 +13654,22 @@
       <c r="GI67" s="32"/>
     </row>
     <row r="68" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A68" s="118" t="s">
+      <c r="A68" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="B68" s="119"/>
+      <c r="B68" s="61"/>
       <c r="C68" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D68" s="65">
+      <c r="D68" s="62">
         <v>1</v>
       </c>
-      <c r="E68" s="66"/>
-      <c r="F68" s="65">
+      <c r="E68" s="63"/>
+      <c r="F68" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G68" s="80"/>
+      <c r="G68" s="64"/>
       <c r="H68" s="47"/>
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
@@ -13854,22 +13856,22 @@
       <c r="GI68" s="32"/>
     </row>
     <row r="69" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A69" s="118" t="s">
+      <c r="A69" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="B69" s="119"/>
+      <c r="B69" s="61"/>
       <c r="C69" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="D69" s="65">
+      <c r="D69" s="62">
         <v>4</v>
       </c>
-      <c r="E69" s="66"/>
-      <c r="F69" s="65">
+      <c r="E69" s="63"/>
+      <c r="F69" s="62">
         <f>SUM(H69:GI69)</f>
         <v>0</v>
       </c>
-      <c r="G69" s="80"/>
+      <c r="G69" s="64"/>
       <c r="H69" s="47"/>
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
@@ -14056,22 +14058,22 @@
       <c r="GI69" s="32"/>
     </row>
     <row r="70" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A70" s="118" t="s">
+      <c r="A70" s="60" t="s">
         <v>133</v>
       </c>
-      <c r="B70" s="119"/>
+      <c r="B70" s="61"/>
       <c r="C70" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="D70" s="65">
+      <c r="D70" s="62">
         <v>8</v>
       </c>
-      <c r="E70" s="66"/>
-      <c r="F70" s="65">
+      <c r="E70" s="63"/>
+      <c r="F70" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G70" s="80"/>
+      <c r="G70" s="64"/>
       <c r="H70" s="47"/>
       <c r="I70" s="12"/>
       <c r="J70" s="12"/>
@@ -14258,22 +14260,22 @@
       <c r="GI70" s="32"/>
     </row>
     <row r="71" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A71" s="118" t="s">
+      <c r="A71" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="B71" s="119"/>
+      <c r="B71" s="61"/>
       <c r="C71" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="D71" s="65">
+      <c r="D71" s="62">
         <v>1</v>
       </c>
-      <c r="E71" s="66"/>
-      <c r="F71" s="65">
+      <c r="E71" s="63"/>
+      <c r="F71" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G71" s="80"/>
+      <c r="G71" s="64"/>
       <c r="H71" s="47"/>
       <c r="I71" s="12"/>
       <c r="J71" s="12"/>
@@ -14460,22 +14462,22 @@
       <c r="GI71" s="32"/>
     </row>
     <row r="72" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A72" s="118" t="s">
+      <c r="A72" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="B72" s="119"/>
+      <c r="B72" s="61"/>
       <c r="C72" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="D72" s="65">
+      <c r="D72" s="62">
         <v>1</v>
       </c>
-      <c r="E72" s="66"/>
-      <c r="F72" s="65">
+      <c r="E72" s="63"/>
+      <c r="F72" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G72" s="80"/>
+      <c r="G72" s="64"/>
       <c r="H72" s="47"/>
       <c r="I72" s="12"/>
       <c r="J72" s="12"/>
@@ -14662,22 +14664,22 @@
       <c r="GI72" s="32"/>
     </row>
     <row r="73" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A73" s="118" t="s">
+      <c r="A73" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="B73" s="119"/>
+      <c r="B73" s="61"/>
       <c r="C73" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="D73" s="65">
+      <c r="D73" s="62">
         <v>4</v>
       </c>
-      <c r="E73" s="66"/>
-      <c r="F73" s="65">
+      <c r="E73" s="63"/>
+      <c r="F73" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G73" s="80"/>
+      <c r="G73" s="64"/>
       <c r="H73" s="47"/>
       <c r="I73" s="12"/>
       <c r="J73" s="12"/>
@@ -14864,22 +14866,22 @@
       <c r="GI73" s="32"/>
     </row>
     <row r="74" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A74" s="118" t="s">
+      <c r="A74" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="B74" s="119"/>
+      <c r="B74" s="61"/>
       <c r="C74" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="D74" s="65">
+      <c r="D74" s="62">
         <v>12</v>
       </c>
-      <c r="E74" s="66"/>
-      <c r="F74" s="65">
+      <c r="E74" s="63"/>
+      <c r="F74" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G74" s="80"/>
+      <c r="G74" s="64"/>
       <c r="H74" s="47"/>
       <c r="I74" s="12"/>
       <c r="J74" s="12"/>
@@ -15066,22 +15068,22 @@
       <c r="GI74" s="32"/>
     </row>
     <row r="75" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A75" s="118" t="s">
+      <c r="A75" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="B75" s="88"/>
+      <c r="B75" s="65"/>
       <c r="C75" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D75" s="65">
+      <c r="D75" s="62">
         <v>16</v>
       </c>
-      <c r="E75" s="66"/>
-      <c r="F75" s="65">
+      <c r="E75" s="63"/>
+      <c r="F75" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G75" s="80"/>
+      <c r="G75" s="64"/>
       <c r="H75" s="47"/>
       <c r="I75" s="12"/>
       <c r="J75" s="12"/>
@@ -15268,22 +15270,22 @@
       <c r="GI75" s="36"/>
     </row>
     <row r="76" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A76" s="118" t="s">
+      <c r="A76" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="B76" s="119"/>
+      <c r="B76" s="61"/>
       <c r="C76" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="D76" s="65">
+      <c r="D76" s="62">
         <v>5</v>
       </c>
-      <c r="E76" s="66"/>
-      <c r="F76" s="65">
+      <c r="E76" s="63"/>
+      <c r="F76" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G76" s="80"/>
+      <c r="G76" s="64"/>
       <c r="H76" s="47"/>
       <c r="I76" s="12"/>
       <c r="J76" s="12"/>
@@ -15470,22 +15472,22 @@
       <c r="GI76" s="32"/>
     </row>
     <row r="77" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A77" s="118" t="s">
+      <c r="A77" s="60" t="s">
         <v>146</v>
       </c>
-      <c r="B77" s="119"/>
+      <c r="B77" s="61"/>
       <c r="C77" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="D77" s="65">
+      <c r="D77" s="62">
         <v>4</v>
       </c>
-      <c r="E77" s="66"/>
-      <c r="F77" s="65">
+      <c r="E77" s="63"/>
+      <c r="F77" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G77" s="80"/>
+      <c r="G77" s="64"/>
       <c r="H77" s="47"/>
       <c r="I77" s="12"/>
       <c r="J77" s="12"/>
@@ -15672,22 +15674,22 @@
       <c r="GI77" s="32"/>
     </row>
     <row r="78" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A78" s="118" t="s">
+      <c r="A78" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="B78" s="119"/>
+      <c r="B78" s="61"/>
       <c r="C78" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="D78" s="65">
+      <c r="D78" s="62">
         <v>16</v>
       </c>
-      <c r="E78" s="66"/>
-      <c r="F78" s="65">
+      <c r="E78" s="63"/>
+      <c r="F78" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G78" s="80"/>
+      <c r="G78" s="64"/>
       <c r="H78" s="47"/>
       <c r="I78" s="12"/>
       <c r="J78" s="12"/>
@@ -15874,22 +15876,22 @@
       <c r="GI78" s="32"/>
     </row>
     <row r="79" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A79" s="73" t="s">
+      <c r="A79" s="84" t="s">
         <v>150</v>
       </c>
-      <c r="B79" s="74"/>
+      <c r="B79" s="85"/>
       <c r="C79" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="D79" s="65">
+      <c r="D79" s="62">
         <v>6</v>
       </c>
-      <c r="E79" s="66"/>
-      <c r="F79" s="65">
+      <c r="E79" s="63"/>
+      <c r="F79" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G79" s="80"/>
+      <c r="G79" s="64"/>
       <c r="H79" s="47"/>
       <c r="I79" s="12"/>
       <c r="J79" s="12"/>
@@ -16076,22 +16078,22 @@
       <c r="GI79" s="36"/>
     </row>
     <row r="80" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A80" s="73" t="s">
+      <c r="A80" s="84" t="s">
         <v>152</v>
       </c>
-      <c r="B80" s="74"/>
+      <c r="B80" s="85"/>
       <c r="C80" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D80" s="65">
+      <c r="D80" s="62">
         <v>6</v>
       </c>
-      <c r="E80" s="66"/>
-      <c r="F80" s="65">
+      <c r="E80" s="63"/>
+      <c r="F80" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G80" s="80"/>
+      <c r="G80" s="64"/>
       <c r="H80" s="47"/>
       <c r="I80" s="12"/>
       <c r="J80" s="12"/>
@@ -16278,21 +16280,21 @@
       <c r="GI80" s="36"/>
     </row>
     <row r="81" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A81" s="115" t="s">
+      <c r="A81" s="78" t="s">
         <v>153</v>
       </c>
-      <c r="B81" s="116"/>
+      <c r="B81" s="79"/>
       <c r="C81" s="39"/>
-      <c r="D81" s="71">
+      <c r="D81" s="80">
         <f>SUM(D82:E82)</f>
         <v>16</v>
       </c>
-      <c r="E81" s="72"/>
-      <c r="F81" s="71">
+      <c r="E81" s="90"/>
+      <c r="F81" s="80">
         <f>SUM(F82:G82)</f>
         <v>0</v>
       </c>
-      <c r="G81" s="75"/>
+      <c r="G81" s="82"/>
       <c r="H81" s="29"/>
       <c r="I81" s="8"/>
       <c r="J81" s="8"/>
@@ -16479,20 +16481,20 @@
       <c r="GI81" s="29"/>
     </row>
     <row r="82" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A82" s="93" t="s">
+      <c r="A82" s="88" t="s">
         <v>153</v>
       </c>
-      <c r="B82" s="94"/>
+      <c r="B82" s="89"/>
       <c r="C82" s="40"/>
-      <c r="D82" s="91">
+      <c r="D82" s="86">
         <v>16</v>
       </c>
-      <c r="E82" s="92"/>
-      <c r="F82" s="65">
+      <c r="E82" s="87"/>
+      <c r="F82" s="62">
         <f>SUM(H82:GI82)</f>
         <v>0</v>
       </c>
-      <c r="G82" s="80"/>
+      <c r="G82" s="64"/>
       <c r="H82" s="26"/>
       <c r="I82" s="12"/>
       <c r="J82" s="12"/>
@@ -16679,21 +16681,21 @@
       <c r="GI82" s="32"/>
     </row>
     <row r="83" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A83" s="110" t="s">
+      <c r="A83" s="106" t="s">
         <v>154</v>
       </c>
-      <c r="B83" s="111"/>
+      <c r="B83" s="107"/>
       <c r="C83" s="41"/>
-      <c r="D83" s="71">
+      <c r="D83" s="80">
         <f>SUM(D84:E84)</f>
         <v>32</v>
       </c>
-      <c r="E83" s="72"/>
-      <c r="F83" s="71">
+      <c r="E83" s="90"/>
+      <c r="F83" s="80">
         <f>SUM(F84:G84)</f>
         <v>0</v>
       </c>
-      <c r="G83" s="75"/>
+      <c r="G83" s="82"/>
       <c r="H83" s="29"/>
       <c r="I83" s="8"/>
       <c r="J83" s="8"/>
@@ -16880,20 +16882,20 @@
       <c r="GI83" s="29"/>
     </row>
     <row r="84" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A84" s="85" t="s">
+      <c r="A84" s="110" t="s">
         <v>154</v>
       </c>
-      <c r="B84" s="86"/>
+      <c r="B84" s="111"/>
       <c r="C84" s="42"/>
-      <c r="D84" s="65">
+      <c r="D84" s="62">
         <v>32</v>
       </c>
-      <c r="E84" s="66"/>
-      <c r="F84" s="65">
+      <c r="E84" s="63"/>
+      <c r="F84" s="62">
         <f>SUM(H84:GI84)</f>
         <v>0</v>
       </c>
-      <c r="G84" s="80"/>
+      <c r="G84" s="64"/>
       <c r="H84" s="26"/>
       <c r="I84" s="12"/>
       <c r="J84" s="12"/>
@@ -17080,21 +17082,21 @@
       <c r="GI84" s="32"/>
     </row>
     <row r="85" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A85" s="89" t="s">
+      <c r="A85" s="113" t="s">
         <v>155</v>
       </c>
-      <c r="B85" s="90"/>
+      <c r="B85" s="114"/>
       <c r="C85" s="43"/>
-      <c r="D85" s="71">
+      <c r="D85" s="80">
         <f>SUM(D86:E86)</f>
         <v>8</v>
       </c>
-      <c r="E85" s="72"/>
-      <c r="F85" s="95">
+      <c r="E85" s="90"/>
+      <c r="F85" s="91">
         <f>SUM(F86:G86)</f>
         <v>0</v>
       </c>
-      <c r="G85" s="96"/>
+      <c r="G85" s="92"/>
       <c r="H85" s="29"/>
       <c r="I85" s="8"/>
       <c r="J85" s="8"/>
@@ -17281,20 +17283,20 @@
       <c r="GI85" s="29"/>
     </row>
     <row r="86" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A86" s="87" t="s">
+      <c r="A86" s="112" t="s">
         <v>156</v>
       </c>
-      <c r="B86" s="88"/>
+      <c r="B86" s="65"/>
       <c r="C86" s="27"/>
-      <c r="D86" s="65">
+      <c r="D86" s="62">
         <v>8</v>
       </c>
-      <c r="E86" s="66"/>
-      <c r="F86" s="65">
+      <c r="E86" s="63"/>
+      <c r="F86" s="62">
         <f>SUM(H86:GI86)</f>
         <v>0</v>
       </c>
-      <c r="G86" s="80"/>
+      <c r="G86" s="64"/>
       <c r="H86" s="26"/>
       <c r="I86" s="12"/>
       <c r="J86" s="12"/>
@@ -17481,20 +17483,20 @@
       <c r="GI86" s="32"/>
     </row>
     <row r="87" spans="1:191" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A87" s="83" t="s">
+      <c r="A87" s="108" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="84"/>
+      <c r="B87" s="109"/>
       <c r="C87" s="43"/>
-      <c r="D87" s="71">
+      <c r="D87" s="80">
         <f>232-D90</f>
         <v>36.349999999999994</v>
       </c>
-      <c r="E87" s="72"/>
-      <c r="F87" s="71">
+      <c r="E87" s="90"/>
+      <c r="F87" s="80">
         <v>0</v>
       </c>
-      <c r="G87" s="75"/>
+      <c r="G87" s="82"/>
       <c r="H87" s="29"/>
       <c r="I87" s="8"/>
       <c r="J87" s="8"/>
@@ -17681,15 +17683,15 @@
       <c r="GI87" s="29"/>
     </row>
     <row r="88" spans="1:191" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="107" t="s">
+      <c r="A88" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="B88" s="108"/>
+      <c r="B88" s="104"/>
       <c r="C88" s="44"/>
-      <c r="D88" s="104"/>
-      <c r="E88" s="105"/>
-      <c r="F88" s="104"/>
-      <c r="G88" s="106"/>
+      <c r="D88" s="100"/>
+      <c r="E88" s="101"/>
+      <c r="F88" s="100"/>
+      <c r="G88" s="102"/>
       <c r="H88" s="28"/>
       <c r="I88" s="17"/>
       <c r="J88" s="17"/>
@@ -17928,21 +17930,21 @@
       <c r="AX89" s="3"/>
     </row>
     <row r="90" spans="1:191" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="102" t="s">
+      <c r="A90" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="103"/>
+      <c r="B90" s="99"/>
       <c r="C90" s="45"/>
-      <c r="D90" s="100">
+      <c r="D90" s="96">
         <f>SUM(D85,D83,D81,D62,D14)</f>
         <v>195.65</v>
       </c>
-      <c r="E90" s="101"/>
-      <c r="F90" s="100">
+      <c r="E90" s="97"/>
+      <c r="F90" s="96">
         <f>SUM(F85,F83,F81,F62,F14)</f>
-        <v>44.725999999999999</v>
-      </c>
-      <c r="G90" s="109"/>
+        <v>45.975999999999999</v>
+      </c>
+      <c r="G90" s="105"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
@@ -17989,132 +17991,190 @@
     </row>
   </sheetData>
   <mergeCells count="334">
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="BR13:BS13"/>
+    <mergeCell ref="BL13:BM13"/>
+    <mergeCell ref="BN13:BO13"/>
+    <mergeCell ref="BR12:DY12"/>
+    <mergeCell ref="DZ13:EA13"/>
+    <mergeCell ref="CL13:CM13"/>
+    <mergeCell ref="CN13:CO13"/>
+    <mergeCell ref="BT13:BU13"/>
+    <mergeCell ref="BV13:BW13"/>
+    <mergeCell ref="BX13:BY13"/>
+    <mergeCell ref="BZ13:CA13"/>
+    <mergeCell ref="CB13:CC13"/>
+    <mergeCell ref="CD13:CE13"/>
+    <mergeCell ref="CF13:CG13"/>
+    <mergeCell ref="CH13:CI13"/>
+    <mergeCell ref="CJ13:CK13"/>
+    <mergeCell ref="CP13:CQ13"/>
+    <mergeCell ref="CR13:CS13"/>
+    <mergeCell ref="CT13:CU13"/>
+    <mergeCell ref="CV13:CW13"/>
+    <mergeCell ref="CX13:CY13"/>
+    <mergeCell ref="CZ13:DA13"/>
+    <mergeCell ref="DB13:DC13"/>
+    <mergeCell ref="DD13:DE13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="P6:X6"/>
+    <mergeCell ref="P5:X5"/>
+    <mergeCell ref="P4:X4"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="H12:BQ12"/>
+    <mergeCell ref="BB13:BC13"/>
+    <mergeCell ref="BD13:BE13"/>
+    <mergeCell ref="BF13:BG13"/>
+    <mergeCell ref="BP13:BQ13"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="AF13:AG13"/>
+    <mergeCell ref="AH13:AI13"/>
+    <mergeCell ref="AJ13:AK13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="AL13:AM13"/>
+    <mergeCell ref="AN13:AO13"/>
+    <mergeCell ref="AP13:AQ13"/>
+    <mergeCell ref="AR13:AS13"/>
+    <mergeCell ref="AT13:AU13"/>
+    <mergeCell ref="AV13:AW13"/>
+    <mergeCell ref="AX13:AY13"/>
+    <mergeCell ref="AZ13:BA13"/>
+    <mergeCell ref="BH13:BI13"/>
+    <mergeCell ref="BJ13:BK13"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="P9:X9"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F11:G13"/>
+    <mergeCell ref="D11:E13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="DF13:DG13"/>
+    <mergeCell ref="DH13:DI13"/>
+    <mergeCell ref="DJ13:DK13"/>
+    <mergeCell ref="DL13:DM13"/>
+    <mergeCell ref="DN13:DO13"/>
+    <mergeCell ref="DP13:DQ13"/>
+    <mergeCell ref="DR13:DS13"/>
+    <mergeCell ref="DT13:DU13"/>
+    <mergeCell ref="DV13:DW13"/>
+    <mergeCell ref="FF13:FG13"/>
+    <mergeCell ref="DX13:DY13"/>
+    <mergeCell ref="FH13:FI13"/>
+    <mergeCell ref="FJ13:FK13"/>
+    <mergeCell ref="EB13:EC13"/>
+    <mergeCell ref="ED13:EE13"/>
+    <mergeCell ref="EF13:EG13"/>
+    <mergeCell ref="EH13:EI13"/>
+    <mergeCell ref="EJ13:EK13"/>
+    <mergeCell ref="EL13:EM13"/>
+    <mergeCell ref="EN13:EO13"/>
+    <mergeCell ref="EP13:EQ13"/>
+    <mergeCell ref="ER13:ES13"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="GD13:GE13"/>
+    <mergeCell ref="GF13:GG13"/>
+    <mergeCell ref="GH13:GI13"/>
+    <mergeCell ref="DZ12:GI12"/>
+    <mergeCell ref="FL13:FM13"/>
+    <mergeCell ref="FN13:FO13"/>
+    <mergeCell ref="FP13:FQ13"/>
+    <mergeCell ref="FR13:FS13"/>
+    <mergeCell ref="FT13:FU13"/>
+    <mergeCell ref="FV13:FW13"/>
+    <mergeCell ref="FX13:FY13"/>
+    <mergeCell ref="FZ13:GA13"/>
+    <mergeCell ref="GB13:GC13"/>
+    <mergeCell ref="ET13:EU13"/>
+    <mergeCell ref="EV13:EW13"/>
+    <mergeCell ref="EX13:EY13"/>
+    <mergeCell ref="EZ13:FA13"/>
+    <mergeCell ref="FB13:FC13"/>
+    <mergeCell ref="FD13:FE13"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="D32:E32"/>
@@ -18139,190 +18199,132 @@
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="GD13:GE13"/>
-    <mergeCell ref="GF13:GG13"/>
-    <mergeCell ref="GH13:GI13"/>
-    <mergeCell ref="DZ12:GI12"/>
-    <mergeCell ref="FL13:FM13"/>
-    <mergeCell ref="FN13:FO13"/>
-    <mergeCell ref="FP13:FQ13"/>
-    <mergeCell ref="FR13:FS13"/>
-    <mergeCell ref="FT13:FU13"/>
-    <mergeCell ref="FV13:FW13"/>
-    <mergeCell ref="FX13:FY13"/>
-    <mergeCell ref="FZ13:GA13"/>
-    <mergeCell ref="GB13:GC13"/>
-    <mergeCell ref="ET13:EU13"/>
-    <mergeCell ref="EV13:EW13"/>
-    <mergeCell ref="EX13:EY13"/>
-    <mergeCell ref="EZ13:FA13"/>
-    <mergeCell ref="FB13:FC13"/>
-    <mergeCell ref="FD13:FE13"/>
-    <mergeCell ref="FF13:FG13"/>
-    <mergeCell ref="DX13:DY13"/>
-    <mergeCell ref="FH13:FI13"/>
-    <mergeCell ref="FJ13:FK13"/>
-    <mergeCell ref="EB13:EC13"/>
-    <mergeCell ref="ED13:EE13"/>
-    <mergeCell ref="EF13:EG13"/>
-    <mergeCell ref="EH13:EI13"/>
-    <mergeCell ref="EJ13:EK13"/>
-    <mergeCell ref="EL13:EM13"/>
-    <mergeCell ref="EN13:EO13"/>
-    <mergeCell ref="EP13:EQ13"/>
-    <mergeCell ref="ER13:ES13"/>
-    <mergeCell ref="DF13:DG13"/>
-    <mergeCell ref="DH13:DI13"/>
-    <mergeCell ref="DJ13:DK13"/>
-    <mergeCell ref="DL13:DM13"/>
-    <mergeCell ref="DN13:DO13"/>
-    <mergeCell ref="DP13:DQ13"/>
-    <mergeCell ref="DR13:DS13"/>
-    <mergeCell ref="DT13:DU13"/>
-    <mergeCell ref="DV13:DW13"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="F90:G90"/>
-    <mergeCell ref="F87:G87"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="BH13:BI13"/>
-    <mergeCell ref="BJ13:BK13"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="P9:X9"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F11:G13"/>
-    <mergeCell ref="D11:E13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="AL13:AM13"/>
-    <mergeCell ref="AN13:AO13"/>
-    <mergeCell ref="AP13:AQ13"/>
-    <mergeCell ref="AR13:AS13"/>
-    <mergeCell ref="AT13:AU13"/>
-    <mergeCell ref="AV13:AW13"/>
-    <mergeCell ref="AX13:AY13"/>
-    <mergeCell ref="AZ13:BA13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="P6:X6"/>
-    <mergeCell ref="P5:X5"/>
-    <mergeCell ref="P4:X4"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="H12:BQ12"/>
-    <mergeCell ref="BB13:BC13"/>
-    <mergeCell ref="BD13:BE13"/>
-    <mergeCell ref="BF13:BG13"/>
-    <mergeCell ref="BP13:BQ13"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="AF13:AG13"/>
-    <mergeCell ref="AH13:AI13"/>
-    <mergeCell ref="AJ13:AK13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="BR13:BS13"/>
-    <mergeCell ref="BL13:BM13"/>
-    <mergeCell ref="BN13:BO13"/>
-    <mergeCell ref="BR12:DY12"/>
-    <mergeCell ref="DZ13:EA13"/>
-    <mergeCell ref="CL13:CM13"/>
-    <mergeCell ref="CN13:CO13"/>
-    <mergeCell ref="BT13:BU13"/>
-    <mergeCell ref="BV13:BW13"/>
-    <mergeCell ref="BX13:BY13"/>
-    <mergeCell ref="BZ13:CA13"/>
-    <mergeCell ref="CB13:CC13"/>
-    <mergeCell ref="CD13:CE13"/>
-    <mergeCell ref="CF13:CG13"/>
-    <mergeCell ref="CH13:CI13"/>
-    <mergeCell ref="CJ13:CK13"/>
-    <mergeCell ref="CP13:CQ13"/>
-    <mergeCell ref="CR13:CS13"/>
-    <mergeCell ref="CT13:CU13"/>
-    <mergeCell ref="CV13:CW13"/>
-    <mergeCell ref="CX13:CY13"/>
-    <mergeCell ref="CZ13:DA13"/>
-    <mergeCell ref="DB13:DC13"/>
-    <mergeCell ref="DD13:DE13"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>

</xml_diff>